<commit_message>
Place skills on the characters
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -227,12 +227,6 @@
     <t>Masquerade</t>
   </si>
   <si>
-    <t>Rake Locks or Pick Locks may be purchased for $1k less than their cost.</t>
-  </si>
-  <si>
-    <t>Rake Locks or Pick Locks may be purchased for $2k less than their cost.</t>
-  </si>
-  <si>
     <t>successful, but loud and disturbing</t>
   </si>
   <si>
@@ -276,6 +270,30 @@
   </si>
   <si>
     <t>much more destructive against cameras and guards, but raises alerts</t>
+  </si>
+  <si>
+    <t>Does everything better, no EXP</t>
+  </si>
+  <si>
+    <t>free, loud and unsuccessful</t>
+  </si>
+  <si>
+    <t>quiet, but not as successful</t>
+  </si>
+  <si>
+    <t>quiet, somewhat successful, but does not subdue the guards</t>
+  </si>
+  <si>
+    <t>great all around if you can get it</t>
+  </si>
+  <si>
+    <t>Rake Locks or Pick Locks may be purchased for $1k less than cost.</t>
+  </si>
+  <si>
+    <t>Rake Locks or Pick Locks may be purchased for $2k less than cost.</t>
+  </si>
+  <si>
+    <t>ExtraHack</t>
   </si>
 </sst>
 </file>
@@ -646,7 +664,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +677,7 @@
     <col min="6" max="6" width="6" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" style="6" bestFit="1" customWidth="1"/>
@@ -785,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -841,7 +859,7 @@
         <v>2</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1456,7 +1474,7 @@
         <v>2</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="J15" s="6">
         <v>4</v>
@@ -1509,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="J16" s="6">
         <v>4</v>
@@ -1562,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="J17" s="6">
         <v>4</v>
@@ -1615,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="J18" s="6">
         <v>4</v>
@@ -1668,7 +1686,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="J19" s="6">
         <v>4</v>
@@ -1702,346 +1720,422 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
+      <c r="C2">
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
+      <c r="C3">
+        <v>2</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="1">
-        <v>4</v>
+      <c r="C5">
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="1">
-        <v>5</v>
+      <c r="C7">
+        <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="1">
-        <v>0</v>
+      <c r="C8">
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
+      <c r="C9">
+        <v>2</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
+      <c r="C10">
+        <v>2</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1">
-        <v>5</v>
+      <c r="C12">
+        <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1">
-        <v>0</v>
+      <c r="C13">
+        <v>4</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
+      <c r="C14">
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
+      <c r="C15">
+        <v>2</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
         <v>3</v>
       </c>
-      <c r="D16" s="1">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="1">
-        <v>0</v>
+      <c r="C17">
+        <v>4</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="1">
-        <v>5</v>
+      <c r="C20">
+        <v>2</v>
       </c>
       <c r="D20" s="1">
-        <v>2</v>
-      </c>
-      <c r="F20" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
getting an initial build of the skills cards
they are messy, but they'll work for now.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -294,6 +294,36 @@
   </si>
   <si>
     <t>ExtraHack</t>
+  </si>
+  <si>
+    <t>CRASH! Success, +5 noise</t>
+  </si>
+  <si>
+    <t>Rolls</t>
+  </si>
+  <si>
+    <t>SMASH! Success, disturb room</t>
+  </si>
+  <si>
+    <t>UNLOCKED! Success!</t>
+  </si>
+  <si>
+    <t>BONK! Fail.</t>
+  </si>
+  <si>
+    <t>BONK! Fail. +2 EXP</t>
+  </si>
+  <si>
+    <t>CRASH! Success, +3 noise</t>
+  </si>
+  <si>
+    <t>CRASH! Success, +4 noise</t>
+  </si>
+  <si>
+    <t>NOPE! Fail.</t>
+  </si>
+  <si>
+    <t>NOPE! Fail</t>
   </si>
 </sst>
 </file>
@@ -337,10 +367,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -664,1052 +697,1052 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="74.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="74.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
         <v>0</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="7">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="6">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6">
-        <v>2</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="G2" s="7">
+        <v>5</v>
+      </c>
+      <c r="H2" s="7">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="7">
         <v>4</v>
       </c>
-      <c r="K2" s="6">
-        <v>2</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="K2" s="7">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="6">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6">
-        <v>2</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="M2" s="7">
+        <v>1</v>
+      </c>
+      <c r="N2" s="7">
+        <v>2</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>2</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="P2" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>2</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6">
-        <v>5</v>
-      </c>
-      <c r="H3" s="6">
-        <v>2</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="G3" s="7">
+        <v>5</v>
+      </c>
+      <c r="H3" s="7">
+        <v>2</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="7">
         <v>4</v>
       </c>
-      <c r="K3" s="6">
-        <v>2</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="7">
+        <v>2</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="6">
-        <v>1</v>
-      </c>
-      <c r="N3" s="6">
-        <v>2</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="M3" s="7">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>2</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="P3" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>2</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
         <v>0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="6">
-        <v>5</v>
-      </c>
-      <c r="H4" s="6">
-        <v>2</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="G4" s="7">
+        <v>5</v>
+      </c>
+      <c r="H4" s="7">
+        <v>2</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="7">
         <v>4</v>
       </c>
-      <c r="K4" s="6">
-        <v>2</v>
-      </c>
-      <c r="L4" s="6" t="s">
+      <c r="K4" s="7">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="6">
-        <v>1</v>
-      </c>
-      <c r="N4" s="6">
-        <v>2</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="M4" s="7">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>2</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="P4" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>2</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
         <v>15</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="6">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6">
-        <v>2</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="G5" s="7">
+        <v>5</v>
+      </c>
+      <c r="H5" s="7">
+        <v>2</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="7">
         <v>4</v>
       </c>
-      <c r="K5" s="6">
-        <v>2</v>
-      </c>
-      <c r="L5" s="6" t="s">
+      <c r="K5" s="7">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="6">
-        <v>1</v>
-      </c>
-      <c r="N5" s="6">
-        <v>2</v>
-      </c>
-      <c r="O5" s="3" t="s">
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
+        <v>2</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="6">
+      <c r="P5" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="6">
-        <v>5</v>
-      </c>
-      <c r="H6" s="6">
-        <v>2</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="G6" s="7">
+        <v>5</v>
+      </c>
+      <c r="H6" s="7">
+        <v>2</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="7">
         <v>4</v>
       </c>
-      <c r="K6" s="6">
-        <v>2</v>
-      </c>
-      <c r="L6" s="6" t="s">
+      <c r="K6" s="7">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="6">
-        <v>1</v>
-      </c>
-      <c r="N6" s="6">
-        <v>2</v>
-      </c>
-      <c r="O6" s="3" t="s">
+      <c r="M6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="6">
+      <c r="P6" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
         <v>15</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="6">
-        <v>5</v>
-      </c>
-      <c r="H7" s="6">
-        <v>2</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="G7" s="7">
+        <v>5</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="7">
         <v>4</v>
       </c>
-      <c r="K7" s="6">
-        <v>2</v>
-      </c>
-      <c r="L7" s="6" t="s">
+      <c r="K7" s="7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6">
-        <v>2</v>
-      </c>
-      <c r="O7" s="3" t="s">
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7">
+        <v>2</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="6">
+      <c r="P7" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
         <v>0</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>15</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="6">
-        <v>5</v>
-      </c>
-      <c r="H8" s="6">
-        <v>2</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="G8" s="7">
+        <v>5</v>
+      </c>
+      <c r="H8" s="7">
+        <v>2</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="7">
         <v>4</v>
       </c>
-      <c r="K8" s="6">
-        <v>2</v>
-      </c>
-      <c r="L8" s="6" t="s">
+      <c r="K8" s="7">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6">
-        <v>2</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
+        <v>2</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="6">
+      <c r="P8" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
         <v>15</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="6">
-        <v>5</v>
-      </c>
-      <c r="H9" s="6">
-        <v>2</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="G9" s="7">
+        <v>5</v>
+      </c>
+      <c r="H9" s="7">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="7">
         <v>4</v>
       </c>
-      <c r="K9" s="6">
-        <v>2</v>
-      </c>
-      <c r="L9" s="6" t="s">
+      <c r="K9" s="7">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="6">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
-        <v>2</v>
-      </c>
-      <c r="O9" s="3" t="s">
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7">
+        <v>2</v>
+      </c>
+      <c r="O9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q9" s="6">
+      <c r="P9" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
         <v>15</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="6">
-        <v>5</v>
-      </c>
-      <c r="H10" s="6">
-        <v>2</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="G10" s="7">
+        <v>5</v>
+      </c>
+      <c r="H10" s="7">
+        <v>2</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="7">
         <v>4</v>
       </c>
-      <c r="K10" s="6">
-        <v>2</v>
-      </c>
-      <c r="L10" s="6" t="s">
+      <c r="K10" s="7">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="6">
-        <v>1</v>
-      </c>
-      <c r="N10" s="6">
-        <v>2</v>
-      </c>
-      <c r="O10" s="3" t="s">
+      <c r="M10" s="7">
+        <v>1</v>
+      </c>
+      <c r="N10" s="7">
+        <v>2</v>
+      </c>
+      <c r="O10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P10" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="6">
+      <c r="P10" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7">
         <v>15</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="6">
-        <v>5</v>
-      </c>
-      <c r="H11" s="6">
-        <v>2</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="G11" s="7">
+        <v>5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>2</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="7">
         <v>4</v>
       </c>
-      <c r="K11" s="6">
-        <v>2</v>
-      </c>
-      <c r="L11" s="6" t="s">
+      <c r="K11" s="7">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="6">
-        <v>1</v>
-      </c>
-      <c r="N11" s="6">
-        <v>2</v>
-      </c>
-      <c r="O11" s="3" t="s">
+      <c r="M11" s="7">
+        <v>1</v>
+      </c>
+      <c r="N11" s="7">
+        <v>2</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P11" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q11" s="6">
+      <c r="P11" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="6">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
         <v>15</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="6">
-        <v>5</v>
-      </c>
-      <c r="H12" s="6">
-        <v>2</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="G12" s="7">
+        <v>5</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="7">
         <v>4</v>
       </c>
-      <c r="K12" s="6">
-        <v>2</v>
-      </c>
-      <c r="L12" s="6" t="s">
+      <c r="K12" s="7">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="6">
-        <v>1</v>
-      </c>
-      <c r="N12" s="6">
-        <v>2</v>
-      </c>
-      <c r="O12" s="3" t="s">
+      <c r="M12" s="7">
+        <v>1</v>
+      </c>
+      <c r="N12" s="7">
+        <v>2</v>
+      </c>
+      <c r="O12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P12" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q12" s="6">
+      <c r="P12" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
         <v>15</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="6">
-        <v>5</v>
-      </c>
-      <c r="H13" s="6">
-        <v>2</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="G13" s="7">
+        <v>5</v>
+      </c>
+      <c r="H13" s="7">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="7">
         <v>4</v>
       </c>
-      <c r="K13" s="6">
-        <v>2</v>
-      </c>
-      <c r="L13" s="6" t="s">
+      <c r="K13" s="7">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="6">
-        <v>1</v>
-      </c>
-      <c r="N13" s="6">
-        <v>2</v>
-      </c>
-      <c r="O13" s="3" t="s">
+      <c r="M13" s="7">
+        <v>1</v>
+      </c>
+      <c r="N13" s="7">
+        <v>2</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q13" s="6">
+      <c r="P13" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6">
-        <v>2</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7">
         <v>15</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="6">
-        <v>5</v>
-      </c>
-      <c r="H14" s="6">
-        <v>2</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="G14" s="7">
+        <v>5</v>
+      </c>
+      <c r="H14" s="7">
+        <v>2</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="7">
         <v>4</v>
       </c>
-      <c r="K14" s="6">
-        <v>2</v>
-      </c>
-      <c r="L14" s="6" t="s">
+      <c r="K14" s="7">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="6">
-        <v>1</v>
-      </c>
-      <c r="N14" s="6">
-        <v>2</v>
-      </c>
-      <c r="O14" s="3" t="s">
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7">
+        <v>2</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="6">
+      <c r="P14" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
         <v>0</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="7">
         <v>15</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="6">
-        <v>5</v>
-      </c>
-      <c r="H15" s="6">
-        <v>2</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="G15" s="7">
+        <v>5</v>
+      </c>
+      <c r="H15" s="7">
+        <v>2</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="7">
         <v>4</v>
       </c>
-      <c r="K15" s="6">
-        <v>2</v>
-      </c>
-      <c r="L15" s="6" t="s">
+      <c r="K15" s="7">
+        <v>2</v>
+      </c>
+      <c r="L15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="6">
-        <v>1</v>
-      </c>
-      <c r="N15" s="6">
-        <v>2</v>
-      </c>
-      <c r="O15" s="3" t="s">
+      <c r="M15" s="7">
+        <v>1</v>
+      </c>
+      <c r="N15" s="7">
+        <v>2</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P15" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q15" s="6">
+      <c r="P15" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
         <v>15</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="6">
-        <v>5</v>
-      </c>
-      <c r="H16" s="6">
-        <v>2</v>
-      </c>
-      <c r="I16" s="6" t="s">
+      <c r="G16" s="7">
+        <v>5</v>
+      </c>
+      <c r="H16" s="7">
+        <v>2</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="7">
         <v>4</v>
       </c>
-      <c r="K16" s="6">
-        <v>2</v>
-      </c>
-      <c r="L16" s="6" t="s">
+      <c r="K16" s="7">
+        <v>2</v>
+      </c>
+      <c r="L16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="6">
-        <v>1</v>
-      </c>
-      <c r="N16" s="6">
-        <v>2</v>
-      </c>
-      <c r="O16" s="3" t="s">
+      <c r="M16" s="7">
+        <v>1</v>
+      </c>
+      <c r="N16" s="7">
+        <v>2</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P16" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q16" s="6">
+      <c r="P16" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
         <v>15</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="6">
-        <v>5</v>
-      </c>
-      <c r="H17" s="6">
-        <v>2</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="G17" s="7">
+        <v>5</v>
+      </c>
+      <c r="H17" s="7">
+        <v>2</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="7">
         <v>4</v>
       </c>
-      <c r="K17" s="6">
-        <v>2</v>
-      </c>
-      <c r="L17" s="6" t="s">
+      <c r="K17" s="7">
+        <v>2</v>
+      </c>
+      <c r="L17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="6">
-        <v>1</v>
-      </c>
-      <c r="N17" s="6">
-        <v>2</v>
-      </c>
-      <c r="O17" s="3" t="s">
+      <c r="M17" s="7">
+        <v>1</v>
+      </c>
+      <c r="N17" s="7">
+        <v>2</v>
+      </c>
+      <c r="O17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P17" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q17" s="6">
+      <c r="P17" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7">
         <v>15</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="6">
-        <v>5</v>
-      </c>
-      <c r="H18" s="6">
-        <v>2</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="G18" s="7">
+        <v>5</v>
+      </c>
+      <c r="H18" s="7">
+        <v>2</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="7">
         <v>4</v>
       </c>
-      <c r="K18" s="6">
-        <v>2</v>
-      </c>
-      <c r="L18" s="6" t="s">
+      <c r="K18" s="7">
+        <v>2</v>
+      </c>
+      <c r="L18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="6">
-        <v>1</v>
-      </c>
-      <c r="N18" s="6">
-        <v>2</v>
-      </c>
-      <c r="O18" s="3" t="s">
+      <c r="M18" s="7">
+        <v>1</v>
+      </c>
+      <c r="N18" s="7">
+        <v>2</v>
+      </c>
+      <c r="O18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P18" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q18" s="6">
+      <c r="P18" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6">
-        <v>2</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
+        <v>2</v>
+      </c>
+      <c r="E19" s="7">
         <v>15</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="6">
-        <v>5</v>
-      </c>
-      <c r="H19" s="6">
-        <v>2</v>
-      </c>
-      <c r="I19" s="6" t="s">
+      <c r="G19" s="7">
+        <v>5</v>
+      </c>
+      <c r="H19" s="7">
+        <v>2</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="7">
         <v>4</v>
       </c>
-      <c r="K19" s="6">
-        <v>2</v>
-      </c>
-      <c r="L19" s="6" t="s">
+      <c r="K19" s="7">
+        <v>2</v>
+      </c>
+      <c r="L19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="6">
-        <v>1</v>
-      </c>
-      <c r="N19" s="6">
-        <v>2</v>
-      </c>
-      <c r="O19" s="3" t="s">
+      <c r="M19" s="7">
+        <v>1</v>
+      </c>
+      <c r="N19" s="7">
+        <v>2</v>
+      </c>
+      <c r="O19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P19" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="6">
+      <c r="P19" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1720,10 +1753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:AB20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,33 +1765,97 @@
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="7" style="2" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10">
+        <v>1</v>
+      </c>
+      <c r="G1" s="10">
+        <v>2</v>
+      </c>
+      <c r="H1" s="10">
+        <v>3</v>
+      </c>
+      <c r="I1" s="10">
+        <v>4</v>
+      </c>
+      <c r="J1" s="10">
+        <v>5</v>
+      </c>
+      <c r="K1" s="10">
+        <v>6</v>
+      </c>
+      <c r="L1" s="10">
+        <v>7</v>
+      </c>
+      <c r="M1" s="10">
+        <v>8</v>
+      </c>
+      <c r="N1" s="10">
+        <v>9</v>
+      </c>
+      <c r="O1" s="10">
+        <v>10</v>
+      </c>
+      <c r="P1" s="10">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="10">
+        <v>12</v>
+      </c>
+      <c r="R1" s="10">
+        <v>13</v>
+      </c>
+      <c r="S1" s="10">
+        <v>14</v>
+      </c>
+      <c r="T1" s="10">
+        <v>15</v>
+      </c>
+      <c r="U1" s="10">
+        <v>16</v>
+      </c>
+      <c r="V1" s="10">
+        <v>17</v>
+      </c>
+      <c r="W1" s="10">
+        <v>18</v>
+      </c>
+      <c r="X1" s="10">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="10">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="AB1" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1774,11 +1871,114 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z2" s="2" t="str">
+        <f>F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G2 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H2 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I2 &amp; CHAR(10)
+&amp; J$1 &amp; ": " &amp; J2 &amp; CHAR(10)
+&amp; K$1 &amp; ": " &amp; K2 &amp; CHAR(10)
+&amp; L$1 &amp; ": " &amp; L2 &amp; CHAR(10)
+&amp; M$1 &amp; ": " &amp; M2 &amp; CHAR(10)
+&amp; N$1 &amp; ": " &amp; N2 &amp; CHAR(10)
+&amp; O$1 &amp; ": " &amp; O2 &amp; CHAR(10)
+&amp; P$1 &amp; ": " &amp; P2 &amp; CHAR(10)
+&amp; Q$1 &amp; ": " &amp; Q2 &amp; CHAR(10)
+&amp; R$1 &amp; ": " &amp; R2 &amp; CHAR(10)
+&amp; S$1 &amp; ": " &amp; S2 &amp; CHAR(10)
+&amp; T$1 &amp; ": " &amp; T2 &amp; CHAR(10)
+&amp; U$1 &amp; ": " &amp; U2 &amp; CHAR(10)
+&amp; V$1 &amp; ": " &amp; V2 &amp; CHAR(10)
+&amp; W$1 &amp; ": " &amp; W2 &amp; CHAR(10)
+&amp; X$1 &amp; ": " &amp; X2 &amp; CHAR(10)
+&amp; Y$1 &amp; ": " &amp; Y2</f>
+        <v>1: CRASH! Success, +3 noise
+2: CRASH! Success, +4 noise
+3: CRASH! Success, +5 noise
+4: CRASH! Success, +5 noise
+5: CRASH! Success, +5 noise
+6: SMASH! Success, disturb room
+7: SMASH! Success, disturb room
+8: SMASH! Success, disturb room
+9: SMASH! Success, disturb room
+10: SMASH! Success, disturb room
+11: BONK! Fail.
+12: BONK! Fail. +2 EXP
+13: BONK! Fail.
+14: CRASH! Success, +5 noise
+15: UNLOCKED! Success!
+16: NOPE! Fail.
+17: NOPE! Fail.
+18: NOPE! Fail
+19: NOPE! Fail.
+20: NOPE! Fail.</v>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1794,11 +1994,53 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="Z3" s="2" t="str">
+        <f t="shared" ref="Z3:Z21" si="0">F$1 &amp; ": " &amp; F3 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G3 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H3 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I3 &amp; CHAR(10)
+&amp; J$1 &amp; ": " &amp; J3 &amp; CHAR(10)
+&amp; K$1 &amp; ": " &amp; K3 &amp; CHAR(10)
+&amp; L$1 &amp; ": " &amp; L3 &amp; CHAR(10)
+&amp; M$1 &amp; ": " &amp; M3 &amp; CHAR(10)
+&amp; N$1 &amp; ": " &amp; N3 &amp; CHAR(10)
+&amp; O$1 &amp; ": " &amp; O3 &amp; CHAR(10)
+&amp; P$1 &amp; ": " &amp; P3 &amp; CHAR(10)
+&amp; Q$1 &amp; ": " &amp; Q3 &amp; CHAR(10)
+&amp; R$1 &amp; ": " &amp; R3 &amp; CHAR(10)
+&amp; S$1 &amp; ": " &amp; S3 &amp; CHAR(10)
+&amp; T$1 &amp; ": " &amp; T3 &amp; CHAR(10)
+&amp; U$1 &amp; ": " &amp; U3 &amp; CHAR(10)
+&amp; V$1 &amp; ": " &amp; V3 &amp; CHAR(10)
+&amp; W$1 &amp; ": " &amp; W3 &amp; CHAR(10)
+&amp; X$1 &amp; ": " &amp; X3 &amp; CHAR(10)
+&amp; Y$1 &amp; ": " &amp; Y3</f>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1814,11 +2056,34 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="Z4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1834,11 +2099,34 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
+      <c r="Z5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1854,11 +2142,34 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="Z6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1874,11 +2185,34 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="G7" t="s">
+      <c r="Z7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1894,11 +2228,34 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" t="s">
+      <c r="Z8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1914,11 +2271,34 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="Z9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1934,11 +2314,34 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
+      <c r="Z10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -1954,11 +2357,34 @@
       <c r="E11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
+      <c r="Z11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1974,11 +2400,34 @@
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="G12" t="s">
+      <c r="Z12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1994,11 +2443,34 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="G13" t="s">
+      <c r="Z13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -2014,11 +2486,34 @@
       <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
+      <c r="Z14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2034,11 +2529,34 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
+      <c r="Z15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2054,11 +2572,34 @@
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="G16" t="s">
+      <c r="Z16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -2074,11 +2615,34 @@
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="G17" t="s">
+      <c r="Z17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2094,11 +2658,34 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="G18" t="s">
+      <c r="Z18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -2114,11 +2701,34 @@
       <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="G19" t="s">
+      <c r="Z19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -2134,7 +2744,30 @@
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" t="s">
+      <c r="Z20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+13: 
+14: 
+15: 
+16: 
+17: 
+18: 
+19: 
+20: </v>
+      </c>
+      <c r="AB20" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start using some unicode characters for iconography
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -248,9 +248,6 @@
     <t>allows you to move your plan tiles sometimes, or do extra recon</t>
   </si>
   <si>
-    <t>Rip Wires</t>
-  </si>
-  <si>
     <t>free, but hardly successful</t>
   </si>
   <si>
@@ -305,30 +302,15 @@
     <t>SMASH! Success, disturb room</t>
   </si>
   <si>
-    <t>UNLOCKED! Success!</t>
-  </si>
-  <si>
     <t>BONK! Fail.</t>
   </si>
   <si>
     <t>BONK! Fail. +2 EXP</t>
   </si>
   <si>
-    <t>CRASH! Success, +3 noise</t>
-  </si>
-  <si>
     <t>CRASH! Success, +4 noise</t>
   </si>
   <si>
-    <t>NOPE! Fail.</t>
-  </si>
-  <si>
-    <t>NOPE! Fail</t>
-  </si>
-  <si>
-    <t>SUCCESS! Disturbed room</t>
-  </si>
-  <si>
     <t>GOT IT! Success, +1 EXP</t>
   </si>
   <si>
@@ -350,9 +332,6 @@
     <t>LET'S GO! Success, disturbed room</t>
   </si>
   <si>
-    <t>LET'S GO! Success! disturbed room</t>
-  </si>
-  <si>
     <t>CLEAN UP! Success +1 EXP</t>
   </si>
   <si>
@@ -365,9 +344,6 @@
     <t>NOPE! Fail, +3 noise</t>
   </si>
   <si>
-    <t>TRIPWIRE! Fail, +2 alerts</t>
-  </si>
-  <si>
     <t>If successful and the tile is marked, move into the tile.</t>
   </si>
   <si>
@@ -389,9 +365,6 @@
     <t>DROP! Subdue, +3 noise</t>
   </si>
   <si>
-    <t>FAIL! +2 EXP</t>
-  </si>
-  <si>
     <t>HESITATE. +3 EXP</t>
   </si>
   <si>
@@ -401,40 +374,49 @@
     <t>PUNCH. Success!</t>
   </si>
   <si>
-    <t>Zzzt. ✔ Disable all cameras</t>
-  </si>
-  <si>
-    <t>CLICK. ✔ Open any lock</t>
-  </si>
-  <si>
     <t>NOTHING</t>
   </si>
   <si>
-    <t>May be used on any open tile.</t>
-  </si>
-  <si>
-    <t>PAGE. ✔Remove 1 Guard.</t>
-  </si>
-  <si>
-    <t>BEEP! +3 noise</t>
-  </si>
-  <si>
-    <t>OOPS! Disturbed room</t>
-  </si>
-  <si>
-    <t>WALK. Move 1 space</t>
-  </si>
-  <si>
-    <t>SPRINT! Move 2 spaces, +2 noise</t>
-  </si>
-  <si>
-    <t>SHUFFLE. Move 1 space, +1 noise</t>
-  </si>
-  <si>
-    <t>SPRINT, +2 noise</t>
-  </si>
-  <si>
-    <t>TRIP! Move 1 space, disturb room.</t>
+    <t>Yank Wires</t>
+  </si>
+  <si>
+    <t>MULE KICK! Success, +3 noise</t>
+  </si>
+  <si>
+    <t>Zzzt. ✔</t>
+  </si>
+  <si>
+    <t>If ✔ disable adjacent cameras.</t>
+  </si>
+  <si>
+    <t>BEEP! +3 🔊</t>
+  </si>
+  <si>
+    <t>CLICK. 🔓 Open adjacent lock.</t>
+  </si>
+  <si>
+    <t>If ✔, move 1 space</t>
+  </si>
+  <si>
+    <t>WALK. ➜</t>
+  </si>
+  <si>
+    <t>SPRINT! ➜➜ 🔊🔊</t>
+  </si>
+  <si>
+    <t>CRACK! ❉</t>
+  </si>
+  <si>
+    <t>Splice In</t>
+  </si>
+  <si>
+    <t>SHUFFLE! ➜🔊</t>
+  </si>
+  <si>
+    <t>FLICKER! ⚠</t>
+  </si>
+  <si>
+    <t>PANIC! ➜➜🔊🔊⚠</t>
   </si>
 </sst>
 </file>
@@ -811,7 +793,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1006,7 +988,7 @@
         <v>2</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1621,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" s="7">
         <v>4</v>
@@ -1674,7 +1656,7 @@
         <v>2</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J16" s="7">
         <v>4</v>
@@ -1727,7 +1709,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J17" s="7">
         <v>4</v>
@@ -1780,7 +1762,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J18" s="7">
         <v>4</v>
@@ -1833,7 +1815,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J19" s="7">
         <v>4</v>
@@ -1867,10 +1849,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,11 +1861,11 @@
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7" style="1" customWidth="1"/>
-    <col min="6" max="26" width="7" style="2" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" style="2" customWidth="1"/>
+    <col min="6" max="18" width="7" style="2" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1935,41 +1917,17 @@
       <c r="Q1" s="10">
         <v>12</v>
       </c>
-      <c r="R1" s="10">
-        <v>13</v>
-      </c>
-      <c r="S1" s="10">
-        <v>14</v>
-      </c>
-      <c r="T1" s="10">
-        <v>15</v>
-      </c>
-      <c r="U1" s="10">
-        <v>16</v>
-      </c>
-      <c r="V1" s="10">
-        <v>17</v>
-      </c>
-      <c r="W1" s="10">
-        <v>18</v>
-      </c>
-      <c r="X1" s="10">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="10">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA1" s="11" t="s">
+      <c r="R1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1986,66 +1944,42 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="T2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z2" s="2" t="str">
+      <c r="R2" s="2" t="str">
         <f>F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G2 &amp; CHAR(10)
 &amp; H$1 &amp; ": " &amp; H2 &amp; CHAR(10)
@@ -2057,16 +1991,8 @@
 &amp; N$1 &amp; ": " &amp; N2 &amp; CHAR(10)
 &amp; O$1 &amp; ": " &amp; O2 &amp; CHAR(10)
 &amp; P$1 &amp; ": " &amp; P2 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q2 &amp; CHAR(10)
-&amp; R$1 &amp; ": " &amp; R2 &amp; CHAR(10)
-&amp; S$1 &amp; ": " &amp; S2 &amp; CHAR(10)
-&amp; T$1 &amp; ": " &amp; T2 &amp; CHAR(10)
-&amp; U$1 &amp; ": " &amp; U2 &amp; CHAR(10)
-&amp; V$1 &amp; ": " &amp; V2 &amp; CHAR(10)
-&amp; W$1 &amp; ": " &amp; W2 &amp; CHAR(10)
-&amp; X$1 &amp; ": " &amp; X2 &amp; CHAR(10)
-&amp; Y$1 &amp; ": " &amp; Y2</f>
-        <v>1: CRASH! Success, +3 noise
+&amp; Q$1 &amp; ": " &amp; Q2 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: MULE KICK! Success, +3 noise
 2: CRASH! Success, +4 noise
 3: CRASH! Success, +5 noise
 4: CRASH! Success, +5 noise
@@ -2078,23 +2004,16 @@
 10: SMASH! Success, disturb room
 11: BONK! Fail.
 12: BONK! Fail. +2 EXP
-13: BONK! Fail.
-14: CRASH! Success, +5 noise
-15: UNLOCKED! Success!
-16: NOPE! Fail.
-17: NOPE! Fail.
-18: NOPE! Fail
-19: NOPE! Fail.
-20: NOPE! Fail.</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB2" t="s">
+</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2111,67 +2030,43 @@
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="P3" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z3" s="2" t="str">
-        <f>F$1 &amp; ": " &amp; F3 &amp; CHAR(10)
+        <v>104</v>
+      </c>
+      <c r="R3" s="2" t="str">
+        <f t="shared" ref="R3:R21" si="0">F$1 &amp; ": " &amp; F3 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G3 &amp; CHAR(10)
 &amp; H$1 &amp; ": " &amp; H3 &amp; CHAR(10)
 &amp; I$1 &amp; ": " &amp; I3 &amp; CHAR(10)
@@ -2182,16 +2077,8 @@
 &amp; N$1 &amp; ": " &amp; N3 &amp; CHAR(10)
 &amp; O$1 &amp; ": " &amp; O3 &amp; CHAR(10)
 &amp; P$1 &amp; ": " &amp; P3 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q3 &amp; CHAR(10)
-&amp; R$1 &amp; ": " &amp; R3 &amp; CHAR(10)
-&amp; S$1 &amp; ": " &amp; S3 &amp; CHAR(10)
-&amp; T$1 &amp; ": " &amp; T3 &amp; CHAR(10)
-&amp; U$1 &amp; ": " &amp; U3 &amp; CHAR(10)
-&amp; V$1 &amp; ": " &amp; V3 &amp; CHAR(10)
-&amp; W$1 &amp; ": " &amp; W3 &amp; CHAR(10)
-&amp; X$1 &amp; ": " &amp; X3 &amp; CHAR(10)
-&amp; Y$1 &amp; ": " &amp; Y3</f>
-        <v>1: CRAP! +2 noise
+&amp; Q$1 &amp; ": " &amp; Q3 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: CRAP! +2 noise
 2: CRAP! +3 noise
 3: LET'S GO! Success, disturbed room
 4: CRAP! +1 noise
@@ -2203,23 +2090,16 @@
 10: NOPE! Fail, +3 noise
 11: LET'S GO! Success, disturbed room
 12: LET'S GO! Success, disturbed room
-13: LET'S GO! Success! disturbed room
-14: TRIPWIRE! Fail, +2 alerts
-15: LET'S GO! Success, disturbed room
-16: CRAP! +2 noise
-17: CRAP! +3 noise
-18: SUCCESS! Disturbed room
-19: SUCCESS! Disturbed room
-20: CRAP! +3 noise</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB3" t="s">
+</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -2236,87 +2116,44 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z4" s="2" t="str">
-        <f t="shared" ref="Z4:Z20" si="0">F$1 &amp; ": " &amp; F4 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G4 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H4 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I4 &amp; CHAR(10)
-&amp; J$1 &amp; ": " &amp; J4 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K4 &amp; CHAR(10)
-&amp; L$1 &amp; ": " &amp; L4 &amp; CHAR(10)
-&amp; M$1 &amp; ": " &amp; M4 &amp; CHAR(10)
-&amp; N$1 &amp; ": " &amp; N4 &amp; CHAR(10)
-&amp; O$1 &amp; ": " &amp; O4 &amp; CHAR(10)
-&amp; P$1 &amp; ": " &amp; P4 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q4 &amp; CHAR(10)
-&amp; R$1 &amp; ": " &amp; R4 &amp; CHAR(10)
-&amp; S$1 &amp; ": " &amp; S4 &amp; CHAR(10)
-&amp; T$1 &amp; ": " &amp; T4 &amp; CHAR(10)
-&amp; U$1 &amp; ": " &amp; U4 &amp; CHAR(10)
-&amp; V$1 &amp; ": " &amp; V4 &amp; CHAR(10)
-&amp; W$1 &amp; ": " &amp; W4 &amp; CHAR(10)
-&amp; X$1 &amp; ": " &amp; X4 &amp; CHAR(10)
-&amp; Y$1 &amp; ": " &amp; Y4</f>
-        <v>1: GOT IT! Success, +1 EXP
+        <v>103</v>
+      </c>
+      <c r="R4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: GOT IT! Success, +1 EXP
 2: ALMOST! +1 EXP
 3: ALMOST! +1 EXP
 4: ALMOST! +1 EXP
@@ -2328,23 +2165,16 @@
 10: DROP! Disturbed room
 11: DROP! Disturbed room
 12: DROP! Disturbed room
-13: GOT IT! Success
-14: ALMOST! +1 EXP
-15: ALMOST! +1 EXP
-16: ALMOST! +1 EXP
-17: GOT IT! Success, +1 EXP
-18: NOPE! Fail
-19: GOT IT! Success
-20: NOPE! Fail.</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB4" t="s">
+</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2360,7 +2190,7 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="Z5" s="2" t="str">
+      <c r="R5" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2374,20 +2204,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB5" t="s">
+</v>
+      </c>
+      <c r="T5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -2403,7 +2226,7 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="Z6" s="2" t="str">
+      <c r="R6" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2417,20 +2240,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB6" t="s">
+</v>
+      </c>
+      <c r="T6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -2446,7 +2262,7 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="Z7" s="2" t="str">
+      <c r="R7" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2460,20 +2276,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+</v>
+      </c>
+      <c r="T7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2490,68 +2299,44 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z8" s="2" t="str">
+        <v>113</v>
+      </c>
+      <c r="R8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1: PUNCH. Success!
+        <v xml:space="preserve">1: PUNCH. Success!
 2: FAIL! Busted.
 3: PUNCH. Subdue 1 guard
 4: FAIL! Busted.
@@ -2562,24 +2347,17 @@
 9: HESITATE. +3 EXP
 10: PUNCH. Subdue 1 guard
 11: PUNCH. Subdue 1 guard, +2 EXP
-12: HESITATE. +2 EXP
-13: HESITATE. +3 EXP
-14: TRIP. Subdue 1 guard
-15: TRIP. Subdue 1 guard
-16: TRIP. Subdue 1 guard
-17: TRIP. Subdue 1 guard
-18: FAIL! +2 EXP
-19: TRIP. Subdue 1 guard
-20: FAIL! +2 EXP</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+12: TRIP. Subdue 1 guard
+</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="T8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -2595,7 +2373,7 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="Z9" s="2" t="str">
+      <c r="R9" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2609,20 +2387,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB9" t="s">
+</v>
+      </c>
+      <c r="T9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2638,7 +2409,7 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="Z10" s="2" t="str">
+      <c r="R10" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2652,20 +2423,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+</v>
+      </c>
+      <c r="T10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -2681,7 +2445,7 @@
       <c r="E11" s="1">
         <v>1</v>
       </c>
-      <c r="Z11" s="2" t="str">
+      <c r="R11" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2695,20 +2459,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+</v>
+      </c>
+      <c r="T11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -2724,7 +2481,7 @@
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="Z12" s="2" t="str">
+      <c r="R12" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2738,20 +2495,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+</v>
+      </c>
+      <c r="T12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2768,93 +2518,65 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="R13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: WALK. ➜
+2: SPRINT! ➜➜ 🔊🔊
+3: WALK. ➜
+4: SHUFFLE! ➜🔊
+5: WALK. ➜
+6: HESITATE. +2 EXP
+7: WALK. ➜
+8: HESITATE. +2 EXP
+9: WALK. ➜
+10: HESITATE. +2 EXP
+11: WALK. ➜
+12: SPRINT! ➜➜ 🔊🔊
+</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="W13" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>1: WALK. Move 1 space
-2: SPRINT! Move 2 spaces, +2 noise
-3: WALK. Move 1 space
-4: SHUFFLE. Move 1 space, +1 noise
-5: WALK. Move 1 space
-6: HESITATE. +2 EXP
-7: WALK. Move 1 space
-8: HESITATE. +2 EXP
-9: WALK. Move 1 space
-10: HESITATE. +2 EXP
-11: WALK. Move 1 space
-12: SPRINT, +2 noise
-13: WALK. Move 1 space
-14: TRIP! Move 1 space, disturb room.
-15: WALK. Move 1 space
-16: SHUFFLE. Move 1 space, +1 noise
-17: WALK. Move 1 space
-18: SHUFFLE. Move 1 space, +1 noise
-19: WALK. Move 1 space
-20: HESITATE. +2 EXP</v>
-      </c>
-      <c r="AB13" t="s">
+      <c r="T13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -2870,7 +2592,7 @@
       <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="Z14" s="2" t="str">
+      <c r="R14" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2884,20 +2606,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB14" t="s">
+</v>
+      </c>
+      <c r="T14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2913,7 +2628,7 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="Z15" s="2" t="str">
+      <c r="R15" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2927,20 +2642,13 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB15" t="s">
+</v>
+      </c>
+      <c r="T15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2956,7 +2664,7 @@
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="Z16" s="2" t="str">
+      <c r="R16" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -2970,22 +2678,15 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB16" t="s">
+</v>
+      </c>
+      <c r="T16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -3000,117 +2701,67 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="R17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: Zzzt. ✔
+2: NOTHING
+3: CRACK! ❉
+4: CLICK. 🔓 Open adjacent lock.
+5: NOTHING
+6: PANIC! ➜➜🔊🔊⚠
+7: Zzzt. ✔
+8: NOTHING
+9: BEEP! +3 🔊
+10: NOTHING
+11: FLICKER! ⚠
+12: NOTHING
+</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="T17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>130</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="W17" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z17" s="2" t="str">
-        <f>F$1 &amp; ": " &amp; F17 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G17 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H17 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I17 &amp; CHAR(10)
-&amp; J$1 &amp; ": " &amp; J17 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K17 &amp; CHAR(10)
-&amp; L$1 &amp; ": " &amp; L17 &amp; CHAR(10)
-&amp; M$1 &amp; ": " &amp; M17 &amp; CHAR(10)
-&amp; N$1 &amp; ": " &amp; N17 &amp; CHAR(10)
-&amp; O$1 &amp; ": " &amp; O17 &amp; CHAR(10)
-&amp; P$1 &amp; ": " &amp; P17 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q17 &amp; CHAR(10)
-&amp; R$1 &amp; ": " &amp; R17 &amp; CHAR(10)
-&amp; S$1 &amp; ": " &amp; S17 &amp; CHAR(10)
-&amp; T$1 &amp; ": " &amp; T17 &amp; CHAR(10)
-&amp; U$1 &amp; ": " &amp; U17 &amp; CHAR(10)
-&amp; V$1 &amp; ": " &amp; V17 &amp; CHAR(10)
-&amp; W$1 &amp; ": " &amp; W17 &amp; CHAR(10)
-&amp; X$1 &amp; ": " &amp; X17 &amp; CHAR(10)
-&amp; Y$1 &amp; ": " &amp; Y17</f>
-        <v>1: Zzzt. ✔ Disable all cameras
-2: NOTHING
-3: OOPS! Disturbed room
-4: CLICK. ✔ Open any lock
-5: NOTHING
-6: NOTHING
-7: Zzzt. ✔ Disable all cameras
-8: NOTHING
-9: BEEP! +3 noise
-10: NOTHING
-11: CLICK. ✔ Open any lock
-12: NOTHING
-13: NOTHING
-14: Zzzt. ✔ Disable all cameras
-15: NOTHING
-16: BEEP! +3 noise
-17: NOTHING
-18: PAGE. ✔Remove 1 Guard.
-19: NOTHING
-20: NOTHING</v>
-      </c>
-      <c r="AA17" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>81</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
@@ -3124,7 +2775,24 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="Z18" s="2" t="str">
+    </row>
+    <row r="19" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -3138,36 +2806,29 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+</v>
+      </c>
+      <c r="T19" t="s">
         <v>82</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="2" t="str">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="R20" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -3181,36 +2842,29 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" t="s">
+</v>
+      </c>
+      <c r="T20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>5</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2</v>
-      </c>
-      <c r="Z20" s="2" t="str">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="R21" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
@@ -3224,17 +2878,10 @@
 10: 
 11: 
 12: 
-13: 
-14: 
-15: 
-16: 
-17: 
-18: 
-19: 
-20: </v>
-      </c>
-      <c r="AB20" t="s">
-        <v>80</v>
+</v>
+      </c>
+      <c r="T21" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tons of data smoothing, brainstorming
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
+    <sheet name="Icon Help" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -167,9 +168,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Brute Force</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -179,12 +177,6 @@
     <t>Rake Locks</t>
   </si>
   <si>
-    <t>free, loud, disturbs rooms</t>
-  </si>
-  <si>
-    <t>cheap, loud, disturbs rooms</t>
-  </si>
-  <si>
     <t>Pick Locks</t>
   </si>
   <si>
@@ -203,9 +195,6 @@
     <t>Ambush</t>
   </si>
   <si>
-    <t>Sneak Attack</t>
-  </si>
-  <si>
     <t>Conceal</t>
   </si>
   <si>
@@ -218,21 +207,12 @@
     <t>expensive, quiet, effective, out of reach for many crew members</t>
   </si>
   <si>
-    <t>Walk</t>
-  </si>
-  <si>
     <t>Inside Man</t>
   </si>
   <si>
     <t>Masquerade</t>
   </si>
   <si>
-    <t>successful, but loud and disturbing</t>
-  </si>
-  <si>
-    <t>Creep</t>
-  </si>
-  <si>
     <t>slow, but quiet</t>
   </si>
   <si>
@@ -275,12 +255,6 @@
     <t>free, loud and unsuccessful</t>
   </si>
   <si>
-    <t>quiet, but not as successful</t>
-  </si>
-  <si>
-    <t>quiet, somewhat successful, but does not subdue the guards</t>
-  </si>
-  <si>
     <t>great all around if you can get it</t>
   </si>
   <si>
@@ -293,118 +267,25 @@
     <t>ExtraHack</t>
   </si>
   <si>
-    <t>CRASH! Success, +5 noise</t>
-  </si>
-  <si>
     <t>Rolls</t>
   </si>
   <si>
-    <t>SMASH! Success, disturb room</t>
-  </si>
-  <si>
-    <t>BONK! Fail.</t>
-  </si>
-  <si>
-    <t>BONK! Fail. +2 EXP</t>
-  </si>
-  <si>
-    <t>CRASH! Success, +4 noise</t>
-  </si>
-  <si>
-    <t>GOT IT! Success, +1 EXP</t>
-  </si>
-  <si>
-    <t>ALMOST! +1 EXP</t>
-  </si>
-  <si>
-    <t>GOT IT! Success</t>
-  </si>
-  <si>
-    <t>CRAP! +2 noise</t>
-  </si>
-  <si>
-    <t>CRAP! +3 noise</t>
-  </si>
-  <si>
-    <t>DROP! Disturbed room</t>
-  </si>
-  <si>
-    <t>LET'S GO! Success, disturbed room</t>
-  </si>
-  <si>
-    <t>CLEAN UP! Success +1 EXP</t>
-  </si>
-  <si>
-    <t>CRAP! +1 noise</t>
-  </si>
-  <si>
-    <t>CRAP! Fail, +1 noise</t>
-  </si>
-  <si>
-    <t>NOPE! Fail, +3 noise</t>
-  </si>
-  <si>
-    <t>If successful and the tile is marked, move into the tile.</t>
-  </si>
-  <si>
     <t>FAIL! Busted.</t>
   </si>
   <si>
-    <t>PUNCH. Subdue 1 guard, +2 EXP</t>
-  </si>
-  <si>
-    <t>PUNCH. Subdue 1 guard</t>
-  </si>
-  <si>
-    <t>TRIP. Subdue 1 guard</t>
-  </si>
-  <si>
-    <t>Can only take out 1 Guard</t>
-  </si>
-  <si>
-    <t>DROP! Subdue, +3 noise</t>
-  </si>
-  <si>
-    <t>HESITATE. +3 EXP</t>
-  </si>
-  <si>
-    <t>HESITATE. +2 EXP</t>
-  </si>
-  <si>
-    <t>PUNCH. Success!</t>
-  </si>
-  <si>
     <t>NOTHING</t>
   </si>
   <si>
     <t>Yank Wires</t>
   </si>
   <si>
-    <t>MULE KICK! Success, +3 noise</t>
-  </si>
-  <si>
-    <t>Zzzt. ✔</t>
-  </si>
-  <si>
-    <t>If ✔ disable adjacent cameras.</t>
-  </si>
-  <si>
-    <t>BEEP! +3 🔊</t>
-  </si>
-  <si>
-    <t>CLICK. 🔓 Open adjacent lock.</t>
-  </si>
-  <si>
-    <t>If ✔, move 1 space</t>
-  </si>
-  <si>
     <t>WALK. ➜</t>
   </si>
   <si>
     <t>SPRINT! ➜➜ 🔊🔊</t>
   </si>
   <si>
-    <t>CRACK! ❉</t>
+    <t>BEEP! 🔊🔊🔊</t>
   </si>
   <si>
     <t>Splice In</t>
@@ -413,10 +294,211 @@
     <t>SHUFFLE! ➜🔊</t>
   </si>
   <si>
-    <t>FLICKER! ⚠</t>
-  </si>
-  <si>
     <t>PANIC! ➜➜🔊🔊⚠</t>
+  </si>
+  <si>
+    <t>Dawdle</t>
+  </si>
+  <si>
+    <t>Slog</t>
+  </si>
+  <si>
+    <t>Prowl</t>
+  </si>
+  <si>
+    <t>STUMBLE. ➜🔊</t>
+  </si>
+  <si>
+    <t>HESITATE.💡</t>
+  </si>
+  <si>
+    <t>Tromp</t>
+  </si>
+  <si>
+    <t>HESITATE.💡💡</t>
+  </si>
+  <si>
+    <t>CLICK. 🔓</t>
+  </si>
+  <si>
+    <t>Mule Kick</t>
+  </si>
+  <si>
+    <t>BAM! 🔓🔊🔊🔊</t>
+  </si>
+  <si>
+    <t>THUD. 🔊</t>
+  </si>
+  <si>
+    <t>CRASH! 🔓🔊💥</t>
+  </si>
+  <si>
+    <t>free, loud, disturbs rooms, no exp gained</t>
+  </si>
+  <si>
+    <t>OOF! 🔊</t>
+  </si>
+  <si>
+    <t>ALMOST!💡💡</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>BAM! 🔓🔊🔊 ➜</t>
+  </si>
+  <si>
+    <t>BAM! 🔓🔊🔊🔊➜</t>
+  </si>
+  <si>
+    <t>CRASH! 🔓🔊💥➜</t>
+  </si>
+  <si>
+    <t>CRACK! 🔓🔊</t>
+  </si>
+  <si>
+    <t>CLUNK. 🔓🔊💥➜</t>
+  </si>
+  <si>
+    <t>cheap, kinda loud, disturbs rooms, gains some experience, but less successful the first time</t>
+  </si>
+  <si>
+    <t>HESITATE. 💡💡💡</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>HESITATE. 💡💡</t>
+  </si>
+  <si>
+    <t>SURPRISE. 👊➜</t>
+  </si>
+  <si>
+    <t>FIGHT! 👊🔊🔊➜</t>
+  </si>
+  <si>
+    <t>TRIP. ➜💥</t>
+  </si>
+  <si>
+    <t>free, slow, but gains exp</t>
+  </si>
+  <si>
+    <t>free, kinda loud, usually moves, might sprint, not much exp</t>
+  </si>
+  <si>
+    <t>CRACK! 💥</t>
+  </si>
+  <si>
+    <t>FLICKER!🔊⚠⚠</t>
+  </si>
+  <si>
+    <t>Zzzt. 📷</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>🔓</t>
+  </si>
+  <si>
+    <t>Unlock 1 lock on or adjacent to your tile</t>
+  </si>
+  <si>
+    <t>BYPASS! 🔓🔓➜</t>
+  </si>
+  <si>
+    <t>🔊</t>
+  </si>
+  <si>
+    <t>Increase the noise level by 1</t>
+  </si>
+  <si>
+    <t>➜</t>
+  </si>
+  <si>
+    <t>📷</t>
+  </si>
+  <si>
+    <t>⚠</t>
+  </si>
+  <si>
+    <t>Increase alert level by 1</t>
+  </si>
+  <si>
+    <t>👊</t>
+  </si>
+  <si>
+    <t>💡</t>
+  </si>
+  <si>
+    <t>Add 1 idea to the current skill</t>
+  </si>
+  <si>
+    <t>Disable all cameras on or adjacent to your tile</t>
+  </si>
+  <si>
+    <t>Move your pawn to an adjacent tile (that you planned)</t>
+  </si>
+  <si>
+    <t>💥</t>
+  </si>
+  <si>
+    <t>Disturb the room you end the turn in.</t>
+  </si>
+  <si>
+    <t>Requires: Splice In</t>
+  </si>
+  <si>
+    <t>Requires: Sniff Packets</t>
+  </si>
+  <si>
+    <t>Roam</t>
+  </si>
+  <si>
+    <t>Requires Dawdle</t>
+  </si>
+  <si>
+    <t>Requires Tromp</t>
+  </si>
+  <si>
+    <t>Requires Slog</t>
+  </si>
+  <si>
+    <t>Requires AND Conceal</t>
+  </si>
+  <si>
+    <t>Assault</t>
+  </si>
+  <si>
+    <t>LISTEN 👂</t>
+  </si>
+  <si>
+    <t>👂</t>
+  </si>
+  <si>
+    <t>Uncover 1 unknown security token</t>
+  </si>
+  <si>
+    <t>BUSTED!</t>
+  </si>
+  <si>
+    <t>ACHOO! 🔊💡</t>
+  </si>
+  <si>
+    <t>Subdue 1 guard on or adjacent to your tile. Cannot be used on 2-guard tiles</t>
+  </si>
+  <si>
+    <t>FIGHT! 👊🔊🔊💥➜</t>
+  </si>
+  <si>
+    <t>HESITATE. 💡</t>
+  </si>
+  <si>
+    <t>BRIBE! 👊 -$1k</t>
+  </si>
+  <si>
+    <t>YOINK! +$1k</t>
   </si>
 </sst>
 </file>
@@ -932,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -988,7 +1070,7 @@
         <v>2</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1603,7 +1685,7 @@
         <v>2</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J15" s="7">
         <v>4</v>
@@ -1656,7 +1738,7 @@
         <v>2</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J16" s="7">
         <v>4</v>
@@ -1709,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J17" s="7">
         <v>4</v>
@@ -1762,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J18" s="7">
         <v>4</v>
@@ -1815,7 +1897,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J19" s="7">
         <v>4</v>
@@ -1849,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,8 +1943,18 @@
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7" style="1" customWidth="1"/>
-    <col min="6" max="18" width="7" style="2" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" style="2" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1876,7 +1968,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
@@ -1918,24 +2010,24 @@
         <v>12</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="S1" s="11" t="s">
         <v>49</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -1944,43 +2036,43 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="R2" s="2" t="str">
-        <f>F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
+        <f t="shared" ref="R2:R8" si="0">F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G2 &amp; CHAR(10)
 &amp; H$1 &amp; ": " &amp; H2 &amp; CHAR(10)
 &amp; I$1 &amp; ": " &amp; I2 &amp; CHAR(10)
@@ -1992,30 +2084,30 @@
 &amp; O$1 &amp; ": " &amp; O2 &amp; CHAR(10)
 &amp; P$1 &amp; ": " &amp; P2 &amp; CHAR(10)
 &amp; Q$1 &amp; ": " &amp; Q2 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: MULE KICK! Success, +3 noise
-2: CRASH! Success, +4 noise
-3: CRASH! Success, +5 noise
-4: CRASH! Success, +5 noise
-5: CRASH! Success, +5 noise
-6: SMASH! Success, disturb room
-7: SMASH! Success, disturb room
-8: SMASH! Success, disturb room
-9: SMASH! Success, disturb room
-10: SMASH! Success, disturb room
-11: BONK! Fail.
-12: BONK! Fail. +2 EXP
+        <v xml:space="preserve">1: BAM! 🔓🔊🔊 ➜
+2: BAM! 🔓🔊🔊🔊➜
+3: THUD. 🔊
+4: BAM! 🔓🔊🔊🔊➜
+5: CRASH! 🔓🔊💥➜
+6: THUD. 🔊
+7: CRASH! 🔓🔊💥➜
+8: BAM! 🔓🔊🔊🔊➜
+9: CRASH! 🔓🔊💥
+10: CRASH! 🔓🔊💥
+11: CRACK! 🔓🔊
+12: BAM! 🔓🔊🔊🔊
 </v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T2" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
@@ -2024,84 +2116,73 @@
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>106</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="M3" s="2" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="R3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: OOF! 🔊
+2: ALMOST!💡💡
+3: CLUNK. 🔓🔊💥➜
+4: OOF! 🔊
+5: ALMOST!💡💡
+6: CLUNK. 🔓🔊💥➜
+7: OOF! 🔊
+8: CLUNK. 🔓🔊💥➜
+9: CLUNK. 🔓🔊💥➜
+10: CLUNK. 🔓🔊💥➜
+11: ALMOST!💡💡
+12: ALMOST!💡💡
+</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="R3" s="2" t="str">
-        <f t="shared" ref="R3:R21" si="0">F$1 &amp; ": " &amp; F3 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G3 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H3 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I3 &amp; CHAR(10)
-&amp; J$1 &amp; ": " &amp; J3 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K3 &amp; CHAR(10)
-&amp; L$1 &amp; ": " &amp; L3 &amp; CHAR(10)
-&amp; M$1 &amp; ": " &amp; M3 &amp; CHAR(10)
-&amp; N$1 &amp; ": " &amp; N3 &amp; CHAR(10)
-&amp; O$1 &amp; ": " &amp; O3 &amp; CHAR(10)
-&amp; P$1 &amp; ": " &amp; P3 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q3 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: CRAP! +2 noise
-2: CRAP! +3 noise
-3: LET'S GO! Success, disturbed room
-4: CRAP! +1 noise
-5: CRAP! +1 noise
-6: LET'S GO! Success, disturbed room
-7: CRAP! +2 noise
-8: CLEAN UP! Success +1 EXP
-9: CRAP! Fail, +1 noise
-10: NOPE! Fail, +3 noise
-11: LET'S GO! Success, disturbed room
-12: LET'S GO! Success, disturbed room
-</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="T3" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -2116,67 +2197,34 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="R4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">1: GOT IT! Success, +1 EXP
-2: ALMOST! +1 EXP
-3: ALMOST! +1 EXP
-4: ALMOST! +1 EXP
-5: GOT IT! Success
-6: CRAP! +2 noise
-7: CRAP! +3 noise
-8: CRAP! +2 noise
-9: GOT IT! Success
-10: DROP! Disturbed room
-11: DROP! Disturbed room
-12: DROP! Disturbed room
+        <v xml:space="preserve">1: BYPASS! 🔓🔓➜
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
 </v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -2206,16 +2254,19 @@
 12: 
 </v>
       </c>
+      <c r="S5" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="T5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2226,10 +2277,16 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="R6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">1: 
-2: 
+        <v xml:space="preserve">1: BRIBE! 👊 -$1k
+2: YOINK! +$1k
 3: 
 4: 
 5: 
@@ -2242,16 +2299,19 @@
 12: 
 </v>
       </c>
+      <c r="S6" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="T6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2278,22 +2338,25 @@
 12: 
 </v>
       </c>
+      <c r="S7" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="T7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -2302,64 +2365,64 @@
         <v>118</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="L8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="N8" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="R8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">1: PUNCH. Success!
+        <v xml:space="preserve">1: SURPRISE. 👊➜
 2: FAIL! Busted.
-3: PUNCH. Subdue 1 guard
+3: FIGHT! 👊🔊🔊➜
 4: FAIL! Busted.
-5: DROP! Subdue, +3 noise
-6: HESITATE. +3 EXP
-7: HESITATE. +2 EXP
-8: HESITATE. +3 EXP
-9: HESITATE. +3 EXP
-10: PUNCH. Subdue 1 guard
-11: PUNCH. Subdue 1 guard, +2 EXP
-12: TRIP. Subdue 1 guard
+5: FIGHT! 👊🔊🔊➜
+6: HESITATE. 💡💡💡
+7: FIGHT! 👊🔊🔊➜
+8: HESITATE. 💡💡
+9: FIGHT! 👊🔊🔊➜
+10: FIGHT! 👊🔊🔊➜
+11: FIGHT! 👊🔊🔊➜
+12: FIGHT! 👊🔊🔊➜
 </v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="T8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -2371,10 +2434,158 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="R9" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="R9:R11" si="1">F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G9 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H9 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I9 &amp; CHAR(10)
+&amp; J$1 &amp; ": " &amp; J9 &amp; CHAR(10)
+&amp; K$1 &amp; ": " &amp; K9 &amp; CHAR(10)
+&amp; L$1 &amp; ": " &amp; L9 &amp; CHAR(10)
+&amp; M$1 &amp; ": " &amp; M9 &amp; CHAR(10)
+&amp; N$1 &amp; ": " &amp; N9 &amp; CHAR(10)
+&amp; O$1 &amp; ": " &amp; O9 &amp; CHAR(10)
+&amp; P$1 &amp; ": " &amp; P9 &amp; CHAR(10)
+&amp; Q$1 &amp; ": " &amp; Q9 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: FIGHT! 👊🔊🔊💥➜
+2: FIGHT! 👊🔊🔊💥➜
+3: HESITATE. 💡
+4: FIGHT! 👊🔊🔊💥➜
+5: FIGHT! 👊🔊🔊💥➜
+6: FIGHT! 👊🔊🔊💥➜
+7: HESITATE. 💡
+8: FIGHT! 👊🔊🔊💥➜
+9: FIGHT! 👊🔊🔊💥➜
+10: HESITATE. 💡
+11: FIGHT! 👊🔊🔊💥➜
+12: FIGHT! 👊🔊🔊💥➜
+</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="R10" s="2" t="e">
+        <f>F$1 &amp; ": " &amp; I10 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G10 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H10 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp;#REF! &amp; CHAR(10)
+&amp; J$1 &amp; ": " &amp; J10 &amp; CHAR(10)
+&amp; K$1 &amp; ": " &amp; K10 &amp; CHAR(10)
+&amp; L$1 &amp; ": " &amp; L10 &amp; CHAR(10)
+&amp; M$1 &amp; ": " &amp; M10 &amp; CHAR(10)
+&amp; N$1 &amp; ": " &amp; N10 &amp; CHAR(10)
+&amp; O$1 &amp; ": " &amp; O10 &amp; CHAR(10)
+&amp; P$1 &amp; ": " &amp; P10 &amp; CHAR(10)
+&amp; Q$1 &amp; ": " &amp; Q10 &amp; CHAR(10)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2389,28 +2600,39 @@
 12: 
 </v>
       </c>
-      <c r="T9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="S11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="R10" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2" t="str">
+        <f t="shared" ref="R12:R25" si="2">F$1 &amp; ": " &amp; F12 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G12 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H12 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I12 &amp; CHAR(10)
+&amp; J$1 &amp; ": " &amp; J12 &amp; CHAR(10)
+&amp; K$1 &amp; ": " &amp; K12 &amp; CHAR(10)
+&amp; L$1 &amp; ": " &amp; L12 &amp; CHAR(10)
+&amp; M$1 &amp; ": " &amp; M12 &amp; CHAR(10)
+&amp; N$1 &amp; ": " &amp; N12 &amp; CHAR(10)
+&amp; O$1 &amp; ": " &amp; O12 &amp; CHAR(10)
+&amp; P$1 &amp; ": " &amp; P12 &amp; CHAR(10)
+&amp; Q$1 &amp; ": " &amp; Q12 &amp; CHAR(10)</f>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2425,28 +2647,28 @@
 12: 
 </v>
       </c>
-      <c r="T10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="S12" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="R11" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="R13" s="2" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2461,28 +2683,253 @@
 12: 
 </v>
       </c>
-      <c r="T11" t="s">
+      <c r="S13" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="T13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2</v>
-      </c>
-      <c r="R12" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="G14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: WALK. ➜
+2: SPRINT! ➜➜ 🔊🔊
+3: WALK. ➜
+4: STUMBLE. ➜🔊
+5: TRIP. ➜💥
+6: HESITATE.💡💡
+7: WALK. ➜
+8: STUMBLE. ➜🔊
+9: WALK. ➜
+10: HESITATE.💡💡
+11: WALK. ➜
+12: SPRINT! ➜➜ 🔊🔊
+</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="R15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: HESITATE.💡
+2: WALK. ➜
+3: HESITATE.💡
+4: WALK. ➜
+5: HESITATE.💡
+6: STUMBLE. ➜🔊
+7: HESITATE.💡
+8: HESITATE.💡
+9: STUMBLE. ➜🔊
+10: STUMBLE. ➜🔊
+11: HESITATE.💡
+12: STUMBLE. ➜🔊
+</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: SHUFFLE! ➜🔊
+2: SHUFFLE! ➜🔊
+3: SPRINT! ➜➜ 🔊🔊
+4: SHUFFLE! ➜🔊
+5: SHUFFLE! ➜🔊
+6: HESITATE.💡💡
+7: SHUFFLE! ➜🔊
+8: SHUFFLE! ➜🔊
+9: HESITATE.💡
+10: SHUFFLE! ➜🔊
+11: SHUFFLE! ➜🔊
+12: SPRINT! ➜➜ 🔊🔊
+</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2497,103 +2944,28 @@
 12: 
 </v>
       </c>
-      <c r="T12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="S17" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="R13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1: WALK. ➜
-2: SPRINT! ➜➜ 🔊🔊
-3: WALK. ➜
-4: SHUFFLE! ➜🔊
-5: WALK. ➜
-6: HESITATE. +2 EXP
-7: WALK. ➜
-8: HESITATE. +2 EXP
-9: WALK. ➜
-10: HESITATE. +2 EXP
-11: WALK. ➜
-12: SPRINT! ➜➜ 🔊🔊
-</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="T13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="R14" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2608,28 +2980,31 @@
 12: 
 </v>
       </c>
-      <c r="T14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="S18" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="T18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="R15" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" s="2" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2644,28 +3019,31 @@
 12: 
 </v>
       </c>
-      <c r="T15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="S19" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="T19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
         <v>3</v>
       </c>
-      <c r="E16" s="1">
-        <v>2</v>
-      </c>
-      <c r="R16" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+      <c r="R20" s="2" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2680,120 +3058,145 @@
 12: 
 </v>
       </c>
-      <c r="T16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="S20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C17">
+      <c r="C21">
         <v>4</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="N17" s="2" t="s">
+      <c r="G21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P21" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1: Zzzt. ✔
+      <c r="Q21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: Zzzt. 📷
 2: NOTHING
-3: CRACK! ❉
-4: CLICK. 🔓 Open adjacent lock.
+3: CRACK! 💥
+4: CLICK. 🔓
 5: NOTHING
 6: PANIC! ➜➜🔊🔊⚠
-7: Zzzt. ✔
+7: Zzzt. 📷
 8: NOTHING
-9: BEEP! +3 🔊
+9: BEEP! 🔊🔊🔊
 10: NOTHING
-11: FLICKER! ⚠
+11: FLICKER!🔊⚠⚠
 12: NOTHING
 </v>
       </c>
-      <c r="S17" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="T17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="S21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="R22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: YOINK! +$1k
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="R19" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="2" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2808,28 +3211,31 @@
 12: 
 </v>
       </c>
-      <c r="T19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="S23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="R20" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="R24" s="2" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2844,28 +3250,31 @@
 12: 
 </v>
       </c>
-      <c r="T20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="S24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="T24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
         <v>22</v>
       </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1">
-        <v>5</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2</v>
-      </c>
-      <c r="R21" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2</v>
+      </c>
+      <c r="R25" s="2" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2880,8 +3289,113 @@
 12: 
 </v>
       </c>
-      <c r="T21" t="s">
-        <v>79</v>
+      <c r="S25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="T25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
characters: new abilities, stats on cards
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="165">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Mastermind</t>
   </si>
   <si>
-    <t>Evil Genius</t>
-  </si>
-  <si>
     <t>Street Urchin</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Picker</t>
   </si>
   <si>
-    <t>Planner</t>
-  </si>
-  <si>
     <t>Mover</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>Unlock</t>
   </si>
   <si>
-    <t>Abilities</t>
-  </si>
-  <si>
     <t>Snark</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t>Grifter</t>
   </si>
   <si>
-    <t>ADRENALINE: May purchase up to 3 extra Attack EXP for $1k each in planning phase</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -258,12 +246,6 @@
     <t>great all around if you can get it</t>
   </si>
   <si>
-    <t>Rake Locks or Pick Locks may be purchased for $1k less than cost.</t>
-  </si>
-  <si>
-    <t>Rake Locks or Pick Locks may be purchased for $2k less than cost.</t>
-  </si>
-  <si>
     <t>ExtraHack</t>
   </si>
   <si>
@@ -499,6 +481,36 @@
   </si>
   <si>
     <t>YOINK! +$1k</t>
+  </si>
+  <si>
+    <t>Reveal (sit for multiple turns and reveal all turns. Must stay still)</t>
+  </si>
+  <si>
+    <t>ADRENALINE: May purchase up to 3 extra Attack 💡for $1k each in planning phase</t>
+  </si>
+  <si>
+    <t>PHISHING: If character gets any cash in the heist, gain $2k upon heist success.</t>
+  </si>
+  <si>
+    <t>FAST LEARNER: In planning phase, add 2 💡 to any one skill.</t>
+  </si>
+  <si>
+    <t>EXTORT GUARDS: Gain $2k from first subdued guard.</t>
+  </si>
+  <si>
+    <t>LOOTER: Gain $1k each time character takes HESITATE.</t>
+  </si>
+  <si>
+    <t>OBSERVANT: After planning and before heist, uncover two security tokens for free.</t>
+  </si>
+  <si>
+    <t>PICKER: Rake Locks may be purchased for $1k.</t>
+  </si>
+  <si>
+    <t>MASTER COPY: If 🔓 on a hacking skill, add 3💡 to Unlock Skill.</t>
+  </si>
+  <si>
+    <t>Special</t>
   </si>
 </sst>
 </file>
@@ -872,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,16 +899,16 @@
     <col min="5" max="5" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="7" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="7" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="7" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="7" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="7" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="7" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="74.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="4"/>
@@ -907,7 +919,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -916,57 +928,57 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="M1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -975,46 +987,46 @@
         <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H2" s="7">
         <v>2</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="7">
+        <v>2</v>
+      </c>
+      <c r="N2" s="7">
+        <v>2</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="7">
         <v>4</v>
       </c>
-      <c r="K2" s="7">
-        <v>2</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="7">
-        <v>1</v>
-      </c>
-      <c r="N2" s="7">
-        <v>2</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="7">
-        <v>5</v>
-      </c>
       <c r="Q2" s="7">
         <v>2</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1022,7 +1034,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -1031,10 +1043,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" s="7">
         <v>5</v>
@@ -1043,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3" s="7">
         <v>4</v>
@@ -1052,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M3" s="7">
         <v>1</v>
@@ -1061,16 +1073,13 @@
         <v>2</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P3" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="7">
         <v>2</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1078,7 +1087,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
@@ -1087,28 +1096,28 @@
         <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H4" s="7">
         <v>2</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K4" s="7">
         <v>2</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M4" s="7">
         <v>1</v>
@@ -1117,16 +1126,16 @@
         <v>2</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P4" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="7">
         <v>2</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1134,37 +1143,37 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H5" s="7">
         <v>2</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J5" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K5" s="7">
         <v>2</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M5" s="7">
         <v>1</v>
@@ -1173,13 +1182,16 @@
         <v>2</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P5" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="7">
         <v>2</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1187,19 +1199,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="7">
         <v>15</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" s="7">
         <v>5</v>
@@ -1208,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J6" s="7">
         <v>4</v>
@@ -1217,7 +1229,7 @@
         <v>2</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M6" s="7">
         <v>1</v>
@@ -1226,10 +1238,10 @@
         <v>2</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P6" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="7">
         <v>2</v>
@@ -1240,7 +1252,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1252,7 +1264,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7">
         <v>5</v>
@@ -1261,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J7" s="7">
         <v>4</v>
@@ -1270,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M7" s="7">
         <v>1</v>
@@ -1279,10 +1291,10 @@
         <v>2</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P7" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="7">
         <v>2</v>
@@ -1290,10 +1302,10 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
@@ -1302,51 +1314,54 @@
         <v>0</v>
       </c>
       <c r="E8" s="7">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H8" s="7">
         <v>2</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J8" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K8" s="7">
         <v>2</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M8" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8" s="7">
         <v>2</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P8" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="7">
         <v>2</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
@@ -1358,7 +1373,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="7">
         <v>5</v>
@@ -1367,25 +1382,25 @@
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K9" s="7">
         <v>2</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M9" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N9" s="7">
         <v>2</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P9" s="7">
         <v>5</v>
@@ -1399,49 +1414,49 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
       </c>
       <c r="D10" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="7">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H10" s="7">
         <v>2</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J10" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K10" s="7">
         <v>2</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M10" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N10" s="7">
         <v>2</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P10" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q10" s="7">
         <v>2</v>
@@ -1449,40 +1464,40 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>10</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7">
-        <v>15</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="G11" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H11" s="7">
         <v>2</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J11" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K11" s="7">
         <v>2</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M11" s="7">
         <v>1</v>
@@ -1491,13 +1506,16 @@
         <v>2</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P11" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="7">
         <v>2</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1505,52 +1523,55 @@
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="7">
         <v>1</v>
       </c>
       <c r="D12" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="7">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G12" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H12" s="7">
         <v>2</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J12" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K12" s="7">
         <v>2</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M12" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="7">
         <v>2</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P12" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="7">
         <v>2</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1558,19 +1579,19 @@
         <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
       </c>
       <c r="D13" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="7">
         <v>15</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G13" s="7">
         <v>5</v>
@@ -1579,7 +1600,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J13" s="7">
         <v>4</v>
@@ -1588,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M13" s="7">
         <v>1</v>
@@ -1597,10 +1618,10 @@
         <v>2</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P13" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="7">
         <v>2</v>
@@ -1608,22 +1629,22 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" s="7">
         <v>1</v>
       </c>
       <c r="D14" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="7">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G14" s="7">
         <v>5</v>
@@ -1632,39 +1653,42 @@
         <v>2</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="J14" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K14" s="7">
         <v>2</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="7">
         <v>2</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P14" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="7">
         <v>2</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
@@ -1673,51 +1697,54 @@
         <v>0</v>
       </c>
       <c r="E15" s="7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G15" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H15" s="7">
         <v>2</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J15" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K15" s="7">
         <v>2</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M15" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N15" s="7">
         <v>2</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P15" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="7">
         <v>2</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
@@ -1729,7 +1756,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G16" s="7">
         <v>5</v>
@@ -1738,7 +1765,7 @@
         <v>2</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J16" s="7">
         <v>4</v>
@@ -1747,7 +1774,7 @@
         <v>2</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M16" s="7">
         <v>1</v>
@@ -1756,10 +1783,10 @@
         <v>2</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P16" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="7">
         <v>2</v>
@@ -1767,10 +1794,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
@@ -1782,7 +1809,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G17" s="7">
         <v>5</v>
@@ -1791,7 +1818,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J17" s="7">
         <v>4</v>
@@ -1800,7 +1827,7 @@
         <v>2</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M17" s="7">
         <v>1</v>
@@ -1809,10 +1836,10 @@
         <v>2</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P17" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="7">
         <v>2</v>
@@ -1820,22 +1847,22 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
       <c r="D18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="7">
         <v>15</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G18" s="7">
         <v>5</v>
@@ -1844,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J18" s="7">
         <v>4</v>
@@ -1853,7 +1880,7 @@
         <v>2</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M18" s="7">
         <v>1</v>
@@ -1862,65 +1889,12 @@
         <v>2</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P18" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="7">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7">
-        <v>2</v>
-      </c>
-      <c r="E19" s="7">
-        <v>15</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="7">
-        <v>5</v>
-      </c>
-      <c r="H19" s="7">
-        <v>2</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="J19" s="7">
-        <v>4</v>
-      </c>
-      <c r="K19" s="7">
-        <v>2</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="7">
-        <v>1</v>
-      </c>
-      <c r="N19" s="7">
-        <v>2</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P19" s="7">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1933,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,13 +1936,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
@@ -2010,21 +1984,21 @@
         <v>12</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -2036,40 +2010,40 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="R2" s="2" t="str">
         <f t="shared" ref="R2:R8" si="0">F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
@@ -2099,18 +2073,18 @@
 </v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2122,40 +2096,40 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="R3" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2174,30 +2148,30 @@
 </v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T3" t="s">
         <v>108</v>
-      </c>
-      <c r="T3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="R4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2216,24 +2190,24 @@
 </v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -2255,18 +2229,18 @@
 </v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2278,10 +2252,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="R6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2300,18 +2274,18 @@
 </v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2339,18 +2313,18 @@
 </v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2362,40 +2336,40 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="R8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2414,18 +2388,18 @@
 </v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2437,40 +2411,40 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="R9" s="2" t="str">
         <f t="shared" ref="R9:R11" si="1">F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
@@ -2502,10 +2476,10 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2517,40 +2491,40 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="R10" s="2" t="e">
         <f>F$1 &amp; ": " &amp; I10 &amp; CHAR(10)
@@ -2570,10 +2544,10 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2601,15 +2575,15 @@
 </v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2648,15 +2622,15 @@
 </v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2684,18 +2658,18 @@
 </v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="T13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2707,40 +2681,40 @@
         <v>0</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R14" s="2" t="str">
         <f t="shared" si="2"/>
@@ -2759,18 +2733,18 @@
 </v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T14" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -2782,40 +2756,40 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="R15" s="2" t="str">
         <f t="shared" si="2"/>
@@ -2834,18 +2808,18 @@
 </v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -2857,40 +2831,40 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="O16" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R16" s="2" t="str">
         <f t="shared" si="2"/>
@@ -2909,15 +2883,15 @@
 </v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -2945,15 +2919,15 @@
 </v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -2981,18 +2955,18 @@
 </v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="T18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -3020,18 +2994,18 @@
 </v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="T19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3059,18 +3033,18 @@
 </v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -3082,40 +3056,40 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="R21" s="2" t="str">
         <f t="shared" si="2"/>
@@ -3134,18 +3108,18 @@
 </v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -3157,7 +3131,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="R22" s="2" t="str">
         <f t="shared" si="2"/>
@@ -3176,15 +3150,15 @@
 </v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -3194,10 +3168,13 @@
       </c>
       <c r="E23" s="1">
         <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="R23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">1: 
+        <v xml:space="preserve">1: Reveal (sit for multiple turns and reveal all turns. Must stay still)
 2: 
 3: 
 4: 
@@ -3212,18 +3189,18 @@
 </v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="T23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -3251,18 +3228,18 @@
 </v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="T24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -3290,10 +3267,10 @@
 </v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="T25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3306,7 +3283,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3316,86 +3293,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
         <v>133</v>
-      </c>
-      <c r="B5" t="s">
-        <v>139</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleanup of skills a bit for printing
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -483,9 +483,6 @@
     <t>YOINK! +$1k</t>
   </si>
   <si>
-    <t>Reveal (sit for multiple turns and reveal all turns. Must stay still)</t>
-  </si>
-  <si>
     <t>ADRENALINE: May purchase up to 3 extra Attack 💡for $1k each in planning phase</t>
   </si>
   <si>
@@ -511,6 +508,9 @@
   </si>
   <si>
     <t>Special</t>
+  </si>
+  <si>
+    <t>IDEA: Reveal (sit for multiple turns and reveal all turns. Must stay still)</t>
   </si>
 </sst>
 </file>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
         <v>39</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S1" s="6" t="s">
         <v>41</v>
@@ -1026,7 +1026,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1191,7 +1191,7 @@
         <v>2</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1353,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1571,7 +1571,7 @@
         <v>2</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1680,7 +1680,7 @@
         <v>2</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1736,7 +1736,7 @@
         <v>2</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1905,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2046,7 @@
         <v>96</v>
       </c>
       <c r="R2" s="2" t="str">
-        <f t="shared" ref="R2:R8" si="0">F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
+        <f t="shared" ref="R2:R25" si="0">F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G2 &amp; CHAR(10)
 &amp; H$1 &amp; ": " &amp; H2 &amp; CHAR(10)
 &amp; I$1 &amp; ": " &amp; I2 &amp; CHAR(10)
@@ -2447,18 +2447,7 @@
         <v>151</v>
       </c>
       <c r="R9" s="2" t="str">
-        <f t="shared" ref="R9:R11" si="1">F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G9 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H9 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I9 &amp; CHAR(10)
-&amp; J$1 &amp; ": " &amp; J9 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K9 &amp; CHAR(10)
-&amp; L$1 &amp; ": " &amp; L9 &amp; CHAR(10)
-&amp; M$1 &amp; ": " &amp; M9 &amp; CHAR(10)
-&amp; N$1 &amp; ": " &amp; N9 &amp; CHAR(10)
-&amp; O$1 &amp; ": " &amp; O9 &amp; CHAR(10)
-&amp; P$1 &amp; ": " &amp; P9 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q9 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: FIGHT! 👊🔊🔊💥➜
 2: FIGHT! 👊🔊🔊💥➜
 3: HESITATE. 💡
@@ -2526,20 +2515,21 @@
       <c r="Q10" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="R10" s="2" t="e">
-        <f>F$1 &amp; ": " &amp; I10 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G10 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H10 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp;#REF! &amp; CHAR(10)
-&amp; J$1 &amp; ": " &amp; J10 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K10 &amp; CHAR(10)
-&amp; L$1 &amp; ": " &amp; L10 &amp; CHAR(10)
-&amp; M$1 &amp; ": " &amp; M10 &amp; CHAR(10)
-&amp; N$1 &amp; ": " &amp; N10 &amp; CHAR(10)
-&amp; O$1 &amp; ": " &amp; O10 &amp; CHAR(10)
-&amp; P$1 &amp; ": " &amp; P10 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q10 &amp; CHAR(10)</f>
-        <v>#REF!</v>
+      <c r="R10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: BUSTED!
+2: HESITATE. 💡💡
+3: LISTEN 👂
+4: LISTEN 👂
+5: LISTEN 👂
+6: HESITATE. 💡💡
+7: BUSTED!
+8: FIGHT! 👊🔊🔊➜
+9: ACHOO! 🔊💡
+10: FIGHT! 👊🔊🔊➜
+11: ACHOO! 🔊💡
+12: FIGHT! 👊🔊🔊➜
+</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2559,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="R11" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2595,18 +2585,7 @@
         <v>1</v>
       </c>
       <c r="R12" s="2" t="str">
-        <f t="shared" ref="R12:R25" si="2">F$1 &amp; ": " &amp; F12 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G12 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H12 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I12 &amp; CHAR(10)
-&amp; J$1 &amp; ": " &amp; J12 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K12 &amp; CHAR(10)
-&amp; L$1 &amp; ": " &amp; L12 &amp; CHAR(10)
-&amp; M$1 &amp; ": " &amp; M12 &amp; CHAR(10)
-&amp; N$1 &amp; ": " &amp; N12 &amp; CHAR(10)
-&amp; O$1 &amp; ": " &amp; O12 &amp; CHAR(10)
-&amp; P$1 &amp; ": " &amp; P12 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q12 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2642,7 +2621,7 @@
         <v>2</v>
       </c>
       <c r="R13" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2717,7 +2696,7 @@
         <v>82</v>
       </c>
       <c r="R14" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: WALK. ➜
 2: SPRINT! ➜➜ 🔊🔊
 3: WALK. ➜
@@ -2792,7 +2771,7 @@
         <v>90</v>
       </c>
       <c r="R15" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: HESITATE.💡
 2: WALK. ➜
 3: HESITATE.💡
@@ -2867,7 +2846,7 @@
         <v>82</v>
       </c>
       <c r="R16" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: SHUFFLE! ➜🔊
 2: SHUFFLE! ➜🔊
 3: SPRINT! ➜➜ 🔊🔊
@@ -2886,7 +2865,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>139</v>
       </c>
@@ -2903,7 +2882,7 @@
         <v>1</v>
       </c>
       <c r="R17" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2922,7 +2901,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -2939,7 +2918,7 @@
         <v>1</v>
       </c>
       <c r="R18" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2961,7 +2940,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2978,7 +2957,7 @@
         <v>1</v>
       </c>
       <c r="R19" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -3000,7 +2979,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -3017,7 +2996,7 @@
         <v>2</v>
       </c>
       <c r="R20" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -3039,7 +3018,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -3092,7 +3071,7 @@
         <v>79</v>
       </c>
       <c r="R21" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Zzzt. 📷
 2: NOTHING
 3: CRACK! 💥
@@ -3114,7 +3093,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -3134,7 +3113,7 @@
         <v>154</v>
       </c>
       <c r="R22" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: YOINK! +$1k
 2: 
 3: 
@@ -3153,7 +3132,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -3169,50 +3148,8 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="R23" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">1: Reveal (sit for multiple turns and reveal all turns. Must stay still)
-2: 
-3: 
-4: 
-5: 
-6: 
-7: 
-8: 
-9: 
-10: 
-11: 
-12: 
-</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="T23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>2</v>
-      </c>
-      <c r="R24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -3227,6 +3164,48 @@
 12: 
 </v>
       </c>
+      <c r="S23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T23" t="s">
+        <v>71</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="R24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: 
+2: 
+3: 
+4: 
+5: 
+6: 
+7: 
+8: 
+9: 
+10: 
+11: 
+12: 
+</v>
+      </c>
       <c r="S24" s="2" t="s">
         <v>137</v>
       </c>
@@ -3234,7 +3213,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3251,7 +3230,7 @@
         <v>2</v>
       </c>
       <c r="R25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: 
 2: 
 3: 

</xml_diff>

<commit_message>
moving to d6 for initial skill cards
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\code\timber-wolf\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
     <sheet name="Icon Help" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -423,12 +428,6 @@
     <t>Move your pawn to an adjacent tile (that you planned)</t>
   </si>
   <si>
-    <t>💥</t>
-  </si>
-  <si>
-    <t>Disturb the room you end the turn in.</t>
-  </si>
-  <si>
     <t>Requires: Splice In</t>
   </si>
   <si>
@@ -511,6 +510,57 @@
   </si>
   <si>
     <t>IDEA: Reveal (sit for multiple turns and reveal all turns. Must stay still)</t>
+  </si>
+  <si>
+    <t>FIGHT! 👊🔊🔊</t>
+  </si>
+  <si>
+    <t>SPRINT! ➜🔊🔊</t>
+  </si>
+  <si>
+    <t>Smash and Grab</t>
+  </si>
+  <si>
+    <t>Tinker</t>
+  </si>
+  <si>
+    <t>STUDY 💡💡</t>
+  </si>
+  <si>
+    <t>Improvise</t>
+  </si>
+  <si>
+    <t>Smash 'n' Grab</t>
+  </si>
+  <si>
+    <t>HESITATE 💡</t>
+  </si>
+  <si>
+    <t>CLUNK. 🔓🔊🔊➜</t>
+  </si>
+  <si>
+    <t>Self-Defense</t>
+  </si>
+  <si>
+    <t>LISTEN👂</t>
+  </si>
+  <si>
+    <t>Zzzt. 📷🔊🔊</t>
+  </si>
+  <si>
+    <t>RUN! 🔊🔊➜➜</t>
+  </si>
+  <si>
+    <t>Hurry</t>
+  </si>
+  <si>
+    <t>Zzzt. 📷🔊🔊➜</t>
+  </si>
+  <si>
+    <t>PUNCH! 👊🔊🔊➜</t>
+  </si>
+  <si>
+    <t>KICK! 👊🔊➜</t>
   </si>
 </sst>
 </file>
@@ -554,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -583,6 +633,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,6 +649,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -640,7 +700,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -675,7 +735,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -967,7 +1027,7 @@
         <v>39</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S1" s="6" t="s">
         <v>41</v>
@@ -1026,7 +1086,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1135,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1191,7 +1251,7 @@
         <v>2</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1353,7 +1413,7 @@
         <v>2</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1515,7 +1575,7 @@
         <v>2</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1571,7 +1631,7 @@
         <v>2</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1680,7 +1740,7 @@
         <v>2</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1736,7 +1796,7 @@
         <v>2</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1905,28 +1965,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" style="2" customWidth="1"/>
     <col min="19" max="19" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -1938,7 +1998,7 @@
       <c r="B1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
@@ -1993,71 +2053,345 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
+    <row r="2" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="13">
+        <v>2</v>
+      </c>
+      <c r="D2" s="13">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
       <c r="R2" s="2" t="str">
-        <f t="shared" ref="R2:R25" si="0">F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
+        <f>F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G2 &amp; CHAR(10)
 &amp; H$1 &amp; ": " &amp; H2 &amp; CHAR(10)
 &amp; I$1 &amp; ": " &amp; I2 &amp; CHAR(10)
 &amp; J$1 &amp; ": " &amp; J2 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K2 &amp; CHAR(10)
-&amp; L$1 &amp; ": " &amp; L2 &amp; CHAR(10)
-&amp; M$1 &amp; ": " &amp; M2 &amp; CHAR(10)
-&amp; N$1 &amp; ": " &amp; N2 &amp; CHAR(10)
-&amp; O$1 &amp; ": " &amp; O2 &amp; CHAR(10)
-&amp; P$1 &amp; ": " &amp; P2 &amp; CHAR(10)
-&amp; Q$1 &amp; ": " &amp; Q2 &amp; CHAR(10)</f>
+&amp; K$1 &amp; ": " &amp; K2 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: RUN! 🔊🔊➜➜
+2: Zzzt. 📷🔊🔊➜
+3: CLUNK. 🔓🔊🔊➜
+4: PUNCH! 👊🔊🔊➜
+5: STUDY 💡💡
+6: RUN! 🔊🔊➜➜
+</v>
+      </c>
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="13">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="2" t="str">
+        <f t="shared" ref="R3:R6" si="0">F$1 &amp; ": " &amp; F3 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G3 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H3 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I3 &amp; CHAR(10)
+&amp; J$1 &amp; ": " &amp; J3 &amp; CHAR(10)
+&amp; K$1 &amp; ": " &amp; K3 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: PUNCH! 👊🔊🔊➜
+2: HESITATE 💡
+3: CLUNK. 🔓🔊🔊➜
+4: HESITATE 💡
+5: CLUNK. 🔓🔊🔊➜
+6: Zzzt. 📷🔊🔊➜
+</v>
+      </c>
+      <c r="S3" s="14"/>
+    </row>
+    <row r="4" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: STUDY 💡💡
+2: RUN! 🔊🔊➜➜
+3: LISTEN👂
+4: STUDY 💡💡
+5: Zzzt. 📷🔊🔊
+6: CLUNK. 🔓🔊🔊➜
+</v>
+      </c>
+      <c r="S4" s="14"/>
+    </row>
+    <row r="5" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="13">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: HESITATE 💡
+2: PUNCH! 👊🔊🔊➜
+3: HESITATE 💡
+4: RUN! 🔊🔊➜➜
+5: PUNCH! 👊🔊🔊➜
+6: KICK! 👊🔊➜
+</v>
+      </c>
+      <c r="S5" s="14"/>
+    </row>
+    <row r="6" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: RUN! 🔊🔊➜➜
+2: HESITATE 💡
+3: RUN! 🔊🔊➜➜
+4: CLUNK. 🔓🔊🔊➜
+5: HESITATE 💡
+6: RUN! 🔊🔊➜➜
+</v>
+      </c>
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="14"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R8" s="2" t="str">
+        <f t="shared" ref="R8:R31" si="1">F$1 &amp; ": " &amp; F8 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G8 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H8 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I8 &amp; CHAR(10)
+&amp; J$1 &amp; ": " &amp; J8 &amp; CHAR(10)
+&amp; K$1 &amp; ": " &amp; K8 &amp; CHAR(10)
+&amp; L$1 &amp; ": " &amp; L8 &amp; CHAR(10)
+&amp; M$1 &amp; ": " &amp; M8 &amp; CHAR(10)
+&amp; N$1 &amp; ": " &amp; N8 &amp; CHAR(10)
+&amp; O$1 &amp; ": " &amp; O8 &amp; CHAR(10)
+&amp; P$1 &amp; ": " &amp; P8 &amp; CHAR(10)
+&amp; Q$1 &amp; ": " &amp; Q8 &amp; CHAR(10)</f>
         <v xml:space="preserve">1: BAM! 🔓🔊🔊 ➜
 2: BAM! 🔓🔊🔊🔊➜
 3: THUD. 🔊
@@ -2072,67 +2406,67 @@
 12: BAM! 🔓🔊🔊🔊
 </v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="R3" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="R9" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: OOF! 🔊
 2: ALMOST!💡💡
 3: CLUNK. 🔓🔊💥➜
@@ -2147,34 +2481,34 @@
 12: ALMOST!💡💡
 </v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
         <v>3</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="R4" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="R10" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: BYPASS! 🔓🔓➜
 2: 
 3: 
@@ -2189,31 +2523,31 @@
 12: 
 </v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="R5" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="R11" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2228,37 +2562,37 @@
 12: 
 </v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S11" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>59</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="R6" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="R12" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: BRIBE! 👊 -$1k
 2: YOINK! +$1k
 3: 
@@ -2273,31 +2607,31 @@
 12: 
 </v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="S12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
         <v>5</v>
       </c>
-      <c r="E7" s="1">
-        <v>2</v>
-      </c>
-      <c r="R7" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="R13" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2312,67 +2646,67 @@
 12: 
 </v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S13" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="R8" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="R14" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: SURPRISE. 👊➜
 2: FAIL! Busted.
 3: FIGHT! 👊🔊🔊➜
@@ -2387,67 +2721,67 @@
 12: FIGHT! 👊🔊🔊➜
 </v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="S14" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="R9" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="R15" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: FIGHT! 👊🔊🔊💥➜
 2: FIGHT! 👊🔊🔊💥➜
 3: HESITATE. 💡
@@ -2463,60 +2797,60 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>110</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="H16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="M10" s="2" t="s">
+      <c r="L16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="O10" s="2" t="s">
+      <c r="N16" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q10" s="2" t="s">
+      <c r="P16" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="R10" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="R16" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: BUSTED!
 2: HESITATE. 💡💡
 3: LISTEN 👂
@@ -2532,24 +2866,24 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="R11" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
+      <c r="R17" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2564,28 +2898,28 @@
 12: 
 </v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="S17" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>55</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="R12" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="R18" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2600,28 +2934,28 @@
 12: 
 </v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="S18" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
         <v>5</v>
       </c>
-      <c r="E13" s="1">
-        <v>2</v>
-      </c>
-      <c r="R13" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="E19" s="1">
+        <v>3</v>
+      </c>
+      <c r="R19" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2636,67 +2970,67 @@
 12: 
 </v>
       </c>
-      <c r="S13" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="S19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>88</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R14" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="R20" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: WALK. ➜
 2: SPRINT! ➜➜ 🔊🔊
 3: WALK. ➜
@@ -2711,67 +3045,67 @@
 12: SPRINT! ➜➜ 🔊🔊
 </v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="S20" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>87</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="N21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="P21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="Q21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R15" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="R21" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: HESITATE.💡
 2: WALK. ➜
 3: HESITATE.💡
@@ -2786,67 +3120,67 @@
 12: STUMBLE. ➜🔊
 </v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="S21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T15" s="2" t="s">
+      <c r="T21" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>92</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="N22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="Q22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R16" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="R22" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: SHUFFLE! ➜🔊
 2: SHUFFLE! ➜🔊
 3: SPRINT! ➜➜ 🔊🔊
@@ -2861,28 +3195,28 @@
 12: SPRINT! ➜➜ 🔊🔊
 </v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="S22" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="R17" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+      <c r="R23" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2897,28 +3231,28 @@
 12: 
 </v>
       </c>
-      <c r="S17" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="S23" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>89</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="R18" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="R24" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2933,31 +3267,31 @@
 12: 
 </v>
       </c>
-      <c r="S18" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="T18" t="s">
+      <c r="S24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="T24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="R19" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2</v>
+      </c>
+      <c r="R25" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -2972,31 +3306,31 @@
 12: 
 </v>
       </c>
-      <c r="S19" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="T19" t="s">
+      <c r="S25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="T25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>64</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
         <v>3</v>
       </c>
-      <c r="E20" s="1">
-        <v>2</v>
-      </c>
-      <c r="R20" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="E26" s="1">
+        <v>3</v>
+      </c>
+      <c r="R26" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -3011,67 +3345,67 @@
 12: 
 </v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="S26" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>80</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="C21">
+      <c r="C27" s="1">
         <v>4</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D27" s="1">
         <v>0</v>
       </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H27" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="L27" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="N27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="O27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="P27" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="Q27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="R21" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="R27" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: Zzzt. 📷
 2: NOTHING
 3: CRACK! 💥
@@ -3086,34 +3420,34 @@
 12: NOTHING
 </v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="S27" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T21" t="s">
+      <c r="T27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>84</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="R22" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="R28" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: YOINK! +$1k
 2: 
 3: 
@@ -3128,28 +3462,28 @@
 12: 
 </v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="S28" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="29" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B29" t="s">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1">
-        <v>2</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="R23" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="R29" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -3164,34 +3498,34 @@
 12: 
 </v>
       </c>
-      <c r="S23" s="2" t="s">
+      <c r="S29" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T23" t="s">
+      <c r="T29" t="s">
         <v>71</v>
       </c>
-      <c r="U23" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="U29" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>70</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>2</v>
-      </c>
-      <c r="R24" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+      <c r="R30" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -3206,31 +3540,31 @@
 12: 
 </v>
       </c>
-      <c r="S24" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="T24" t="s">
+      <c r="S30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>67</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B31" t="s">
         <v>21</v>
       </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
         <v>5</v>
       </c>
-      <c r="E25" s="1">
-        <v>2</v>
-      </c>
-      <c r="R25" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="E31" s="1">
+        <v>3</v>
+      </c>
+      <c r="R31" s="2" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
 2: 
 3: 
@@ -3245,24 +3579,58 @@
 12: 
 </v>
       </c>
-      <c r="S25" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="T25" t="s">
+      <c r="S31" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T31" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>166</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3300,7 +3668,7 @@
         <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -3330,28 +3698,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more skill data balancing
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="178">
   <si>
     <t>Name</t>
   </si>
@@ -512,15 +512,6 @@
     <t>IDEA: Reveal (sit for multiple turns and reveal all turns. Must stay still)</t>
   </si>
   <si>
-    <t>FIGHT! 👊🔊🔊</t>
-  </si>
-  <si>
-    <t>SPRINT! ➜🔊🔊</t>
-  </si>
-  <si>
-    <t>Smash and Grab</t>
-  </si>
-  <si>
     <t>Tinker</t>
   </si>
   <si>
@@ -561,6 +552,9 @@
   </si>
   <si>
     <t>KICK! 👊🔊➜</t>
+  </si>
+  <si>
+    <t>YANK! 💡💡💡🔊🔊</t>
   </si>
 </sst>
 </file>
@@ -1965,10 +1959,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="E10" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2049,7 @@
     </row>
     <row r="2" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C2" s="13">
         <v>2</v>
@@ -2067,22 +2061,22 @@
         <v>1</v>
       </c>
       <c r="F2" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>178</v>
-      </c>
       <c r="J2" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
@@ -2109,7 +2103,7 @@
     </row>
     <row r="3" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C3" s="13">
         <v>2</v>
@@ -2121,22 +2115,22 @@
         <v>1</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
@@ -2163,7 +2157,7 @@
     </row>
     <row r="4" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C4" s="13">
         <v>2</v>
@@ -2175,22 +2169,22 @@
         <v>1</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -2203,7 +2197,7 @@
         <v xml:space="preserve">1: STUDY 💡💡
 2: RUN! 🔊🔊➜➜
 3: LISTEN👂
-4: STUDY 💡💡
+4: YANK! 💡💡💡🔊🔊
 5: Zzzt. 📷🔊🔊
 6: CLUNK. 🔓🔊🔊➜
 </v>
@@ -2212,7 +2206,7 @@
     </row>
     <row r="5" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C5" s="13">
         <v>2</v>
@@ -2224,22 +2218,22 @@
         <v>1</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I5" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="J5" s="13" t="s">
-        <v>178</v>
-      </c>
       <c r="K5" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -2261,7 +2255,7 @@
     </row>
     <row r="6" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C6" s="13">
         <v>2</v>
@@ -2273,22 +2267,22 @@
         <v>1</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -2339,9 +2333,6 @@
       </c>
       <c r="D8" s="1">
         <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>103</v>
@@ -2426,9 +2417,6 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
       <c r="F9" s="1" t="s">
         <v>100</v>
       </c>
@@ -2501,9 +2489,6 @@
       <c r="D10" s="1">
         <v>3</v>
       </c>
-      <c r="E10" s="1">
-        <v>2</v>
-      </c>
       <c r="F10" s="1" t="s">
         <v>123</v>
       </c>
@@ -2543,9 +2528,6 @@
       <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="E11" s="1">
-        <v>3</v>
-      </c>
       <c r="R11" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -2582,9 +2564,6 @@
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="E12" s="1">
-        <v>2</v>
-      </c>
       <c r="F12" s="1" t="s">
         <v>151</v>
       </c>
@@ -2627,9 +2606,6 @@
       <c r="D13" s="1">
         <v>5</v>
       </c>
-      <c r="E13" s="1">
-        <v>3</v>
-      </c>
       <c r="R13" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -2666,9 +2642,6 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
       <c r="F14" s="1" t="s">
         <v>112</v>
       </c>
@@ -2741,9 +2714,6 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
       <c r="F15" s="1" t="s">
         <v>149</v>
       </c>
@@ -2810,9 +2780,6 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
       <c r="F16" s="1" t="s">
         <v>146</v>
       </c>
@@ -2879,9 +2846,6 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="1">
-        <v>2</v>
-      </c>
       <c r="R17" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -2915,9 +2879,6 @@
       <c r="D18" s="1">
         <v>2</v>
       </c>
-      <c r="E18" s="1">
-        <v>2</v>
-      </c>
       <c r="R18" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -2951,9 +2912,6 @@
       <c r="D19" s="1">
         <v>5</v>
       </c>
-      <c r="E19" s="1">
-        <v>3</v>
-      </c>
       <c r="R19" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -2990,9 +2948,6 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
       <c r="F20" s="1" t="s">
         <v>81</v>
       </c>
@@ -3065,9 +3020,6 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
       <c r="F21" s="1" t="s">
         <v>91</v>
       </c>
@@ -3140,9 +3092,6 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
       <c r="F22" s="1" t="s">
         <v>85</v>
       </c>
@@ -3212,9 +3161,6 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="1">
-        <v>2</v>
-      </c>
       <c r="R23" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -3248,9 +3194,6 @@
       <c r="D24" s="1">
         <v>1</v>
       </c>
-      <c r="E24" s="1">
-        <v>2</v>
-      </c>
       <c r="R24" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -3287,9 +3230,6 @@
       <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="E25" s="1">
-        <v>2</v>
-      </c>
       <c r="R25" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -3326,9 +3266,6 @@
       <c r="D26" s="1">
         <v>3</v>
       </c>
-      <c r="E26" s="1">
-        <v>3</v>
-      </c>
       <c r="R26" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -3365,9 +3302,6 @@
       <c r="D27" s="1">
         <v>0</v>
       </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
       <c r="F27" s="1" t="s">
         <v>119</v>
       </c>
@@ -3440,9 +3374,6 @@
       <c r="D28" s="1">
         <v>2</v>
       </c>
-      <c r="E28" s="1">
-        <v>2</v>
-      </c>
       <c r="F28" s="1" t="s">
         <v>152</v>
       </c>
@@ -3479,9 +3410,6 @@
       <c r="D29" s="1">
         <v>2</v>
       </c>
-      <c r="E29" s="1">
-        <v>2</v>
-      </c>
       <c r="R29" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -3521,9 +3449,6 @@
       <c r="D30" s="1">
         <v>2</v>
       </c>
-      <c r="E30" s="1">
-        <v>3</v>
-      </c>
       <c r="R30" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -3560,9 +3485,6 @@
       <c r="D31" s="1">
         <v>5</v>
       </c>
-      <c r="E31" s="1">
-        <v>3</v>
-      </c>
       <c r="R31" s="2" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: 
@@ -3584,39 +3506,6 @@
       </c>
       <c r="T31" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>166</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
characters: rewrote lvl1s almost entirely
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="170">
   <si>
     <t>Name</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Script Kiddie</t>
   </si>
   <si>
-    <t>n00b</t>
-  </si>
-  <si>
     <t>Hacktivist</t>
   </si>
   <si>
@@ -104,42 +101,15 @@
     <t>Move</t>
   </si>
   <si>
-    <t>Skill1</t>
-  </si>
-  <si>
-    <t>Skill2</t>
-  </si>
-  <si>
-    <t>Skill3</t>
-  </si>
-  <si>
-    <t>Skill4</t>
-  </si>
-  <si>
     <t>Attack</t>
   </si>
   <si>
-    <t>Skill1Exp</t>
-  </si>
-  <si>
-    <t>Skill1MaxLevel</t>
-  </si>
-  <si>
-    <t>Skill2Exp</t>
-  </si>
-  <si>
     <t>Skill2MaxLevel</t>
   </si>
   <si>
-    <t>Skill3Exp</t>
-  </si>
-  <si>
     <t>Skill3MaxLevel</t>
   </si>
   <si>
-    <t>Skill4Exp</t>
-  </si>
-  <si>
     <t>Skill4MaxLevel</t>
   </si>
   <si>
@@ -251,9 +221,6 @@
     <t>great all around if you can get it</t>
   </si>
   <si>
-    <t>ExtraHack</t>
-  </si>
-  <si>
     <t>Rolls</t>
   </si>
   <si>
@@ -455,12 +422,6 @@
     <t>LISTEN 👂</t>
   </si>
   <si>
-    <t>👂</t>
-  </si>
-  <si>
-    <t>Uncover 1 unknown security token</t>
-  </si>
-  <si>
     <t>BUSTED!</t>
   </si>
   <si>
@@ -482,15 +443,9 @@
     <t>YOINK! +$1k</t>
   </si>
   <si>
-    <t>ADRENALINE: May purchase up to 3 extra Attack 💡for $1k each in planning phase</t>
-  </si>
-  <si>
     <t>PHISHING: If character gets any cash in the heist, gain $2k upon heist success.</t>
   </si>
   <si>
-    <t>FAST LEARNER: In planning phase, add 2 💡 to any one skill.</t>
-  </si>
-  <si>
     <t>EXTORT GUARDS: Gain $2k from first subdued guard.</t>
   </si>
   <si>
@@ -500,12 +455,6 @@
     <t>OBSERVANT: After planning and before heist, uncover two security tokens for free.</t>
   </si>
   <si>
-    <t>PICKER: Rake Locks may be purchased for $1k.</t>
-  </si>
-  <si>
-    <t>MASTER COPY: If 🔓 on a hacking skill, add 3💡 to Unlock Skill.</t>
-  </si>
-  <si>
     <t>Special</t>
   </si>
   <si>
@@ -533,12 +482,6 @@
     <t>Self-Defense</t>
   </si>
   <si>
-    <t>LISTEN👂</t>
-  </si>
-  <si>
-    <t>Zzzt. 📷🔊🔊</t>
-  </si>
-  <si>
     <t>RUN! 🔊🔊➜➜</t>
   </si>
   <si>
@@ -551,10 +494,43 @@
     <t>PUNCH! 👊🔊🔊➜</t>
   </si>
   <si>
-    <t>KICK! 👊🔊➜</t>
-  </si>
-  <si>
     <t>YANK! 💡💡💡🔊🔊</t>
+  </si>
+  <si>
+    <t>Zzzt. 📷🔊</t>
+  </si>
+  <si>
+    <t>KICK! 👊🔊➜➜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICKER: Gain 💡 on 🔓 </t>
+  </si>
+  <si>
+    <t>ADRENALINE: May purchase up to 3💡for $1k each in planning phase on skills with 👊</t>
+  </si>
+  <si>
+    <t>Skill1Ideas</t>
+  </si>
+  <si>
+    <t>Skill2Ideas</t>
+  </si>
+  <si>
+    <t>SLIPPERY: 2 free💡when escaping</t>
+  </si>
+  <si>
+    <t>ADRENALINE: Gain 💡 on 👊</t>
+  </si>
+  <si>
+    <t>DISCOVER 🔍</t>
+  </si>
+  <si>
+    <t>🔍</t>
+  </si>
+  <si>
+    <t>Uncover 1 unknown security token anywhere</t>
+  </si>
+  <si>
+    <t>HAZ TEH CODES? Once per turn, may 🔍but gain 🔊🔊</t>
   </si>
 </sst>
 </file>
@@ -938,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,29 +927,20 @@
     <col min="3" max="3" width="4.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="7" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="7" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="7" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="7" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="74.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="6" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="14.42578125" style="7" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="74.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -982,113 +949,71 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="7">
-        <v>12</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>26</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="7">
+        <v>3</v>
       </c>
       <c r="G2" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" s="7">
         <v>2</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>31</v>
+      <c r="I2" s="7">
+        <v>2</v>
       </c>
       <c r="J2" s="7">
-        <v>1</v>
-      </c>
-      <c r="K2" s="7">
-        <v>2</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="7">
-        <v>2</v>
-      </c>
-      <c r="N2" s="7">
-        <v>2</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="7">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="7">
-        <v>2</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -1097,543 +1022,339 @@
         <v>1</v>
       </c>
       <c r="E3" s="7">
-        <v>14</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="7">
+        <v>3</v>
       </c>
       <c r="G3" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H3" s="7">
         <v>2</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>31</v>
+      <c r="I3" s="7">
+        <v>2</v>
       </c>
       <c r="J3" s="7">
-        <v>4</v>
-      </c>
-      <c r="K3" s="7">
-        <v>2</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="7">
-        <v>1</v>
-      </c>
-      <c r="N3" s="7">
-        <v>2</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="7">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>26</v>
+      <c r="F4" s="7">
+        <v>2</v>
       </c>
       <c r="G4" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="7">
         <v>2</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>31</v>
+      <c r="I4" s="7">
+        <v>2</v>
       </c>
       <c r="J4" s="7">
-        <v>3</v>
-      </c>
-      <c r="K4" s="7">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="7">
-        <v>1</v>
-      </c>
-      <c r="N4" s="7">
-        <v>2</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>2</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="7">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>26</v>
+      <c r="F5" s="7">
+        <v>1</v>
       </c>
       <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>2</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2</v>
+      </c>
+      <c r="J5" s="7">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>8</v>
+      </c>
+      <c r="F6" s="7">
         <v>3</v>
       </c>
-      <c r="H5" s="7">
-        <v>2</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="7">
-        <v>2</v>
-      </c>
-      <c r="K5" s="7">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>2</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P5" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>2</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>2</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>2</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>9</v>
+      </c>
+      <c r="F7" s="7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>6</v>
+      </c>
+      <c r="F8" s="7">
+        <v>4</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>2</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7">
+        <v>2</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7">
+        <v>4</v>
+      </c>
+      <c r="H9" s="7">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2</v>
+      </c>
+      <c r="J9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7">
+        <v>15</v>
+      </c>
+      <c r="F10" s="7">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7">
+        <v>4</v>
+      </c>
+      <c r="H10" s="7">
+        <v>2</v>
+      </c>
+      <c r="I10" s="7">
+        <v>2</v>
+      </c>
+      <c r="J10" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7">
         <v>15</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F11" s="7">
         <v>5</v>
       </c>
-      <c r="H6" s="7">
-        <v>2</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="7">
+      <c r="G11" s="7">
         <v>4</v>
       </c>
-      <c r="K6" s="7">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
-      <c r="N6" s="7">
-        <v>2</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="H11" s="7">
+        <v>2</v>
+      </c>
+      <c r="I11" s="7">
+        <v>2</v>
+      </c>
+      <c r="J11" s="7">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
         <v>15</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F12" s="7">
         <v>5</v>
       </c>
-      <c r="H7" s="7">
-        <v>2</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="7">
-        <v>4</v>
-      </c>
-      <c r="K7" s="7">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="7">
-        <v>2</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P7" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7">
-        <v>13</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="7">
-        <v>2</v>
-      </c>
-      <c r="H8" s="7">
-        <v>2</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="7">
-        <v>2</v>
-      </c>
-      <c r="K8" s="7">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="7">
-        <v>2</v>
-      </c>
-      <c r="N8" s="7">
-        <v>2</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P8" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="7">
-        <v>2</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="7">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7">
-        <v>15</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="G12" s="7">
         <v>5</v>
       </c>
-      <c r="H9" s="7">
-        <v>2</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="7">
-        <v>5</v>
-      </c>
-      <c r="K9" s="7">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="7">
-        <v>5</v>
-      </c>
-      <c r="N9" s="7">
-        <v>2</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P9" s="7">
-        <v>5</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="7">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
-        <v>2</v>
-      </c>
-      <c r="E10" s="7">
-        <v>20</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="7">
-        <v>7</v>
-      </c>
-      <c r="H10" s="7">
-        <v>2</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" s="7">
-        <v>7</v>
-      </c>
-      <c r="K10" s="7">
-        <v>2</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="7">
-        <v>7</v>
-      </c>
-      <c r="N10" s="7">
-        <v>2</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P10" s="7">
-        <v>7</v>
-      </c>
-      <c r="Q10" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="7">
-        <v>3</v>
-      </c>
-      <c r="H11" s="7">
-        <v>2</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="7">
-        <v>1</v>
-      </c>
-      <c r="K11" s="7">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="7">
-        <v>1</v>
-      </c>
-      <c r="N11" s="7">
-        <v>2</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>2</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7">
-        <v>12</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="7">
-        <v>2</v>
-      </c>
       <c r="H12" s="7">
         <v>2</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>31</v>
+      <c r="I12" s="7">
+        <v>2</v>
       </c>
       <c r="J12" s="7">
         <v>2</v>
       </c>
-      <c r="K12" s="7">
-        <v>2</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="7">
-        <v>2</v>
-      </c>
-      <c r="N12" s="7">
-        <v>2</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="7">
-        <v>2</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K12" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
@@ -1644,315 +1365,157 @@
       <c r="E13" s="7">
         <v>15</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>26</v>
+      <c r="F13" s="7">
+        <v>5</v>
       </c>
       <c r="G13" s="7">
+        <v>4</v>
+      </c>
+      <c r="H13" s="7">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>2</v>
+      </c>
+      <c r="J13" s="7">
+        <v>2</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7">
+        <v>15</v>
+      </c>
+      <c r="F14" s="7">
         <v>5</v>
       </c>
-      <c r="H13" s="7">
-        <v>2</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="7">
+      <c r="G14" s="7">
         <v>4</v>
       </c>
-      <c r="K13" s="7">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="7">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7">
-        <v>2</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P13" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="H14" s="7">
+        <v>2</v>
+      </c>
+      <c r="I14" s="7">
+        <v>2</v>
+      </c>
+      <c r="J14" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
         <v>3</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
-        <v>9</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="7">
-        <v>5</v>
-      </c>
-      <c r="H14" s="7">
-        <v>2</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="7">
-        <v>2</v>
-      </c>
-      <c r="K14" s="7">
-        <v>2</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="7">
-        <v>2</v>
-      </c>
-      <c r="N14" s="7">
-        <v>2</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P14" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="7">
-        <v>2</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
       <c r="E15" s="7">
-        <v>10</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="F15" s="7">
+        <v>7</v>
       </c>
       <c r="G15" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H15" s="7">
         <v>2</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>76</v>
+      <c r="I15" s="7">
+        <v>2</v>
       </c>
       <c r="J15" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
         <v>3</v>
-      </c>
-      <c r="K15" s="7">
-        <v>2</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="7">
-        <v>3</v>
-      </c>
-      <c r="N15" s="7">
-        <v>2</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P15" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="7">
-        <v>2</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7">
-        <v>1</v>
       </c>
       <c r="E16" s="7">
         <v>15</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>26</v>
+      <c r="F16" s="7">
+        <v>5</v>
       </c>
       <c r="G16" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16" s="7">
         <v>2</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>76</v>
+      <c r="I16" s="7">
+        <v>2</v>
       </c>
       <c r="J16" s="7">
-        <v>4</v>
-      </c>
-      <c r="K16" s="7">
-        <v>2</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M16" s="7">
-        <v>1</v>
-      </c>
-      <c r="N16" s="7">
-        <v>2</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P16" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
       <c r="D17" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="7">
         <v>15</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>26</v>
+      <c r="F17" s="7">
+        <v>5</v>
       </c>
       <c r="G17" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H17" s="7">
         <v>2</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>76</v>
+      <c r="I17" s="7">
+        <v>2</v>
       </c>
       <c r="J17" s="7">
-        <v>4</v>
-      </c>
-      <c r="K17" s="7">
-        <v>2</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="7">
-        <v>1</v>
-      </c>
-      <c r="N17" s="7">
-        <v>2</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P17" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7">
-        <v>2</v>
-      </c>
-      <c r="E18" s="7">
-        <v>15</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="7">
-        <v>5</v>
-      </c>
-      <c r="H18" s="7">
-        <v>2</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J18" s="7">
-        <v>4</v>
-      </c>
-      <c r="K18" s="7">
-        <v>2</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M18" s="7">
-        <v>1</v>
-      </c>
-      <c r="N18" s="7">
-        <v>2</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P18" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="7">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:S18">
+    <sortCondition ref="D2:D18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1961,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E9:E10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,13 +1553,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
@@ -2038,18 +1601,18 @@
         <v>12</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C2" s="13">
         <v>2</v>
@@ -2061,22 +1624,22 @@
         <v>1</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
@@ -2103,7 +1666,7 @@
     </row>
     <row r="3" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C3" s="13">
         <v>2</v>
@@ -2115,22 +1678,22 @@
         <v>1</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
@@ -2157,7 +1720,7 @@
     </row>
     <row r="4" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="C4" s="13">
         <v>2</v>
@@ -2169,22 +1732,22 @@
         <v>1</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -2196,9 +1759,9 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: STUDY 💡💡
 2: RUN! 🔊🔊➜➜
-3: LISTEN👂
+3: DISCOVER 🔍
 4: YANK! 💡💡💡🔊🔊
-5: Zzzt. 📷🔊🔊
+5: Zzzt. 📷🔊
 6: CLUNK. 🔓🔊🔊➜
 </v>
       </c>
@@ -2206,7 +1769,7 @@
     </row>
     <row r="5" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="C5" s="13">
         <v>2</v>
@@ -2218,44 +1781,48 @@
         <v>1</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="L5" s="13"/>
+        <v>156</v>
+      </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>F$1 &amp; ": " &amp; F5 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G5 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H5 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I5 &amp; CHAR(10)
+&amp; J$1 &amp; ": " &amp; K5 &amp; CHAR(10)
+&amp; K$1 &amp; ": " &amp; J5 &amp; CHAR(10)</f>
         <v xml:space="preserve">1: HESITATE 💡
 2: PUNCH! 👊🔊🔊➜
 3: HESITATE 💡
 4: RUN! 🔊🔊➜➜
 5: PUNCH! 👊🔊🔊➜
-6: KICK! 👊🔊➜
+6: KICK! 👊🔊➜➜
 </v>
       </c>
       <c r="S5" s="14"/>
     </row>
     <row r="6" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="C6" s="13">
         <v>2</v>
@@ -2267,22 +1834,22 @@
         <v>1</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -2323,10 +1890,10 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -2335,40 +1902,40 @@
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="R8" s="2" t="str">
         <f t="shared" ref="R8:R31" si="1">F$1 &amp; ": " &amp; F8 &amp; CHAR(10)
@@ -2398,18 +1965,18 @@
 </v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T8" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -2418,40 +1985,40 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="R9" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2470,18 +2037,18 @@
 </v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T9" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -2490,7 +2057,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="R10" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2509,18 +2076,18 @@
 </v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T10" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -2545,18 +2112,18 @@
 </v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T11" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -2565,10 +2132,10 @@
         <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="R12" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2587,18 +2154,18 @@
 </v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -2623,18 +2190,18 @@
 </v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T13" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -2643,40 +2210,40 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="R14" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2695,18 +2262,18 @@
 </v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -2715,40 +2282,40 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="R15" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2769,10 +2336,10 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -2781,40 +2348,40 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="R16" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2835,10 +2402,10 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -2863,15 +2430,15 @@
 </v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -2896,15 +2463,15 @@
 </v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -2929,18 +2496,18 @@
 </v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="T19" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -2949,40 +2516,40 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="L20" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="R20" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3001,18 +2568,18 @@
 </v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T20" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -3021,40 +2588,40 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="R21" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3073,18 +2640,18 @@
 </v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -3093,40 +2660,40 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="L22" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="R22" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3145,15 +2712,15 @@
 </v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
@@ -3178,15 +2745,15 @@
 </v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -3211,18 +2778,18 @@
 </v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="T24" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
@@ -3247,18 +2814,18 @@
 </v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="T25" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
@@ -3283,18 +2850,18 @@
 </v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T26" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="1">
         <v>4</v>
@@ -3303,40 +2870,40 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="R27" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3355,18 +2922,18 @@
 </v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T27" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -3375,7 +2942,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="R28" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3394,15 +2961,15 @@
 </v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
@@ -3427,21 +2994,21 @@
 </v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="T29" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
@@ -3466,18 +3033,18 @@
 </v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="T30" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
@@ -3502,10 +3069,10 @@
 </v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="T31" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3519,7 +3086,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3529,78 +3096,78 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
whole new alert tracker, & new skills
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="200">
   <si>
     <t>Name</t>
   </si>
@@ -496,9 +496,6 @@
   </si>
   <si>
     <t>Looter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PICKER%nGain 💡 on 🔓 </t>
   </si>
   <si>
     <t>ADRENALINE%nGain 💡 on 👊</t>
@@ -655,13 +652,22 @@
     <t>Crawl ➜</t>
   </si>
   <si>
-    <t>Saunter 🔊➜</t>
-  </si>
-  <si>
     <t>I CAN HAZ TEH CODES?%nOnce per turn, may  🔊🔊🔍.%nI CAN HEARTBLEED%nIf outdoors, may spend 💡💡 to 🔍</t>
   </si>
   <si>
     <t>HESITATE  💡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICK  🔓 </t>
+  </si>
+  <si>
+    <t>PICKER%nGain 💡 when you 🔓%nMASTER KEY%nWhen outdoors, may use  💡💡 to enable one player to 🔓</t>
+  </si>
+  <si>
+    <t>Saunter 🔊➜➜</t>
+  </si>
+  <si>
+    <t>Shimmy  🔊➜➜</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1125,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,8 +1138,8 @@
     <col min="6" max="6" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="14.42578125" style="6" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="74.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="3"/>
@@ -1171,10 +1177,10 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>136</v>
@@ -1183,7 +1189,7 @@
         <v>29</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1200,7 +1206,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="25">
         <v>3</v>
@@ -1218,13 +1224,13 @@
         <v>2</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L2" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="M2" s="26" t="s">
         <v>197</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>158</v>
       </c>
       <c r="O2" s="25">
         <f>F2+G2</f>
@@ -1263,13 +1269,13 @@
         <v>2</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O3" s="25">
         <f t="shared" ref="O3:O16" si="0">F3+G3</f>
@@ -1308,13 +1314,13 @@
         <v>2</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L4" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O4" s="25">
         <f t="shared" si="0"/>
@@ -1353,13 +1359,13 @@
         <v>2</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O5" s="25">
         <f t="shared" si="0"/>
@@ -1398,13 +1404,13 @@
         <v>2</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M6" s="26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O6" s="25">
         <f t="shared" si="0"/>
@@ -1446,10 +1452,10 @@
         <v>193</v>
       </c>
       <c r="L7" s="28" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O7" s="28">
         <f>F7+G7</f>
@@ -1488,13 +1494,13 @@
         <v>2</v>
       </c>
       <c r="K8" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O8" s="28">
         <f t="shared" si="0"/>
@@ -1533,13 +1539,13 @@
         <v>2</v>
       </c>
       <c r="K9" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L9" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M9" s="29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O9" s="28">
         <f t="shared" si="0"/>
@@ -1578,13 +1584,13 @@
         <v>2</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L10" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M10" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O10" s="28">
         <f t="shared" si="0"/>
@@ -1623,13 +1629,13 @@
         <v>2</v>
       </c>
       <c r="K11" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L11" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M11" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O11" s="28">
         <f>F11+G11</f>
@@ -1668,13 +1674,13 @@
         <v>2</v>
       </c>
       <c r="K12" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L12" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M12" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O12" s="31">
         <f t="shared" si="0"/>
@@ -1713,13 +1719,13 @@
         <v>2</v>
       </c>
       <c r="K13" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M13" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O13" s="31">
         <f t="shared" si="0"/>
@@ -1758,13 +1764,13 @@
         <v>2</v>
       </c>
       <c r="K14" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L14" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M14" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O14" s="31">
         <f t="shared" si="0"/>
@@ -1773,7 +1779,7 @@
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>22</v>
@@ -1797,13 +1803,13 @@
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M15" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O15" s="31">
         <f t="shared" si="0"/>
@@ -1842,13 +1848,13 @@
         <v>2</v>
       </c>
       <c r="K16" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="L16" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="L16" s="31" t="s">
-        <v>197</v>
-      </c>
       <c r="M16" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O16" s="31">
         <f t="shared" si="0"/>
@@ -1941,10 +1947,10 @@
         <v>113</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S1" s="13" t="s">
         <v>33</v>
@@ -2333,13 +2339,13 @@
         <v>148</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>151</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K7" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2393,22 +2399,22 @@
         <v>2</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>175</v>
-      </c>
       <c r="J8" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K8" s="22" t="str">
         <f t="shared" ref="K8:K11" si="2">E$1 &amp; ": " &amp; E8 &amp; CHAR(10)
@@ -2472,22 +2478,22 @@
         <v>2</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>139</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I9" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>181</v>
       </c>
       <c r="K9" s="22" t="str">
         <f t="shared" si="2"/>
@@ -2541,22 +2547,22 @@
         <v>2</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>145</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>145</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K10" s="22" t="str">
         <f t="shared" si="2"/>
@@ -2598,7 +2604,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" s="9">
         <v>2</v>
@@ -2613,16 +2619,16 @@
         <v>149</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>151</v>
@@ -2722,7 +2728,7 @@
         <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2770,10 +2776,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overhauls of skills, better skill backs
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="212">
   <si>
     <t>Name</t>
   </si>
@@ -438,9 +438,6 @@
     <t>Tinker</t>
   </si>
   <si>
-    <t>STUDY 💡💡</t>
-  </si>
-  <si>
     <t>Improvise</t>
   </si>
   <si>
@@ -450,21 +447,9 @@
     <t>Self-Defense</t>
   </si>
   <si>
-    <t>RUN! 🔊🔊➜➜</t>
-  </si>
-  <si>
     <t>Hurry</t>
   </si>
   <si>
-    <t>Zzzt. 📷🔊🔊➜</t>
-  </si>
-  <si>
-    <t>YANK! 💡💡💡🔊🔊</t>
-  </si>
-  <si>
-    <t>KICK! 👊🔊➜➜</t>
-  </si>
-  <si>
     <t>Skill1Ideas</t>
   </si>
   <si>
@@ -486,9 +471,6 @@
     <t>SLIPPERY%n2 free💡when escaping</t>
   </si>
   <si>
-    <t>EXTORT GUARDS%nGain $2k from first subdued guard.</t>
-  </si>
-  <si>
     <t>OBSERVANT%nAfter planning and before heist, may 🔍🔍</t>
   </si>
   <si>
@@ -504,32 +486,131 @@
     <t>DENIAL OF SERVICE%nOnce per heist, disconnect all known cameras, and lower alert by 1.</t>
   </si>
   <si>
-    <t xml:space="preserve"> 👊</t>
-  </si>
-  <si>
-    <t>SPRAY. 📷🔊➜</t>
-  </si>
-  <si>
     <t>Bypass</t>
   </si>
   <si>
-    <t>PICK. 🔓🔓➜➜</t>
-  </si>
-  <si>
-    <t>ROUNDHOUSE. 👊👊🔊🔊</t>
-  </si>
-  <si>
-    <t>JAB. 👊💡➜</t>
-  </si>
-  <si>
-    <t>CUT. 🔓🔊➜</t>
-  </si>
-  <si>
-    <t>SLINK.💡➜</t>
+    <t>$</t>
+  </si>
+  <si>
+    <t>Subdue 1 guard on or adjacent to your tile.</t>
+  </si>
+  <si>
+    <t>For a cost of $1k (on your person), may move into a space with a guard.</t>
+  </si>
+  <si>
+    <t>BOLT%nMay spend 💡for ➜</t>
+  </si>
+  <si>
+    <t>LOOTER%nGain $1k each time you take HESITATE.</t>
+  </si>
+  <si>
+    <t>Total Ideas</t>
+  </si>
+  <si>
+    <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires</t>
+  </si>
+  <si>
+    <t>COMMAND &amp; CONTROL%nMay spend 💡for 🔍, up to three times per turn.</t>
+  </si>
+  <si>
+    <t>REPORT IN%nWhen  👊, lower the noise level by 3. Do not change the ⚠ level.</t>
+  </si>
+  <si>
+    <t>DISGUISE%nMay spend 💡 to enter space with guards.</t>
+  </si>
+  <si>
+    <t>Default 1</t>
+  </si>
+  <si>
+    <t>Default 2</t>
+  </si>
+  <si>
+    <t>Walk 🔊➜</t>
+  </si>
+  <si>
+    <t>Crawl ➜</t>
+  </si>
+  <si>
+    <t>I CAN HAZ TEH CODES?%nOnce per turn, may  🔊🔊🔍.%nI CAN HEARTBLEED%nIf outdoors, may spend 💡💡 to 🔍</t>
+  </si>
+  <si>
+    <t>PICKER%nGain 💡 when you 🔓%nMASTER KEY%nWhen outdoors, may use  💡💡 to enable one player to 🔓</t>
+  </si>
+  <si>
+    <t>Saunter 🔊➜➜</t>
+  </si>
+  <si>
+    <t>Shimmy  🔊➜➜</t>
+  </si>
+  <si>
+    <t>Unplug%n📷🔊🔊➜</t>
+  </si>
+  <si>
+    <t>Run%n🔊🔊➜➜</t>
+  </si>
+  <si>
+    <t>Punch%n👊🔊🔊➜</t>
+  </si>
+  <si>
+    <t>Study%n💡💡</t>
+  </si>
+  <si>
+    <t>Examine%n💡💡💡🔊🔊</t>
+  </si>
+  <si>
+    <t>Reveal%n🔍</t>
+  </si>
+  <si>
+    <t>Hesitate%n💡</t>
+  </si>
+  <si>
+    <t>Smackdown 🔊👊</t>
+  </si>
+  <si>
+    <t>Kick%n👊🔊➜➜</t>
+  </si>
+  <si>
+    <t>Upgrade1</t>
+  </si>
+  <si>
+    <t>Upgrade2</t>
+  </si>
+  <si>
+    <t>Upgrade1Rolls</t>
+  </si>
+  <si>
+    <t>Upgrade2Rolls</t>
+  </si>
+  <si>
+    <t>Hesitate  💡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick  🔓 </t>
+  </si>
+  <si>
+    <t>Spy Stuff 🔓 👊</t>
+  </si>
+  <si>
+    <t>EXTORT GUARDS%nGain $1k from each subdued guard.</t>
+  </si>
+  <si>
+    <t>Spin Kick%n👊👊🔊🔊</t>
+  </si>
+  <si>
+    <t>Jab%n👊💡➜</t>
+  </si>
+  <si>
+    <t>Shim%n🔓🔊🔊➜</t>
+  </si>
+  <si>
+    <t>Rake%n🔓🔓🔊➜</t>
+  </si>
+  <si>
+    <t>Recon%n💡💡🔊🔍</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">BRIBE! </t>
+      <t>Bribe%n</t>
     </r>
     <r>
       <rPr>
@@ -554,144 +635,52 @@
     </r>
   </si>
   <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>Subdue 1 guard on or adjacent to your tile.</t>
-  </si>
-  <si>
-    <t>For a cost of $1k (on your person), may move into a space with a guard.</t>
-  </si>
-  <si>
-    <t>LOOP. 📷🔍</t>
-  </si>
-  <si>
-    <t>RECON! 💡💡🔊🔍</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">BRIBE </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">$ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>🔊➜</t>
-    </r>
-  </si>
-  <si>
-    <t>DEFEAT  🔓📷🔊➜</t>
-  </si>
-  <si>
-    <t>RAKE. 🔓🔓🔊➜</t>
-  </si>
-  <si>
-    <t>BOLT%nMay spend 💡for ➜</t>
-  </si>
-  <si>
-    <t>LOOTER%nGain $1k each time you take HESITATE.</t>
-  </si>
-  <si>
-    <t>Total Ideas</t>
-  </si>
-  <si>
-    <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires</t>
-  </si>
-  <si>
-    <t>COMMAND &amp; CONTROL%nMay spend 💡for 🔍, up to three times per turn.</t>
-  </si>
-  <si>
-    <t>REPORT IN%nWhen  👊, lower the noise level by 3. Do not change the ⚠ level.</t>
-  </si>
-  <si>
-    <t>DISGUISE%nMay spend 💡 to enter space with guards.</t>
-  </si>
-  <si>
-    <t>Default 1</t>
-  </si>
-  <si>
-    <t>Default 2</t>
-  </si>
-  <si>
-    <t>Walk 🔊➜</t>
-  </si>
-  <si>
-    <t>Crawl ➜</t>
-  </si>
-  <si>
-    <t>I CAN HAZ TEH CODES?%nOnce per turn, may  🔊🔊🔍.%nI CAN HEARTBLEED%nIf outdoors, may spend 💡💡 to 🔍</t>
-  </si>
-  <si>
-    <t>HESITATE  💡</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PICK  🔓 </t>
-  </si>
-  <si>
-    <t>PICKER%nGain 💡 when you 🔓%nMASTER KEY%nWhen outdoors, may use  💡💡 to enable one player to 🔓</t>
-  </si>
-  <si>
-    <t>Saunter 🔊➜➜</t>
-  </si>
-  <si>
-    <t>Shimmy  🔊➜➜</t>
-  </si>
-  <si>
-    <t>Unplug%n📷🔊🔊➜</t>
-  </si>
-  <si>
-    <t>Run%n🔊🔊➜➜</t>
-  </si>
-  <si>
-    <t>Punch%n👊🔊🔊➜</t>
-  </si>
-  <si>
-    <t>Study%n💡💡</t>
-  </si>
-  <si>
-    <t>Examine%n💡💡💡🔊🔊</t>
-  </si>
-  <si>
-    <t>Reveal%n🔍</t>
-  </si>
-  <si>
-    <t>Hesitate%n💡</t>
-  </si>
-  <si>
-    <t>Smackdown 🔊👊</t>
-  </si>
-  <si>
-    <t>Kick%n👊🔊➜➜</t>
-  </si>
-  <si>
-    <t>Rake%n🔓🔊🔊➜</t>
-  </si>
-  <si>
-    <t>Upgrade1</t>
-  </si>
-  <si>
-    <t>Upgrade2</t>
-  </si>
-  <si>
-    <t>Upgrade1Rolls</t>
-  </si>
-  <si>
-    <t>Upgrade2Rolls</t>
+    <t>Spray%n📷🔊➜</t>
+  </si>
+  <si>
+    <t>Slink%n💡➜</t>
+  </si>
+  <si>
+    <t>Loop%n📷🔍</t>
+  </si>
+  <si>
+    <t>Remote Exploit</t>
+  </si>
+  <si>
+    <t>Packet Sniff%n💡💡🔍🔍</t>
+  </si>
+  <si>
+    <t>Rampage%n👊👊🔊🔊➜➜</t>
+  </si>
+  <si>
+    <t>Redirect%n🔓👊📷🔊</t>
+  </si>
+  <si>
+    <t>Circumvent</t>
+  </si>
+  <si>
+    <t>Disable%n📷🔊➜</t>
+  </si>
+  <si>
+    <t>Pick%n🔓🔊➜</t>
+  </si>
+  <si>
+    <t>Sleeper Hold%n👊➜</t>
+  </si>
+  <si>
+    <t>Detonate. 🔓👊📷🔊🔊🔊➜</t>
+  </si>
+  <si>
+    <t>Sprint%n🔊🔊➜➜➜</t>
+  </si>
+  <si>
+    <t>Defeat%n🔓📷🔊➜</t>
+  </si>
+  <si>
+    <t>(none)</t>
+  </si>
+  <si>
+    <t>Sneak%n🔍➜➜</t>
   </si>
 </sst>
 </file>
@@ -741,11 +730,20 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -762,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -794,8 +792,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -824,16 +831,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1141,7 +1155,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,10 +1192,10 @@
         <v>16</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>25</v>
@@ -1193,10 +1207,10 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>135</v>
@@ -1205,674 +1219,674 @@
         <v>29</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="18">
-        <v>1</v>
-      </c>
-      <c r="D2" s="18">
-        <v>1</v>
-      </c>
-      <c r="E2" s="18">
+      <c r="C2" s="21">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21">
+        <v>1</v>
+      </c>
+      <c r="E2" s="21">
         <v>7</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="21">
         <v>3</v>
       </c>
-      <c r="G2" s="18">
-        <v>1</v>
-      </c>
-      <c r="H2" s="18">
-        <v>2</v>
-      </c>
-      <c r="I2" s="18">
-        <v>2</v>
-      </c>
-      <c r="J2" s="18">
-        <v>2</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="O2" s="18">
+      <c r="G2" s="21">
+        <v>1</v>
+      </c>
+      <c r="H2" s="21">
+        <v>2</v>
+      </c>
+      <c r="I2" s="21">
+        <v>2</v>
+      </c>
+      <c r="J2" s="21">
+        <v>2</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="O2" s="21">
         <f>F2+G2</f>
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="18">
-        <v>1</v>
-      </c>
-      <c r="D3" s="18">
-        <v>1</v>
-      </c>
-      <c r="E3" s="18">
+      <c r="C3" s="21">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21">
+        <v>1</v>
+      </c>
+      <c r="E3" s="21">
         <v>7</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="21">
         <v>3</v>
       </c>
-      <c r="G3" s="18">
-        <v>1</v>
-      </c>
-      <c r="H3" s="18">
-        <v>2</v>
-      </c>
-      <c r="I3" s="18">
-        <v>2</v>
-      </c>
-      <c r="J3" s="18">
-        <v>2</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="O3" s="18">
+      <c r="G3" s="21">
+        <v>1</v>
+      </c>
+      <c r="H3" s="21">
+        <v>2</v>
+      </c>
+      <c r="I3" s="21">
+        <v>2</v>
+      </c>
+      <c r="J3" s="21">
+        <v>2</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O3" s="21">
         <f t="shared" ref="O3:O16" si="0">F3+G3</f>
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="18">
-        <v>1</v>
-      </c>
-      <c r="D4" s="18">
-        <v>1</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="C4" s="21">
+        <v>1</v>
+      </c>
+      <c r="D4" s="21">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21">
         <v>9</v>
       </c>
-      <c r="F4" s="18">
-        <v>2</v>
-      </c>
-      <c r="G4" s="18">
-        <v>1</v>
-      </c>
-      <c r="H4" s="18">
-        <v>2</v>
-      </c>
-      <c r="I4" s="18">
-        <v>2</v>
-      </c>
-      <c r="J4" s="18">
-        <v>2</v>
-      </c>
-      <c r="K4" s="18" t="s">
+      <c r="F4" s="21">
+        <v>2</v>
+      </c>
+      <c r="G4" s="21">
+        <v>1</v>
+      </c>
+      <c r="H4" s="21">
+        <v>2</v>
+      </c>
+      <c r="I4" s="21">
+        <v>2</v>
+      </c>
+      <c r="J4" s="21">
+        <v>2</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="L4" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="O4" s="18">
+      <c r="M4" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="O4" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="18">
-        <v>1</v>
-      </c>
-      <c r="D5" s="18">
-        <v>1</v>
-      </c>
-      <c r="E5" s="18">
+      <c r="B5" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="21">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21">
         <v>8</v>
       </c>
-      <c r="F5" s="18">
-        <v>2</v>
-      </c>
-      <c r="G5" s="18">
-        <v>1</v>
-      </c>
-      <c r="H5" s="18">
-        <v>2</v>
-      </c>
-      <c r="I5" s="18">
-        <v>2</v>
-      </c>
-      <c r="J5" s="18">
-        <v>2</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="M5" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="O5" s="18">
+      <c r="F5" s="21">
+        <v>2</v>
+      </c>
+      <c r="G5" s="21">
+        <v>1</v>
+      </c>
+      <c r="H5" s="21">
+        <v>2</v>
+      </c>
+      <c r="I5" s="21">
+        <v>2</v>
+      </c>
+      <c r="J5" s="21">
+        <v>2</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="O5" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="18">
-        <v>1</v>
-      </c>
-      <c r="D6" s="18">
-        <v>1</v>
-      </c>
-      <c r="E6" s="18">
+      <c r="C6" s="21">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21">
+        <v>1</v>
+      </c>
+      <c r="E6" s="21">
         <v>6</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="21">
         <v>5</v>
       </c>
-      <c r="G6" s="18">
-        <v>1</v>
-      </c>
-      <c r="H6" s="18">
-        <v>2</v>
-      </c>
-      <c r="I6" s="18">
-        <v>2</v>
-      </c>
-      <c r="J6" s="18">
-        <v>2</v>
-      </c>
-      <c r="K6" s="18" t="s">
+      <c r="G6" s="21">
+        <v>1</v>
+      </c>
+      <c r="H6" s="21">
+        <v>2</v>
+      </c>
+      <c r="I6" s="21">
+        <v>2</v>
+      </c>
+      <c r="J6" s="21">
+        <v>2</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="L6" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="L6" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="O6" s="18">
+      <c r="M6" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="O6" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="21">
-        <v>1</v>
-      </c>
-      <c r="D7" s="21">
-        <v>2</v>
-      </c>
-      <c r="E7" s="21">
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>2</v>
+      </c>
+      <c r="E7" s="24">
         <v>8</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="24">
         <v>4</v>
       </c>
-      <c r="G7" s="21">
-        <v>2</v>
-      </c>
-      <c r="H7" s="21">
-        <v>2</v>
-      </c>
-      <c r="I7" s="21">
-        <v>2</v>
-      </c>
-      <c r="J7" s="21">
-        <v>2</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="O7" s="21">
+      <c r="G7" s="24">
+        <v>2</v>
+      </c>
+      <c r="H7" s="24">
+        <v>2</v>
+      </c>
+      <c r="I7" s="24">
+        <v>2</v>
+      </c>
+      <c r="J7" s="24">
+        <v>2</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="O7" s="24">
         <f>F7+G7</f>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="21">
-        <v>1</v>
-      </c>
-      <c r="D8" s="21">
-        <v>2</v>
-      </c>
-      <c r="E8" s="21">
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
+        <v>2</v>
+      </c>
+      <c r="E8" s="24">
         <v>7</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="24">
         <v>5</v>
       </c>
-      <c r="G8" s="21">
-        <v>2</v>
-      </c>
-      <c r="H8" s="21">
-        <v>2</v>
-      </c>
-      <c r="I8" s="21">
-        <v>2</v>
-      </c>
-      <c r="J8" s="21">
-        <v>2</v>
-      </c>
-      <c r="K8" s="21" t="s">
+      <c r="G8" s="24">
+        <v>2</v>
+      </c>
+      <c r="H8" s="24">
+        <v>2</v>
+      </c>
+      <c r="I8" s="24">
+        <v>2</v>
+      </c>
+      <c r="J8" s="24">
+        <v>2</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L8" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="L8" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="O8" s="21">
+      <c r="M8" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="O8" s="24">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="21">
-        <v>1</v>
-      </c>
-      <c r="D9" s="21">
-        <v>2</v>
-      </c>
-      <c r="E9" s="21">
+      <c r="C9" s="24">
+        <v>1</v>
+      </c>
+      <c r="D9" s="24">
+        <v>2</v>
+      </c>
+      <c r="E9" s="24">
         <v>8</v>
       </c>
-      <c r="F9" s="21">
-        <v>4</v>
-      </c>
-      <c r="G9" s="21">
-        <v>2</v>
-      </c>
-      <c r="H9" s="21">
-        <v>2</v>
-      </c>
-      <c r="I9" s="21">
-        <v>2</v>
-      </c>
-      <c r="J9" s="21">
-        <v>2</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="L9" s="21" t="s">
+      <c r="F9" s="24">
+        <v>2</v>
+      </c>
+      <c r="G9" s="24">
+        <v>1</v>
+      </c>
+      <c r="H9" s="24">
+        <v>2</v>
+      </c>
+      <c r="I9" s="24">
+        <v>2</v>
+      </c>
+      <c r="J9" s="24">
+        <v>2</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="O9" s="24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="24">
+        <v>1</v>
+      </c>
+      <c r="D10" s="24">
+        <v>2</v>
+      </c>
+      <c r="E10" s="24">
+        <v>7</v>
+      </c>
+      <c r="F10" s="24">
+        <v>3</v>
+      </c>
+      <c r="G10" s="24">
+        <v>3</v>
+      </c>
+      <c r="H10" s="24">
+        <v>2</v>
+      </c>
+      <c r="I10" s="24">
+        <v>2</v>
+      </c>
+      <c r="J10" s="24">
+        <v>2</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="M10" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="M9" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="O9" s="21">
+      <c r="O10" s="24">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="21">
-        <v>1</v>
-      </c>
-      <c r="D10" s="21">
-        <v>2</v>
-      </c>
-      <c r="E10" s="21">
+    <row r="11" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1</v>
+      </c>
+      <c r="D11" s="24">
+        <v>2</v>
+      </c>
+      <c r="E11" s="24">
         <v>7</v>
       </c>
-      <c r="F10" s="21">
-        <v>3</v>
-      </c>
-      <c r="G10" s="21">
-        <v>3</v>
-      </c>
-      <c r="H10" s="21">
-        <v>2</v>
-      </c>
-      <c r="I10" s="21">
-        <v>2</v>
-      </c>
-      <c r="J10" s="21">
-        <v>2</v>
-      </c>
-      <c r="K10" s="21" t="s">
+      <c r="F11" s="24">
+        <v>5</v>
+      </c>
+      <c r="G11" s="24">
+        <v>1</v>
+      </c>
+      <c r="H11" s="24">
+        <v>2</v>
+      </c>
+      <c r="I11" s="24">
+        <v>2</v>
+      </c>
+      <c r="J11" s="24">
+        <v>2</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L11" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="L10" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="M10" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="O10" s="21">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="21">
-        <v>1</v>
-      </c>
-      <c r="D11" s="21">
-        <v>2</v>
-      </c>
-      <c r="E11" s="21">
-        <v>7</v>
-      </c>
-      <c r="F11" s="21">
-        <v>5</v>
-      </c>
-      <c r="G11" s="21">
-        <v>1</v>
-      </c>
-      <c r="H11" s="21">
-        <v>2</v>
-      </c>
-      <c r="I11" s="21">
-        <v>2</v>
-      </c>
-      <c r="J11" s="21">
-        <v>2</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="L11" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="M11" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="O11" s="21">
+      <c r="M11" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="O11" s="24">
         <f>F11+G11</f>
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="24">
-        <v>1</v>
-      </c>
-      <c r="D12" s="24">
+      <c r="C12" s="27">
+        <v>1</v>
+      </c>
+      <c r="D12" s="27">
         <v>3</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="27">
         <v>9</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="27">
         <v>4</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="27">
         <v>4</v>
       </c>
-      <c r="H12" s="24">
-        <v>2</v>
-      </c>
-      <c r="I12" s="24">
-        <v>2</v>
-      </c>
-      <c r="J12" s="24">
-        <v>2</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="H12" s="27">
+        <v>2</v>
+      </c>
+      <c r="I12" s="27">
+        <v>2</v>
+      </c>
+      <c r="J12" s="27">
+        <v>2</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="L12" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="M12" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="O12" s="24">
+      <c r="M12" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="O12" s="27">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+    <row r="13" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="24">
-        <v>1</v>
-      </c>
-      <c r="D13" s="24">
+      <c r="C13" s="27">
+        <v>1</v>
+      </c>
+      <c r="D13" s="27">
         <v>3</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="27">
         <v>12</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="27">
         <v>5</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="27">
         <v>4</v>
       </c>
-      <c r="H13" s="24">
-        <v>2</v>
-      </c>
-      <c r="I13" s="24">
-        <v>2</v>
-      </c>
-      <c r="J13" s="24">
-        <v>2</v>
-      </c>
-      <c r="K13" s="24" t="s">
+      <c r="H13" s="27">
+        <v>2</v>
+      </c>
+      <c r="I13" s="27">
+        <v>2</v>
+      </c>
+      <c r="J13" s="27">
+        <v>2</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="L13" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="L13" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="M13" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="O13" s="24">
+      <c r="M13" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="O13" s="27">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="24">
-        <v>1</v>
-      </c>
-      <c r="D14" s="24">
+      <c r="C14" s="27">
+        <v>1</v>
+      </c>
+      <c r="D14" s="27">
         <v>3</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="27">
         <v>7</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="27">
         <v>7</v>
       </c>
-      <c r="G14" s="24">
-        <v>1</v>
-      </c>
-      <c r="H14" s="24">
-        <v>2</v>
-      </c>
-      <c r="I14" s="24">
-        <v>2</v>
-      </c>
-      <c r="J14" s="24">
-        <v>2</v>
-      </c>
-      <c r="K14" s="24" t="s">
+      <c r="G14" s="27">
+        <v>1</v>
+      </c>
+      <c r="H14" s="27">
+        <v>2</v>
+      </c>
+      <c r="I14" s="27">
+        <v>2</v>
+      </c>
+      <c r="J14" s="27">
+        <v>2</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="L14" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="L14" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="M14" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="O14" s="24">
+      <c r="M14" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="O14" s="27">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B15" s="23" t="s">
+    <row r="15" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="24">
-        <v>1</v>
-      </c>
-      <c r="D15" s="24">
+      <c r="C15" s="27">
+        <v>1</v>
+      </c>
+      <c r="D15" s="27">
         <v>3</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="27">
         <v>8</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="27">
         <v>4</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="27">
         <v>3</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24" t="s">
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="L15" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="L15" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="M15" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="O15" s="24">
+      <c r="M15" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="O15" s="27">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+    <row r="16" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="24">
-        <v>1</v>
-      </c>
-      <c r="D16" s="24">
+      <c r="C16" s="27">
+        <v>1</v>
+      </c>
+      <c r="D16" s="27">
         <v>3</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="27">
         <v>10</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="27">
         <v>4</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="27">
         <v>3</v>
       </c>
-      <c r="H16" s="24">
-        <v>2</v>
-      </c>
-      <c r="I16" s="24">
-        <v>2</v>
-      </c>
-      <c r="J16" s="24">
-        <v>2</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="M16" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="O16" s="24">
+      <c r="H16" s="27">
+        <v>2</v>
+      </c>
+      <c r="I16" s="27">
+        <v>2</v>
+      </c>
+      <c r="J16" s="27">
+        <v>2</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="O16" s="27">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1887,39 +1901,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="9" customWidth="1"/>
-    <col min="4" max="4" width="18" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" style="14" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="15" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="15" customWidth="1"/>
     <col min="15" max="15" width="3.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="3.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.7109375" style="9" customWidth="1"/>
-    <col min="21" max="21" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="16"/>
+    <col min="20" max="21" width="3.7109375" style="9" customWidth="1"/>
+    <col min="22" max="22" width="2.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1951,16 +1968,16 @@
         <v>62</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>206</v>
+        <v>182</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>207</v>
+        <v>183</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>116</v>
@@ -1975,21 +1992,24 @@
         <v>112</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="U1" s="11" t="s">
-        <v>169</v>
+      <c r="U1" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="V1" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="W1" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>139</v>
+    <row r="2" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="B2" s="8">
         <v>2</v>
@@ -1998,24 +2018,24 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="J2" s="14" t="str">
+        <v>174</v>
+      </c>
+      <c r="J2" s="15" t="str">
         <f>D$1 &amp; ": " &amp; D2 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E2 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
@@ -2024,7 +2044,7 @@
 &amp; I$1 &amp; ": " &amp; I2 &amp; CHAR(10)</f>
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Unplug%n📷🔊🔊➜
-3: Rake%n🔓🔊🔊➜
+3: Shim%n🔓🔊🔊➜
 4: Punch%n👊🔊🔊➜
 5: Study%n💡💡
 6: Run%n🔊🔊➜➜
@@ -2033,41 +2053,31 @@
       <c r="K2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="8" t="str">
-        <f>D$1 &amp; ": " &amp; D9 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E9 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G9 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H9 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I9 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: DEFEAT  🔓📷🔊➜
-2: BRIBE $ 🔊➜
-3: STUDY 💡💡
-4: BRIBE $ 🔊➜
-5: RECON! 💡💡🔊🔍
-6: BRIBE $ 🔊➜
+      <c r="L2" s="16" t="str">
+        <f>VLOOKUP(K2,$A$7:$J$11,10,FALSE)</f>
+        <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
+2: Bribe%n$ 🔊➜
+3: Study%n💡💡
+4: Bribe%n$ 🔊➜
+5: Recon%n💡💡🔊🔍
+6: Bribe%n$ 🔊➜
 </v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="N2" s="14" t="str">
-        <f>D$1 &amp; ": " &amp; D11 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E11 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F11 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G11 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H11 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I11 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: YANK! 💡💡💡🔊🔊
-2: PICK. 🔓🔓➜➜
-3: BRIBE $ 🔊➜
-4: RAKE. 🔓🔓🔊➜
-5: LOOP. 📷🔍
-6: KICK! 👊🔊➜➜
+        <v>154</v>
+      </c>
+      <c r="N2" s="15" t="str">
+        <f>VLOOKUP(M2,$A$7:$J$11,10,FALSE)</f>
+        <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
+2: Rake%n🔓🔓🔊➜
+3: Bribe%n$ 🔊➜
+4: Rake%n🔓🔓🔊➜
+5: Loop%n📷🔍
+6: Punch%n👊🔊🔊➜
 </v>
       </c>
       <c r="O2" s="8">
-        <f t="shared" ref="O2:U11" si="0">(LEN($D2)-LEN(SUBSTITUTE($D2,O$1,"")))/LEN(O$1) +
+        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,O$1,"")))/LEN(O$1) +
 (LEN($E2)-LEN(SUBSTITUTE($E2,O$1,"")))/LEN(O$1) +
 (LEN($F2)-LEN(SUBSTITUTE($F2,O$1,"")))/LEN(O$1) +
 (LEN($G2)-LEN(SUBSTITUTE($G2,O$1,"")))/LEN(O$1) +
@@ -2085,29 +2095,63 @@
         <v>10</v>
       </c>
       <c r="Q2" s="8">
-        <f t="shared" si="0"/>
+        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,Q$1,"")))/LEN(Q$1) +
+(LEN($E2)-LEN(SUBSTITUTE($E2,Q$1,"")))/LEN(Q$1) +
+(LEN($F2)-LEN(SUBSTITUTE($F2,Q$1,"")))/LEN(Q$1) +
+(LEN($G2)-LEN(SUBSTITUTE($G2,Q$1,"")))/LEN(Q$1) +
+(LEN($H2)-LEN(SUBSTITUTE($H2,Q$1,"")))/LEN(Q$1) +
+(LEN($I2)-LEN(SUBSTITUTE($I2,Q$1,"")))/LEN(Q$1)</f>
         <v>7</v>
       </c>
       <c r="R2" s="8">
-        <f t="shared" si="0"/>
+        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,R$1,"")))/LEN(R$1) +
+(LEN($E2)-LEN(SUBSTITUTE($E2,R$1,"")))/LEN(R$1) +
+(LEN($F2)-LEN(SUBSTITUTE($F2,R$1,"")))/LEN(R$1) +
+(LEN($G2)-LEN(SUBSTITUTE($G2,R$1,"")))/LEN(R$1) +
+(LEN($H2)-LEN(SUBSTITUTE($H2,R$1,"")))/LEN(R$1) +
+(LEN($I2)-LEN(SUBSTITUTE($I2,R$1,"")))/LEN(R$1)</f>
         <v>1</v>
       </c>
       <c r="S2" s="8">
-        <f t="shared" si="0"/>
+        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,S$1,"")))/LEN(S$1) +
+(LEN($E2)-LEN(SUBSTITUTE($E2,S$1,"")))/LEN(S$1) +
+(LEN($F2)-LEN(SUBSTITUTE($F2,S$1,"")))/LEN(S$1) +
+(LEN($G2)-LEN(SUBSTITUTE($G2,S$1,"")))/LEN(S$1) +
+(LEN($H2)-LEN(SUBSTITUTE($H2,S$1,"")))/LEN(S$1) +
+(LEN($I2)-LEN(SUBSTITUTE($I2,S$1,"")))/LEN(S$1)</f>
+        <v>1</v>
+      </c>
+      <c r="T2" s="8">
+        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,T$1,"")))/LEN(T$1) +
+(LEN($E2)-LEN(SUBSTITUTE($E2,T$1,"")))/LEN(T$1) +
+(LEN($F2)-LEN(SUBSTITUTE($F2,T$1,"")))/LEN(T$1) +
+(LEN($G2)-LEN(SUBSTITUTE($G2,T$1,"")))/LEN(T$1) +
+(LEN($H2)-LEN(SUBSTITUTE($H2,T$1,"")))/LEN(T$1) +
+(LEN($I2)-LEN(SUBSTITUTE($I2,T$1,"")))/LEN(T$1)</f>
+        <v>1</v>
+      </c>
+      <c r="U2" s="8">
+        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,U$1,"")))/LEN(U$1) +
+(LEN($E2)-LEN(SUBSTITUTE($E2,U$1,"")))/LEN(U$1) +
+(LEN($F2)-LEN(SUBSTITUTE($F2,U$1,"")))/LEN(U$1) +
+(LEN($G2)-LEN(SUBSTITUTE($G2,U$1,"")))/LEN(U$1) +
+(LEN($H2)-LEN(SUBSTITUTE($H2,U$1,"")))/LEN(U$1) +
+(LEN($I2)-LEN(SUBSTITUTE($I2,U$1,"")))/LEN(U$1)</f>
         <v>0</v>
       </c>
-      <c r="T2" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="U2" s="8">
-        <f t="shared" si="0"/>
+      <c r="V2" s="8">
+        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,V$1,"")))/LEN(V$1) +
+(LEN($E2)-LEN(SUBSTITUTE($E2,V$1,"")))/LEN(V$1) +
+(LEN($F2)-LEN(SUBSTITUTE($F2,V$1,"")))/LEN(V$1) +
+(LEN($G2)-LEN(SUBSTITUTE($G2,V$1,"")))/LEN(V$1) +
+(LEN($H2)-LEN(SUBSTITUTE($H2,V$1,"")))/LEN(V$1) +
+(LEN($I2)-LEN(SUBSTITUTE($I2,V$1,"")))/LEN(V$1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>140</v>
+    <row r="3" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>139</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
@@ -2116,24 +2160,24 @@
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="J3" s="14" t="str">
+        <v>173</v>
+      </c>
+      <c r="J3" s="15" t="str">
         <f>D$1 &amp; ": " &amp; D3 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E3 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F3 &amp; CHAR(10)
@@ -2142,84 +2186,78 @@
 &amp; I$1 &amp; ": " &amp; I3 &amp; CHAR(10)</f>
         <v xml:space="preserve">1: Punch%n👊🔊🔊➜
 2: Hesitate%n💡
-3: Rake%n🔓🔊🔊➜
+3: Shim%n🔓🔊🔊➜
 4: Hesitate%n💡
-5: Rake%n🔓🔊🔊➜
+5: Shim%n🔓🔊🔊➜
 6: Unplug%n📷🔊🔊➜
 </v>
       </c>
       <c r="K3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="9" t="str">
-        <f>D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E7 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F7 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G7 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H7 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I7 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: Zzzt. 📷🔊🔊➜
+      <c r="L3" s="15" t="str">
+        <f t="shared" ref="L3:L6" si="0">VLOOKUP(K3,$A$7:$J$11,10,FALSE)</f>
+        <v xml:space="preserve">1: Unplug%n📷🔊🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
-4: ROUNDHOUSE. 👊👊🔊🔊
-5: KICK! 👊🔊➜➜
-6: JAB. 👊💡➜
+4: Spin Kick%n👊👊🔊🔊
+5: Kick%n👊🔊➜➜
+6: Jab%n👊💡➜
 </v>
       </c>
       <c r="M3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="8" t="str">
-        <f>F$1 &amp; ": " &amp; F10 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G10 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H10 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I10 &amp; CHAR(10)
-&amp; J$1 &amp; ": " &amp; J10 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K10 &amp; CHAR(10)</f>
-        <v xml:space="preserve">3: RUN! 🔊🔊➜➜
-4: LOOP. 📷🔍
-5: RUN! 🔊🔊➜➜
-6: CUT. 🔓🔊➜
-Rolls: 1: RECON! 💡💡🔊🔍
-2: LOOP. 📷🔍
-3: RUN! 🔊🔊➜➜
-4: LOOP. 📷🔍
-5: RUN! 🔊🔊➜➜
-6: CUT. 🔓🔊➜
-Upgrade1: 
+      <c r="N3" s="16" t="str">
+        <f t="shared" ref="N3:N6" si="1">VLOOKUP(M3,$A$7:$J$11,10,FALSE)</f>
+        <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
+2: Bribe%n$ 🔊➜
+3: Study%n💡💡
+4: Bribe%n$ 🔊➜
+5: Recon%n💡💡🔊🔍
+6: Bribe%n$ 🔊➜
 </v>
       </c>
       <c r="O3" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="O3:V16" si="2">(LEN($D3)-LEN(SUBSTITUTE($D3,O$1,"")))/LEN(O$1) +
+(LEN($E3)-LEN(SUBSTITUTE($E3,O$1,"")))/LEN(O$1) +
+(LEN($F3)-LEN(SUBSTITUTE($F3,O$1,"")))/LEN(O$1) +
+(LEN($G3)-LEN(SUBSTITUTE($G3,O$1,"")))/LEN(O$1) +
+(LEN($H3)-LEN(SUBSTITUTE($H3,O$1,"")))/LEN(O$1) +
+(LEN($I3)-LEN(SUBSTITUTE($I3,O$1,"")))/LEN(O$1)</f>
         <v>2</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Q3" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="R3" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S3" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T3" s="8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U3" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T3" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="U3" s="8">
-        <f t="shared" si="0"/>
+      <c r="V3" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>137</v>
       </c>
       <c r="B4" s="8">
@@ -2229,24 +2267,24 @@
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="J4" s="14" t="str">
+        <v>192</v>
+      </c>
+      <c r="J4" s="15" t="str">
         <f>D$1 &amp; ": " &amp; D4 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E4 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F4 &amp; CHAR(10)
@@ -2258,77 +2296,71 @@
 3: Reveal%n🔍
 4: Examine%n💡💡💡🔊🔊
 5: Unplug%n📷🔊🔊➜
-6: Rake%n🔓🔊🔊➜
+6: Shim%n🔓🔊🔊➜
 </v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="L4" s="14" t="str">
-        <f>D$1 &amp; ": " &amp; D11 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E11 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F11 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G11 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H11 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I11 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: YANK! 💡💡💡🔊🔊
-2: PICK. 🔓🔓➜➜
-3: BRIBE $ 🔊➜
-4: RAKE. 🔓🔓🔊➜
-5: LOOP. 📷🔍
-6: KICK! 👊🔊➜➜
+        <v>154</v>
+      </c>
+      <c r="L4" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
+2: Rake%n🔓🔓🔊➜
+3: Bribe%n$ 🔊➜
+4: Rake%n🔓🔓🔊➜
+5: Loop%n📷🔍
+6: Punch%n👊🔊🔊➜
 </v>
       </c>
       <c r="M4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="14" t="str">
-        <f>D$1 &amp; ": " &amp; D10 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E10 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F10 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G10 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H10 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I10 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: RECON! 💡💡🔊🔍
-2: LOOP. 📷🔍
-3: RUN! 🔊🔊➜➜
-4: LOOP. 📷🔍
-5: RUN! 🔊🔊➜➜
-6: CUT. 🔓🔊➜
+      <c r="N4" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">1: Recon%n💡💡🔊🔍
+2: Loop%n📷🔍
+3: Run%n🔊🔊➜➜
+4: Loop%n📷🔍
+5: Run%n🔊🔊➜➜
+6: Rake%n🔓🔓🔊➜
 </v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Q4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="R4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V4" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>141</v>
+    <row r="5" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>140</v>
       </c>
       <c r="B5" s="8">
         <v>2</v>
@@ -2337,24 +2369,24 @@
         <v>1</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="J5" s="14" t="str">
+        <v>175</v>
+      </c>
+      <c r="J5" s="15" t="str">
         <f>D$1 &amp; ": " &amp; D5 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E5 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F5 &amp; CHAR(10)
@@ -2372,102 +2404,91 @@
       <c r="K5" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="8" t="str">
-        <f>D$1 &amp; ": " &amp; D8 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E8 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F8 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G8 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H8 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I8 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: SPRAY. 📷🔊➜
-2: CUT. 🔓🔊➜
-3: SPRAY. 📷🔊➜
-4: SLINK.💡➜
-5: BRIBE! $ 🔊➜
-6: SLINK.💡➜
+      <c r="L5" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: Spray%n📷🔊➜
+2: Rake%n🔓🔓🔊➜
+3: Spray%n📷🔊➜
+4: Slink%n💡➜
+5: Bribe%n$ 🔊➜
+6: Slink%n💡➜
 </v>
       </c>
       <c r="M5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="9" t="str">
-        <f>F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G9 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H9 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I9 &amp; CHAR(10)
-&amp; J$1 &amp; ": " &amp; J9 &amp; CHAR(10)
-&amp; K$1 &amp; ": " &amp; K9 &amp; CHAR(10)</f>
-        <v xml:space="preserve">3: STUDY 💡💡
-4: BRIBE $ 🔊➜
-5: RECON! 💡💡🔊🔍
-6: BRIBE $ 🔊➜
-Rolls: 1: DEFEAT  🔓📷🔊➜
-2: BRIBE $ 🔊➜
-3: STUDY 💡💡
-4: BRIBE $ 🔊➜
-5: RECON! 💡💡🔊🔍
-6: BRIBE $ 🔊➜
-Upgrade1: 
+      <c r="N5" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">1: Unplug%n📷🔊🔊➜
+2: Run%n🔊🔊➜➜
+3: Punch%n👊🔊🔊➜
+4: Spin Kick%n👊👊🔊🔊
+5: Kick%n👊🔊➜➜
+6: Jab%n👊💡➜
 </v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="Q5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="T5" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T5" s="8">
-        <f t="shared" si="0"/>
+      <c r="U5" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U5" s="8">
-        <f t="shared" si="0"/>
+      <c r="V5" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="29">
-        <v>2</v>
-      </c>
-      <c r="C6" s="29">
-        <v>1</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="J6" s="30" t="str">
+    <row r="6" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="32">
+        <v>2</v>
+      </c>
+      <c r="C6" s="32">
+        <v>1</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="J6" s="34" t="str">
         <f>D$1 &amp; ": " &amp; D6 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E6 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F6 &amp; CHAR(10)
@@ -2477,459 +2498,1061 @@
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Hesitate%n💡
 3: Run%n🔊🔊➜➜
-4: Rake%n🔓🔊🔊➜
+4: Shim%n🔓🔊🔊➜
 5: Hesitate%n💡
 6: Run%n🔊🔊➜➜
 </v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="28" t="str">
+      <c r="L6" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">1: Recon%n💡💡🔊🔍
+2: Loop%n📷🔍
+3: Run%n🔊🔊➜➜
+4: Loop%n📷🔍
+5: Run%n🔊🔊➜➜
+6: Rake%n🔓🔓🔊➜
+</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">1: Spray%n📷🔊➜
+2: Rake%n🔓🔓🔊➜
+3: Spray%n📷🔊➜
+4: Slink%n💡➜
+5: Bribe%n$ 🔊➜
+6: Slink%n💡➜
+</v>
+      </c>
+      <c r="O6" s="32">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P6" s="32">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Q6" s="32">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="R6" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U6" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="J7" s="18" t="str">
+        <f>D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
+&amp; E$1 &amp; ": " &amp; E7 &amp; CHAR(10)
+&amp; F$1 &amp; ": " &amp; F7 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G7 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H7 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I7 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: Unplug%n📷🔊🔊➜
+2: Run%n🔊🔊➜➜
+3: Punch%n👊🔊🔊➜
+4: Spin Kick%n👊👊🔊🔊
+5: Kick%n👊🔊➜➜
+6: Jab%n👊💡➜
+</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="30" t="str">
+        <f>VLOOKUP(K7,$A$12:$J$16,10,FALSE)</f>
+        <v xml:space="preserve">1: Sneak%n🔍➜➜
+2: Sleeper Hold%n👊➜
+3: Slink%n💡➜
+4: Sleeper Hold%n👊➜
+5: Sneak%n🔍➜➜
+6: Defeat%n🔓📷🔊➜
+</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="N7" s="18" t="str">
+        <f>VLOOKUP(M7,$A$12:$J$16,10,FALSE)</f>
+        <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
+2: Sprint%n🔊🔊➜➜➜
+3: Slink%n💡➜
+4: Rampage%n👊👊🔊🔊➜➜
+5: Detonate. 🔓👊📷🔊🔊🔊➜
+6: Jab%n👊💡➜
+</v>
+      </c>
+      <c r="O7" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P7" s="10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="Q7" s="10">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S7" s="10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="T7" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="9">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="J8" s="18" t="str">
+        <f>D$1 &amp; ": " &amp; D8 &amp; CHAR(10)
+&amp; E$1 &amp; ": " &amp; E8 &amp; CHAR(10)
+&amp; F$1 &amp; ": " &amp; F8 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G8 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H8 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I8 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: Spray%n📷🔊➜
+2: Rake%n🔓🔓🔊➜
+3: Spray%n📷🔊➜
+4: Slink%n💡➜
+5: Bribe%n$ 🔊➜
+6: Slink%n💡➜
+</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="30" t="str">
+        <f t="shared" ref="L8:L11" si="3">VLOOKUP(K8,$A$12:$J$16,10,FALSE)</f>
+        <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
+2: Slink%n💡➜
+3: Redirect%n🔓👊📷🔊
+4: Sneak%n🔍➜➜
+5: Jab%n👊💡➜
+6: Examine%n💡💡💡🔊🔊
+</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="18" t="str">
+        <f t="shared" ref="N8:N11" si="4">VLOOKUP(M8,$A$12:$J$16,10,FALSE)</f>
+        <v xml:space="preserve">1: Sneak%n🔍➜➜
+2: Sleeper Hold%n👊➜
+3: Slink%n💡➜
+4: Sleeper Hold%n👊➜
+5: Sneak%n🔍➜➜
+6: Defeat%n🔓📷🔊➜
+</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" ref="O8:V8" si="5">(LEN($D8)-LEN(SUBSTITUTE($D8,O$1,"")))/LEN(O$1) +
+(LEN($E8)-LEN(SUBSTITUTE($E8,O$1,"")))/LEN(O$1) +
+(LEN($F8)-LEN(SUBSTITUTE($F8,O$1,"")))/LEN(O$1) +
+(LEN($G8)-LEN(SUBSTITUTE($G8,O$1,"")))/LEN(O$1) +
+(LEN($H8)-LEN(SUBSTITUTE($H8,O$1,"")))/LEN(O$1) +
+(LEN($I8)-LEN(SUBSTITUTE($I8,O$1,"")))/LEN(O$1)</f>
+        <v>2</v>
+      </c>
+      <c r="P8" s="8">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="Q8" s="8">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="R8" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U8" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="J9" s="18" t="str">
+        <f>D$1 &amp; ": " &amp; D9 &amp; CHAR(10)
+&amp; E$1 &amp; ": " &amp; E9 &amp; CHAR(10)
+&amp; F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G9 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H9 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I9 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
+2: Bribe%n$ 🔊➜
+3: Study%n💡💡
+4: Bribe%n$ 🔊➜
+5: Recon%n💡💡🔊🔍
+6: Bribe%n$ 🔊➜
+</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="L9" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">1: Run%n🔊🔊➜➜
+2: Disable%n📷🔊➜
+3: Pick%n🔓🔊➜
+4: Jab%n👊💡➜
+5: Reveal%n🔍
+6: Punch%n👊🔊🔊➜
+</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
+2: Slink%n💡➜
+3: Redirect%n🔓👊📷🔊
+4: Sneak%n🔍➜➜
+5: Jab%n👊💡➜
+6: Examine%n💡💡💡🔊🔊
+</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="P9" s="8">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="Q9" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="R9" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S9" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U9" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V9" s="8">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="J10" s="18" t="str">
         <f>D$1 &amp; ": " &amp; D10 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E10 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F10 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G10 &amp; CHAR(10)
 &amp; H$1 &amp; ": " &amp; H10 &amp; CHAR(10)
 &amp; I$1 &amp; ": " &amp; I10 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: RECON! 💡💡🔊🔍
-2: LOOP. 📷🔍
-3: RUN! 🔊🔊➜➜
-4: LOOP. 📷🔍
-5: RUN! 🔊🔊➜➜
-6: CUT. 🔓🔊➜
+        <v xml:space="preserve">1: Recon%n💡💡🔊🔍
+2: Loop%n📷🔍
+3: Run%n🔊🔊➜➜
+4: Loop%n📷🔍
+5: Run%n🔊🔊➜➜
+6: Rake%n🔓🔓🔊➜
 </v>
       </c>
-      <c r="M6" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="N6" s="30" t="str">
-        <f>D$1 &amp; ": " &amp; D8 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E8 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F8 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G8 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H8 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I8 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: SPRAY. 📷🔊➜
-2: CUT. 🔓🔊➜
-3: SPRAY. 📷🔊➜
-4: SLINK.💡➜
-5: BRIBE! $ 🔊➜
-6: SLINK.💡➜
+      <c r="K10" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="L10" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
+2: Hesitate%n💡
+3: Loop%n📷🔍
+4: Redirect%n🔓👊📷🔊
+5: Packet Sniff%n💡💡🔍🔍
+6: Hesitate%n💡
 </v>
       </c>
-      <c r="O6" s="29">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="P6" s="29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Q6" s="29">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R6" s="29">
-        <f t="shared" si="0"/>
+      <c r="M10" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N10" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">1: Run%n🔊🔊➜➜
+2: Disable%n📷🔊➜
+3: Pick%n🔓🔊➜
+4: Jab%n👊💡➜
+5: Reveal%n🔍
+6: Punch%n👊🔊🔊➜
+</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P10" s="8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="Q10" s="8">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="R10" s="8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="S10" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S6" s="29">
-        <f t="shared" si="0"/>
+      <c r="T10" s="8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U10" s="8">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="V10" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T6" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="U6" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="10">
-        <v>2</v>
-      </c>
-      <c r="C7" s="10">
-        <v>2</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="8" t="s">
+    </row>
+    <row r="11" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="33">
+        <v>2</v>
+      </c>
+      <c r="C11" s="33">
+        <v>2</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="F11" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="J7" s="15" t="str">
-        <f>D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E7 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F7 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G7 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H7 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I7 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: Zzzt. 📷🔊🔊➜
-2: Run%n🔊🔊➜➜
-3: Punch%n👊🔊🔊➜
-4: ROUNDHOUSE. 👊👊🔊🔊
-5: KICK! 👊🔊➜➜
-6: JAB. 👊💡➜
-</v>
-      </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P7" s="10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="Q7" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R7" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S7" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T7" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U7" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J8" s="15" t="str">
-        <f>D$1 &amp; ": " &amp; D8 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E8 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F8 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G8 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H8 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I8 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: SPRAY. 📷🔊➜
-2: CUT. 🔓🔊➜
-3: SPRAY. 📷🔊➜
-4: SLINK.💡➜
-5: BRIBE! $ 🔊➜
-6: SLINK.💡➜
-</v>
-      </c>
-      <c r="N8" s="15"/>
-      <c r="O8" s="8">
-        <f t="shared" ref="O8:U8" si="1">(LEN($D8)-LEN(SUBSTITUTE($D8,O$1,"")))/LEN(O$1) +
-(LEN($E8)-LEN(SUBSTITUTE($E8,O$1,"")))/LEN(O$1) +
-(LEN($F8)-LEN(SUBSTITUTE($F8,O$1,"")))/LEN(O$1) +
-(LEN($G8)-LEN(SUBSTITUTE($G8,O$1,"")))/LEN(O$1) +
-(LEN($H8)-LEN(SUBSTITUTE($H8,O$1,"")))/LEN(O$1) +
-(LEN($I8)-LEN(SUBSTITUTE($I8,O$1,"")))/LEN(O$1)</f>
-        <v>2</v>
-      </c>
-      <c r="P8" s="8">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q8" s="8">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="R8" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="S8" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T8" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="U8" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="9">
-        <v>2</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="G11" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="I11" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="J9" s="15" t="str">
-        <f>D$1 &amp; ": " &amp; D9 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E9 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G9 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H9 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I9 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: DEFEAT  🔓📷🔊➜
-2: BRIBE $ 🔊➜
-3: STUDY 💡💡
-4: BRIBE $ 🔊➜
-5: RECON! 💡💡🔊🔍
-6: BRIBE $ 🔊➜
-</v>
-      </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="P9" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q9" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R9" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S9" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T9" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="U9" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="9">
-        <v>2</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="J10" s="15" t="str">
-        <f>D$1 &amp; ": " &amp; D10 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E10 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F10 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G10 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H10 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I10 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: RECON! 💡💡🔊🔍
-2: LOOP. 📷🔍
-3: RUN! 🔊🔊➜➜
-4: LOOP. 📷🔍
-5: RUN! 🔊🔊➜➜
-6: CUT. 🔓🔊➜
-</v>
-      </c>
-      <c r="N10" s="15"/>
-      <c r="O10" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="P10" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="Q10" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="R10" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="S10" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T10" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="U10" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" s="9">
-        <v>2</v>
-      </c>
-      <c r="C11" s="9">
-        <v>2</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="J11" s="15" t="str">
+      <c r="J11" s="18" t="str">
         <f>D$1 &amp; ": " &amp; D11 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E11 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F11 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G11 &amp; CHAR(10)
 &amp; H$1 &amp; ": " &amp; H11 &amp; CHAR(10)
 &amp; I$1 &amp; ": " &amp; I11 &amp; CHAR(10)</f>
-        <v xml:space="preserve">1: YANK! 💡💡💡🔊🔊
-2: PICK. 🔓🔓➜➜
-3: BRIBE $ 🔊➜
-4: RAKE. 🔓🔓🔊➜
-5: LOOP. 📷🔍
-6: KICK! 👊🔊➜➜
+        <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
+2: Rake%n🔓🔓🔊➜
+3: Bribe%n$ 🔊➜
+4: Rake%n🔓🔓🔊➜
+5: Loop%n📷🔍
+6: Punch%n👊🔊🔊➜
 </v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="8">
-        <f t="shared" si="0"/>
+      <c r="K11" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" s="35" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
+2: Sprint%n🔊🔊➜➜➜
+3: Slink%n💡➜
+4: Rampage%n👊👊🔊🔊➜➜
+5: Detonate. 🔓👊📷🔊🔊🔊➜
+6: Jab%n👊💡➜
+</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="N11" s="34" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
+2: Hesitate%n💡
+3: Loop%n📷🔍
+4: Redirect%n🔓👊📷🔊
+5: Packet Sniff%n💡💡🔍🔍
+6: Hesitate%n💡
+</v>
+      </c>
+      <c r="O11" s="32">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="P11" s="8">
-        <f t="shared" si="0"/>
+      <c r="P11" s="32">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="Q11" s="32">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="R11" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S11" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T11" s="32">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="U11" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V11" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>3</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="J12" s="17" t="str">
+        <f t="shared" ref="J12:J16" si="6">D$1 &amp; ": " &amp; D12 &amp; CHAR(10)
+&amp; E$1 &amp; ": " &amp; E12 &amp; CHAR(10)
+&amp; F$1 &amp; ": " &amp; F12 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G12 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H12 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I12 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
+2: Sprint%n🔊🔊➜➜➜
+3: Slink%n💡➜
+4: Rampage%n👊👊🔊🔊➜➜
+5: Detonate. 🔓👊📷🔊🔊🔊➜
+6: Jab%n👊💡➜
+</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="O12" s="10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P12" s="10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Q12" s="10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="R12" s="10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="S12" s="10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="T12" s="10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U12" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>3</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="J13" s="18" t="str">
+        <f>D$1 &amp; ": " &amp; D13 &amp; CHAR(10)
+&amp; E$1 &amp; ": " &amp; E13 &amp; CHAR(10)
+&amp; F$1 &amp; ": " &amp; F13 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G13 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H13 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I13 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: Sneak%n🔍➜➜
+2: Sleeper Hold%n👊➜
+3: Slink%n💡➜
+4: Sleeper Hold%n👊➜
+5: Sneak%n🔍➜➜
+6: Defeat%n🔓📷🔊➜
+</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="O13" s="10">
+        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,O$1,"")))/LEN(O$1) +
+(LEN($E13)-LEN(SUBSTITUTE($E13,O$1,"")))/LEN(O$1) +
+(LEN($F13)-LEN(SUBSTITUTE($F13,O$1,"")))/LEN(O$1) +
+(LEN($G13)-LEN(SUBSTITUTE($G13,O$1,"")))/LEN(O$1) +
+(LEN($H13)-LEN(SUBSTITUTE($H13,O$1,"")))/LEN(O$1) +
+(LEN($I13)-LEN(SUBSTITUTE($I13,O$1,"")))/LEN(O$1)</f>
+        <v>1</v>
+      </c>
+      <c r="P13" s="10">
+        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,P$1,"")))/LEN(P$1) +
+(LEN($E13)-LEN(SUBSTITUTE($E13,P$1,"")))/LEN(P$1) +
+(LEN($F13)-LEN(SUBSTITUTE($F13,P$1,"")))/LEN(P$1) +
+(LEN($G13)-LEN(SUBSTITUTE($G13,P$1,"")))/LEN(P$1) +
+(LEN($H13)-LEN(SUBSTITUTE($H13,P$1,"")))/LEN(P$1) +
+(LEN($I13)-LEN(SUBSTITUTE($I13,P$1,"")))/LEN(P$1)</f>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="10">
+        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,Q$1,"")))/LEN(Q$1) +
+(LEN($E13)-LEN(SUBSTITUTE($E13,Q$1,"")))/LEN(Q$1) +
+(LEN($F13)-LEN(SUBSTITUTE($F13,Q$1,"")))/LEN(Q$1) +
+(LEN($G13)-LEN(SUBSTITUTE($G13,Q$1,"")))/LEN(Q$1) +
+(LEN($H13)-LEN(SUBSTITUTE($H13,Q$1,"")))/LEN(Q$1) +
+(LEN($I13)-LEN(SUBSTITUTE($I13,Q$1,"")))/LEN(Q$1)</f>
+        <v>8</v>
+      </c>
+      <c r="R13" s="10">
+        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,R$1,"")))/LEN(R$1) +
+(LEN($E13)-LEN(SUBSTITUTE($E13,R$1,"")))/LEN(R$1) +
+(LEN($F13)-LEN(SUBSTITUTE($F13,R$1,"")))/LEN(R$1) +
+(LEN($G13)-LEN(SUBSTITUTE($G13,R$1,"")))/LEN(R$1) +
+(LEN($H13)-LEN(SUBSTITUTE($H13,R$1,"")))/LEN(R$1) +
+(LEN($I13)-LEN(SUBSTITUTE($I13,R$1,"")))/LEN(R$1)</f>
+        <v>1</v>
+      </c>
+      <c r="S13" s="10">
+        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,S$1,"")))/LEN(S$1) +
+(LEN($E13)-LEN(SUBSTITUTE($E13,S$1,"")))/LEN(S$1) +
+(LEN($F13)-LEN(SUBSTITUTE($F13,S$1,"")))/LEN(S$1) +
+(LEN($G13)-LEN(SUBSTITUTE($G13,S$1,"")))/LEN(S$1) +
+(LEN($H13)-LEN(SUBSTITUTE($H13,S$1,"")))/LEN(S$1) +
+(LEN($I13)-LEN(SUBSTITUTE($I13,S$1,"")))/LEN(S$1)</f>
+        <v>2</v>
+      </c>
+      <c r="T13" s="10">
+        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,T$1,"")))/LEN(T$1) +
+(LEN($E13)-LEN(SUBSTITUTE($E13,T$1,"")))/LEN(T$1) +
+(LEN($F13)-LEN(SUBSTITUTE($F13,T$1,"")))/LEN(T$1) +
+(LEN($G13)-LEN(SUBSTITUTE($G13,T$1,"")))/LEN(T$1) +
+(LEN($H13)-LEN(SUBSTITUTE($H13,T$1,"")))/LEN(T$1) +
+(LEN($I13)-LEN(SUBSTITUTE($I13,T$1,"")))/LEN(T$1)</f>
+        <v>1</v>
+      </c>
+      <c r="U13" s="10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="V13" s="10">
+        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,V$1,"")))/LEN(V$1) +
+(LEN($E13)-LEN(SUBSTITUTE($E13,V$1,"")))/LEN(V$1) +
+(LEN($F13)-LEN(SUBSTITUTE($F13,V$1,"")))/LEN(V$1) +
+(LEN($G13)-LEN(SUBSTITUTE($G13,V$1,"")))/LEN(V$1) +
+(LEN($H13)-LEN(SUBSTITUTE($H13,V$1,"")))/LEN(V$1) +
+(LEN($I13)-LEN(SUBSTITUTE($I13,V$1,"")))/LEN(V$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="9">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J14" s="18" t="str">
+        <f>D$1 &amp; ": " &amp; D14 &amp; CHAR(10)
+&amp; E$1 &amp; ": " &amp; E14 &amp; CHAR(10)
+&amp; F$1 &amp; ": " &amp; F14 &amp; CHAR(10)
+&amp; G$1 &amp; ": " &amp; G14 &amp; CHAR(10)
+&amp; H$1 &amp; ": " &amp; H14 &amp; CHAR(10)
+&amp; I$1 &amp; ": " &amp; I14 &amp; CHAR(10)</f>
+        <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
+2: Slink%n💡➜
+3: Redirect%n🔓👊📷🔊
+4: Sneak%n🔍➜➜
+5: Jab%n👊💡➜
+6: Examine%n💡💡💡🔊🔊
+</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="O14" s="10">
+        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,O$1,"")))/LEN(O$1) +
+(LEN($E14)-LEN(SUBSTITUTE($E14,O$1,"")))/LEN(O$1) +
+(LEN($F14)-LEN(SUBSTITUTE($F14,O$1,"")))/LEN(O$1) +
+(LEN($G14)-LEN(SUBSTITUTE($G14,O$1,"")))/LEN(O$1) +
+(LEN($H14)-LEN(SUBSTITUTE($H14,O$1,"")))/LEN(O$1) +
+(LEN($I14)-LEN(SUBSTITUTE($I14,O$1,"")))/LEN(O$1)</f>
         <v>5</v>
       </c>
-      <c r="Q11" s="8">
-        <f t="shared" si="0"/>
+      <c r="P14" s="10">
+        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,P$1,"")))/LEN(P$1) +
+(LEN($E14)-LEN(SUBSTITUTE($E14,P$1,"")))/LEN(P$1) +
+(LEN($F14)-LEN(SUBSTITUTE($F14,P$1,"")))/LEN(P$1) +
+(LEN($G14)-LEN(SUBSTITUTE($G14,P$1,"")))/LEN(P$1) +
+(LEN($H14)-LEN(SUBSTITUTE($H14,P$1,"")))/LEN(P$1) +
+(LEN($I14)-LEN(SUBSTITUTE($I14,P$1,"")))/LEN(P$1)</f>
+        <v>4</v>
+      </c>
+      <c r="Q14" s="10">
+        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,Q$1,"")))/LEN(Q$1) +
+(LEN($E14)-LEN(SUBSTITUTE($E14,Q$1,"")))/LEN(Q$1) +
+(LEN($F14)-LEN(SUBSTITUTE($F14,Q$1,"")))/LEN(Q$1) +
+(LEN($G14)-LEN(SUBSTITUTE($G14,Q$1,"")))/LEN(Q$1) +
+(LEN($H14)-LEN(SUBSTITUTE($H14,Q$1,"")))/LEN(Q$1) +
+(LEN($I14)-LEN(SUBSTITUTE($I14,Q$1,"")))/LEN(Q$1)</f>
+        <v>4</v>
+      </c>
+      <c r="R14" s="10">
+        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,R$1,"")))/LEN(R$1) +
+(LEN($E14)-LEN(SUBSTITUTE($E14,R$1,"")))/LEN(R$1) +
+(LEN($F14)-LEN(SUBSTITUTE($F14,R$1,"")))/LEN(R$1) +
+(LEN($G14)-LEN(SUBSTITUTE($G14,R$1,"")))/LEN(R$1) +
+(LEN($H14)-LEN(SUBSTITUTE($H14,R$1,"")))/LEN(R$1) +
+(LEN($I14)-LEN(SUBSTITUTE($I14,R$1,"")))/LEN(R$1)</f>
+        <v>2</v>
+      </c>
+      <c r="S14" s="10">
+        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,S$1,"")))/LEN(S$1) +
+(LEN($E14)-LEN(SUBSTITUTE($E14,S$1,"")))/LEN(S$1) +
+(LEN($F14)-LEN(SUBSTITUTE($F14,S$1,"")))/LEN(S$1) +
+(LEN($G14)-LEN(SUBSTITUTE($G14,S$1,"")))/LEN(S$1) +
+(LEN($H14)-LEN(SUBSTITUTE($H14,S$1,"")))/LEN(S$1) +
+(LEN($I14)-LEN(SUBSTITUTE($I14,S$1,"")))/LEN(S$1)</f>
+        <v>3</v>
+      </c>
+      <c r="T14" s="10">
+        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,T$1,"")))/LEN(T$1) +
+(LEN($E14)-LEN(SUBSTITUTE($E14,T$1,"")))/LEN(T$1) +
+(LEN($F14)-LEN(SUBSTITUTE($F14,T$1,"")))/LEN(T$1) +
+(LEN($G14)-LEN(SUBSTITUTE($G14,T$1,"")))/LEN(T$1) +
+(LEN($H14)-LEN(SUBSTITUTE($H14,T$1,"")))/LEN(T$1) +
+(LEN($I14)-LEN(SUBSTITUTE($I14,T$1,"")))/LEN(T$1)</f>
+        <v>2</v>
+      </c>
+      <c r="U14" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V14" s="10">
+        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,V$1,"")))/LEN(V$1) +
+(LEN($E14)-LEN(SUBSTITUTE($E14,V$1,"")))/LEN(V$1) +
+(LEN($F14)-LEN(SUBSTITUTE($F14,V$1,"")))/LEN(V$1) +
+(LEN($G14)-LEN(SUBSTITUTE($G14,V$1,"")))/LEN(V$1) +
+(LEN($H14)-LEN(SUBSTITUTE($H14,V$1,"")))/LEN(V$1) +
+(LEN($I14)-LEN(SUBSTITUTE($I14,V$1,"")))/LEN(V$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" s="9">
+        <v>2</v>
+      </c>
+      <c r="C15" s="9">
+        <v>3</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="J15" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
+2: Hesitate%n💡
+3: Loop%n📷🔍
+4: Redirect%n🔓👊📷🔊
+5: Packet Sniff%n💡💡🔍🔍
+6: Hesitate%n💡
+</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="O15" s="10">
+        <f t="shared" ref="O15:V15" si="7">(LEN($D15)-LEN(SUBSTITUTE($D15,O$1,"")))/LEN(O$1) +
+(LEN($E15)-LEN(SUBSTITUTE($E15,O$1,"")))/LEN(O$1) +
+(LEN($F15)-LEN(SUBSTITUTE($F15,O$1,"")))/LEN(O$1) +
+(LEN($G15)-LEN(SUBSTITUTE($G15,O$1,"")))/LEN(O$1) +
+(LEN($H15)-LEN(SUBSTITUTE($H15,O$1,"")))/LEN(O$1) +
+(LEN($I15)-LEN(SUBSTITUTE($I15,O$1,"")))/LEN(O$1)</f>
+        <v>7</v>
+      </c>
+      <c r="P15" s="10">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q15" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="10">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="S15" s="10">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T15" s="10">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U15" s="10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="V15" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="33">
+        <v>2</v>
+      </c>
+      <c r="C16" s="33">
+        <v>3</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="J16" s="34" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">1: Run%n🔊🔊➜➜
+2: Disable%n📷🔊➜
+3: Pick%n🔓🔊➜
+4: Jab%n👊💡➜
+5: Reveal%n🔍
+6: Punch%n👊🔊🔊➜
+</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="L16" s="34"/>
+      <c r="M16" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="N16" s="34"/>
+      <c r="O16" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P16" s="32">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="R11" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S11" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T11" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="U11" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
+      <c r="Q16" s="32">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="R16" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S16" s="32">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="T16" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U16" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V16" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2981,7 +3604,7 @@
         <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -3021,18 +3644,18 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3045,7 +3668,7 @@
   <dimension ref="A7:S31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
redesigning the character cards
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -471,15 +471,9 @@
     <t>SLIPPERY%n2 free💡when escaping</t>
   </si>
   <si>
-    <t>OBSERVANT%nAfter planning and before heist, may 🔍🔍</t>
-  </si>
-  <si>
     <t>Sewer Rat</t>
   </si>
   <si>
-    <t>TUNNEL%nMay begin the heist on any tile on the outside of the map for  🔊🔊🔊</t>
-  </si>
-  <si>
     <t>INSPIRE%nEach turn, gain a free 💡 and give it to player.</t>
   </si>
   <si>
@@ -501,9 +495,6 @@
     <t>BOLT%nMay spend 💡for ➜</t>
   </si>
   <si>
-    <t>LOOTER%nGain $1k each time you take HESITATE.</t>
-  </si>
-  <si>
     <t>Total Ideas</t>
   </si>
   <si>
@@ -513,36 +504,9 @@
     <t>COMMAND &amp; CONTROL%nMay spend 💡for 🔍, up to three times per turn.</t>
   </si>
   <si>
-    <t>REPORT IN%nWhen  👊, lower the noise level by 3. Do not change the ⚠ level.</t>
-  </si>
-  <si>
     <t>DISGUISE%nMay spend 💡 to enter space with guards.</t>
   </si>
   <si>
-    <t>Default 1</t>
-  </si>
-  <si>
-    <t>Default 2</t>
-  </si>
-  <si>
-    <t>Walk 🔊➜</t>
-  </si>
-  <si>
-    <t>Crawl ➜</t>
-  </si>
-  <si>
-    <t>I CAN HAZ TEH CODES?%nOnce per turn, may  🔊🔊🔍.%nI CAN HEARTBLEED%nIf outdoors, may spend 💡💡 to 🔍</t>
-  </si>
-  <si>
-    <t>PICKER%nGain 💡 when you 🔓%nMASTER KEY%nWhen outdoors, may use  💡💡 to enable one player to 🔓</t>
-  </si>
-  <si>
-    <t>Saunter 🔊➜➜</t>
-  </si>
-  <si>
-    <t>Shimmy  🔊➜➜</t>
-  </si>
-  <si>
     <t>Unplug%n📷🔊🔊➜</t>
   </si>
   <si>
@@ -564,9 +528,6 @@
     <t>Hesitate%n💡</t>
   </si>
   <si>
-    <t>Smackdown 🔊👊</t>
-  </si>
-  <si>
     <t>Kick%n👊🔊➜➜</t>
   </si>
   <si>
@@ -580,15 +541,6 @@
   </si>
   <si>
     <t>Upgrade2Rolls</t>
-  </si>
-  <si>
-    <t>Hesitate  💡</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick  🔓 </t>
-  </si>
-  <si>
-    <t>Spy Stuff 🔓 👊</t>
   </si>
   <si>
     <t>EXTORT GUARDS%nGain $1k from each subdued guard.</t>
@@ -681,6 +633,54 @@
   </si>
   <si>
     <t>Sneak%n🔍➜➜</t>
+  </si>
+  <si>
+    <t>I CAN HAZ TEH CODES?%nOnce per turn, may  🔊🔊🔍%n %nI CAN HEARTBLEED%nIf outdoors, may spend 💡💡 to 🔍</t>
+  </si>
+  <si>
+    <t>Default1</t>
+  </si>
+  <si>
+    <t>Default2</t>
+  </si>
+  <si>
+    <t>Hesitate %n💡</t>
+  </si>
+  <si>
+    <t>Walk%n🔊➜</t>
+  </si>
+  <si>
+    <t>Saunter%n🔊➜➜</t>
+  </si>
+  <si>
+    <t>Spy Stuff%n🔓👊</t>
+  </si>
+  <si>
+    <t>Shimmy%n🔊➜➜</t>
+  </si>
+  <si>
+    <t>Crawl%n➜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick%n🔓 </t>
+  </si>
+  <si>
+    <t>Bash%n🔊🔊👊</t>
+  </si>
+  <si>
+    <t>OBSERVANT%nWhen outdoors, may spend $1k for 🔍🔍🔍</t>
+  </si>
+  <si>
+    <t>LOOTER%nGain $1k each time you take "Hestitate"</t>
+  </si>
+  <si>
+    <t>TUNNEL%nMay begin the heist on any tile on the outside of the map for 🔊🔊🔊🔊</t>
+  </si>
+  <si>
+    <t>YOU WILL REPORT IN%nWhen  👊, lower the noise level by 3. Do not change the ⚠ level.</t>
+  </si>
+  <si>
+    <t>PICKER%nGain 💡 when you 🔓%n %nMASTER KEY%nWhen outdoors, may use  💡💡 to enable one player to 🔓</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,8 +1168,8 @@
     <col min="6" max="6" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="14.42578125" style="6" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="74.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="3"/>
@@ -1207,10 +1207,10 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>135</v>
@@ -1219,7 +1219,7 @@
         <v>29</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1254,13 +1254,13 @@
         <v>2</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="O2" s="21">
         <f>F2+G2</f>
@@ -1299,10 +1299,10 @@
         <v>2</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>147</v>
@@ -1344,10 +1344,10 @@
         <v>2</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M4" s="22" t="s">
         <v>148</v>
@@ -1389,13 +1389,13 @@
         <v>2</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="O5" s="21">
         <f t="shared" si="0"/>
@@ -1434,13 +1434,13 @@
         <v>2</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="O6" s="21">
         <f t="shared" si="0"/>
@@ -1479,13 +1479,13 @@
         <v>2</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="O7" s="24">
         <f>F7+G7</f>
@@ -1524,13 +1524,13 @@
         <v>2</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O8" s="24">
         <f t="shared" si="0"/>
@@ -1569,13 +1569,13 @@
         <v>2</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="O9" s="24">
         <f t="shared" si="0"/>
@@ -1614,13 +1614,13 @@
         <v>2</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="O10" s="24">
         <f t="shared" si="0"/>
@@ -1659,13 +1659,13 @@
         <v>2</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M11" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O11" s="24">
         <f>F11+G11</f>
@@ -1704,13 +1704,13 @@
         <v>2</v>
       </c>
       <c r="K12" s="27" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M12" s="28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O12" s="27">
         <f t="shared" si="0"/>
@@ -1749,13 +1749,13 @@
         <v>2</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L13" s="27" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M13" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O13" s="27">
         <f t="shared" si="0"/>
@@ -1794,13 +1794,13 @@
         <v>2</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L14" s="27" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M14" s="28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O14" s="27">
         <f t="shared" si="0"/>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="15" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>22</v>
@@ -1833,13 +1833,13 @@
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
       <c r="K15" s="27" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="L15" s="27" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M15" s="28" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="O15" s="27">
         <f t="shared" si="0"/>
@@ -1878,13 +1878,13 @@
         <v>2</v>
       </c>
       <c r="K16" s="27" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="L16" s="27" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M16" s="28" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="O16" s="27">
         <f t="shared" si="0"/>
@@ -1903,11 +1903,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U15" sqref="U15"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,16 +1968,16 @@
         <v>62</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>116</v>
@@ -2001,7 +2001,7 @@
         <v>144</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="W1" s="11" t="s">
         <v>33</v>
@@ -2018,25 +2018,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="J2" s="15" t="str">
-        <f>D$1 &amp; ": " &amp; D2 &amp; CHAR(10)
+        <f t="shared" ref="J2:J11" si="0">D$1 &amp; ": " &amp; D2 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E2 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F2 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G2 &amp; CHAR(10)
@@ -2064,7 +2064,7 @@
 </v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N2" s="15" t="str">
         <f>VLOOKUP(M2,$A$7:$J$11,10,FALSE)</f>
@@ -2077,7 +2077,7 @@
 </v>
       </c>
       <c r="O2" s="8">
-        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O2:V2" si="1">(LEN($D2)-LEN(SUBSTITUTE($D2,O$1,"")))/LEN(O$1) +
 (LEN($E2)-LEN(SUBSTITUTE($E2,O$1,"")))/LEN(O$1) +
 (LEN($F2)-LEN(SUBSTITUTE($F2,O$1,"")))/LEN(O$1) +
 (LEN($G2)-LEN(SUBSTITUTE($G2,O$1,"")))/LEN(O$1) +
@@ -2086,66 +2086,31 @@
         <v>2</v>
       </c>
       <c r="P2" s="8">
-        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,P$1,"")))/LEN(P$1) +
-(LEN($E2)-LEN(SUBSTITUTE($E2,P$1,"")))/LEN(P$1) +
-(LEN($F2)-LEN(SUBSTITUTE($F2,P$1,"")))/LEN(P$1) +
-(LEN($G2)-LEN(SUBSTITUTE($G2,P$1,"")))/LEN(P$1) +
-(LEN($H2)-LEN(SUBSTITUTE($H2,P$1,"")))/LEN(P$1) +
-(LEN($I2)-LEN(SUBSTITUTE($I2,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Q2" s="8">
-        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,Q$1,"")))/LEN(Q$1) +
-(LEN($E2)-LEN(SUBSTITUTE($E2,Q$1,"")))/LEN(Q$1) +
-(LEN($F2)-LEN(SUBSTITUTE($F2,Q$1,"")))/LEN(Q$1) +
-(LEN($G2)-LEN(SUBSTITUTE($G2,Q$1,"")))/LEN(Q$1) +
-(LEN($H2)-LEN(SUBSTITUTE($H2,Q$1,"")))/LEN(Q$1) +
-(LEN($I2)-LEN(SUBSTITUTE($I2,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="R2" s="8">
-        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,R$1,"")))/LEN(R$1) +
-(LEN($E2)-LEN(SUBSTITUTE($E2,R$1,"")))/LEN(R$1) +
-(LEN($F2)-LEN(SUBSTITUTE($F2,R$1,"")))/LEN(R$1) +
-(LEN($G2)-LEN(SUBSTITUTE($G2,R$1,"")))/LEN(R$1) +
-(LEN($H2)-LEN(SUBSTITUTE($H2,R$1,"")))/LEN(R$1) +
-(LEN($I2)-LEN(SUBSTITUTE($I2,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S2" s="8">
-        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,S$1,"")))/LEN(S$1) +
-(LEN($E2)-LEN(SUBSTITUTE($E2,S$1,"")))/LEN(S$1) +
-(LEN($F2)-LEN(SUBSTITUTE($F2,S$1,"")))/LEN(S$1) +
-(LEN($G2)-LEN(SUBSTITUTE($G2,S$1,"")))/LEN(S$1) +
-(LEN($H2)-LEN(SUBSTITUTE($H2,S$1,"")))/LEN(S$1) +
-(LEN($I2)-LEN(SUBSTITUTE($I2,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T2" s="8">
-        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,T$1,"")))/LEN(T$1) +
-(LEN($E2)-LEN(SUBSTITUTE($E2,T$1,"")))/LEN(T$1) +
-(LEN($F2)-LEN(SUBSTITUTE($F2,T$1,"")))/LEN(T$1) +
-(LEN($G2)-LEN(SUBSTITUTE($G2,T$1,"")))/LEN(T$1) +
-(LEN($H2)-LEN(SUBSTITUTE($H2,T$1,"")))/LEN(T$1) +
-(LEN($I2)-LEN(SUBSTITUTE($I2,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U2" s="8">
-        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,U$1,"")))/LEN(U$1) +
-(LEN($E2)-LEN(SUBSTITUTE($E2,U$1,"")))/LEN(U$1) +
-(LEN($F2)-LEN(SUBSTITUTE($F2,U$1,"")))/LEN(U$1) +
-(LEN($G2)-LEN(SUBSTITUTE($G2,U$1,"")))/LEN(U$1) +
-(LEN($H2)-LEN(SUBSTITUTE($H2,U$1,"")))/LEN(U$1) +
-(LEN($I2)-LEN(SUBSTITUTE($I2,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V2" s="8">
-        <f>(LEN($D2)-LEN(SUBSTITUTE($D2,V$1,"")))/LEN(V$1) +
-(LEN($E2)-LEN(SUBSTITUTE($E2,V$1,"")))/LEN(V$1) +
-(LEN($F2)-LEN(SUBSTITUTE($F2,V$1,"")))/LEN(V$1) +
-(LEN($G2)-LEN(SUBSTITUTE($G2,V$1,"")))/LEN(V$1) +
-(LEN($H2)-LEN(SUBSTITUTE($H2,V$1,"")))/LEN(V$1) +
-(LEN($I2)-LEN(SUBSTITUTE($I2,V$1,"")))/LEN(V$1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2160,30 +2125,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="J3" s="15" t="str">
-        <f>D$1 &amp; ": " &amp; D3 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E3 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F3 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G3 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H3 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I3 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Punch%n👊🔊🔊➜
 2: Hesitate%n💡
 3: Shim%n🔓🔊🔊➜
@@ -2196,7 +2156,7 @@
         <v>40</v>
       </c>
       <c r="L3" s="15" t="str">
-        <f t="shared" ref="L3:L6" si="0">VLOOKUP(K3,$A$7:$J$11,10,FALSE)</f>
+        <f t="shared" ref="L3:L6" si="2">VLOOKUP(K3,$A$7:$J$11,10,FALSE)</f>
         <v xml:space="preserve">1: Unplug%n📷🔊🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
@@ -2209,7 +2169,7 @@
         <v>45</v>
       </c>
       <c r="N3" s="16" t="str">
-        <f t="shared" ref="N3:N6" si="1">VLOOKUP(M3,$A$7:$J$11,10,FALSE)</f>
+        <f t="shared" ref="N3:N6" si="3">VLOOKUP(M3,$A$7:$J$11,10,FALSE)</f>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Bribe%n$ 🔊➜
 3: Study%n💡💡
@@ -2219,7 +2179,7 @@
 </v>
       </c>
       <c r="O3" s="8">
-        <f t="shared" ref="O3:V16" si="2">(LEN($D3)-LEN(SUBSTITUTE($D3,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O3:V16" si="4">(LEN($D3)-LEN(SUBSTITUTE($D3,O$1,"")))/LEN(O$1) +
 (LEN($E3)-LEN(SUBSTITUTE($E3,O$1,"")))/LEN(O$1) +
 (LEN($F3)-LEN(SUBSTITUTE($F3,O$1,"")))/LEN(O$1) +
 (LEN($G3)-LEN(SUBSTITUTE($G3,O$1,"")))/LEN(O$1) +
@@ -2228,31 +2188,31 @@
         <v>2</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="Q3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2267,30 +2227,25 @@
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>192</v>
-      </c>
       <c r="J4" s="15" t="str">
-        <f>D$1 &amp; ": " &amp; D4 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E4 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F4 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G4 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H4 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I4 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Study%n💡💡
 2: Run%n🔊🔊➜➜
 3: Reveal%n🔍
@@ -2300,10 +2255,10 @@
 </v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L4" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Rake%n🔓🔓🔊➜
 3: Bribe%n$ 🔊➜
@@ -2316,7 +2271,7 @@
         <v>69</v>
       </c>
       <c r="N4" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
@@ -2326,35 +2281,35 @@
 </v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="Q4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2369,30 +2324,25 @@
         <v>1</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="J5" s="15" t="str">
-        <f>D$1 &amp; ": " &amp; D5 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E5 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F5 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G5 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H5 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I5 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Hesitate%n💡
 2: Punch%n👊🔊🔊➜
 3: Hesitate%n💡
@@ -2405,7 +2355,7 @@
         <v>74</v>
       </c>
       <c r="L5" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: Spray%n📷🔊➜
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
@@ -2418,7 +2368,7 @@
         <v>40</v>
       </c>
       <c r="N5" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">1: Unplug%n📷🔊🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
@@ -2428,35 +2378,35 @@
 </v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="Q5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="T5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2471,30 +2421,25 @@
         <v>1</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="J6" s="34" t="str">
-        <f>D$1 &amp; ": " &amp; D6 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E6 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F6 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G6 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H6 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I6 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Hesitate%n💡
 3: Run%n🔊🔊➜➜
@@ -2507,7 +2452,7 @@
         <v>69</v>
       </c>
       <c r="L6" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
@@ -2520,7 +2465,7 @@
         <v>74</v>
       </c>
       <c r="N6" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">1: Spray%n📷🔊➜
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
@@ -2530,35 +2475,35 @@
 </v>
       </c>
       <c r="O6" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="P6" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="Q6" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="R6" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S6" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T6" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U6" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V6" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2573,30 +2518,25 @@
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="H7" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>191</v>
-      </c>
       <c r="J7" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E7 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F7 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G7 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H7 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I7 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Unplug%n📷🔊🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
@@ -2632,35 +2572,35 @@
 </v>
       </c>
       <c r="O7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="Q7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="R7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="T7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2675,30 +2615,25 @@
         <v>2</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="J8" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D8 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E8 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F8 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G8 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H8 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I8 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Spray%n📷🔊➜
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
@@ -2711,7 +2646,7 @@
         <v>46</v>
       </c>
       <c r="L8" s="30" t="str">
-        <f t="shared" ref="L8:L11" si="3">VLOOKUP(K8,$A$12:$J$16,10,FALSE)</f>
+        <f t="shared" ref="L8:L11" si="5">VLOOKUP(K8,$A$12:$J$16,10,FALSE)</f>
         <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
 2: Slink%n💡➜
 3: Redirect%n🔓👊📷🔊
@@ -2724,7 +2659,7 @@
         <v>42</v>
       </c>
       <c r="N8" s="18" t="str">
-        <f t="shared" ref="N8:N11" si="4">VLOOKUP(M8,$A$12:$J$16,10,FALSE)</f>
+        <f t="shared" ref="N8:N11" si="6">VLOOKUP(M8,$A$12:$J$16,10,FALSE)</f>
         <v xml:space="preserve">1: Sneak%n🔍➜➜
 2: Sleeper Hold%n👊➜
 3: Slink%n💡➜
@@ -2734,7 +2669,7 @@
 </v>
       </c>
       <c r="O8" s="8">
-        <f t="shared" ref="O8:V8" si="5">(LEN($D8)-LEN(SUBSTITUTE($D8,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O8:V8" si="7">(LEN($D8)-LEN(SUBSTITUTE($D8,O$1,"")))/LEN(O$1) +
 (LEN($E8)-LEN(SUBSTITUTE($E8,O$1,"")))/LEN(O$1) +
 (LEN($F8)-LEN(SUBSTITUTE($F8,O$1,"")))/LEN(O$1) +
 (LEN($G8)-LEN(SUBSTITUTE($G8,O$1,"")))/LEN(O$1) +
@@ -2743,31 +2678,31 @@
         <v>2</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="Q8" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="R8" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="S8" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V8" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2782,30 +2717,25 @@
         <v>2</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="J9" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D9 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E9 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G9 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H9 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I9 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Bribe%n$ 🔊➜
 3: Study%n💡💡
@@ -2815,10 +2745,10 @@
 </v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="L9" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Disable%n📷🔊➜
 3: Pick%n🔓🔊➜
@@ -2831,7 +2761,7 @@
         <v>46</v>
       </c>
       <c r="N9" s="18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
 2: Slink%n💡➜
 3: Redirect%n🔓👊📷🔊
@@ -2841,35 +2771,35 @@
 </v>
       </c>
       <c r="O9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="P9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Q9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -2884,30 +2814,25 @@
         <v>2</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="J10" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D10 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E10 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F10 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G10 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H10 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I10 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
@@ -2917,10 +2842,10 @@
 </v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="L10" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Hesitate%n💡
 3: Loop%n📷🔍
@@ -2930,10 +2855,10 @@
 </v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="N10" s="18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Disable%n📷🔊➜
 3: Pick%n🔓🔊➜
@@ -2943,41 +2868,41 @@
 </v>
       </c>
       <c r="O10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="P10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="Q10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="R10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="S10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="V10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B11" s="33">
         <v>2</v>
@@ -2986,30 +2911,25 @@
         <v>2</v>
       </c>
       <c r="D11" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>193</v>
-      </c>
       <c r="F11" s="33" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="J11" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D11 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E11 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F11 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G11 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H11 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I11 &amp; CHAR(10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Rake%n🔓🔓🔊➜
 3: Bribe%n$ 🔊➜
@@ -3022,7 +2942,7 @@
         <v>127</v>
       </c>
       <c r="L11" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Sprint%n🔊🔊➜➜➜
 3: Slink%n💡➜
@@ -3032,10 +2952,10 @@
 </v>
       </c>
       <c r="M11" s="32" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="N11" s="34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Hesitate%n💡
 3: Loop%n📷🔍
@@ -3045,35 +2965,35 @@
 </v>
       </c>
       <c r="O11" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="P11" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="Q11" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R11" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S11" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T11" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="U11" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V11" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3088,25 +3008,25 @@
         <v>3</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="J12" s="17" t="str">
-        <f t="shared" ref="J12:J16" si="6">D$1 &amp; ": " &amp; D12 &amp; CHAR(10)
+        <f t="shared" ref="J12:J16" si="8">D$1 &amp; ": " &amp; D12 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E12 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F12 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G12 &amp; CHAR(10)
@@ -3121,41 +3041,41 @@
 </v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="Q12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="R12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="S12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="T12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3170,22 +3090,22 @@
         <v>3</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="J13" s="18" t="str">
         <f>D$1 &amp; ": " &amp; D13 &amp; CHAR(10)
@@ -3203,13 +3123,13 @@
 </v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="O13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O13:T14" si="9">(LEN($D13)-LEN(SUBSTITUTE($D13,O$1,"")))/LEN(O$1) +
 (LEN($E13)-LEN(SUBSTITUTE($E13,O$1,"")))/LEN(O$1) +
 (LEN($F13)-LEN(SUBSTITUTE($F13,O$1,"")))/LEN(O$1) +
 (LEN($G13)-LEN(SUBSTITUTE($G13,O$1,"")))/LEN(O$1) +
@@ -3218,52 +3138,27 @@
         <v>1</v>
       </c>
       <c r="P13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,P$1,"")))/LEN(P$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,P$1,"")))/LEN(P$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,P$1,"")))/LEN(P$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,P$1,"")))/LEN(P$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,P$1,"")))/LEN(P$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Q13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,Q$1,"")))/LEN(Q$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,Q$1,"")))/LEN(Q$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,Q$1,"")))/LEN(Q$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,Q$1,"")))/LEN(Q$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,Q$1,"")))/LEN(Q$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="R13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,R$1,"")))/LEN(R$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,R$1,"")))/LEN(R$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,R$1,"")))/LEN(R$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,R$1,"")))/LEN(R$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,R$1,"")))/LEN(R$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="S13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,S$1,"")))/LEN(S$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,S$1,"")))/LEN(S$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,S$1,"")))/LEN(S$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,S$1,"")))/LEN(S$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,S$1,"")))/LEN(S$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="T13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,T$1,"")))/LEN(T$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,T$1,"")))/LEN(T$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,T$1,"")))/LEN(T$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,T$1,"")))/LEN(T$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,T$1,"")))/LEN(T$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="U13" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V13" s="10">
@@ -3287,22 +3182,22 @@
         <v>3</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="J14" s="18" t="str">
         <f>D$1 &amp; ": " &amp; D14 &amp; CHAR(10)
@@ -3320,67 +3215,37 @@
 </v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="O14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,O$1,"")))/LEN(O$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,O$1,"")))/LEN(O$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,O$1,"")))/LEN(O$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,O$1,"")))/LEN(O$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,O$1,"")))/LEN(O$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="P14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,P$1,"")))/LEN(P$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,P$1,"")))/LEN(P$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,P$1,"")))/LEN(P$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,P$1,"")))/LEN(P$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,P$1,"")))/LEN(P$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="Q14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,Q$1,"")))/LEN(Q$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,Q$1,"")))/LEN(Q$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,Q$1,"")))/LEN(Q$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,Q$1,"")))/LEN(Q$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,Q$1,"")))/LEN(Q$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="R14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,R$1,"")))/LEN(R$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,R$1,"")))/LEN(R$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,R$1,"")))/LEN(R$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,R$1,"")))/LEN(R$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,R$1,"")))/LEN(R$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="S14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,S$1,"")))/LEN(S$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,S$1,"")))/LEN(S$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,S$1,"")))/LEN(S$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,S$1,"")))/LEN(S$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,S$1,"")))/LEN(S$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="T14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,T$1,"")))/LEN(T$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,T$1,"")))/LEN(T$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,T$1,"")))/LEN(T$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,T$1,"")))/LEN(T$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,T$1,"")))/LEN(T$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="U14" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V14" s="10">
@@ -3395,7 +3260,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="B15" s="9">
         <v>2</v>
@@ -3404,25 +3269,25 @@
         <v>3</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="J15" s="18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Hesitate%n💡
 3: Loop%n📷🔍
@@ -3432,13 +3297,13 @@
 </v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" ref="O15:V15" si="7">(LEN($D15)-LEN(SUBSTITUTE($D15,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O15:V15" si="10">(LEN($D15)-LEN(SUBSTITUTE($D15,O$1,"")))/LEN(O$1) +
 (LEN($E15)-LEN(SUBSTITUTE($E15,O$1,"")))/LEN(O$1) +
 (LEN($F15)-LEN(SUBSTITUTE($F15,O$1,"")))/LEN(O$1) +
 (LEN($G15)-LEN(SUBSTITUTE($G15,O$1,"")))/LEN(O$1) +
@@ -3447,37 +3312,37 @@
         <v>7</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="Q15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="R15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="S15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="T15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="U15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="V15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="B16" s="33">
         <v>2</v>
@@ -3486,25 +3351,25 @@
         <v>3</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="J16" s="34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Disable%n📷🔊➜
 3: Pick%n🔓🔊➜
@@ -3514,43 +3379,43 @@
 </v>
       </c>
       <c r="K16" s="33" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="L16" s="34"/>
       <c r="M16" s="33" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="N16" s="34"/>
       <c r="O16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="Q16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="R16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="T16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3604,7 +3469,7 @@
         <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -3652,10 +3517,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" t="s">
         <v>155</v>
-      </c>
-      <c r="B10" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some new ideas for skills and ideas
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="238">
   <si>
     <t>Name</t>
   </si>
@@ -370,12 +370,6 @@
     <t>Add 1 idea to the current skill</t>
   </si>
   <si>
-    <t>Disable all cameras on or adjacent to your tile</t>
-  </si>
-  <si>
-    <t>Move your pawn to an adjacent tile (that you planned)</t>
-  </si>
-  <si>
     <t>Requires: Splice In</t>
   </si>
   <si>
@@ -451,9 +445,6 @@
     <t>🔍</t>
   </si>
   <si>
-    <t>Uncover 1 unknown security token anywhere</t>
-  </si>
-  <si>
     <t>Looter</t>
   </si>
   <si>
@@ -463,9 +454,6 @@
     <t>Sewer Rat</t>
   </si>
   <si>
-    <t>INSPIRE%nEach turn, gain a free 💡 and give it to player.</t>
-  </si>
-  <si>
     <t>DENIAL OF SERVICE%nOnce per heist, disconnect all known cameras, and lower alert by 1.</t>
   </si>
   <si>
@@ -478,19 +466,10 @@
     <t>Subdue 1 guard on or adjacent to your tile.</t>
   </si>
   <si>
-    <t>For a cost of $1k (on your person), may move into a space with a guard.</t>
-  </si>
-  <si>
     <t>BOLT%nMay spend 💡for ➜</t>
   </si>
   <si>
     <t>Total Ideas</t>
-  </si>
-  <si>
-    <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires</t>
-  </si>
-  <si>
-    <t>DISGUISE%nMay spend 💡 to enter space with guards.</t>
   </si>
   <si>
     <t>Unplug%n📷🔊🔊➜</t>
@@ -648,15 +627,9 @@
     <t>Bash%n🔊🔊👊</t>
   </si>
   <si>
-    <t>OBSERVANT%nWhen outdoors, may spend $1k for 🔍🔍🔍</t>
-  </si>
-  <si>
     <t>LOOTER%nGain $1k each time you take "Hestitate"</t>
   </si>
   <si>
-    <t>TUNNEL%nMay begin the heist on any tile on the outside of the map for 🔊🔊🔊🔊</t>
-  </si>
-  <si>
     <t>YOU WILL REPORT IN%nWhen  👊, lower the noise level by 3. Do not change the ⚠ level.</t>
   </si>
   <si>
@@ -699,15 +672,9 @@
     <t>LevelUp2</t>
   </si>
   <si>
-    <t xml:space="preserve">GREAT IN A PINCH%nMay prevent a gate from shutting for 💡💡💡 </t>
-  </si>
-  <si>
     <t>Key In%n🔍🔓</t>
   </si>
   <si>
-    <t>ESCAPE ARTIST%nGain 💡💡💡 when escaping</t>
-  </si>
-  <si>
     <t>SLIPPERY%nGain💡when escaping</t>
   </si>
   <si>
@@ -738,10 +705,61 @@
     <t>💰</t>
   </si>
   <si>
-    <t>Gain $1k for your person.</t>
-  </si>
-  <si>
     <t>Steal</t>
+  </si>
+  <si>
+    <t>Disable 1 camera on or adjacent to your tile</t>
+  </si>
+  <si>
+    <t>👣</t>
+  </si>
+  <si>
+    <t>Move your pawn to a planned adjacent tile</t>
+  </si>
+  <si>
+    <t>Reveal 1 security token anywhere</t>
+  </si>
+  <si>
+    <t>Bribe: for $1k on your person, may move into a space with a guard.</t>
+  </si>
+  <si>
+    <t>Gain $1k on your person.</t>
+  </si>
+  <si>
+    <t>Move 1 guard to an adjacent space.</t>
+  </si>
+  <si>
+    <t>THEY TRUST ME%nMay start on any space without a security token.</t>
+  </si>
+  <si>
+    <t>INSPIRE%nWhen outdoors, give 💡 to a player of your choosing.</t>
+  </si>
+  <si>
+    <t>DISGUISE%nMay spend 💡 to enter space with guards.%n %nSWAP DUFFEL BAGS%nIf busted, team still gains loot.</t>
+  </si>
+  <si>
+    <t>DIG!%nFor 🔊🔊⚠, may treat a tile across 1 empty hex space as adjacent.</t>
+  </si>
+  <si>
+    <t>SEWER CRAWL%nMay begin the heist on any tile on the outside of the map for 🔊🔊🔊🔊</t>
+  </si>
+  <si>
+    <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires%n %nPACKS A SQUIB%nIf busted, fakes death and escapes (still counts toward busted count).</t>
+  </si>
+  <si>
+    <t>Tunneler Master</t>
+  </si>
+  <si>
+    <t>Guy on the Inside</t>
+  </si>
+  <si>
+    <t>False Alarm%n💡👣</t>
+  </si>
+  <si>
+    <t>GREAT IN A PINCH%nMay prevent a gate from shutting for 💡💡💡%n %nPACKS A SQUIB%nIf busted, loses loot but continues to next heist.</t>
+  </si>
+  <si>
+    <t>Toss Pebble%n🔊👣</t>
   </si>
 </sst>
 </file>
@@ -1212,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,31 +1268,31 @@
         <v>16</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1300,19 +1318,19 @@
         <v>1</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="N2" s="21">
         <f>F2+G2</f>
@@ -1342,10 +1360,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="J3" s="20" t="s">
         <v>9</v>
@@ -1354,7 +1372,7 @@
         <v>8</v>
       </c>
       <c r="L3" s="22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="N3" s="21">
         <f t="shared" ref="N3:N7" si="0">F3+G3</f>
@@ -1384,10 +1402,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J4" s="20" t="s">
         <v>12</v>
@@ -1396,7 +1414,7 @@
         <v>10</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="N4" s="21">
         <f t="shared" si="0"/>
@@ -1408,7 +1426,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C5" s="21">
         <v>1</v>
@@ -1426,10 +1444,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>14</v>
@@ -1438,7 +1456,7 @@
         <v>15</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="N5" s="21">
         <f t="shared" si="0"/>
@@ -1468,10 +1486,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J6" s="20" t="s">
         <v>4</v>
@@ -1480,7 +1498,7 @@
         <v>5</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="N6" s="21">
         <f t="shared" si="0"/>
@@ -1489,10 +1507,10 @@
     </row>
     <row r="7" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C7" s="21">
         <v>1</v>
@@ -1510,19 +1528,19 @@
         <v>2</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>42</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="N7" s="21">
         <f t="shared" si="0"/>
@@ -1552,22 +1570,22 @@
         <v>2</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>154</v>
+        <v>232</v>
       </c>
       <c r="N8" s="24">
-        <f>F8+G8</f>
+        <f t="shared" ref="N8:N19" si="1">F8+G8</f>
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>22</v>
@@ -1588,16 +1606,16 @@
         <v>3</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L9" s="25" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="N9" s="24">
-        <f>F9+G9</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -1624,16 +1642,16 @@
         <v>2</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>192</v>
+        <v>235</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="N10" s="24">
-        <f>F10+G10</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -1660,16 +1678,16 @@
         <v>1</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="N11" s="24">
-        <f>F11+G11</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1696,16 +1714,16 @@
         <v>3</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L12" s="25" t="s">
-        <v>155</v>
+        <v>229</v>
       </c>
       <c r="N12" s="24">
-        <f>F12+G12</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -1732,22 +1750,22 @@
         <v>4</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>192</v>
+        <v>237</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="N13" s="24">
-        <f>F13+G13</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>22</v>
@@ -1768,16 +1786,16 @@
         <v>2</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="N14" s="24">
-        <f>F14+G14</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1804,16 +1822,16 @@
         <v>3</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="N15" s="24">
-        <f>F15+G15</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -1840,16 +1858,16 @@
         <v>1</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L16" s="25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N16" s="24">
-        <f>F16+G16</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1876,25 +1894,25 @@
         <v>1</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="N17" s="24">
-        <f>F17+G17</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C18" s="24">
         <v>1</v>
@@ -1912,25 +1930,25 @@
         <v>3</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="N18" s="24">
-        <f>F18+G18</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>42</v>
+        <v>234</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C19" s="24">
         <v>1</v>
@@ -1948,16 +1966,16 @@
         <v>1</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="N19" s="24">
-        <f>F19+G19</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1973,11 +1991,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,16 +2057,16 @@
         <v>59</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>113</v>
@@ -2069,13 +2087,13 @@
         <v>103</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="X1" s="11" t="s">
         <v>30</v>
@@ -2083,7 +2101,7 @@
     </row>
     <row r="2" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" s="8">
         <v>2</v>
@@ -2092,22 +2110,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="J2" s="15" t="str">
         <f t="shared" ref="J2:J6" si="0">D$1 &amp; ": " &amp; D2 &amp; CHAR(10)
@@ -2125,10 +2143,10 @@
 </v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="L2" s="16" t="str">
-        <f>VLOOKUP(K2,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" ref="L2:L7" si="1">VLOOKUP(K2,$A$8:$J$21,10,FALSE)</f>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Bribe%n$ 🔊➜
 3: Study%n💡💡
@@ -2138,10 +2156,10 @@
 </v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N2" s="15" t="str">
-        <f>VLOOKUP(M2,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" ref="N2:N7" si="2">VLOOKUP(M2,$A$8:$J$21,10,FALSE)</f>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Rake%n🔓🔓🔊➜
 3: Bribe%n$ 🔊➜
@@ -2151,7 +2169,7 @@
 </v>
       </c>
       <c r="O2" s="8">
-        <f t="shared" ref="O2:W17" si="1">(LEN($D2)-LEN(SUBSTITUTE($D2,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O2:W17" si="3">(LEN($D2)-LEN(SUBSTITUTE($D2,O$1,"")))/LEN(O$1) +
 (LEN($E2)-LEN(SUBSTITUTE($E2,O$1,"")))/LEN(O$1) +
 (LEN($F2)-LEN(SUBSTITUTE($F2,O$1,"")))/LEN(O$1) +
 (LEN($G2)-LEN(SUBSTITUTE($G2,O$1,"")))/LEN(O$1) +
@@ -2160,41 +2178,41 @@
         <v>2</v>
       </c>
       <c r="P2" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="Q2" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="R2" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S2" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T2" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="U2" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V2" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W2" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
@@ -2203,22 +2221,22 @@
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="J3" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2234,7 +2252,7 @@
         <v>37</v>
       </c>
       <c r="L3" s="16" t="str">
-        <f>VLOOKUP(K3,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: Rake%n🔓🔓🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
@@ -2244,10 +2262,10 @@
 </v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="N3" s="15" t="str">
-        <f>VLOOKUP(M3,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: Bribe%n$ 🔊➜
 2: Yoink%n 💰🔊
 3: Run%n🔊🔊➜➜
@@ -2257,7 +2275,7 @@
 </v>
       </c>
       <c r="O3" s="8">
-        <f t="shared" ref="O3:V6" si="2">(LEN($D3)-LEN(SUBSTITUTE($D3,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O3:U6" si="4">(LEN($D3)-LEN(SUBSTITUTE($D3,O$1,"")))/LEN(O$1) +
 (LEN($E3)-LEN(SUBSTITUTE($E3,O$1,"")))/LEN(O$1) +
 (LEN($F3)-LEN(SUBSTITUTE($F3,O$1,"")))/LEN(O$1) +
 (LEN($G3)-LEN(SUBSTITUTE($G3,O$1,"")))/LEN(O$1) +
@@ -2266,41 +2284,41 @@
         <v>2</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="Q3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U3" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V3" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W3" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
@@ -2309,22 +2327,22 @@
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J4" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2340,7 +2358,7 @@
         <v>66</v>
       </c>
       <c r="L4" s="16" t="str">
-        <f>VLOOKUP(K4,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
@@ -2350,10 +2368,10 @@
 </v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="N4" s="15" t="str">
-        <f>VLOOKUP(M4,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Hesitate%n💡
 3: Loop%n📷🔍
@@ -2363,45 +2381,45 @@
 </v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="Q4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V4" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W4" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" s="8">
         <v>2</v>
@@ -2410,22 +2428,22 @@
         <v>1</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="J5" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2438,10 +2456,10 @@
 </v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="L5" s="16" t="str">
-        <f>VLOOKUP(K5,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: Yoink%n 💰🔊
 2: Examine%n💡💡💡🔊🔊
 3: Kick%n👊🔊➜➜
@@ -2451,10 +2469,10 @@
 </v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N5" s="15" t="str">
-        <f>VLOOKUP(M5,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Sprint%n🔊🔊➜➜➜
 3: Slink%n💡➜
@@ -2464,45 +2482,45 @@
 </v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="Q5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="T5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B6" s="8">
         <v>2</v>
@@ -2511,22 +2529,22 @@
         <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="J6" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2542,7 +2560,7 @@
         <v>71</v>
       </c>
       <c r="L6" s="16" t="str">
-        <f>VLOOKUP(K6,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: Spray%n📷🔊➜
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
@@ -2552,10 +2570,10 @@
 </v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="N6" s="15" t="str">
-        <f>VLOOKUP(M6,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Disable%n📷🔊➜
 3: Pick &amp; Walk%n🔓🔊➜
@@ -2565,45 +2583,45 @@
 </v>
       </c>
       <c r="O6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="Q6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="R6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="T6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B7" s="29">
         <v>2</v>
@@ -2612,25 +2630,25 @@
         <v>1</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="J7" s="31" t="str">
-        <f>D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
+        <f t="shared" ref="J7:J19" si="5">D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E7 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F7 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G7 &amp; CHAR(10)
@@ -2648,7 +2666,7 @@
         <v>43</v>
       </c>
       <c r="L7" s="32" t="str">
-        <f>VLOOKUP(K7,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
 2: Slink%n💡➜
 3: Redirect%n🔓👊📷🔊
@@ -2661,7 +2679,7 @@
         <v>39</v>
       </c>
       <c r="N7" s="31" t="str">
-        <f>VLOOKUP(M7,$A$8:$J$21,10,FALSE)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">1: Sneak%n🔍➜➜
 2: Sleeper Hold%n👊➜
 3: Slink%n💡➜
@@ -2671,7 +2689,7 @@
 </v>
       </c>
       <c r="O7" s="29">
-        <f>(LEN($D7)-LEN(SUBSTITUTE($D7,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O7:U19" si="6">(LEN($D7)-LEN(SUBSTITUTE($D7,O$1,"")))/LEN(O$1) +
 (LEN($E7)-LEN(SUBSTITUTE($E7,O$1,"")))/LEN(O$1) +
 (LEN($F7)-LEN(SUBSTITUTE($F7,O$1,"")))/LEN(O$1) +
 (LEN($G7)-LEN(SUBSTITUTE($G7,O$1,"")))/LEN(O$1) +
@@ -2680,71 +2698,41 @@
         <v>2</v>
       </c>
       <c r="P7" s="29">
-        <f>(LEN($D7)-LEN(SUBSTITUTE($D7,P$1,"")))/LEN(P$1) +
-(LEN($E7)-LEN(SUBSTITUTE($E7,P$1,"")))/LEN(P$1) +
-(LEN($F7)-LEN(SUBSTITUTE($F7,P$1,"")))/LEN(P$1) +
-(LEN($G7)-LEN(SUBSTITUTE($G7,P$1,"")))/LEN(P$1) +
-(LEN($H7)-LEN(SUBSTITUTE($H7,P$1,"")))/LEN(P$1) +
-(LEN($I7)-LEN(SUBSTITUTE($I7,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="Q7" s="29">
-        <f>(LEN($D7)-LEN(SUBSTITUTE($D7,Q$1,"")))/LEN(Q$1) +
-(LEN($E7)-LEN(SUBSTITUTE($E7,Q$1,"")))/LEN(Q$1) +
-(LEN($F7)-LEN(SUBSTITUTE($F7,Q$1,"")))/LEN(Q$1) +
-(LEN($G7)-LEN(SUBSTITUTE($G7,Q$1,"")))/LEN(Q$1) +
-(LEN($H7)-LEN(SUBSTITUTE($H7,Q$1,"")))/LEN(Q$1) +
-(LEN($I7)-LEN(SUBSTITUTE($I7,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="R7" s="29">
-        <f>(LEN($D7)-LEN(SUBSTITUTE($D7,R$1,"")))/LEN(R$1) +
-(LEN($E7)-LEN(SUBSTITUTE($E7,R$1,"")))/LEN(R$1) +
-(LEN($F7)-LEN(SUBSTITUTE($F7,R$1,"")))/LEN(R$1) +
-(LEN($G7)-LEN(SUBSTITUTE($G7,R$1,"")))/LEN(R$1) +
-(LEN($H7)-LEN(SUBSTITUTE($H7,R$1,"")))/LEN(R$1) +
-(LEN($I7)-LEN(SUBSTITUTE($I7,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S7" s="29">
-        <f>(LEN($D7)-LEN(SUBSTITUTE($D7,S$1,"")))/LEN(S$1) +
-(LEN($E7)-LEN(SUBSTITUTE($E7,S$1,"")))/LEN(S$1) +
-(LEN($F7)-LEN(SUBSTITUTE($F7,S$1,"")))/LEN(S$1) +
-(LEN($G7)-LEN(SUBSTITUTE($G7,S$1,"")))/LEN(S$1) +
-(LEN($H7)-LEN(SUBSTITUTE($H7,S$1,"")))/LEN(S$1) +
-(LEN($I7)-LEN(SUBSTITUTE($I7,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T7" s="29">
-        <f>(LEN($D7)-LEN(SUBSTITUTE($D7,T$1,"")))/LEN(T$1) +
-(LEN($E7)-LEN(SUBSTITUTE($E7,T$1,"")))/LEN(T$1) +
-(LEN($F7)-LEN(SUBSTITUTE($F7,T$1,"")))/LEN(T$1) +
-(LEN($G7)-LEN(SUBSTITUTE($G7,T$1,"")))/LEN(T$1) +
-(LEN($H7)-LEN(SUBSTITUTE($H7,T$1,"")))/LEN(T$1) +
-(LEN($I7)-LEN(SUBSTITUTE($I7,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U7" s="29">
-        <f>(LEN($D7)-LEN(SUBSTITUTE($D7,U$1,"")))/LEN(U$1) +
-(LEN($E7)-LEN(SUBSTITUTE($E7,U$1,"")))/LEN(U$1) +
-(LEN($F7)-LEN(SUBSTITUTE($F7,U$1,"")))/LEN(U$1) +
-(LEN($G7)-LEN(SUBSTITUTE($G7,U$1,"")))/LEN(U$1) +
-(LEN($H7)-LEN(SUBSTITUTE($H7,U$1,"")))/LEN(U$1) +
-(LEN($I7)-LEN(SUBSTITUTE($I7,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V7" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W7" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="B8" s="9">
         <v>2</v>
@@ -2753,30 +2741,25 @@
         <v>2</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="J8" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D8 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E8 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F8 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G8 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H8 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I8 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Bribe%n$ 🔊➜
 3: Study%n💡💡
@@ -2786,88 +2769,53 @@
 </v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L8" s="27"/>
       <c r="M8" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N8" s="18"/>
       <c r="O8" s="8">
-        <f>(LEN($D8)-LEN(SUBSTITUTE($D8,O$1,"")))/LEN(O$1) +
-(LEN($E8)-LEN(SUBSTITUTE($E8,O$1,"")))/LEN(O$1) +
-(LEN($F8)-LEN(SUBSTITUTE($F8,O$1,"")))/LEN(O$1) +
-(LEN($G8)-LEN(SUBSTITUTE($G8,O$1,"")))/LEN(O$1) +
-(LEN($H8)-LEN(SUBSTITUTE($H8,O$1,"")))/LEN(O$1) +
-(LEN($I8)-LEN(SUBSTITUTE($I8,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="P8" s="8">
-        <f>(LEN($D8)-LEN(SUBSTITUTE($D8,P$1,"")))/LEN(P$1) +
-(LEN($E8)-LEN(SUBSTITUTE($E8,P$1,"")))/LEN(P$1) +
-(LEN($F8)-LEN(SUBSTITUTE($F8,P$1,"")))/LEN(P$1) +
-(LEN($G8)-LEN(SUBSTITUTE($G8,P$1,"")))/LEN(P$1) +
-(LEN($H8)-LEN(SUBSTITUTE($H8,P$1,"")))/LEN(P$1) +
-(LEN($I8)-LEN(SUBSTITUTE($I8,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="Q8" s="8">
-        <f>(LEN($D8)-LEN(SUBSTITUTE($D8,Q$1,"")))/LEN(Q$1) +
-(LEN($E8)-LEN(SUBSTITUTE($E8,Q$1,"")))/LEN(Q$1) +
-(LEN($F8)-LEN(SUBSTITUTE($F8,Q$1,"")))/LEN(Q$1) +
-(LEN($G8)-LEN(SUBSTITUTE($G8,Q$1,"")))/LEN(Q$1) +
-(LEN($H8)-LEN(SUBSTITUTE($H8,Q$1,"")))/LEN(Q$1) +
-(LEN($I8)-LEN(SUBSTITUTE($I8,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="R8" s="8">
-        <f>(LEN($D8)-LEN(SUBSTITUTE($D8,R$1,"")))/LEN(R$1) +
-(LEN($E8)-LEN(SUBSTITUTE($E8,R$1,"")))/LEN(R$1) +
-(LEN($F8)-LEN(SUBSTITUTE($F8,R$1,"")))/LEN(R$1) +
-(LEN($G8)-LEN(SUBSTITUTE($G8,R$1,"")))/LEN(R$1) +
-(LEN($H8)-LEN(SUBSTITUTE($H8,R$1,"")))/LEN(R$1) +
-(LEN($I8)-LEN(SUBSTITUTE($I8,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="S8" s="8">
-        <f>(LEN($D8)-LEN(SUBSTITUTE($D8,S$1,"")))/LEN(S$1) +
-(LEN($E8)-LEN(SUBSTITUTE($E8,S$1,"")))/LEN(S$1) +
-(LEN($F8)-LEN(SUBSTITUTE($F8,S$1,"")))/LEN(S$1) +
-(LEN($G8)-LEN(SUBSTITUTE($G8,S$1,"")))/LEN(S$1) +
-(LEN($H8)-LEN(SUBSTITUTE($H8,S$1,"")))/LEN(S$1) +
-(LEN($I8)-LEN(SUBSTITUTE($I8,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T8" s="8">
-        <f>(LEN($D8)-LEN(SUBSTITUTE($D8,T$1,"")))/LEN(T$1) +
-(LEN($E8)-LEN(SUBSTITUTE($E8,T$1,"")))/LEN(T$1) +
-(LEN($F8)-LEN(SUBSTITUTE($F8,T$1,"")))/LEN(T$1) +
-(LEN($G8)-LEN(SUBSTITUTE($G8,T$1,"")))/LEN(T$1) +
-(LEN($H8)-LEN(SUBSTITUTE($H8,T$1,"")))/LEN(T$1) +
-(LEN($I8)-LEN(SUBSTITUTE($I8,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U8" s="8">
-        <f>(LEN($D8)-LEN(SUBSTITUTE($D8,U$1,"")))/LEN(U$1) +
-(LEN($E8)-LEN(SUBSTITUTE($E8,U$1,"")))/LEN(U$1) +
-(LEN($F8)-LEN(SUBSTITUTE($F8,U$1,"")))/LEN(U$1) +
-(LEN($G8)-LEN(SUBSTITUTE($G8,U$1,"")))/LEN(U$1) +
-(LEN($H8)-LEN(SUBSTITUTE($H8,U$1,"")))/LEN(U$1) +
-(LEN($I8)-LEN(SUBSTITUTE($I8,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="V8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="W8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B9" s="34">
         <v>2</v>
@@ -2876,30 +2824,25 @@
         <v>2</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="J9" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D9 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E9 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F9 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G9 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H9 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I9 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Rake%n🔓🔓🔊➜
 3: Bribe%n$ 🔊➜
@@ -2909,82 +2852,47 @@
 </v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L9" s="27"/>
       <c r="M9" s="34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N9" s="18"/>
       <c r="O9" s="10">
-        <f>(LEN($D9)-LEN(SUBSTITUTE($D9,O$1,"")))/LEN(O$1) +
-(LEN($E9)-LEN(SUBSTITUTE($E9,O$1,"")))/LEN(O$1) +
-(LEN($F9)-LEN(SUBSTITUTE($F9,O$1,"")))/LEN(O$1) +
-(LEN($G9)-LEN(SUBSTITUTE($G9,O$1,"")))/LEN(O$1) +
-(LEN($H9)-LEN(SUBSTITUTE($H9,O$1,"")))/LEN(O$1) +
-(LEN($I9)-LEN(SUBSTITUTE($I9,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="P9" s="10">
-        <f>(LEN($D9)-LEN(SUBSTITUTE($D9,P$1,"")))/LEN(P$1) +
-(LEN($E9)-LEN(SUBSTITUTE($E9,P$1,"")))/LEN(P$1) +
-(LEN($F9)-LEN(SUBSTITUTE($F9,P$1,"")))/LEN(P$1) +
-(LEN($G9)-LEN(SUBSTITUTE($G9,P$1,"")))/LEN(P$1) +
-(LEN($H9)-LEN(SUBSTITUTE($H9,P$1,"")))/LEN(P$1) +
-(LEN($I9)-LEN(SUBSTITUTE($I9,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="Q9" s="10">
-        <f>(LEN($D9)-LEN(SUBSTITUTE($D9,Q$1,"")))/LEN(Q$1) +
-(LEN($E9)-LEN(SUBSTITUTE($E9,Q$1,"")))/LEN(Q$1) +
-(LEN($F9)-LEN(SUBSTITUTE($F9,Q$1,"")))/LEN(Q$1) +
-(LEN($G9)-LEN(SUBSTITUTE($G9,Q$1,"")))/LEN(Q$1) +
-(LEN($H9)-LEN(SUBSTITUTE($H9,Q$1,"")))/LEN(Q$1) +
-(LEN($I9)-LEN(SUBSTITUTE($I9,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="R9" s="10">
-        <f>(LEN($D9)-LEN(SUBSTITUTE($D9,R$1,"")))/LEN(R$1) +
-(LEN($E9)-LEN(SUBSTITUTE($E9,R$1,"")))/LEN(R$1) +
-(LEN($F9)-LEN(SUBSTITUTE($F9,R$1,"")))/LEN(R$1) +
-(LEN($G9)-LEN(SUBSTITUTE($G9,R$1,"")))/LEN(R$1) +
-(LEN($H9)-LEN(SUBSTITUTE($H9,R$1,"")))/LEN(R$1) +
-(LEN($I9)-LEN(SUBSTITUTE($I9,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="S9" s="10">
-        <f>(LEN($D9)-LEN(SUBSTITUTE($D9,S$1,"")))/LEN(S$1) +
-(LEN($E9)-LEN(SUBSTITUTE($E9,S$1,"")))/LEN(S$1) +
-(LEN($F9)-LEN(SUBSTITUTE($F9,S$1,"")))/LEN(S$1) +
-(LEN($G9)-LEN(SUBSTITUTE($G9,S$1,"")))/LEN(S$1) +
-(LEN($H9)-LEN(SUBSTITUTE($H9,S$1,"")))/LEN(S$1) +
-(LEN($I9)-LEN(SUBSTITUTE($I9,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="T9" s="10">
-        <f>(LEN($D9)-LEN(SUBSTITUTE($D9,T$1,"")))/LEN(T$1) +
-(LEN($E9)-LEN(SUBSTITUTE($E9,T$1,"")))/LEN(T$1) +
-(LEN($F9)-LEN(SUBSTITUTE($F9,T$1,"")))/LEN(T$1) +
-(LEN($G9)-LEN(SUBSTITUTE($G9,T$1,"")))/LEN(T$1) +
-(LEN($H9)-LEN(SUBSTITUTE($H9,T$1,"")))/LEN(T$1) +
-(LEN($I9)-LEN(SUBSTITUTE($I9,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="U9" s="10">
-        <f>(LEN($D9)-LEN(SUBSTITUTE($D9,U$1,"")))/LEN(U$1) +
-(LEN($E9)-LEN(SUBSTITUTE($E9,U$1,"")))/LEN(U$1) +
-(LEN($F9)-LEN(SUBSTITUTE($F9,U$1,"")))/LEN(U$1) +
-(LEN($G9)-LEN(SUBSTITUTE($G9,U$1,"")))/LEN(U$1) +
-(LEN($H9)-LEN(SUBSTITUTE($H9,U$1,"")))/LEN(U$1) +
-(LEN($I9)-LEN(SUBSTITUTE($I9,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="V9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="W9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2999,30 +2907,25 @@
         <v>2</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H10" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="J10" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D10 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E10 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F10 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G10 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H10 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I10 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Rake%n🔓🔓🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
@@ -3032,88 +2935,53 @@
 </v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L10" s="27"/>
       <c r="M10" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N10" s="18"/>
       <c r="O10" s="10">
-        <f>(LEN($D10)-LEN(SUBSTITUTE($D10,O$1,"")))/LEN(O$1) +
-(LEN($E10)-LEN(SUBSTITUTE($E10,O$1,"")))/LEN(O$1) +
-(LEN($F10)-LEN(SUBSTITUTE($F10,O$1,"")))/LEN(O$1) +
-(LEN($G10)-LEN(SUBSTITUTE($G10,O$1,"")))/LEN(O$1) +
-(LEN($H10)-LEN(SUBSTITUTE($H10,O$1,"")))/LEN(O$1) +
-(LEN($I10)-LEN(SUBSTITUTE($I10,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P10" s="10">
-        <f>(LEN($D10)-LEN(SUBSTITUTE($D10,P$1,"")))/LEN(P$1) +
-(LEN($E10)-LEN(SUBSTITUTE($E10,P$1,"")))/LEN(P$1) +
-(LEN($F10)-LEN(SUBSTITUTE($F10,P$1,"")))/LEN(P$1) +
-(LEN($G10)-LEN(SUBSTITUTE($G10,P$1,"")))/LEN(P$1) +
-(LEN($H10)-LEN(SUBSTITUTE($H10,P$1,"")))/LEN(P$1) +
-(LEN($I10)-LEN(SUBSTITUTE($I10,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="Q10" s="10">
-        <f>(LEN($D10)-LEN(SUBSTITUTE($D10,Q$1,"")))/LEN(Q$1) +
-(LEN($E10)-LEN(SUBSTITUTE($E10,Q$1,"")))/LEN(Q$1) +
-(LEN($F10)-LEN(SUBSTITUTE($F10,Q$1,"")))/LEN(Q$1) +
-(LEN($G10)-LEN(SUBSTITUTE($G10,Q$1,"")))/LEN(Q$1) +
-(LEN($H10)-LEN(SUBSTITUTE($H10,Q$1,"")))/LEN(Q$1) +
-(LEN($I10)-LEN(SUBSTITUTE($I10,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="R10" s="10">
-        <f>(LEN($D10)-LEN(SUBSTITUTE($D10,R$1,"")))/LEN(R$1) +
-(LEN($E10)-LEN(SUBSTITUTE($E10,R$1,"")))/LEN(R$1) +
-(LEN($F10)-LEN(SUBSTITUTE($F10,R$1,"")))/LEN(R$1) +
-(LEN($G10)-LEN(SUBSTITUTE($G10,R$1,"")))/LEN(R$1) +
-(LEN($H10)-LEN(SUBSTITUTE($H10,R$1,"")))/LEN(R$1) +
-(LEN($I10)-LEN(SUBSTITUTE($I10,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S10" s="10">
-        <f>(LEN($D10)-LEN(SUBSTITUTE($D10,S$1,"")))/LEN(S$1) +
-(LEN($E10)-LEN(SUBSTITUTE($E10,S$1,"")))/LEN(S$1) +
-(LEN($F10)-LEN(SUBSTITUTE($F10,S$1,"")))/LEN(S$1) +
-(LEN($G10)-LEN(SUBSTITUTE($G10,S$1,"")))/LEN(S$1) +
-(LEN($H10)-LEN(SUBSTITUTE($H10,S$1,"")))/LEN(S$1) +
-(LEN($I10)-LEN(SUBSTITUTE($I10,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="T10" s="8">
-        <f>(LEN($D10)-LEN(SUBSTITUTE($D10,T$1,"")))/LEN(T$1) +
-(LEN($E10)-LEN(SUBSTITUTE($E10,T$1,"")))/LEN(T$1) +
-(LEN($F10)-LEN(SUBSTITUTE($F10,T$1,"")))/LEN(T$1) +
-(LEN($G10)-LEN(SUBSTITUTE($G10,T$1,"")))/LEN(T$1) +
-(LEN($H10)-LEN(SUBSTITUTE($H10,T$1,"")))/LEN(T$1) +
-(LEN($I10)-LEN(SUBSTITUTE($I10,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="U10" s="8">
-        <f>(LEN($D10)-LEN(SUBSTITUTE($D10,U$1,"")))/LEN(U$1) +
-(LEN($E10)-LEN(SUBSTITUTE($E10,U$1,"")))/LEN(U$1) +
-(LEN($F10)-LEN(SUBSTITUTE($F10,U$1,"")))/LEN(U$1) +
-(LEN($G10)-LEN(SUBSTITUTE($G10,U$1,"")))/LEN(U$1) +
-(LEN($H10)-LEN(SUBSTITUTE($H10,U$1,"")))/LEN(U$1) +
-(LEN($I10)-LEN(SUBSTITUTE($I10,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B11" s="9">
         <v>2</v>
@@ -3122,30 +2990,25 @@
         <v>2</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="J11" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D11 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E11 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F11 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G11 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H11 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I11 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Bribe%n$ 🔊➜
 2: Yoink%n 💰🔊
 3: Run%n🔊🔊➜➜
@@ -3155,80 +3018,45 @@
 </v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="O11" s="10">
-        <f>(LEN($D11)-LEN(SUBSTITUTE($D11,O$1,"")))/LEN(O$1) +
-(LEN($E11)-LEN(SUBSTITUTE($E11,O$1,"")))/LEN(O$1) +
-(LEN($F11)-LEN(SUBSTITUTE($F11,O$1,"")))/LEN(O$1) +
-(LEN($G11)-LEN(SUBSTITUTE($G11,O$1,"")))/LEN(O$1) +
-(LEN($H11)-LEN(SUBSTITUTE($H11,O$1,"")))/LEN(O$1) +
-(LEN($I11)-LEN(SUBSTITUTE($I11,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P11" s="10">
-        <f>(LEN($D11)-LEN(SUBSTITUTE($D11,P$1,"")))/LEN(P$1) +
-(LEN($E11)-LEN(SUBSTITUTE($E11,P$1,"")))/LEN(P$1) +
-(LEN($F11)-LEN(SUBSTITUTE($F11,P$1,"")))/LEN(P$1) +
-(LEN($G11)-LEN(SUBSTITUTE($G11,P$1,"")))/LEN(P$1) +
-(LEN($H11)-LEN(SUBSTITUTE($H11,P$1,"")))/LEN(P$1) +
-(LEN($I11)-LEN(SUBSTITUTE($I11,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="Q11" s="10">
-        <f>(LEN($D11)-LEN(SUBSTITUTE($D11,Q$1,"")))/LEN(Q$1) +
-(LEN($E11)-LEN(SUBSTITUTE($E11,Q$1,"")))/LEN(Q$1) +
-(LEN($F11)-LEN(SUBSTITUTE($F11,Q$1,"")))/LEN(Q$1) +
-(LEN($G11)-LEN(SUBSTITUTE($G11,Q$1,"")))/LEN(Q$1) +
-(LEN($H11)-LEN(SUBSTITUTE($H11,Q$1,"")))/LEN(Q$1) +
-(LEN($I11)-LEN(SUBSTITUTE($I11,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="R11" s="10">
-        <f>(LEN($D11)-LEN(SUBSTITUTE($D11,R$1,"")))/LEN(R$1) +
-(LEN($E11)-LEN(SUBSTITUTE($E11,R$1,"")))/LEN(R$1) +
-(LEN($F11)-LEN(SUBSTITUTE($F11,R$1,"")))/LEN(R$1) +
-(LEN($G11)-LEN(SUBSTITUTE($G11,R$1,"")))/LEN(R$1) +
-(LEN($H11)-LEN(SUBSTITUTE($H11,R$1,"")))/LEN(R$1) +
-(LEN($I11)-LEN(SUBSTITUTE($I11,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S11" s="10">
-        <f>(LEN($D11)-LEN(SUBSTITUTE($D11,S$1,"")))/LEN(S$1) +
-(LEN($E11)-LEN(SUBSTITUTE($E11,S$1,"")))/LEN(S$1) +
-(LEN($F11)-LEN(SUBSTITUTE($F11,S$1,"")))/LEN(S$1) +
-(LEN($G11)-LEN(SUBSTITUTE($G11,S$1,"")))/LEN(S$1) +
-(LEN($H11)-LEN(SUBSTITUTE($H11,S$1,"")))/LEN(S$1) +
-(LEN($I11)-LEN(SUBSTITUTE($I11,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T11" s="8">
-        <f>(LEN($D11)-LEN(SUBSTITUTE($D11,T$1,"")))/LEN(T$1) +
-(LEN($E11)-LEN(SUBSTITUTE($E11,T$1,"")))/LEN(T$1) +
-(LEN($F11)-LEN(SUBSTITUTE($F11,T$1,"")))/LEN(T$1) +
-(LEN($G11)-LEN(SUBSTITUTE($G11,T$1,"")))/LEN(T$1) +
-(LEN($H11)-LEN(SUBSTITUTE($H11,T$1,"")))/LEN(T$1) +
-(LEN($I11)-LEN(SUBSTITUTE($I11,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="U11" s="8">
-        <f>(LEN($D11)-LEN(SUBSTITUTE($D11,U$1,"")))/LEN(U$1) +
-(LEN($E11)-LEN(SUBSTITUTE($E11,U$1,"")))/LEN(U$1) +
-(LEN($F11)-LEN(SUBSTITUTE($F11,U$1,"")))/LEN(U$1) +
-(LEN($G11)-LEN(SUBSTITUTE($G11,U$1,"")))/LEN(U$1) +
-(LEN($H11)-LEN(SUBSTITUTE($H11,U$1,"")))/LEN(U$1) +
-(LEN($I11)-LEN(SUBSTITUTE($I11,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="V11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="W11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3243,30 +3071,25 @@
         <v>2</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="J12" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D12 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E12 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F12 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G12 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H12 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I12 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
@@ -3276,88 +3099,53 @@
 </v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L12" s="27"/>
       <c r="M12" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N12" s="18"/>
       <c r="O12" s="8">
-        <f>(LEN($D12)-LEN(SUBSTITUTE($D12,O$1,"")))/LEN(O$1) +
-(LEN($E12)-LEN(SUBSTITUTE($E12,O$1,"")))/LEN(O$1) +
-(LEN($F12)-LEN(SUBSTITUTE($F12,O$1,"")))/LEN(O$1) +
-(LEN($G12)-LEN(SUBSTITUTE($G12,O$1,"")))/LEN(O$1) +
-(LEN($H12)-LEN(SUBSTITUTE($H12,O$1,"")))/LEN(O$1) +
-(LEN($I12)-LEN(SUBSTITUTE($I12,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="P12" s="8">
-        <f>(LEN($D12)-LEN(SUBSTITUTE($D12,P$1,"")))/LEN(P$1) +
-(LEN($E12)-LEN(SUBSTITUTE($E12,P$1,"")))/LEN(P$1) +
-(LEN($F12)-LEN(SUBSTITUTE($F12,P$1,"")))/LEN(P$1) +
-(LEN($G12)-LEN(SUBSTITUTE($G12,P$1,"")))/LEN(P$1) +
-(LEN($H12)-LEN(SUBSTITUTE($H12,P$1,"")))/LEN(P$1) +
-(LEN($I12)-LEN(SUBSTITUTE($I12,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="Q12" s="8">
-        <f>(LEN($D12)-LEN(SUBSTITUTE($D12,Q$1,"")))/LEN(Q$1) +
-(LEN($E12)-LEN(SUBSTITUTE($E12,Q$1,"")))/LEN(Q$1) +
-(LEN($F12)-LEN(SUBSTITUTE($F12,Q$1,"")))/LEN(Q$1) +
-(LEN($G12)-LEN(SUBSTITUTE($G12,Q$1,"")))/LEN(Q$1) +
-(LEN($H12)-LEN(SUBSTITUTE($H12,Q$1,"")))/LEN(Q$1) +
-(LEN($I12)-LEN(SUBSTITUTE($I12,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="R12" s="8">
-        <f>(LEN($D12)-LEN(SUBSTITUTE($D12,R$1,"")))/LEN(R$1) +
-(LEN($E12)-LEN(SUBSTITUTE($E12,R$1,"")))/LEN(R$1) +
-(LEN($F12)-LEN(SUBSTITUTE($F12,R$1,"")))/LEN(R$1) +
-(LEN($G12)-LEN(SUBSTITUTE($G12,R$1,"")))/LEN(R$1) +
-(LEN($H12)-LEN(SUBSTITUTE($H12,R$1,"")))/LEN(R$1) +
-(LEN($I12)-LEN(SUBSTITUTE($I12,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="S12" s="8">
-        <f>(LEN($D12)-LEN(SUBSTITUTE($D12,S$1,"")))/LEN(S$1) +
-(LEN($E12)-LEN(SUBSTITUTE($E12,S$1,"")))/LEN(S$1) +
-(LEN($F12)-LEN(SUBSTITUTE($F12,S$1,"")))/LEN(S$1) +
-(LEN($G12)-LEN(SUBSTITUTE($G12,S$1,"")))/LEN(S$1) +
-(LEN($H12)-LEN(SUBSTITUTE($H12,S$1,"")))/LEN(S$1) +
-(LEN($I12)-LEN(SUBSTITUTE($I12,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T12" s="8">
-        <f>(LEN($D12)-LEN(SUBSTITUTE($D12,T$1,"")))/LEN(T$1) +
-(LEN($E12)-LEN(SUBSTITUTE($E12,T$1,"")))/LEN(T$1) +
-(LEN($F12)-LEN(SUBSTITUTE($F12,T$1,"")))/LEN(T$1) +
-(LEN($G12)-LEN(SUBSTITUTE($G12,T$1,"")))/LEN(T$1) +
-(LEN($H12)-LEN(SUBSTITUTE($H12,T$1,"")))/LEN(T$1) +
-(LEN($I12)-LEN(SUBSTITUTE($I12,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="U12" s="8">
-        <f>(LEN($D12)-LEN(SUBSTITUTE($D12,U$1,"")))/LEN(U$1) +
-(LEN($E12)-LEN(SUBSTITUTE($E12,U$1,"")))/LEN(U$1) +
-(LEN($F12)-LEN(SUBSTITUTE($F12,U$1,"")))/LEN(U$1) +
-(LEN($G12)-LEN(SUBSTITUTE($G12,U$1,"")))/LEN(U$1) +
-(LEN($H12)-LEN(SUBSTITUTE($H12,U$1,"")))/LEN(U$1) +
-(LEN($I12)-LEN(SUBSTITUTE($I12,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="V12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B13" s="9">
         <v>2</v>
@@ -3366,30 +3154,25 @@
         <v>2</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J13" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D13 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E13 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F13 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G13 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H13 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I13 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Hesitate%n💡
 3: Loop%n📷🔍
@@ -3399,86 +3182,51 @@
 </v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="O13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,O$1,"")))/LEN(O$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,O$1,"")))/LEN(O$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,O$1,"")))/LEN(O$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,O$1,"")))/LEN(O$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,O$1,"")))/LEN(O$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="P13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,P$1,"")))/LEN(P$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,P$1,"")))/LEN(P$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,P$1,"")))/LEN(P$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,P$1,"")))/LEN(P$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,P$1,"")))/LEN(P$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="Q13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,Q$1,"")))/LEN(Q$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,Q$1,"")))/LEN(Q$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,Q$1,"")))/LEN(Q$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,Q$1,"")))/LEN(Q$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,Q$1,"")))/LEN(Q$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,R$1,"")))/LEN(R$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,R$1,"")))/LEN(R$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,R$1,"")))/LEN(R$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,R$1,"")))/LEN(R$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,R$1,"")))/LEN(R$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="S13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,S$1,"")))/LEN(S$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,S$1,"")))/LEN(S$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,S$1,"")))/LEN(S$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,S$1,"")))/LEN(S$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,S$1,"")))/LEN(S$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="T13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,T$1,"")))/LEN(T$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,T$1,"")))/LEN(T$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,T$1,"")))/LEN(T$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,T$1,"")))/LEN(T$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,T$1,"")))/LEN(T$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U13" s="10">
-        <f>(LEN($D13)-LEN(SUBSTITUTE($D13,U$1,"")))/LEN(U$1) +
-(LEN($E13)-LEN(SUBSTITUTE($E13,U$1,"")))/LEN(U$1) +
-(LEN($F13)-LEN(SUBSTITUTE($F13,U$1,"")))/LEN(U$1) +
-(LEN($G13)-LEN(SUBSTITUTE($G13,U$1,"")))/LEN(U$1) +
-(LEN($H13)-LEN(SUBSTITUTE($H13,U$1,"")))/LEN(U$1) +
-(LEN($I13)-LEN(SUBSTITUTE($I13,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="V13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="B14" s="9">
         <v>2</v>
@@ -3487,30 +3235,25 @@
         <v>2</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="J14" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D14 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E14 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F14 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G14 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H14 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I14 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Yoink%n 💰🔊
 2: Examine%n💡💡💡🔊🔊
 3: Kick%n👊🔊➜➜
@@ -3520,86 +3263,51 @@
 </v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="O14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,O$1,"")))/LEN(O$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,O$1,"")))/LEN(O$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,O$1,"")))/LEN(O$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,O$1,"")))/LEN(O$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,O$1,"")))/LEN(O$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="P14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,P$1,"")))/LEN(P$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,P$1,"")))/LEN(P$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,P$1,"")))/LEN(P$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,P$1,"")))/LEN(P$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,P$1,"")))/LEN(P$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="Q14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,Q$1,"")))/LEN(Q$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,Q$1,"")))/LEN(Q$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,Q$1,"")))/LEN(Q$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,Q$1,"")))/LEN(Q$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,Q$1,"")))/LEN(Q$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="R14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,R$1,"")))/LEN(R$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,R$1,"")))/LEN(R$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,R$1,"")))/LEN(R$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,R$1,"")))/LEN(R$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,R$1,"")))/LEN(R$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="S14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,S$1,"")))/LEN(S$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,S$1,"")))/LEN(S$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,S$1,"")))/LEN(S$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,S$1,"")))/LEN(S$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,S$1,"")))/LEN(S$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="T14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,T$1,"")))/LEN(T$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,T$1,"")))/LEN(T$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,T$1,"")))/LEN(T$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,T$1,"")))/LEN(T$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,T$1,"")))/LEN(T$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U14" s="10">
-        <f>(LEN($D14)-LEN(SUBSTITUTE($D14,U$1,"")))/LEN(U$1) +
-(LEN($E14)-LEN(SUBSTITUTE($E14,U$1,"")))/LEN(U$1) +
-(LEN($F14)-LEN(SUBSTITUTE($F14,U$1,"")))/LEN(U$1) +
-(LEN($G14)-LEN(SUBSTITUTE($G14,U$1,"")))/LEN(U$1) +
-(LEN($H14)-LEN(SUBSTITUTE($H14,U$1,"")))/LEN(U$1) +
-(LEN($I14)-LEN(SUBSTITUTE($I14,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B15" s="9">
         <v>2</v>
@@ -3608,30 +3316,25 @@
         <v>2</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="J15" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D15 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E15 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F15 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G15 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H15 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I15 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Sprint%n🔊🔊➜➜➜
 3: Slink%n💡➜
@@ -3641,80 +3344,45 @@
 </v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="O15" s="10">
-        <f>(LEN($D15)-LEN(SUBSTITUTE($D15,O$1,"")))/LEN(O$1) +
-(LEN($E15)-LEN(SUBSTITUTE($E15,O$1,"")))/LEN(O$1) +
-(LEN($F15)-LEN(SUBSTITUTE($F15,O$1,"")))/LEN(O$1) +
-(LEN($G15)-LEN(SUBSTITUTE($G15,O$1,"")))/LEN(O$1) +
-(LEN($H15)-LEN(SUBSTITUTE($H15,O$1,"")))/LEN(O$1) +
-(LEN($I15)-LEN(SUBSTITUTE($I15,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="P15" s="10">
-        <f>(LEN($D15)-LEN(SUBSTITUTE($D15,P$1,"")))/LEN(P$1) +
-(LEN($E15)-LEN(SUBSTITUTE($E15,P$1,"")))/LEN(P$1) +
-(LEN($F15)-LEN(SUBSTITUTE($F15,P$1,"")))/LEN(P$1) +
-(LEN($G15)-LEN(SUBSTITUTE($G15,P$1,"")))/LEN(P$1) +
-(LEN($H15)-LEN(SUBSTITUTE($H15,P$1,"")))/LEN(P$1) +
-(LEN($I15)-LEN(SUBSTITUTE($I15,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="Q15" s="10">
-        <f>(LEN($D15)-LEN(SUBSTITUTE($D15,Q$1,"")))/LEN(Q$1) +
-(LEN($E15)-LEN(SUBSTITUTE($E15,Q$1,"")))/LEN(Q$1) +
-(LEN($F15)-LEN(SUBSTITUTE($F15,Q$1,"")))/LEN(Q$1) +
-(LEN($G15)-LEN(SUBSTITUTE($G15,Q$1,"")))/LEN(Q$1) +
-(LEN($H15)-LEN(SUBSTITUTE($H15,Q$1,"")))/LEN(Q$1) +
-(LEN($I15)-LEN(SUBSTITUTE($I15,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="R15" s="10">
-        <f>(LEN($D15)-LEN(SUBSTITUTE($D15,R$1,"")))/LEN(R$1) +
-(LEN($E15)-LEN(SUBSTITUTE($E15,R$1,"")))/LEN(R$1) +
-(LEN($F15)-LEN(SUBSTITUTE($F15,R$1,"")))/LEN(R$1) +
-(LEN($G15)-LEN(SUBSTITUTE($G15,R$1,"")))/LEN(R$1) +
-(LEN($H15)-LEN(SUBSTITUTE($H15,R$1,"")))/LEN(R$1) +
-(LEN($I15)-LEN(SUBSTITUTE($I15,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="S15" s="10">
-        <f>(LEN($D15)-LEN(SUBSTITUTE($D15,S$1,"")))/LEN(S$1) +
-(LEN($E15)-LEN(SUBSTITUTE($E15,S$1,"")))/LEN(S$1) +
-(LEN($F15)-LEN(SUBSTITUTE($F15,S$1,"")))/LEN(S$1) +
-(LEN($G15)-LEN(SUBSTITUTE($G15,S$1,"")))/LEN(S$1) +
-(LEN($H15)-LEN(SUBSTITUTE($H15,S$1,"")))/LEN(S$1) +
-(LEN($I15)-LEN(SUBSTITUTE($I15,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="T15" s="10">
-        <f>(LEN($D15)-LEN(SUBSTITUTE($D15,T$1,"")))/LEN(T$1) +
-(LEN($E15)-LEN(SUBSTITUTE($E15,T$1,"")))/LEN(T$1) +
-(LEN($F15)-LEN(SUBSTITUTE($F15,T$1,"")))/LEN(T$1) +
-(LEN($G15)-LEN(SUBSTITUTE($G15,T$1,"")))/LEN(T$1) +
-(LEN($H15)-LEN(SUBSTITUTE($H15,T$1,"")))/LEN(T$1) +
-(LEN($I15)-LEN(SUBSTITUTE($I15,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="U15" s="10">
-        <f>(LEN($D15)-LEN(SUBSTITUTE($D15,U$1,"")))/LEN(U$1) +
-(LEN($E15)-LEN(SUBSTITUTE($E15,U$1,"")))/LEN(U$1) +
-(LEN($F15)-LEN(SUBSTITUTE($F15,U$1,"")))/LEN(U$1) +
-(LEN($G15)-LEN(SUBSTITUTE($G15,U$1,"")))/LEN(U$1) +
-(LEN($H15)-LEN(SUBSTITUTE($H15,U$1,"")))/LEN(U$1) +
-(LEN($I15)-LEN(SUBSTITUTE($I15,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3729,30 +3397,25 @@
         <v>2</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="J16" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D16 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E16 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F16 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G16 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H16 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I16 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Spray%n📷🔊➜
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
@@ -3762,88 +3425,53 @@
 </v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L16" s="27"/>
       <c r="M16" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="8">
-        <f>(LEN($D16)-LEN(SUBSTITUTE($D16,O$1,"")))/LEN(O$1) +
-(LEN($E16)-LEN(SUBSTITUTE($E16,O$1,"")))/LEN(O$1) +
-(LEN($F16)-LEN(SUBSTITUTE($F16,O$1,"")))/LEN(O$1) +
-(LEN($G16)-LEN(SUBSTITUTE($G16,O$1,"")))/LEN(O$1) +
-(LEN($H16)-LEN(SUBSTITUTE($H16,O$1,"")))/LEN(O$1) +
-(LEN($I16)-LEN(SUBSTITUTE($I16,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="P16" s="8">
-        <f>(LEN($D16)-LEN(SUBSTITUTE($D16,P$1,"")))/LEN(P$1) +
-(LEN($E16)-LEN(SUBSTITUTE($E16,P$1,"")))/LEN(P$1) +
-(LEN($F16)-LEN(SUBSTITUTE($F16,P$1,"")))/LEN(P$1) +
-(LEN($G16)-LEN(SUBSTITUTE($G16,P$1,"")))/LEN(P$1) +
-(LEN($H16)-LEN(SUBSTITUTE($H16,P$1,"")))/LEN(P$1) +
-(LEN($I16)-LEN(SUBSTITUTE($I16,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="Q16" s="8">
-        <f>(LEN($D16)-LEN(SUBSTITUTE($D16,Q$1,"")))/LEN(Q$1) +
-(LEN($E16)-LEN(SUBSTITUTE($E16,Q$1,"")))/LEN(Q$1) +
-(LEN($F16)-LEN(SUBSTITUTE($F16,Q$1,"")))/LEN(Q$1) +
-(LEN($G16)-LEN(SUBSTITUTE($G16,Q$1,"")))/LEN(Q$1) +
-(LEN($H16)-LEN(SUBSTITUTE($H16,Q$1,"")))/LEN(Q$1) +
-(LEN($I16)-LEN(SUBSTITUTE($I16,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="R16" s="8">
-        <f>(LEN($D16)-LEN(SUBSTITUTE($D16,R$1,"")))/LEN(R$1) +
-(LEN($E16)-LEN(SUBSTITUTE($E16,R$1,"")))/LEN(R$1) +
-(LEN($F16)-LEN(SUBSTITUTE($F16,R$1,"")))/LEN(R$1) +
-(LEN($G16)-LEN(SUBSTITUTE($G16,R$1,"")))/LEN(R$1) +
-(LEN($H16)-LEN(SUBSTITUTE($H16,R$1,"")))/LEN(R$1) +
-(LEN($I16)-LEN(SUBSTITUTE($I16,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="S16" s="8">
-        <f>(LEN($D16)-LEN(SUBSTITUTE($D16,S$1,"")))/LEN(S$1) +
-(LEN($E16)-LEN(SUBSTITUTE($E16,S$1,"")))/LEN(S$1) +
-(LEN($F16)-LEN(SUBSTITUTE($F16,S$1,"")))/LEN(S$1) +
-(LEN($G16)-LEN(SUBSTITUTE($G16,S$1,"")))/LEN(S$1) +
-(LEN($H16)-LEN(SUBSTITUTE($H16,S$1,"")))/LEN(S$1) +
-(LEN($I16)-LEN(SUBSTITUTE($I16,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T16" s="8">
-        <f>(LEN($D16)-LEN(SUBSTITUTE($D16,T$1,"")))/LEN(T$1) +
-(LEN($E16)-LEN(SUBSTITUTE($E16,T$1,"")))/LEN(T$1) +
-(LEN($F16)-LEN(SUBSTITUTE($F16,T$1,"")))/LEN(T$1) +
-(LEN($G16)-LEN(SUBSTITUTE($G16,T$1,"")))/LEN(T$1) +
-(LEN($H16)-LEN(SUBSTITUTE($H16,T$1,"")))/LEN(T$1) +
-(LEN($I16)-LEN(SUBSTITUTE($I16,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="U16" s="8">
-        <f>(LEN($D16)-LEN(SUBSTITUTE($D16,U$1,"")))/LEN(U$1) +
-(LEN($E16)-LEN(SUBSTITUTE($E16,U$1,"")))/LEN(U$1) +
-(LEN($F16)-LEN(SUBSTITUTE($F16,U$1,"")))/LEN(U$1) +
-(LEN($G16)-LEN(SUBSTITUTE($G16,U$1,"")))/LEN(U$1) +
-(LEN($H16)-LEN(SUBSTITUTE($H16,U$1,"")))/LEN(U$1) +
-(LEN($I16)-LEN(SUBSTITUTE($I16,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V16" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="W16" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B17" s="34">
         <v>2</v>
@@ -3852,30 +3480,25 @@
         <v>2</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="J17" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D17 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E17 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F17 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G17 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H17 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I17 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Disable%n📷🔊➜
 3: Pick &amp; Walk%n🔓🔊➜
@@ -3885,82 +3508,47 @@
 </v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N17" s="18"/>
       <c r="O17" s="10">
-        <f>(LEN($D17)-LEN(SUBSTITUTE($D17,O$1,"")))/LEN(O$1) +
-(LEN($E17)-LEN(SUBSTITUTE($E17,O$1,"")))/LEN(O$1) +
-(LEN($F17)-LEN(SUBSTITUTE($F17,O$1,"")))/LEN(O$1) +
-(LEN($G17)-LEN(SUBSTITUTE($G17,O$1,"")))/LEN(O$1) +
-(LEN($H17)-LEN(SUBSTITUTE($H17,O$1,"")))/LEN(O$1) +
-(LEN($I17)-LEN(SUBSTITUTE($I17,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P17" s="10">
-        <f>(LEN($D17)-LEN(SUBSTITUTE($D17,P$1,"")))/LEN(P$1) +
-(LEN($E17)-LEN(SUBSTITUTE($E17,P$1,"")))/LEN(P$1) +
-(LEN($F17)-LEN(SUBSTITUTE($F17,P$1,"")))/LEN(P$1) +
-(LEN($G17)-LEN(SUBSTITUTE($G17,P$1,"")))/LEN(P$1) +
-(LEN($H17)-LEN(SUBSTITUTE($H17,P$1,"")))/LEN(P$1) +
-(LEN($I17)-LEN(SUBSTITUTE($I17,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="Q17" s="10">
-        <f>(LEN($D17)-LEN(SUBSTITUTE($D17,Q$1,"")))/LEN(Q$1) +
-(LEN($E17)-LEN(SUBSTITUTE($E17,Q$1,"")))/LEN(Q$1) +
-(LEN($F17)-LEN(SUBSTITUTE($F17,Q$1,"")))/LEN(Q$1) +
-(LEN($G17)-LEN(SUBSTITUTE($G17,Q$1,"")))/LEN(Q$1) +
-(LEN($H17)-LEN(SUBSTITUTE($H17,Q$1,"")))/LEN(Q$1) +
-(LEN($I17)-LEN(SUBSTITUTE($I17,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="R17" s="10">
-        <f>(LEN($D17)-LEN(SUBSTITUTE($D17,R$1,"")))/LEN(R$1) +
-(LEN($E17)-LEN(SUBSTITUTE($E17,R$1,"")))/LEN(R$1) +
-(LEN($F17)-LEN(SUBSTITUTE($F17,R$1,"")))/LEN(R$1) +
-(LEN($G17)-LEN(SUBSTITUTE($G17,R$1,"")))/LEN(R$1) +
-(LEN($H17)-LEN(SUBSTITUTE($H17,R$1,"")))/LEN(R$1) +
-(LEN($I17)-LEN(SUBSTITUTE($I17,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="S17" s="10">
-        <f>(LEN($D17)-LEN(SUBSTITUTE($D17,S$1,"")))/LEN(S$1) +
-(LEN($E17)-LEN(SUBSTITUTE($E17,S$1,"")))/LEN(S$1) +
-(LEN($F17)-LEN(SUBSTITUTE($F17,S$1,"")))/LEN(S$1) +
-(LEN($G17)-LEN(SUBSTITUTE($G17,S$1,"")))/LEN(S$1) +
-(LEN($H17)-LEN(SUBSTITUTE($H17,S$1,"")))/LEN(S$1) +
-(LEN($I17)-LEN(SUBSTITUTE($I17,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="T17" s="10">
-        <f>(LEN($D17)-LEN(SUBSTITUTE($D17,T$1,"")))/LEN(T$1) +
-(LEN($E17)-LEN(SUBSTITUTE($E17,T$1,"")))/LEN(T$1) +
-(LEN($F17)-LEN(SUBSTITUTE($F17,T$1,"")))/LEN(T$1) +
-(LEN($G17)-LEN(SUBSTITUTE($G17,T$1,"")))/LEN(T$1) +
-(LEN($H17)-LEN(SUBSTITUTE($H17,T$1,"")))/LEN(T$1) +
-(LEN($I17)-LEN(SUBSTITUTE($I17,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U17" s="10">
-        <f>(LEN($D17)-LEN(SUBSTITUTE($D17,U$1,"")))/LEN(U$1) +
-(LEN($E17)-LEN(SUBSTITUTE($E17,U$1,"")))/LEN(U$1) +
-(LEN($F17)-LEN(SUBSTITUTE($F17,U$1,"")))/LEN(U$1) +
-(LEN($G17)-LEN(SUBSTITUTE($G17,U$1,"")))/LEN(U$1) +
-(LEN($H17)-LEN(SUBSTITUTE($H17,U$1,"")))/LEN(U$1) +
-(LEN($I17)-LEN(SUBSTITUTE($I17,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="V17" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W17" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3975,30 +3563,25 @@
         <v>2</v>
       </c>
       <c r="D18" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="E18" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>188</v>
-      </c>
       <c r="H18" s="10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="J18" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D18 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E18 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F18 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G18 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H18 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I18 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
 2: Slink%n💡➜
 3: Redirect%n🔓👊📷🔊
@@ -4008,78 +3591,43 @@
 </v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L18" s="18"/>
       <c r="M18" s="34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="10">
-        <f>(LEN($D18)-LEN(SUBSTITUTE($D18,O$1,"")))/LEN(O$1) +
-(LEN($E18)-LEN(SUBSTITUTE($E18,O$1,"")))/LEN(O$1) +
-(LEN($F18)-LEN(SUBSTITUTE($F18,O$1,"")))/LEN(O$1) +
-(LEN($G18)-LEN(SUBSTITUTE($G18,O$1,"")))/LEN(O$1) +
-(LEN($H18)-LEN(SUBSTITUTE($H18,O$1,"")))/LEN(O$1) +
-(LEN($I18)-LEN(SUBSTITUTE($I18,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="P18" s="10">
-        <f>(LEN($D18)-LEN(SUBSTITUTE($D18,P$1,"")))/LEN(P$1) +
-(LEN($E18)-LEN(SUBSTITUTE($E18,P$1,"")))/LEN(P$1) +
-(LEN($F18)-LEN(SUBSTITUTE($F18,P$1,"")))/LEN(P$1) +
-(LEN($G18)-LEN(SUBSTITUTE($G18,P$1,"")))/LEN(P$1) +
-(LEN($H18)-LEN(SUBSTITUTE($H18,P$1,"")))/LEN(P$1) +
-(LEN($I18)-LEN(SUBSTITUTE($I18,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="Q18" s="10">
-        <f>(LEN($D18)-LEN(SUBSTITUTE($D18,Q$1,"")))/LEN(Q$1) +
-(LEN($E18)-LEN(SUBSTITUTE($E18,Q$1,"")))/LEN(Q$1) +
-(LEN($F18)-LEN(SUBSTITUTE($F18,Q$1,"")))/LEN(Q$1) +
-(LEN($G18)-LEN(SUBSTITUTE($G18,Q$1,"")))/LEN(Q$1) +
-(LEN($H18)-LEN(SUBSTITUTE($H18,Q$1,"")))/LEN(Q$1) +
-(LEN($I18)-LEN(SUBSTITUTE($I18,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="R18" s="10">
-        <f>(LEN($D18)-LEN(SUBSTITUTE($D18,R$1,"")))/LEN(R$1) +
-(LEN($E18)-LEN(SUBSTITUTE($E18,R$1,"")))/LEN(R$1) +
-(LEN($F18)-LEN(SUBSTITUTE($F18,R$1,"")))/LEN(R$1) +
-(LEN($G18)-LEN(SUBSTITUTE($G18,R$1,"")))/LEN(R$1) +
-(LEN($H18)-LEN(SUBSTITUTE($H18,R$1,"")))/LEN(R$1) +
-(LEN($I18)-LEN(SUBSTITUTE($I18,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="S18" s="10">
-        <f>(LEN($D18)-LEN(SUBSTITUTE($D18,S$1,"")))/LEN(S$1) +
-(LEN($E18)-LEN(SUBSTITUTE($E18,S$1,"")))/LEN(S$1) +
-(LEN($F18)-LEN(SUBSTITUTE($F18,S$1,"")))/LEN(S$1) +
-(LEN($G18)-LEN(SUBSTITUTE($G18,S$1,"")))/LEN(S$1) +
-(LEN($H18)-LEN(SUBSTITUTE($H18,S$1,"")))/LEN(S$1) +
-(LEN($I18)-LEN(SUBSTITUTE($I18,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="T18" s="10">
-        <f>(LEN($D18)-LEN(SUBSTITUTE($D18,T$1,"")))/LEN(T$1) +
-(LEN($E18)-LEN(SUBSTITUTE($E18,T$1,"")))/LEN(T$1) +
-(LEN($F18)-LEN(SUBSTITUTE($F18,T$1,"")))/LEN(T$1) +
-(LEN($G18)-LEN(SUBSTITUTE($G18,T$1,"")))/LEN(T$1) +
-(LEN($H18)-LEN(SUBSTITUTE($H18,T$1,"")))/LEN(T$1) +
-(LEN($I18)-LEN(SUBSTITUTE($I18,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="U18" s="10">
-        <f>(LEN($D18)-LEN(SUBSTITUTE($D18,U$1,"")))/LEN(U$1) +
-(LEN($E18)-LEN(SUBSTITUTE($E18,U$1,"")))/LEN(U$1) +
-(LEN($F18)-LEN(SUBSTITUTE($F18,U$1,"")))/LEN(U$1) +
-(LEN($G18)-LEN(SUBSTITUTE($G18,U$1,"")))/LEN(U$1) +
-(LEN($H18)-LEN(SUBSTITUTE($H18,U$1,"")))/LEN(U$1) +
-(LEN($I18)-LEN(SUBSTITUTE($I18,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="V18" s="8">
-        <f t="shared" ref="V18:W19" si="3">(LEN($D18)-LEN(SUBSTITUTE($D18,V$1,"")))/LEN(V$1) +
+        <f t="shared" ref="V18:W19" si="7">(LEN($D18)-LEN(SUBSTITUTE($D18,V$1,"")))/LEN(V$1) +
 (LEN($E18)-LEN(SUBSTITUTE($E18,V$1,"")))/LEN(V$1) +
 (LEN($F18)-LEN(SUBSTITUTE($F18,V$1,"")))/LEN(V$1) +
 (LEN($G18)-LEN(SUBSTITUTE($G18,V$1,"")))/LEN(V$1) +
@@ -4088,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="W18" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4103,30 +3651,25 @@
         <v>2</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="I19" s="34" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="J19" s="18" t="str">
-        <f>D$1 &amp; ": " &amp; D19 &amp; CHAR(10)
-&amp; E$1 &amp; ": " &amp; E19 &amp; CHAR(10)
-&amp; F$1 &amp; ": " &amp; F19 &amp; CHAR(10)
-&amp; G$1 &amp; ": " &amp; G19 &amp; CHAR(10)
-&amp; H$1 &amp; ": " &amp; H19 &amp; CHAR(10)
-&amp; I$1 &amp; ": " &amp; I19 &amp; CHAR(10)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">1: Sneak%n🔍➜➜
 2: Sleeper Hold%n👊➜
 3: Slink%n💡➜
@@ -4136,82 +3679,47 @@
 </v>
       </c>
       <c r="K19" s="34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N19" s="18"/>
       <c r="O19" s="10">
-        <f>(LEN($D19)-LEN(SUBSTITUTE($D19,O$1,"")))/LEN(O$1) +
-(LEN($E19)-LEN(SUBSTITUTE($E19,O$1,"")))/LEN(O$1) +
-(LEN($F19)-LEN(SUBSTITUTE($F19,O$1,"")))/LEN(O$1) +
-(LEN($G19)-LEN(SUBSTITUTE($G19,O$1,"")))/LEN(O$1) +
-(LEN($H19)-LEN(SUBSTITUTE($H19,O$1,"")))/LEN(O$1) +
-(LEN($I19)-LEN(SUBSTITUTE($I19,O$1,"")))/LEN(O$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P19" s="10">
-        <f>(LEN($D19)-LEN(SUBSTITUTE($D19,P$1,"")))/LEN(P$1) +
-(LEN($E19)-LEN(SUBSTITUTE($E19,P$1,"")))/LEN(P$1) +
-(LEN($F19)-LEN(SUBSTITUTE($F19,P$1,"")))/LEN(P$1) +
-(LEN($G19)-LEN(SUBSTITUTE($G19,P$1,"")))/LEN(P$1) +
-(LEN($H19)-LEN(SUBSTITUTE($H19,P$1,"")))/LEN(P$1) +
-(LEN($I19)-LEN(SUBSTITUTE($I19,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q19" s="10">
-        <f>(LEN($D19)-LEN(SUBSTITUTE($D19,Q$1,"")))/LEN(Q$1) +
-(LEN($E19)-LEN(SUBSTITUTE($E19,Q$1,"")))/LEN(Q$1) +
-(LEN($F19)-LEN(SUBSTITUTE($F19,Q$1,"")))/LEN(Q$1) +
-(LEN($G19)-LEN(SUBSTITUTE($G19,Q$1,"")))/LEN(Q$1) +
-(LEN($H19)-LEN(SUBSTITUTE($H19,Q$1,"")))/LEN(Q$1) +
-(LEN($I19)-LEN(SUBSTITUTE($I19,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="R19" s="10">
-        <f>(LEN($D19)-LEN(SUBSTITUTE($D19,R$1,"")))/LEN(R$1) +
-(LEN($E19)-LEN(SUBSTITUTE($E19,R$1,"")))/LEN(R$1) +
-(LEN($F19)-LEN(SUBSTITUTE($F19,R$1,"")))/LEN(R$1) +
-(LEN($G19)-LEN(SUBSTITUTE($G19,R$1,"")))/LEN(R$1) +
-(LEN($H19)-LEN(SUBSTITUTE($H19,R$1,"")))/LEN(R$1) +
-(LEN($I19)-LEN(SUBSTITUTE($I19,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="S19" s="10">
-        <f>(LEN($D19)-LEN(SUBSTITUTE($D19,S$1,"")))/LEN(S$1) +
-(LEN($E19)-LEN(SUBSTITUTE($E19,S$1,"")))/LEN(S$1) +
-(LEN($F19)-LEN(SUBSTITUTE($F19,S$1,"")))/LEN(S$1) +
-(LEN($G19)-LEN(SUBSTITUTE($G19,S$1,"")))/LEN(S$1) +
-(LEN($H19)-LEN(SUBSTITUTE($H19,S$1,"")))/LEN(S$1) +
-(LEN($I19)-LEN(SUBSTITUTE($I19,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="T19" s="10">
-        <f>(LEN($D19)-LEN(SUBSTITUTE($D19,T$1,"")))/LEN(T$1) +
-(LEN($E19)-LEN(SUBSTITUTE($E19,T$1,"")))/LEN(T$1) +
-(LEN($F19)-LEN(SUBSTITUTE($F19,T$1,"")))/LEN(T$1) +
-(LEN($G19)-LEN(SUBSTITUTE($G19,T$1,"")))/LEN(T$1) +
-(LEN($H19)-LEN(SUBSTITUTE($H19,T$1,"")))/LEN(T$1) +
-(LEN($I19)-LEN(SUBSTITUTE($I19,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U19" s="10">
-        <f>(LEN($D19)-LEN(SUBSTITUTE($D19,U$1,"")))/LEN(U$1) +
-(LEN($E19)-LEN(SUBSTITUTE($E19,U$1,"")))/LEN(U$1) +
-(LEN($F19)-LEN(SUBSTITUTE($F19,U$1,"")))/LEN(U$1) +
-(LEN($G19)-LEN(SUBSTITUTE($G19,U$1,"")))/LEN(U$1) +
-(LEN($H19)-LEN(SUBSTITUTE($H19,U$1,"")))/LEN(U$1) +
-(LEN($I19)-LEN(SUBSTITUTE($I19,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="V19" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W19" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4245,15 +3753,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4269,7 +3778,7 @@
         <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4286,7 +3795,7 @@
         <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -4295,57 +3804,64 @@
         <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>141</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>149</v>
+        <v>221</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>229</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>230</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -4630,10 +4146,10 @@
         <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -4796,40 +4312,40 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="R14" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F14 &amp; CHAR(10)
@@ -4862,37 +4378,37 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>93</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>95</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>95</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>95</v>
@@ -4916,7 +4432,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
@@ -5046,7 +4562,7 @@
         <v>#REF!</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -5261,7 +4777,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -5300,7 +4816,7 @@
         <v>#REF!</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -5347,7 +4863,7 @@
         <v>#REF!</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -5394,7 +4910,7 @@
         <v>#REF!</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -5529,7 +5045,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -5652,7 +5168,7 @@
         <v>#REF!</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -5699,7 +5215,7 @@
         <v>#REF!</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -5719,7 +5235,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -5743,7 +5259,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5754,10 +5270,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5771,7 +5287,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5785,7 +5301,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5799,7 +5315,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5813,21 +5329,21 @@
         <v>5</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>42</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more character ideas merged in
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy\code\project-timber-wolf\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\code\timber-wolf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="232">
   <si>
     <t>Name</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Hacker</t>
   </si>
   <si>
-    <t>Mover</t>
-  </si>
-  <si>
     <t>Move</t>
   </si>
   <si>
@@ -451,18 +448,12 @@
     <t>Uncover 1 unknown security token anywhere</t>
   </si>
   <si>
-    <t>Looter</t>
-  </si>
-  <si>
     <t>ADRENALINE%nGain 💡 on 👊</t>
   </si>
   <si>
     <t>Sewer Rat</t>
   </si>
   <si>
-    <t>INSPIRE%nEach turn, gain a free 💡 and give it to player.</t>
-  </si>
-  <si>
     <t>DENIAL OF SERVICE%nOnce per heist, disconnect all known cameras, and lower alert by 1.</t>
   </si>
   <si>
@@ -482,12 +473,6 @@
   </si>
   <si>
     <t>Total Ideas</t>
-  </si>
-  <si>
-    <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires</t>
-  </si>
-  <si>
-    <t>DISGUISE%nMay spend 💡 to enter space with guards.</t>
   </si>
   <si>
     <t>Unplug%n📷🔊🔊➜</t>
@@ -636,15 +621,9 @@
     <t>Bash%n🔊🔊👊</t>
   </si>
   <si>
-    <t>OBSERVANT%nWhen outdoors, may spend $1k for 🔍🔍🔍</t>
-  </si>
-  <si>
     <t>LOOTER%nGain $1k each time you take "Hestitate"</t>
   </si>
   <si>
-    <t>TUNNEL%nMay begin the heist on any tile on the outside of the map for 🔊🔊🔊🔊</t>
-  </si>
-  <si>
     <t>YOU WILL REPORT IN%nWhen  👊, lower the noise level by 3. Do not change the ⚠ level.</t>
   </si>
   <si>
@@ -687,21 +666,12 @@
     <t>LevelUp2</t>
   </si>
   <si>
-    <t xml:space="preserve">GREAT IN A PINCH%nMay prevent a gate from shutting for 💡💡💡 </t>
-  </si>
-  <si>
     <t>Key In%n🔍🔓</t>
   </si>
   <si>
-    <t>ESCAPE ARTIST%nGain 💡💡💡 when escaping</t>
-  </si>
-  <si>
     <t>SLIPPERY%nGain💡when escaping</t>
   </si>
   <si>
-    <t>COMMAND &amp; CONTROL%nMay spend 💡for 🔍, up to three times per turn.%n %nINTERCEPT%nFor 💡💡💡, may prevent reinforcements. Raise alert by 2.</t>
-  </si>
-  <si>
     <t>EARLY WARNING%nOnce per turn, may 🔍%n %nMISDIRECT%nWhen outdoors, may use 💡💡💡 to change the security roll by 1.</t>
   </si>
   <si>
@@ -739,6 +709,39 @@
   </si>
   <si>
     <t>Dash%n🔊➜➜</t>
+  </si>
+  <si>
+    <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires%n %nPACKS A SQUIB%nIf busted, fakes death and escapes (still counts toward busted count).</t>
+  </si>
+  <si>
+    <t>False Alarm%n👣</t>
+  </si>
+  <si>
+    <t>DISGUISE%nMay spend 💡 to enter space with guards.%n %nSWAP DUFFEL BAGS%nIf busted, team still gains loot.</t>
+  </si>
+  <si>
+    <t>COMMAND &amp; CONTROL%nMay spend 💡for 🔍, up to three times per turn.%n %nINTERCEPT%nFor 💡💡💡⚠⚠, may prevent reinforcements.</t>
+  </si>
+  <si>
+    <t>INSPIRE%nEach turn, give a free💡 to a player of your choosing.</t>
+  </si>
+  <si>
+    <t>Tunnel Master</t>
+  </si>
+  <si>
+    <t>SEWER CRAWL%nFor 🔊🔊⚠, may treat a tile directly across 1 empty hex space as adjacent.</t>
+  </si>
+  <si>
+    <t>DIG!%nMay begin the heist on any tile on the outside of the map for 🔊🔊🔊🔊</t>
+  </si>
+  <si>
+    <t>GREAT IN A PINCH%nMay prevent a gate from shutting for 💡💡💡%n %nPACKS A SQUIB%nIf busted, fakes death and escapes (still counts toward busted count).</t>
+  </si>
+  <si>
+    <t>Guy on the Inside</t>
+  </si>
+  <si>
+    <t>THEY TRUST ME%nMay start the heist on any space without a security token.</t>
   </si>
 </sst>
 </file>
@@ -1261,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,31 +1302,31 @@
         <v>16</v>
       </c>
       <c r="F1" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="48" t="s">
-        <v>139</v>
-      </c>
       <c r="H1" s="48" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I1" s="48" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N1" s="49" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1331,7 +1334,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C2" s="28">
         <v>1</v>
@@ -1349,22 +1352,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J2" s="27" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="N2" s="28">
-        <f>F2+G2</f>
+        <f t="shared" ref="N2:N19" si="0">F2+G2</f>
         <v>4</v>
       </c>
     </row>
@@ -1373,7 +1376,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C3" s="28">
         <v>1</v>
@@ -1391,28 +1394,28 @@
         <v>2</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
       <c r="L3" s="29" t="s">
-        <v>153</v>
+        <v>221</v>
       </c>
       <c r="M3" s="29"/>
       <c r="N3" s="28">
-        <f>F3+G3</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>144</v>
+        <v>226</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C4" s="28">
         <v>1</v>
@@ -1430,19 +1433,19 @@
         <v>3</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
       <c r="L4" s="29" t="s">
-        <v>198</v>
+        <v>228</v>
       </c>
       <c r="M4" s="29"/>
       <c r="N4" s="28">
-        <f>F4+G4</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1451,7 +1454,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="35">
         <v>1</v>
@@ -1469,10 +1472,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J5" s="32" t="s">
         <v>9</v>
@@ -1481,11 +1484,11 @@
         <v>8</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M5" s="37"/>
       <c r="N5" s="35">
-        <f>F5+G5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1494,7 +1497,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="35">
         <v>1</v>
@@ -1512,19 +1515,19 @@
         <v>2</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
       <c r="L6" s="37" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="M6" s="37"/>
       <c r="N6" s="35">
-        <f>F6+G6</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1533,7 +1536,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="35">
         <v>1</v>
@@ -1548,23 +1551,23 @@
         <v>2</v>
       </c>
       <c r="G7" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="J7" s="37"/>
       <c r="K7" s="37"/>
       <c r="L7" s="37" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="M7" s="37"/>
       <c r="N7" s="35">
-        <f>F7+G7</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -1572,7 +1575,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="33">
         <v>1</v>
@@ -1590,10 +1593,10 @@
         <v>1</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="J8" s="30" t="s">
         <v>12</v>
@@ -1602,11 +1605,11 @@
         <v>10</v>
       </c>
       <c r="L8" s="36" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="M8" s="36"/>
       <c r="N8" s="33">
-        <f>F8+G8</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1615,7 +1618,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="33">
         <v>1</v>
@@ -1633,19 +1636,19 @@
         <v>3</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="36" t="s">
-        <v>154</v>
+        <v>223</v>
       </c>
       <c r="M9" s="36"/>
       <c r="N9" s="33">
-        <f>F9+G9</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1654,7 +1657,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="33">
         <v>1</v>
@@ -1672,19 +1675,19 @@
         <v>4</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
       <c r="L10" s="36" t="s">
-        <v>145</v>
+        <v>225</v>
       </c>
       <c r="M10" s="36"/>
       <c r="N10" s="33">
-        <f>F10+G10</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -1711,10 +1714,10 @@
         <v>1</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="J11" s="41" t="s">
         <v>4</v>
@@ -1723,11 +1726,11 @@
         <v>5</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M11" s="39"/>
       <c r="N11" s="42">
-        <f>F11+G11</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1754,19 +1757,19 @@
         <v>1</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J12" s="39"/>
       <c r="K12" s="39"/>
       <c r="L12" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M12" s="39"/>
       <c r="N12" s="42">
-        <f>F12+G12</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1793,19 +1796,19 @@
         <v>1</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
       <c r="L13" s="39" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="M13" s="39"/>
       <c r="N13" s="42">
-        <f>F13+G13</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -1814,7 +1817,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
       <c r="C14" s="34">
         <v>1</v>
@@ -1832,10 +1835,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="J14" s="31" t="s">
         <v>14</v>
@@ -1844,19 +1847,19 @@
         <v>15</v>
       </c>
       <c r="L14" s="38" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="N14" s="34">
-        <f>F14+G14</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>21</v>
       </c>
       <c r="C15" s="34">
         <v>1</v>
@@ -1874,16 +1877,16 @@
         <v>2</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L15" s="38" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
       <c r="N15" s="34">
-        <f>F15+G15</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1892,7 +1895,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C16" s="34">
         <v>1</v>
@@ -1910,28 +1913,28 @@
         <v>3</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
       <c r="L16" s="38" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M16" s="38"/>
       <c r="N16" s="34">
-        <f>F16+G16</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C17" s="44">
         <v>1</v>
@@ -1949,32 +1952,32 @@
         <v>2</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="J17" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="K17" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="40" t="s">
         <v>208</v>
-      </c>
-      <c r="K17" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="L17" s="40" t="s">
-        <v>218</v>
       </c>
       <c r="M17" s="40"/>
       <c r="N17" s="44">
-        <f>F17+G17</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C18" s="44">
         <v>1</v>
@@ -1992,25 +1995,25 @@
         <v>3</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I18" s="44" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L18" s="40" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="N18" s="44">
-        <f>F18+G18</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>41</v>
+        <v>230</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C19" s="44">
         <v>1</v>
@@ -2028,16 +2031,16 @@
         <v>1</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I19" s="44" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="L19" s="40" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="N19" s="44">
-        <f>F19+G19</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -2058,7 +2061,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,54 +2120,54 @@
         <v>6</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -2173,22 +2176,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J2" s="10" t="str">
         <f t="shared" ref="J2:J5" si="0">D$1 &amp; ": " &amp; D2 &amp; CHAR(10)
@@ -2206,7 +2209,7 @@
 </v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="L2" s="11" t="str">
         <f t="shared" ref="L2:L7" si="1">VLOOKUP(K2,$A$8:$J$21,10,FALSE)</f>
@@ -2219,7 +2222,7 @@
 </v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N2" s="10" t="str">
         <f t="shared" ref="N2:N7" si="2">VLOOKUP(M2,$A$8:$J$21,10,FALSE)</f>
@@ -2275,7 +2278,7 @@
     </row>
     <row r="3" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -2284,22 +2287,22 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J3" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2312,7 +2315,7 @@
 </v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2325,7 +2328,7 @@
 </v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="N3" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2381,7 +2384,7 @@
     </row>
     <row r="4" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -2390,22 +2393,22 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J4" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2418,7 +2421,7 @@
 </v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L4" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2431,7 +2434,7 @@
 </v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="N4" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2482,7 +2485,7 @@
     </row>
     <row r="5" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -2491,22 +2494,22 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J5" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2519,7 +2522,7 @@
 </v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="L5" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2532,7 +2535,7 @@
 </v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N5" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2583,7 +2586,7 @@
     </row>
     <row r="6" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -2592,22 +2595,22 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J6" s="10" t="str">
         <f>D$1 &amp; ": " &amp; D6 &amp; CHAR(10)
@@ -2625,7 +2628,7 @@
 </v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L6" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2638,7 +2641,7 @@
 </v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="N6" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2651,7 +2654,7 @@
 </v>
       </c>
       <c r="O6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O6:W6" si="5">(LEN($D6)-LEN(SUBSTITUTE($D6,O$1,"")))/LEN(O$1) +
 (LEN($E6)-LEN(SUBSTITUTE($E6,O$1,"")))/LEN(O$1) +
 (LEN($F6)-LEN(SUBSTITUTE($F6,O$1,"")))/LEN(O$1) +
 (LEN($G6)-LEN(SUBSTITUTE($G6,O$1,"")))/LEN(O$1) +
@@ -2660,81 +2663,41 @@
         <v>4</v>
       </c>
       <c r="P6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,P$1,"")))/LEN(P$1) +
-(LEN($E6)-LEN(SUBSTITUTE($E6,P$1,"")))/LEN(P$1) +
-(LEN($F6)-LEN(SUBSTITUTE($F6,P$1,"")))/LEN(P$1) +
-(LEN($G6)-LEN(SUBSTITUTE($G6,P$1,"")))/LEN(P$1) +
-(LEN($H6)-LEN(SUBSTITUTE($H6,P$1,"")))/LEN(P$1) +
-(LEN($I6)-LEN(SUBSTITUTE($I6,P$1,"")))/LEN(P$1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="Q6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,Q$1,"")))/LEN(Q$1) +
-(LEN($E6)-LEN(SUBSTITUTE($E6,Q$1,"")))/LEN(Q$1) +
-(LEN($F6)-LEN(SUBSTITUTE($F6,Q$1,"")))/LEN(Q$1) +
-(LEN($G6)-LEN(SUBSTITUTE($G6,Q$1,"")))/LEN(Q$1) +
-(LEN($H6)-LEN(SUBSTITUTE($H6,Q$1,"")))/LEN(Q$1) +
-(LEN($I6)-LEN(SUBSTITUTE($I6,Q$1,"")))/LEN(Q$1)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="R6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,R$1,"")))/LEN(R$1) +
-(LEN($E6)-LEN(SUBSTITUTE($E6,R$1,"")))/LEN(R$1) +
-(LEN($F6)-LEN(SUBSTITUTE($F6,R$1,"")))/LEN(R$1) +
-(LEN($G6)-LEN(SUBSTITUTE($G6,R$1,"")))/LEN(R$1) +
-(LEN($H6)-LEN(SUBSTITUTE($H6,R$1,"")))/LEN(R$1) +
-(LEN($I6)-LEN(SUBSTITUTE($I6,R$1,"")))/LEN(R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,S$1,"")))/LEN(S$1) +
-(LEN($E6)-LEN(SUBSTITUTE($E6,S$1,"")))/LEN(S$1) +
-(LEN($F6)-LEN(SUBSTITUTE($F6,S$1,"")))/LEN(S$1) +
-(LEN($G6)-LEN(SUBSTITUTE($G6,S$1,"")))/LEN(S$1) +
-(LEN($H6)-LEN(SUBSTITUTE($H6,S$1,"")))/LEN(S$1) +
-(LEN($I6)-LEN(SUBSTITUTE($I6,S$1,"")))/LEN(S$1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="T6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,T$1,"")))/LEN(T$1) +
-(LEN($E6)-LEN(SUBSTITUTE($E6,T$1,"")))/LEN(T$1) +
-(LEN($F6)-LEN(SUBSTITUTE($F6,T$1,"")))/LEN(T$1) +
-(LEN($G6)-LEN(SUBSTITUTE($G6,T$1,"")))/LEN(T$1) +
-(LEN($H6)-LEN(SUBSTITUTE($H6,T$1,"")))/LEN(T$1) +
-(LEN($I6)-LEN(SUBSTITUTE($I6,T$1,"")))/LEN(T$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,U$1,"")))/LEN(U$1) +
-(LEN($E6)-LEN(SUBSTITUTE($E6,U$1,"")))/LEN(U$1) +
-(LEN($F6)-LEN(SUBSTITUTE($F6,U$1,"")))/LEN(U$1) +
-(LEN($G6)-LEN(SUBSTITUTE($G6,U$1,"")))/LEN(U$1) +
-(LEN($H6)-LEN(SUBSTITUTE($H6,U$1,"")))/LEN(U$1) +
-(LEN($I6)-LEN(SUBSTITUTE($I6,U$1,"")))/LEN(U$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="V6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,V$1,"")))/LEN(V$1) +
-(LEN($E6)-LEN(SUBSTITUTE($E6,V$1,"")))/LEN(V$1) +
-(LEN($F6)-LEN(SUBSTITUTE($F6,V$1,"")))/LEN(V$1) +
-(LEN($G6)-LEN(SUBSTITUTE($G6,V$1,"")))/LEN(V$1) +
-(LEN($H6)-LEN(SUBSTITUTE($H6,V$1,"")))/LEN(V$1) +
-(LEN($I6)-LEN(SUBSTITUTE($I6,V$1,"")))/LEN(V$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W6" s="3">
-        <f>(LEN($D6)-LEN(SUBSTITUTE($D6,W$1,"")))/LEN(W$1) +
-(LEN($E6)-LEN(SUBSTITUTE($E6,W$1,"")))/LEN(W$1) +
-(LEN($F6)-LEN(SUBSTITUTE($F6,W$1,"")))/LEN(W$1) +
-(LEN($G6)-LEN(SUBSTITUTE($G6,W$1,"")))/LEN(W$1) +
-(LEN($H6)-LEN(SUBSTITUTE($H6,W$1,"")))/LEN(W$1) +
-(LEN($I6)-LEN(SUBSTITUTE($I6,W$1,"")))/LEN(W$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="18">
         <v>2</v>
@@ -2743,25 +2706,25 @@
         <v>1</v>
       </c>
       <c r="D7" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="F7" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="I7" s="18" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J7" s="20" t="str">
-        <f t="shared" ref="J7:J19" si="5">D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
+        <f t="shared" ref="J7:J19" si="6">D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
 &amp; E$1 &amp; ": " &amp; E7 &amp; CHAR(10)
 &amp; F$1 &amp; ": " &amp; F7 &amp; CHAR(10)
 &amp; G$1 &amp; ": " &amp; G7 &amp; CHAR(10)
@@ -2776,7 +2739,7 @@
 </v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" s="21" t="str">
         <f t="shared" si="1"/>
@@ -2789,7 +2752,7 @@
 </v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N7" s="20" t="str">
         <f t="shared" si="2"/>
@@ -2802,7 +2765,7 @@
 </v>
       </c>
       <c r="O7" s="18">
-        <f t="shared" ref="O7:U19" si="6">(LEN($D7)-LEN(SUBSTITUTE($D7,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O7:U19" si="7">(LEN($D7)-LEN(SUBSTITUTE($D7,O$1,"")))/LEN(O$1) +
 (LEN($E7)-LEN(SUBSTITUTE($E7,O$1,"")))/LEN(O$1) +
 (LEN($F7)-LEN(SUBSTITUTE($F7,O$1,"")))/LEN(O$1) +
 (LEN($G7)-LEN(SUBSTITUTE($G7,O$1,"")))/LEN(O$1) +
@@ -2811,27 +2774,27 @@
         <v>2</v>
       </c>
       <c r="P7" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="Q7" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="R7" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S7" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T7" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="U7" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V7" s="18">
@@ -2845,7 +2808,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
@@ -2854,25 +2817,25 @@
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J8" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Bribe%n$ 🔊➜
 3: Study%n💡💡
@@ -2882,39 +2845,39 @@
 </v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N8" s="13"/>
       <c r="O8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="P8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="R8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="U8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V8" s="3">
@@ -2928,7 +2891,7 @@
     </row>
     <row r="9" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B9" s="23">
         <v>2</v>
@@ -2937,25 +2900,25 @@
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E9" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>175</v>
-      </c>
       <c r="I9" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J9" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Rake%n🔓🔓🔊➜
 3: Bribe%n$ 🔊➜
@@ -2965,39 +2928,39 @@
 </v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="23" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="P9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="Q9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="R9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="T9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="U9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V9" s="3">
@@ -3011,7 +2974,7 @@
     </row>
     <row r="10" spans="1:24" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="5">
         <v>2</v>
@@ -3020,25 +2983,25 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="I10" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="J10" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Rake%n🔓🔓🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
@@ -3048,39 +3011,39 @@
 </v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="P10" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="Q10" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="R10" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S10" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="T10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="U10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V10" s="3">
@@ -3094,7 +3057,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
@@ -3103,25 +3066,25 @@
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J11" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Bribe%n$ 🔊➜
 2: Yoink%n 💰🔊
 3: Run%n🔊🔊➜➜
@@ -3131,37 +3094,37 @@
 </v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="Q11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="R11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="U11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V11" s="3">
@@ -3175,7 +3138,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="4">
         <v>2</v>
@@ -3184,25 +3147,25 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="J12" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
@@ -3212,39 +3175,39 @@
 </v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N12" s="13"/>
       <c r="O12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="P12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="Q12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="R12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="S12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="U12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="V12" s="3">
@@ -3258,7 +3221,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B13" s="4">
         <v>2</v>
@@ -3267,25 +3230,25 @@
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="J13" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊🔊
 2: Hesitate%n💡
 3: Loop%n📷🔍
@@ -3295,37 +3258,37 @@
 </v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="P13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="Q13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="S13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="T13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="U13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="V13" s="3">
@@ -3339,7 +3302,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B14" s="4">
         <v>2</v>
@@ -3348,25 +3311,25 @@
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="J14" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Yoink%n 💰🔊
 2: Examine%n💡💡💡🔊🔊
 3: Kick%n👊🔊➜➜
@@ -3376,37 +3339,37 @@
 </v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="Q14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="R14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="T14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V14" s="3">
@@ -3420,7 +3383,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" s="4">
         <v>2</v>
@@ -3429,25 +3392,25 @@
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="J15" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
 2: Sprint%n🔊🔊➜➜➜
 3: Slink%n💡➜
@@ -3457,37 +3420,37 @@
 </v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="P15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="T15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="U15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V15" s="3">
@@ -3501,7 +3464,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4">
         <v>2</v>
@@ -3510,25 +3473,25 @@
         <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="J16" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Spray%n📷🔊➜
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
@@ -3538,39 +3501,39 @@
 </v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N16" s="13"/>
       <c r="O16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="P16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="R16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="S16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="U16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V16" s="3">
@@ -3584,7 +3547,7 @@
     </row>
     <row r="17" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B17" s="23">
         <v>2</v>
@@ -3593,25 +3556,25 @@
         <v>2</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J17" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Disable%n📷🔊➜
 3: Pick &amp; Walk%n🔓🔊➜
@@ -3621,39 +3584,39 @@
 </v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="23" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N17" s="13"/>
       <c r="O17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="P17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="Q17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="R17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="T17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="U17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V17" s="3">
@@ -3667,7 +3630,7 @@
     </row>
     <row r="18" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="23">
         <v>2</v>
@@ -3676,25 +3639,25 @@
         <v>2</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E18" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="F18" s="23" t="s">
-        <v>179</v>
-      </c>
       <c r="G18" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J18" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
 2: Slink%n💡➜
 3: Redirect%n🔓👊📷🔊
@@ -3704,43 +3667,43 @@
 </v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L18" s="13"/>
       <c r="M18" s="23" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N18" s="13"/>
       <c r="O18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="R18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="T18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="U18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V18" s="3">
-        <f t="shared" ref="V18:W19" si="7">(LEN($D18)-LEN(SUBSTITUTE($D18,V$1,"")))/LEN(V$1) +
+        <f t="shared" ref="V18:W19" si="8">(LEN($D18)-LEN(SUBSTITUTE($D18,V$1,"")))/LEN(V$1) +
 (LEN($E18)-LEN(SUBSTITUTE($E18,V$1,"")))/LEN(V$1) +
 (LEN($F18)-LEN(SUBSTITUTE($F18,V$1,"")))/LEN(V$1) +
 (LEN($G18)-LEN(SUBSTITUTE($G18,V$1,"")))/LEN(V$1) +
@@ -3749,13 +3712,13 @@
         <v>0</v>
       </c>
       <c r="W18" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="23">
         <v>2</v>
@@ -3764,25 +3727,25 @@
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="J19" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">1: Sneak%n🔍➜➜
 2: Sleeper Hold%n👊➜
 3: Slink%n💡➜
@@ -3792,47 +3755,47 @@
 </v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="23" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N19" s="13"/>
       <c r="O19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="P19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="R19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="T19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="U19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="V19" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W19" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3868,8 +3831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3879,94 +3842,94 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
         <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>103</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
         <v>105</v>
-      </c>
-      <c r="B6" t="s">
-        <v>106</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
         <v>109</v>
-      </c>
-      <c r="B7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
         <v>112</v>
-      </c>
-      <c r="B8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
         <v>140</v>
-      </c>
-      <c r="B9" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B11" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3998,55 +3961,55 @@
   <sheetData>
     <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="R7" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F7 &amp; CHAR(10)
@@ -4064,15 +4027,15 @@
         <v>#REF!</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -4081,43 +4044,43 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="Q8" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R8" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F8 &amp; CHAR(10)
@@ -4135,15 +4098,15 @@
         <v>#REF!</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -4152,10 +4115,10 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -4184,15 +4147,15 @@
         <v>#REF!</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -4201,7 +4164,7 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -4231,15 +4194,15 @@
         <v>#REF!</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -4248,13 +4211,13 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -4282,15 +4245,15 @@
         <v>#REF!</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -4299,7 +4262,7 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -4329,15 +4292,15 @@
         <v>#REF!</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -4346,43 +4309,43 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R13" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F13 &amp; CHAR(10)
@@ -4400,15 +4363,15 @@
         <v>#REF!</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -4417,40 +4380,40 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="M14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="P14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R14" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F14 &amp; CHAR(10)
@@ -4471,52 +4434,52 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L15" s="1" t="s">
+      <c r="O15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="Q15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R15" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F15 &amp; CHAR(10)
@@ -4537,10 +4500,10 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -4576,15 +4539,15 @@
         <v>#REF!</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -4620,15 +4583,15 @@
         <v>#REF!</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -4637,7 +4600,7 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -4667,15 +4630,15 @@
         <v>#REF!</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -4684,43 +4647,43 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="H19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q19" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="R19" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F19 &amp; CHAR(10)
@@ -4738,15 +4701,15 @@
         <v>#REF!</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -4755,43 +4718,43 @@
         <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="M20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="Q20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R20" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F20 &amp; CHAR(10)
@@ -4809,57 +4772,57 @@
         <v>#REF!</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="L21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R21" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F21 &amp; CHAR(10)
@@ -4877,15 +4840,15 @@
         <v>#REF!</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -4921,15 +4884,15 @@
         <v>#REF!</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
@@ -4938,7 +4901,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -4968,24 +4931,24 @@
         <v>#REF!</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>44</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>45</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -5015,15 +4978,15 @@
         <v>#REF!</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
@@ -5032,7 +4995,7 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -5062,12 +5025,12 @@
         <v>#REF!</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
@@ -5079,43 +5042,43 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="Q26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R26" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F26 &amp; CHAR(10)
@@ -5133,12 +5096,12 @@
         <v>#REF!</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
@@ -5150,7 +5113,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -5179,12 +5142,12 @@
         <v>#REF!</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
@@ -5196,7 +5159,7 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -5226,12 +5189,12 @@
         <v>#REF!</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
@@ -5243,7 +5206,7 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -5273,12 +5236,12 @@
         <v>#REF!</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
@@ -5290,7 +5253,7 @@
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -5320,7 +5283,7 @@
         <v>#REF!</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -5340,7 +5303,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -5364,7 +5327,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5375,10 +5338,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5392,7 +5355,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5406,7 +5369,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5420,7 +5383,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5434,21 +5397,21 @@
         <v>5</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last-minute tweaks before playtesting
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="236">
   <si>
     <t>Name</t>
   </si>
@@ -340,9 +340,6 @@
     <t>🔊</t>
   </si>
   <si>
-    <t>Increase the noise level by 1</t>
-  </si>
-  <si>
     <t>➜</t>
   </si>
   <si>
@@ -352,21 +349,12 @@
     <t>⚠</t>
   </si>
   <si>
-    <t>Increase alert level by 1</t>
-  </si>
-  <si>
     <t>👊</t>
   </si>
   <si>
     <t>💡</t>
   </si>
   <si>
-    <t>Add 1 idea to the current skill</t>
-  </si>
-  <si>
-    <t>Disable all cameras on or adjacent to your tile</t>
-  </si>
-  <si>
     <t>Move your pawn to an adjacent tile (that you planned)</t>
   </si>
   <si>
@@ -445,18 +433,12 @@
     <t>🔍</t>
   </si>
   <si>
-    <t>Uncover 1 unknown security token anywhere</t>
-  </si>
-  <si>
     <t>ADRENALINE%nGain 💡 on 👊</t>
   </si>
   <si>
     <t>Sewer Rat</t>
   </si>
   <si>
-    <t>DENIAL OF SERVICE%nOnce per heist, disconnect all known cameras, and lower alert by 1.</t>
-  </si>
-  <si>
     <t>Bypass</t>
   </si>
   <si>
@@ -464,9 +446,6 @@
   </si>
   <si>
     <t>Subdue 1 guard on or adjacent to your tile.</t>
-  </si>
-  <si>
-    <t>For a cost of $1k (on your person), may move into a space with a guard.</t>
   </si>
   <si>
     <t>BOLT%nMay spend 💡for ➜</t>
@@ -696,9 +675,6 @@
     <t>💰</t>
   </si>
   <si>
-    <t>Gain $1k for your person.</t>
-  </si>
-  <si>
     <t>Steal</t>
   </si>
   <si>
@@ -742,6 +718,42 @@
   </si>
   <si>
     <t>THEY TRUST ME%nMay start the heist on any space without a security token.</t>
+  </si>
+  <si>
+    <t>🚶</t>
+  </si>
+  <si>
+    <t>Toss Pebble%n🚶🔊➜</t>
+  </si>
+  <si>
+    <t>False Alarm%n🚶🔍🔊</t>
+  </si>
+  <si>
+    <t>Loot. Gain $1k for your person.</t>
+  </si>
+  <si>
+    <t>Bribe. For a cost of $1k (on your person), may move into a space with a guard.</t>
+  </si>
+  <si>
+    <t>Reveal. Uncover 1 unknown security token anywhere</t>
+  </si>
+  <si>
+    <t>Idea. Add 1 idea to the current skill</t>
+  </si>
+  <si>
+    <t>Alert. Increase alert level by 1</t>
+  </si>
+  <si>
+    <t>Noise. Increase the noise level by 1</t>
+  </si>
+  <si>
+    <t>Disable 1 ajdacent camera</t>
+  </si>
+  <si>
+    <t>Distract. Move an 1 guard on or adjacent to your tile 1 space.</t>
+  </si>
+  <si>
+    <t>DENIAL OF SERVICE%nOnce per heist, disconnect all known cameras, and lower alert by 1.%n %nACTIVATE SPRINKLERS%nWhen outdoors, may use a 🚶 on any known guard without being on or adjacent to him</t>
   </si>
 </sst>
 </file>
@@ -1264,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,31 +1314,31 @@
         <v>16</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="I1" s="48" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="M1" s="49" t="s">
         <v>24</v>
       </c>
       <c r="N1" s="49" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1334,7 +1346,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C2" s="28">
         <v>1</v>
@@ -1352,19 +1364,19 @@
         <v>1</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="J2" s="27" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="N2" s="28">
         <f t="shared" ref="N2:N19" si="0">F2+G2</f>
@@ -1376,7 +1388,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C3" s="28">
         <v>1</v>
@@ -1394,15 +1406,15 @@
         <v>2</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
       <c r="L3" s="29" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="M3" s="29"/>
       <c r="N3" s="28">
@@ -1412,10 +1424,10 @@
     </row>
     <row r="4" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C4" s="28">
         <v>1</v>
@@ -1433,15 +1445,15 @@
         <v>3</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
       <c r="L4" s="29" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="M4" s="29"/>
       <c r="N4" s="28">
@@ -1472,10 +1484,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="J5" s="32" t="s">
         <v>9</v>
@@ -1484,7 +1496,7 @@
         <v>8</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="M5" s="37"/>
       <c r="N5" s="35">
@@ -1515,15 +1527,15 @@
         <v>2</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
       <c r="L6" s="37" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="M6" s="37"/>
       <c r="N6" s="35">
@@ -1554,15 +1566,15 @@
         <v>2</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="J7" s="37"/>
       <c r="K7" s="37"/>
       <c r="L7" s="37" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="M7" s="37"/>
       <c r="N7" s="35">
@@ -1593,10 +1605,10 @@
         <v>1</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="J8" s="30" t="s">
         <v>12</v>
@@ -1605,7 +1617,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="36" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="M8" s="36"/>
       <c r="N8" s="33">
@@ -1636,15 +1648,15 @@
         <v>3</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="36" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="M9" s="36"/>
       <c r="N9" s="33">
@@ -1675,15 +1687,15 @@
         <v>4</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
       <c r="L10" s="36" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="M10" s="36"/>
       <c r="N10" s="33">
@@ -1714,10 +1726,10 @@
         <v>1</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="J11" s="41" t="s">
         <v>4</v>
@@ -1726,7 +1738,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="M11" s="39"/>
       <c r="N11" s="42">
@@ -1757,15 +1769,15 @@
         <v>1</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="J12" s="39"/>
       <c r="K12" s="39"/>
       <c r="L12" s="39" t="s">
-        <v>143</v>
+        <v>235</v>
       </c>
       <c r="M12" s="39"/>
       <c r="N12" s="42">
@@ -1796,15 +1808,15 @@
         <v>1</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
       <c r="L13" s="39" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="M13" s="39"/>
       <c r="N13" s="42">
@@ -1835,10 +1847,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="J14" s="31" t="s">
         <v>14</v>
@@ -1847,7 +1859,7 @@
         <v>15</v>
       </c>
       <c r="L14" s="38" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="N14" s="34">
         <f t="shared" si="0"/>
@@ -1856,7 +1868,7 @@
     </row>
     <row r="15" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>14</v>
@@ -1877,13 +1889,13 @@
         <v>2</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="L15" s="38" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="N15" s="34">
         <f t="shared" si="0"/>
@@ -1907,34 +1919,34 @@
         <v>12</v>
       </c>
       <c r="F16" s="34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G16" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
       <c r="L16" s="38" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="M16" s="38"/>
       <c r="N16" s="34">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C17" s="44">
         <v>1</v>
@@ -1952,19 +1964,19 @@
         <v>2</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="J17" s="43" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K17" s="43" t="s">
         <v>40</v>
       </c>
       <c r="L17" s="40" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="M17" s="40"/>
       <c r="N17" s="44">
@@ -1974,10 +1986,10 @@
     </row>
     <row r="18" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C18" s="44">
         <v>1</v>
@@ -1995,13 +2007,13 @@
         <v>3</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="I18" s="44" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="L18" s="40" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="N18" s="44">
         <f t="shared" si="0"/>
@@ -2010,10 +2022,10 @@
     </row>
     <row r="19" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C19" s="44">
         <v>1</v>
@@ -2031,13 +2043,13 @@
         <v>1</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I19" s="44" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="L19" s="40" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="N19" s="44">
         <f t="shared" si="0"/>
@@ -2061,7 +2073,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,43 +2135,43 @@
         <v>57</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>104</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>101</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="V1" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="V1" s="9" t="s">
-        <v>145</v>
-      </c>
       <c r="W1" s="9" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="X1" s="6" t="s">
         <v>28</v>
@@ -2167,7 +2179,7 @@
     </row>
     <row r="2" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -2176,22 +2188,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>152</v>
+        <v>225</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="J2" s="10" t="str">
         <f t="shared" ref="J2:J5" si="0">D$1 &amp; ": " &amp; D2 &amp; CHAR(10)
@@ -2203,13 +2215,13 @@
         <v xml:space="preserve">1: Run%n🔊🔊➜➜
 2: Unplug%n📷🔊🔊➜
 3: Shim%n🔓🔊🔊➜
-4: Punch%n👊🔊🔊➜
+4: Toss Pebble%n🚶🔊➜
 5: Study%n💡💡
 6: Run%n🔊🔊➜➜
 </v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="L2" s="11" t="str">
         <f t="shared" ref="L2:L7" si="1">VLOOKUP(K2,$A$8:$J$21,10,FALSE)</f>
@@ -2222,7 +2234,7 @@
 </v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="N2" s="10" t="str">
         <f t="shared" ref="N2:N7" si="2">VLOOKUP(M2,$A$8:$J$21,10,FALSE)</f>
@@ -2245,7 +2257,7 @@
       </c>
       <c r="P2" s="3">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q2" s="3">
         <f t="shared" si="3"/>
@@ -2257,7 +2269,7 @@
       </c>
       <c r="S2" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" s="3">
         <f t="shared" si="3"/>
@@ -2278,7 +2290,7 @@
     </row>
     <row r="3" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -2287,22 +2299,22 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J3" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2328,7 +2340,7 @@
 </v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="N3" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2384,7 +2396,7 @@
     </row>
     <row r="4" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -2393,22 +2405,22 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="J4" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2428,13 +2440,13 @@
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
-4: Loop%n📷🔍
+4: False Alarm%n🚶🔍🔊
 5: Run%n🔊🔊➜➜
 6: Rake%n🔓🔓🔊➜
 </v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="N4" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2485,7 +2497,7 @@
     </row>
     <row r="5" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -2494,22 +2506,22 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="J5" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2522,7 +2534,7 @@
 </v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="L5" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2535,7 +2547,7 @@
 </v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="N5" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2586,7 +2598,7 @@
     </row>
     <row r="6" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -2595,22 +2607,22 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>152</v>
+        <v>225</v>
       </c>
       <c r="J6" s="10" t="str">
         <f>D$1 &amp; ": " &amp; D6 &amp; CHAR(10)
@@ -2624,7 +2636,7 @@
 3: Study%n💡💡
 4: Punch%n👊🔊🔊➜
 5: Study%n💡💡
-6: Punch%n👊🔊🔊➜
+6: Toss Pebble%n🚶🔊➜
 </v>
       </c>
       <c r="K6" s="3" t="s">
@@ -2632,7 +2644,7 @@
       </c>
       <c r="L6" s="11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">1: Spray%n📷🔊➜
+        <v xml:space="preserve">1: False Alarm%n🚶🔍🔊
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
 4: Slink%n💡➜
@@ -2641,7 +2653,7 @@
 </v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="N6" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2664,7 +2676,7 @@
       </c>
       <c r="P6" s="3">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="3">
         <f t="shared" si="5"/>
@@ -2676,7 +2688,7 @@
       </c>
       <c r="S6" s="3">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T6" s="3">
         <f t="shared" si="5"/>
@@ -2697,7 +2709,7 @@
     </row>
     <row r="7" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B7" s="18">
         <v>2</v>
@@ -2706,22 +2718,22 @@
         <v>1</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="J7" s="20" t="str">
         <f t="shared" ref="J7:J19" si="6">D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
@@ -2808,7 +2820,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
@@ -2817,22 +2829,22 @@
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J8" s="13" t="str">
         <f t="shared" si="6"/>
@@ -2845,11 +2857,11 @@
 </v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="N8" s="13"/>
       <c r="O8" s="3">
@@ -2891,7 +2903,7 @@
     </row>
     <row r="9" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B9" s="23">
         <v>2</v>
@@ -2900,22 +2912,22 @@
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="J9" s="13" t="str">
         <f t="shared" si="6"/>
@@ -2928,11 +2940,11 @@
 </v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="5">
@@ -2983,22 +2995,22 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="J10" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3011,11 +3023,11 @@
 </v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="5">
@@ -3057,7 +3069,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
@@ -3066,22 +3078,22 @@
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="J11" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3094,10 +3106,10 @@
 </v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="7"/>
@@ -3147,39 +3159,39 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>170</v>
+        <v>226</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J12" s="13" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
-4: Loop%n📷🔍
+4: False Alarm%n🚶🔍🔊
 5: Run%n🔊🔊➜➜
 6: Rake%n🔓🔓🔊➜
 </v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="N12" s="13"/>
       <c r="O12" s="3">
@@ -3188,7 +3200,7 @@
       </c>
       <c r="P12" s="3">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q12" s="3">
         <f t="shared" si="7"/>
@@ -3196,7 +3208,7 @@
       </c>
       <c r="R12" s="3">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S12" s="3">
         <f t="shared" si="7"/>
@@ -3221,7 +3233,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B13" s="4">
         <v>2</v>
@@ -3230,22 +3242,22 @@
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="J13" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3258,10 +3270,10 @@
 </v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O13" s="5">
         <f t="shared" si="7"/>
@@ -3302,7 +3314,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B14" s="4">
         <v>2</v>
@@ -3311,22 +3323,22 @@
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="J14" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3339,10 +3351,10 @@
 </v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O14" s="5">
         <f t="shared" si="7"/>
@@ -3383,7 +3395,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B15" s="4">
         <v>2</v>
@@ -3392,22 +3404,22 @@
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="J15" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3420,10 +3432,10 @@
 </v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O15" s="5">
         <f t="shared" si="7"/>
@@ -3472,27 +3484,27 @@
       <c r="C16" s="4">
         <v>2</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>168</v>
+      <c r="D16" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="J16" s="13" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">1: Spray%n📷🔊➜
+        <v xml:space="preserve">1: False Alarm%n🚶🔍🔊
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
 4: Slink%n💡➜
@@ -3501,11 +3513,11 @@
 </v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="N16" s="13"/>
       <c r="O16" s="3">
@@ -3518,11 +3530,11 @@
       </c>
       <c r="Q16" s="3">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R16" s="3">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S16" s="3">
         <f t="shared" si="7"/>
@@ -3534,7 +3546,7 @@
       </c>
       <c r="U16" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16" s="3">
         <f t="shared" si="3"/>
@@ -3547,7 +3559,7 @@
     </row>
     <row r="17" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B17" s="23">
         <v>2</v>
@@ -3556,22 +3568,22 @@
         <v>2</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="J17" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3584,11 +3596,11 @@
 </v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="N17" s="13"/>
       <c r="O17" s="5">
@@ -3639,22 +3651,22 @@
         <v>2</v>
       </c>
       <c r="D18" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>181</v>
-      </c>
       <c r="H18" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="J18" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3667,11 +3679,11 @@
 </v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L18" s="13"/>
       <c r="M18" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="N18" s="13"/>
       <c r="O18" s="5">
@@ -3727,22 +3739,22 @@
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="J19" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3755,11 +3767,11 @@
 </v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="N19" s="13"/>
       <c r="O19" s="5">
@@ -3829,10 +3841,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3850,10 +3862,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3867,19 +3879,19 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>233</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -3888,48 +3900,56 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>232</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4214,10 +4234,10 @@
         <v>33</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -4380,40 +4400,40 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="R14" s="2" t="e">
         <f>Skills!D$1 &amp; ": " &amp; F14 &amp; CHAR(10)
@@ -4446,37 +4466,37 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>91</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>91</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>93</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>93</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>93</v>
@@ -4500,7 +4520,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -4630,7 +4650,7 @@
         <v>#REF!</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -4845,7 +4865,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -4884,7 +4904,7 @@
         <v>#REF!</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -4931,7 +4951,7 @@
         <v>#REF!</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -4978,7 +4998,7 @@
         <v>#REF!</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -5113,7 +5133,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -5236,7 +5256,7 @@
         <v>#REF!</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -5283,7 +5303,7 @@
         <v>#REF!</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -5303,7 +5323,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -5327,7 +5347,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5338,10 +5358,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5355,7 +5375,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5369,7 +5389,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5383,7 +5403,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5397,21 +5417,21 @@
         <v>5</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
characters: switch to global ideas
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="234">
   <si>
     <t>Name</t>
   </si>
@@ -424,12 +424,6 @@
     <t>Hurry</t>
   </si>
   <si>
-    <t>Skill1Ideas</t>
-  </si>
-  <si>
-    <t>Skill2Ideas</t>
-  </si>
-  <si>
     <t>🔍</t>
   </si>
   <si>
@@ -449,9 +443,6 @@
   </si>
   <si>
     <t>BOLT%nMay spend 💡for ➜</t>
-  </si>
-  <si>
-    <t>Total Ideas</t>
   </si>
   <si>
     <t>Unplug%n📷🔊🔊➜</t>
@@ -651,9 +642,6 @@
     <t>SLIPPERY%nGain💡when escaping</t>
   </si>
   <si>
-    <t>EARLY WARNING%nOnce per turn, may 🔍%n %nMISDIRECT%nWhen outdoors, may use 💡💡💡 to change the security roll by 1.</t>
-  </si>
-  <si>
     <t>Pick &amp; Walk%n🔓🔊➜</t>
   </si>
   <si>
@@ -690,15 +678,9 @@
     <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires%n %nPACKS A SQUIB%nIf busted, fakes death and escapes (still counts toward busted count).</t>
   </si>
   <si>
-    <t>False Alarm%n👣</t>
-  </si>
-  <si>
     <t>DISGUISE%nMay spend 💡 to enter space with guards.%n %nSWAP DUFFEL BAGS%nIf busted, team still gains loot.</t>
   </si>
   <si>
-    <t>COMMAND &amp; CONTROL%nMay spend 💡for 🔍, up to three times per turn.%n %nINTERCEPT%nFor 💡💡💡⚠⚠, may prevent reinforcements.</t>
-  </si>
-  <si>
     <t>INSPIRE%nEach turn, give a free💡 to a player of your choosing.</t>
   </si>
   <si>
@@ -754,6 +736,18 @@
   </si>
   <si>
     <t>DENIAL OF SERVICE%nOnce per heist, disconnect all known cameras, and lower alert by 1.%n %nACTIVATE SPRINKLERS%nWhen outdoors, may use a 🚶 on any known guard without being on or adjacent to him</t>
+  </si>
+  <si>
+    <t>Ideas</t>
+  </si>
+  <si>
+    <t>INTERCEPT%nFor 💡💡💡⚠⚠, may prevent reinforcements.</t>
+  </si>
+  <si>
+    <t>EARLY WARNING%nOnce per turn, may 🔍%n %nMISDIRECT%nMay use 💡💡💡 to change the security roll by 1.</t>
+  </si>
+  <si>
+    <t>False Alarm%n🚶</t>
   </si>
 </sst>
 </file>
@@ -1274,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,17 +1281,17 @@
     <col min="3" max="3" width="4.140625" style="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="46" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.42578125" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="45" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="74.28515625" style="45" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="45"/>
+    <col min="6" max="6" width="8.5703125" style="46" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="45" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="74.28515625" style="45" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="45" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -1314,39 +1308,33 @@
         <v>16</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>133</v>
+        <v>230</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>177</v>
+        <v>174</v>
+      </c>
+      <c r="I1" s="49" t="s">
+        <v>194</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>198</v>
+        <v>126</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="49" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C2" s="28">
         <v>1</v>
@@ -1360,35 +1348,31 @@
       <c r="F2" s="28">
         <v>3</v>
       </c>
-      <c r="G2" s="28">
-        <v>1</v>
+      <c r="G2" s="28" t="s">
+        <v>176</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="I2" s="28" t="s">
-        <v>182</v>
+      <c r="I2" s="27" t="s">
+        <v>6</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>183</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="N2" s="28">
-        <f t="shared" ref="N2:N19" si="0">F2+G2</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C3" s="28">
         <v>1</v>
@@ -1402,32 +1386,27 @@
       <c r="F3" s="28">
         <v>5</v>
       </c>
-      <c r="G3" s="28">
-        <v>2</v>
+      <c r="G3" s="28" t="s">
+        <v>176</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="I3" s="28" t="s">
-        <v>182</v>
-      </c>
+      <c r="I3" s="29"/>
       <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="K3" s="29" t="s">
+        <v>209</v>
+      </c>
       <c r="L3" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="M3" s="29"/>
-      <c r="N3" s="28">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C4" s="28">
         <v>1</v>
@@ -1441,27 +1420,22 @@
       <c r="F4" s="28">
         <v>4</v>
       </c>
-      <c r="G4" s="28">
-        <v>3</v>
+      <c r="G4" s="28" t="s">
+        <v>176</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>146</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="I4" s="29"/>
       <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
+      <c r="K4" s="29" t="s">
+        <v>214</v>
+      </c>
       <c r="L4" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="28">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>7</v>
       </c>
@@ -1480,31 +1454,26 @@
       <c r="F5" s="35">
         <v>3</v>
       </c>
-      <c r="G5" s="35">
-        <v>1</v>
+      <c r="G5" s="35" t="s">
+        <v>176</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>183</v>
+        <v>180</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="32" t="s">
         <v>8</v>
       </c>
+      <c r="K5" s="37" t="s">
+        <v>134</v>
+      </c>
       <c r="L5" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="M5" s="37"/>
-      <c r="N5" s="35">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="39" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
@@ -1521,29 +1490,24 @@
         <v>9</v>
       </c>
       <c r="F6" s="35">
-        <v>3</v>
-      </c>
-      <c r="G6" s="35">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>176</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="I6" s="35" t="s">
-        <v>214</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="I6" s="37"/>
       <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
+      <c r="K6" s="37" t="s">
+        <v>207</v>
+      </c>
       <c r="L6" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="M6" s="37"/>
-      <c r="N6" s="35">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>8</v>
       </c>
@@ -1560,29 +1524,24 @@
         <v>9</v>
       </c>
       <c r="F7" s="35">
-        <v>2</v>
-      </c>
-      <c r="G7" s="35">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>176</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>180</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="I7" s="37"/>
       <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
+      <c r="K7" s="37" t="s">
+        <v>182</v>
+      </c>
       <c r="L7" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="M7" s="37"/>
-      <c r="N7" s="35">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>11</v>
       </c>
@@ -1601,31 +1560,26 @@
       <c r="F8" s="33">
         <v>2</v>
       </c>
-      <c r="G8" s="33">
-        <v>1</v>
+      <c r="G8" s="33" t="s">
+        <v>176</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>178</v>
+        <v>175</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>12</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="30" t="s">
         <v>10</v>
       </c>
+      <c r="K8" s="36" t="s">
+        <v>197</v>
+      </c>
       <c r="L8" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="M8" s="36"/>
-      <c r="N8" s="33">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
@@ -1642,29 +1596,24 @@
         <v>11</v>
       </c>
       <c r="F9" s="33">
-        <v>4</v>
-      </c>
-      <c r="G9" s="33">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>208</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>146</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="I9" s="36"/>
       <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
+      <c r="K9" s="36" t="s">
+        <v>210</v>
+      </c>
       <c r="L9" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="M9" s="36"/>
-      <c r="N9" s="33">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>10</v>
       </c>
@@ -1681,29 +1630,24 @@
         <v>10</v>
       </c>
       <c r="F10" s="33">
-        <v>4</v>
-      </c>
-      <c r="G10" s="33">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>176</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>214</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="I10" s="36"/>
       <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
+      <c r="K10" s="36" t="s">
+        <v>211</v>
+      </c>
       <c r="L10" s="36" t="s">
-        <v>217</v>
-      </c>
-      <c r="M10" s="36"/>
-      <c r="N10" s="33">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>3</v>
       </c>
@@ -1722,31 +1666,26 @@
       <c r="F11" s="42">
         <v>5</v>
       </c>
-      <c r="G11" s="42">
-        <v>1</v>
+      <c r="G11" s="42" t="s">
+        <v>176</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>178</v>
+        <v>175</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>4</v>
       </c>
       <c r="J11" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="41" t="s">
         <v>5</v>
       </c>
+      <c r="K11" s="39" t="s">
+        <v>172</v>
+      </c>
       <c r="L11" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="M11" s="39"/>
-      <c r="N11" s="42">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>4</v>
       </c>
@@ -1763,29 +1702,24 @@
         <v>8</v>
       </c>
       <c r="F12" s="42">
-        <v>5</v>
-      </c>
-      <c r="G12" s="42">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>176</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="I12" s="42" t="s">
-        <v>180</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="I12" s="39"/>
       <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
+      <c r="K12" s="39" t="s">
+        <v>229</v>
+      </c>
       <c r="L12" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="M12" s="39"/>
-      <c r="N12" s="42">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>5</v>
       </c>
@@ -1802,29 +1736,24 @@
         <v>8</v>
       </c>
       <c r="F13" s="42">
-        <v>7</v>
-      </c>
-      <c r="G13" s="42">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>176</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="I13" s="42" t="s">
-        <v>148</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="I13" s="39"/>
       <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
+      <c r="K13" s="39" t="s">
+        <v>231</v>
+      </c>
       <c r="L13" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="M13" s="39"/>
-      <c r="N13" s="42">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>13</v>
       </c>
@@ -1843,32 +1772,28 @@
       <c r="F14" s="34">
         <v>2</v>
       </c>
-      <c r="G14" s="34">
-        <v>1</v>
+      <c r="G14" s="34" t="s">
+        <v>178</v>
       </c>
       <c r="H14" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="I14" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="J14" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="31" t="s">
-        <v>15</v>
-      </c>
       <c r="L14" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="N14" s="34">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>14</v>
@@ -1885,24 +1810,20 @@
       <c r="F15" s="34">
         <v>4</v>
       </c>
-      <c r="G15" s="34">
-        <v>2</v>
+      <c r="G15" s="34" t="s">
+        <v>178</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="I15" s="34" t="s">
-        <v>212</v>
+        <v>208</v>
+      </c>
+      <c r="K15" s="38" t="s">
+        <v>213</v>
       </c>
       <c r="L15" s="38" t="s">
-        <v>219</v>
-      </c>
-      <c r="N15" s="34">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="39" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>15</v>
       </c>
@@ -1921,32 +1842,27 @@
       <c r="F16" s="34">
         <v>2</v>
       </c>
-      <c r="G16" s="34">
-        <v>2</v>
+      <c r="G16" s="34" t="s">
+        <v>178</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="I16" s="34" t="s">
-        <v>178</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="I16" s="38"/>
       <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="K16" s="38" t="s">
+        <v>139</v>
+      </c>
       <c r="L16" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="M16" s="38"/>
-      <c r="N16" s="34">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="39" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C17" s="44">
         <v>1</v>
@@ -1958,38 +1874,33 @@
         <v>6</v>
       </c>
       <c r="F17" s="44">
-        <v>2</v>
-      </c>
-      <c r="G17" s="44">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>176</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="I17" s="44" t="s">
-        <v>178</v>
+        <v>175</v>
+      </c>
+      <c r="I17" s="43" t="s">
+        <v>191</v>
       </c>
       <c r="J17" s="43" t="s">
-        <v>194</v>
-      </c>
-      <c r="K17" s="43" t="s">
         <v>40</v>
       </c>
+      <c r="K17" s="40" t="s">
+        <v>232</v>
+      </c>
       <c r="L17" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="M17" s="40"/>
-      <c r="N17" s="44">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C18" s="44">
         <v>1</v>
@@ -2003,29 +1914,25 @@
       <c r="F18" s="44">
         <v>3</v>
       </c>
-      <c r="G18" s="44">
-        <v>3</v>
+      <c r="G18" s="44" t="s">
+        <v>178</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="I18" s="44" t="s">
-        <v>146</v>
+        <v>143</v>
+      </c>
+      <c r="K18" s="40" t="s">
+        <v>215</v>
       </c>
       <c r="L18" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="N18" s="44">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C19" s="44">
         <v>1</v>
@@ -2037,23 +1944,24 @@
         <v>10</v>
       </c>
       <c r="F19" s="44">
-        <v>3</v>
-      </c>
-      <c r="G19" s="44">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>176</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="I19" s="44" t="s">
-        <v>199</v>
+        <v>196</v>
+      </c>
+      <c r="K19" s="40" t="s">
+        <v>217</v>
       </c>
       <c r="L19" s="40" t="s">
-        <v>223</v>
-      </c>
-      <c r="N19" s="44">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L20" s="40" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2073,7 +1981,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,16 +2043,16 @@
         <v>57</v>
       </c>
       <c r="K1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>154</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>109</v>
@@ -2165,13 +2073,13 @@
         <v>101</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="X1" s="6" t="s">
         <v>28</v>
@@ -2188,22 +2096,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J2" s="10" t="str">
         <f t="shared" ref="J2:J5" si="0">D$1 &amp; ": " &amp; D2 &amp; CHAR(10)
@@ -2221,7 +2129,7 @@
 </v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="L2" s="11" t="str">
         <f t="shared" ref="L2:L7" si="1">VLOOKUP(K2,$A$8:$J$21,10,FALSE)</f>
@@ -2234,7 +2142,7 @@
 </v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N2" s="10" t="str">
         <f t="shared" ref="N2:N7" si="2">VLOOKUP(M2,$A$8:$J$21,10,FALSE)</f>
@@ -2299,22 +2207,22 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J3" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2340,7 +2248,7 @@
 </v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="N3" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2405,22 +2313,22 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="H4" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J4" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2446,7 +2354,7 @@
 </v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="N4" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2506,22 +2414,22 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J5" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2534,7 +2442,7 @@
 </v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="L5" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2598,7 +2506,7 @@
     </row>
     <row r="6" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -2607,22 +2515,22 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="J6" s="10" t="str">
         <f>D$1 &amp; ": " &amp; D6 &amp; CHAR(10)
@@ -2653,7 +2561,7 @@
 </v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N6" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2718,22 +2626,22 @@
         <v>1</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J7" s="20" t="str">
         <f t="shared" ref="J7:J19" si="6">D$1 &amp; ": " &amp; D7 &amp; CHAR(10)
@@ -2820,7 +2728,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
@@ -2829,22 +2737,22 @@
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J8" s="13" t="str">
         <f t="shared" si="6"/>
@@ -2857,11 +2765,11 @@
 </v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N8" s="13"/>
       <c r="O8" s="3">
@@ -2903,7 +2811,7 @@
     </row>
     <row r="9" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B9" s="23">
         <v>2</v>
@@ -2912,22 +2820,22 @@
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F9" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G9" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>163</v>
-      </c>
       <c r="I9" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J9" s="13" t="str">
         <f t="shared" si="6"/>
@@ -2940,11 +2848,11 @@
 </v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="5">
@@ -2995,22 +2903,22 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J10" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3023,11 +2931,11 @@
 </v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="5">
@@ -3069,7 +2977,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
@@ -3078,22 +2986,22 @@
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J11" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3106,10 +3014,10 @@
 </v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="7"/>
@@ -3159,22 +3067,22 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J12" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3187,11 +3095,11 @@
 </v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N12" s="13"/>
       <c r="O12" s="3">
@@ -3233,31 +3141,31 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="4">
-        <v>2</v>
-      </c>
-      <c r="C13" s="4">
-        <v>2</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="H13" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J13" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3270,10 +3178,10 @@
 </v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O13" s="5">
         <f t="shared" si="7"/>
@@ -3314,7 +3222,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B14" s="4">
         <v>2</v>
@@ -3323,22 +3231,22 @@
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>150</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J14" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3351,10 +3259,10 @@
 </v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O14" s="5">
         <f t="shared" si="7"/>
@@ -3404,22 +3312,22 @@
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J15" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3432,10 +3340,10 @@
 </v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O15" s="5">
         <f t="shared" si="7"/>
@@ -3485,22 +3393,22 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="G16" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J16" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3513,11 +3421,11 @@
 </v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N16" s="13"/>
       <c r="O16" s="3">
@@ -3559,7 +3467,7 @@
     </row>
     <row r="17" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B17" s="23">
         <v>2</v>
@@ -3568,22 +3476,22 @@
         <v>2</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J17" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3596,11 +3504,11 @@
 </v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N17" s="13"/>
       <c r="O17" s="5">
@@ -3651,22 +3559,22 @@
         <v>2</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J18" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3679,11 +3587,11 @@
 </v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L18" s="13"/>
       <c r="M18" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N18" s="13"/>
       <c r="O18" s="5">
@@ -3739,22 +3647,22 @@
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J19" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3767,11 +3675,11 @@
 </v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N19" s="13"/>
       <c r="O19" s="5">
@@ -3882,7 +3790,7 @@
         <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -3891,7 +3799,7 @@
         <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -3900,7 +3808,7 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -3909,7 +3817,7 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3917,39 +3825,39 @@
         <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -5347,7 +5255,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5358,10 +5266,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5375,7 +5283,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5389,7 +5297,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5403,7 +5311,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5417,21 +5325,21 @@
         <v>5</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
another pass on characters and skills
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,18 @@
     <sheet name="Helps" sheetId="3" r:id="rId3"/>
     <sheet name="Skill Ideas" sheetId="4" r:id="rId4"/>
     <sheet name="Character Ideas" sheetId="5" r:id="rId5"/>
+    <sheet name="Actions" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="ActionList">Actions!$A$1:$A$37</definedName>
+    <definedName name="Actions">Actions!$A$1:$A$37</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="233">
   <si>
     <t>Name</t>
   </si>
@@ -479,9 +484,6 @@
   </si>
   <si>
     <t>Upgrade2Rolls</t>
-  </si>
-  <si>
-    <t>Spin Kick%n👊👊🔊🔊</t>
   </si>
   <si>
     <t>Jab%n👊💡➜</t>
@@ -534,9 +536,6 @@
     <t>Remote Exploit</t>
   </si>
   <si>
-    <t>Packet Sniff%n💡💡🔍🔍</t>
-  </si>
-  <si>
     <t>Rampage%n👊👊🔊🔊➜➜</t>
   </si>
   <si>
@@ -573,9 +572,6 @@
     <t>Default2</t>
   </si>
   <si>
-    <t>Hesitate %n💡</t>
-  </si>
-  <si>
     <t>Walk%n🔊➜</t>
   </si>
   <si>
@@ -585,18 +581,9 @@
     <t>Crawl%n➜</t>
   </si>
   <si>
-    <t xml:space="preserve">Pick%n🔓 </t>
-  </si>
-  <si>
-    <t>Bash%n🔊🔊👊</t>
-  </si>
-  <si>
     <t>LOOTER%nGain $1k each time you take "Hestitate"</t>
   </si>
   <si>
-    <t>YOU WILL REPORT IN%nWhen  👊, lower the noise level by 3. Do not change the ⚠ level.</t>
-  </si>
-  <si>
     <t>PICKER%nGain 💡 when you 🔓%n %nMASTER KEY%nWhen outdoors, may use  💡💡 to enable one player to 🔓</t>
   </si>
   <si>
@@ -669,15 +656,9 @@
     <t>Bypasser</t>
   </si>
   <si>
-    <t>EXTORT GUARDS%nGain $1k on 👊</t>
-  </si>
-  <si>
     <t>Dash%n🔊➜➜</t>
   </si>
   <si>
-    <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires%n %nPACKS A SQUIB%nIf busted, fakes death and escapes (still counts toward busted count).</t>
-  </si>
-  <si>
     <t>DISGUISE%nMay spend 💡 to enter space with guards.%n %nSWAP DUFFEL BAGS%nIf busted, team still gains loot.</t>
   </si>
   <si>
@@ -690,12 +671,6 @@
     <t>SEWER CRAWL%nFor 🔊🔊⚠, may treat a tile directly across 1 empty hex space as adjacent.</t>
   </si>
   <si>
-    <t>DIG!%nMay begin the heist on any tile on the outside of the map for 🔊🔊🔊🔊</t>
-  </si>
-  <si>
-    <t>GREAT IN A PINCH%nMay prevent a gate from shutting for 💡💡💡%n %nPACKS A SQUIB%nIf busted, fakes death and escapes (still counts toward busted count).</t>
-  </si>
-  <si>
     <t>Guy on the Inside</t>
   </si>
   <si>
@@ -708,9 +683,6 @@
     <t>Toss Pebble%n🚶🔊➜</t>
   </si>
   <si>
-    <t>False Alarm%n🚶🔍🔊</t>
-  </si>
-  <si>
     <t>Loot. Gain $1k for your person.</t>
   </si>
   <si>
@@ -741,13 +713,43 @@
     <t>Ideas</t>
   </si>
   <si>
-    <t>INTERCEPT%nFor 💡💡💡⚠⚠, may prevent reinforcements.</t>
-  </si>
-  <si>
     <t>EARLY WARNING%nOnce per turn, may 🔍%n %nMISDIRECT%nMay use 💡💡💡 to change the security roll by 1.</t>
   </si>
   <si>
-    <t>False Alarm%n🚶</t>
+    <t>Pick%n🔓</t>
+  </si>
+  <si>
+    <t>Bribe%n$ 🔊➜</t>
+  </si>
+  <si>
+    <t>Spin Kick%n👊👊👊🔊🔊</t>
+  </si>
+  <si>
+    <t>False Alarm%n🚶🔊🔍</t>
+  </si>
+  <si>
+    <t>Misdirect%n🚶</t>
+  </si>
+  <si>
+    <t>Bash%n👊🔊</t>
+  </si>
+  <si>
+    <t>DIG!%nMay begin the heist on any non-security tile on the outside of the map for 🔊🔊🔊🔊</t>
+  </si>
+  <si>
+    <t>INTERCEPT%nFor 💡💡💡⚠, may prevent reinforcements.</t>
+  </si>
+  <si>
+    <t>EXTORT GUARDS%nMay use 💡💡 to change security roll by 1</t>
+  </si>
+  <si>
+    <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires</t>
+  </si>
+  <si>
+    <t>GREAT IN A PINCH%nMay prevent a gate from shutting for 💡💡💡%n %nPACKS A SQUIB%nIf busted, fakes death and plays next heist, but loses loot.</t>
+  </si>
+  <si>
+    <t>YOU WILL REPORT IN%nWhen  👊, lower the noise level by 2. Do not change the ⚠ level.</t>
   </si>
 </sst>
 </file>
@@ -1270,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,19 +1310,19 @@
         <v>16</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I1" s="49" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="K1" s="49" t="s">
         <v>126</v>
@@ -1334,7 +1336,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C2" s="28">
         <v>1</v>
@@ -1349,10 +1351,10 @@
         <v>3</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>179</v>
+        <v>221</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>6</v>
@@ -1361,7 +1363,7 @@
         <v>135</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="L2" s="29" t="s">
         <v>82</v>
@@ -1372,7 +1374,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C3" s="28">
         <v>1</v>
@@ -1387,15 +1389,15 @@
         <v>5</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>179</v>
+        <v>221</v>
       </c>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
       <c r="K3" s="29" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="L3" s="29" t="s">
         <v>82</v>
@@ -1403,10 +1405,10 @@
     </row>
     <row r="4" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C4" s="28">
         <v>1</v>
@@ -1421,7 +1423,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>143</v>
@@ -1429,7 +1431,7 @@
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="29" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="L4" s="29" t="s">
         <v>82</v>
@@ -1455,10 +1457,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>180</v>
+        <v>226</v>
       </c>
       <c r="I5" s="32" t="s">
         <v>9</v>
@@ -1493,15 +1495,15 @@
         <v>4</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>233</v>
+        <v>147</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="L6" s="37" t="s">
         <v>82</v>
@@ -1527,15 +1529,15 @@
         <v>4</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="37"/>
       <c r="K7" s="37" t="s">
-        <v>182</v>
+        <v>232</v>
       </c>
       <c r="L7" s="37" t="s">
         <v>82</v>
@@ -1561,10 +1563,10 @@
         <v>2</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="I8" s="30" t="s">
         <v>12</v>
@@ -1573,7 +1575,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="L8" s="36" t="s">
         <v>82</v>
@@ -1599,7 +1601,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="H9" s="33" t="s">
         <v>143</v>
@@ -1607,7 +1609,7 @@
       <c r="I9" s="36"/>
       <c r="J9" s="36"/>
       <c r="K9" s="36" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="L9" s="36" t="s">
         <v>82</v>
@@ -1633,15 +1635,15 @@
         <v>5</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
       <c r="K10" s="36" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L10" s="36" t="s">
         <v>82</v>
@@ -1667,10 +1669,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="I11" s="41" t="s">
         <v>4</v>
@@ -1679,7 +1681,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L11" s="39" t="s">
         <v>82</v>
@@ -1705,15 +1707,15 @@
         <v>6</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
       <c r="K12" s="39" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="L12" s="39" t="s">
         <v>82</v>
@@ -1739,7 +1741,7 @@
         <v>6</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H13" s="42" t="s">
         <v>145</v>
@@ -1747,7 +1749,7 @@
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
       <c r="K13" s="39" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L13" s="39" t="s">
         <v>82</v>
@@ -1773,10 +1775,10 @@
         <v>2</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="I14" s="31" t="s">
         <v>14</v>
@@ -1785,7 +1787,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="38" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="L14" s="38" t="s">
         <v>82</v>
@@ -1811,13 +1813,13 @@
         <v>4</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="K15" s="38" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="L15" s="38" t="s">
         <v>82</v>
@@ -1843,10 +1845,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="I16" s="38"/>
       <c r="J16" s="38"/>
@@ -1859,10 +1861,10 @@
     </row>
     <row r="17" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C17" s="44">
         <v>1</v>
@@ -1877,19 +1879,19 @@
         <v>4</v>
       </c>
       <c r="G17" s="44" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="I17" s="43" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="J17" s="43" t="s">
         <v>40</v>
       </c>
       <c r="K17" s="40" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="L17" s="40" t="s">
         <v>82</v>
@@ -1897,10 +1899,10 @@
     </row>
     <row r="18" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C18" s="44">
         <v>1</v>
@@ -1915,13 +1917,13 @@
         <v>3</v>
       </c>
       <c r="G18" s="44" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H18" s="44" t="s">
         <v>143</v>
       </c>
       <c r="K18" s="40" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="L18" s="40" t="s">
         <v>82</v>
@@ -1929,10 +1931,10 @@
     </row>
     <row r="19" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C19" s="44">
         <v>1</v>
@@ -1947,13 +1949,13 @@
         <v>5</v>
       </c>
       <c r="G19" s="44" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="K19" s="40" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="L19" s="40" t="s">
         <v>82</v>
@@ -1968,6 +1970,12 @@
   <sortState ref="A2:N19">
     <sortCondition ref="B2:B19"/>
   </sortState>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H19">
+      <formula1>ActionList</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1975,13 +1983,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X20"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,21 +2005,22 @@
     <col min="9" max="9" width="22.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.140625" style="10" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" style="10" customWidth="1"/>
+    <col min="12" max="12" width="13" style="10" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="10" customWidth="1"/>
+    <col min="14" max="14" width="14" style="10" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="3.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="3.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.7109375" style="4" customWidth="1"/>
-    <col min="22" max="22" width="2.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="14"/>
+    <col min="20" max="22" width="3.7109375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="2.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.28515625" style="14" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2070,22 +2079,26 @@
         <v>108</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="W1" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>129</v>
       </c>
@@ -2102,10 +2115,10 @@
         <v>140</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>143</v>
@@ -2129,7 +2142,7 @@
 </v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="L2" s="11" t="str">
         <f t="shared" ref="L2:L7" si="1">VLOOKUP(K2,$A$8:$J$21,10,FALSE)</f>
@@ -2155,7 +2168,7 @@
 </v>
       </c>
       <c r="O2" s="3">
-        <f t="shared" ref="O2:W17" si="3">(LEN($D2)-LEN(SUBSTITUTE($D2,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O2:X17" si="3">(LEN($D2)-LEN(SUBSTITUTE($D2,O$1,"")))/LEN(O$1) +
 (LEN($E2)-LEN(SUBSTITUTE($E2,O$1,"")))/LEN(O$1) +
 (LEN($F2)-LEN(SUBSTITUTE($F2,O$1,"")))/LEN(O$1) +
 (LEN($G2)-LEN(SUBSTITUTE($G2,O$1,"")))/LEN(O$1) +
@@ -2185,7 +2198,7 @@
       </c>
       <c r="U2" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="3">
         <f t="shared" si="3"/>
@@ -2195,8 +2208,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>130</v>
       </c>
@@ -2210,16 +2228,16 @@
         <v>142</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>140</v>
@@ -2227,9 +2245,9 @@
       <c r="J3" s="10" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: Punch%n👊🔊🔊➜
-2: Hesitate%n💡
+2: Yoink%n 💰🔊
 3: Shim%n🔓🔊🔊➜
-4: Hesitate%n💡
+4: Recon%n💡💡🔊🔍
 5: Shim%n🔓🔊🔊➜
 6: Unplug%n📷🔊🔊➜
 </v>
@@ -2242,13 +2260,13 @@
         <v xml:space="preserve">1: Rake%n🔓🔓🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
-4: Spin Kick%n👊👊🔊🔊
+4: Spin Kick%n👊👊👊🔊🔊
 5: Kick%n👊🔊➜➜
 6: Jab%n👊💡➜
 </v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="N3" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2261,7 +2279,7 @@
 </v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" ref="O3:U5" si="4">(LEN($D3)-LEN(SUBSTITUTE($D3,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O3:V5" si="4">(LEN($D3)-LEN(SUBSTITUTE($D3,O$1,"")))/LEN(O$1) +
 (LEN($E3)-LEN(SUBSTITUTE($E3,O$1,"")))/LEN(O$1) +
 (LEN($F3)-LEN(SUBSTITUTE($F3,O$1,"")))/LEN(O$1) +
 (LEN($G3)-LEN(SUBSTITUTE($G3,O$1,"")))/LEN(O$1) +
@@ -2271,7 +2289,7 @@
       </c>
       <c r="P3" s="3">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q3" s="3">
         <f t="shared" si="4"/>
@@ -2286,23 +2304,28 @@
         <v>1</v>
       </c>
       <c r="T3" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U3" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V3" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="W3" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X3" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Y3" s="3"/>
+    </row>
+    <row r="4" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>128</v>
       </c>
@@ -2319,7 +2342,7 @@
         <v>141</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>145</v>
+        <v>225</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>144</v>
@@ -2328,13 +2351,13 @@
         <v>140</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J4" s="10" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: Study%n💡💡
 2: Run%n🔊🔊➜➜
-3: Reveal%n🔍
+3: Misdirect%n🚶
 4: Examine%n💡💡💡🔊🔊
 5: Unplug%n📷🔊🔊➜
 6: Shim%n🔓🔊🔊➜
@@ -2348,13 +2371,13 @@
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
-4: False Alarm%n🚶🔍🔊
+4: False Alarm%n🚶🔊🔍
 5: Run%n🔊🔊➜➜
 6: Rake%n🔓🔓🔊➜
 </v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N4" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2362,8 +2385,8 @@
 2: Hesitate%n💡
 3: Loop%n📷🔍
 4: Redirect%n🔓👊📷🔊
-5: Packet Sniff%n💡💡🔍🔍
-6: Hesitate%n💡
+5: Recon%n💡💡🔊🔍
+6: Pick%n🔓
 </v>
       </c>
       <c r="O4" s="3">
@@ -2387,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="U4" s="3">
@@ -2395,15 +2418,20 @@
         <v>1</v>
       </c>
       <c r="V4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W4" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3"/>
+    </row>
+    <row r="5" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>131</v>
       </c>
@@ -2414,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>142</v>
@@ -2423,7 +2451,7 @@
         <v>141</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>147</v>
@@ -2433,21 +2461,21 @@
       </c>
       <c r="J5" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">1: Hesitate%n💡
+        <v xml:space="preserve">1: Study%n💡💡
 2: Punch%n👊🔊🔊➜
 3: Run%n🔊🔊➜➜
-4: Run%n🔊🔊➜➜
+4: Disable%n📷🔊➜
 5: Kick%n👊🔊➜➜
 6: Punch%n👊🔊🔊➜
 </v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="L5" s="11" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1: Yoink%n 💰🔊
-2: Examine%n💡💡💡🔊🔊
+2: Rake%n🔓🔓🔊➜
 3: Kick%n👊🔊➜➜
 4: Study%n💡💡
 5: Spray%n📷🔊➜
@@ -2464,31 +2492,31 @@
 3: Slink%n💡➜
 4: Rampage%n👊👊🔊🔊➜➜
 5: Detonate%n🔓👊📷🔊🔊⚠
-6: Jab%n👊💡➜
+6: Punch%n👊🔊🔊➜
 </v>
       </c>
       <c r="O5" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" s="3">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q5" s="3">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R5" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U5" s="3">
@@ -2496,17 +2524,22 @@
         <v>0</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W5" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -2518,7 +2551,7 @@
         <v>145</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>143</v>
@@ -2530,7 +2563,7 @@
         <v>143</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="J6" s="10" t="str">
         <f>D$1 &amp; ": " &amp; D6 &amp; CHAR(10)
@@ -2552,7 +2585,7 @@
       </c>
       <c r="L6" s="11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">1: False Alarm%n🚶🔍🔊
+        <v xml:space="preserve">1: False Alarm%n🚶🔊🔍
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
 4: Slink%n💡➜
@@ -2561,7 +2594,7 @@
 </v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="N6" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2574,7 +2607,7 @@
 </v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" ref="O6:W6" si="5">(LEN($D6)-LEN(SUBSTITUTE($D6,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O6:X6" si="5">(LEN($D6)-LEN(SUBSTITUTE($D6,O$1,"")))/LEN(O$1) +
 (LEN($E6)-LEN(SUBSTITUTE($E6,O$1,"")))/LEN(O$1) +
 (LEN($F6)-LEN(SUBSTITUTE($F6,O$1,"")))/LEN(O$1) +
 (LEN($G6)-LEN(SUBSTITUTE($G6,O$1,"")))/LEN(O$1) +
@@ -2599,7 +2632,7 @@
         <v>1</v>
       </c>
       <c r="T6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="U6" s="3">
@@ -2608,14 +2641,19 @@
       </c>
       <c r="V6" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X6" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>132</v>
       </c>
@@ -2635,7 +2673,7 @@
         <v>141</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>146</v>
@@ -2680,12 +2718,12 @@
 2: Sleeper Hold%n👊➜
 3: Slink%n💡➜
 4: Sleeper Hold%n👊➜
-5: Sneak%n🔍➜➜
+5: Slink%n💡➜
 6: Defeat%n🔓📷🔊➜
 </v>
       </c>
       <c r="O7" s="18">
-        <f t="shared" ref="O7:U19" si="7">(LEN($D7)-LEN(SUBSTITUTE($D7,O$1,"")))/LEN(O$1) +
+        <f t="shared" ref="O7:V19" si="7">(LEN($D7)-LEN(SUBSTITUTE($D7,O$1,"")))/LEN(O$1) +
 (LEN($E7)-LEN(SUBSTITUTE($E7,O$1,"")))/LEN(O$1) +
 (LEN($F7)-LEN(SUBSTITUTE($F7,O$1,"")))/LEN(O$1) +
 (LEN($G7)-LEN(SUBSTITUTE($G7,O$1,"")))/LEN(O$1) +
@@ -2710,25 +2748,30 @@
         <v>0</v>
       </c>
       <c r="T7" s="18">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U7" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W7" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X7" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="18"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
@@ -2737,22 +2780,22 @@
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>143</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="J8" s="13" t="str">
         <f t="shared" si="6"/>
@@ -2765,11 +2808,11 @@
 </v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N8" s="13"/>
       <c r="O8" s="3">
@@ -2793,23 +2836,28 @@
         <v>0</v>
       </c>
       <c r="T8" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U8" s="3">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V8" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="W8" s="3">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="W8" s="3">
+      <c r="X8" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>136</v>
       </c>
@@ -2823,16 +2871,16 @@
         <v>144</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>142</v>
@@ -2848,11 +2896,11 @@
 </v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="5">
@@ -2876,23 +2924,28 @@
         <v>1</v>
       </c>
       <c r="T9" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="5">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="U9" s="5">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="V9" s="3">
-        <f t="shared" si="3"/>
+      <c r="V9" s="5">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W9" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="X9" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>35</v>
       </c>
@@ -2903,7 +2956,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>141</v>
@@ -2912,30 +2965,30 @@
         <v>142</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>147</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J10" s="13" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">1: Rake%n🔓🔓🔊➜
 2: Run%n🔊🔊➜➜
 3: Punch%n👊🔊🔊➜
-4: Spin Kick%n👊👊🔊🔊
+4: Spin Kick%n👊👊👊🔊🔊
 5: Kick%n👊🔊➜➜
 6: Jab%n👊💡➜
 </v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="5">
@@ -2956,28 +3009,33 @@
       </c>
       <c r="S10" s="5">
         <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="T10" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="T10" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U10" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W10" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X10" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
@@ -2986,19 +3044,19 @@
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>141</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>141</v>
@@ -3014,10 +3072,10 @@
 </v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="7"/>
@@ -3039,24 +3097,29 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T11" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="T11" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U11" s="3">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W11" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X11" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>64</v>
       </c>
@@ -3067,39 +3130,39 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>141</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>141</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J12" s="13" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">1: Recon%n💡💡🔊🔍
 2: Loop%n📷🔍
 3: Run%n🔊🔊➜➜
-4: False Alarm%n🚶🔍🔊
+4: False Alarm%n🚶🔊🔍
 5: Run%n🔊🔊➜➜
 6: Rake%n🔓🔓🔊➜
 </v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N12" s="13"/>
       <c r="O12" s="3">
@@ -3123,25 +3186,30 @@
         <v>0</v>
       </c>
       <c r="T12" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="U12" s="3">
         <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="V12" s="3">
+        <f t="shared" si="7"/>
         <v>3</v>
-      </c>
-      <c r="V12" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
       </c>
       <c r="W12" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X12" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="4">
         <v>2</v>
@@ -3156,16 +3224,16 @@
         <v>146</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>146</v>
+        <v>221</v>
       </c>
       <c r="J13" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3173,23 +3241,23 @@
 2: Hesitate%n💡
 3: Loop%n📷🔍
 4: Redirect%n🔓👊📷🔊
-5: Packet Sniff%n💡💡🔍🔍
-6: Hesitate%n💡
+5: Recon%n💡💡🔊🔍
+6: Pick%n🔓
 </v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O13" s="5">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P13" s="5">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q13" s="5">
         <f t="shared" si="7"/>
@@ -3204,25 +3272,30 @@
         <v>1</v>
       </c>
       <c r="T13" s="5">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U13" s="5">
         <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="V13" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="V13" s="5">
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="W13" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X13" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B14" s="4">
         <v>2</v>
@@ -3231,10 +3304,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>147</v>
@@ -3243,7 +3316,7 @@
         <v>143</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>147</v>
@@ -3251,7 +3324,7 @@
       <c r="J14" s="13" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">1: Yoink%n 💰🔊
-2: Examine%n💡💡💡🔊🔊
+2: Rake%n🔓🔓🔊➜
 3: Kick%n👊🔊➜➜
 4: Study%n💡💡
 5: Spray%n📷🔊➜
@@ -3259,23 +3332,23 @@
 </v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O14" s="5">
         <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="P14" s="5">
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="P14" s="5">
+      <c r="Q14" s="5">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="Q14" s="5">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
       <c r="R14" s="5">
         <f t="shared" si="7"/>
         <v>1</v>
@@ -3285,23 +3358,28 @@
         <v>2</v>
       </c>
       <c r="T14" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U14" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V14" s="3">
-        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="V14" s="5">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W14" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="X14" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Y14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>118</v>
       </c>
@@ -3312,22 +3390,22 @@
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="J15" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3336,22 +3414,22 @@
 3: Slink%n💡➜
 4: Rampage%n👊👊🔊🔊➜➜
 5: Detonate%n🔓👊📷🔊🔊⚠
-6: Jab%n👊💡➜
+6: Punch%n👊🔊🔊➜
 </v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O15" s="5">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P15" s="5">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q15" s="5">
         <f t="shared" si="7"/>
@@ -3366,23 +3444,28 @@
         <v>4</v>
       </c>
       <c r="T15" s="5">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U15" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V15" s="3">
-        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="V15" s="5">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W15" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X15" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="3"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>69</v>
       </c>
@@ -3393,26 +3476,26 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J16" s="13" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">1: False Alarm%n🚶🔍🔊
+        <v xml:space="preserve">1: False Alarm%n🚶🔊🔍
 2: Rake%n🔓🔓🔊➜
 3: Spray%n📷🔊➜
 4: Slink%n💡➜
@@ -3421,11 +3504,11 @@
 </v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N16" s="13"/>
       <c r="O16" s="3">
@@ -3449,25 +3532,30 @@
         <v>0</v>
       </c>
       <c r="T16" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="U16" s="3">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W16" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="X16" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="3"/>
+    </row>
+    <row r="17" spans="1:25" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B17" s="23">
         <v>2</v>
@@ -3479,13 +3567,13 @@
         <v>141</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>145</v>
@@ -3504,11 +3592,11 @@
 </v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N17" s="13"/>
       <c r="O17" s="5">
@@ -3532,23 +3620,28 @@
         <v>2</v>
       </c>
       <c r="T17" s="5">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U17" s="5">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="V17" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="V17" s="5">
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="W17" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X17" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="3"/>
+    </row>
+    <row r="18" spans="1:25" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>41</v>
       </c>
@@ -3559,19 +3652,19 @@
         <v>2</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>144</v>
@@ -3587,11 +3680,11 @@
 </v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L18" s="13"/>
       <c r="M18" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N18" s="13"/>
       <c r="O18" s="5">
@@ -3616,27 +3709,32 @@
       </c>
       <c r="T18" s="5">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U18" s="5">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="V18" s="3">
-        <f t="shared" ref="V18:W19" si="8">(LEN($D18)-LEN(SUBSTITUTE($D18,V$1,"")))/LEN(V$1) +
-(LEN($E18)-LEN(SUBSTITUTE($E18,V$1,"")))/LEN(V$1) +
-(LEN($F18)-LEN(SUBSTITUTE($F18,V$1,"")))/LEN(V$1) +
-(LEN($G18)-LEN(SUBSTITUTE($G18,V$1,"")))/LEN(V$1) +
-(LEN($H18)-LEN(SUBSTITUTE($H18,V$1,"")))/LEN(V$1) +
-(LEN($I18)-LEN(SUBSTITUTE($I18,V$1,"")))/LEN(V$1)</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="V18" s="5">
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="W18" s="3">
+        <f t="shared" ref="W18:X19" si="8">(LEN($D18)-LEN(SUBSTITUTE($D18,W$1,"")))/LEN(W$1) +
+(LEN($E18)-LEN(SUBSTITUTE($E18,W$1,"")))/LEN(W$1) +
+(LEN($F18)-LEN(SUBSTITUTE($F18,W$1,"")))/LEN(W$1) +
+(LEN($G18)-LEN(SUBSTITUTE($G18,W$1,"")))/LEN(W$1) +
+(LEN($H18)-LEN(SUBSTITUTE($H18,W$1,"")))/LEN(W$1) +
+(LEN($I18)-LEN(SUBSTITUTE($I18,W$1,"")))/LEN(W$1)</f>
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y18" s="3"/>
+    </row>
+    <row r="19" spans="1:25" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>37</v>
       </c>
@@ -3647,22 +3745,22 @@
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" s="23" t="s">
         <v>167</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>169</v>
       </c>
       <c r="J19" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3670,21 +3768,21 @@
 2: Sleeper Hold%n👊➜
 3: Slink%n💡➜
 4: Sleeper Hold%n👊➜
-5: Sneak%n🔍➜➜
+5: Slink%n💡➜
 6: Defeat%n🔓📷🔊➜
 </v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N19" s="13"/>
       <c r="O19" s="5">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="7"/>
@@ -3692,7 +3790,7 @@
       </c>
       <c r="Q19" s="5">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R19" s="5">
         <f t="shared" si="7"/>
@@ -3704,22 +3802,27 @@
       </c>
       <c r="T19" s="5">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19" s="5">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="V19" s="3">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="V19" s="5">
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="W19" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X19" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="3"/>
+    </row>
+    <row r="20" spans="1:25" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -3740,8 +3843,14 @@
       <c r="S20" s="26"/>
       <c r="T20" s="26"/>
       <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I19">
+      <formula1>ActionList</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3799,7 +3908,7 @@
         <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -3808,7 +3917,7 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -3817,7 +3926,7 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3825,7 +3934,7 @@
         <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3833,7 +3942,7 @@
         <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3841,23 +3950,23 @@
         <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -5255,7 +5364,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5269,7 +5378,7 @@
         <v>135</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5283,7 +5392,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5297,7 +5406,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5311,7 +5420,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5325,21 +5434,224 @@
         <v>5</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>189</v>
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new helps! yay simpler :punch:
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -358,9 +358,6 @@
     <t>💡</t>
   </si>
   <si>
-    <t>Move your pawn to an adjacent tile (that you planned)</t>
-  </si>
-  <si>
     <t>Requires: Splice In</t>
   </si>
   <si>
@@ -439,9 +436,6 @@
     <t>Bypass</t>
   </si>
   <si>
-    <t>Subdue 1 guard on or adjacent to your tile.</t>
-  </si>
-  <si>
     <t>Unplug%n📷🔊🔊➜</t>
   </si>
   <si>
@@ -625,12 +619,6 @@
     <t>Loot. Gain $1k for your person.</t>
   </si>
   <si>
-    <t>Reveal. Uncover 1 unknown security token anywhere</t>
-  </si>
-  <si>
-    <t>Idea. Add 1 idea to the current skill</t>
-  </si>
-  <si>
     <t>Alert. Increase alert level by 1</t>
   </si>
   <si>
@@ -697,9 +685,6 @@
     <t>Disable 1 camera on or adjacent to your tile</t>
   </si>
   <si>
-    <t>Unlock 1 adjacent to your tile</t>
-  </si>
-  <si>
     <t>Good all-around with double-moves, but louder overall and fewer ideas</t>
   </si>
   <si>
@@ -785,6 +770,21 @@
   </si>
   <si>
     <t>LOOTER%n💰 each time you take "Hestitate"</t>
+  </si>
+  <si>
+    <t>Reveal 1 security token anywhere</t>
+  </si>
+  <si>
+    <t>Subdue 1 guard on or adjacent to your tile</t>
+  </si>
+  <si>
+    <t>Move to adjacent, planned, not locked tile</t>
+  </si>
+  <si>
+    <t>Unlock 1 locked, adjacent tile</t>
+  </si>
+  <si>
+    <t>Idea. Add 1 Idea to your character</t>
   </si>
 </sst>
 </file>
@@ -1459,7 +1459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -1497,22 +1497,22 @@
         <v>16</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L1" s="37" t="s">
         <v>24</v>
@@ -1523,7 +1523,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" s="16">
         <v>1</v>
@@ -1538,19 +1538,19 @@
         <v>3</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L2" s="17" t="s">
         <v>82</v>
@@ -1561,7 +1561,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C3" s="16">
         <v>1</v>
@@ -1576,15 +1576,15 @@
         <v>5</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
       <c r="K3" s="17" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L3" s="17" t="s">
         <v>82</v>
@@ -1592,10 +1592,10 @@
     </row>
     <row r="4" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C4" s="16">
         <v>1</v>
@@ -1610,15 +1610,15 @@
         <v>4</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="L4" s="17" t="s">
         <v>82</v>
@@ -1644,10 +1644,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>9</v>
@@ -1656,7 +1656,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L5" s="25" t="s">
         <v>82</v>
@@ -1682,15 +1682,15 @@
         <v>4</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
       <c r="K6" s="25" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>82</v>
@@ -1716,15 +1716,15 @@
         <v>4</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
       <c r="K7" s="25" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="L7" s="25" t="s">
         <v>82</v>
@@ -1750,10 +1750,10 @@
         <v>2</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>12</v>
@@ -1762,7 +1762,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L8" s="24" t="s">
         <v>82</v>
@@ -1788,18 +1788,18 @@
         <v>6</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1822,15 +1822,15 @@
         <v>3</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="24" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="L10" s="24" t="s">
         <v>82</v>
@@ -1856,10 +1856,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I11" s="29" t="s">
         <v>4</v>
@@ -1868,7 +1868,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="L11" s="27" t="s">
         <v>82</v>
@@ -1894,15 +1894,15 @@
         <v>6</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L12" s="27" t="s">
         <v>82</v>
@@ -1928,15 +1928,15 @@
         <v>6</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="L13" s="27" t="s">
         <v>82</v>
@@ -1962,10 +1962,10 @@
         <v>2</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>14</v>
@@ -1974,7 +1974,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="L14" s="26" t="s">
         <v>82</v>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="15" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>14</v>
@@ -2000,13 +2000,13 @@
         <v>4</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L15" s="26" t="s">
         <v>82</v>
@@ -2032,15 +2032,15 @@
         <v>2</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="L16" s="26" t="s">
         <v>82</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="17" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C17" s="32">
         <v>1</v>
@@ -2066,19 +2066,19 @@
         <v>4</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J17" s="31" t="s">
         <v>40</v>
       </c>
       <c r="K17" s="28" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="L17" s="28" t="s">
         <v>82</v>
@@ -2086,10 +2086,10 @@
     </row>
     <row r="18" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>178</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>180</v>
       </c>
       <c r="C18" s="32">
         <v>1</v>
@@ -2104,13 +2104,13 @@
         <v>3</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K18" s="28" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="L18" s="28" t="s">
         <v>82</v>
@@ -2118,10 +2118,10 @@
     </row>
     <row r="19" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C19" s="32">
         <v>1</v>
@@ -2136,13 +2136,13 @@
         <v>5</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="L19" s="28" t="s">
         <v>82</v>
@@ -2217,7 +2217,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E1" s="6">
         <v>1</v>
@@ -2241,16 +2241,16 @@
         <v>57</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>146</v>
-      </c>
       <c r="N1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>108</v>
@@ -2271,10 +2271,10 @@
         <v>101</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="X1" s="5" t="s">
         <v>28</v>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="2" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B2" s="46">
         <v>2</v>
@@ -2291,25 +2291,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F2" s="48" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H2" s="46" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K2" s="49" t="str">
         <f t="shared" ref="K2:K19" si="0">E$1 &amp; ": " &amp; E2 &amp; CHAR(10)
@@ -2334,7 +2334,7 @@
         <v>#N/A</v>
       </c>
       <c r="N2" s="46" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O2" s="49" t="e">
         <f>VLOOKUP(N2,$A$8:$K$21,10,FALSE)</f>
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -2392,25 +2392,25 @@
         <v>2</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E3" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>153</v>
-      </c>
       <c r="I3" s="48" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="K3" s="50" t="str">
         <f t="shared" si="0"/>
@@ -2423,11 +2423,11 @@
 </v>
       </c>
       <c r="L3" s="48" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M3" s="51"/>
       <c r="N3" s="48" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O3" s="50"/>
       <c r="P3" s="46">
@@ -2463,12 +2463,12 @@
         <v>2</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B4" s="53">
         <v>2</v>
@@ -2477,25 +2477,25 @@
         <v>2</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I4" s="54" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J4" s="54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K4" s="50" t="str">
         <f t="shared" si="0"/>
@@ -2508,11 +2508,11 @@
 </v>
       </c>
       <c r="L4" s="53" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M4" s="50"/>
       <c r="N4" s="53" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O4" s="50"/>
       <c r="P4" s="54">
@@ -2548,12 +2548,12 @@
         <v>0</v>
       </c>
       <c r="X4" s="45" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="44">
         <v>2</v>
@@ -2562,25 +2562,25 @@
         <v>1</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="I5" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="I5" s="44" t="s">
-        <v>140</v>
-      </c>
       <c r="J5" s="44" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K5" s="41" t="str">
         <f t="shared" si="0"/>
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="38" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -2653,25 +2653,25 @@
         <v>2</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G6" s="43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J6" s="44" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="K6" s="41" t="str">
         <f t="shared" si="0"/>
@@ -2684,11 +2684,11 @@
 </v>
       </c>
       <c r="L6" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M6" s="41"/>
       <c r="N6" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O6" s="41"/>
       <c r="P6" s="44">
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="38" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -2738,25 +2738,25 @@
         <v>2</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F7" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="43" t="s">
         <v>160</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="H7" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="I7" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="J7" s="43" t="s">
-        <v>162</v>
       </c>
       <c r="K7" s="41" t="str">
         <f t="shared" si="0"/>
@@ -2769,11 +2769,11 @@
 </v>
       </c>
       <c r="L7" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M7" s="41"/>
       <c r="N7" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="44">
@@ -2809,12 +2809,12 @@
         <v>0</v>
       </c>
       <c r="X7" s="55" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:24" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B8" s="57">
         <v>2</v>
@@ -2823,25 +2823,25 @@
         <v>1</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="59" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="59" t="s">
-        <v>149</v>
-      </c>
-      <c r="H8" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="I8" s="57" t="s">
-        <v>140</v>
-      </c>
       <c r="J8" s="57" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K8" s="60" t="str">
         <f t="shared" si="0"/>
@@ -2854,14 +2854,14 @@
 </v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M8" s="58" t="e">
         <f>VLOOKUP(L8,$A$8:$K$21,10,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="N8" s="57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O8" s="60" t="str">
         <f>VLOOKUP(N8,$A$8:$K$21,10,FALSE)</f>
@@ -2900,12 +2900,12 @@
         <v>0</v>
       </c>
       <c r="X8" s="61" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B9" s="59">
         <v>2</v>
@@ -2914,25 +2914,25 @@
         <v>2</v>
       </c>
       <c r="D9" s="60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G9" s="57" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H9" s="59" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I9" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="J9" s="59" t="s">
         <v>162</v>
-      </c>
-      <c r="J9" s="59" t="s">
-        <v>164</v>
       </c>
       <c r="K9" s="63" t="str">
         <f t="shared" si="0"/>
@@ -2945,11 +2945,11 @@
 </v>
       </c>
       <c r="L9" s="59" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M9" s="64"/>
       <c r="N9" s="59" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O9" s="63"/>
       <c r="P9" s="57">
@@ -2985,12 +2985,12 @@
         <v>0</v>
       </c>
       <c r="X9" s="65" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:24" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="66">
         <v>2</v>
@@ -2999,25 +2999,25 @@
         <v>2</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G10" s="66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H10" s="66" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I10" s="67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J10" s="67" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K10" s="63" t="str">
         <f t="shared" si="0"/>
@@ -3030,11 +3030,11 @@
 </v>
       </c>
       <c r="L10" s="66" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M10" s="64"/>
       <c r="N10" s="66" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O10" s="63"/>
       <c r="P10" s="67">
@@ -3070,12 +3070,12 @@
         <v>0</v>
       </c>
       <c r="X10" s="62" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" s="69">
         <v>2</v>
@@ -3084,25 +3084,25 @@
         <v>1</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11" s="69" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F11" s="69" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G11" s="69" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H11" s="69" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I11" s="69" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J11" s="69" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K11" s="71" t="str">
         <f t="shared" si="0"/>
@@ -3115,14 +3115,14 @@
 </v>
       </c>
       <c r="L11" s="69" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M11" s="70" t="str">
         <f>VLOOKUP(L11,$A$8:$K$21,10,FALSE)</f>
         <v>Kick%n👊🔊➜➜</v>
       </c>
       <c r="N11" s="69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O11" s="71" t="str">
         <f>VLOOKUP(N11,$A$8:$K$21,10,FALSE)</f>
@@ -3161,12 +3161,12 @@
         <v>0</v>
       </c>
       <c r="X11" s="72" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="73" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B12" s="74">
         <v>2</v>
@@ -3175,25 +3175,25 @@
         <v>2</v>
       </c>
       <c r="D12" s="71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E12" s="74" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F12" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="H12" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="I12" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="G12" s="75" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="I12" s="74" t="s">
-        <v>152</v>
-      </c>
       <c r="J12" s="75" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K12" s="76" t="str">
         <f t="shared" si="0"/>
@@ -3206,11 +3206,11 @@
 </v>
       </c>
       <c r="L12" s="74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M12" s="71"/>
       <c r="N12" s="74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O12" s="71"/>
       <c r="P12" s="75">
@@ -3251,12 +3251,12 @@
         <v>2</v>
       </c>
       <c r="X12" s="72" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="73" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="74">
         <v>2</v>
@@ -3265,25 +3265,25 @@
         <v>2</v>
       </c>
       <c r="D13" s="71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E13" s="74" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F13" s="69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G13" s="74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H13" s="74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I13" s="74" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J13" s="75" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K13" s="76" t="str">
         <f t="shared" si="0"/>
@@ -3296,11 +3296,11 @@
 </v>
       </c>
       <c r="L13" s="74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M13" s="71"/>
       <c r="N13" s="74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O13" s="71"/>
       <c r="P13" s="75">
@@ -3336,12 +3336,12 @@
         <v>0</v>
       </c>
       <c r="X13" s="72" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" s="78">
         <v>2</v>
@@ -3350,25 +3350,25 @@
         <v>1</v>
       </c>
       <c r="D14" s="79" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E14" s="78" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F14" s="78" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G14" s="80" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H14" s="78" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I14" s="80" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J14" s="80" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K14" s="81" t="str">
         <f t="shared" si="0"/>
@@ -3388,7 +3388,7 @@
         <v>Jab%n👊💡➜</v>
       </c>
       <c r="N14" s="80" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="O14" s="81" t="str">
         <f>VLOOKUP(N14,$A$8:$K$21,10,FALSE)</f>
@@ -3427,7 +3427,7 @@
         <v>1</v>
       </c>
       <c r="X14" s="82" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
@@ -3441,25 +3441,25 @@
         <v>2</v>
       </c>
       <c r="D15" s="85" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E15" s="80" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G15" s="78" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H15" s="84" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I15" s="84" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J15" s="84" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K15" s="86" t="str">
         <f t="shared" si="0"/>
@@ -3472,11 +3472,11 @@
 </v>
       </c>
       <c r="L15" s="80" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M15" s="85"/>
       <c r="N15" s="80" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O15" s="86"/>
       <c r="P15" s="84">
@@ -3514,34 +3514,34 @@
     </row>
     <row r="16" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" s="80">
+        <v>2</v>
+      </c>
+      <c r="C16" s="80">
+        <v>2</v>
+      </c>
+      <c r="D16" s="81" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="80" t="s">
         <v>187</v>
       </c>
-      <c r="B16" s="80">
-        <v>2</v>
-      </c>
-      <c r="C16" s="80">
-        <v>2</v>
-      </c>
-      <c r="D16" s="81" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="80" t="s">
-        <v>189</v>
-      </c>
       <c r="F16" s="80" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G16" s="78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H16" s="78" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I16" s="87" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J16" s="78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K16" s="86" t="str">
         <f t="shared" si="0"/>
@@ -3554,11 +3554,11 @@
 </v>
       </c>
       <c r="L16" s="80" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M16" s="81"/>
       <c r="N16" s="80" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O16" s="81"/>
       <c r="P16" s="84">
@@ -3596,7 +3596,7 @@
     </row>
     <row r="17" spans="1:24" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="88" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="89">
         <v>2</v>
@@ -3605,25 +3605,25 @@
         <v>1</v>
       </c>
       <c r="D17" s="90" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E17" s="89" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F17" s="89" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G17" s="89" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H17" s="89" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I17" s="91" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J17" s="91" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K17" s="92" t="str">
         <f t="shared" si="0"/>
@@ -3643,7 +3643,7 @@
         <v>Rake%n🔓🔓🔊➜</v>
       </c>
       <c r="N17" s="91" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O17" s="92" t="str">
         <f>VLOOKUP(N17,$A$8:$K$21,10,FALSE)</f>
@@ -3693,25 +3693,25 @@
         <v>2</v>
       </c>
       <c r="D18" s="92" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" s="89" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F18" s="89" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G18" s="89" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H18" s="89" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I18" s="89" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J18" s="91" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K18" s="94" t="str">
         <f t="shared" si="0"/>
@@ -3724,11 +3724,11 @@
 </v>
       </c>
       <c r="L18" s="91" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M18" s="95"/>
       <c r="N18" s="91" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O18" s="94"/>
       <c r="P18" s="89">
@@ -3766,34 +3766,34 @@
     </row>
     <row r="19" spans="1:24" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="91">
+        <v>2</v>
+      </c>
+      <c r="C19" s="91">
+        <v>2</v>
+      </c>
+      <c r="D19" s="92" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="97" t="s">
+        <v>211</v>
+      </c>
+      <c r="F19" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" s="89" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="B19" s="91">
-        <v>2</v>
-      </c>
-      <c r="C19" s="91">
-        <v>2</v>
-      </c>
-      <c r="D19" s="92" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="97" t="s">
-        <v>215</v>
-      </c>
-      <c r="F19" s="89" t="s">
-        <v>138</v>
-      </c>
-      <c r="G19" s="89" t="s">
-        <v>154</v>
-      </c>
-      <c r="H19" s="89" t="s">
-        <v>157</v>
-      </c>
       <c r="I19" s="89" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J19" s="89" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K19" s="94" t="str">
         <f t="shared" si="0"/>
@@ -3806,11 +3806,11 @@
 </v>
       </c>
       <c r="L19" s="91" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M19" s="92"/>
       <c r="N19" s="91" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O19" s="92"/>
       <c r="P19" s="97">
@@ -3846,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="93" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3891,8 +3891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3913,7 +3913,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3921,7 +3921,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -3930,7 +3930,7 @@
         <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>248</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -3939,49 +3939,48 @@
         <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4004,15 +4003,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -4020,7 +4019,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -4028,55 +4027,55 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -4084,31 +4083,31 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -4116,7 +4115,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -4124,15 +4123,15 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
@@ -4140,47 +4139,47 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B18" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B22" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -4188,7 +4187,7 @@
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
@@ -4196,15 +4195,15 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
@@ -4212,31 +4211,31 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B27" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B28" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -4244,31 +4243,31 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
@@ -4276,18 +4275,18 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -4575,10 +4574,10 @@
         <v>33</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -4741,40 +4740,40 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="M14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="P14" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R14" s="2" t="e">
         <f>Skills!E$1 &amp; ": " &amp; F14 &amp; CHAR(10)
@@ -4807,37 +4806,37 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>91</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>91</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>93</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>93</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>93</v>
@@ -4861,7 +4860,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -4991,7 +4990,7 @@
         <v>#REF!</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -5206,7 +5205,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -5245,7 +5244,7 @@
         <v>#REF!</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -5292,7 +5291,7 @@
         <v>#REF!</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -5339,7 +5338,7 @@
         <v>#REF!</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -5474,7 +5473,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -5597,7 +5596,7 @@
         <v>#REF!</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -5644,7 +5643,7 @@
         <v>#REF!</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -5664,7 +5663,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -5688,7 +5687,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5699,10 +5698,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5716,7 +5715,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5730,7 +5729,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5744,7 +5743,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5758,31 +5757,31 @@
         <v>5</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -5802,10 +5801,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
characters: minor tweaks to look and feel
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -757,9 +757,6 @@
     <t>THEY TRUST ME%nMay start the heist on any blank space (i.e. without security tokens, security systems, or loot) for 🔊🔊</t>
   </si>
   <si>
-    <t>EXTORT GUARDS%nMay use 💡💡 to change security roll by 1%n %nMANIPULATE%nOnce per turn, on an auto-Reveal, may draw two tokens from the bag and choose the next one for 💡</t>
-  </si>
-  <si>
     <t>SWAP DUFFEL BAGS%nIf busted, may transfer loot to another player in the building within ➜➜➜%n %nALWAYS HAVE A GETAWAY%nIf busted, leaves heist but remains for next heist.</t>
   </si>
   <si>
@@ -785,6 +782,9 @@
   </si>
   <si>
     <t>Idea. Add 1 Idea to your character</t>
+  </si>
+  <si>
+    <t>EXTORT GUARDS%nMay use 💡💡 to change security roll by 1%n %nMANIPULATE%nOnce per turn when anyone 🔍, may spend 💡 to draw two tokens from the bag and choose the next one</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1460,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1690,7 @@
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
       <c r="K6" s="25" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>82</v>
@@ -1796,10 +1796,10 @@
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="L9" s="24" t="s">
         <v>243</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1974,7 +1974,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L14" s="26" t="s">
         <v>82</v>
@@ -2040,7 +2040,7 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L16" s="26" t="s">
         <v>82</v>
@@ -3913,7 +3913,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3921,7 +3921,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -3930,7 +3930,7 @@
         <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -3948,7 +3948,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3956,7 +3956,7 @@
         <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
reworking the skill backs
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="251">
   <si>
     <t>Name</t>
   </si>
@@ -581,9 +581,6 @@
   </si>
   <si>
     <t>Pick &amp; Walk%n🔓🔊➜</t>
-  </si>
-  <si>
-    <t>Corrupt</t>
   </si>
   <si>
     <t>Loot</t>
@@ -1459,7 +1456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -1497,7 +1494,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>163</v>
@@ -1523,7 +1520,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="16">
         <v>1</v>
@@ -1541,7 +1538,7 @@
         <v>165</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>6</v>
@@ -1561,7 +1558,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="16">
         <v>1</v>
@@ -1579,12 +1576,12 @@
         <v>167</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
       <c r="K3" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L3" s="17" t="s">
         <v>82</v>
@@ -1592,10 +1589,10 @@
     </row>
     <row r="4" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="16">
         <v>1</v>
@@ -1618,7 +1615,7 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L4" s="17" t="s">
         <v>82</v>
@@ -1647,7 +1644,7 @@
         <v>165</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>9</v>
@@ -1690,7 +1687,7 @@
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
       <c r="K6" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>82</v>
@@ -1724,7 +1721,7 @@
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
       <c r="K7" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L7" s="25" t="s">
         <v>82</v>
@@ -1788,7 +1785,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>138</v>
@@ -1796,10 +1793,10 @@
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="L9" s="24" t="s">
         <v>242</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1825,12 +1822,12 @@
         <v>165</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L10" s="24" t="s">
         <v>82</v>
@@ -1868,7 +1865,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L11" s="27" t="s">
         <v>82</v>
@@ -1902,7 +1899,7 @@
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L12" s="27" t="s">
         <v>82</v>
@@ -1931,12 +1928,12 @@
         <v>165</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L13" s="27" t="s">
         <v>82</v>
@@ -1974,7 +1971,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L14" s="26" t="s">
         <v>82</v>
@@ -2006,7 +2003,7 @@
         <v>140</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L15" s="26" t="s">
         <v>82</v>
@@ -2040,7 +2037,7 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L16" s="26" t="s">
         <v>82</v>
@@ -2078,7 +2075,7 @@
         <v>40</v>
       </c>
       <c r="K17" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L17" s="28" t="s">
         <v>82</v>
@@ -2110,7 +2107,7 @@
         <v>138</v>
       </c>
       <c r="K18" s="28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L18" s="28" t="s">
         <v>82</v>
@@ -2118,7 +2115,7 @@
     </row>
     <row r="19" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>178</v>
@@ -2142,7 +2139,7 @@
         <v>181</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L19" s="28" t="s">
         <v>82</v>
@@ -2172,11 +2169,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,11 +2188,11 @@
     <col min="8" max="8" width="25.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5" style="9" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="9" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14" style="9" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="9" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13" style="9" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="14" style="9" customWidth="1"/>
     <col min="16" max="16" width="3.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -2217,7 +2214,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E1" s="6">
         <v>1</v>
@@ -2274,7 +2271,7 @@
         <v>131</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="X1" s="5" t="s">
         <v>28</v>
@@ -2282,7 +2279,7 @@
     </row>
     <row r="2" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" s="46">
         <v>2</v>
@@ -2291,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E2" s="46" t="s">
         <v>139</v>
@@ -2329,16 +2326,28 @@
       <c r="L2" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="47" t="e">
-        <f>VLOOKUP(L2,$A$8:$K$21,10,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M2" s="47" t="str">
+        <f>IF(L2="(none)","",VLOOKUP(L2,$A$2:$K$19,11,FALSE))</f>
+        <v xml:space="preserve">1: Recon%n💡💡🔊🔍
+2: Rake%n🔓🔓🔊➜
+3: Spray%n📷🔊➜
+4: Slink%n💡➜
+5: Jab%n👊💡➜
+6: Nab%n💰💰
+</v>
       </c>
       <c r="N2" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="O2" s="49" t="e">
-        <f>VLOOKUP(N2,$A$8:$K$21,10,FALSE)</f>
-        <v>#N/A</v>
+      <c r="O2" s="49" t="str">
+        <f>IF(N2="(none)","",VLOOKUP(N2,$A$2:$K$19,11,FALSE))</f>
+        <v xml:space="preserve">1: Run%n🔊🔊➜➜
+2: Disable%n📷🔊➜
+3: Pick &amp; Walk%n🔓🔊➜
+4: Jab%n👊💡➜
+5: Reveal%n🔍
+6: Punch%n👊🔊🔊➜
+</v>
       </c>
       <c r="P2" s="46">
         <f t="shared" ref="P2:W11" si="1">(LEN($E2)-LEN(SUBSTITUTE($E2,P$1,"")))/LEN(P$1) +
@@ -2378,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -2392,7 +2401,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" s="46" t="s">
         <v>149</v>
@@ -2410,7 +2419,7 @@
         <v>146</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K3" s="50" t="str">
         <f t="shared" si="0"/>
@@ -2425,11 +2434,17 @@
       <c r="L3" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="M3" s="51"/>
+      <c r="M3" s="51" t="str">
+        <f t="shared" ref="M3:M19" si="2">IF(L3="(none)","",VLOOKUP(L3,$A$2:$K$19,11,FALSE))</f>
+        <v/>
+      </c>
       <c r="N3" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="O3" s="50"/>
+      <c r="O3" s="49" t="str">
+        <f t="shared" ref="O3:O19" si="3">IF(N3="(none)","",VLOOKUP(N3,$A$2:$K$19,11,FALSE))</f>
+        <v/>
+      </c>
       <c r="P3" s="46">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2463,7 +2478,7 @@
         <v>2</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -2477,7 +2492,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" s="54" t="s">
         <v>136</v>
@@ -2510,11 +2525,17 @@
       <c r="L4" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="M4" s="50"/>
+      <c r="M4" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N4" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="O4" s="50"/>
+      <c r="O4" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P4" s="54">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2548,7 +2569,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -2595,16 +2616,28 @@
       <c r="L5" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="42" t="e">
-        <f>VLOOKUP(L5,$A$8:$K$21,10,FALSE)</f>
-        <v>#N/A</v>
+      <c r="M5" s="42" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: Redirect%n🔓👊📷🔊
+2: Slink%n💡➜
+3: Redirect%n🔓👊📷🔊
+4: Sneak%n🔍➜➜
+5: Jab%n👊💡➜
+6: Examine%n💡💡💡🔊
+</v>
       </c>
       <c r="N5" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="41" t="e">
-        <f>VLOOKUP(N5,$A$8:$K$21,10,FALSE)</f>
-        <v>#N/A</v>
+      <c r="O5" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">1: Sneak%n🔍➜➜
+2: Sleeper Hold%n👊➜
+3: Slink%n💡➜
+4: Sleeper Hold%n👊➜
+5: Slink%n💡➜
+6: Defeat%n🔓📷🔊➜
+</v>
       </c>
       <c r="P5" s="44">
         <f t="shared" si="1"/>
@@ -2639,7 +2672,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -2671,7 +2704,7 @@
         <v>146</v>
       </c>
       <c r="J6" s="44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K6" s="41" t="str">
         <f t="shared" si="0"/>
@@ -2686,11 +2719,17 @@
       <c r="L6" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="M6" s="41"/>
+      <c r="M6" s="41" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N6" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="O6" s="41"/>
+      <c r="O6" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P6" s="44">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2724,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -2771,11 +2810,17 @@
       <c r="L7" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="M7" s="41"/>
+      <c r="M7" s="41" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N7" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="O7" s="41"/>
+      <c r="O7" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P7" s="44">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -2809,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="X7" s="55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:24" s="61" customFormat="1" x14ac:dyDescent="0.25">
@@ -2854,18 +2899,30 @@
 </v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>184</v>
-      </c>
-      <c r="M8" s="58" t="e">
-        <f>VLOOKUP(L8,$A$8:$K$21,10,FALSE)</f>
-        <v>#N/A</v>
+        <v>229</v>
+      </c>
+      <c r="M8" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: Study%n💡💡
+2: Discover%n🔍🔍
+3: Jab%n👊💡➜
+4: Examine%n💡💡💡🔊
+5: Defeat%n🔓📷🔊➜
+6: Sneak%n🔍➜➜
+</v>
       </c>
       <c r="N8" s="57" t="s">
         <v>134</v>
       </c>
       <c r="O8" s="60" t="str">
-        <f>VLOOKUP(N8,$A$8:$K$21,10,FALSE)</f>
-        <v>Loop%n📷🔍</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">1: Examine%n💡💡💡🔊
+2: Defeat%n🔓📷🔊➜
+3: Punch%n👊🔊🔊➜
+4: Pick &amp; Walk%n🔓🔊➜
+5: Punch%n👊🔊🔊➜
+6: Loop%n📷🔍
+</v>
       </c>
       <c r="P8" s="57">
         <f t="shared" si="1"/>
@@ -2900,12 +2957,12 @@
         <v>0</v>
       </c>
       <c r="X8" s="61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9" s="59">
         <v>2</v>
@@ -2920,13 +2977,13 @@
         <v>138</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G9" s="57" t="s">
         <v>146</v>
       </c>
       <c r="H9" s="59" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I9" s="57" t="s">
         <v>160</v>
@@ -2947,11 +3004,17 @@
       <c r="L9" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="M9" s="64"/>
+      <c r="M9" s="64" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N9" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="O9" s="63"/>
+      <c r="O9" s="63" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P9" s="57">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2985,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:24" s="62" customFormat="1" x14ac:dyDescent="0.25">
@@ -3002,7 +3065,7 @@
         <v>127</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F10" s="66" t="s">
         <v>160</v>
@@ -3032,11 +3095,17 @@
       <c r="L10" s="66" t="s">
         <v>161</v>
       </c>
-      <c r="M10" s="64"/>
+      <c r="M10" s="64" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N10" s="66" t="s">
         <v>161</v>
       </c>
-      <c r="O10" s="63"/>
+      <c r="O10" s="63" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P10" s="67">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -3070,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="62" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -3115,18 +3184,30 @@
 </v>
       </c>
       <c r="L11" s="69" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M11" s="70" t="str">
-        <f>VLOOKUP(L11,$A$8:$K$21,10,FALSE)</f>
-        <v>Kick%n👊🔊➜➜</v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: Nab%n💰💰
+2: Rake%n🔓🔓🔊➜
+3: Kick%n👊🔊➜➜
+4: Study%n💡💡
+5: Spray%n📷🔊➜
+6: Kick%n👊🔊➜➜
+</v>
       </c>
       <c r="N11" s="69" t="s">
         <v>116</v>
       </c>
       <c r="O11" s="71" t="str">
-        <f>VLOOKUP(N11,$A$8:$K$21,10,FALSE)</f>
-        <v>Punch%n👊🔊🔊➜</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">1: Defeat%n🔓📷🔊➜
+2: Sprint%n🔊🔊➜➜➜
+3: Slink%n💡➜
+4: Rampage%n👊👊🔊🔊➜➜
+5: Detonate%n🔓👊📷🔊🔊⚠
+6: Punch%n👊🔊🔊➜
+</v>
       </c>
       <c r="P11" s="69">
         <f t="shared" si="1"/>
@@ -3161,12 +3242,12 @@
         <v>0</v>
       </c>
       <c r="X11" s="72" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12" s="74">
         <v>2</v>
@@ -3178,7 +3259,7 @@
         <v>129</v>
       </c>
       <c r="E12" s="74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F12" s="75" t="s">
         <v>148</v>
@@ -3208,13 +3289,19 @@
       <c r="L12" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="M12" s="71"/>
+      <c r="M12" s="71" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N12" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="O12" s="71"/>
+      <c r="O12" s="71" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P12" s="75">
-        <f t="shared" ref="P12:W19" si="2">(LEN($E12)-LEN(SUBSTITUTE($E12,P$1,"")))/LEN(P$1) +
+        <f t="shared" ref="P12:W19" si="4">(LEN($E12)-LEN(SUBSTITUTE($E12,P$1,"")))/LEN(P$1) +
 (LEN($F12)-LEN(SUBSTITUTE($F12,P$1,"")))/LEN(P$1) +
 (LEN($G12)-LEN(SUBSTITUTE($G12,P$1,"")))/LEN(P$1) +
 (LEN($H12)-LEN(SUBSTITUTE($H12,P$1,"")))/LEN(P$1) +
@@ -3223,35 +3310,35 @@
         <v>2</v>
       </c>
       <c r="Q12" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R12" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="S12" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T12" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U12" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V12" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W12" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="X12" s="72" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -3280,7 +3367,7 @@
         <v>154</v>
       </c>
       <c r="I13" s="74" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J13" s="75" t="s">
         <v>137</v>
@@ -3298,45 +3385,51 @@
       <c r="L13" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="M13" s="71"/>
+      <c r="M13" s="71" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N13" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="O13" s="71"/>
+      <c r="O13" s="71" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P13" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q13" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="R13" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="S13" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="T13" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="U13" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V13" s="75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W13" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X13" s="72" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
@@ -3356,7 +3449,7 @@
         <v>137</v>
       </c>
       <c r="F14" s="78" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G14" s="80" t="s">
         <v>147</v>
@@ -3384,50 +3477,62 @@
         <v>35</v>
       </c>
       <c r="M14" s="79" t="str">
-        <f>VLOOKUP(L14,$A$8:$K$21,10,FALSE)</f>
-        <v>Jab%n👊💡➜</v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: Rake%n🔓🔓🔊➜
+2: Run%n🔊🔊➜➜
+3: Yoink%n💰🔊
+4: Spin Kick%n👊👊👊🔊🔊
+5: Kick%n👊🔊➜➜
+6: Jab%n👊💡➜
+</v>
       </c>
       <c r="N14" s="80" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O14" s="81" t="str">
-        <f>VLOOKUP(N14,$A$8:$K$21,10,FALSE)</f>
-        <v>Run%n🔊🔊➜➜</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">1: Detonate%n🔓👊📷🔊🔊⚠
+2: Nab%n💰💰
+3: Run%n🔊🔊➜➜
+4: Sneak%n🔍➜➜
+5: Rake%n🔓🔓🔊➜
+6: Run%n🔊🔊➜➜
+</v>
       </c>
       <c r="P14" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Q14" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="R14" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S14" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T14" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U14" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V14" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W14" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="X14" s="82" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
@@ -3450,10 +3555,10 @@
         <v>136</v>
       </c>
       <c r="G15" s="78" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H15" s="84" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I15" s="84" t="s">
         <v>141</v>
@@ -3474,47 +3579,53 @@
       <c r="L15" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="M15" s="85"/>
+      <c r="M15" s="85" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N15" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="O15" s="86"/>
+      <c r="O15" s="86" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P15" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q15" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="R15" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="S15" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T15" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="U15" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V15" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W15" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="80">
         <v>2</v>
@@ -3526,10 +3637,10 @@
         <v>128</v>
       </c>
       <c r="E16" s="80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F16" s="80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G16" s="78" t="s">
         <v>136</v>
@@ -3556,41 +3667,47 @@
       <c r="L16" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="M16" s="81"/>
+      <c r="M16" s="81" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N16" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="O16" s="81"/>
+      <c r="O16" s="81" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P16" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q16" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="R16" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S16" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T16" s="84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U16" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="V16" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="W16" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -3614,10 +3731,10 @@
         <v>136</v>
       </c>
       <c r="G17" s="89" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H17" s="89" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I17" s="91" t="s">
         <v>135</v>
@@ -3639,46 +3756,58 @@
         <v>64</v>
       </c>
       <c r="M17" s="90" t="str">
-        <f>VLOOKUP(L17,$A$8:$K$21,10,FALSE)</f>
-        <v>Rake%n🔓🔓🔊➜</v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">1: Loop%n📷🔍
+2: Recon%n💡💡🔊🔍
+3: Run%n🔊🔊➜➜
+4: Punch%n👊🔊🔊➜
+5: Run%n🔊🔊➜➜
+6: Rake%n🔓🔓🔊➜
+</v>
       </c>
       <c r="N17" s="91" t="s">
         <v>153</v>
       </c>
       <c r="O17" s="92" t="str">
-        <f>VLOOKUP(N17,$A$8:$K$21,10,FALSE)</f>
-        <v>Pick%n🔓</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">1: Examine%n💡💡💡🔊
+2: Run%n🔊🔊➜➜
+3: Loop%n📷🔍
+4: Redirect%n🔓👊📷🔊
+5: Recon%n💡💡🔊🔍
+6: Pick%n🔓
+</v>
       </c>
       <c r="P17" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Q17" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="R17" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S17" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T17" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U17" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V17" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W17" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3726,41 +3855,47 @@
       <c r="L18" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="M18" s="95"/>
+      <c r="M18" s="95" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N18" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="O18" s="94"/>
+      <c r="O18" s="94" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P18" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Q18" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="R18" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="S18" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T18" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U18" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V18" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="W18" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3778,7 +3913,7 @@
         <v>126</v>
       </c>
       <c r="E19" s="97" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F19" s="89" t="s">
         <v>136</v>
@@ -3793,7 +3928,7 @@
         <v>149</v>
       </c>
       <c r="J19" s="89" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K19" s="94" t="str">
         <f t="shared" si="0"/>
@@ -3808,45 +3943,51 @@
       <c r="L19" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="M19" s="92"/>
+      <c r="M19" s="92" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="N19" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="O19" s="92"/>
+      <c r="O19" s="92" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="P19" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Q19" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="R19" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="S19" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="T19" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U19" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V19" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="W19" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X19" s="93" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3913,7 +4054,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3921,7 +4062,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -3930,7 +4071,7 @@
         <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -3939,7 +4080,7 @@
         <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -3948,7 +4089,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3956,15 +4097,15 @@
         <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3972,7 +4113,7 @@
         <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3980,7 +4121,7 @@
         <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4003,10 +4144,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4019,7 +4160,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -4030,15 +4171,15 @@
         <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4046,15 +4187,15 @@
         <v>157</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4062,7 +4203,7 @@
         <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4070,7 +4211,7 @@
         <v>146</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4086,7 +4227,7 @@
         <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4094,15 +4235,15 @@
         <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4115,7 +4256,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -4126,7 +4267,7 @@
         <v>137</v>
       </c>
       <c r="B16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -4142,7 +4283,7 @@
         <v>154</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -4150,7 +4291,7 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -4158,7 +4299,7 @@
         <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -4166,15 +4307,15 @@
         <v>139</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4198,7 +4339,7 @@
         <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -4214,15 +4355,15 @@
         <v>162</v>
       </c>
       <c r="B27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -4230,7 +4371,7 @@
         <v>150</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -4246,7 +4387,7 @@
         <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -4254,7 +4395,7 @@
         <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -4262,7 +4403,7 @@
         <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -4275,18 +4416,18 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -5776,12 +5917,12 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -5801,10 +5942,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" t="s">
         <v>222</v>
-      </c>
-      <c r="B1" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
characters: big rewrite of character abilities
Key design decisions:
* Make all characters keep their abilities (to some degree). Sometimes the ability itself levels up a bit
* Really try to keep the characters to have the same "feel" as they level up. It is a role-playing game, after all!
* The Level 1 characters should have the strategy-defining abilities, which are underpowered, and then leveling up powers them up (e.g. Dart for Burglar, Bolt for Grease Man)
* New strategy-defining ability ideas like Breach
* Started adding more weaknesses to the characters too, e.g. Con Artist. Trying to make the weaknesses implicit rather than explicit, though.

Tons of my old character abilities are shoved into the ideas page, with some other ideas sitting around.

And of course, better wording on things and such.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\code\timber-wolf\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local\workspaces\ruby\project-timber-wolf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,18 @@
     <sheet name="Skill Ideas" sheetId="4" r:id="rId5"/>
     <sheet name="Character Ideas" sheetId="5" r:id="rId6"/>
     <sheet name="Event Ideas" sheetId="7" r:id="rId7"/>
+    <sheet name="Tile ideas" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="ActionList">Actions!$A$1:$A$36</definedName>
-    <definedName name="Actions">Actions!$A$1:$A$36</definedName>
+    <definedName name="ActionList">Actions!$A$2:$A$37</definedName>
+    <definedName name="Actions">Actions!$A$2:$A$37</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="285">
   <si>
     <t>Name</t>
   </si>
@@ -535,9 +536,6 @@
     <t>Crawl%n➜</t>
   </si>
   <si>
-    <t>PICKER%nGain 💡 when you 🔓%n %nMASTER KEY%nWhen outdoors, may use  💡💡 to enable one player to 🔓</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -607,12 +605,6 @@
     <t>Tunnel Master</t>
   </si>
   <si>
-    <t>SEWER CRAWL%nFor 🔊🔊⚠, may treat a tile directly across 1 empty hex space as adjacent.</t>
-  </si>
-  <si>
-    <t>Guy on the Inside</t>
-  </si>
-  <si>
     <t>Loot. Gain $1k for your person.</t>
   </si>
   <si>
@@ -625,9 +617,6 @@
     <t>Ideas</t>
   </si>
   <si>
-    <t>EARLY WARNING%nOnce per turn, may 🔍%n %nMISDIRECT%nMay use 💡💡💡 to change the security roll by 1.</t>
-  </si>
-  <si>
     <t>Pick%n🔓</t>
   </si>
   <si>
@@ -637,21 +626,9 @@
     <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires</t>
   </si>
   <si>
-    <t>GREAT IN A PINCH%nMay prevent a gate from shutting for 💡💡💡%n %nPACKS A SQUIB%nIf busted, fakes death and plays next heist, but loses loot.</t>
-  </si>
-  <si>
-    <t>YOU WILL REPORT IN%nWhen  👊, lower the noise level by 2. Do not change the ⚠ level.</t>
-  </si>
-  <si>
     <t>Bash%n👊👊🔊</t>
   </si>
   <si>
-    <t>I CAN HAZ TEH CODES?%nMay spend 💡💡 to prevent Power Cycle event %n %nI CAN HEARTBLEED%nIf outdoors, may spend 💡💡 to 🔍</t>
-  </si>
-  <si>
-    <t>DENIAL OF SERVICE%nFor 💡💡💡, disconnect all known cameras%n %nACTIVATE SPRINKLERS%nWhen outdoors, may use a 💡💡to 👊 any known guard without being on or adjacent to him</t>
-  </si>
-  <si>
     <t>Yoink%n💰🔊</t>
   </si>
   <si>
@@ -742,53 +719,179 @@
     <t>Subdue%n👊</t>
   </si>
   <si>
-    <t>INSPIRE%nOnce per turn, give a free💡 to a player of your choosing.</t>
-  </si>
-  <si>
-    <t>REROUTE%nOnce per turn, may spend 💡 to re-place any player's planning token%n %nINTERCEPT%nFor 💡💡💡, may prevent a security event that places a guard on a player's space</t>
+    <t>SWAP DUFFEL BAGS%nIf busted, may transfer loot to another player in the building within ➜➜➜%n %nALWAYS HAVE A GETAWAY%nIf busted, leaves heist but remains for next heist.</t>
+  </si>
+  <si>
+    <t>BOLT%nMay spend 💡for ➜ up to four times in a turn.</t>
+  </si>
+  <si>
+    <t>Reveal 1 security token anywhere</t>
+  </si>
+  <si>
+    <t>Subdue 1 guard on or adjacent to your tile</t>
+  </si>
+  <si>
+    <t>Move to adjacent, planned, not locked tile</t>
+  </si>
+  <si>
+    <t>Unlock 1 locked, adjacent tile</t>
+  </si>
+  <si>
+    <t>Idea. Add 1 Idea to your character</t>
+  </si>
+  <si>
+    <t>Crowded!</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>Allow the security system to apply to a passage, too. So just the ring and you can't step on it. That also means you can't step on that square until it's disabled, so you can't camp out on a jewel</t>
+  </si>
+  <si>
+    <t>You can't have more than 1 player on that space.</t>
+  </si>
+  <si>
+    <t>SLIPPERY%nGain💡when escaping%n %nTHERE ARE BETTER WAYS%n %nCannot 👊. May escape a guard with 💡(Escape phase unaffected).</t>
+  </si>
+  <si>
+    <t>SLIPPERY%nGain💡when escaping%n %nINSPIRE%nOnce per turn, give a free💡 to a player of your choosing.</t>
+  </si>
+  <si>
+    <t>EXTORT GUARDS%nMay use 💡💡 to change security roll by 1%n %n</t>
+  </si>
+  <si>
+    <t>MANIPULATE%nOnce per turn when anyone 🔍, may spend 💡 to draw two tokens from the bag and choose the next one</t>
+  </si>
+  <si>
+    <t>PACKS A SQUIB%nIf busted, fakes death and plays next heist, but loses loot.</t>
+  </si>
+  <si>
+    <t>INTERCEPT%nFor 💡💡💡, may prevent a security event that places a guard on a player's space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I CAN HAZ TEH CODES?%nMay spend 💡💡 to prevent Power Cycle event </t>
+  </si>
+  <si>
+    <t>I CAN HEARTBLEED%nIf outdoors, may spend 💡 to 🔍</t>
+  </si>
+  <si>
+    <t>ADRENALINE%nGain 💡 on 👊%n %nYOU WILL REPORT IN%nWhen  👊, lower the noise level by 2. Do not change the ⚠ level.</t>
+  </si>
+  <si>
+    <t>PICKER%nGain 💡 when you 🔓</t>
+  </si>
+  <si>
+    <t>ADRENALINE%nGain 💡 on 👊%n %nBRING IT ON%nGain 💡💡💡 if standing on a Reinforcements beacon when Reinforcements is triggered.</t>
+  </si>
+  <si>
+    <t>EARLY WARNING%nWhen outdoors, may 🔍 once per turn%n %nMISDIRECT%nOnce per heist, may use 💡💡💡 to change the security roll by 1.</t>
+  </si>
+  <si>
+    <t>EARLY WARNING%nWhen outdoors, may 🔍 once per turn%n %nGREAT IN A PINCH%nMay prevent a gate from shutting for 💡💡💡</t>
+  </si>
+  <si>
+    <t>EARLY WARNING%nWhen outdoors, may 🔍 once per turn%n %nTHEY TRUST ME%nMay start the heist on any blank space (i.e. without security tokens, security systems, or loot) for 🔊🔊</t>
+  </si>
+  <si>
+    <t>PICKER%nGain 💡 when you 🔓%n %nI'LL WALK YOU THROUGH IT%nMay use  💡💡 to enable one player to 🔓</t>
+  </si>
+  <si>
+    <t>DART%nMay spend 💡for ➜ once per turn</t>
   </si>
   <si>
     <t>DIG!%nMay begin the heist on any non-security tile on bordering the outside of the map for 🔊🔊</t>
   </si>
   <si>
-    <t>THEY TRUST ME%nMay start the heist on any blank space (i.e. without security tokens, security systems, or loot) for 🔊🔊</t>
-  </si>
-  <si>
-    <t>SWAP DUFFEL BAGS%nIf busted, may transfer loot to another player in the building within ➜➜➜%n %nALWAYS HAVE A GETAWAY%nIf busted, leaves heist but remains for next heist.</t>
-  </si>
-  <si>
-    <t>Or was it the backpacks?</t>
-  </si>
-  <si>
-    <t>BOLT%nMay spend 💡for ➜ up to four times in a turn.</t>
-  </si>
-  <si>
-    <t>LOOTER%n💰 each time you take "Hestitate"</t>
-  </si>
-  <si>
-    <t>Reveal 1 security token anywhere</t>
-  </si>
-  <si>
-    <t>Subdue 1 guard on or adjacent to your tile</t>
-  </si>
-  <si>
-    <t>Move to adjacent, planned, not locked tile</t>
-  </si>
-  <si>
-    <t>Unlock 1 locked, adjacent tile</t>
-  </si>
-  <si>
-    <t>Idea. Add 1 Idea to your character</t>
-  </si>
-  <si>
-    <t>EXTORT GUARDS%nMay use 💡💡 to change security roll by 1%n %nMANIPULATE%nOnce per turn when anyone 🔍, may spend 💡 to draw two tokens from the bag and choose the next one</t>
+    <t>PICKER%nGain 💡 when you 🔓%n %nBREACH%nFor 💡💡💡, may create a new Exit on current tile if it has an open side. Initiate Escape phase when this happens.</t>
+  </si>
+  <si>
+    <t>HAS THE CODE%nOnce per turn, may spend 💡💡 to re-position 1 planning token of any player%n %nACTIVATE SPRINKLERS%nWhen outdoors, may use a 💡💡to give a free 👊 to any player</t>
+  </si>
+  <si>
+    <t>I CAN HAZ TEH CODES?%nOnce per turn, may spend 💡💡💡 to re-position 1 planning token of any player%n %nDENIAL OF SERVICE%nWhen outdoors, may use 💡💡 to disconnect all known cameras</t>
+  </si>
+  <si>
+    <t>I CAN HAZ TEH CODES?%nOnce per turn, may spend 💡💡💡 to re-position 1 planning token of any player</t>
+  </si>
+  <si>
+    <t>DART%nMay spend 💡for ➜ once per turn%n %nSEWER CRAWL%nFor 🔊🔊⚠, may treat a tile directly across 1 non-tiled gap as adjacent.</t>
+  </si>
+  <si>
+    <t>Bruiser</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>1-slot</t>
+  </si>
+  <si>
+    <t>2-slot</t>
+  </si>
+  <si>
+    <t>3-slot</t>
+  </si>
+  <si>
+    <t>4-slot</t>
+  </si>
+  <si>
+    <t>5-slot</t>
+  </si>
+  <si>
+    <t>6-slot</t>
+  </si>
+  <si>
+    <t>Something more with cameras - these aren't interesting enough</t>
+  </si>
+  <si>
+    <t>Raise alerts and noise if multiple people are on the same square. Really punish three people on the same square. Punish three people next to each other too.</t>
+  </si>
+  <si>
+    <t>Super camera? Or Super Guard? Some sort of security tile that is the same as what we had before, but more.</t>
+  </si>
+  <si>
+    <t>Double Security Tile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just put more security chits on it and handle them. So a second security-backed chit. </t>
+  </si>
+  <si>
+    <t>Known Double-Guards</t>
+  </si>
+  <si>
+    <t>Put two guards on a single space at design time</t>
+  </si>
+  <si>
+    <t>Known Guard-Lock</t>
+  </si>
+  <si>
+    <t>Put a guard and a lock that is already known at a key spot.</t>
+  </si>
+  <si>
+    <t>Cramped Space/Tight Squeeze</t>
+  </si>
+  <si>
+    <t>Known Camera-Lock</t>
+  </si>
+  <si>
+    <t>Put a camera and a lock but known.</t>
+  </si>
+  <si>
+    <t>Add a guard to an empty space adjacent to a guard.</t>
+  </si>
+  <si>
+    <t>Convert a camera to a double-camera.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -804,8 +907,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -874,12 +986,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -915,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1112,49 +1218,68 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1456,23 +1581,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" style="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.140625" style="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="34" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="34" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="74.28515625" style="33" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="158.85546875" style="33" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" style="33" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="33"/>
   </cols>
@@ -1494,7 +1619,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>163</v>
@@ -1503,10 +1628,10 @@
         <v>164</v>
       </c>
       <c r="I1" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>179</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>180</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>124</v>
@@ -1520,7 +1645,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="16">
         <v>1</v>
@@ -1538,16 +1663,16 @@
         <v>165</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>168</v>
+        <v>249</v>
       </c>
       <c r="L2" s="17" t="s">
         <v>82</v>
@@ -1558,7 +1683,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="16">
         <v>1</v>
@@ -1576,12 +1701,12 @@
         <v>167</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
       <c r="K3" s="17" t="s">
-        <v>201</v>
+        <v>254</v>
       </c>
       <c r="L3" s="17" t="s">
         <v>82</v>
@@ -1589,10 +1714,10 @@
     </row>
     <row r="4" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="16">
         <v>1</v>
@@ -1607,15 +1732,15 @@
         <v>4</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>138</v>
+        <v>195</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="L4" s="17" t="s">
         <v>82</v>
@@ -1644,10 +1769,10 @@
         <v>165</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>9</v>
+        <v>262</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>8</v>
@@ -1661,7 +1786,7 @@
     </row>
     <row r="6" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>9</v>
+        <v>262</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>25</v>
@@ -1682,7 +1807,7 @@
         <v>165</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>141</v>
+        <v>198</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
@@ -1721,7 +1846,7 @@
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
       <c r="K7" s="25" t="s">
-        <v>203</v>
+        <v>248</v>
       </c>
       <c r="L7" s="25" t="s">
         <v>82</v>
@@ -1759,7 +1884,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L8" s="24" t="s">
         <v>82</v>
@@ -1782,10 +1907,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="21">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>138</v>
@@ -1793,11 +1918,9 @@
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>242</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -1822,12 +1945,12 @@
         <v>165</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="24" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="L10" s="24" t="s">
         <v>82</v>
@@ -1865,11 +1988,9 @@
         <v>5</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>82</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
@@ -1894,12 +2015,12 @@
         <v>165</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27" t="s">
-        <v>206</v>
+        <v>259</v>
       </c>
       <c r="L12" s="27" t="s">
         <v>82</v>
@@ -1928,12 +2049,12 @@
         <v>165</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="L13" s="27" t="s">
         <v>82</v>
@@ -1959,7 +2080,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="H14" s="22" t="s">
         <v>140</v>
@@ -1971,7 +2092,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="L14" s="26" t="s">
         <v>82</v>
@@ -2000,10 +2121,10 @@
         <v>167</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>140</v>
+        <v>189</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>192</v>
+        <v>261</v>
       </c>
       <c r="L15" s="26" t="s">
         <v>82</v>
@@ -2029,7 +2150,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>139</v>
+        <v>199</v>
       </c>
       <c r="H16" s="22" t="s">
         <v>140</v>
@@ -2037,7 +2158,7 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="L16" s="26" t="s">
         <v>82</v>
@@ -2045,10 +2166,10 @@
     </row>
     <row r="17" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="C17" s="32">
         <v>1</v>
@@ -2069,13 +2190,13 @@
         <v>140</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J17" s="31" t="s">
         <v>40</v>
       </c>
       <c r="K17" s="28" t="s">
-        <v>198</v>
+        <v>251</v>
       </c>
       <c r="L17" s="28" t="s">
         <v>82</v>
@@ -2083,10 +2204,10 @@
     </row>
     <row r="18" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C18" s="32">
         <v>1</v>
@@ -2101,13 +2222,13 @@
         <v>3</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="H18" s="32" t="s">
         <v>138</v>
       </c>
       <c r="K18" s="28" t="s">
-        <v>202</v>
+        <v>252</v>
       </c>
       <c r="L18" s="28" t="s">
         <v>82</v>
@@ -2115,10 +2236,10 @@
     </row>
     <row r="19" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>193</v>
+        <v>40</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C19" s="32">
         <v>1</v>
@@ -2136,10 +2257,10 @@
         <v>165</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="L19" s="28" t="s">
         <v>82</v>
@@ -2173,7 +2294,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,7 +2335,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E1" s="6">
         <v>1</v>
@@ -2271,7 +2392,7 @@
         <v>131</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="X1" s="5" t="s">
         <v>28</v>
@@ -2279,7 +2400,7 @@
     </row>
     <row r="2" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" s="46">
         <v>2</v>
@@ -2288,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E2" s="46" t="s">
         <v>139</v>
@@ -2387,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -2401,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E3" s="46" t="s">
         <v>149</v>
@@ -2419,7 +2540,7 @@
         <v>146</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="K3" s="50" t="str">
         <f t="shared" si="0"/>
@@ -2478,7 +2599,7 @@
         <v>2</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -2492,7 +2613,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E4" s="54" t="s">
         <v>136</v>
@@ -2501,7 +2622,7 @@
         <v>157</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H4" s="54" t="s">
         <v>146</v>
@@ -2569,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="45" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -2672,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="38" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -2704,7 +2825,7 @@
         <v>146</v>
       </c>
       <c r="J6" s="44" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="K6" s="41" t="str">
         <f t="shared" si="0"/>
@@ -2763,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="38" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -2854,7 +2975,7 @@
         <v>0</v>
       </c>
       <c r="X7" s="55" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:24" s="61" customFormat="1" x14ac:dyDescent="0.25">
@@ -2899,7 +3020,7 @@
 </v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="M8" s="58" t="str">
         <f t="shared" si="2"/>
@@ -2957,12 +3078,12 @@
         <v>0</v>
       </c>
       <c r="X8" s="61" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B9" s="59">
         <v>2</v>
@@ -2977,13 +3098,13 @@
         <v>138</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="G9" s="57" t="s">
         <v>146</v>
       </c>
       <c r="H9" s="59" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="I9" s="57" t="s">
         <v>160</v>
@@ -3048,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="65" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:24" s="62" customFormat="1" x14ac:dyDescent="0.25">
@@ -3065,7 +3186,7 @@
         <v>127</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F10" s="66" t="s">
         <v>160</v>
@@ -3074,7 +3195,7 @@
         <v>137</v>
       </c>
       <c r="H10" s="66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I10" s="67" t="s">
         <v>137</v>
@@ -3139,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="62" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -3184,7 +3305,7 @@
 </v>
       </c>
       <c r="L11" s="69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M11" s="70" t="str">
         <f t="shared" si="2"/>
@@ -3242,12 +3363,12 @@
         <v>0</v>
       </c>
       <c r="X11" s="72" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12" s="74">
         <v>2</v>
@@ -3259,7 +3380,7 @@
         <v>129</v>
       </c>
       <c r="E12" s="74" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F12" s="75" t="s">
         <v>148</v>
@@ -3338,7 +3459,7 @@
         <v>2</v>
       </c>
       <c r="X12" s="72" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -3367,7 +3488,7 @@
         <v>154</v>
       </c>
       <c r="I13" s="74" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J13" s="75" t="s">
         <v>137</v>
@@ -3429,41 +3550,41 @@
         <v>0</v>
       </c>
       <c r="X13" s="72" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="77" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="93" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="78">
-        <v>2</v>
-      </c>
-      <c r="C14" s="78">
-        <v>1</v>
-      </c>
-      <c r="D14" s="79" t="s">
+      <c r="B14" s="89">
+        <v>2</v>
+      </c>
+      <c r="C14" s="89">
+        <v>1</v>
+      </c>
+      <c r="D14" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="E14" s="78" t="s">
+      <c r="E14" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="F14" s="78" t="s">
-        <v>207</v>
-      </c>
-      <c r="G14" s="80" t="s">
+      <c r="F14" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="G14" s="91" t="s">
         <v>147</v>
       </c>
-      <c r="H14" s="78" t="s">
+      <c r="H14" s="89" t="s">
         <v>138</v>
       </c>
-      <c r="I14" s="80" t="s">
+      <c r="I14" s="91" t="s">
         <v>147</v>
       </c>
-      <c r="J14" s="80" t="s">
+      <c r="J14" s="91" t="s">
         <v>135</v>
       </c>
-      <c r="K14" s="81" t="str">
+      <c r="K14" s="92" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: Punch%n👊🔊🔊➜
 2: Yoink%n💰🔊
@@ -3473,10 +3594,10 @@
 6: Unplug%n📷🔊🔊➜
 </v>
       </c>
-      <c r="L14" s="80" t="s">
+      <c r="L14" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="79" t="str">
+      <c r="M14" s="90" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">1: Rake%n🔓🔓🔊➜
 2: Run%n🔊🔊➜➜
@@ -3486,10 +3607,10 @@
 6: Jab%n👊💡➜
 </v>
       </c>
-      <c r="N14" s="80" t="s">
-        <v>184</v>
-      </c>
-      <c r="O14" s="81" t="str">
+      <c r="N14" s="91" t="s">
+        <v>183</v>
+      </c>
+      <c r="O14" s="92" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">1: Detonate%n🔓👊📷🔊🔊⚠
 2: Nab%n💰💰
@@ -3499,74 +3620,74 @@
 6: Run%n🔊🔊➜➜
 </v>
       </c>
-      <c r="P14" s="78">
+      <c r="P14" s="89">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="Q14" s="78">
+      <c r="Q14" s="89">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="R14" s="78">
+      <c r="R14" s="89">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S14" s="78">
+      <c r="S14" s="89">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="T14" s="78">
+      <c r="T14" s="89">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U14" s="78">
+      <c r="U14" s="89">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="V14" s="78">
+      <c r="V14" s="89">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W14" s="78">
+      <c r="W14" s="89">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="X14" s="82" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="83" t="s">
+      <c r="X14" s="93" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="93" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="84">
-        <v>2</v>
-      </c>
-      <c r="C15" s="84">
-        <v>2</v>
-      </c>
-      <c r="D15" s="85" t="s">
+      <c r="B15" s="95">
+        <v>2</v>
+      </c>
+      <c r="C15" s="95">
+        <v>2</v>
+      </c>
+      <c r="D15" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="80" t="s">
+      <c r="E15" s="91" t="s">
         <v>148</v>
       </c>
-      <c r="F15" s="78" t="s">
+      <c r="F15" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="G15" s="78" t="s">
-        <v>207</v>
-      </c>
-      <c r="H15" s="84" t="s">
-        <v>200</v>
-      </c>
-      <c r="I15" s="84" t="s">
+      <c r="G15" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="H15" s="95" t="s">
+        <v>196</v>
+      </c>
+      <c r="I15" s="95" t="s">
         <v>141</v>
       </c>
-      <c r="J15" s="84" t="s">
+      <c r="J15" s="95" t="s">
         <v>146</v>
       </c>
-      <c r="K15" s="86" t="str">
+      <c r="K15" s="97" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: Rake%n🔓🔓🔊➜
 2: Run%n🔊🔊➜➜
@@ -3576,85 +3697,85 @@
 6: Jab%n👊💡➜
 </v>
       </c>
-      <c r="L15" s="80" t="s">
+      <c r="L15" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="M15" s="85" t="str">
+      <c r="M15" s="96" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="N15" s="80" t="s">
+      <c r="N15" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="O15" s="86" t="str">
+      <c r="O15" s="97" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P15" s="84">
+      <c r="P15" s="95">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q15" s="84">
+      <c r="Q15" s="95">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="R15" s="84">
+      <c r="R15" s="95">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="S15" s="84">
+      <c r="S15" s="95">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T15" s="84">
+      <c r="T15" s="95">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="U15" s="78">
+      <c r="U15" s="89">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="V15" s="78">
+      <c r="V15" s="89">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W15" s="78">
+      <c r="W15" s="89">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="83" t="s">
-        <v>184</v>
-      </c>
-      <c r="B16" s="80">
-        <v>2</v>
-      </c>
-      <c r="C16" s="80">
-        <v>2</v>
-      </c>
-      <c r="D16" s="81" t="s">
+    <row r="16" spans="1:24" s="93" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="94" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="91">
+        <v>2</v>
+      </c>
+      <c r="C16" s="91">
+        <v>2</v>
+      </c>
+      <c r="D16" s="92" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="80" t="s">
-        <v>186</v>
-      </c>
-      <c r="F16" s="80" t="s">
-        <v>208</v>
-      </c>
-      <c r="G16" s="78" t="s">
+      <c r="E16" s="91" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="91" t="s">
+        <v>200</v>
+      </c>
+      <c r="G16" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="H16" s="78" t="s">
+      <c r="H16" s="89" t="s">
         <v>162</v>
       </c>
-      <c r="I16" s="87" t="s">
+      <c r="I16" s="98" t="s">
         <v>148</v>
       </c>
-      <c r="J16" s="78" t="s">
+      <c r="J16" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="K16" s="86" t="str">
+      <c r="K16" s="97" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: Detonate%n🔓👊📷🔊🔊⚠
 2: Nab%n💰💰
@@ -3664,85 +3785,85 @@
 6: Run%n🔊🔊➜➜
 </v>
       </c>
-      <c r="L16" s="80" t="s">
+      <c r="L16" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="M16" s="81" t="str">
+      <c r="M16" s="92" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="N16" s="80" t="s">
+      <c r="N16" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="O16" s="81" t="str">
+      <c r="O16" s="92" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P16" s="84">
+      <c r="P16" s="95">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="84">
+      <c r="Q16" s="95">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="R16" s="84">
+      <c r="R16" s="95">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="S16" s="84">
+      <c r="S16" s="95">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="T16" s="84">
+      <c r="T16" s="95">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U16" s="78">
+      <c r="U16" s="89">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="V16" s="78">
+      <c r="V16" s="89">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="W16" s="78">
+      <c r="W16" s="89">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88" t="s">
+    <row r="17" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="89">
-        <v>2</v>
-      </c>
-      <c r="C17" s="89">
-        <v>1</v>
-      </c>
-      <c r="D17" s="90" t="s">
+      <c r="B17" s="78">
+        <v>2</v>
+      </c>
+      <c r="C17" s="78">
+        <v>1</v>
+      </c>
+      <c r="D17" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="E17" s="89" t="s">
+      <c r="E17" s="78" t="s">
         <v>138</v>
       </c>
-      <c r="F17" s="89" t="s">
+      <c r="F17" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="G17" s="89" t="s">
-        <v>236</v>
-      </c>
-      <c r="H17" s="89" t="s">
-        <v>210</v>
-      </c>
-      <c r="I17" s="91" t="s">
+      <c r="G17" s="78" t="s">
+        <v>228</v>
+      </c>
+      <c r="H17" s="78" t="s">
+        <v>202</v>
+      </c>
+      <c r="I17" s="80" t="s">
         <v>135</v>
       </c>
-      <c r="J17" s="91" t="s">
+      <c r="J17" s="80" t="s">
         <v>147</v>
       </c>
-      <c r="K17" s="92" t="str">
+      <c r="K17" s="81" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: Study%n💡💡
 2: Run%n🔊🔊➜➜
@@ -3752,10 +3873,10 @@
 6: Shim%n🔓🔊🔊➜
 </v>
       </c>
-      <c r="L17" s="91" t="s">
+      <c r="L17" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="M17" s="90" t="str">
+      <c r="M17" s="79" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">1: Loop%n📷🔍
 2: Recon%n💡💡🔊🔍
@@ -3765,10 +3886,10 @@
 6: Rake%n🔓🔓🔊➜
 </v>
       </c>
-      <c r="N17" s="91" t="s">
+      <c r="N17" s="80" t="s">
         <v>153</v>
       </c>
-      <c r="O17" s="92" t="str">
+      <c r="O17" s="81" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊
 2: Run%n🔊🔊➜➜
@@ -3778,71 +3899,71 @@
 6: Pick%n🔓
 </v>
       </c>
-      <c r="P17" s="89">
+      <c r="P17" s="78">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="Q17" s="89">
+      <c r="Q17" s="78">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="R17" s="89">
+      <c r="R17" s="78">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S17" s="89">
+      <c r="S17" s="78">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="T17" s="89">
+      <c r="T17" s="78">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U17" s="89">
+      <c r="U17" s="78">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="V17" s="89">
+      <c r="V17" s="78">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W17" s="89">
+      <c r="W17" s="78">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88" t="s">
+    <row r="18" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="91">
-        <v>2</v>
-      </c>
-      <c r="C18" s="91">
-        <v>2</v>
-      </c>
-      <c r="D18" s="92" t="s">
+      <c r="B18" s="80">
+        <v>2</v>
+      </c>
+      <c r="C18" s="80">
+        <v>2</v>
+      </c>
+      <c r="D18" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="89" t="s">
+      <c r="E18" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="F18" s="89" t="s">
+      <c r="F18" s="78" t="s">
         <v>149</v>
       </c>
-      <c r="G18" s="89" t="s">
+      <c r="G18" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="89" t="s">
+      <c r="H18" s="78" t="s">
         <v>137</v>
       </c>
-      <c r="I18" s="89" t="s">
+      <c r="I18" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="J18" s="91" t="s">
+      <c r="J18" s="80" t="s">
         <v>148</v>
       </c>
-      <c r="K18" s="94" t="str">
+      <c r="K18" s="83" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: Loop%n📷🔍
 2: Recon%n💡💡🔊🔍
@@ -3852,85 +3973,85 @@
 6: Rake%n🔓🔓🔊➜
 </v>
       </c>
-      <c r="L18" s="91" t="s">
+      <c r="L18" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="M18" s="95" t="str">
+      <c r="M18" s="84" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="N18" s="91" t="s">
+      <c r="N18" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="O18" s="94" t="str">
+      <c r="O18" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P18" s="89">
+      <c r="P18" s="78">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="Q18" s="89">
+      <c r="Q18" s="78">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="R18" s="89">
+      <c r="R18" s="78">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="S18" s="89">
+      <c r="S18" s="78">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="T18" s="89">
+      <c r="T18" s="78">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U18" s="89">
+      <c r="U18" s="78">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="V18" s="89">
+      <c r="V18" s="78">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="W18" s="89">
+      <c r="W18" s="78">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="96" t="s">
+    <row r="19" spans="1:24" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="B19" s="91">
-        <v>2</v>
-      </c>
-      <c r="C19" s="91">
-        <v>2</v>
-      </c>
-      <c r="D19" s="92" t="s">
+      <c r="B19" s="80">
+        <v>2</v>
+      </c>
+      <c r="C19" s="80">
+        <v>2</v>
+      </c>
+      <c r="D19" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="97" t="s">
-        <v>210</v>
-      </c>
-      <c r="F19" s="89" t="s">
+      <c r="E19" s="86" t="s">
+        <v>202</v>
+      </c>
+      <c r="F19" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="G19" s="89" t="s">
+      <c r="G19" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="H19" s="89" t="s">
+      <c r="H19" s="78" t="s">
         <v>155</v>
       </c>
-      <c r="I19" s="89" t="s">
+      <c r="I19" s="78" t="s">
         <v>149</v>
       </c>
-      <c r="J19" s="89" t="s">
-        <v>199</v>
-      </c>
-      <c r="K19" s="94" t="str">
+      <c r="J19" s="78" t="s">
+        <v>195</v>
+      </c>
+      <c r="K19" s="83" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">1: Examine%n💡💡💡🔊
 2: Run%n🔊🔊➜➜
@@ -3940,54 +4061,54 @@
 6: Pick%n🔓
 </v>
       </c>
-      <c r="L19" s="91" t="s">
+      <c r="L19" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="M19" s="92" t="str">
+      <c r="M19" s="81" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="N19" s="91" t="s">
+      <c r="N19" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="O19" s="92" t="str">
+      <c r="O19" s="81" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P19" s="97">
+      <c r="P19" s="86">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="Q19" s="97">
+      <c r="Q19" s="86">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="R19" s="97">
+      <c r="R19" s="86">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="S19" s="97">
+      <c r="S19" s="86">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="T19" s="97">
+      <c r="T19" s="86">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U19" s="97">
+      <c r="U19" s="86">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="V19" s="97">
+      <c r="V19" s="86">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="W19" s="89">
+      <c r="W19" s="78">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X19" s="93" t="s">
-        <v>215</v>
+      <c r="X19" s="82" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4054,7 +4175,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4062,7 +4183,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -4071,7 +4192,7 @@
         <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -4080,7 +4201,7 @@
         <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -4089,7 +4210,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4097,15 +4218,15 @@
         <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4113,7 +4234,7 @@
         <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4121,7 +4242,7 @@
         <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4131,310 +4252,1209 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="9" width="6" style="100" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="87" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="99" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="99" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="99" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="H1" s="99" t="s">
+        <v>269</v>
+      </c>
+      <c r="I1" s="99" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="100">
+        <f>COUNTIF(Skills!E:E,$A2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="100">
+        <f>COUNTIF(Skills!F:F,$A2)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="100">
+        <f>COUNTIF(Skills!G:G,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="100">
+        <f>COUNTIF(Skills!H:H,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="100">
+        <f>COUNTIF(Skills!I:I,$A2)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="100">
+        <f>COUNTIF(Skills!J:J,$A2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="100">
+        <f>COUNTIF(Skills!E:E,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="100">
+        <f>COUNTIF(Skills!F:F,$A3)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="100">
+        <f>COUNTIF(Skills!G:G,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="100">
+        <f>COUNTIF(Skills!H:H,$A3)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="100">
+        <f>COUNTIF(Skills!I:I,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="100">
+        <f>COUNTIF(Skills!J:J,$A3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="100">
+        <f>COUNTIF(Skills!E:E,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="100">
+        <f>COUNTIF(Skills!F:F,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="100">
+        <f>COUNTIF(Skills!G:G,$A4)</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="100">
+        <f>COUNTIF(Skills!H:H,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="100">
+        <f>COUNTIF(Skills!I:I,$A4)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="100">
+        <f>COUNTIF(Skills!J:J,$A4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="100">
+        <f>COUNTIF(Skills!E:E,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="100">
+        <f>COUNTIF(Skills!F:F,$A5)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="100">
+        <f>COUNTIF(Skills!G:G,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="100">
+        <f>COUNTIF(Skills!H:H,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="100">
+        <f>COUNTIF(Skills!I:I,$A5)</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="100">
+        <f>COUNTIF(Skills!J:J,$A5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" t="s">
         <v>204</v>
       </c>
-      <c r="B1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D6" s="100">
+        <f>COUNTIF(Skills!E:E,$A6)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="100">
+        <f>COUNTIF(Skills!F:F,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="100">
+        <f>COUNTIF(Skills!G:G,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="100">
+        <f>COUNTIF(Skills!H:H,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="100">
+        <f>COUNTIF(Skills!I:I,$A6)</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="100">
+        <f>COUNTIF(Skills!J:J,$A6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="100">
+        <f>COUNTIF(Skills!E:E,$A7)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="100">
+        <f>COUNTIF(Skills!F:F,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="100">
+        <f>COUNTIF(Skills!G:G,$A7)</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="100">
+        <f>COUNTIF(Skills!H:H,$A7)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="100">
+        <f>COUNTIF(Skills!I:I,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="100">
+        <f>COUNTIF(Skills!J:J,$A7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="100">
+        <f>COUNTIF(Skills!E:E,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="100">
+        <f>COUNTIF(Skills!F:F,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="100">
+        <f>COUNTIF(Skills!G:G,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="100">
+        <f>COUNTIF(Skills!H:H,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="100">
+        <f>COUNTIF(Skills!I:I,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="100">
+        <f>COUNTIF(Skills!J:J,$A8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="100">
+        <f>COUNTIF(Skills!E:E,$A9)</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="100">
+        <f>COUNTIF(Skills!F:F,$A9)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="100">
+        <f>COUNTIF(Skills!G:G,$A9)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="100">
+        <f>COUNTIF(Skills!H:H,$A9)</f>
+        <v>2</v>
+      </c>
+      <c r="H9" s="100">
+        <f>COUNTIF(Skills!I:I,$A9)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="100">
+        <f>COUNTIF(Skills!J:J,$A9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="100">
+        <f>COUNTIF(Skills!E:E,$A10)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="100">
+        <f>COUNTIF(Skills!F:F,$A10)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="100">
+        <f>COUNTIF(Skills!G:G,$A10)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="100">
+        <f>COUNTIF(Skills!H:H,$A10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="100">
+        <f>COUNTIF(Skills!I:I,$A10)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="100">
+        <f>COUNTIF(Skills!J:J,$A10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="100">
+        <f>COUNTIF(Skills!E:E,$A11)</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="100">
+        <f>COUNTIF(Skills!F:F,$A11)</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="100">
+        <f>COUNTIF(Skills!G:G,$A11)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="100">
+        <f>COUNTIF(Skills!H:H,$A11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="100">
+        <f>COUNTIF(Skills!I:I,$A11)</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="100">
+        <f>COUNTIF(Skills!J:J,$A11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="100">
+        <f>COUNTIF(Skills!E:E,$A12)</f>
+        <v>3</v>
+      </c>
+      <c r="E12" s="100">
+        <f>COUNTIF(Skills!F:F,$A12)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="100">
+        <f>COUNTIF(Skills!G:G,$A12)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="100">
+        <f>COUNTIF(Skills!H:H,$A12)</f>
+        <v>2</v>
+      </c>
+      <c r="H12" s="100">
+        <f>COUNTIF(Skills!I:I,$A12)</f>
+        <v>3</v>
+      </c>
+      <c r="I12" s="100">
+        <f>COUNTIF(Skills!J:J,$A12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="100">
+        <f>COUNTIF(Skills!E:E,$A13)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="100">
+        <f>COUNTIF(Skills!F:F,$A13)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="100">
+        <f>COUNTIF(Skills!G:G,$A13)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="100">
+        <f>COUNTIF(Skills!H:H,$A13)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="100">
+        <f>COUNTIF(Skills!I:I,$A13)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="100">
+        <f>COUNTIF(Skills!J:J,$A13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="100">
+        <f>COUNTIF(Skills!E:E,$A14)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="100">
+        <f>COUNTIF(Skills!F:F,$A14)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="100">
+        <f>COUNTIF(Skills!G:G,$A14)</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="100">
+        <f>COUNTIF(Skills!H:H,$A14)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="100">
+        <f>COUNTIF(Skills!I:I,$A14)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="100">
+        <f>COUNTIF(Skills!J:J,$A14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>167</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D15" s="100">
+        <f>COUNTIF(Skills!E:E,$A15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="100">
+        <f>COUNTIF(Skills!F:F,$A15)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="100">
+        <f>COUNTIF(Skills!G:G,$A15)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="100">
+        <f>COUNTIF(Skills!H:H,$A15)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="100">
+        <f>COUNTIF(Skills!I:I,$A15)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="100">
+        <f>COUNTIF(Skills!J:J,$A15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D16" s="100">
+        <f>COUNTIF(Skills!E:E,$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="100">
+        <f>COUNTIF(Skills!F:F,$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="100">
+        <f>COUNTIF(Skills!G:G,$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="100">
+        <f>COUNTIF(Skills!H:H,$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="100">
+        <f>COUNTIF(Skills!I:I,$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="100">
+        <f>COUNTIF(Skills!J:J,$A16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="100">
+        <f>COUNTIF(Skills!E:E,$A17)</f>
+        <v>3</v>
+      </c>
+      <c r="E17" s="100">
+        <f>COUNTIF(Skills!F:F,$A17)</f>
+        <v>3</v>
+      </c>
+      <c r="F17" s="100">
+        <f>COUNTIF(Skills!G:G,$A17)</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="100">
+        <f>COUNTIF(Skills!H:H,$A17)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="100">
+        <f>COUNTIF(Skills!I:I,$A17)</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="100">
+        <f>COUNTIF(Skills!J:J,$A17)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="100">
+        <f>COUNTIF(Skills!E:E,$A18)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="100">
+        <f>COUNTIF(Skills!F:F,$A18)</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="100">
+        <f>COUNTIF(Skills!G:G,$A18)</f>
+        <v>2</v>
+      </c>
+      <c r="G18" s="100">
+        <f>COUNTIF(Skills!H:H,$A18)</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="100">
+        <f>COUNTIF(Skills!I:I,$A18)</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="100">
+        <f>COUNTIF(Skills!J:J,$A18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="100">
+        <f>COUNTIF(Skills!E:E,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="100">
+        <f>COUNTIF(Skills!F:F,$A19)</f>
+        <v>2</v>
+      </c>
+      <c r="F19" s="100">
+        <f>COUNTIF(Skills!G:G,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="100">
+        <f>COUNTIF(Skills!H:H,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="100">
+        <f>COUNTIF(Skills!I:I,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="100">
+        <f>COUNTIF(Skills!J:J,$A19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="100">
+        <f>COUNTIF(Skills!E:E,$A20)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="100">
+        <f>COUNTIF(Skills!F:F,$A20)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="100">
+        <f>COUNTIF(Skills!G:G,$A20)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="100">
+        <f>COUNTIF(Skills!H:H,$A20)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="100">
+        <f>COUNTIF(Skills!I:I,$A20)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="100">
+        <f>COUNTIF(Skills!J:J,$A20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" t="s">
+        <v>206</v>
+      </c>
+      <c r="D21" s="100">
+        <f>COUNTIF(Skills!E:E,$A21)</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="100">
+        <f>COUNTIF(Skills!F:F,$A21)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="100">
+        <f>COUNTIF(Skills!G:G,$A21)</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="100">
+        <f>COUNTIF(Skills!H:H,$A21)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="100">
+        <f>COUNTIF(Skills!I:I,$A21)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="100">
+        <f>COUNTIF(Skills!J:J,$A21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" s="100">
+        <f>COUNTIF(Skills!E:E,$A22)</f>
+        <v>1</v>
+      </c>
+      <c r="E22" s="100">
+        <f>COUNTIF(Skills!F:F,$A22)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="100">
+        <f>COUNTIF(Skills!G:G,$A22)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="100">
+        <f>COUNTIF(Skills!H:H,$A22)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="100">
+        <f>COUNTIF(Skills!I:I,$A22)</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="100">
+        <f>COUNTIF(Skills!J:J,$A22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D23" s="100">
+        <f>COUNTIF(Skills!E:E,$A23)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="100">
+        <f>COUNTIF(Skills!F:F,$A23)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="100">
+        <f>COUNTIF(Skills!G:G,$A23)</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="100">
+        <f>COUNTIF(Skills!H:H,$A23)</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="100">
+        <f>COUNTIF(Skills!I:I,$A23)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="100">
+        <f>COUNTIF(Skills!J:J,$A23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" s="100">
+        <f>COUNTIF(Skills!E:E,$A24)</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="100">
+        <f>COUNTIF(Skills!F:F,$A24)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="100">
+        <f>COUNTIF(Skills!G:G,$A24)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="100">
+        <f>COUNTIF(Skills!H:H,$A24)</f>
+        <v>2</v>
+      </c>
+      <c r="H24" s="100">
+        <f>COUNTIF(Skills!I:I,$A24)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="100">
+        <f>COUNTIF(Skills!J:J,$A24)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" t="s">
+        <v>205</v>
+      </c>
+      <c r="D25" s="100">
+        <f>COUNTIF(Skills!E:E,$A25)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="100">
+        <f>COUNTIF(Skills!F:F,$A25)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="100">
+        <f>COUNTIF(Skills!G:G,$A25)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="100">
+        <f>COUNTIF(Skills!H:H,$A25)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="100">
+        <f>COUNTIF(Skills!I:I,$A25)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="100">
+        <f>COUNTIF(Skills!J:J,$A25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>146</v>
       </c>
-      <c r="B9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B26" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" s="100">
+        <f>COUNTIF(Skills!E:E,$A26)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="100">
+        <f>COUNTIF(Skills!F:F,$A26)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="100">
+        <f>COUNTIF(Skills!G:G,$A26)</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="100">
+        <f>COUNTIF(Skills!H:H,$A26)</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="100">
+        <f>COUNTIF(Skills!I:I,$A26)</f>
+        <v>2</v>
+      </c>
+      <c r="I26" s="100">
+        <f>COUNTIF(Skills!J:J,$A26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="100">
+        <f>COUNTIF(Skills!E:E,$A27)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="100">
+        <f>COUNTIF(Skills!F:F,$A27)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="100">
+        <f>COUNTIF(Skills!G:G,$A27)</f>
+        <v>1</v>
+      </c>
+      <c r="G27" s="100">
+        <f>COUNTIF(Skills!H:H,$A27)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="100">
+        <f>COUNTIF(Skills!I:I,$A27)</f>
+        <v>2</v>
+      </c>
+      <c r="I27" s="100">
+        <f>COUNTIF(Skills!J:J,$A27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" s="100">
+        <f>COUNTIF(Skills!E:E,$A28)</f>
+        <v>1</v>
+      </c>
+      <c r="E28" s="100">
+        <f>COUNTIF(Skills!F:F,$A28)</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="100">
+        <f>COUNTIF(Skills!G:G,$A28)</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="100">
+        <f>COUNTIF(Skills!H:H,$A28)</f>
+        <v>3</v>
+      </c>
+      <c r="H28" s="100">
+        <f>COUNTIF(Skills!I:I,$A28)</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="100">
+        <f>COUNTIF(Skills!J:J,$A28)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" s="100">
+        <f>COUNTIF(Skills!E:E,$A29)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="100">
+        <f>COUNTIF(Skills!F:F,$A29)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="100">
+        <f>COUNTIF(Skills!G:G,$A29)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="100">
+        <f>COUNTIF(Skills!H:H,$A29)</f>
+        <v>1</v>
+      </c>
+      <c r="H29" s="100">
+        <f>COUNTIF(Skills!I:I,$A29)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="100">
+        <f>COUNTIF(Skills!J:J,$A29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" t="s">
+        <v>205</v>
+      </c>
+      <c r="D30" s="100">
+        <f>COUNTIF(Skills!E:E,$A30)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="100">
+        <f>COUNTIF(Skills!F:F,$A30)</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="100">
+        <f>COUNTIF(Skills!G:G,$A30)</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="100">
+        <f>COUNTIF(Skills!H:H,$A30)</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="100">
+        <f>COUNTIF(Skills!I:I,$A30)</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="100">
+        <f>COUNTIF(Skills!J:J,$A30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s">
+        <v>205</v>
+      </c>
+      <c r="D31" s="100">
+        <f>COUNTIF(Skills!E:E,$A31)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="100">
+        <f>COUNTIF(Skills!F:F,$A31)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="100">
+        <f>COUNTIF(Skills!G:G,$A31)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="100">
+        <f>COUNTIF(Skills!H:H,$A31)</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="100">
+        <f>COUNTIF(Skills!I:I,$A31)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="100">
+        <f>COUNTIF(Skills!J:J,$A31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>228</v>
+      </c>
+      <c r="B32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" s="100">
+        <f>COUNTIF(Skills!E:E,$A32)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="100">
+        <f>COUNTIF(Skills!F:F,$A32)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="100">
+        <f>COUNTIF(Skills!G:G,$A32)</f>
+        <v>1</v>
+      </c>
+      <c r="G32" s="100">
+        <f>COUNTIF(Skills!H:H,$A32)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="100">
+        <f>COUNTIF(Skills!I:I,$A32)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="100">
+        <f>COUNTIF(Skills!J:J,$A32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>180</v>
+      </c>
+      <c r="B33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D33" s="100">
+        <f>COUNTIF(Skills!E:E,$A33)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="100">
+        <f>COUNTIF(Skills!F:F,$A33)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="100">
+        <f>COUNTIF(Skills!G:G,$A33)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="100">
+        <f>COUNTIF(Skills!H:H,$A33)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="100">
+        <f>COUNTIF(Skills!I:I,$A33)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="100">
+        <f>COUNTIF(Skills!J:J,$A33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>199</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D34" s="100">
+        <f>COUNTIF(Skills!E:E,$A34)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="100">
+        <f>COUNTIF(Skills!F:F,$A34)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="100">
+        <f>COUNTIF(Skills!G:G,$A34)</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="100">
+        <f>COUNTIF(Skills!H:H,$A34)</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="100">
+        <f>COUNTIF(Skills!I:I,$A34)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="100">
+        <f>COUNTIF(Skills!J:J,$A34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D35" s="100">
+        <f>COUNTIF(Skills!E:E,$A35)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="100">
+        <f>COUNTIF(Skills!F:F,$A35)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="100">
+        <f>COUNTIF(Skills!G:G,$A35)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="100">
+        <f>COUNTIF(Skills!H:H,$A35)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="100">
+        <f>COUNTIF(Skills!I:I,$A35)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="100">
+        <f>COUNTIF(Skills!J:J,$A35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>148</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B36" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>155</v>
-      </c>
-      <c r="B20" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>230</v>
-      </c>
-      <c r="B22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D36" s="100">
+        <f>COUNTIF(Skills!E:E,$A36)</f>
+        <v>1</v>
+      </c>
+      <c r="E36" s="100">
+        <f>COUNTIF(Skills!F:F,$A36)</f>
+        <v>2</v>
+      </c>
+      <c r="F36" s="100">
+        <f>COUNTIF(Skills!G:G,$A36)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="100">
+        <f>COUNTIF(Skills!H:H,$A36)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="100">
+        <f>COUNTIF(Skills!I:I,$A36)</f>
+        <v>1</v>
+      </c>
+      <c r="I36" s="100">
+        <f>COUNTIF(Skills!J:J,$A36)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>147</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B37" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>151</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>200</v>
-      </c>
-      <c r="B28" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B29" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>159</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>166</v>
-      </c>
-      <c r="B31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>138</v>
-      </c>
-      <c r="B32" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>236</v>
-      </c>
-      <c r="B35" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>207</v>
-      </c>
-      <c r="B36" t="s">
-        <v>184</v>
+      <c r="D37" s="100">
+        <f>COUNTIF(Skills!E:E,$A37)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="100">
+        <f>COUNTIF(Skills!F:F,$A37)</f>
+        <v>1</v>
+      </c>
+      <c r="F37" s="100">
+        <f>COUNTIF(Skills!G:G,$A37)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="100">
+        <f>COUNTIF(Skills!H:H,$A37)</f>
+        <v>1</v>
+      </c>
+      <c r="H37" s="100">
+        <f>COUNTIF(Skills!I:I,$A37)</f>
+        <v>1</v>
+      </c>
+      <c r="I37" s="100">
+        <f>COUNTIF(Skills!J:J,$A37)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B34">
-    <sortCondition ref="A1:A34"/>
+  <sortState ref="A2:B37">
+    <sortCondition ref="B2:B37"/>
   </sortState>
+  <conditionalFormatting sqref="D2:I37">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5814,10 +6834,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5828,7 +6848,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5842,7 +6862,7 @@
         <v>133</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5856,7 +6876,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5870,7 +6890,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5884,7 +6904,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5898,31 +6918,76 @@
         <v>5</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>220</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -5932,20 +6997,117 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="101" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hackers: trying out EXPLOIT
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -22,14 +22,14 @@
     <sheet name="Tile ideas" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Actions">Actions!$A$2:$B$37</definedName>
+    <definedName name="Actions">Actions!$A$2:$B$38</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="358">
   <si>
     <t>Name</t>
   </si>
@@ -619,9 +619,6 @@
     <t>Concoct</t>
   </si>
   <si>
-    <t>Discover%n🔍🔍</t>
-  </si>
-  <si>
     <t>Tons of ideas and recon, low noise, but has everything in one move</t>
   </si>
   <si>
@@ -1090,10 +1087,22 @@
     <t>One character loses all of his ideas if he is standing on a gate or something</t>
   </si>
   <si>
-    <t>I CAN HAZ TEH CODES?%nOnce per turn, may spend 💡💡💡 to re-position 1 planning token of any player.%n %nLISTEN TO ME%nMay use Action to provide an available Skill sub-action to another player.</t>
-  </si>
-  <si>
-    <t>HAS THE CODE%nOnce per turn, may spend 💡💡 to re-position 1 planning token of any player%n %nLISTEN TO ME%nMay use Action to provide an available Skill sub-action to another player.</t>
+    <t>Stride</t>
+  </si>
+  <si>
+    <t>🔊➜🔍</t>
+  </si>
+  <si>
+    <t>Stride%n🔊➜🔍</t>
+  </si>
+  <si>
+    <t>Exploit%n(see above)</t>
+  </si>
+  <si>
+    <t>I CAN HAZ TEH CODES?%nOnce per turn, may spend 💡💡💡 to re-position 1 planning token of any player.%n %nEXPLOIT%nUse this Action to enable another player to 👊🔊, 📷🔊 or 🔓🔊. Spend 💡 when you do this.</t>
+  </si>
+  <si>
+    <t>HAS THE CODE%nOnce per turn, may spend 💡💡 to re-position 1 planning token of any player%n %nEXPLOIT%nUse this Action to enable another player to 👊🔊, 📷🔊 or 🔓🔊. Spend 💡 when you do this.</t>
   </si>
 </sst>
 </file>
@@ -2010,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2032,7 @@
     <col min="5" max="5" width="8.5703125" style="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.7109375" style="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="29" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="28" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" style="28" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="158.85546875" style="28" bestFit="1" customWidth="1"/>
@@ -2098,10 +2107,10 @@
         <v>6</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>82</v>
@@ -2135,7 +2144,7 @@
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>82</v>
@@ -2143,7 +2152,7 @@
     </row>
     <row r="4" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>165</v>
@@ -2169,7 +2178,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>82</v>
@@ -2201,7 +2210,7 @@
         <v>173</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J5" s="15" t="s">
         <v>8</v>
@@ -2215,7 +2224,7 @@
     </row>
     <row r="6" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>25</v>
@@ -2241,7 +2250,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>82</v>
@@ -2275,7 +2284,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L7" s="20" t="s">
         <v>82</v>
@@ -2313,7 +2322,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L8" s="19" t="s">
         <v>82</v>
@@ -2347,7 +2356,7 @@
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L9" s="19"/>
     </row>
@@ -2379,7 +2388,7 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>82</v>
@@ -2405,10 +2414,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>146</v>
+        <v>354</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>196</v>
+        <v>355</v>
       </c>
       <c r="I11" s="24" t="s">
         <v>4</v>
@@ -2417,7 +2426,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="L11" s="22"/>
     </row>
@@ -2441,15 +2450,15 @@
         <v>6</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>146</v>
+        <v>354</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>196</v>
+        <v>355</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="L12" s="22" t="s">
         <v>82</v>
@@ -2475,15 +2484,15 @@
         <v>6</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>146</v>
+        <v>354</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>196</v>
+        <v>355</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="L13" s="22" t="s">
         <v>82</v>
@@ -2521,7 +2530,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L14" s="21" t="s">
         <v>82</v>
@@ -2553,7 +2562,7 @@
         <v>136</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L15" s="21" t="s">
         <v>82</v>
@@ -2587,7 +2596,7 @@
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
       <c r="K16" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L16" s="21" t="s">
         <v>82</v>
@@ -2619,13 +2628,13 @@
         <v>136</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J17" s="26" t="s">
         <v>40</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L17" s="23" t="s">
         <v>82</v>
@@ -2633,7 +2642,7 @@
     </row>
     <row r="18" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>157</v>
@@ -2657,7 +2666,7 @@
         <v>135</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L18" s="23" t="s">
         <v>82</v>
@@ -2689,7 +2698,7 @@
         <v>160</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L19" s="23" t="s">
         <v>82</v>
@@ -2718,7 +2727,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB19" sqref="AB19"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,40 +2783,40 @@
         <v>176</v>
       </c>
       <c r="E1" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="F1" s="101" t="s">
         <v>251</v>
       </c>
-      <c r="F1" s="101" t="s">
-        <v>252</v>
-      </c>
       <c r="G1" s="118" t="s">
+        <v>317</v>
+      </c>
+      <c r="H1" s="100" t="s">
         <v>318</v>
       </c>
-      <c r="H1" s="100" t="s">
+      <c r="I1" s="105" t="s">
         <v>319</v>
       </c>
-      <c r="I1" s="105" t="s">
+      <c r="J1" s="101" t="s">
         <v>320</v>
       </c>
-      <c r="J1" s="101" t="s">
+      <c r="K1" s="118" t="s">
         <v>321</v>
       </c>
-      <c r="K1" s="118" t="s">
+      <c r="L1" s="100" t="s">
         <v>322</v>
       </c>
-      <c r="L1" s="100" t="s">
+      <c r="M1" s="105" t="s">
         <v>323</v>
       </c>
-      <c r="M1" s="105" t="s">
+      <c r="N1" s="101" t="s">
         <v>324</v>
       </c>
-      <c r="N1" s="101" t="s">
+      <c r="O1" s="118" t="s">
         <v>325</v>
       </c>
-      <c r="O1" s="118" t="s">
+      <c r="P1" s="101" t="s">
         <v>326</v>
-      </c>
-      <c r="P1" s="101" t="s">
-        <v>327</v>
       </c>
       <c r="Q1" s="100">
         <v>1</v>
@@ -2891,35 +2900,35 @@
         <v>🔍</v>
       </c>
       <c r="G2" s="119" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H2" s="42" t="str">
         <f t="shared" ref="H2:H19" si="1">VLOOKUP(G2,Actions,2,FALSE)</f>
         <v>🔓🔊🔊➜</v>
       </c>
       <c r="I2" s="106" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J2" s="87" t="str">
         <f t="shared" ref="J2:J19" si="2">VLOOKUP(I2,Actions,2,FALSE)</f>
         <v>📷🔊➜</v>
       </c>
       <c r="K2" s="119" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L2" s="42" t="str">
         <f t="shared" ref="L2:L19" si="3">VLOOKUP(K2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M2" s="106" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N2" s="87" t="str">
         <f t="shared" ref="N2:N19" si="4">VLOOKUP(M2,Actions,2,FALSE)</f>
         <v>💡💡</v>
       </c>
       <c r="O2" s="119" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P2" s="87" t="str">
         <f t="shared" ref="P2:P19" si="5">VLOOKUP(O2,Actions,2,FALSE)</f>
@@ -3027,42 +3036,42 @@
         <v>162</v>
       </c>
       <c r="E3" s="107" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F3" s="88" t="str">
         <f t="shared" si="0"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="G3" s="120" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H3" s="44" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="I3" s="107" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J3" s="88" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K3" s="120" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L3" s="44" t="str">
         <f t="shared" si="3"/>
         <v>💡➜</v>
       </c>
       <c r="M3" s="107" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N3" s="88" t="str">
         <f t="shared" si="4"/>
         <v>👊💡➜</v>
       </c>
       <c r="O3" s="120" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P3" s="88" t="str">
         <f t="shared" si="5"/>
@@ -3165,28 +3174,28 @@
         <v>162</v>
       </c>
       <c r="E4" s="107" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F4" s="88" t="str">
         <f t="shared" si="0"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G4" s="120" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H4" s="44" t="str">
         <f t="shared" si="1"/>
         <v>📷🔊➜</v>
       </c>
       <c r="I4" s="107" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J4" s="88" t="str">
         <f t="shared" si="2"/>
         <v>🔓🔊➜</v>
       </c>
       <c r="K4" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L4" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3200,7 +3209,7 @@
         <v>🔍</v>
       </c>
       <c r="O4" s="120" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P4" s="88" t="str">
         <f t="shared" si="5"/>
@@ -3298,42 +3307,42 @@
         <v>130</v>
       </c>
       <c r="E5" s="108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F5" s="89" t="str">
         <f t="shared" si="0"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G5" s="121" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H5" s="37" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I5" s="109" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J5" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K5" s="127" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L5" s="37" t="str">
         <f t="shared" si="3"/>
         <v>🔓🔊🔊➜</v>
       </c>
       <c r="M5" s="109" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N5" s="89" t="str">
         <f t="shared" si="4"/>
         <v>💡💡</v>
       </c>
       <c r="O5" s="121" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P5" s="89" t="str">
         <f t="shared" si="5"/>
@@ -3431,42 +3440,42 @@
         <v>130</v>
       </c>
       <c r="E6" s="109" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F6" s="90" t="str">
         <f t="shared" si="0"/>
         <v>🔓👊📷🔊</v>
       </c>
       <c r="G6" s="121" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H6" s="35" t="str">
         <f t="shared" si="1"/>
         <v>💡➜</v>
       </c>
       <c r="I6" s="109" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J6" s="90" t="str">
         <f t="shared" si="2"/>
         <v>🔓👊📷🔊</v>
       </c>
       <c r="K6" s="121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L6" s="35" t="str">
         <f t="shared" si="3"/>
         <v>🔍➜➜</v>
       </c>
       <c r="M6" s="109" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N6" s="90" t="str">
         <f t="shared" si="4"/>
         <v>👊💡➜</v>
       </c>
       <c r="O6" s="121" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P6" s="90" t="str">
         <f t="shared" si="5"/>
@@ -3564,42 +3573,42 @@
         <v>130</v>
       </c>
       <c r="E7" s="109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7" s="90" t="str">
         <f t="shared" si="0"/>
         <v>🔍➜➜</v>
       </c>
       <c r="G7" s="121" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H7" s="36" t="str">
         <f t="shared" si="1"/>
         <v>👊➜</v>
       </c>
       <c r="I7" s="109" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J7" s="90" t="str">
         <f t="shared" si="2"/>
         <v>💡➜</v>
       </c>
       <c r="K7" s="128" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L7" s="36" t="str">
         <f t="shared" si="3"/>
         <v>👊➜</v>
       </c>
       <c r="M7" s="109" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N7" s="90" t="str">
         <f t="shared" si="4"/>
         <v>💡➜</v>
       </c>
       <c r="O7" s="121" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P7" s="90" t="str">
         <f t="shared" si="5"/>
@@ -3697,42 +3706,42 @@
         <v>127</v>
       </c>
       <c r="E8" s="110" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F8" s="91" t="str">
         <f t="shared" si="0"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G8" s="122" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H8" s="53" t="str">
         <f t="shared" si="1"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="I8" s="111" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J8" s="91" t="str">
         <f t="shared" si="2"/>
         <v>🔓🔊🔊➜</v>
       </c>
       <c r="K8" s="129" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L8" s="53" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M8" s="111" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N8" s="91" t="str">
         <f t="shared" si="4"/>
         <v>💡💡</v>
       </c>
       <c r="O8" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P8" s="91" t="str">
         <f t="shared" si="5"/>
@@ -3830,42 +3839,42 @@
         <v>127</v>
       </c>
       <c r="E9" s="111" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F9" s="92" t="str">
         <f t="shared" si="0"/>
         <v>💡💡</v>
       </c>
       <c r="G9" s="122" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H9" s="55" t="str">
         <f t="shared" si="1"/>
         <v>🔍🔍</v>
       </c>
       <c r="I9" s="111" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J9" s="92" t="str">
         <f t="shared" si="2"/>
         <v>👊💡➜</v>
       </c>
       <c r="K9" s="122" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L9" s="55" t="str">
         <f t="shared" si="3"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="M9" s="111" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N9" s="92" t="str">
         <f t="shared" si="4"/>
         <v>🔓📷🔊➜</v>
       </c>
       <c r="O9" s="122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P9" s="92" t="str">
         <f t="shared" si="5"/>
@@ -3946,7 +3955,7 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:36" s="57" customFormat="1" x14ac:dyDescent="0.25">
@@ -3963,42 +3972,42 @@
         <v>127</v>
       </c>
       <c r="E10" s="111" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F10" s="92" t="str">
         <f t="shared" si="0"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="G10" s="122" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H10" s="58" t="str">
         <f t="shared" si="1"/>
         <v>🔓📷🔊➜</v>
       </c>
       <c r="I10" s="111" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J10" s="92" t="str">
         <f t="shared" si="2"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="K10" s="130" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L10" s="58" t="str">
         <f t="shared" si="3"/>
         <v>🔓🔊➜</v>
       </c>
       <c r="M10" s="111" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N10" s="92" t="str">
         <f t="shared" si="4"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="O10" s="122" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P10" s="92" t="str">
         <f t="shared" si="5"/>
@@ -4079,7 +4088,7 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:36" s="67" customFormat="1" x14ac:dyDescent="0.25">
@@ -4096,42 +4105,42 @@
         <v>129</v>
       </c>
       <c r="E11" s="112" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F11" s="93" t="str">
         <f t="shared" si="0"/>
         <v>💡💡</v>
       </c>
       <c r="G11" s="123" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H11" s="65" t="str">
         <f t="shared" si="1"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="I11" s="113" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J11" s="93" t="str">
         <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K11" s="131" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L11" s="65" t="str">
         <f t="shared" si="3"/>
         <v>📷🔊➜</v>
       </c>
       <c r="M11" s="113" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N11" s="93" t="str">
         <f t="shared" si="4"/>
         <v>👊🔊➜➜</v>
       </c>
       <c r="O11" s="123" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P11" s="93" t="str">
         <f t="shared" si="5"/>
@@ -4212,7 +4221,7 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:36" s="67" customFormat="1" x14ac:dyDescent="0.25">
@@ -4229,42 +4238,42 @@
         <v>129</v>
       </c>
       <c r="E12" s="113" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F12" s="94" t="str">
         <f t="shared" si="0"/>
         <v>💰💰</v>
       </c>
       <c r="G12" s="123" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H12" s="66" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="I12" s="113" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J12" s="94" t="str">
         <f t="shared" si="2"/>
         <v>👊🔊➜➜</v>
       </c>
       <c r="K12" s="123" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L12" s="66" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M12" s="113" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N12" s="94" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊➜</v>
       </c>
       <c r="O12" s="123" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P12" s="94" t="str">
         <f t="shared" si="5"/>
@@ -4350,7 +4359,7 @@
         <v>2</v>
       </c>
       <c r="AJ12" s="67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:36" s="67" customFormat="1" x14ac:dyDescent="0.25">
@@ -4367,42 +4376,42 @@
         <v>129</v>
       </c>
       <c r="E13" s="113" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F13" s="94" t="str">
         <f t="shared" si="0"/>
         <v>🔓📷🔊➜</v>
       </c>
       <c r="G13" s="123" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H13" s="66" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I13" s="113" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J13" s="94" t="str">
         <f t="shared" si="2"/>
         <v>💡➜</v>
       </c>
       <c r="K13" s="123" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L13" s="66" t="str">
         <f t="shared" si="3"/>
         <v>👊👊🔊🔊➜➜</v>
       </c>
       <c r="M13" s="113" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N13" s="94" t="str">
         <f t="shared" si="4"/>
         <v>🔓👊📷🔊🔊⚠</v>
       </c>
       <c r="O13" s="123" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P13" s="94" t="str">
         <f t="shared" si="5"/>
@@ -4483,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="AJ13" s="67" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:36" s="78" customFormat="1" x14ac:dyDescent="0.25">
@@ -4500,42 +4509,42 @@
         <v>128</v>
       </c>
       <c r="E14" s="114" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F14" s="95" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G14" s="124" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H14" s="75" t="str">
         <f t="shared" si="1"/>
         <v>💰🔊</v>
       </c>
       <c r="I14" s="115" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J14" s="95" t="str">
         <f t="shared" si="2"/>
         <v>🔓🔊🔊➜</v>
       </c>
       <c r="K14" s="132" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L14" s="75" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M14" s="115" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N14" s="95" t="str">
         <f t="shared" si="4"/>
         <v>🔓🔊🔊➜</v>
       </c>
       <c r="O14" s="124" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P14" s="95" t="str">
         <f t="shared" si="5"/>
@@ -4633,42 +4642,42 @@
         <v>128</v>
       </c>
       <c r="E15" s="114" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F15" s="95" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G15" s="124" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H15" s="81" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I15" s="115" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J15" s="95" t="str">
         <f t="shared" si="2"/>
         <v>💰🔊</v>
       </c>
       <c r="K15" s="133" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L15" s="81" t="str">
         <f t="shared" si="3"/>
         <v>👊👊👊🔊🔊</v>
       </c>
       <c r="M15" s="115" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N15" s="95" t="str">
         <f t="shared" si="4"/>
         <v>👊🔊➜➜</v>
       </c>
       <c r="O15" s="124" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P15" s="95" t="str">
         <f t="shared" si="5"/>
@@ -4763,42 +4772,42 @@
         <v>128</v>
       </c>
       <c r="E16" s="115" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F16" s="96" t="str">
         <f t="shared" si="0"/>
         <v>🔓👊📷🔊🔊⚠</v>
       </c>
       <c r="G16" s="124" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H16" s="77" t="str">
         <f t="shared" si="1"/>
         <v>💰💰</v>
       </c>
       <c r="I16" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J16" s="96" t="str">
         <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K16" s="124" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L16" s="77" t="str">
         <f t="shared" si="3"/>
         <v>🔍➜➜</v>
       </c>
       <c r="M16" s="115" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N16" s="96" t="str">
         <f t="shared" si="4"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="O16" s="124" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P16" s="96" t="str">
         <f t="shared" si="5"/>
@@ -4893,14 +4902,14 @@
         <v>126</v>
       </c>
       <c r="E17" s="137" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F17" s="138" t="str">
         <f t="shared" si="0"/>
         <v>💡💡</v>
       </c>
       <c r="G17" s="139" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H17" s="136" t="str">
         <f t="shared" si="1"/>
@@ -4914,21 +4923,21 @@
         <v>👊</v>
       </c>
       <c r="K17" s="141" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L17" s="136" t="str">
         <f t="shared" si="3"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="M17" s="140" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N17" s="138" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O17" s="139" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P17" s="138" t="str">
         <f t="shared" si="5"/>
@@ -5023,42 +5032,42 @@
         <v>126</v>
       </c>
       <c r="E18" s="140" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F18" s="145" t="str">
         <f t="shared" si="0"/>
         <v>📷🔍</v>
       </c>
       <c r="G18" s="139" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H18" s="143" t="str">
         <f t="shared" si="1"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="I18" s="140" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J18" s="145" t="str">
         <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K18" s="139" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L18" s="143" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M18" s="140" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N18" s="145" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="O18" s="139" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P18" s="145" t="str">
         <f t="shared" si="5"/>
@@ -5153,42 +5162,42 @@
         <v>126</v>
       </c>
       <c r="E19" s="140" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F19" s="145" t="str">
         <f t="shared" si="0"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="G19" s="139" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H19" s="143" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I19" s="140" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J19" s="145" t="str">
         <f t="shared" si="2"/>
         <v>📷🔍</v>
       </c>
       <c r="K19" s="139" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L19" s="143" t="str">
         <f t="shared" si="3"/>
         <v>🔓👊📷🔊</v>
       </c>
       <c r="M19" s="140" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N19" s="145" t="str">
         <f t="shared" si="4"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="O19" s="139" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P19" s="145" t="str">
         <f t="shared" si="5"/>
@@ -5334,7 +5343,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5355,7 +5364,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5363,7 +5372,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -5372,7 +5381,7 @@
         <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -5390,7 +5399,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5398,7 +5407,7 @@
         <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5432,10 +5441,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5449,39 +5458,39 @@
   <sheetData>
     <row r="1" spans="1:10" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="72" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="72" t="s">
-        <v>317</v>
-      </c>
-      <c r="C1" s="72" t="s">
+      <c r="E1" s="84" t="s">
         <v>229</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="F1" s="84" t="s">
         <v>230</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="G1" s="84" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="H1" s="84" t="s">
         <v>232</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="I1" s="84" t="s">
         <v>233</v>
       </c>
-      <c r="I1" s="84" t="s">
+      <c r="J1" s="84" t="s">
         <v>234</v>
-      </c>
-      <c r="J1" s="84" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" t="s">
         <v>265</v>
-      </c>
-      <c r="B2" t="s">
-        <v>266</v>
       </c>
       <c r="C2" t="s">
         <v>179</v>
@@ -5513,7 +5522,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s">
         <v>104</v>
@@ -5548,10 +5557,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" t="s">
         <v>268</v>
-      </c>
-      <c r="B4" t="s">
-        <v>269</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -5583,10 +5592,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C5" t="s">
         <v>177</v>
@@ -5618,10 +5627,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C6" t="s">
         <v>178</v>
@@ -5653,10 +5662,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7" t="s">
         <v>272</v>
-      </c>
-      <c r="B7" t="s">
-        <v>273</v>
       </c>
       <c r="C7" t="s">
         <v>177</v>
@@ -5688,10 +5697,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" t="s">
         <v>274</v>
-      </c>
-      <c r="B8" t="s">
-        <v>275</v>
       </c>
       <c r="C8" t="s">
         <v>180</v>
@@ -5723,10 +5732,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C9" t="s">
         <v>170</v>
@@ -5758,7 +5767,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B10" t="s">
         <v>108</v>
@@ -5793,10 +5802,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>277</v>
+      </c>
+      <c r="B11" t="s">
         <v>278</v>
-      </c>
-      <c r="B11" t="s">
-        <v>279</v>
       </c>
       <c r="C11" t="s">
         <v>179</v>
@@ -5828,10 +5837,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
@@ -5863,10 +5872,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" t="s">
         <v>281</v>
-      </c>
-      <c r="B13" t="s">
-        <v>282</v>
       </c>
       <c r="C13" t="s">
         <v>179</v>
@@ -5898,10 +5907,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C14" t="s">
         <v>180</v>
@@ -5933,10 +5942,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C15" t="s">
         <v>161</v>
@@ -5968,45 +5977,18 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>313</v>
+        <v>352</v>
       </c>
       <c r="B16" t="s">
-        <v>287</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="85">
-        <f>COUNTIF(Skills!Q:Q,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="85">
-        <f>COUNTIF(Skills!R:R,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="85">
-        <f>COUNTIF(Skills!S:S,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="85">
-        <f>COUNTIF(Skills!T:T,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="85">
-        <f>COUNTIF(Skills!U:U,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="85">
-        <f>COUNTIF(Skills!V:V,#REF!)</f>
-        <v>0</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>285</v>
+        <v>312</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>286</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -6038,13 +6020,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>261</v>
+        <v>284</v>
       </c>
       <c r="B18" t="s">
-        <v>288</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>23</v>
       </c>
       <c r="E18" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6073,13 +6055,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>179</v>
       </c>
       <c r="E19" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6108,13 +6090,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
       <c r="B20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>23</v>
       </c>
       <c r="E20" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6143,13 +6125,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>253</v>
+        <v>289</v>
       </c>
       <c r="B21" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C21" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="E21" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6178,13 +6160,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B22" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E22" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6213,13 +6195,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>254</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
+        <v>292</v>
       </c>
       <c r="C23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E23" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6248,13 +6230,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>254</v>
+        <v>180</v>
       </c>
       <c r="B24" t="s">
-        <v>294</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="E24" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6281,15 +6263,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="B25" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E25" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6316,15 +6298,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="B26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C26" t="s">
-        <v>179</v>
+        <v>23</v>
       </c>
       <c r="E26" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6353,13 +6335,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="B27" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="E27" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6388,13 +6370,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>256</v>
+        <v>297</v>
       </c>
       <c r="B28" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C28" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
       <c r="E28" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6423,13 +6405,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>315</v>
+        <v>255</v>
       </c>
       <c r="B29" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E29" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6458,13 +6440,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B30" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="C30" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E30" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6493,13 +6475,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B31" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="E31" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6528,13 +6510,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="B32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C32" t="s">
-        <v>178</v>
+        <v>21</v>
       </c>
       <c r="E32" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6563,13 +6545,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>257</v>
+        <v>315</v>
       </c>
       <c r="B33" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C33" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="E33" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6598,13 +6580,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>256</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>305</v>
       </c>
       <c r="C34" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E34" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6633,13 +6615,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>307</v>
+        <v>179</v>
       </c>
       <c r="B35" t="s">
-        <v>308</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E35" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6668,13 +6650,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="B36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="E36" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6703,13 +6685,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
       <c r="B37" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
       <c r="E37" s="85">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6736,8 +6718,43 @@
         <v>0</v>
       </c>
     </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>309</v>
+      </c>
+      <c r="B38" t="s">
+        <v>310</v>
+      </c>
+      <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" s="85">
+        <f>COUNTIF(Skills!Q:Q,#REF!)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="85">
+        <f>COUNTIF(Skills!R:R,#REF!)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="85">
+        <f>COUNTIF(Skills!S:S,#REF!)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="85">
+        <f>COUNTIF(Skills!T:T,#REF!)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="85">
+        <f>COUNTIF(Skills!U:U,#REF!)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="85">
+        <f>COUNTIF(Skills!V:V,#REF!)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:J37">
+  <conditionalFormatting sqref="E2:J38">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -6752,7 +6769,7 @@
   <dimension ref="A7:S31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8141,13 +8158,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E1" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="F1" s="72" t="s">
         <v>328</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="G1" s="72" t="s">
         <v>329</v>
-      </c>
-      <c r="G1" s="72" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8164,13 +8181,13 @@
         <v>149</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8187,10 +8204,10 @@
         <v>150</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="G3" t="s">
         <v>332</v>
-      </c>
-      <c r="G3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8207,13 +8224,13 @@
         <v>151</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8230,7 +8247,7 @@
         <v>152</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8247,13 +8264,13 @@
         <v>154</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8270,13 +8287,13 @@
         <v>153</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -8291,7 +8308,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -8301,37 +8318,37 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -8362,35 +8379,35 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="86" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -8413,50 +8430,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" t="s">
         <v>210</v>
-      </c>
-      <c r="B1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" t="s">
         <v>239</v>
-      </c>
-      <c r="B3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" t="s">
         <v>241</v>
-      </c>
-      <c r="B4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" t="s">
         <v>243</v>
-      </c>
-      <c r="B5" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B6" t="s">
         <v>246</v>
-      </c>
-      <c r="B6" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skills: add "Lacks" to card. :bulb:
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="383">
   <si>
     <t>Name</t>
   </si>
@@ -520,9 +520,6 @@
     <t>Dash%n🔊➜➜</t>
   </si>
   <si>
-    <t>Loot. Gain $1k for your person.</t>
-  </si>
-  <si>
     <t>Alert. Increase alert level by 1</t>
   </si>
   <si>
@@ -622,12 +619,6 @@
     <t>Move to adjacent, planned, not locked tile</t>
   </si>
   <si>
-    <t>Unlock 1 locked, adjacent tile</t>
-  </si>
-  <si>
-    <t>Idea. Add 1 Idea to your character</t>
-  </si>
-  <si>
     <t>Crowded!</t>
   </si>
   <si>
@@ -1105,9 +1096,6 @@
     <t>Zap</t>
   </si>
   <si>
-    <t>Shortcircuit</t>
-  </si>
-  <si>
     <t>Lacks</t>
   </si>
   <si>
@@ -1175,6 +1163,21 @@
   </si>
   <si>
     <t>Cameras, Multi-moves</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Unlock 1 lock adjacent to your tile</t>
+  </si>
+  <si>
+    <t>Loot. Add $1k to your character</t>
+  </si>
+  <si>
+    <t>Add 1 Idea to your character</t>
+  </si>
+  <si>
+    <t>These are the old skill ideas</t>
   </si>
 </sst>
 </file>
@@ -2126,7 +2129,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G1" s="31" t="s">
         <v>141</v>
@@ -2170,16 +2173,16 @@
         <v>145</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>81</v>
@@ -2208,12 +2211,12 @@
         <v>145</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>81</v>
@@ -2221,7 +2224,7 @@
     </row>
     <row r="4" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>161</v>
@@ -2242,12 +2245,12 @@
         <v>145</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>81</v>
@@ -2276,10 +2279,10 @@
         <v>143</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J5" s="15" t="s">
         <v>8</v>
@@ -2293,7 +2296,7 @@
     </row>
     <row r="6" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>25</v>
@@ -2314,12 +2317,12 @@
         <v>143</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>81</v>
@@ -2353,7 +2356,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L7" s="20" t="s">
         <v>81</v>
@@ -2391,7 +2394,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L8" s="19" t="s">
         <v>81</v>
@@ -2425,7 +2428,7 @@
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L9" s="19"/>
     </row>
@@ -2457,7 +2460,7 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>81</v>
@@ -2483,10 +2486,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I11" s="24" t="s">
         <v>4</v>
@@ -2495,7 +2498,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="L11" s="22"/>
     </row>
@@ -2519,15 +2522,15 @@
         <v>6</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="L12" s="22" t="s">
         <v>81</v>
@@ -2553,15 +2556,15 @@
         <v>6</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="L13" s="22" t="s">
         <v>81</v>
@@ -2587,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>133</v>
@@ -2599,7 +2602,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="L14" s="21" t="s">
         <v>81</v>
@@ -2625,13 +2628,13 @@
         <v>4</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>133</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L15" s="21" t="s">
         <v>81</v>
@@ -2657,7 +2660,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>133</v>
@@ -2665,7 +2668,7 @@
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
       <c r="K16" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L16" s="21" t="s">
         <v>81</v>
@@ -2697,13 +2700,13 @@
         <v>133</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J17" s="26" t="s">
         <v>39</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L17" s="23" t="s">
         <v>81</v>
@@ -2711,7 +2714,7 @@
     </row>
     <row r="18" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>154</v>
@@ -2735,7 +2738,7 @@
         <v>132</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="L18" s="23" t="s">
         <v>81</v>
@@ -2767,7 +2770,7 @@
         <v>157</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="L19" s="23" t="s">
         <v>81</v>
@@ -2796,7 +2799,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2852,43 +2855,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="99" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E1" s="104" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F1" s="100" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G1" s="117" t="s">
+        <v>301</v>
+      </c>
+      <c r="H1" s="99" t="s">
+        <v>302</v>
+      </c>
+      <c r="I1" s="104" t="s">
+        <v>303</v>
+      </c>
+      <c r="J1" s="100" t="s">
         <v>304</v>
       </c>
-      <c r="H1" s="99" t="s">
+      <c r="K1" s="117" t="s">
         <v>305</v>
       </c>
-      <c r="I1" s="104" t="s">
+      <c r="L1" s="99" t="s">
         <v>306</v>
       </c>
-      <c r="J1" s="100" t="s">
+      <c r="M1" s="104" t="s">
         <v>307</v>
       </c>
-      <c r="K1" s="117" t="s">
+      <c r="N1" s="100" t="s">
         <v>308</v>
       </c>
-      <c r="L1" s="99" t="s">
+      <c r="O1" s="117" t="s">
         <v>309</v>
       </c>
-      <c r="M1" s="104" t="s">
+      <c r="P1" s="100" t="s">
         <v>310</v>
-      </c>
-      <c r="N1" s="100" t="s">
-        <v>311</v>
-      </c>
-      <c r="O1" s="117" t="s">
-        <v>312</v>
-      </c>
-      <c r="P1" s="100" t="s">
-        <v>313</v>
       </c>
       <c r="Q1" s="99">
         <v>1</v>
@@ -2948,16 +2951,16 @@
         <v>159</v>
       </c>
       <c r="AJ1" s="98" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="AK1" s="98" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="AL1" s="98" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="AM1" s="98" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:40" s="39" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2974,45 +2977,45 @@
         <v>126</v>
       </c>
       <c r="E2" s="105" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F2" s="86" t="str">
-        <f>VLOOKUP(E2,Actions,2,FALSE)</f>
+        <f t="shared" ref="F2:F19" si="0">VLOOKUP(E2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G2" s="118" t="s">
+        <v>291</v>
+      </c>
+      <c r="H2" s="41" t="str">
+        <f t="shared" ref="H2:H19" si="1">VLOOKUP(G2,Actions,2,FALSE)</f>
+        <v>📷🔊🔊➜</v>
+      </c>
+      <c r="I2" s="105" t="s">
+        <v>175</v>
+      </c>
+      <c r="J2" s="86" t="str">
+        <f t="shared" ref="J2:J19" si="2">VLOOKUP(I2,Actions,2,FALSE)</f>
+        <v>🔍</v>
+      </c>
+      <c r="K2" s="118" t="s">
+        <v>248</v>
+      </c>
+      <c r="L2" s="41" t="str">
+        <f t="shared" ref="L2:L19" si="3">VLOOKUP(K2,Actions,2,FALSE)</f>
+        <v>👊🔊🔊➜</v>
+      </c>
+      <c r="M2" s="105" t="s">
+        <v>291</v>
+      </c>
+      <c r="N2" s="86" t="str">
+        <f t="shared" ref="N2:N19" si="4">VLOOKUP(M2,Actions,2,FALSE)</f>
+        <v>📷🔊🔊➜</v>
+      </c>
+      <c r="O2" s="118" t="s">
         <v>294</v>
       </c>
-      <c r="H2" s="41" t="str">
-        <f>VLOOKUP(G2,Actions,2,FALSE)</f>
-        <v>📷🔊🔊➜</v>
-      </c>
-      <c r="I2" s="105" t="s">
-        <v>176</v>
-      </c>
-      <c r="J2" s="86" t="str">
-        <f>VLOOKUP(I2,Actions,2,FALSE)</f>
-        <v>🔍</v>
-      </c>
-      <c r="K2" s="118" t="s">
-        <v>251</v>
-      </c>
-      <c r="L2" s="41" t="str">
-        <f>VLOOKUP(K2,Actions,2,FALSE)</f>
-        <v>👊🔊🔊➜</v>
-      </c>
-      <c r="M2" s="105" t="s">
-        <v>294</v>
-      </c>
-      <c r="N2" s="86" t="str">
-        <f>VLOOKUP(M2,Actions,2,FALSE)</f>
-        <v>📷🔊🔊➜</v>
-      </c>
-      <c r="O2" s="118" t="s">
-        <v>297</v>
-      </c>
       <c r="P2" s="86" t="str">
-        <f>VLOOKUP(O2,Actions,2,FALSE)</f>
+        <f t="shared" ref="P2:P19" si="5">VLOOKUP(O2,Actions,2,FALSE)</f>
         <v>💰🔊</v>
       </c>
       <c r="Q2" s="40" t="str">
@@ -3040,7 +3043,7 @@
         <v>Yoink%n💰🔊</v>
       </c>
       <c r="W2" s="43" t="str">
-        <f>Q2 &amp; "%n"
+        <f t="shared" ref="W2:W19" si="6">Q2 &amp; "%n"
 &amp; R2 &amp; "%n"
 &amp; S2 &amp; "%n"
 &amp; T2 &amp; "%n"
@@ -3052,14 +3055,14 @@
         <v>68</v>
       </c>
       <c r="Y2" s="41" t="str">
-        <f>IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" ref="Y2:Y19" si="7">IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
         <v>Recon%n💡💡🔊🔍%nRake%n🔓🔓🔊🔊➜%nUnplug%n📷🔊🔊➜%nSlink%n💡➜%nJab%n👊💡➜%nNab%n💰💰</v>
       </c>
       <c r="Z2" s="40" t="s">
         <v>139</v>
       </c>
       <c r="AA2" s="43" t="str">
-        <f>IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" ref="AA2:AA19" si="8">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
         <v>Run%n🔊🔊➜➜%nDisable%n📷🔊➜%nRake%n🔓🔓🔊🔊➜%nJab%n👊💡➜%nReveal%n🔍%nPunch%n👊🔊🔊➜</v>
       </c>
       <c r="AB2" s="40">
@@ -3067,44 +3070,44 @@
         <v>0</v>
       </c>
       <c r="AC2" s="40">
-        <f t="shared" ref="AC2:AI17" si="0">(LEN($W2)-LEN(SUBSTITUTE($W2,AC$1,"")))/LEN(AC$1)</f>
+        <f t="shared" ref="AC2:AI17" si="9">(LEN($W2)-LEN(SUBSTITUTE($W2,AC$1,"")))/LEN(AC$1)</f>
         <v>9</v>
       </c>
       <c r="AD2" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE2" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF2" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG2" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH2" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI2" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ2" s="39" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="AK2" s="39" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="AL2" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="AM2" s="39" t="s">
         <v>349</v>
-      </c>
-      <c r="AM2" s="39" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:40" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -3121,137 +3124,132 @@
         <v>127</v>
       </c>
       <c r="E3" s="107" t="s">
+        <v>241</v>
+      </c>
+      <c r="F3" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>🔊🔊➜➜</v>
+      </c>
+      <c r="G3" s="120" t="s">
+        <v>281</v>
+      </c>
+      <c r="H3" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v>🔓🔊</v>
+      </c>
+      <c r="I3" s="108" t="s">
+        <v>241</v>
+      </c>
+      <c r="J3" s="88" t="str">
+        <f t="shared" si="2"/>
+        <v>🔊🔊➜➜</v>
+      </c>
+      <c r="K3" s="126" t="s">
         <v>244</v>
       </c>
-      <c r="F3" s="88" t="str">
-        <f>VLOOKUP(E3,Actions,2,FALSE)</f>
-        <v>🔊🔊➜➜</v>
-      </c>
-      <c r="G3" s="120" t="s">
-        <v>284</v>
-      </c>
-      <c r="H3" s="36" t="str">
-        <f>VLOOKUP(G3,Actions,2,FALSE)</f>
-        <v>🔓🔊</v>
-      </c>
-      <c r="I3" s="108" t="s">
-        <v>244</v>
-      </c>
-      <c r="J3" s="88" t="str">
-        <f>VLOOKUP(I3,Actions,2,FALSE)</f>
-        <v>🔊🔊➜➜</v>
-      </c>
-      <c r="K3" s="126" t="s">
-        <v>247</v>
-      </c>
       <c r="L3" s="36" t="str">
-        <f>VLOOKUP(K3,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M3" s="108" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="N3" s="88" t="str">
-        <f>VLOOKUP(M3,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O3" s="120" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="P3" s="88" t="str">
-        <f>VLOOKUP(O3,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q3" s="38" t="str">
-        <f t="shared" ref="Q3:Q19" si="1">E3&amp;"%n"&amp;F3</f>
+        <f t="shared" ref="Q3:Q19" si="10">E3&amp;"%n"&amp;F3</f>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="R3" s="38" t="str">
-        <f t="shared" ref="R3:R19" si="2">G3&amp;"%n"&amp;H3</f>
+        <f t="shared" ref="R3:R19" si="11">G3&amp;"%n"&amp;H3</f>
         <v>Shim%n🔓🔊</v>
       </c>
       <c r="S3" s="38" t="str">
-        <f t="shared" ref="S3:S19" si="3">I3&amp;"%n"&amp;J3</f>
+        <f t="shared" ref="S3:S19" si="12">I3&amp;"%n"&amp;J3</f>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="T3" s="37" t="str">
-        <f t="shared" ref="T3:T19" si="4">K3&amp;"%n"&amp;L3</f>
+        <f t="shared" ref="T3:T19" si="13">K3&amp;"%n"&amp;L3</f>
         <v>Study%n💡💡</v>
       </c>
       <c r="U3" s="38" t="str">
-        <f t="shared" ref="U3:U19" si="5">M3&amp;"%n"&amp;N3</f>
+        <f t="shared" ref="U3:U19" si="14">M3&amp;"%n"&amp;N3</f>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="V3" s="38" t="str">
-        <f t="shared" ref="V3:V19" si="6">O3&amp;"%n"&amp;P3</f>
+        <f t="shared" ref="V3:V19" si="15">O3&amp;"%n"&amp;P3</f>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="W3" s="35" t="str">
-        <f>Q3 &amp; "%n"
-&amp; R3 &amp; "%n"
-&amp; S3 &amp; "%n"
-&amp; T3 &amp; "%n"
-&amp; U3 &amp; "%n"
-&amp; V3</f>
+        <f t="shared" si="6"/>
         <v>Run%n🔊🔊➜➜%nShim%n🔓🔊%nRun%n🔊🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="X3" s="38" t="s">
         <v>40</v>
       </c>
       <c r="Y3" s="36" t="str">
-        <f>IF(X3="(none)","",VLOOKUP(X3,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v>Redirect%n🔓👊📷🔊%nSlink%n💡➜%nRedirect%n🔓👊📷🔊%nSneak%n🔍➜➜%nJab%n👊💡➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="Z3" s="38" t="s">
         <v>36</v>
       </c>
       <c r="AA3" s="35" t="str">
-        <f>IF(Z3="(none)","",VLOOKUP(Z3,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v>Sneak%n🔍➜➜%nSleeper Hold%n👊➜%nSlink%n💡➜%nSleeper Hold%n👊➜%nSlink%n💡➜%nDefeat%n🔓📷🔊➜</v>
       </c>
       <c r="AB3" s="40">
-        <f t="shared" ref="AB3:AI19" si="7">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
+        <f t="shared" ref="AB3:AI19" si="16">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
         <v>5</v>
       </c>
       <c r="AC3" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AD3" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AE3" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF3" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG3" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH3" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI3" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="33" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="AK3" s="33" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="AL3" s="33" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AM3" s="39" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:40" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -3268,142 +3266,137 @@
         <v>125</v>
       </c>
       <c r="E4" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="90" t="str">
-        <f>VLOOKUP(E4,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>🔍</v>
       </c>
       <c r="G4" s="121" t="s">
+        <v>351</v>
+      </c>
+      <c r="H4" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>🔓👊🔊🔊</v>
+      </c>
+      <c r="I4" s="110" t="s">
+        <v>378</v>
+      </c>
+      <c r="J4" s="90" t="str">
+        <f t="shared" si="2"/>
+        <v>🔓📷🔊🔊</v>
+      </c>
+      <c r="K4" s="128" t="s">
         <v>354</v>
       </c>
-      <c r="H4" s="52" t="str">
-        <f>VLOOKUP(G4,Actions,2,FALSE)</f>
-        <v>🔓👊🔊🔊</v>
-      </c>
-      <c r="I4" s="110" t="s">
-        <v>358</v>
-      </c>
-      <c r="J4" s="90" t="str">
-        <f>VLOOKUP(I4,Actions,2,FALSE)</f>
-        <v>🔓📷🔊🔊</v>
-      </c>
-      <c r="K4" s="128" t="s">
-        <v>357</v>
-      </c>
       <c r="L4" s="52" t="str">
-        <f>VLOOKUP(K4,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>👊📷🔊🔊</v>
       </c>
       <c r="M4" s="110" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="N4" s="90" t="str">
-        <f>VLOOKUP(M4,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O4" s="121" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="P4" s="90" t="str">
-        <f>VLOOKUP(O4,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="Q4" s="51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Reveal%n🔍</v>
       </c>
       <c r="R4" s="53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Strongarm%n🔓👊🔊🔊</v>
       </c>
       <c r="S4" s="53" t="str">
-        <f t="shared" si="3"/>
-        <v>Shortcircuit%n🔓📷🔊🔊</v>
+        <f t="shared" si="12"/>
+        <v>Short%n🔓📷🔊🔊</v>
       </c>
       <c r="T4" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Zap%n👊📷🔊🔊</v>
       </c>
       <c r="U4" s="51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Yoink%n💰🔊</v>
       </c>
       <c r="V4" s="51" t="str">
+        <f t="shared" si="15"/>
+        <v>Run%n🔊🔊➜➜</v>
+      </c>
+      <c r="W4" s="54" t="str">
         <f t="shared" si="6"/>
-        <v>Run%n🔊🔊➜➜</v>
-      </c>
-      <c r="W4" s="54" t="str">
-        <f>Q4 &amp; "%n"
-&amp; R4 &amp; "%n"
-&amp; S4 &amp; "%n"
-&amp; T4 &amp; "%n"
-&amp; U4 &amp; "%n"
-&amp; V4</f>
-        <v>Reveal%n🔍%nStrongarm%n🔓👊🔊🔊%nShortcircuit%n🔓📷🔊🔊%nZap%n👊📷🔊🔊%nYoink%n💰🔊%nRun%n🔊🔊➜➜</v>
+        <v>Reveal%n🔍%nStrongarm%n🔓👊🔊🔊%nShort%n🔓📷🔊🔊%nZap%n👊📷🔊🔊%nYoink%n💰🔊%nRun%n🔊🔊➜➜</v>
       </c>
       <c r="X4" s="51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Y4" s="52" t="str">
-        <f>IF(X4="(none)","",VLOOKUP(X4,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v>Study%n💡💡%nDiscover%n🔍🔍%nJab%n👊💡➜%nExamine%n💡💡💡🔊%nDefeat%n🔓📷🔊➜%nSneak%n🔍➜➜</v>
       </c>
       <c r="Z4" s="51" t="s">
         <v>131</v>
       </c>
       <c r="AA4" s="54" t="str">
-        <f>IF(Z4="(none)","",VLOOKUP(Z4,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v>Rake%n🔓🔓🔊🔊➜%nStudy%n💡💡%nShim%n🔓🔊%nSprint%n🔊🔊➜➜➜%nRun%n🔊🔊➜➜%nShim%n🔓🔊</v>
       </c>
       <c r="AB4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC4" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="AD4" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AE4" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF4" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG4" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH4" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI4" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ4" s="55" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="AK4" s="55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AL4" s="55" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="AM4" s="39" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:40" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B5" s="63">
         <v>2</v>
@@ -3412,140 +3405,135 @@
         <v>1</v>
       </c>
       <c r="D5" s="64" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E5" s="111" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F5" s="92" t="str">
-        <f>VLOOKUP(E5,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>👊🔊</v>
       </c>
       <c r="G5" s="122" t="s">
+        <v>241</v>
+      </c>
+      <c r="H5" s="64" t="str">
+        <f t="shared" si="1"/>
+        <v>🔊🔊➜➜</v>
+      </c>
+      <c r="I5" s="112" t="s">
+        <v>252</v>
+      </c>
+      <c r="J5" s="92" t="str">
+        <f t="shared" si="2"/>
+        <v>👊👊🔊</v>
+      </c>
+      <c r="K5" s="130" t="s">
+        <v>241</v>
+      </c>
+      <c r="L5" s="64" t="str">
+        <f t="shared" si="3"/>
+        <v>🔊🔊➜➜</v>
+      </c>
+      <c r="M5" s="112" t="s">
+        <v>361</v>
+      </c>
+      <c r="N5" s="92" t="str">
+        <f t="shared" si="4"/>
+        <v>👊🔊</v>
+      </c>
+      <c r="O5" s="122" t="s">
         <v>244</v>
       </c>
-      <c r="H5" s="64" t="str">
-        <f>VLOOKUP(G5,Actions,2,FALSE)</f>
-        <v>🔊🔊➜➜</v>
-      </c>
-      <c r="I5" s="112" t="s">
-        <v>255</v>
-      </c>
-      <c r="J5" s="92" t="str">
-        <f>VLOOKUP(I5,Actions,2,FALSE)</f>
-        <v>👊👊🔊</v>
-      </c>
-      <c r="K5" s="130" t="s">
-        <v>244</v>
-      </c>
-      <c r="L5" s="64" t="str">
-        <f>VLOOKUP(K5,Actions,2,FALSE)</f>
-        <v>🔊🔊➜➜</v>
-      </c>
-      <c r="M5" s="112" t="s">
-        <v>365</v>
-      </c>
-      <c r="N5" s="92" t="str">
-        <f>VLOOKUP(M5,Actions,2,FALSE)</f>
-        <v>👊🔊</v>
-      </c>
-      <c r="O5" s="122" t="s">
-        <v>247</v>
-      </c>
       <c r="P5" s="92" t="str">
-        <f>VLOOKUP(O5,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>💡💡</v>
       </c>
       <c r="Q5" s="63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Tackle%n👊🔊</v>
       </c>
       <c r="R5" s="63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="S5" s="63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Bash%n👊👊🔊</v>
       </c>
       <c r="T5" s="63" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="U5" s="63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Tackle%n👊🔊</v>
       </c>
       <c r="V5" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="W5" s="65" t="str">
         <f t="shared" si="6"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="W5" s="65" t="str">
-        <f>Q5 &amp; "%n"
-&amp; R5 &amp; "%n"
-&amp; S5 &amp; "%n"
-&amp; T5 &amp; "%n"
-&amp; U5 &amp; "%n"
-&amp; V5</f>
         <v>Tackle%n👊🔊%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nRun%n🔊🔊➜➜%nTackle%n👊🔊%nStudy%n💡💡</v>
       </c>
       <c r="X5" s="63" t="s">
         <v>160</v>
       </c>
       <c r="Y5" s="64" t="str">
-        <f>IF(X5="(none)","",VLOOKUP(X5,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v>Nab%n💰💰%nRake%n🔓🔓🔊🔊➜%nKick%n👊🔊➜➜%nStudy%n💡💡%nUnplug%n📷🔊🔊➜%nKick%n👊🔊➜➜</v>
       </c>
       <c r="Z5" s="63" t="s">
         <v>115</v>
       </c>
       <c r="AA5" s="65" t="str">
-        <f>IF(Z5="(none)","",VLOOKUP(Z5,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v>Defeat%n🔓📷🔊➜%nSprint%n🔊🔊➜➜➜%nSlink%n💡➜%nRampage%n👊👊🔊🔊➜➜%nDetonate%n🔓👊📷🔊🔊⚠%nPunch%n👊🔊🔊➜</v>
       </c>
       <c r="AB5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC5" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AD5" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE5" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF5" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AG5" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH5" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI5" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="66" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="AK5" s="66" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="AL5" s="66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AM5" s="66" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="AN5" s="66"/>
     </row>
@@ -3563,137 +3551,132 @@
         <v>131</v>
       </c>
       <c r="E6" s="113" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F6" s="94" t="str">
-        <f>VLOOKUP(E6,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="G6" s="123" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H6" s="74" t="str">
-        <f>VLOOKUP(G6,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I6" s="114" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J6" s="94" t="str">
-        <f>VLOOKUP(I6,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>🔓🔊</v>
       </c>
       <c r="K6" s="131" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="L6" s="74" t="str">
-        <f>VLOOKUP(K6,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M6" s="114" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N6" s="94" t="str">
-        <f>VLOOKUP(M6,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="O6" s="123" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="P6" s="94" t="str">
-        <f>VLOOKUP(O6,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>🔓🔊</v>
       </c>
       <c r="Q6" s="73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Rake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="R6" s="73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="S6" s="75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Shim%n🔓🔊</v>
       </c>
       <c r="T6" s="73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="U6" s="75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="V6" s="75" t="str">
+        <f t="shared" si="15"/>
+        <v>Shim%n🔓🔊</v>
+      </c>
+      <c r="W6" s="76" t="str">
         <f t="shared" si="6"/>
-        <v>Shim%n🔓🔊</v>
-      </c>
-      <c r="W6" s="76" t="str">
-        <f>Q6 &amp; "%n"
-&amp; R6 &amp; "%n"
-&amp; S6 &amp; "%n"
-&amp; T6 &amp; "%n"
-&amp; U6 &amp; "%n"
-&amp; V6</f>
         <v>Rake%n🔓🔓🔊🔊➜%nStudy%n💡💡%nShim%n🔓🔊%nSprint%n🔊🔊➜➜➜%nRun%n🔊🔊➜➜%nShim%n🔓🔊</v>
       </c>
       <c r="X6" s="75" t="s">
         <v>34</v>
       </c>
       <c r="Y6" s="74" t="str">
-        <f>IF(X6="(none)","",VLOOKUP(X6,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v>Rake%n🔓🔓🔊🔊➜%nRun%n🔊🔊➜➜%nYoink%n💰🔊%nSpin Kick%n👊👊👊🔊🔊%nKick%n👊🔊➜➜%nJab%n👊💡➜</v>
       </c>
       <c r="Z6" s="75" t="s">
         <v>158</v>
       </c>
       <c r="AA6" s="76" t="str">
-        <f>IF(Z6="(none)","",VLOOKUP(Z6,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v>Detonate%n🔓👊📷🔊🔊⚠%nNab%n💰💰%nRun%n🔊🔊➜➜%nSneak%n🔍➜➜%nRake%n🔓🔓🔊🔊➜%nRun%n🔊🔊➜➜</v>
       </c>
       <c r="AB6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC6" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AD6" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE6" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF6" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG6" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH6" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI6" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="77" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="AK6" s="77" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="AL6" s="77" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AM6" s="77" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="AN6" s="77"/>
     </row>
@@ -3711,137 +3694,132 @@
         <v>59</v>
       </c>
       <c r="E7" s="136" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F7" s="137" t="str">
-        <f>VLOOKUP(E7,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>📷📷🔊🔊➜</v>
       </c>
       <c r="G7" s="138" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H7" s="135" t="str">
-        <f>VLOOKUP(G7,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I7" s="139" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J7" s="137" t="str">
-        <f>VLOOKUP(I7,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="K7" s="140" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L7" s="135" t="str">
-        <f>VLOOKUP(K7,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>🔍</v>
       </c>
       <c r="M7" s="139" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="N7" s="137" t="str">
-        <f>VLOOKUP(M7,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="O7" s="138" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="P7" s="137" t="str">
-        <f>VLOOKUP(O7,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="Q7" s="134" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Shatter%n📷📷🔊🔊➜</v>
       </c>
       <c r="R7" s="134" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="S7" s="134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Unplug%n📷🔊🔊➜</v>
       </c>
       <c r="T7" s="134" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Reveal%n🔍</v>
       </c>
       <c r="U7" s="141" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="V7" s="141" t="str">
+        <f t="shared" si="15"/>
+        <v>Unplug%n📷🔊🔊➜</v>
+      </c>
+      <c r="W7" s="142" t="str">
         <f t="shared" si="6"/>
-        <v>Unplug%n📷🔊🔊➜</v>
-      </c>
-      <c r="W7" s="142" t="str">
-        <f>Q7 &amp; "%n"
-&amp; R7 &amp; "%n"
-&amp; S7 &amp; "%n"
-&amp; T7 &amp; "%n"
-&amp; U7 &amp; "%n"
-&amp; V7</f>
         <v>Shatter%n📷📷🔊🔊➜%nSprint%n🔊🔊➜➜➜%nUnplug%n📷🔊🔊➜%nReveal%n🔍%nExamine%n💡💡💡🔊%nUnplug%n📷🔊🔊➜</v>
       </c>
       <c r="X7" s="141" t="s">
         <v>63</v>
       </c>
       <c r="Y7" s="135" t="str">
-        <f>IF(X7="(none)","",VLOOKUP(X7,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v>Loop%n📷🔍%nRecon%n💡💡🔊🔍%nRun%n🔊🔊➜➜%nPunch%n👊🔊🔊➜%nRun%n🔊🔊➜➜%nRake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="Z7" s="141" t="s">
         <v>138</v>
       </c>
       <c r="AA7" s="142" t="str">
-        <f>IF(Z7="(none)","",VLOOKUP(Z7,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v>Examine%n💡💡💡🔊%nRun%n🔊🔊➜➜%nLoop%n📷🔍%nRedirect%n🔓👊📷🔊%nRecon%n💡💡🔊🔍%nPick%n🔓</v>
       </c>
       <c r="AB7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="AC7" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="AD7" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE7" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AF7" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG7" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH7" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI7" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="143" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="AK7" s="143" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AL7" s="143" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="AM7" s="143" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="AN7" s="143"/>
     </row>
@@ -3859,128 +3837,123 @@
         <v>126</v>
       </c>
       <c r="E8" s="106" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F8" s="87" t="str">
-        <f>VLOOKUP(E8,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="G8" s="119" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H8" s="43" t="str">
-        <f>VLOOKUP(G8,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="I8" s="106" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J8" s="87" t="str">
-        <f>VLOOKUP(I8,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="K8" s="119" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="L8" s="43" t="str">
-        <f>VLOOKUP(K8,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>💡➜</v>
       </c>
       <c r="M8" s="106" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="N8" s="87" t="str">
-        <f>VLOOKUP(M8,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>👊💡➜</v>
       </c>
       <c r="O8" s="119" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="P8" s="87" t="str">
-        <f>VLOOKUP(O8,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>💰💰</v>
       </c>
       <c r="Q8" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Recon%n💡💡🔊🔍</v>
       </c>
       <c r="R8" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Rake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="S8" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Unplug%n📷🔊🔊➜</v>
       </c>
       <c r="T8" s="42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Slink%n💡➜</v>
       </c>
       <c r="U8" s="42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Jab%n👊💡➜</v>
       </c>
       <c r="V8" s="42" t="str">
+        <f t="shared" si="15"/>
+        <v>Nab%n💰💰</v>
+      </c>
+      <c r="W8" s="44" t="str">
         <f t="shared" si="6"/>
-        <v>Nab%n💰💰</v>
-      </c>
-      <c r="W8" s="44" t="str">
-        <f>Q8 &amp; "%n"
-&amp; R8 &amp; "%n"
-&amp; S8 &amp; "%n"
-&amp; T8 &amp; "%n"
-&amp; U8 &amp; "%n"
-&amp; V8</f>
         <v>Recon%n💡💡🔊🔍%nRake%n🔓🔓🔊🔊➜%nUnplug%n📷🔊🔊➜%nSlink%n💡➜%nJab%n👊💡➜%nNab%n💰💰</v>
       </c>
       <c r="X8" s="42" t="s">
         <v>140</v>
       </c>
       <c r="Y8" s="45" t="str">
-        <f>IF(X8="(none)","",VLOOKUP(X8,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z8" s="42" t="s">
         <v>140</v>
       </c>
       <c r="AA8" s="43" t="str">
-        <f>IF(Z8="(none)","",VLOOKUP(Z8,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="AC8" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AD8" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE8" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF8" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AG8" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH8" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI8" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AN8" s="55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:40" s="59" customFormat="1" x14ac:dyDescent="0.25">
@@ -3997,128 +3970,123 @@
         <v>126</v>
       </c>
       <c r="E9" s="106" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F9" s="87" t="str">
-        <f>VLOOKUP(E9,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G9" s="119" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H9" s="43" t="str">
-        <f>VLOOKUP(G9,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>📷🔊➜</v>
       </c>
       <c r="I9" s="106" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J9" s="87" t="str">
-        <f>VLOOKUP(I9,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="K9" s="119" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="L9" s="43" t="str">
-        <f>VLOOKUP(K9,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>👊💡➜</v>
       </c>
       <c r="M9" s="106" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N9" s="87" t="str">
-        <f>VLOOKUP(M9,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>🔍</v>
       </c>
       <c r="O9" s="119" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="P9" s="87" t="str">
-        <f>VLOOKUP(O9,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="Q9" s="48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="R9" s="47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="S9" s="47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Rake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="T9" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Jab%n👊💡➜</v>
       </c>
       <c r="U9" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Reveal%n🔍</v>
       </c>
       <c r="V9" s="48" t="str">
+        <f t="shared" si="15"/>
+        <v>Punch%n👊🔊🔊➜</v>
+      </c>
+      <c r="W9" s="44" t="str">
         <f t="shared" si="6"/>
-        <v>Punch%n👊🔊🔊➜</v>
-      </c>
-      <c r="W9" s="44" t="str">
-        <f>Q9 &amp; "%n"
-&amp; R9 &amp; "%n"
-&amp; S9 &amp; "%n"
-&amp; T9 &amp; "%n"
-&amp; U9 &amp; "%n"
-&amp; V9</f>
         <v>Run%n🔊🔊➜➜%nDisable%n📷🔊➜%nRake%n🔓🔓🔊🔊➜%nJab%n👊💡➜%nReveal%n🔍%nPunch%n👊🔊🔊➜</v>
       </c>
       <c r="X9" s="47" t="s">
         <v>140</v>
       </c>
       <c r="Y9" s="44" t="str">
-        <f>IF(X9="(none)","",VLOOKUP(X9,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z9" s="47" t="s">
         <v>140</v>
       </c>
       <c r="AA9" s="43" t="str">
-        <f>IF(Z9="(none)","",VLOOKUP(Z9,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AC9" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AD9" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE9" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF9" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG9" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH9" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI9" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AN9" s="59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:40" s="56" customFormat="1" x14ac:dyDescent="0.25">
@@ -4135,128 +4103,123 @@
         <v>127</v>
       </c>
       <c r="E10" s="108" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>🔓👊📷🔊</v>
+      </c>
+      <c r="G10" s="120" t="s">
+        <v>283</v>
+      </c>
+      <c r="H10" s="34" t="str">
+        <f t="shared" si="1"/>
+        <v>💡➜</v>
+      </c>
+      <c r="I10" s="108" t="s">
+        <v>242</v>
+      </c>
+      <c r="J10" s="89" t="str">
+        <f t="shared" si="2"/>
+        <v>🔓👊📷🔊</v>
+      </c>
+      <c r="K10" s="120" t="s">
+        <v>243</v>
+      </c>
+      <c r="L10" s="34" t="str">
+        <f t="shared" si="3"/>
+        <v>🔍➜➜</v>
+      </c>
+      <c r="M10" s="108" t="s">
+        <v>265</v>
+      </c>
+      <c r="N10" s="89" t="str">
+        <f t="shared" si="4"/>
+        <v>👊💡➜</v>
+      </c>
+      <c r="O10" s="120" t="s">
         <v>245</v>
       </c>
-      <c r="F10" s="89" t="str">
-        <f>VLOOKUP(E10,Actions,2,FALSE)</f>
-        <v>🔓👊📷🔊</v>
-      </c>
-      <c r="G10" s="120" t="s">
-        <v>286</v>
-      </c>
-      <c r="H10" s="34" t="str">
-        <f>VLOOKUP(G10,Actions,2,FALSE)</f>
-        <v>💡➜</v>
-      </c>
-      <c r="I10" s="108" t="s">
-        <v>245</v>
-      </c>
-      <c r="J10" s="89" t="str">
-        <f>VLOOKUP(I10,Actions,2,FALSE)</f>
-        <v>🔓👊📷🔊</v>
-      </c>
-      <c r="K10" s="120" t="s">
-        <v>246</v>
-      </c>
-      <c r="L10" s="34" t="str">
-        <f>VLOOKUP(K10,Actions,2,FALSE)</f>
-        <v>🔍➜➜</v>
-      </c>
-      <c r="M10" s="108" t="s">
-        <v>268</v>
-      </c>
-      <c r="N10" s="89" t="str">
-        <f>VLOOKUP(M10,Actions,2,FALSE)</f>
-        <v>👊💡➜</v>
-      </c>
-      <c r="O10" s="120" t="s">
-        <v>248</v>
-      </c>
       <c r="P10" s="89" t="str">
-        <f>VLOOKUP(O10,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q10" s="37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Redirect%n🔓👊📷🔊</v>
       </c>
       <c r="R10" s="37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Slink%n💡➜</v>
       </c>
       <c r="S10" s="37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Redirect%n🔓👊📷🔊</v>
       </c>
       <c r="T10" s="38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Sneak%n🔍➜➜</v>
       </c>
       <c r="U10" s="38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Jab%n👊💡➜</v>
       </c>
       <c r="V10" s="38" t="str">
+        <f t="shared" si="15"/>
+        <v>Examine%n💡💡💡🔊</v>
+      </c>
+      <c r="W10" s="35" t="str">
         <f t="shared" si="6"/>
-        <v>Examine%n💡💡💡🔊</v>
-      </c>
-      <c r="W10" s="35" t="str">
-        <f>Q10 &amp; "%n"
-&amp; R10 &amp; "%n"
-&amp; S10 &amp; "%n"
-&amp; T10 &amp; "%n"
-&amp; U10 &amp; "%n"
-&amp; V10</f>
         <v>Redirect%n🔓👊📷🔊%nSlink%n💡➜%nRedirect%n🔓👊📷🔊%nSneak%n🔍➜➜%nJab%n👊💡➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="X10" s="37" t="s">
         <v>140</v>
       </c>
       <c r="Y10" s="35" t="str">
-        <f>IF(X10="(none)","",VLOOKUP(X10,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z10" s="37" t="s">
         <v>140</v>
       </c>
       <c r="AA10" s="35" t="str">
-        <f>IF(Z10="(none)","",VLOOKUP(Z10,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AC10" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AD10" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE10" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF10" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AG10" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH10" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI10" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AN10" s="56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:40" s="66" customFormat="1" x14ac:dyDescent="0.25">
@@ -4273,133 +4236,128 @@
         <v>127</v>
       </c>
       <c r="E11" s="108" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F11" s="89" t="str">
-        <f>VLOOKUP(E11,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>🔍➜➜</v>
       </c>
       <c r="G11" s="120" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H11" s="35" t="str">
-        <f>VLOOKUP(G11,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>👊➜</v>
       </c>
       <c r="I11" s="108" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J11" s="89" t="str">
-        <f>VLOOKUP(I11,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>💡➜</v>
       </c>
       <c r="K11" s="127" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="L11" s="35" t="str">
-        <f>VLOOKUP(K11,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>👊➜</v>
       </c>
       <c r="M11" s="108" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="N11" s="89" t="str">
-        <f>VLOOKUP(M11,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>💡➜</v>
       </c>
       <c r="O11" s="120" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="P11" s="89" t="str">
-        <f>VLOOKUP(O11,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>🔓📷🔊➜</v>
       </c>
       <c r="Q11" s="38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Sneak%n🔍➜➜</v>
       </c>
       <c r="R11" s="38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Sleeper Hold%n👊➜</v>
       </c>
       <c r="S11" s="37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Slink%n💡➜</v>
       </c>
       <c r="T11" s="38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Sleeper Hold%n👊➜</v>
       </c>
       <c r="U11" s="38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Slink%n💡➜</v>
       </c>
       <c r="V11" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v>Defeat%n🔓📷🔊➜</v>
+      </c>
+      <c r="W11" s="35" t="str">
         <f t="shared" si="6"/>
-        <v>Defeat%n🔓📷🔊➜</v>
-      </c>
-      <c r="W11" s="35" t="str">
-        <f>Q11 &amp; "%n"
-&amp; R11 &amp; "%n"
-&amp; S11 &amp; "%n"
-&amp; T11 &amp; "%n"
-&amp; U11 &amp; "%n"
-&amp; V11</f>
         <v>Sneak%n🔍➜➜%nSleeper Hold%n👊➜%nSlink%n💡➜%nSleeper Hold%n👊➜%nSlink%n💡➜%nDefeat%n🔓📷🔊➜</v>
       </c>
       <c r="X11" s="37" t="s">
         <v>140</v>
       </c>
       <c r="Y11" s="35" t="str">
-        <f>IF(X11="(none)","",VLOOKUP(X11,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z11" s="37" t="s">
         <v>140</v>
       </c>
       <c r="AA11" s="35" t="str">
-        <f>IF(Z11="(none)","",VLOOKUP(Z11,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC11" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AD11" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AE11" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF11" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG11" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH11" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI11" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AN11" s="66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:40" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B12" s="53">
         <v>2</v>
@@ -4411,133 +4369,128 @@
         <v>125</v>
       </c>
       <c r="E12" s="110" t="s">
+        <v>244</v>
+      </c>
+      <c r="F12" s="91" t="str">
+        <f t="shared" si="0"/>
+        <v>💡💡</v>
+      </c>
+      <c r="G12" s="121" t="s">
+        <v>261</v>
+      </c>
+      <c r="H12" s="54" t="str">
+        <f t="shared" si="1"/>
+        <v>🔍🔍</v>
+      </c>
+      <c r="I12" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="J12" s="91" t="str">
+        <f t="shared" si="2"/>
+        <v>👊💡➜</v>
+      </c>
+      <c r="K12" s="121" t="s">
+        <v>245</v>
+      </c>
+      <c r="L12" s="54" t="str">
+        <f t="shared" si="3"/>
+        <v>💡💡💡🔊</v>
+      </c>
+      <c r="M12" s="110" t="s">
         <v>247</v>
       </c>
-      <c r="F12" s="91" t="str">
-        <f>VLOOKUP(E12,Actions,2,FALSE)</f>
-        <v>💡💡</v>
-      </c>
-      <c r="G12" s="121" t="s">
-        <v>264</v>
-      </c>
-      <c r="H12" s="54" t="str">
-        <f>VLOOKUP(G12,Actions,2,FALSE)</f>
-        <v>🔍🔍</v>
-      </c>
-      <c r="I12" s="110" t="s">
-        <v>268</v>
-      </c>
-      <c r="J12" s="91" t="str">
-        <f>VLOOKUP(I12,Actions,2,FALSE)</f>
-        <v>👊💡➜</v>
-      </c>
-      <c r="K12" s="121" t="s">
-        <v>248</v>
-      </c>
-      <c r="L12" s="54" t="str">
-        <f>VLOOKUP(K12,Actions,2,FALSE)</f>
-        <v>💡💡💡🔊</v>
-      </c>
-      <c r="M12" s="110" t="s">
-        <v>250</v>
-      </c>
       <c r="N12" s="91" t="str">
-        <f>VLOOKUP(M12,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>🔓📷🔊➜</v>
       </c>
       <c r="O12" s="121" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="P12" s="91" t="str">
-        <f>VLOOKUP(O12,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>🔍➜➜</v>
       </c>
       <c r="Q12" s="53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="R12" s="53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Discover%n🔍🔍</v>
       </c>
       <c r="S12" s="51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Jab%n👊💡➜</v>
       </c>
       <c r="T12" s="53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="U12" s="51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Defeat%n🔓📷🔊➜</v>
       </c>
       <c r="V12" s="53" t="str">
+        <f t="shared" si="15"/>
+        <v>Sneak%n🔍➜➜</v>
+      </c>
+      <c r="W12" s="57" t="str">
         <f t="shared" si="6"/>
-        <v>Sneak%n🔍➜➜</v>
-      </c>
-      <c r="W12" s="57" t="str">
-        <f>Q12 &amp; "%n"
-&amp; R12 &amp; "%n"
-&amp; S12 &amp; "%n"
-&amp; T12 &amp; "%n"
-&amp; U12 &amp; "%n"
-&amp; V12</f>
         <v>Study%n💡💡%nDiscover%n🔍🔍%nJab%n👊💡➜%nExamine%n💡💡💡🔊%nDefeat%n🔓📷🔊➜%nSneak%n🔍➜➜</v>
       </c>
       <c r="X12" s="53" t="s">
         <v>140</v>
       </c>
       <c r="Y12" s="58" t="str">
-        <f>IF(X12="(none)","",VLOOKUP(X12,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z12" s="53" t="s">
         <v>140</v>
       </c>
       <c r="AA12" s="57" t="str">
-        <f>IF(Z12="(none)","",VLOOKUP(Z12,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="AC12" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AD12" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE12" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF12" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AG12" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH12" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AI12" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AN12" s="66" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:40" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B13" s="60">
         <v>2</v>
@@ -4549,128 +4502,123 @@
         <v>125</v>
       </c>
       <c r="E13" s="110" t="s">
+        <v>245</v>
+      </c>
+      <c r="F13" s="91" t="str">
+        <f t="shared" si="0"/>
+        <v>💡💡💡🔊</v>
+      </c>
+      <c r="G13" s="121" t="s">
+        <v>247</v>
+      </c>
+      <c r="H13" s="57" t="str">
+        <f t="shared" si="1"/>
+        <v>🔓📷🔊➜</v>
+      </c>
+      <c r="I13" s="110" t="s">
         <v>248</v>
       </c>
-      <c r="F13" s="91" t="str">
-        <f>VLOOKUP(E13,Actions,2,FALSE)</f>
-        <v>💡💡💡🔊</v>
-      </c>
-      <c r="G13" s="121" t="s">
-        <v>250</v>
-      </c>
-      <c r="H13" s="57" t="str">
-        <f>VLOOKUP(G13,Actions,2,FALSE)</f>
-        <v>🔓📷🔊➜</v>
-      </c>
-      <c r="I13" s="110" t="s">
+      <c r="J13" s="91" t="str">
+        <f t="shared" si="2"/>
+        <v>👊🔊🔊➜</v>
+      </c>
+      <c r="K13" s="129" t="s">
+        <v>249</v>
+      </c>
+      <c r="L13" s="57" t="str">
+        <f t="shared" si="3"/>
+        <v>🔓🔓🔊🔊➜</v>
+      </c>
+      <c r="M13" s="110" t="s">
+        <v>248</v>
+      </c>
+      <c r="N13" s="91" t="str">
+        <f t="shared" si="4"/>
+        <v>👊🔊🔊➜</v>
+      </c>
+      <c r="O13" s="121" t="s">
         <v>251</v>
       </c>
-      <c r="J13" s="91" t="str">
-        <f>VLOOKUP(I13,Actions,2,FALSE)</f>
-        <v>👊🔊🔊➜</v>
-      </c>
-      <c r="K13" s="129" t="s">
-        <v>252</v>
-      </c>
-      <c r="L13" s="57" t="str">
-        <f>VLOOKUP(K13,Actions,2,FALSE)</f>
-        <v>🔓🔓🔊🔊➜</v>
-      </c>
-      <c r="M13" s="110" t="s">
-        <v>251</v>
-      </c>
-      <c r="N13" s="91" t="str">
-        <f>VLOOKUP(M13,Actions,2,FALSE)</f>
-        <v>👊🔊🔊➜</v>
-      </c>
-      <c r="O13" s="121" t="s">
-        <v>254</v>
-      </c>
       <c r="P13" s="91" t="str">
-        <f>VLOOKUP(O13,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>📷🔍</v>
       </c>
       <c r="Q13" s="61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="R13" s="60" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Defeat%n🔓📷🔊➜</v>
       </c>
       <c r="S13" s="60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Punch%n👊🔊🔊➜</v>
       </c>
       <c r="T13" s="60" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Rake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="U13" s="61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Punch%n👊🔊🔊➜</v>
       </c>
       <c r="V13" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>Loop%n📷🔍</v>
+      </c>
+      <c r="W13" s="57" t="str">
         <f t="shared" si="6"/>
-        <v>Loop%n📷🔍</v>
-      </c>
-      <c r="W13" s="57" t="str">
-        <f>Q13 &amp; "%n"
-&amp; R13 &amp; "%n"
-&amp; S13 &amp; "%n"
-&amp; T13 &amp; "%n"
-&amp; U13 &amp; "%n"
-&amp; V13</f>
         <v>Examine%n💡💡💡🔊%nDefeat%n🔓📷🔊➜%nPunch%n👊🔊🔊➜%nRake%n🔓🔓🔊🔊➜%nPunch%n👊🔊🔊➜%nLoop%n📷🔍</v>
       </c>
       <c r="X13" s="60" t="s">
         <v>140</v>
       </c>
       <c r="Y13" s="58" t="str">
-        <f>IF(X13="(none)","",VLOOKUP(X13,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z13" s="60" t="s">
         <v>140</v>
       </c>
       <c r="AA13" s="57" t="str">
-        <f>IF(Z13="(none)","",VLOOKUP(Z13,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="AC13" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AD13" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE13" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF13" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG13" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AH13" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI13" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AN13" s="66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:40" s="77" customFormat="1" x14ac:dyDescent="0.25">
@@ -4684,131 +4632,126 @@
         <v>2</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E14" s="112" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="93" t="str">
+        <f t="shared" si="0"/>
+        <v>💰💰</v>
+      </c>
+      <c r="G14" s="122" t="s">
         <v>249</v>
       </c>
-      <c r="F14" s="93" t="str">
-        <f>VLOOKUP(E14,Actions,2,FALSE)</f>
-        <v>💰💰</v>
-      </c>
-      <c r="G14" s="122" t="s">
-        <v>252</v>
-      </c>
       <c r="H14" s="65" t="str">
-        <f>VLOOKUP(G14,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="I14" s="112" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J14" s="93" t="str">
-        <f>VLOOKUP(I14,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>👊🔊➜➜</v>
       </c>
       <c r="K14" s="122" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="L14" s="65" t="str">
-        <f>VLOOKUP(K14,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M14" s="112" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="N14" s="93" t="str">
-        <f>VLOOKUP(M14,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O14" s="122" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="P14" s="93" t="str">
-        <f>VLOOKUP(O14,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>👊🔊➜➜</v>
       </c>
       <c r="Q14" s="68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Nab%n💰💰</v>
       </c>
       <c r="R14" s="69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Rake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="S14" s="69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Kick%n👊🔊➜➜</v>
       </c>
       <c r="T14" s="63" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="U14" s="68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Unplug%n📷🔊🔊➜</v>
       </c>
       <c r="V14" s="69" t="str">
+        <f t="shared" si="15"/>
+        <v>Kick%n👊🔊➜➜</v>
+      </c>
+      <c r="W14" s="70" t="str">
         <f t="shared" si="6"/>
-        <v>Kick%n👊🔊➜➜</v>
-      </c>
-      <c r="W14" s="70" t="str">
-        <f>Q14 &amp; "%n"
-&amp; R14 &amp; "%n"
-&amp; S14 &amp; "%n"
-&amp; T14 &amp; "%n"
-&amp; U14 &amp; "%n"
-&amp; V14</f>
         <v>Nab%n💰💰%nRake%n🔓🔓🔊🔊➜%nKick%n👊🔊➜➜%nStudy%n💡💡%nUnplug%n📷🔊🔊➜%nKick%n👊🔊➜➜</v>
       </c>
       <c r="X14" s="68" t="s">
         <v>140</v>
       </c>
       <c r="Y14" s="65" t="str">
-        <f>IF(X14="(none)","",VLOOKUP(X14,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z14" s="68" t="s">
         <v>140</v>
       </c>
       <c r="AA14" s="65" t="str">
-        <f>IF(Z14="(none)","",VLOOKUP(Z14,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC14" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AD14" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE14" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF14" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG14" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH14" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI14" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AN14" s="77" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:40" s="77" customFormat="1" x14ac:dyDescent="0.25">
@@ -4822,131 +4765,126 @@
         <v>2</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E15" s="112" t="s">
+        <v>247</v>
+      </c>
+      <c r="F15" s="93" t="str">
+        <f t="shared" si="0"/>
+        <v>🔓📷🔊➜</v>
+      </c>
+      <c r="G15" s="122" t="s">
+        <v>287</v>
+      </c>
+      <c r="H15" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>🔊🔊➜➜➜</v>
+      </c>
+      <c r="I15" s="112" t="s">
+        <v>283</v>
+      </c>
+      <c r="J15" s="93" t="str">
+        <f t="shared" si="2"/>
+        <v>💡➜</v>
+      </c>
+      <c r="K15" s="122" t="s">
+        <v>276</v>
+      </c>
+      <c r="L15" s="65" t="str">
+        <f t="shared" si="3"/>
+        <v>👊👊🔊🔊➜➜</v>
+      </c>
+      <c r="M15" s="112" t="s">
         <v>250</v>
       </c>
-      <c r="F15" s="93" t="str">
-        <f>VLOOKUP(E15,Actions,2,FALSE)</f>
-        <v>🔓📷🔊➜</v>
-      </c>
-      <c r="G15" s="122" t="s">
-        <v>290</v>
-      </c>
-      <c r="H15" s="65" t="str">
-        <f>VLOOKUP(G15,Actions,2,FALSE)</f>
-        <v>🔊🔊➜➜➜</v>
-      </c>
-      <c r="I15" s="112" t="s">
-        <v>286</v>
-      </c>
-      <c r="J15" s="93" t="str">
-        <f>VLOOKUP(I15,Actions,2,FALSE)</f>
-        <v>💡➜</v>
-      </c>
-      <c r="K15" s="122" t="s">
-        <v>279</v>
-      </c>
-      <c r="L15" s="65" t="str">
-        <f>VLOOKUP(K15,Actions,2,FALSE)</f>
-        <v>👊👊🔊🔊➜➜</v>
-      </c>
-      <c r="M15" s="112" t="s">
-        <v>253</v>
-      </c>
       <c r="N15" s="93" t="str">
-        <f>VLOOKUP(M15,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>🔓👊📷🔊🔊⚠</v>
       </c>
       <c r="O15" s="122" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="P15" s="93" t="str">
-        <f>VLOOKUP(O15,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="Q15" s="68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Defeat%n🔓📷🔊➜</v>
       </c>
       <c r="R15" s="63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="S15" s="68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Slink%n💡➜</v>
       </c>
       <c r="T15" s="68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Rampage%n👊👊🔊🔊➜➜</v>
       </c>
       <c r="U15" s="68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Detonate%n🔓👊📷🔊🔊⚠</v>
       </c>
       <c r="V15" s="69" t="str">
+        <f t="shared" si="15"/>
+        <v>Punch%n👊🔊🔊➜</v>
+      </c>
+      <c r="W15" s="70" t="str">
         <f t="shared" si="6"/>
-        <v>Punch%n👊🔊🔊➜</v>
-      </c>
-      <c r="W15" s="70" t="str">
-        <f>Q15 &amp; "%n"
-&amp; R15 &amp; "%n"
-&amp; S15 &amp; "%n"
-&amp; T15 &amp; "%n"
-&amp; U15 &amp; "%n"
-&amp; V15</f>
         <v>Defeat%n🔓📷🔊➜%nSprint%n🔊🔊➜➜➜%nSlink%n💡➜%nRampage%n👊👊🔊🔊➜➜%nDetonate%n🔓👊📷🔊🔊⚠%nPunch%n👊🔊🔊➜</v>
       </c>
       <c r="X15" s="68" t="s">
         <v>140</v>
       </c>
       <c r="Y15" s="65" t="str">
-        <f>IF(X15="(none)","",VLOOKUP(X15,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z15" s="68" t="s">
         <v>140</v>
       </c>
       <c r="AA15" s="65" t="str">
-        <f>IF(Z15="(none)","",VLOOKUP(Z15,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AC15" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="AD15" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AE15" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF15" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AG15" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH15" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI15" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AN15" s="77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:40" s="77" customFormat="1" x14ac:dyDescent="0.25">
@@ -4963,124 +4901,119 @@
         <v>126</v>
       </c>
       <c r="E16" s="113" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F16" s="94" t="str">
-        <f>VLOOKUP(E16,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="G16" s="123" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H16" s="80" t="str">
-        <f>VLOOKUP(G16,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I16" s="114" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J16" s="94" t="str">
-        <f>VLOOKUP(I16,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>💰🔊</v>
       </c>
       <c r="K16" s="132" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L16" s="80" t="str">
-        <f>VLOOKUP(K16,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>👊👊👊🔊🔊</v>
       </c>
       <c r="M16" s="114" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="N16" s="94" t="str">
-        <f>VLOOKUP(M16,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>👊🔊➜➜</v>
       </c>
       <c r="O16" s="123" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="P16" s="94" t="str">
-        <f>VLOOKUP(O16,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>👊💡➜</v>
       </c>
       <c r="Q16" s="75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Rake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="R16" s="73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="S16" s="73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Yoink%n💰🔊</v>
       </c>
       <c r="T16" s="79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Spin Kick%n👊👊👊🔊🔊</v>
       </c>
       <c r="U16" s="79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Kick%n👊🔊➜➜</v>
       </c>
       <c r="V16" s="79" t="str">
+        <f t="shared" si="15"/>
+        <v>Jab%n👊💡➜</v>
+      </c>
+      <c r="W16" s="81" t="str">
         <f t="shared" si="6"/>
-        <v>Jab%n👊💡➜</v>
-      </c>
-      <c r="W16" s="81" t="str">
-        <f>Q16 &amp; "%n"
-&amp; R16 &amp; "%n"
-&amp; S16 &amp; "%n"
-&amp; T16 &amp; "%n"
-&amp; U16 &amp; "%n"
-&amp; V16</f>
         <v>Rake%n🔓🔓🔊🔊➜%nRun%n🔊🔊➜➜%nYoink%n💰🔊%nSpin Kick%n👊👊👊🔊🔊%nKick%n👊🔊➜➜%nJab%n👊💡➜</v>
       </c>
       <c r="X16" s="75" t="s">
         <v>140</v>
       </c>
       <c r="Y16" s="80" t="str">
-        <f>IF(X16="(none)","",VLOOKUP(X16,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z16" s="75" t="s">
         <v>140</v>
       </c>
       <c r="AA16" s="81" t="str">
-        <f>IF(Z16="(none)","",VLOOKUP(Z16,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AC16" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AD16" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE16" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF16" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AG16" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH16" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI16" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -5098,124 +5031,119 @@
         <v>126</v>
       </c>
       <c r="E17" s="114" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F17" s="95" t="str">
-        <f>VLOOKUP(E17,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>🔓👊📷🔊🔊⚠</v>
       </c>
       <c r="G17" s="123" t="s">
+        <v>246</v>
+      </c>
+      <c r="H17" s="76" t="str">
+        <f t="shared" si="1"/>
+        <v>💰💰</v>
+      </c>
+      <c r="I17" s="114" t="s">
+        <v>241</v>
+      </c>
+      <c r="J17" s="95" t="str">
+        <f t="shared" si="2"/>
+        <v>🔊🔊➜➜</v>
+      </c>
+      <c r="K17" s="123" t="s">
+        <v>243</v>
+      </c>
+      <c r="L17" s="76" t="str">
+        <f t="shared" si="3"/>
+        <v>🔍➜➜</v>
+      </c>
+      <c r="M17" s="114" t="s">
         <v>249</v>
       </c>
-      <c r="H17" s="76" t="str">
-        <f>VLOOKUP(G17,Actions,2,FALSE)</f>
-        <v>💰💰</v>
-      </c>
-      <c r="I17" s="114" t="s">
-        <v>244</v>
-      </c>
-      <c r="J17" s="95" t="str">
-        <f>VLOOKUP(I17,Actions,2,FALSE)</f>
+      <c r="N17" s="95" t="str">
+        <f t="shared" si="4"/>
+        <v>🔓🔓🔊🔊➜</v>
+      </c>
+      <c r="O17" s="123" t="s">
+        <v>241</v>
+      </c>
+      <c r="P17" s="95" t="str">
+        <f t="shared" si="5"/>
         <v>🔊🔊➜➜</v>
       </c>
-      <c r="K17" s="123" t="s">
-        <v>246</v>
-      </c>
-      <c r="L17" s="76" t="str">
-        <f>VLOOKUP(K17,Actions,2,FALSE)</f>
-        <v>🔍➜➜</v>
-      </c>
-      <c r="M17" s="114" t="s">
-        <v>252</v>
-      </c>
-      <c r="N17" s="95" t="str">
-        <f>VLOOKUP(M17,Actions,2,FALSE)</f>
-        <v>🔓🔓🔊🔊➜</v>
-      </c>
-      <c r="O17" s="123" t="s">
-        <v>244</v>
-      </c>
-      <c r="P17" s="95" t="str">
-        <f>VLOOKUP(O17,Actions,2,FALSE)</f>
-        <v>🔊🔊➜➜</v>
-      </c>
       <c r="Q17" s="75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Detonate%n🔓👊📷🔊🔊⚠</v>
       </c>
       <c r="R17" s="75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Nab%n💰💰</v>
       </c>
       <c r="S17" s="73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="T17" s="73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Sneak%n🔍➜➜</v>
       </c>
       <c r="U17" s="82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Rake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="V17" s="73" t="str">
+        <f t="shared" si="15"/>
+        <v>Run%n🔊🔊➜➜</v>
+      </c>
+      <c r="W17" s="81" t="str">
         <f t="shared" si="6"/>
-        <v>Run%n🔊🔊➜➜</v>
-      </c>
-      <c r="W17" s="81" t="str">
-        <f>Q17 &amp; "%n"
-&amp; R17 &amp; "%n"
-&amp; S17 &amp; "%n"
-&amp; T17 &amp; "%n"
-&amp; U17 &amp; "%n"
-&amp; V17</f>
         <v>Detonate%n🔓👊📷🔊🔊⚠%nNab%n💰💰%nRun%n🔊🔊➜➜%nSneak%n🔍➜➜%nRake%n🔓🔓🔊🔊➜%nRun%n🔊🔊➜➜</v>
       </c>
       <c r="X17" s="75" t="s">
         <v>140</v>
       </c>
       <c r="Y17" s="76" t="str">
-        <f>IF(X17="(none)","",VLOOKUP(X17,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z17" s="75" t="s">
         <v>140</v>
       </c>
       <c r="AA17" s="76" t="str">
-        <f>IF(Z17="(none)","",VLOOKUP(Z17,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC17" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AD17" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AE17" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF17" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AG17" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AH17" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI17" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
     </row>
@@ -5233,124 +5161,119 @@
         <v>59</v>
       </c>
       <c r="E18" s="139" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F18" s="144" t="str">
-        <f>VLOOKUP(E18,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>📷🔍</v>
       </c>
       <c r="G18" s="138" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H18" s="142" t="str">
-        <f>VLOOKUP(G18,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="I18" s="139" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="J18" s="144" t="str">
-        <f>VLOOKUP(I18,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K18" s="138" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="L18" s="142" t="str">
-        <f>VLOOKUP(K18,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M18" s="139" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N18" s="144" t="str">
-        <f>VLOOKUP(M18,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="O18" s="138" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="P18" s="144" t="str">
-        <f>VLOOKUP(O18,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="Q18" s="134" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Loop%n📷🔍</v>
       </c>
       <c r="R18" s="134" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Recon%n💡💡🔊🔍</v>
       </c>
       <c r="S18" s="134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="T18" s="134" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Punch%n👊🔊🔊➜</v>
       </c>
       <c r="U18" s="134" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="V18" s="141" t="str">
+        <f t="shared" si="15"/>
+        <v>Rake%n🔓🔓🔊🔊➜</v>
+      </c>
+      <c r="W18" s="145" t="str">
         <f t="shared" si="6"/>
-        <v>Rake%n🔓🔓🔊🔊➜</v>
-      </c>
-      <c r="W18" s="145" t="str">
-        <f>Q18 &amp; "%n"
-&amp; R18 &amp; "%n"
-&amp; S18 &amp; "%n"
-&amp; T18 &amp; "%n"
-&amp; U18 &amp; "%n"
-&amp; V18</f>
         <v>Loop%n📷🔍%nRecon%n💡💡🔊🔍%nRun%n🔊🔊➜➜%nPunch%n👊🔊🔊➜%nRun%n🔊🔊➜➜%nRake%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="X18" s="141" t="s">
         <v>140</v>
       </c>
       <c r="Y18" s="146" t="str">
-        <f>IF(X18="(none)","",VLOOKUP(X18,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z18" s="141" t="s">
         <v>140</v>
       </c>
       <c r="AA18" s="145" t="str">
-        <f>IF(Z18="(none)","",VLOOKUP(Z18,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB18" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC18" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="AD18" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="AE18" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AF18" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AG18" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AH18" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AI18" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -5368,128 +5291,123 @@
         <v>59</v>
       </c>
       <c r="E19" s="139" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F19" s="144" t="str">
-        <f>VLOOKUP(E19,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="G19" s="138" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H19" s="142" t="str">
-        <f>VLOOKUP(G19,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I19" s="139" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J19" s="144" t="str">
-        <f>VLOOKUP(I19,Actions,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>📷🔍</v>
       </c>
       <c r="K19" s="138" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L19" s="142" t="str">
-        <f>VLOOKUP(K19,Actions,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>🔓👊📷🔊</v>
       </c>
       <c r="M19" s="139" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N19" s="144" t="str">
-        <f>VLOOKUP(M19,Actions,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="O19" s="138" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="P19" s="144" t="str">
-        <f>VLOOKUP(O19,Actions,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>🔓</v>
       </c>
       <c r="Q19" s="148" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="R19" s="134" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="S19" s="134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Loop%n📷🔍</v>
       </c>
       <c r="T19" s="134" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>Redirect%n🔓👊📷🔊</v>
       </c>
       <c r="U19" s="134" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>Recon%n💡💡🔊🔍</v>
       </c>
       <c r="V19" s="134" t="str">
+        <f t="shared" si="15"/>
+        <v>Pick%n🔓</v>
+      </c>
+      <c r="W19" s="145" t="str">
         <f t="shared" si="6"/>
-        <v>Pick%n🔓</v>
-      </c>
-      <c r="W19" s="145" t="str">
-        <f>Q19 &amp; "%n"
-&amp; R19 &amp; "%n"
-&amp; S19 &amp; "%n"
-&amp; T19 &amp; "%n"
-&amp; U19 &amp; "%n"
-&amp; V19</f>
         <v>Examine%n💡💡💡🔊%nRun%n🔊🔊➜➜%nLoop%n📷🔍%nRedirect%n🔓👊📷🔊%nRecon%n💡💡🔊🔍%nPick%n🔓</v>
       </c>
       <c r="X19" s="141" t="s">
         <v>140</v>
       </c>
       <c r="Y19" s="142" t="str">
-        <f>IF(X19="(none)","",VLOOKUP(X19,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z19" s="141" t="s">
         <v>140</v>
       </c>
       <c r="AA19" s="142" t="str">
-        <f>IF(Z19="(none)","",VLOOKUP(Z19,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB19" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AC19" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AD19" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AE19" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AF19" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AG19" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AH19" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AI19" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN19" s="143" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -5554,7 +5472,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5575,7 +5493,7 @@
         <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5583,7 +5501,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>379</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -5592,7 +5510,7 @@
         <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -5601,7 +5519,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -5610,7 +5528,7 @@
         <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>198</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5618,7 +5536,7 @@
         <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5626,7 +5544,7 @@
         <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5634,7 +5552,7 @@
         <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5642,7 +5560,7 @@
         <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -5655,7 +5573,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5669,48 +5587,48 @@
   <sheetData>
     <row r="1" spans="1:12" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="83" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" s="83" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="71" t="s">
-        <v>303</v>
-      </c>
-      <c r="C1" s="71" t="s">
+      <c r="G1" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="H1" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="I1" s="83" t="s">
         <v>221</v>
       </c>
-      <c r="G1" s="83" t="s">
+      <c r="J1" s="83" t="s">
         <v>222</v>
       </c>
-      <c r="H1" s="83" t="s">
-        <v>223</v>
-      </c>
-      <c r="I1" s="83" t="s">
-        <v>224</v>
-      </c>
-      <c r="J1" s="83" t="s">
-        <v>225</v>
-      </c>
       <c r="K1" s="71" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -5739,13 +5657,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -5774,13 +5692,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E4" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -5809,13 +5727,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -5844,13 +5762,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E6" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -5879,13 +5797,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E7" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -5914,13 +5832,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E8" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -5949,24 +5867,24 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>358</v>
+        <v>378</v>
       </c>
       <c r="B9" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B10" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E10" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -5995,13 +5913,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6030,13 +5948,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B12" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6065,13 +5983,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B13" t="s">
         <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E13" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6100,13 +6018,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E14" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6135,13 +6053,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B15" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E15" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6170,10 +6088,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C16" t="s">
         <v>158</v>
@@ -6205,10 +6123,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B17" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C17" t="s">
         <v>158</v>
@@ -6240,7 +6158,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B18" t="s">
         <v>103</v>
@@ -6275,10 +6193,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B19" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -6310,10 +6228,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B20" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -6345,10 +6263,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B21" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
@@ -6380,10 +6298,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B22" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
@@ -6415,10 +6333,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B23" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -6450,13 +6368,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B24" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E24" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6485,13 +6403,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E25" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6520,13 +6438,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B26" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E26" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6555,13 +6473,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B27" t="s">
         <v>128</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E27" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6590,13 +6508,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B28" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E28" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6625,13 +6543,13 @@
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B29" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E29" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6660,13 +6578,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B30" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E30" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6695,13 +6613,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B31" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E31" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6730,13 +6648,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B32" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E32" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6765,13 +6683,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E33" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6800,13 +6718,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E34" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6835,13 +6753,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B35" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E35" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6870,24 +6788,24 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B36" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
         <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E37" s="84">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6916,10 +6834,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B38" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
@@ -6951,7 +6869,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
@@ -6983,7 +6901,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B40" t="s">
         <v>100</v>
@@ -7018,10 +6936,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B41" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -7053,10 +6971,10 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B42" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -7102,10 +7020,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:S31"/>
+  <dimension ref="A7:S33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8469,6 +8387,11 @@
         <v>124</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>382</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8494,13 +8417,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E1" s="71" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8517,13 +8440,13 @@
         <v>146</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8540,10 +8463,10 @@
         <v>147</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8560,13 +8483,13 @@
         <v>148</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>329</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8583,7 +8506,7 @@
         <v>149</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8600,13 +8523,13 @@
         <v>151</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>333</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8623,68 +8546,68 @@
         <v>150</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -8707,43 +8630,43 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
         <v>182</v>
-      </c>
-      <c r="B1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="85" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -8766,50 +8689,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix skill upgrades for skill_backs
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -2894,16 +2894,16 @@
   <dimension ref="A1:BD20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="113" bestFit="1" customWidth="1"/>
@@ -2925,10 +2925,10 @@
     <col min="21" max="21" width="20.140625" style="3" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="25.140625" style="3" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="130.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="13" style="4" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="14" style="4" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="15.140625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="13" style="4" customWidth="1"/>
+    <col min="26" max="26" width="15.140625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="14" style="4" customWidth="1"/>
     <col min="28" max="28" width="3.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="3.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="3.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -3169,49 +3169,49 @@
         <v>Punch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nReveal%n🔍%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nGrab%n💰🔊</v>
       </c>
       <c r="X2" s="40" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
       <c r="Y2" s="41" t="str">
-        <f>IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
-        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSneak%n📷➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <f t="shared" ref="Y2:Y19" si="7">IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
+        <v>Flip%n👊🔊➜%nDisable%n📷🔊➜%nStudy%n💡💡%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nRansack%n💰💰🔊</v>
       </c>
       <c r="Z2" s="40" t="s">
-        <v>139</v>
+        <v>380</v>
       </c>
       <c r="AA2" s="43" t="str">
-        <f>IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
-        <v>Rake%n🔓🔓🔊➜%nStudy%n💡💡%nSpy Stuff%n🔓👊%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShort%n🔓📷🔊🔊</v>
+        <f t="shared" ref="AA2:AA19" si="8">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
+        <v>Punch%n👊🔊🔊➜%nUnplug%n📷📷➜%nKey In%n🔍🔓%nFlip%n👊🔊➜%nDisable%n📷🔊➜%nGrab%n💰🔊</v>
       </c>
       <c r="AB2" s="40">
         <f>(LEN($W2)-LEN(SUBSTITUTE($W2,AB$1,"")))/LEN(AB$1)</f>
         <v>0</v>
       </c>
       <c r="AC2" s="40">
-        <f t="shared" ref="AC2:AI17" si="7">(LEN($W2)-LEN(SUBSTITUTE($W2,AC$1,"")))/LEN(AC$1)</f>
+        <f t="shared" ref="AC2:AI17" si="9">(LEN($W2)-LEN(SUBSTITUTE($W2,AC$1,"")))/LEN(AC$1)</f>
         <v>9</v>
       </c>
       <c r="AD2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ2" s="39" t="s">
@@ -3300,27 +3300,27 @@
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q3" s="38" t="str">
-        <f t="shared" ref="Q3:Q19" si="8">E3&amp;"%n"&amp;F3</f>
+        <f t="shared" ref="Q3:Q19" si="10">E3&amp;"%n"&amp;F3</f>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="R3" s="38" t="str">
-        <f t="shared" ref="R3:R19" si="9">G3&amp;"%n"&amp;H3</f>
+        <f t="shared" ref="R3:R19" si="11">G3&amp;"%n"&amp;H3</f>
         <v>Shim%n🔓🔊</v>
       </c>
       <c r="S3" s="38" t="str">
-        <f t="shared" ref="S3:S19" si="10">I3&amp;"%n"&amp;J3</f>
+        <f t="shared" ref="S3:S19" si="12">I3&amp;"%n"&amp;J3</f>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="T3" s="37" t="str">
-        <f t="shared" ref="T3:T19" si="11">K3&amp;"%n"&amp;L3</f>
+        <f t="shared" ref="T3:T19" si="13">K3&amp;"%n"&amp;L3</f>
         <v>Study%n💡💡</v>
       </c>
       <c r="U3" s="38" t="str">
-        <f t="shared" ref="U3:U19" si="12">M3&amp;"%n"&amp;N3</f>
+        <f t="shared" ref="U3:U19" si="14">M3&amp;"%n"&amp;N3</f>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="V3" s="38" t="str">
-        <f t="shared" ref="V3:V19" si="13">O3&amp;"%n"&amp;P3</f>
+        <f t="shared" ref="V3:V19" si="15">O3&amp;"%n"&amp;P3</f>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="W3" s="35" t="str">
@@ -3328,49 +3328,49 @@
         <v>Run%n🔊🔊➜➜%nShim%n🔓🔊%nRun%n🔊🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="X3" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="36" t="e">
-        <f>IF(X3="(none)","",VLOOKUP(X3,$A$2:$W$19,23,FALSE))</f>
-        <v>#N/A</v>
+        <v>36</v>
+      </c>
+      <c r="Y3" s="36" t="str">
+        <f t="shared" si="7"/>
+        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="Z3" s="38" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="AA3" s="35" t="str">
-        <f>IF(Z3="(none)","",VLOOKUP(Z3,$A$2:$W$19,23,FALSE))</f>
-        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <f t="shared" si="8"/>
+        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSneak%n📷➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="AB3" s="40">
-        <f t="shared" ref="AB3:AI19" si="14">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
+        <f t="shared" ref="AB3:AI19" si="16">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
         <v>5</v>
       </c>
       <c r="AC3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AD3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AE3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="33" t="s">
@@ -3414,7 +3414,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>125</v>
+        <v>385</v>
       </c>
       <c r="E4" s="106" t="s">
         <v>175</v>
@@ -3459,27 +3459,27 @@
         <v>🔊🔊➜➜</v>
       </c>
       <c r="Q4" s="50" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Reveal%n🔍</v>
       </c>
       <c r="R4" s="52" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Strongarm%n🔓👊🔊🔊</v>
       </c>
       <c r="S4" s="52" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Short%n🔓📷🔊🔊</v>
       </c>
       <c r="T4" s="50" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Zap%n👊📷🔊🔊</v>
       </c>
       <c r="U4" s="50" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Grab%n💰🔊</v>
       </c>
       <c r="V4" s="50" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="W4" s="53" t="str">
@@ -3490,46 +3490,46 @@
         <v>181</v>
       </c>
       <c r="Y4" s="51" t="str">
-        <f>IF(X4="(none)","",VLOOKUP(X4,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v>Study%n💡💡%nSpy Stuff%n🔓👊%nShort%n🔓📷🔊🔊%nZap%n👊📷🔊🔊%nGrab%n💰🔊%nDash%n🔊➜➜</v>
       </c>
       <c r="Z4" s="50" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="AA4" s="53" t="str">
-        <f>IF(Z4="(none)","",VLOOKUP(Z4,$A$2:$W$19,23,FALSE))</f>
-        <v>Bump%n🔓🔓🔊🔊➜%nStudy%n💡💡%nShim%n🔓🔊%nSprint%n🔊🔊➜➜➜%nRun%n🔊🔊➜➜%nShim%n🔓🔊</v>
+        <f t="shared" si="8"/>
+        <v>Redirect%n🔓👊📷🔊%nStrongarm%n🔓👊🔊🔊%nShort%n🔓📷🔊🔊%nShock%n👊📷%nGrab%n💰🔊%nDash%n🔊➜➜</v>
       </c>
       <c r="AB4" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="AD4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AE4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ4" s="54" t="s">
@@ -3618,27 +3618,27 @@
         <v>💡💡</v>
       </c>
       <c r="Q5" s="61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Tackle%n👊🔊</v>
       </c>
       <c r="R5" s="61" t="str">
-        <f t="shared" si="9"/>
-        <v>Run%n🔊🔊➜➜</v>
-      </c>
-      <c r="S5" s="61" t="str">
-        <f t="shared" si="10"/>
-        <v>Bash%n👊👊🔊</v>
-      </c>
-      <c r="T5" s="61" t="str">
         <f t="shared" si="11"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
+      <c r="S5" s="61" t="str">
+        <f t="shared" si="12"/>
+        <v>Bash%n👊👊🔊</v>
+      </c>
+      <c r="T5" s="61" t="str">
+        <f t="shared" si="13"/>
+        <v>Run%n🔊🔊➜➜</v>
+      </c>
       <c r="U5" s="61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Tackle%n👊🔊</v>
       </c>
       <c r="V5" s="61" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="W5" s="63" t="str">
@@ -3646,49 +3646,49 @@
         <v>Tackle%n👊🔊%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nRun%n🔊🔊➜➜%nTackle%n👊🔊%nStudy%n💡💡</v>
       </c>
       <c r="X5" s="61" t="s">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="Y5" s="62" t="str">
-        <f>IF(X5="(none)","",VLOOKUP(X5,$A$2:$W$19,23,FALSE))</f>
-        <v>Flip%n👊🔊➜%nDisable%n📷🔊➜%nStudy%n💡💡%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nRansack%n💰💰🔊</v>
+        <f t="shared" si="7"/>
+        <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nRampage%n👊👊🔊🔊➜➜%nRun%n🔊🔊➜➜%nStrongarm%n🔓👊🔊🔊%nStudy%n💡💡</v>
       </c>
       <c r="Z5" s="61" t="s">
-        <v>115</v>
+        <v>394</v>
       </c>
       <c r="AA5" s="63" t="str">
-        <f>IF(Z5="(none)","",VLOOKUP(Z5,$A$2:$W$19,23,FALSE))</f>
-        <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nRampage%n👊👊🔊🔊➜➜%nRun%n🔊🔊➜➜%nStrongarm%n🔓👊🔊🔊%nStudy%n💡💡</v>
+        <f t="shared" si="8"/>
+        <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nDetonate%n🔓👊📷🔊🔊⚠%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nStudy%n💡💡</v>
       </c>
       <c r="AB5" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AD5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AG5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="64" t="s">
@@ -3777,27 +3777,27 @@
         <v>🔓🔊</v>
       </c>
       <c r="Q6" s="70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Bump%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="R6" s="70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="S6" s="72" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Shim%n🔓🔊</v>
       </c>
       <c r="T6" s="70" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="U6" s="72" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="V6" s="72" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Shim%n🔓🔊</v>
       </c>
       <c r="W6" s="73" t="str">
@@ -3805,49 +3805,49 @@
         <v>Bump%n🔓🔓🔊🔊➜%nStudy%n💡💡%nShim%n🔓🔊%nSprint%n🔊🔊➜➜➜%nRun%n🔊🔊➜➜%nShim%n🔓🔊</v>
       </c>
       <c r="X6" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y6" s="71" t="e">
-        <f>IF(X6="(none)","",VLOOKUP(X6,$A$2:$W$19,23,FALSE))</f>
-        <v>#N/A</v>
+        <v>401</v>
+      </c>
+      <c r="Y6" s="71" t="str">
+        <f t="shared" si="7"/>
+        <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShim%n🔓🔊</v>
       </c>
       <c r="Z6" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="AA6" s="73" t="e">
-        <f>IF(Z6="(none)","",VLOOKUP(Z6,$A$2:$W$19,23,FALSE))</f>
-        <v>#N/A</v>
+        <v>139</v>
+      </c>
+      <c r="AA6" s="73" t="str">
+        <f t="shared" si="8"/>
+        <v>Rake%n🔓🔓🔊➜%nStudy%n💡💡%nSpy Stuff%n🔓👊%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShort%n🔓📷🔊🔊</v>
       </c>
       <c r="AB6" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AD6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="74" t="s">
@@ -3936,27 +3936,27 @@
         <v>📷🔊🔊➜</v>
       </c>
       <c r="Q7" s="131" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Shatter%n📷📷🔊🔊➜</v>
       </c>
       <c r="R7" s="131" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="S7" s="131" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Smash%n📷🔊🔊➜</v>
       </c>
       <c r="T7" s="131" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Reveal%n🔍</v>
       </c>
       <c r="U7" s="138" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="V7" s="138" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Smash%n📷🔊🔊➜</v>
       </c>
       <c r="W7" s="139" t="str">
@@ -3967,46 +3967,46 @@
         <v>63</v>
       </c>
       <c r="Y7" s="132" t="str">
-        <f>IF(X7="(none)","",VLOOKUP(X7,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v>Unplug%n📷📷➜%nSprint%n🔊🔊➜➜➜%nDisable%n📷🔊➜%nDiscover%n🔍🔍%nRecon%n💡💡🔊🔍%nDisable%n📷🔊➜</v>
       </c>
       <c r="Z7" s="138" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA7" s="139" t="e">
-        <f>IF(Z7="(none)","",VLOOKUP(Z7,$A$2:$W$19,23,FALSE))</f>
-        <v>#N/A</v>
+        <v>406</v>
+      </c>
+      <c r="AA7" s="139" t="str">
+        <f t="shared" si="8"/>
+        <v>Unplug%n📷📷➜%nDash%n🔊➜➜%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
       </c>
       <c r="AB7" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="AC7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="AD7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AF7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="140" t="s">
@@ -4095,27 +4095,27 @@
         <v>💰💰🔊</v>
       </c>
       <c r="Q8" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Flip%n👊🔊➜</v>
       </c>
       <c r="R8" s="42" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="S8" s="42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="T8" s="42" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Punch%n👊🔊🔊➜</v>
       </c>
       <c r="U8" s="42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Smash%n📷🔊🔊➜</v>
       </c>
       <c r="V8" s="42" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Ransack%n💰💰🔊</v>
       </c>
       <c r="W8" s="44" t="str">
@@ -4126,46 +4126,46 @@
         <v>140</v>
       </c>
       <c r="Y8" s="45" t="str">
-        <f>IF(X8="(none)","",VLOOKUP(X8,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z8" s="42" t="s">
         <v>140</v>
       </c>
       <c r="AA8" s="43" t="str">
-        <f>IF(Z8="(none)","",VLOOKUP(Z8,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB8" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AD8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AJ8" s="146" t="s">
@@ -4254,27 +4254,27 @@
         <v>💰🔊</v>
       </c>
       <c r="Q9" s="48" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Punch%n👊🔊🔊➜</v>
       </c>
       <c r="R9" s="47" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Unplug%n📷📷➜</v>
       </c>
       <c r="S9" s="47" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Key In%n🔍🔓</v>
       </c>
       <c r="T9" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Flip%n👊🔊➜</v>
       </c>
       <c r="U9" s="48" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="V9" s="48" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Grab%n💰🔊</v>
       </c>
       <c r="W9" s="44" t="str">
@@ -4285,46 +4285,46 @@
         <v>140</v>
       </c>
       <c r="Y9" s="44" t="str">
-        <f>IF(X9="(none)","",VLOOKUP(X9,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z9" s="47" t="s">
         <v>140</v>
       </c>
       <c r="AA9" s="43" t="str">
-        <f>IF(Z9="(none)","",VLOOKUP(Z9,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB9" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AD9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AF9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ9" s="46" t="s">
@@ -4413,27 +4413,27 @@
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q10" s="37" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="R10" s="37" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Shim%n🔓🔊</v>
       </c>
       <c r="S10" s="37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Sleeper Hold%n👊➜</v>
       </c>
       <c r="T10" s="38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="U10" s="38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="V10" s="38" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="W10" s="35" t="str">
@@ -4444,46 +4444,46 @@
         <v>140</v>
       </c>
       <c r="Y10" s="35" t="str">
-        <f>IF(X10="(none)","",VLOOKUP(X10,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z10" s="37" t="s">
         <v>140</v>
       </c>
       <c r="AA10" s="35" t="str">
-        <f>IF(Z10="(none)","",VLOOKUP(Z10,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB10" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AC10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AD10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AG10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ10" s="148" t="s">
@@ -4572,27 +4572,27 @@
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q11" s="38" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="R11" s="38" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Shim%n🔓🔊</v>
       </c>
       <c r="S11" s="37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Sneak%n📷➜➜</v>
       </c>
       <c r="T11" s="38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="U11" s="38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="V11" s="37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="W11" s="35" t="str">
@@ -4603,46 +4603,46 @@
         <v>140</v>
       </c>
       <c r="Y11" s="35" t="str">
-        <f>IF(X11="(none)","",VLOOKUP(X11,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z11" s="37" t="s">
         <v>140</v>
       </c>
       <c r="AA11" s="35" t="str">
-        <f>IF(Z11="(none)","",VLOOKUP(Z11,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB11" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AC11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AD11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AE11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="148" t="s">
@@ -4686,7 +4686,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>125</v>
+        <v>385</v>
       </c>
       <c r="E12" s="107" t="s">
         <v>235</v>
@@ -4731,27 +4731,27 @@
         <v>🔊➜➜</v>
       </c>
       <c r="Q12" s="52" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="R12" s="52" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Spy Stuff%n🔓👊</v>
       </c>
       <c r="S12" s="50" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Short%n🔓📷🔊🔊</v>
       </c>
       <c r="T12" s="52" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Zap%n👊📷🔊🔊</v>
       </c>
       <c r="U12" s="50" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Grab%n💰🔊</v>
       </c>
       <c r="V12" s="52" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="W12" s="56" t="str">
@@ -4762,46 +4762,46 @@
         <v>140</v>
       </c>
       <c r="Y12" s="57" t="str">
-        <f>IF(X12="(none)","",VLOOKUP(X12,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z12" s="52" t="s">
         <v>140</v>
       </c>
       <c r="AA12" s="56" t="str">
-        <f>IF(Z12="(none)","",VLOOKUP(Z12,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB12" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AD12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AE12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AH12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ12" s="54" t="s">
@@ -4845,7 +4845,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>125</v>
+        <v>385</v>
       </c>
       <c r="E13" s="107" t="s">
         <v>233</v>
@@ -4890,27 +4890,27 @@
         <v>🔊➜➜</v>
       </c>
       <c r="Q13" s="60" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Redirect%n🔓👊📷🔊</v>
       </c>
       <c r="R13" s="59" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Strongarm%n🔓👊🔊🔊</v>
       </c>
       <c r="S13" s="59" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Short%n🔓📷🔊🔊</v>
       </c>
       <c r="T13" s="59" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Shock%n👊📷</v>
       </c>
       <c r="U13" s="60" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Grab%n💰🔊</v>
       </c>
       <c r="V13" s="60" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="W13" s="56" t="str">
@@ -4921,46 +4921,46 @@
         <v>140</v>
       </c>
       <c r="Y13" s="57" t="str">
-        <f>IF(X13="(none)","",VLOOKUP(X13,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z13" s="59" t="s">
         <v>140</v>
       </c>
       <c r="AA13" s="56" t="str">
-        <f>IF(Z13="(none)","",VLOOKUP(Z13,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB13" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AD13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AE13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AF13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AG13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AH13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ13" s="54" t="s">
@@ -5049,27 +5049,27 @@
         <v>💡💡</v>
       </c>
       <c r="Q14" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Bash%n👊👊🔊</v>
       </c>
       <c r="R14" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="S14" s="67" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Rampage%n👊👊🔊🔊➜➜</v>
       </c>
       <c r="T14" s="61" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="U14" s="66" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Strongarm%n🔓👊🔊🔊</v>
       </c>
       <c r="V14" s="67" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="W14" s="68" t="str">
@@ -5080,46 +5080,46 @@
         <v>140</v>
       </c>
       <c r="Y14" s="63" t="str">
-        <f>IF(X14="(none)","",VLOOKUP(X14,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z14" s="66" t="s">
         <v>140</v>
       </c>
       <c r="AA14" s="63" t="str">
-        <f>IF(Z14="(none)","",VLOOKUP(Z14,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB14" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AD14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AG14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="64" t="s">
@@ -5208,27 +5208,27 @@
         <v>💡💡</v>
       </c>
       <c r="Q15" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Bash%n👊👊🔊</v>
       </c>
       <c r="R15" s="61" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="S15" s="66" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Detonate%n🔓👊📷🔊🔊⚠</v>
       </c>
       <c r="T15" s="66" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="U15" s="66" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Bash%n👊👊🔊</v>
       </c>
       <c r="V15" s="67" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="W15" s="68" t="str">
@@ -5239,46 +5239,46 @@
         <v>140</v>
       </c>
       <c r="Y15" s="63" t="str">
-        <f>IF(X15="(none)","",VLOOKUP(X15,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z15" s="66" t="s">
         <v>140</v>
       </c>
       <c r="AA15" s="63" t="str">
-        <f>IF(Z15="(none)","",VLOOKUP(Z15,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB15" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AD15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AE15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AG15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="64" t="s">
@@ -5365,27 +5365,27 @@
         <v>🔓🔊</v>
       </c>
       <c r="Q16" s="72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Rake%n🔓🔓🔊➜</v>
       </c>
       <c r="R16" s="70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Recon%n💡💡🔊🔍</v>
       </c>
       <c r="S16" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Swipe%n🔓💰</v>
       </c>
       <c r="T16" s="76" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="U16" s="76" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="V16" s="76" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Shim%n🔓🔊</v>
       </c>
       <c r="W16" s="78" t="str">
@@ -5396,46 +5396,46 @@
         <v>140</v>
       </c>
       <c r="Y16" s="77" t="str">
-        <f>IF(X16="(none)","",VLOOKUP(X16,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z16" s="72" t="s">
         <v>140</v>
       </c>
       <c r="AA16" s="78" t="str">
-        <f>IF(Z16="(none)","",VLOOKUP(Z16,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB16" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AD16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ16" s="74" t="s">
@@ -5524,27 +5524,27 @@
         <v>🔓📷🔊🔊</v>
       </c>
       <c r="Q17" s="72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Rake%n🔓🔓🔊➜</v>
       </c>
       <c r="R17" s="72" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="S17" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Spy Stuff%n🔓👊</v>
       </c>
       <c r="T17" s="70" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="U17" s="79" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="V17" s="70" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Short%n🔓📷🔊🔊</v>
       </c>
       <c r="W17" s="78" t="str">
@@ -5555,46 +5555,46 @@
         <v>140</v>
       </c>
       <c r="Y17" s="73" t="str">
-        <f>IF(X17="(none)","",VLOOKUP(X17,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z17" s="72" t="s">
         <v>140</v>
       </c>
       <c r="AA17" s="73" t="str">
-        <f>IF(Z17="(none)","",VLOOKUP(Z17,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB17" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AD17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AE17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AG17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="74" t="s">
@@ -5683,27 +5683,27 @@
         <v>📷🔊➜</v>
       </c>
       <c r="Q18" s="131" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Unplug%n📷📷➜</v>
       </c>
       <c r="R18" s="131" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="S18" s="131" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="T18" s="131" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Discover%n🔍🔍</v>
       </c>
       <c r="U18" s="131" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Recon%n💡💡🔊🔍</v>
       </c>
       <c r="V18" s="138" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="W18" s="142" t="str">
@@ -5714,46 +5714,46 @@
         <v>140</v>
       </c>
       <c r="Y18" s="143" t="str">
-        <f>IF(X18="(none)","",VLOOKUP(X18,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z18" s="138" t="s">
         <v>140</v>
       </c>
       <c r="AA18" s="142" t="str">
-        <f>IF(Z18="(none)","",VLOOKUP(Z18,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB18" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC18" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AD18" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="AE18" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="AF18" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG18" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AH18" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="AI18" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AJ18" s="140" t="s">
@@ -5839,27 +5839,27 @@
         <v>📷🔊➜</v>
       </c>
       <c r="Q19" s="145" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Unplug%n📷📷➜</v>
       </c>
       <c r="R19" s="131" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="S19" s="131" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="T19" s="131" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>Stride%n🔊➜🔍</v>
       </c>
       <c r="U19" s="131" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="V19" s="131" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="W19" s="142" t="str">
@@ -5870,46 +5870,46 @@
         <v>140</v>
       </c>
       <c r="Y19" s="139" t="str">
-        <f>IF(X19="(none)","",VLOOKUP(X19,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z19" s="138" t="s">
         <v>140</v>
       </c>
       <c r="AA19" s="139" t="str">
-        <f>IF(Z19="(none)","",VLOOKUP(Z19,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB19" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC19" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="AD19" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="AE19" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="AF19" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG19" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AH19" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AI19" s="40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AJ19" s="140" t="s">
@@ -8999,7 +8999,7 @@
         <v>284</v>
       </c>
       <c r="B48" t="str">
-        <f>VLOOKUP(A48,Actions,2,FALSE)</f>
+        <f t="shared" ref="B48:B55" si="0">VLOOKUP(A48,Actions,2,FALSE)</f>
         <v>👊➜</v>
       </c>
     </row>
@@ -9008,7 +9008,7 @@
         <v>265</v>
       </c>
       <c r="B49" t="str">
-        <f>VLOOKUP(A49,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>👊👊🔊🔊➜➜</v>
       </c>
     </row>
@@ -9017,7 +9017,7 @@
         <v>241</v>
       </c>
       <c r="B50" t="str">
-        <f>VLOOKUP(A50,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>🔓👊📷🔊🔊⚠</v>
       </c>
     </row>
@@ -9026,7 +9026,7 @@
         <v>272</v>
       </c>
       <c r="B51" t="str">
-        <f>VLOOKUP(A51,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>💡➜</v>
       </c>
     </row>
@@ -9035,7 +9035,7 @@
         <v>259</v>
       </c>
       <c r="B52" t="str">
-        <f>VLOOKUP(A52,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>👊🔊➜➜</v>
       </c>
     </row>
@@ -9044,7 +9044,7 @@
         <v>237</v>
       </c>
       <c r="B53" t="e">
-        <f>VLOOKUP(A53,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -9053,7 +9053,7 @@
         <v>231</v>
       </c>
       <c r="B54" t="str">
-        <f>VLOOKUP(A54,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>💡💡🔊🔍</v>
       </c>
     </row>
@@ -9062,7 +9062,7 @@
         <v>252</v>
       </c>
       <c r="B55" t="str">
-        <f>VLOOKUP(A55,Actions,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>🔍🔍</v>
       </c>
     </row>
@@ -9076,7 +9076,7 @@
         <v>256</v>
       </c>
       <c r="B58" t="str">
-        <f>VLOOKUP(A58,Actions,2,FALSE)</f>
+        <f t="shared" ref="B58:B63" si="1">VLOOKUP(A58,Actions,2,FALSE)</f>
         <v>👊💡➜</v>
       </c>
     </row>
@@ -9085,7 +9085,7 @@
         <v>233</v>
       </c>
       <c r="B59" t="str">
-        <f>VLOOKUP(A59,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>🔓👊📷🔊</v>
       </c>
     </row>
@@ -9094,25 +9094,25 @@
         <v>285</v>
       </c>
       <c r="B60" t="str">
-        <f>VLOOKUP(A60,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>👊👊👊🔊🔊</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B61" t="e">
-        <f>VLOOKUP(A61,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B62" t="e">
-        <f>VLOOKUP(A62,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B63" t="e">
-        <f>VLOOKUP(A63,Actions,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rebalancing skills & actions
Lesson: everyone takes the zero-noise move whenever they can. That delays the game and is a bit OP.

* Zero-noise default moves are just too powerful, soo...
  * Pick now has 1 noise
  * Spy Stuff now has 1 noise
  * Key In has 1 noise
* Script kiddie et al. is more powerful wrt re-planning
* Locksmith people have more planning memory
* BRING IT ON is really just three ideas for Reinforcements
* THERE ARE BETTER WAYS: nerf the Escape phase.
* Mastermind: Inspire must be used as an action
* No more Dash as a default move - make it Run unless it's a Con Artist
* Nab is gone. Just Yoink is fine. Should be opportunistic, not the strategy
* Lookout et al. has Run, not Dash. Run is still quite powerful as a default skill
* Unplug has 1 noise now. Balanced with similar moves.
* Sneak has 1 noise now
* Other wording revisions

Also: revised the look-and-feel of the prototype cards to match the mockups.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="409">
   <si>
     <t>Name</t>
   </si>
@@ -418,9 +418,6 @@
     <t>🔍</t>
   </si>
   <si>
-    <t>ADRENALINE%nGain 💡 on 👊</t>
-  </si>
-  <si>
     <t>Sewer Rat</t>
   </si>
   <si>
@@ -463,9 +460,6 @@
     <t>Walk%n🔊➜</t>
   </si>
   <si>
-    <t>Spy Stuff%n🔓👊</t>
-  </si>
-  <si>
     <t>Crawl%n➜</t>
   </si>
   <si>
@@ -502,9 +496,6 @@
     <t>LevelUp2</t>
   </si>
   <si>
-    <t>Key In%n🔍🔓</t>
-  </si>
-  <si>
     <t>Loot</t>
   </si>
   <si>
@@ -529,9 +520,6 @@
     <t>Ideas</t>
   </si>
   <si>
-    <t>Pick%n🔓</t>
-  </si>
-  <si>
     <t>KNOWS A GUY%nCan sell an extra $1k for each jewel or painting the team acquires</t>
   </si>
   <si>
@@ -541,9 +529,6 @@
     <t>Yoink%n💰🔊</t>
   </si>
   <si>
-    <t>Nab%n💰💰</t>
-  </si>
-  <si>
     <t>Root</t>
   </si>
   <si>
@@ -622,15 +607,9 @@
     <t>I CAN HEARTBLEED%nIf outdoors, may spend 💡 to 🔍</t>
   </si>
   <si>
-    <t>ADRENALINE%nGain 💡 on 👊%n %nYOU WILL REPORT IN%nWhen  👊, lower the noise level by 2. Do not change the ⚠ level.</t>
-  </si>
-  <si>
     <t>PICKER%nGain 💡 when you 🔓</t>
   </si>
   <si>
-    <t>ADRENALINE%nGain 💡 on 👊%n %nBRING IT ON%nGain 💡💡💡 if standing on a Reinforcements beacon when Reinforcements is triggered.</t>
-  </si>
-  <si>
     <t>EARLY WARNING%nWhen outdoors, may 🔍 once per turn%n %nMISDIRECT%nOnce per heist, may use 💡💡💡 to change the security roll by 1.</t>
   </si>
   <si>
@@ -778,9 +757,6 @@
     <t>🔓📷🔊➜</t>
   </si>
   <si>
-    <t>🔓👊📷🔊🔊⚠</t>
-  </si>
-  <si>
     <t>Disable</t>
   </si>
   <si>
@@ -805,9 +781,6 @@
     <t>👊💡➜</t>
   </si>
   <si>
-    <t>🔍🔓</t>
-  </si>
-  <si>
     <t>Kick</t>
   </si>
   <si>
@@ -835,9 +808,6 @@
     <t>💡💡🔊🔍</t>
   </si>
   <si>
-    <t>🔓👊📷🔊</t>
-  </si>
-  <si>
     <t>🔊🔊➜➜</t>
   </si>
   <si>
@@ -862,9 +832,6 @@
     <t>🔊🔊➜➜➜</t>
   </si>
   <si>
-    <t>🔓👊</t>
-  </si>
-  <si>
     <t>💡💡</t>
   </si>
   <si>
@@ -976,12 +943,6 @@
     <t>re-planning anyone</t>
   </si>
   <si>
-    <t>THERE ARE BETTER WAYS%nCannot 👊. May escape guards for 💡 each (Escape phase too)</t>
-  </si>
-  <si>
-    <t>THERE ARE BETTER WAYS%nCannot 👊. May escape guards for 💡 each (Escape phase too)%n %nINSPIRE%nOnce per turn, give a free💡 to a player of your choosing</t>
-  </si>
-  <si>
     <t>revealing</t>
   </si>
   <si>
@@ -1012,12 +973,6 @@
     <t>Exploit%n(see above)</t>
   </si>
   <si>
-    <t>I CAN HAZ TEH CODES?%nOnce per turn, may spend 💡💡💡 to re-position 1 planning token of any player.%n %nEXPLOIT%nUse this Action to enable another player to 👊🔊, 📷🔊 or 🔓🔊. Spend 💡 when you do this.</t>
-  </si>
-  <si>
-    <t>HAS THE CODE%nOnce per turn, may spend 💡💡 to re-position 1 planning token of any player%n %nEXPLOIT%nUse this Action to enable another player to 👊🔊, 📷🔊 or 🔓🔊. Spend 💡 when you do this.</t>
-  </si>
-  <si>
     <t>Good at</t>
   </si>
   <si>
@@ -1159,9 +1114,6 @@
     <t>Smash</t>
   </si>
   <si>
-    <t>📷📷➜</t>
-  </si>
-  <si>
     <t>Grab</t>
   </si>
   <si>
@@ -1183,9 +1135,6 @@
     <t>Multi-moves, Ideas, Camera</t>
   </si>
   <si>
-    <t>📷➜➜</t>
-  </si>
-  <si>
     <t>Wing It</t>
   </si>
   <si>
@@ -1255,10 +1204,58 @@
     <t>(extra quiet)</t>
   </si>
   <si>
-    <t>I CAN HAZ TEH CODES?%nOnce per turn, may spend 💡💡💡 to re-position 1 planning token of any player.%n %nREMOTE EXPLOIT%nUse this Action to enable another player to 👊, 📷, or 🔓. Spend 💡 when you do this.</t>
-  </si>
-  <si>
-    <t>Remote  Exploit%n(see above)</t>
+    <t>Run%n🔊🔊➜➜</t>
+  </si>
+  <si>
+    <t>🔓👊🔊</t>
+  </si>
+  <si>
+    <t>Spy Stuff%n🔓👊🔊</t>
+  </si>
+  <si>
+    <t>Pick%n🔓🔊</t>
+  </si>
+  <si>
+    <t>Key In%n🔍🔓🔊</t>
+  </si>
+  <si>
+    <t>THERE ARE BETTER WAYS%nCannot 👊. May escape guards for 💡 each (does not apply to Escape phase).</t>
+  </si>
+  <si>
+    <t>Inspire%n(see above)</t>
+  </si>
+  <si>
+    <t>THERE ARE BETTER WAYS%nCannot 👊. May escape guards for 💡 each (does not apply to Escape phase)%n %nINSPIRE%nUse this action to give a free💡💡  to a player of your choosing</t>
+  </si>
+  <si>
+    <t>🔓👊📷🔊🔊</t>
+  </si>
+  <si>
+    <t>🔓👊👊📷🔊⚠</t>
+  </si>
+  <si>
+    <t>📷🔊➜➜</t>
+  </si>
+  <si>
+    <t>📷📷🔊➜</t>
+  </si>
+  <si>
+    <t>🔍🔓🔊</t>
+  </si>
+  <si>
+    <t>ADRENALINE%nGain 💡 when you 👊</t>
+  </si>
+  <si>
+    <t>ADRENALINE%nGain 💡 when you 👊%n %nBRING IT ON%nGain 💡💡💡 when Reinforcements event occurs.</t>
+  </si>
+  <si>
+    <t>ADRENALINE%nGain 💡  when you 👊%n %nYOU WILL REPORT IN%nWhen  👊, lower the noise level by 2. Do not change the ⚠ level.</t>
+  </si>
+  <si>
+    <t>I CAN HAZ TEH CODES?%nOnce per turn, may spend 💡💡 to re-position 3 planning tokens of any one player%n %nEXPLOIT%nUse this Action and a 💡 to enable another player to 👊🔊, 📷🔊, or 🔓🔊</t>
+  </si>
+  <si>
+    <t>HAS THE CODE%nOnce per turn, may spend 💡💡 to re-position 4 planning tokens of any one player%n %nEXPLOIT%nUse this Action and a 💡 to enable another player to 👊🔊, 📷🔊, or 🔓🔊</t>
   </si>
 </sst>
 </file>
@@ -2196,7 +2193,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,19 +2230,19 @@
         <v>16</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G1" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="31" t="s">
-        <v>142</v>
-      </c>
       <c r="I1" s="32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K1" s="32" t="s">
         <v>123</v>
@@ -2259,7 +2256,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C2" s="11">
         <v>1</v>
@@ -2274,19 +2271,19 @@
         <v>3</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>166</v>
+        <v>394</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>81</v>
@@ -2297,7 +2294,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C3" s="11">
         <v>1</v>
@@ -2306,21 +2303,21 @@
         <v>2</v>
       </c>
       <c r="E3" s="11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="11">
         <v>5</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>166</v>
+        <v>394</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>81</v>
@@ -2328,10 +2325,10 @@
     </row>
     <row r="4" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C4" s="11">
         <v>1</v>
@@ -2340,21 +2337,21 @@
         <v>2</v>
       </c>
       <c r="E4" s="11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="11">
         <v>4</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>166</v>
+        <v>394</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>81</v>
@@ -2380,19 +2377,19 @@
         <v>3</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="J5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>129</v>
+        <v>404</v>
       </c>
       <c r="L5" s="20" t="s">
         <v>81</v>
@@ -2400,7 +2397,7 @@
     </row>
     <row r="6" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>25</v>
@@ -2418,15 +2415,15 @@
         <v>4</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20" t="s">
-        <v>199</v>
+        <v>405</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>81</v>
@@ -2452,15 +2449,15 @@
         <v>4</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>144</v>
+        <v>393</v>
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20" t="s">
-        <v>197</v>
+        <v>406</v>
       </c>
       <c r="L7" s="20" t="s">
         <v>81</v>
@@ -2486,10 +2483,10 @@
         <v>2</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>12</v>
@@ -2498,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>315</v>
+        <v>396</v>
       </c>
       <c r="L8" s="19" t="s">
         <v>81</v>
@@ -2524,15 +2521,15 @@
         <v>3</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19" t="s">
-        <v>315</v>
+        <v>396</v>
       </c>
       <c r="L9" s="19"/>
     </row>
@@ -2556,15 +2553,15 @@
         <v>3</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>162</v>
+        <v>397</v>
       </c>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
-        <v>316</v>
+        <v>398</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>81</v>
@@ -2590,10 +2587,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="I11" s="24" t="s">
         <v>4</v>
@@ -2602,7 +2599,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>327</v>
+        <v>407</v>
       </c>
       <c r="L11" s="22"/>
     </row>
@@ -2620,21 +2617,21 @@
         <v>2</v>
       </c>
       <c r="E12" s="25">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12" s="25">
         <v>6</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>325</v>
+        <v>391</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>409</v>
+        <v>313</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L12" s="22" t="s">
         <v>81</v>
@@ -2660,15 +2657,15 @@
         <v>6</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22" t="s">
-        <v>328</v>
+        <v>408</v>
       </c>
       <c r="L13" s="22" t="s">
         <v>81</v>
@@ -2694,10 +2691,10 @@
         <v>2</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>14</v>
@@ -2706,7 +2703,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="L14" s="21" t="s">
         <v>81</v>
@@ -2714,7 +2711,7 @@
     </row>
     <row r="15" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>14</v>
@@ -2726,19 +2723,19 @@
         <v>2</v>
       </c>
       <c r="E15" s="17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F15" s="17">
         <v>4</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L15" s="21" t="s">
         <v>81</v>
@@ -2764,15 +2761,15 @@
         <v>2</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
       <c r="K16" s="21" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L16" s="21" t="s">
         <v>81</v>
@@ -2780,10 +2777,10 @@
     </row>
     <row r="17" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C17" s="27">
         <v>1</v>
@@ -2798,19 +2795,19 @@
         <v>4</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>162</v>
+        <v>391</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="J17" s="26" t="s">
         <v>39</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L17" s="23" t="s">
         <v>81</v>
@@ -2818,10 +2815,10 @@
     </row>
     <row r="18" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C18" s="27">
         <v>1</v>
@@ -2836,13 +2833,13 @@
         <v>3</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>162</v>
+        <v>391</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="L18" s="23" t="s">
         <v>81</v>
@@ -2853,7 +2850,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C19" s="27">
         <v>1</v>
@@ -2868,13 +2865,13 @@
         <v>5</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>143</v>
+        <v>391</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>157</v>
+        <v>395</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="L19" s="23" t="s">
         <v>81</v>
@@ -2903,7 +2900,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X7" sqref="X7"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2961,43 +2958,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="96" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E1" s="101" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F1" s="97" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G1" s="114" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="H1" s="96" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="I1" s="101" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="J1" s="97" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="K1" s="114" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="L1" s="96" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="M1" s="101" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="N1" s="97" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="O1" s="114" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="P1" s="97" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="Q1" s="96">
         <v>1</v>
@@ -3021,16 +3018,16 @@
         <v>56</v>
       </c>
       <c r="X1" s="96" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y1" s="98" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z1" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="Y1" s="98" t="s">
+      <c r="AA1" s="98" t="s">
         <v>136</v>
-      </c>
-      <c r="Z1" s="96" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA1" s="98" t="s">
-        <v>137</v>
       </c>
       <c r="AB1" s="99" t="s">
         <v>107</v>
@@ -3054,19 +3051,19 @@
         <v>128</v>
       </c>
       <c r="AI1" s="100" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AJ1" s="95" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="AK1" s="95" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="AL1" s="95" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="AM1" s="95" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="AN1" s="149"/>
       <c r="AO1" s="149"/>
@@ -3100,42 +3097,42 @@
         <v>126</v>
       </c>
       <c r="E2" s="102" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F2" s="83" t="str">
         <f t="shared" ref="F2:F19" si="0">VLOOKUP(E2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G2" s="115" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="H2" s="41" t="str">
         <f t="shared" ref="H2:H19" si="1">VLOOKUP(G2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="I2" s="102" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J2" s="83" t="str">
         <f t="shared" ref="J2:J19" si="2">VLOOKUP(I2,Actions,2,FALSE)</f>
         <v>🔍</v>
       </c>
       <c r="K2" s="115" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="L2" s="41" t="str">
         <f t="shared" ref="L2:L19" si="3">VLOOKUP(K2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M2" s="102" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="N2" s="83" t="str">
         <f t="shared" ref="N2:N19" si="4">VLOOKUP(M2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O2" s="115" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="P2" s="83" t="str">
         <f t="shared" ref="P2:P19" si="5">VLOOKUP(O2,Actions,2,FALSE)</f>
@@ -3175,18 +3172,18 @@
         <v>Punch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nReveal%n🔍%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nGrab%n💰🔊</v>
       </c>
       <c r="X2" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="Y2" s="41" t="str">
         <f t="shared" ref="Y2:Y19" si="7">IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
         <v>Flip%n👊🔊➜%nDisable%n📷🔊➜%nStudy%n💡💡%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nRansack%n💰💰🔊</v>
       </c>
       <c r="Z2" s="40" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="AA2" s="43" t="str">
         <f t="shared" ref="AA2:AA19" si="8">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
-        <v>Punch%n👊🔊🔊➜%nUnplug%n📷📷➜%nKey In%n🔍🔓%nFlip%n👊🔊➜%nDisable%n📷🔊➜%nGrab%n💰🔊</v>
+        <v>Punch%n👊🔊🔊➜%nUnplug%n📷📷🔊➜%nKey In%n🔍🔓🔊%nFlip%n👊🔊➜%nDisable%n📷🔊➜%nGrab%n💰🔊</v>
       </c>
       <c r="AB2" s="40">
         <f>(LEN($W2)-LEN(SUBSTITUTE($W2,AB$1,"")))/LEN(AB$1)</f>
@@ -3221,16 +3218,16 @@
         <v>1</v>
       </c>
       <c r="AJ2" s="39" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="AK2" s="39" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="AL2" s="39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AM2" s="39" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="AN2" s="151"/>
       <c r="AO2" s="151"/>
@@ -3264,42 +3261,42 @@
         <v>127</v>
       </c>
       <c r="E3" s="104" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F3" s="85" t="str">
         <f t="shared" si="0"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G3" s="117" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="H3" s="36" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I3" s="105" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="J3" s="85" t="str">
         <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K3" s="123" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="L3" s="36" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M3" s="105" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="N3" s="85" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O3" s="117" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="P3" s="85" t="str">
         <f t="shared" si="5"/>
@@ -3345,7 +3342,7 @@
       </c>
       <c r="AA3" s="35" t="str">
         <f t="shared" si="8"/>
-        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSneak%n📷➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSneak%n📷🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="AB3" s="40">
         <f t="shared" ref="AB3:AI19" si="16">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
@@ -3380,16 +3377,16 @@
         <v>0</v>
       </c>
       <c r="AJ3" s="33" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="AK3" s="33" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="AL3" s="33" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="AM3" s="33" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="AN3" s="151"/>
       <c r="AO3" s="151"/>
@@ -3411,7 +3408,7 @@
     </row>
     <row r="4" spans="1:56" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="B4" s="50">
         <v>2</v>
@@ -3420,45 +3417,45 @@
         <v>1</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="E4" s="106" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F4" s="87" t="str">
         <f t="shared" si="0"/>
         <v>🔍</v>
       </c>
       <c r="G4" s="118" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="H4" s="51" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊</v>
       </c>
       <c r="I4" s="107" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="J4" s="87" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊</v>
       </c>
       <c r="K4" s="125" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="L4" s="51" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊</v>
       </c>
       <c r="M4" s="107" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="N4" s="87" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O4" s="118" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="P4" s="87" t="str">
         <f t="shared" si="5"/>
@@ -3493,18 +3490,18 @@
         <v>Reveal%n🔍%nStrongarm%n🔓👊🔊🔊%nShort%n🔓📷🔊🔊%nZap%n👊📷🔊🔊%nGrab%n💰🔊%nRun%n🔊🔊➜➜</v>
       </c>
       <c r="X4" s="50" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="Y4" s="51" t="str">
         <f t="shared" si="7"/>
-        <v>Study%n💡💡%nSpy Stuff%n🔓👊%nShort%n🔓📷🔊🔊%nZap%n👊📷🔊🔊%nGrab%n💰🔊%nDash%n🔊➜➜</v>
+        <v>Study%n💡💡%nSpy Stuff%n🔓👊🔊%nShort%n🔓📷🔊🔊%nZap%n👊📷🔊🔊%nGrab%n💰🔊%nDash%n🔊➜➜</v>
       </c>
       <c r="Z4" s="50" t="s">
         <v>125</v>
       </c>
       <c r="AA4" s="53" t="str">
         <f t="shared" si="8"/>
-        <v>Redirect%n🔓👊📷🔊%nStrongarm%n🔓👊🔊🔊%nShort%n🔓📷🔊🔊%nShock%n👊📷%nGrab%n💰🔊%nDash%n🔊➜➜</v>
+        <v>Redirect%n🔓👊📷🔊🔊%nStrongarm%n🔓👊🔊🔊%nShort%n🔓📷🔊🔊%nShock%n👊📷%nGrab%n💰🔊%nDash%n🔊➜➜</v>
       </c>
       <c r="AB4" s="40">
         <f t="shared" si="16"/>
@@ -3539,16 +3536,16 @@
         <v>1</v>
       </c>
       <c r="AJ4" s="54" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="AK4" s="54" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AL4" s="54" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="AM4" s="54" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="AN4" s="151"/>
       <c r="AO4" s="151"/>
@@ -3570,7 +3567,7 @@
     </row>
     <row r="5" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="B5" s="61">
         <v>2</v>
@@ -3579,45 +3576,45 @@
         <v>1</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E5" s="108" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="F5" s="89" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊</v>
       </c>
       <c r="G5" s="119" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H5" s="62" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I5" s="109" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="J5" s="89" t="str">
         <f t="shared" si="2"/>
         <v>👊👊🔊</v>
       </c>
       <c r="K5" s="127" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="L5" s="62" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M5" s="109" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="N5" s="89" t="str">
         <f t="shared" si="4"/>
         <v>👊🔊</v>
       </c>
       <c r="O5" s="119" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="P5" s="89" t="str">
         <f t="shared" si="5"/>
@@ -3659,11 +3656,11 @@
         <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nRampage%n👊👊🔊🔊➜➜%nRun%n🔊🔊➜➜%nStrongarm%n🔓👊🔊🔊%nStudy%n💡💡</v>
       </c>
       <c r="Z5" s="61" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="AA5" s="63" t="str">
         <f t="shared" si="8"/>
-        <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nDetonate%n🔓👊📷🔊🔊⚠%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nStudy%n💡💡</v>
+        <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nDetonate%n🔓👊👊📷🔊⚠%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nStudy%n💡💡</v>
       </c>
       <c r="AB5" s="40">
         <f t="shared" si="16"/>
@@ -3698,16 +3695,16 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="64" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="AK5" s="64" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="AL5" s="64" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AM5" s="64" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="AN5" s="151"/>
       <c r="AO5" s="151"/>
@@ -3729,7 +3726,7 @@
     </row>
     <row r="6" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="70">
         <v>2</v>
@@ -3738,45 +3735,45 @@
         <v>1</v>
       </c>
       <c r="D6" s="71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="110" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="F6" s="91" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="G6" s="120" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="H6" s="71" t="str">
         <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I6" s="111" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="J6" s="91" t="str">
         <f t="shared" si="2"/>
         <v>🔓🔊</v>
       </c>
       <c r="K6" s="128" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="L6" s="71" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M6" s="111" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="N6" s="91" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="O6" s="120" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="P6" s="91" t="str">
         <f t="shared" si="5"/>
@@ -3811,18 +3808,18 @@
         <v>Bump%n🔓🔓🔊🔊➜%nStudy%n💡💡%nShim%n🔓🔊%nSprint%n🔊🔊➜➜➜%nRun%n🔊🔊➜➜%nShim%n🔓🔊</v>
       </c>
       <c r="X6" s="72" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="Y6" s="71" t="str">
         <f t="shared" si="7"/>
         <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShim%n🔓🔊</v>
       </c>
       <c r="Z6" s="72" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA6" s="73" t="str">
         <f t="shared" si="8"/>
-        <v>Rake%n🔓🔓🔊➜%nStudy%n💡💡%nSpy Stuff%n🔓👊%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShort%n🔓📷🔊🔊</v>
+        <v>Rake%n🔓🔓🔊➜%nStudy%n💡💡%nSpy Stuff%n🔓👊🔊%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShort%n🔓📷🔊🔊</v>
       </c>
       <c r="AB6" s="40">
         <f t="shared" si="16"/>
@@ -3857,16 +3854,16 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="74" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="AK6" s="74" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="AL6" s="74" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AM6" s="74" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="AN6" s="151"/>
       <c r="AO6" s="151"/>
@@ -3900,42 +3897,42 @@
         <v>59</v>
       </c>
       <c r="E7" s="133" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="F7" s="134" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊🔊➜</v>
       </c>
       <c r="G7" s="135" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="H7" s="132" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I7" s="136" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="J7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="K7" s="137" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="L7" s="132" t="str">
         <f t="shared" si="3"/>
         <v>🔍</v>
       </c>
       <c r="M7" s="136" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="N7" s="134" t="str">
         <f t="shared" si="4"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="O7" s="135" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="P7" s="134" t="str">
         <f t="shared" si="5"/>
@@ -3974,14 +3971,14 @@
       </c>
       <c r="Y7" s="132" t="str">
         <f t="shared" si="7"/>
-        <v>Unplug%n📷📷➜%nSprint%n🔊🔊➜➜➜%nDisable%n📷🔊➜%nDiscover%n🔍🔍%nRecon%n💡💡🔊🔍%nDisable%n📷🔊➜</v>
+        <v>Unplug%n📷📷🔊➜%nSprint%n🔊🔊➜➜➜%nDisable%n📷🔊➜%nDiscover%n🔍🔍%nRecon%n💡💡🔊🔍%nDisable%n📷🔊➜</v>
       </c>
       <c r="Z7" s="138" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="AA7" s="139" t="str">
         <f t="shared" si="8"/>
-        <v>Unplug%n📷📷➜%nDash%n🔊➜➜%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
+        <v>Unplug%n📷📷🔊➜%nDash%n🔊➜➜%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
       </c>
       <c r="AB7" s="40">
         <f t="shared" si="16"/>
@@ -4016,16 +4013,16 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="140" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="AK7" s="140" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="AL7" s="140" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="AM7" s="140" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="AN7" s="152"/>
       <c r="AO7" s="152"/>
@@ -4047,7 +4044,7 @@
     </row>
     <row r="8" spans="1:56" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B8" s="42">
         <v>2</v>
@@ -4059,42 +4056,42 @@
         <v>126</v>
       </c>
       <c r="E8" s="103" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="F8" s="84" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊➜</v>
       </c>
       <c r="G8" s="116" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H8" s="43" t="str">
         <f t="shared" si="1"/>
         <v>📷🔊➜</v>
       </c>
       <c r="I8" s="103" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="J8" s="84" t="str">
         <f t="shared" si="2"/>
         <v>💡💡</v>
       </c>
       <c r="K8" s="116" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="L8" s="43" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M8" s="103" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="N8" s="84" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O8" s="116" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="P8" s="84" t="str">
         <f t="shared" si="5"/>
@@ -4129,14 +4126,14 @@
         <v>Flip%n👊🔊➜%nDisable%n📷🔊➜%nStudy%n💡💡%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nRansack%n💰💰🔊</v>
       </c>
       <c r="X8" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y8" s="45" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z8" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA8" s="43" t="str">
         <f t="shared" si="8"/>
@@ -4175,16 +4172,16 @@
         <v>2</v>
       </c>
       <c r="AJ8" s="146" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="AK8" s="146" t="s">
+        <v>357</v>
+      </c>
+      <c r="AL8" s="146" t="s">
         <v>372</v>
       </c>
-      <c r="AL8" s="146" t="s">
-        <v>389</v>
-      </c>
       <c r="AM8" s="146" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="AN8" s="151"/>
       <c r="AO8" s="151"/>
@@ -4206,7 +4203,7 @@
     </row>
     <row r="9" spans="1:56" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="B9" s="47">
         <v>2</v>
@@ -4218,42 +4215,42 @@
         <v>126</v>
       </c>
       <c r="E9" s="103" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F9" s="84" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G9" s="116" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="H9" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>📷📷➜</v>
+        <v>📷📷🔊➜</v>
       </c>
       <c r="I9" s="103" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="J9" s="84" t="str">
         <f t="shared" si="2"/>
-        <v>🔍🔓</v>
+        <v>🔍🔓🔊</v>
       </c>
       <c r="K9" s="116" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="L9" s="43" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊➜</v>
       </c>
       <c r="M9" s="103" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="N9" s="84" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊➜</v>
       </c>
       <c r="O9" s="116" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="P9" s="84" t="str">
         <f t="shared" si="5"/>
@@ -4265,11 +4262,11 @@
       </c>
       <c r="R9" s="47" t="str">
         <f t="shared" si="11"/>
-        <v>Unplug%n📷📷➜</v>
+        <v>Unplug%n📷📷🔊➜</v>
       </c>
       <c r="S9" s="47" t="str">
         <f t="shared" si="12"/>
-        <v>Key In%n🔍🔓</v>
+        <v>Key In%n🔍🔓🔊</v>
       </c>
       <c r="T9" s="48" t="str">
         <f t="shared" si="13"/>
@@ -4285,17 +4282,17 @@
       </c>
       <c r="W9" s="44" t="str">
         <f t="shared" si="6"/>
-        <v>Punch%n👊🔊🔊➜%nUnplug%n📷📷➜%nKey In%n🔍🔓%nFlip%n👊🔊➜%nDisable%n📷🔊➜%nGrab%n💰🔊</v>
+        <v>Punch%n👊🔊🔊➜%nUnplug%n📷📷🔊➜%nKey In%n🔍🔓🔊%nFlip%n👊🔊➜%nDisable%n📷🔊➜%nGrab%n💰🔊</v>
       </c>
       <c r="X9" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y9" s="44" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z9" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA9" s="43" t="str">
         <f t="shared" si="8"/>
@@ -4307,7 +4304,7 @@
       </c>
       <c r="AC9" s="40">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD9" s="40">
         <f t="shared" si="9"/>
@@ -4334,16 +4331,16 @@
         <v>1</v>
       </c>
       <c r="AJ9" s="46" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="AK9" s="46" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="AL9" s="46" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="AM9" s="46" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="AN9" s="152"/>
       <c r="AO9" s="152"/>
@@ -4377,42 +4374,42 @@
         <v>127</v>
       </c>
       <c r="E10" s="105" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F10" s="86" t="str">
         <f t="shared" si="0"/>
         <v>🔊➜➜</v>
       </c>
       <c r="G10" s="117" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="H10" s="34" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I10" s="105" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="J10" s="86" t="str">
         <f t="shared" si="2"/>
         <v>👊➜</v>
       </c>
       <c r="K10" s="117" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="L10" s="34" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M10" s="105" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="N10" s="86" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O10" s="117" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="P10" s="86" t="str">
         <f t="shared" si="5"/>
@@ -4447,14 +4444,14 @@
         <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="X10" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y10" s="35" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z10" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA10" s="35" t="str">
         <f t="shared" si="8"/>
@@ -4493,16 +4490,16 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="148" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="AK10" s="148" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="AL10" s="148" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="AM10" s="148" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="AN10" s="152"/>
       <c r="AO10" s="152"/>
@@ -4536,42 +4533,42 @@
         <v>127</v>
       </c>
       <c r="E11" s="105" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F11" s="86" t="str">
         <f t="shared" si="0"/>
         <v>🔊➜➜</v>
       </c>
       <c r="G11" s="117" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="H11" s="35" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I11" s="105" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="J11" s="86" t="str">
         <f t="shared" si="2"/>
-        <v>📷➜➜</v>
+        <v>📷🔊➜➜</v>
       </c>
       <c r="K11" s="124" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="L11" s="35" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M11" s="105" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="N11" s="86" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O11" s="117" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="P11" s="86" t="str">
         <f t="shared" si="5"/>
@@ -4587,7 +4584,7 @@
       </c>
       <c r="S11" s="37" t="str">
         <f t="shared" si="12"/>
-        <v>Sneak%n📷➜➜</v>
+        <v>Sneak%n📷🔊➜➜</v>
       </c>
       <c r="T11" s="38" t="str">
         <f t="shared" si="13"/>
@@ -4603,17 +4600,17 @@
       </c>
       <c r="W11" s="35" t="str">
         <f t="shared" si="6"/>
-        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSneak%n📷➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSneak%n📷🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="X11" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y11" s="35" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z11" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA11" s="35" t="str">
         <f t="shared" si="8"/>
@@ -4625,7 +4622,7 @@
       </c>
       <c r="AC11" s="40">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AD11" s="40">
         <f t="shared" si="9"/>
@@ -4652,16 +4649,16 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="148" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="AK11" s="147" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="AL11" s="147" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="AM11" s="147" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="AN11" s="151"/>
       <c r="AO11" s="151"/>
@@ -4683,7 +4680,7 @@
     </row>
     <row r="12" spans="1:56" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B12" s="52">
         <v>2</v>
@@ -4692,45 +4689,45 @@
         <v>2</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="E12" s="107" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F12" s="88" t="str">
         <f t="shared" si="0"/>
         <v>💡💡</v>
       </c>
       <c r="G12" s="118" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="H12" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>🔓👊</v>
+        <v>🔓👊🔊</v>
       </c>
       <c r="I12" s="107" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="J12" s="88" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊</v>
       </c>
       <c r="K12" s="118" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="L12" s="53" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊</v>
       </c>
       <c r="M12" s="107" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="N12" s="88" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O12" s="118" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="P12" s="88" t="str">
         <f t="shared" si="5"/>
@@ -4742,7 +4739,7 @@
       </c>
       <c r="R12" s="52" t="str">
         <f t="shared" si="11"/>
-        <v>Spy Stuff%n🔓👊</v>
+        <v>Spy Stuff%n🔓👊🔊</v>
       </c>
       <c r="S12" s="50" t="str">
         <f t="shared" si="12"/>
@@ -4762,17 +4759,17 @@
       </c>
       <c r="W12" s="56" t="str">
         <f t="shared" si="6"/>
-        <v>Study%n💡💡%nSpy Stuff%n🔓👊%nShort%n🔓📷🔊🔊%nZap%n👊📷🔊🔊%nGrab%n💰🔊%nDash%n🔊➜➜</v>
+        <v>Study%n💡💡%nSpy Stuff%n🔓👊🔊%nShort%n🔓📷🔊🔊%nZap%n👊📷🔊🔊%nGrab%n💰🔊%nDash%n🔊➜➜</v>
       </c>
       <c r="X12" s="52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y12" s="57" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z12" s="52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA12" s="56" t="str">
         <f t="shared" si="8"/>
@@ -4784,7 +4781,7 @@
       </c>
       <c r="AC12" s="40">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD12" s="40">
         <f t="shared" si="9"/>
@@ -4811,16 +4808,16 @@
         <v>1</v>
       </c>
       <c r="AJ12" s="54" t="s">
-        <v>386</v>
+        <v>369</v>
       </c>
       <c r="AK12" s="54" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="AL12" s="54" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="AM12" s="54" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="AN12" s="151"/>
       <c r="AO12" s="151"/>
@@ -4851,45 +4848,45 @@
         <v>2</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="E13" s="107" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="F13" s="88" t="str">
         <f t="shared" si="0"/>
-        <v>🔓👊📷🔊</v>
+        <v>🔓👊📷🔊🔊</v>
       </c>
       <c r="G13" s="118" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="H13" s="56" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊</v>
       </c>
       <c r="I13" s="107" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="J13" s="88" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊</v>
       </c>
       <c r="K13" s="126" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
       <c r="L13" s="56" t="str">
         <f t="shared" si="3"/>
         <v>👊📷</v>
       </c>
       <c r="M13" s="107" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="N13" s="88" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O13" s="118" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="P13" s="88" t="str">
         <f t="shared" si="5"/>
@@ -4897,7 +4894,7 @@
       </c>
       <c r="Q13" s="60" t="str">
         <f t="shared" si="10"/>
-        <v>Redirect%n🔓👊📷🔊</v>
+        <v>Redirect%n🔓👊📷🔊🔊</v>
       </c>
       <c r="R13" s="59" t="str">
         <f t="shared" si="11"/>
@@ -4921,17 +4918,17 @@
       </c>
       <c r="W13" s="56" t="str">
         <f t="shared" si="6"/>
-        <v>Redirect%n🔓👊📷🔊%nStrongarm%n🔓👊🔊🔊%nShort%n🔓📷🔊🔊%nShock%n👊📷%nGrab%n💰🔊%nDash%n🔊➜➜</v>
+        <v>Redirect%n🔓👊📷🔊🔊%nStrongarm%n🔓👊🔊🔊%nShort%n🔓📷🔊🔊%nShock%n👊📷%nGrab%n💰🔊%nDash%n🔊➜➜</v>
       </c>
       <c r="X13" s="59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y13" s="57" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z13" s="59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA13" s="56" t="str">
         <f t="shared" si="8"/>
@@ -4943,7 +4940,7 @@
       </c>
       <c r="AC13" s="40">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD13" s="40">
         <f t="shared" si="9"/>
@@ -4970,16 +4967,16 @@
         <v>1</v>
       </c>
       <c r="AJ13" s="54" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="AK13" s="54" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="AL13" s="54" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="AM13" s="54" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="AN13" s="151"/>
       <c r="AO13" s="151"/>
@@ -5010,45 +5007,45 @@
         <v>2</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E14" s="109" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F14" s="90" t="str">
         <f t="shared" si="0"/>
         <v>👊👊🔊</v>
       </c>
       <c r="G14" s="119" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H14" s="63" t="str">
         <f t="shared" si="1"/>
         <v>🔊➜➜</v>
       </c>
       <c r="I14" s="109" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="J14" s="90" t="str">
         <f t="shared" si="2"/>
         <v>👊👊🔊🔊➜➜</v>
       </c>
       <c r="K14" s="119" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="L14" s="63" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M14" s="109" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="N14" s="90" t="str">
         <f t="shared" si="4"/>
         <v>🔓👊🔊🔊</v>
       </c>
       <c r="O14" s="119" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="P14" s="90" t="str">
         <f t="shared" si="5"/>
@@ -5083,14 +5080,14 @@
         <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nRampage%n👊👊🔊🔊➜➜%nRun%n🔊🔊➜➜%nStrongarm%n🔓👊🔊🔊%nStudy%n💡💡</v>
       </c>
       <c r="X14" s="66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y14" s="63" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z14" s="66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA14" s="63" t="str">
         <f t="shared" si="8"/>
@@ -5129,16 +5126,16 @@
         <v>0</v>
       </c>
       <c r="AJ14" s="64" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="AK14" s="64" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="AL14" s="64" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="AM14" s="64" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="AN14" s="151"/>
       <c r="AO14" s="151"/>
@@ -5160,7 +5157,7 @@
     </row>
     <row r="15" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="B15" s="66">
         <v>2</v>
@@ -5169,45 +5166,45 @@
         <v>2</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E15" s="109" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F15" s="90" t="str">
         <f t="shared" si="0"/>
         <v>👊👊🔊</v>
       </c>
       <c r="G15" s="119" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H15" s="63" t="str">
         <f t="shared" si="1"/>
         <v>🔊➜➜</v>
       </c>
       <c r="I15" s="109" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="J15" s="90" t="str">
-        <f t="shared" si="2"/>
-        <v>🔓👊📷🔊🔊⚠</v>
+        <f>VLOOKUP(I15,Actions,2,FALSE)</f>
+        <v>🔓👊👊📷🔊⚠</v>
       </c>
       <c r="K15" s="119" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="L15" s="63" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M15" s="109" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="N15" s="90" t="str">
         <f t="shared" si="4"/>
         <v>👊👊🔊</v>
       </c>
       <c r="O15" s="119" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="P15" s="90" t="str">
         <f t="shared" si="5"/>
@@ -5223,7 +5220,7 @@
       </c>
       <c r="S15" s="66" t="str">
         <f t="shared" si="12"/>
-        <v>Detonate%n🔓👊📷🔊🔊⚠</v>
+        <v>Detonate%n🔓👊👊📷🔊⚠</v>
       </c>
       <c r="T15" s="66" t="str">
         <f t="shared" si="13"/>
@@ -5239,17 +5236,17 @@
       </c>
       <c r="W15" s="68" t="str">
         <f t="shared" si="6"/>
-        <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nDetonate%n🔓👊📷🔊🔊⚠%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nStudy%n💡💡</v>
+        <v>Bash%n👊👊🔊%nDash%n🔊➜➜%nDetonate%n🔓👊👊📷🔊⚠%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nStudy%n💡💡</v>
       </c>
       <c r="X15" s="66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y15" s="63" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z15" s="66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA15" s="63" t="str">
         <f t="shared" si="8"/>
@@ -5261,7 +5258,7 @@
       </c>
       <c r="AC15" s="40">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AD15" s="40">
         <f t="shared" si="9"/>
@@ -5273,7 +5270,7 @@
       </c>
       <c r="AF15" s="40">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AG15" s="40">
         <f t="shared" si="9"/>
@@ -5288,14 +5285,14 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="64" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="AK15" s="64"/>
       <c r="AL15" s="64" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="AM15" s="64" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="AN15" s="151"/>
       <c r="AO15" s="151"/>
@@ -5317,7 +5314,7 @@
     </row>
     <row r="16" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="B16" s="76">
         <v>2</v>
@@ -5326,45 +5323,45 @@
         <v>2</v>
       </c>
       <c r="D16" s="77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E16" s="110" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F16" s="91" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G16" s="120" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H16" s="77" t="str">
         <f t="shared" si="1"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="I16" s="111" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
       <c r="J16" s="91" t="str">
         <f t="shared" si="2"/>
         <v>🔓💰</v>
       </c>
       <c r="K16" s="129" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="L16" s="77" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M16" s="111" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="N16" s="91" t="str">
         <f t="shared" si="4"/>
         <v>🔊➜➜</v>
       </c>
       <c r="O16" s="120" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="P16" s="91" t="str">
         <f t="shared" si="5"/>
@@ -5399,14 +5396,14 @@
         <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShim%n🔓🔊</v>
       </c>
       <c r="X16" s="72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y16" s="77" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z16" s="72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA16" s="78" t="str">
         <f t="shared" si="8"/>
@@ -5445,16 +5442,16 @@
         <v>1</v>
       </c>
       <c r="AJ16" s="74" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="AK16" s="74" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="AL16" s="74" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="AM16" s="74" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="AN16" s="151"/>
       <c r="AO16" s="151"/>
@@ -5476,7 +5473,7 @@
     </row>
     <row r="17" spans="1:56" s="140" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="72">
         <v>2</v>
@@ -5485,45 +5482,45 @@
         <v>2</v>
       </c>
       <c r="D17" s="73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E17" s="111" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F17" s="92" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G17" s="120" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="H17" s="73" t="str">
         <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I17" s="111" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="J17" s="92" t="str">
         <f t="shared" si="2"/>
-        <v>🔓👊</v>
+        <v>🔓👊🔊</v>
       </c>
       <c r="K17" s="120" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="L17" s="73" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M17" s="111" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="N17" s="92" t="str">
         <f t="shared" si="4"/>
         <v>🔊➜➜</v>
       </c>
       <c r="O17" s="120" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="P17" s="92" t="str">
         <f t="shared" si="5"/>
@@ -5539,7 +5536,7 @@
       </c>
       <c r="S17" s="70" t="str">
         <f t="shared" si="12"/>
-        <v>Spy Stuff%n🔓👊</v>
+        <v>Spy Stuff%n🔓👊🔊</v>
       </c>
       <c r="T17" s="70" t="str">
         <f t="shared" si="13"/>
@@ -5555,17 +5552,17 @@
       </c>
       <c r="W17" s="78" t="str">
         <f t="shared" si="6"/>
-        <v>Rake%n🔓🔓🔊➜%nStudy%n💡💡%nSpy Stuff%n🔓👊%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShort%n🔓📷🔊🔊</v>
+        <v>Rake%n🔓🔓🔊➜%nStudy%n💡💡%nSpy Stuff%n🔓👊🔊%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShort%n🔓📷🔊🔊</v>
       </c>
       <c r="X17" s="72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y17" s="73" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z17" s="72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA17" s="73" t="str">
         <f t="shared" si="8"/>
@@ -5577,12 +5574,12 @@
       </c>
       <c r="AC17" s="40">
         <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="AD17" s="40">
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="AD17" s="40">
-        <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
       <c r="AE17" s="40">
         <f t="shared" si="9"/>
         <v>1</v>
@@ -5604,16 +5601,16 @@
         <v>0</v>
       </c>
       <c r="AJ17" s="74" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="AK17" s="74" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="AL17" s="74" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="AM17" s="74" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="AN17" s="152"/>
       <c r="AO17" s="152"/>
@@ -5647,42 +5644,42 @@
         <v>59</v>
       </c>
       <c r="E18" s="136" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="F18" s="141" t="str">
         <f t="shared" si="0"/>
-        <v>📷📷➜</v>
+        <v>📷📷🔊➜</v>
       </c>
       <c r="G18" s="135" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="H18" s="139" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I18" s="136" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="J18" s="141" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K18" s="135" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="L18" s="139" t="str">
         <f t="shared" si="3"/>
         <v>🔍🔍</v>
       </c>
       <c r="M18" s="136" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="N18" s="141" t="str">
         <f t="shared" si="4"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="O18" s="135" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="P18" s="141" t="str">
         <f t="shared" si="5"/>
@@ -5690,7 +5687,7 @@
       </c>
       <c r="Q18" s="131" t="str">
         <f t="shared" si="10"/>
-        <v>Unplug%n📷📷➜</v>
+        <v>Unplug%n📷📷🔊➜</v>
       </c>
       <c r="R18" s="131" t="str">
         <f t="shared" si="11"/>
@@ -5714,17 +5711,17 @@
       </c>
       <c r="W18" s="142" t="str">
         <f t="shared" si="6"/>
-        <v>Unplug%n📷📷➜%nSprint%n🔊🔊➜➜➜%nDisable%n📷🔊➜%nDiscover%n🔍🔍%nRecon%n💡💡🔊🔍%nDisable%n📷🔊➜</v>
+        <v>Unplug%n📷📷🔊➜%nSprint%n🔊🔊➜➜➜%nDisable%n📷🔊➜%nDiscover%n🔍🔍%nRecon%n💡💡🔊🔍%nDisable%n📷🔊➜</v>
       </c>
       <c r="X18" s="138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y18" s="143" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z18" s="138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA18" s="142" t="str">
         <f t="shared" si="8"/>
@@ -5736,7 +5733,7 @@
       </c>
       <c r="AC18" s="40">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AD18" s="40">
         <f t="shared" si="16"/>
@@ -5763,13 +5760,13 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="140" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="AK18" s="140" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="AM18" s="140" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="AN18" s="152"/>
       <c r="AO18" s="152"/>
@@ -5791,7 +5788,7 @@
     </row>
     <row r="19" spans="1:56" s="140" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="139" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B19" s="138">
         <v>2</v>
@@ -5803,42 +5800,42 @@
         <v>59</v>
       </c>
       <c r="E19" s="136" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="F19" s="141" t="str">
         <f t="shared" si="0"/>
-        <v>📷📷➜</v>
+        <v>📷📷🔊➜</v>
       </c>
       <c r="G19" s="135" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H19" s="139" t="str">
         <f t="shared" si="1"/>
         <v>🔊➜➜</v>
       </c>
       <c r="I19" s="136" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="J19" s="141" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K19" s="135" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="L19" s="139" t="str">
         <f t="shared" si="3"/>
         <v>🔊➜🔍</v>
       </c>
       <c r="M19" s="136" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="N19" s="141" t="str">
         <f t="shared" si="4"/>
         <v>💡💡</v>
       </c>
       <c r="O19" s="135" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="P19" s="141" t="str">
         <f t="shared" si="5"/>
@@ -5846,7 +5843,7 @@
       </c>
       <c r="Q19" s="145" t="str">
         <f t="shared" si="10"/>
-        <v>Unplug%n📷📷➜</v>
+        <v>Unplug%n📷📷🔊➜</v>
       </c>
       <c r="R19" s="131" t="str">
         <f t="shared" si="11"/>
@@ -5870,17 +5867,17 @@
       </c>
       <c r="W19" s="142" t="str">
         <f t="shared" si="6"/>
-        <v>Unplug%n📷📷➜%nDash%n🔊➜➜%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
+        <v>Unplug%n📷📷🔊➜%nDash%n🔊➜➜%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
       </c>
       <c r="X19" s="138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y19" s="139" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z19" s="138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA19" s="139" t="str">
         <f t="shared" si="8"/>
@@ -5892,7 +5889,7 @@
       </c>
       <c r="AC19" s="40">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD19" s="40">
         <f t="shared" si="16"/>
@@ -5919,16 +5916,16 @@
         <v>0</v>
       </c>
       <c r="AJ19" s="140" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="AK19" s="140" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="AL19" s="140" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="AM19" s="140" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="AN19" s="152"/>
       <c r="AO19" s="152"/>
@@ -6049,7 +6046,7 @@
         <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6057,7 +6054,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -6066,7 +6063,7 @@
         <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -6075,7 +6072,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -6084,7 +6081,7 @@
         <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6092,15 +6089,15 @@
         <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6108,7 +6105,7 @@
         <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6116,7 +6113,7 @@
         <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -6128,8 +6125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6143,48 +6140,48 @@
   <sheetData>
     <row r="1" spans="1:12" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="80" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="80" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" s="80" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" s="80" t="s">
+        <v>205</v>
+      </c>
+      <c r="J1" s="80" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="69" t="s">
-        <v>287</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>207</v>
-      </c>
-      <c r="E1" s="80" t="s">
-        <v>208</v>
-      </c>
-      <c r="F1" s="80" t="s">
-        <v>209</v>
-      </c>
-      <c r="G1" s="80" t="s">
-        <v>210</v>
-      </c>
-      <c r="H1" s="80" t="s">
-        <v>211</v>
-      </c>
-      <c r="I1" s="80" t="s">
-        <v>212</v>
-      </c>
-      <c r="J1" s="80" t="s">
-        <v>213</v>
-      </c>
       <c r="K1" s="69" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="L1" s="69" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E2" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6213,13 +6210,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E3" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6248,32 +6245,32 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>376</v>
+        <v>402</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="B6" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="C6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E6" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6302,13 +6299,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E7" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6337,13 +6334,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B8" t="s">
-        <v>249</v>
+        <v>400</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E8" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6372,13 +6369,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>268</v>
+        <v>399</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E9" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6407,13 +6404,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="B10" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E10" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6442,24 +6439,24 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="B11" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="B12" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E12" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6488,24 +6485,24 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
       <c r="B13" t="s">
-        <v>387</v>
+        <v>370</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B14" t="s">
-        <v>277</v>
+        <v>392</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E14" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6534,21 +6531,21 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
       <c r="B15" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B16" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E16" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6577,13 +6574,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B17" t="s">
         <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E17" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6612,13 +6609,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E18" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6647,13 +6644,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B19" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E19" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6682,13 +6679,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="B20" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="C20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E20" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6717,13 +6714,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="B21" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E21" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6752,7 +6749,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B22" t="s">
         <v>103</v>
@@ -6787,10 +6784,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B23" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -6822,10 +6819,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
@@ -6857,10 +6854,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B25" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -6892,10 +6889,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B26" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
@@ -6927,10 +6924,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
@@ -6962,13 +6959,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B28" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C28" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E28" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -6997,13 +6994,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B29" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C29" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E29" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7032,13 +7029,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="B30" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="C30" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E30" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7067,13 +7064,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
         <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E31" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7102,13 +7099,13 @@
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B32" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C32" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E32" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7137,13 +7134,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B33" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C33" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E33" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7172,13 +7169,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B34" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C34" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E34" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7207,21 +7204,21 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="B35" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B36" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C36" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E36" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7250,13 +7247,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B37" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C37" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E37" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7285,13 +7282,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B38" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C38" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E38" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7320,13 +7317,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="B39" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E39" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7355,24 +7352,24 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="B40" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C40" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B41" t="s">
         <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E41" s="81">
         <f>COUNTIF(Skills!Q:Q,#REF!)</f>
@@ -7401,10 +7398,10 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B42" t="s">
-        <v>258</v>
+        <v>403</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -7436,10 +7433,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>316</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -7471,10 +7468,10 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="B44" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
@@ -7506,18 +7503,18 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B45" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B46" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="C46" t="s">
         <v>23</v>
@@ -8932,7 +8929,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="69" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -8942,7 +8939,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -8957,17 +8954,17 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="55" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="55" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="65" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -8982,7 +8979,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="75" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -8992,17 +8989,17 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="144" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="69" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" ref="B48:B55" si="0">VLOOKUP(A48,Actions,2,FALSE)</f>
@@ -9011,7 +9008,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
@@ -9020,16 +9017,16 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
-        <v>🔓👊📷🔊🔊⚠</v>
+        <v>🔓👊👊📷🔊⚠</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -9038,7 +9035,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
@@ -9047,7 +9044,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B53" t="e">
         <f t="shared" si="0"/>
@@ -9056,7 +9053,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
@@ -9065,7 +9062,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
@@ -9074,12 +9071,12 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="69" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" ref="B58:B63" si="1">VLOOKUP(A58,Actions,2,FALSE)</f>
@@ -9088,16 +9085,16 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="1"/>
-        <v>🔓👊📷🔊</v>
+        <v>🔓👊📷🔊🔊</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="1"/>
@@ -9148,13 +9145,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E1" s="69" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F1" s="69" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="G1" s="69" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -9165,19 +9162,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -9191,13 +9188,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="G3" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -9211,16 +9208,16 @@
         <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -9234,10 +9231,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -9251,94 +9248,94 @@
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -9361,43 +9358,43 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="82" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -9420,50 +9417,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skills: diversifying a little bit
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -2192,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,11 +2896,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3978,7 +3978,7 @@
       </c>
       <c r="AA7" s="139" t="str">
         <f t="shared" si="8"/>
-        <v>Unplug%n📷📷🔊➜%nDash%n🔊➜➜%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
+        <v>Unplug%n📷📷🔊➜%nStride%n🔊➜🔍%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
       </c>
       <c r="AB7" s="40">
         <f t="shared" si="16"/>
@@ -5807,11 +5807,11 @@
         <v>📷📷🔊➜</v>
       </c>
       <c r="G19" s="135" t="s">
-        <v>239</v>
+        <v>310</v>
       </c>
       <c r="H19" s="139" t="str">
         <f t="shared" si="1"/>
-        <v>🔊➜➜</v>
+        <v>🔊➜🔍</v>
       </c>
       <c r="I19" s="136" t="s">
         <v>242</v>
@@ -5847,7 +5847,7 @@
       </c>
       <c r="R19" s="131" t="str">
         <f t="shared" si="11"/>
-        <v>Dash%n🔊➜➜</v>
+        <v>Stride%n🔊➜🔍</v>
       </c>
       <c r="S19" s="131" t="str">
         <f t="shared" si="12"/>
@@ -5867,7 +5867,7 @@
       </c>
       <c r="W19" s="142" t="str">
         <f t="shared" si="6"/>
-        <v>Unplug%n📷📷🔊➜%nDash%n🔊➜➜%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
+        <v>Unplug%n📷📷🔊➜%nStride%n🔊➜🔍%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
       </c>
       <c r="X19" s="138" t="s">
         <v>139</v>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="AD19" s="40">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE19" s="40">
         <f t="shared" si="16"/>
@@ -5909,7 +5909,7 @@
       </c>
       <c r="AH19" s="40">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI19" s="40">
         <f t="shared" si="16"/>

</xml_diff>

<commit_message>
characters: tweak street urchin et al., wording fixes
Street Urchin et al.
* Mastermind's Dash becomes Run, to sweeten the case for Grifter
* THERE ARE BETTER WAYS gets a little bit of a buff so it's used more.

Operative
* Nerf the noise lowering - it's still awesome but not as powerful.

Fix some wording on BREACH
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1231,15 +1231,6 @@
     <t>BOLT%nUse this action to spend 💡for 🔊➜➜, or 💡💡 for 🔊➜➜➜</t>
   </si>
   <si>
-    <t>PICKER%nGain 💡 when you 🔓%n %nBREACH%nUse this action and💡💡💡💡 to create a new Exit on current tile if it has an open, external side. Initiate Escape phase immediately.</t>
-  </si>
-  <si>
-    <t>THERE ARE BETTER WAYS%nCannot 👊. May exit a space with guard(s) for 💡 (does not apply to Escape phase).</t>
-  </si>
-  <si>
-    <t>THERE ARE BETTER WAYS%nCannot 👊. May exit a space with guard(s) for 💡 (does not apply to Escape phase).%n %nINSPIRE%nUse this action and a 🔊 to give a free💡💡  to a player of your choosing.</t>
-  </si>
-  <si>
     <t>Mover</t>
   </si>
   <si>
@@ -1249,13 +1240,22 @@
     <t>I CAN HAZ TEH CODES?%nOnce per heist may spend 💡💡 to re-position up to 3 planning tokens of any color(s)%n %nEXPLOIT%nUse this Action and a 💡 to enable another character to 👊🔊, 📷🔊, or 🔓🔊</t>
   </si>
   <si>
-    <t>ADRENALINE%nGain 💡  when you 👊%n %nYOU WILL REPORT IN%nWhen you  👊, lower the noise level by 2. Do not change the ⚠ level.</t>
-  </si>
-  <si>
     <t>ADRENALINE%nGain 💡 when you 👊%n %nBRING IT ON%nBash gets an 🔓 after Reinforcements event triggered.</t>
   </si>
   <si>
     <t>Pick II%n🔓🔓🔊</t>
+  </si>
+  <si>
+    <t>THERE ARE BETTER WAYS%nCannot 👊. May exit a space with guard(s) for 💡. In Escape, requires only 1 Escape Move to exit a space with guards.</t>
+  </si>
+  <si>
+    <t>THERE ARE BETTER WAYS%nCannot 👊. May exit a space with guard(s) for 💡. In Escape, requires only 1 Escape Move to exit a space with guards.%n %nINSPIRE%nUse this action and a 🔊 to give a free💡💡  to a player of your choosing.</t>
+  </si>
+  <si>
+    <t>ADRENALINE%nGain 💡  when you 👊%n %nYOU WILL REPORT IN%nWhen you  👊, lower the noise level by 1. Do not change the ⚠ level.</t>
+  </si>
+  <si>
+    <t>PICKER%nGain 💡 when you 🔓%n %nBREACH%nUse this action and💡💡💡💡 to create a new Exit on an open, external side of the current tile. Initiate Escape phase immediately.</t>
   </si>
 </sst>
 </file>
@@ -2176,7 +2176,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,7 +2300,7 @@
         <v>142</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
@@ -2343,7 +2343,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>81</v>
@@ -2417,7 +2417,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>81</v>
@@ -2452,7 +2452,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M7" s="20" t="s">
         <v>81</v>
@@ -2463,7 +2463,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
@@ -2491,7 +2491,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>81</v>
@@ -2502,7 +2502,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2526,7 +2526,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="M9" s="19"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -2550,7 +2550,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>158</v>
+        <v>371</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>394</v>
@@ -2559,7 +2559,7 @@
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>81</v>
@@ -2598,7 +2598,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="M11" s="22"/>
     </row>
@@ -2631,7 +2631,7 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>81</v>
@@ -2666,7 +2666,7 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
skills: balancing and naming fixes
* Reveal is not good enough for a Skill action. Changed to Discover throughout
* Shim is no more. It's Pick to be consistent with Angry Locksmith. Shim is a good word, so it might come back later though.
* Tackle became Hit, so that Hit 'n' Run actually Hits and Runs.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,14 @@
     <sheet name="Tile ideas" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Actions">Actions!$A$2:$B$48</definedName>
+    <definedName name="Actions">Actions!$A$2:$B$47</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="408">
   <si>
     <t>Name</t>
   </si>
@@ -775,9 +775,6 @@
     <t>🔊🔊➜➜</t>
   </si>
   <si>
-    <t>Shim</t>
-  </si>
-  <si>
     <t>👊➜</t>
   </si>
   <si>
@@ -976,9 +973,6 @@
     <t>Hit 'n' Run</t>
   </si>
   <si>
-    <t>Tackle</t>
-  </si>
-  <si>
     <t>👊🔊</t>
   </si>
   <si>
@@ -1256,6 +1250,9 @@
   </si>
   <si>
     <t>PICKER%nGain 💡 when you 🔓%n %nBREACH%nUse this action and💡💡💡💡 to create a new Exit on an open, external side of the current tile. Initiate Escape phase immediately.</t>
+  </si>
+  <si>
+    <t>Hit</t>
   </si>
 </sst>
 </file>
@@ -2175,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2223,7 +2220,7 @@
         <v>141</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J1" s="32" t="s">
         <v>152</v>
@@ -2261,7 +2258,7 @@
         <v>142</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="10" t="s">
@@ -2300,7 +2297,7 @@
         <v>142</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
@@ -2335,15 +2332,15 @@
         <v>142</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>81</v>
@@ -2382,7 +2379,7 @@
         <v>8</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="M5" s="20" t="s">
         <v>81</v>
@@ -2417,7 +2414,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>81</v>
@@ -2446,13 +2443,13 @@
         <v>142</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M7" s="20" t="s">
         <v>81</v>
@@ -2463,7 +2460,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
@@ -2491,7 +2488,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>81</v>
@@ -2502,7 +2499,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2526,7 +2523,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M9" s="19"/>
     </row>
@@ -2535,7 +2532,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -2550,16 +2547,16 @@
         <v>3</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>81</v>
@@ -2585,10 +2582,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="24" t="s">
@@ -2598,7 +2595,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="M11" s="22"/>
     </row>
@@ -2622,16 +2619,16 @@
         <v>6</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>81</v>
@@ -2657,16 +2654,16 @@
         <v>6</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>81</v>
@@ -2695,7 +2692,7 @@
         <v>142</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>132</v>
@@ -2707,7 +2704,7 @@
         <v>15</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>81</v>
@@ -2736,13 +2733,13 @@
         <v>142</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>132</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="M15" s="21" t="s">
         <v>81</v>
@@ -2771,7 +2768,7 @@
         <v>142</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>132</v>
@@ -2779,7 +2776,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>81</v>
@@ -2805,14 +2802,14 @@
         <v>4</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H17" s="27" t="s">
         <v>132</v>
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K17" s="26" t="s">
         <v>39</v>
@@ -2826,7 +2823,7 @@
     </row>
     <row r="18" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>151</v>
@@ -2844,14 +2841,14 @@
         <v>3</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H18" s="27" t="s">
         <v>131</v>
       </c>
       <c r="I18" s="27"/>
       <c r="L18" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M18" s="23" t="s">
         <v>81</v>
@@ -2877,14 +2874,14 @@
         <v>5</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I19" s="27"/>
       <c r="L19" s="23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M19" s="23" t="s">
         <v>81</v>
@@ -2909,11 +2906,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="E38" sqref="E38:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,34 +2977,34 @@
         <v>212</v>
       </c>
       <c r="G1" s="112" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="94" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="I1" s="99" t="s">
         <v>266</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="J1" s="95" t="s">
         <v>267</v>
       </c>
-      <c r="J1" s="95" t="s">
+      <c r="K1" s="112" t="s">
         <v>268</v>
       </c>
-      <c r="K1" s="112" t="s">
+      <c r="L1" s="94" t="s">
         <v>269</v>
       </c>
-      <c r="L1" s="94" t="s">
+      <c r="M1" s="99" t="s">
         <v>270</v>
       </c>
-      <c r="M1" s="99" t="s">
+      <c r="N1" s="95" t="s">
         <v>271</v>
       </c>
-      <c r="N1" s="95" t="s">
+      <c r="O1" s="112" t="s">
         <v>272</v>
       </c>
-      <c r="O1" s="112" t="s">
+      <c r="P1" s="95" t="s">
         <v>273</v>
-      </c>
-      <c r="P1" s="95" t="s">
-        <v>274</v>
       </c>
       <c r="Q1" s="94">
         <v>1</v>
@@ -3067,16 +3064,16 @@
         <v>155</v>
       </c>
       <c r="AJ1" s="93" t="s">
+        <v>298</v>
+      </c>
+      <c r="AK1" s="93" t="s">
+        <v>308</v>
+      </c>
+      <c r="AL1" s="93" t="s">
         <v>299</v>
       </c>
-      <c r="AK1" s="93" t="s">
-        <v>309</v>
-      </c>
-      <c r="AL1" s="93" t="s">
-        <v>300</v>
-      </c>
       <c r="AM1" s="93" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AN1" s="147"/>
       <c r="AO1" s="147"/>
@@ -3117,18 +3114,18 @@
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G2" s="113" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H2" s="41" t="str">
         <f t="shared" ref="H2:H19" si="1">VLOOKUP(G2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="I2" s="100" t="s">
-        <v>168</v>
+        <v>233</v>
       </c>
       <c r="J2" s="81" t="str">
         <f t="shared" ref="J2:J19" si="2">VLOOKUP(I2,Actions,2,FALSE)</f>
-        <v>🔍</v>
+        <v>🔍🔍</v>
       </c>
       <c r="K2" s="113" t="s">
         <v>221</v>
@@ -3138,14 +3135,14 @@
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M2" s="100" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="N2" s="81" t="str">
         <f t="shared" ref="N2:N19" si="4">VLOOKUP(M2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O2" s="113" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="P2" s="81" t="str">
         <f t="shared" ref="P2:P19" si="5">VLOOKUP(O2,Actions,2,FALSE)</f>
@@ -3161,7 +3158,7 @@
       </c>
       <c r="S2" s="40" t="str">
         <f>I2&amp;"%n"&amp;J2</f>
-        <v>Reveal%n🔍</v>
+        <v>Discover%n🔍🔍</v>
       </c>
       <c r="T2" s="40" t="str">
         <f>K2&amp;"%n"&amp;L2</f>
@@ -3182,7 +3179,7 @@
 &amp; T2 &amp; "%n"
 &amp; U2 &amp; "%n"
 &amp; V2</f>
-        <v>Punch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nReveal%n🔍%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nGrab%n💰🔊</v>
+        <v>Punch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nDiscover%n🔍🔍%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nGrab%n💰🔊</v>
       </c>
       <c r="X2" s="40" t="s">
         <v>156</v>
@@ -3192,7 +3189,7 @@
         <v>Flip%n👊🔊➜%nDisable%n📷🔊➜%nStudy%n💡💡%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nRansack%n💰💰🔊</v>
       </c>
       <c r="Z2" s="40" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="AA2" s="43" t="str">
         <f t="shared" ref="AA2:AA19" si="8">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
@@ -3224,23 +3221,23 @@
       </c>
       <c r="AH2" s="40">
         <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="AI2" s="40">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="AI2" s="40">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
       <c r="AJ2" s="39" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AK2" s="39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AL2" s="39" t="s">
         <v>154</v>
       </c>
       <c r="AM2" s="39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AN2" s="149"/>
       <c r="AO2" s="149"/>
@@ -3281,7 +3278,7 @@
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G3" s="115" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H3" s="36" t="str">
         <f t="shared" si="1"/>
@@ -3302,7 +3299,7 @@
         <v>💡💡</v>
       </c>
       <c r="M3" s="103" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N3" s="83" t="str">
         <f t="shared" si="4"/>
@@ -3321,7 +3318,7 @@
       </c>
       <c r="R3" s="38" t="str">
         <f t="shared" ref="R3:R19" si="11">G3&amp;"%n"&amp;H3</f>
-        <v>Shim%n🔓🔊</v>
+        <v>Pick%n🔓🔊</v>
       </c>
       <c r="S3" s="38" t="str">
         <f t="shared" ref="S3:S19" si="12">I3&amp;"%n"&amp;J3</f>
@@ -3341,21 +3338,21 @@
       </c>
       <c r="W3" s="35" t="str">
         <f t="shared" si="6"/>
-        <v>Run%n🔊🔊➜➜%nShim%n🔓🔊%nRun%n🔊🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Run%n🔊🔊➜➜%nPick%n🔓🔊%nRun%n🔊🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="X3" s="38" t="s">
         <v>36</v>
       </c>
       <c r="Y3" s="36" t="str">
         <f t="shared" si="7"/>
-        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Dash%n🔊➜➜%nPick%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="Z3" s="38" t="s">
         <v>68</v>
       </c>
       <c r="AA3" s="35" t="str">
         <f t="shared" si="8"/>
-        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSneak%n📷🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Dash%n🔊➜➜%nPick%n🔓🔊%nSneak%n📷🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="AB3" s="40">
         <f t="shared" ref="AB3:AI19" si="16">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
@@ -3390,16 +3387,16 @@
         <v>0</v>
       </c>
       <c r="AJ3" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AK3" s="33" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AL3" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM3" s="33" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN3" s="149"/>
       <c r="AO3" s="149"/>
@@ -3421,7 +3418,7 @@
     </row>
     <row r="4" spans="1:56" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B4" s="50">
         <v>2</v>
@@ -3430,45 +3427,45 @@
         <v>1</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>168</v>
+        <v>233</v>
       </c>
       <c r="F4" s="85" t="str">
         <f t="shared" si="0"/>
-        <v>🔍</v>
+        <v>🔍🔍</v>
       </c>
       <c r="G4" s="116" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H4" s="51" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="I4" s="105" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J4" s="85" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K4" s="123" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L4" s="51" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M4" s="105" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="N4" s="85" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O4" s="116" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="P4" s="85" t="str">
         <f t="shared" si="5"/>
@@ -3476,7 +3473,7 @@
       </c>
       <c r="Q4" s="50" t="str">
         <f t="shared" si="10"/>
-        <v>Reveal%n🔍</v>
+        <v>Discover%n🔍🔍</v>
       </c>
       <c r="R4" s="52" t="str">
         <f t="shared" si="11"/>
@@ -3500,7 +3497,7 @@
       </c>
       <c r="W4" s="53" t="str">
         <f t="shared" si="6"/>
-        <v>Reveal%n🔍%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nScamper%n🔊🔊🔊➜➜</v>
+        <v>Discover%n🔍🔍%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nScamper%n🔊🔊🔊➜➜</v>
       </c>
       <c r="X4" s="50" t="s">
         <v>174</v>
@@ -3542,23 +3539,23 @@
       </c>
       <c r="AH4" s="40">
         <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="AI4" s="40">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="AI4" s="40">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
       <c r="AJ4" s="54" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AK4" s="54" t="s">
         <v>161</v>
       </c>
       <c r="AL4" s="54" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AM4" s="54" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AN4" s="149"/>
       <c r="AO4" s="149"/>
@@ -3580,7 +3577,7 @@
     </row>
     <row r="5" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B5" s="61">
         <v>2</v>
@@ -3589,10 +3586,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E5" s="106" t="s">
-        <v>315</v>
+        <v>407</v>
       </c>
       <c r="F5" s="87" t="str">
         <f t="shared" si="0"/>
@@ -3620,7 +3617,7 @@
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M5" s="107" t="s">
-        <v>315</v>
+        <v>407</v>
       </c>
       <c r="N5" s="87" t="str">
         <f t="shared" si="4"/>
@@ -3635,7 +3632,7 @@
       </c>
       <c r="Q5" s="61" t="str">
         <f t="shared" si="10"/>
-        <v>Tackle%n👊🔊</v>
+        <v>Hit%n👊🔊</v>
       </c>
       <c r="R5" s="61" t="str">
         <f t="shared" si="11"/>
@@ -3651,7 +3648,7 @@
       </c>
       <c r="U5" s="61" t="str">
         <f t="shared" si="14"/>
-        <v>Tackle%n👊🔊</v>
+        <v>Hit%n👊🔊</v>
       </c>
       <c r="V5" s="61" t="str">
         <f t="shared" si="15"/>
@@ -3659,7 +3656,7 @@
       </c>
       <c r="W5" s="63" t="str">
         <f t="shared" si="6"/>
-        <v>Tackle%n👊🔊%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nRun%n🔊🔊➜➜%nTackle%n👊🔊%nStudy%n💡💡</v>
+        <v>Hit%n👊🔊%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nRun%n🔊🔊➜➜%nHit%n👊🔊%nStudy%n💡💡</v>
       </c>
       <c r="X5" s="61" t="s">
         <v>115</v>
@@ -3669,7 +3666,7 @@
         <v>Bash%n👊👊🔊%nRun%n🔊🔊➜➜%nRampage%n👊👊🔊🔊🔊➜➜%nRun%n🔊🔊➜➜%nStrongarm%n🔓👊🔊🔊➜%nStudy%n💡💡</v>
       </c>
       <c r="Z5" s="61" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AA5" s="63" t="str">
         <f t="shared" si="8"/>
@@ -3708,16 +3705,16 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="64" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AK5" s="64" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AL5" s="64" t="s">
         <v>161</v>
       </c>
       <c r="AM5" s="64" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN5" s="149"/>
       <c r="AO5" s="149"/>
@@ -3751,7 +3748,7 @@
         <v>130</v>
       </c>
       <c r="E6" s="108" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F6" s="89" t="str">
         <f t="shared" si="0"/>
@@ -3765,14 +3762,14 @@
         <v>💡💡</v>
       </c>
       <c r="I6" s="109" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="J6" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔓🔊</v>
       </c>
       <c r="K6" s="126" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L6" s="71" t="str">
         <f t="shared" si="3"/>
@@ -3786,7 +3783,7 @@
         <v>🔊🔊➜➜</v>
       </c>
       <c r="O6" s="118" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="P6" s="89" t="str">
         <f t="shared" si="5"/>
@@ -3802,7 +3799,7 @@
       </c>
       <c r="S6" s="72" t="str">
         <f t="shared" si="12"/>
-        <v>Shim%n🔓🔊</v>
+        <v>Pick%n🔓🔊</v>
       </c>
       <c r="T6" s="70" t="str">
         <f t="shared" si="13"/>
@@ -3814,18 +3811,18 @@
       </c>
       <c r="V6" s="72" t="str">
         <f t="shared" si="15"/>
-        <v>Shim%n🔓🔊</v>
+        <v>Pick%n🔓🔊</v>
       </c>
       <c r="W6" s="73" t="str">
         <f t="shared" si="6"/>
-        <v>Bump%n🔓🔓🔊🔊➜%nStudy%n💡💡%nShim%n🔓🔊%nSprint%n🔊🔊➜➜➜%nRun%n🔊🔊➜➜%nShim%n🔓🔊</v>
+        <v>Bump%n🔓🔓🔊🔊➜%nStudy%n💡💡%nPick%n🔓🔊%nSprint%n🔊🔊➜➜➜%nRun%n🔊🔊➜➜%nPick%n🔓🔊</v>
       </c>
       <c r="X6" s="72" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="Y6" s="71" t="str">
         <f t="shared" si="7"/>
-        <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShim%n🔓🔊</v>
+        <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nPick%n🔓🔊</v>
       </c>
       <c r="Z6" s="72" t="s">
         <v>138</v>
@@ -3867,16 +3864,16 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="74" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AK6" s="74" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AL6" s="74" t="s">
         <v>161</v>
       </c>
       <c r="AM6" s="74" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AN6" s="149"/>
       <c r="AO6" s="149"/>
@@ -3910,32 +3907,32 @@
         <v>59</v>
       </c>
       <c r="E7" s="131" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F7" s="132" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊🔊➜</v>
       </c>
       <c r="G7" s="133" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H7" s="130" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I7" s="134" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J7" s="132" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="K7" s="135" t="s">
-        <v>168</v>
+        <v>233</v>
       </c>
       <c r="L7" s="130" t="str">
         <f t="shared" si="3"/>
-        <v>🔍</v>
+        <v>🔍🔍</v>
       </c>
       <c r="M7" s="134" t="s">
         <v>218</v>
@@ -3945,7 +3942,7 @@
         <v>💡💡💡🔊</v>
       </c>
       <c r="O7" s="133" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="P7" s="132" t="str">
         <f t="shared" si="5"/>
@@ -3965,7 +3962,7 @@
       </c>
       <c r="T7" s="129" t="str">
         <f t="shared" si="13"/>
-        <v>Reveal%n🔍</v>
+        <v>Discover%n🔍🔍</v>
       </c>
       <c r="U7" s="136" t="str">
         <f t="shared" si="14"/>
@@ -3977,7 +3974,7 @@
       </c>
       <c r="W7" s="137" t="str">
         <f t="shared" si="6"/>
-        <v>Shatter%n📷📷🔊🔊➜%nSprint%n🔊🔊➜➜➜%nSmash%n📷🔊🔊➜%nReveal%n🔍%nExamine%n💡💡💡🔊%nSmash%n📷🔊🔊➜</v>
+        <v>Shatter%n📷📷🔊🔊➜%nSprint%n🔊🔊➜➜➜%nSmash%n📷🔊🔊➜%nDiscover%n🔍🔍%nExamine%n💡💡💡🔊%nSmash%n📷🔊🔊➜</v>
       </c>
       <c r="X7" s="136" t="s">
         <v>63</v>
@@ -3987,7 +3984,7 @@
         <v>Unplug%n📷📷🔊➜%nSprint%n🔊🔊➜➜➜%nDisable%n📷🔊➜%nDiscover%n🔍🔍%nRecon%n💡💡🔊🔍%nDisable%n📷🔊➜</v>
       </c>
       <c r="Z7" s="136" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AA7" s="137" t="str">
         <f t="shared" si="8"/>
@@ -4019,23 +4016,23 @@
       </c>
       <c r="AH7" s="40">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI7" s="40">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="138" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AK7" s="138" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AL7" s="138" t="s">
         <v>168</v>
       </c>
       <c r="AM7" s="138" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AN7" s="150"/>
       <c r="AO7" s="150"/>
@@ -4069,7 +4066,7 @@
         <v>126</v>
       </c>
       <c r="E8" s="101" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F8" s="82" t="str">
         <f t="shared" si="0"/>
@@ -4097,14 +4094,14 @@
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M8" s="101" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="N8" s="82" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O8" s="114" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="P8" s="82" t="str">
         <f t="shared" si="5"/>
@@ -4185,16 +4182,16 @@
         <v>2</v>
       </c>
       <c r="AJ8" s="144" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AK8" s="144" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AL8" s="144" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AM8" s="144" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN8" s="149"/>
       <c r="AO8" s="149"/>
@@ -4216,7 +4213,7 @@
     </row>
     <row r="9" spans="1:56" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B9" s="47">
         <v>2</v>
@@ -4235,21 +4232,21 @@
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G9" s="114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H9" s="43" t="str">
         <f t="shared" si="1"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="I9" s="101" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J9" s="82" t="str">
         <f t="shared" si="2"/>
         <v>🔍🔓🔊</v>
       </c>
       <c r="K9" s="114" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="L9" s="43" t="str">
         <f t="shared" si="3"/>
@@ -4263,7 +4260,7 @@
         <v>📷🔊➜</v>
       </c>
       <c r="O9" s="114" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="P9" s="82" t="str">
         <f t="shared" si="5"/>
@@ -4344,16 +4341,16 @@
         <v>1</v>
       </c>
       <c r="AJ9" s="46" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AK9" s="46" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AL9" s="46" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AM9" s="46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AN9" s="150"/>
       <c r="AO9" s="150"/>
@@ -4394,14 +4391,14 @@
         <v>🔊➜➜</v>
       </c>
       <c r="G10" s="115" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H10" s="34" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I10" s="103" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J10" s="84" t="str">
         <f t="shared" si="2"/>
@@ -4415,7 +4412,7 @@
         <v>💡💡</v>
       </c>
       <c r="M10" s="103" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N10" s="84" t="str">
         <f t="shared" si="4"/>
@@ -4434,7 +4431,7 @@
       </c>
       <c r="R10" s="37" t="str">
         <f t="shared" si="11"/>
-        <v>Shim%n🔓🔊</v>
+        <v>Pick%n🔓🔊</v>
       </c>
       <c r="S10" s="37" t="str">
         <f t="shared" si="12"/>
@@ -4454,7 +4451,7 @@
       </c>
       <c r="W10" s="35" t="str">
         <f t="shared" si="6"/>
-        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Dash%n🔊➜➜%nPick%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="X10" s="37" t="s">
         <v>139</v>
@@ -4503,16 +4500,16 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="146" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="AK10" s="146" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AL10" s="146" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM10" s="146" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AN10" s="150"/>
       <c r="AO10" s="150"/>
@@ -4553,7 +4550,7 @@
         <v>🔊➜➜</v>
       </c>
       <c r="G11" s="115" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H11" s="35" t="str">
         <f t="shared" si="1"/>
@@ -4574,7 +4571,7 @@
         <v>💡💡</v>
       </c>
       <c r="M11" s="103" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N11" s="84" t="str">
         <f t="shared" si="4"/>
@@ -4593,7 +4590,7 @@
       </c>
       <c r="R11" s="38" t="str">
         <f t="shared" si="11"/>
-        <v>Shim%n🔓🔊</v>
+        <v>Pick%n🔓🔊</v>
       </c>
       <c r="S11" s="37" t="str">
         <f t="shared" si="12"/>
@@ -4613,7 +4610,7 @@
       </c>
       <c r="W11" s="35" t="str">
         <f t="shared" si="6"/>
-        <v>Dash%n🔊➜➜%nShim%n🔓🔊%nSneak%n📷🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Dash%n🔊➜➜%nPick%n🔓🔊%nSneak%n📷🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
       </c>
       <c r="X11" s="37" t="s">
         <v>139</v>
@@ -4662,16 +4659,16 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="146" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AK11" s="145" t="s">
         <v>167</v>
       </c>
       <c r="AL11" s="145" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM11" s="145" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AN11" s="149"/>
       <c r="AO11" s="149"/>
@@ -4702,7 +4699,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E12" s="105" t="s">
         <v>217</v>
@@ -4712,28 +4709,28 @@
         <v>💡💡</v>
       </c>
       <c r="G12" s="116" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H12" s="53" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊</v>
       </c>
       <c r="I12" s="105" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J12" s="86" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K12" s="116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L12" s="53" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M12" s="105" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="N12" s="86" t="str">
         <f t="shared" si="4"/>
@@ -4821,16 +4818,16 @@
         <v>1</v>
       </c>
       <c r="AJ12" s="54" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AK12" s="54" t="s">
         <v>168</v>
       </c>
       <c r="AL12" s="54" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AM12" s="54" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN12" s="149"/>
       <c r="AO12" s="149"/>
@@ -4861,7 +4858,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E13" s="105" t="s">
         <v>215</v>
@@ -4871,28 +4868,28 @@
         <v>🔓👊📷🔊🔊</v>
       </c>
       <c r="G13" s="116" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H13" s="56" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="I13" s="105" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J13" s="86" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K13" s="124" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L13" s="56" t="str">
         <f t="shared" si="3"/>
         <v>👊📷</v>
       </c>
       <c r="M13" s="105" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="N13" s="86" t="str">
         <f t="shared" si="4"/>
@@ -4980,16 +4977,16 @@
         <v>1</v>
       </c>
       <c r="AJ13" s="54" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AK13" s="54" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AL13" s="54" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AM13" s="54" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN13" s="149"/>
       <c r="AO13" s="149"/>
@@ -5020,7 +5017,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E14" s="107" t="s">
         <v>225</v>
@@ -5051,7 +5048,7 @@
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M14" s="107" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N14" s="88" t="str">
         <f t="shared" si="4"/>
@@ -5139,16 +5136,16 @@
         <v>0</v>
       </c>
       <c r="AJ14" s="64" t="s">
+        <v>315</v>
+      </c>
+      <c r="AK14" s="64" t="s">
+        <v>343</v>
+      </c>
+      <c r="AL14" s="64" t="s">
+        <v>354</v>
+      </c>
+      <c r="AM14" s="64" t="s">
         <v>317</v>
-      </c>
-      <c r="AK14" s="64" t="s">
-        <v>345</v>
-      </c>
-      <c r="AL14" s="64" t="s">
-        <v>356</v>
-      </c>
-      <c r="AM14" s="64" t="s">
-        <v>319</v>
       </c>
       <c r="AN14" s="149"/>
       <c r="AO14" s="149"/>
@@ -5170,7 +5167,7 @@
     </row>
     <row r="15" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B15" s="66">
         <v>2</v>
@@ -5179,7 +5176,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E15" s="107" t="s">
         <v>225</v>
@@ -5298,14 +5295,14 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="64" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AK15" s="64"/>
       <c r="AL15" s="64" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AM15" s="64" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="AN15" s="149"/>
       <c r="AO15" s="149"/>
@@ -5327,7 +5324,7 @@
     </row>
     <row r="16" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B16" s="76">
         <v>2</v>
@@ -5353,14 +5350,14 @@
         <v>💡💡🔊🔍</v>
       </c>
       <c r="I16" s="109" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J16" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔓💰</v>
       </c>
       <c r="K16" s="127" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L16" s="77" t="str">
         <f t="shared" si="3"/>
@@ -5374,7 +5371,7 @@
         <v>🔊➜➜</v>
       </c>
       <c r="O16" s="118" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="P16" s="89" t="str">
         <f t="shared" si="5"/>
@@ -5402,11 +5399,11 @@
       </c>
       <c r="V16" s="76" t="str">
         <f t="shared" si="15"/>
-        <v>Shim%n🔓🔊</v>
+        <v>Pick%n🔓🔊</v>
       </c>
       <c r="W16" s="78" t="str">
         <f t="shared" si="6"/>
-        <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShim%n🔓🔊</v>
+        <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nPick%n🔓🔊</v>
       </c>
       <c r="X16" s="72" t="s">
         <v>139</v>
@@ -5455,16 +5452,16 @@
         <v>1</v>
       </c>
       <c r="AJ16" s="74" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AK16" s="74" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AL16" s="74" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AM16" s="74" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN16" s="149"/>
       <c r="AO16" s="149"/>
@@ -5512,14 +5509,14 @@
         <v>💡💡</v>
       </c>
       <c r="I17" s="109" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J17" s="90" t="str">
         <f t="shared" si="2"/>
         <v>🔓👊🔊</v>
       </c>
       <c r="K17" s="118" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L17" s="73" t="str">
         <f t="shared" si="3"/>
@@ -5533,7 +5530,7 @@
         <v>🔊➜➜</v>
       </c>
       <c r="O17" s="118" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P17" s="90" t="str">
         <f t="shared" si="5"/>
@@ -5614,16 +5611,16 @@
         <v>0</v>
       </c>
       <c r="AJ17" s="74" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AK17" s="74" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AL17" s="74" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AM17" s="74" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN17" s="150"/>
       <c r="AO17" s="150"/>
@@ -5657,14 +5654,14 @@
         <v>59</v>
       </c>
       <c r="E18" s="134" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F18" s="139" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="G18" s="133" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H18" s="137" t="str">
         <f t="shared" si="1"/>
@@ -5773,13 +5770,13 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="138" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="AK18" s="138" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AM18" s="138" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AN18" s="150"/>
       <c r="AO18" s="150"/>
@@ -5801,7 +5798,7 @@
     </row>
     <row r="19" spans="1:56" s="138" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="137" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B19" s="136">
         <v>2</v>
@@ -5813,14 +5810,14 @@
         <v>59</v>
       </c>
       <c r="E19" s="134" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F19" s="139" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="G19" s="133" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H19" s="137" t="str">
         <f t="shared" si="1"/>
@@ -5834,7 +5831,7 @@
         <v>📷🔊➜</v>
       </c>
       <c r="K19" s="133" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L19" s="137" t="str">
         <f t="shared" si="3"/>
@@ -5929,16 +5926,16 @@
         <v>0</v>
       </c>
       <c r="AJ19" s="138" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AK19" s="138" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AL19" s="138" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AM19" s="138" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AN19" s="150"/>
       <c r="AO19" s="150"/>
@@ -6067,7 +6064,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -6094,7 +6091,7 @@
         <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6110,7 +6107,7 @@
         <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6136,10 +6133,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6155,13 +6152,13 @@
         <v>194</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1" s="69" t="s">
         <v>195</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6199,7 +6196,7 @@
         <v>216</v>
       </c>
       <c r="B4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -6211,10 +6208,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -6226,10 +6223,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -6241,10 +6238,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -6259,7 +6256,7 @@
         <v>223</v>
       </c>
       <c r="B8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C8" t="s">
         <v>166</v>
@@ -6274,7 +6271,7 @@
         <v>215</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C9" t="s">
         <v>166</v>
@@ -6286,10 +6283,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C10" t="s">
         <v>166</v>
@@ -6301,10 +6298,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B11" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C11" t="s">
         <v>166</v>
@@ -6316,10 +6313,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B12" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C12" t="s">
         <v>166</v>
@@ -6331,10 +6328,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C13" t="s">
         <v>166</v>
@@ -6346,10 +6343,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C14" t="s">
         <v>166</v>
@@ -6361,10 +6358,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D15" s="1">
         <f>COUNTIF(Skills!E:E,A15) + COUNTIF(Skills!I:I,A15) + COUNTIF(Skills!K:K,A15) + COUNTIF(Skills!M:M,A15) + COUNTIF(Skills!O:O,A15)</f>
@@ -6421,7 +6418,7 @@
         <v>217</v>
       </c>
       <c r="B19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C19" t="s">
         <v>161</v>
@@ -6433,10 +6430,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C20" t="s">
         <v>154</v>
@@ -6448,10 +6445,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C21" t="s">
         <v>154</v>
@@ -6508,10 +6505,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B25" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -6523,10 +6520,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" t="s">
         <v>250</v>
-      </c>
-      <c r="B26" t="s">
-        <v>251</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
@@ -6538,10 +6535,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>252</v>
+      </c>
+      <c r="B27" t="s">
         <v>253</v>
-      </c>
-      <c r="B27" t="s">
-        <v>254</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
@@ -6556,7 +6553,7 @@
         <v>243</v>
       </c>
       <c r="B28" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>
@@ -6578,7 +6575,7 @@
       </c>
       <c r="D29" s="1">
         <f>COUNTIF(Skills!E:E,A29) + COUNTIF(Skills!I:I,A29) + COUNTIF(Skills!K:K,A29) + COUNTIF(Skills!M:M,A29) + COUNTIF(Skills!O:O,A29)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -6598,10 +6595,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>295</v>
+      </c>
+      <c r="B31" t="s">
         <v>296</v>
-      </c>
-      <c r="B31" t="s">
-        <v>297</v>
       </c>
       <c r="C31" t="s">
         <v>168</v>
@@ -6623,7 +6620,7 @@
       </c>
       <c r="D32" s="1">
         <f>COUNTIF(Skills!E:E,A32) + COUNTIF(Skills!I:I,A32) + COUNTIF(Skills!K:K,A32) + COUNTIF(Skills!M:M,A32) + COUNTIF(Skills!O:O,A32)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6673,10 +6670,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B36" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D36" s="1">
         <f>COUNTIF(Skills!E:E,A36) + COUNTIF(Skills!I:I,A36) + COUNTIF(Skills!K:K,A36) + COUNTIF(Skills!M:M,A36) + COUNTIF(Skills!O:O,A36)</f>
@@ -6703,7 +6700,7 @@
         <v>245</v>
       </c>
       <c r="B38" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C38" t="s">
         <v>167</v>
@@ -6715,10 +6712,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C39" t="s">
         <v>167</v>
@@ -6730,10 +6727,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C40" t="s">
         <v>167</v>
@@ -6745,10 +6742,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>315</v>
+        <v>407</v>
       </c>
       <c r="B41" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C41" t="s">
         <v>167</v>
@@ -6775,10 +6772,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -6793,22 +6790,22 @@
         <v>242</v>
       </c>
       <c r="B44" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="1">
         <f>COUNTIF(Skills!E:E,A44) + COUNTIF(Skills!I:I,A44) + COUNTIF(Skills!K:K,A44) + COUNTIF(Skills!M:M,A44) + COUNTIF(Skills!O:O,A44)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B45" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
@@ -6823,26 +6820,11 @@
         <v>222</v>
       </c>
       <c r="B46" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D46" s="1">
         <f>COUNTIF(Skills!E:E,A46) + COUNTIF(Skills!I:I,A46) + COUNTIF(Skills!K:K,A46) + COUNTIF(Skills!M:M,A46) + COUNTIF(Skills!O:O,A46)</f>
         <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>248</v>
-      </c>
-      <c r="B47" t="s">
-        <v>301</v>
-      </c>
-      <c r="C47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="1">
-        <f>COUNTIF(Skills!E:E,A47) + COUNTIF(Skills!I:I,A47) + COUNTIF(Skills!K:K,A47) + COUNTIF(Skills!M:M,A47) + COUNTIF(Skills!O:O,A47)</f>
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8225,7 +8207,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="69" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -8255,7 +8237,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="55" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -8290,12 +8272,12 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="69" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" ref="B48:B55" si="0">VLOOKUP(A48,Actions,2,FALSE)</f>
@@ -8322,7 +8304,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -8367,7 +8349,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="69" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -8390,7 +8372,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="1"/>
@@ -8441,13 +8423,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E1" s="69" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="G1" s="69" t="s">
         <v>276</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8464,13 +8446,13 @@
         <v>143</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8487,10 +8469,10 @@
         <v>144</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" t="s">
         <v>279</v>
-      </c>
-      <c r="G3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8507,13 +8489,13 @@
         <v>145</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8530,7 +8512,7 @@
         <v>146</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8547,13 +8529,13 @@
         <v>148</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>291</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8570,13 +8552,13 @@
         <v>147</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -8690,7 +8672,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skills: make improvise better
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -2172,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,11 +2906,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3511,7 +3511,7 @@
       </c>
       <c r="AA4" s="53" t="str">
         <f t="shared" si="8"/>
-        <v>Redirect%n🔓👊📷🔊🔊%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nShock%n👊📷%nGrab%n💰🔊%nRun%n🔊🔊➜➜</v>
+        <v>Redirect%n🔓👊📷🔊🔊%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nDash%n🔊➜➜</v>
       </c>
       <c r="AB4" s="40">
         <f t="shared" si="16"/>
@@ -4882,11 +4882,11 @@
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K13" s="124" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="L13" s="56" t="str">
         <f t="shared" si="3"/>
-        <v>👊📷</v>
+        <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M13" s="105" t="s">
         <v>339</v>
@@ -4896,11 +4896,11 @@
         <v>💰🔊</v>
       </c>
       <c r="O13" s="116" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="P13" s="86" t="str">
         <f t="shared" si="5"/>
-        <v>🔊🔊➜➜</v>
+        <v>🔊➜➜</v>
       </c>
       <c r="Q13" s="60" t="str">
         <f t="shared" si="10"/>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="T13" s="59" t="str">
         <f t="shared" si="13"/>
-        <v>Shock%n👊📷</v>
+        <v>Zap%n👊📷🔊🔊➜</v>
       </c>
       <c r="U13" s="60" t="str">
         <f t="shared" si="14"/>
@@ -4924,11 +4924,11 @@
       </c>
       <c r="V13" s="60" t="str">
         <f t="shared" si="15"/>
-        <v>Run%n🔊🔊➜➜</v>
+        <v>Dash%n🔊➜➜</v>
       </c>
       <c r="W13" s="56" t="str">
         <f t="shared" si="6"/>
-        <v>Redirect%n🔓👊📷🔊🔊%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nShock%n👊📷%nGrab%n💰🔊%nRun%n🔊🔊➜➜</v>
+        <v>Redirect%n🔓👊📷🔊🔊%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nDash%n🔊➜➜</v>
       </c>
       <c r="X13" s="59" t="s">
         <v>139</v>
@@ -4950,11 +4950,11 @@
       </c>
       <c r="AC13" s="40">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD13" s="40">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE13" s="40">
         <f t="shared" si="9"/>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="D10" s="1">
         <f>COUNTIF(Skills!E:E,A10) + COUNTIF(Skills!I:I,A10) + COUNTIF(Skills!K:K,A10) + COUNTIF(Skills!M:M,A10) + COUNTIF(Skills!O:O,A10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="D13" s="1">
         <f>COUNTIF(Skills!E:E,A13) + COUNTIF(Skills!I:I,A13) + COUNTIF(Skills!K:K,A13) + COUNTIF(Skills!M:M,A13) + COUNTIF(Skills!O:O,A13)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6485,7 +6485,7 @@
       </c>
       <c r="D23" s="1">
         <f>COUNTIF(Skills!E:E,A23) + COUNTIF(Skills!I:I,A23) + COUNTIF(Skills!K:K,A23) + COUNTIF(Skills!M:M,A23) + COUNTIF(Skills!O:O,A23)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -6500,7 +6500,7 @@
       </c>
       <c r="D24" s="1">
         <f>COUNTIF(Skills!E:E,A24) + COUNTIF(Skills!I:I,A24) + COUNTIF(Skills!K:K,A24) + COUNTIF(Skills!M:M,A24) + COUNTIF(Skills!O:O,A24)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
skill backs: new design
bad code, but we'll refactor it
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -2907,10 +2907,10 @@
   <dimension ref="A1:BD20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2931,13 +2931,13 @@
     <col min="14" max="14" width="12.140625" style="92" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.5703125" style="120" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.140625" style="92" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25" style="3" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="20" style="3" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="25.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="20.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="25.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="130.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="25" style="3" customWidth="1"/>
+    <col min="18" max="18" width="20" style="3" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" style="3" customWidth="1"/>
+    <col min="20" max="20" width="25.140625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="20.140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="130.140625" style="4" customWidth="1"/>
     <col min="24" max="24" width="15.140625" style="3" customWidth="1"/>
     <col min="25" max="25" width="13" style="4" customWidth="1"/>
     <col min="26" max="26" width="15.140625" style="3" customWidth="1"/>
@@ -3173,58 +3173,58 @@
         <v>Grab%n💰🔊</v>
       </c>
       <c r="W2" s="43" t="str">
-        <f t="shared" ref="W2:W19" si="6">Q2 &amp; "%n"
-&amp; R2 &amp; "%n"
-&amp; S2 &amp; "%n"
-&amp; T2 &amp; "%n"
-&amp; U2 &amp; "%n"
+        <f>Q2 &amp; "/"
+&amp; R2 &amp; "/"
+&amp; S2 &amp; "/"
+&amp; T2 &amp; "/"
+&amp; U2 &amp; "/"
 &amp; V2</f>
-        <v>Punch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nDiscover%n🔍🔍%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nGrab%n💰🔊</v>
+        <v>Punch%n👊🔊🔊➜/Smash%n📷🔊🔊➜/Discover%n🔍🔍/Punch%n👊🔊🔊➜/Smash%n📷🔊🔊➜/Grab%n💰🔊</v>
       </c>
       <c r="X2" s="40" t="s">
         <v>156</v>
       </c>
       <c r="Y2" s="41" t="str">
-        <f t="shared" ref="Y2:Y19" si="7">IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
-        <v>Flip%n👊🔊➜%nDisable%n📷🔊➜%nStudy%n💡💡%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nRansack%n💰💰🔊</v>
+        <f>IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
+        <v>Flip%n👊🔊➜/Disable%n📷🔊➜/Study%n💡💡/Punch%n👊🔊🔊➜/Smash%n📷🔊🔊➜/Ransack%n💰💰🔊</v>
       </c>
       <c r="Z2" s="40" t="s">
         <v>342</v>
       </c>
       <c r="AA2" s="43" t="str">
-        <f t="shared" ref="AA2:AA19" si="8">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
-        <v>Punch%n👊🔊🔊➜%nUnplug%n📷📷🔊➜%nKey In%n🔍🔓🔊%nFlip%n👊🔊➜%nDisable%n📷🔊➜%nGrab%n💰🔊</v>
+        <f t="shared" ref="AA2:AA19" si="6">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
+        <v>Punch%n👊🔊🔊➜/Unplug%n📷📷🔊➜/Key In%n🔍🔓🔊/Flip%n👊🔊➜/Disable%n📷🔊➜/Grab%n💰🔊</v>
       </c>
       <c r="AB2" s="40">
         <f>(LEN($W2)-LEN(SUBSTITUTE($W2,AB$1,"")))/LEN(AB$1)</f>
         <v>0</v>
       </c>
       <c r="AC2" s="40">
-        <f t="shared" ref="AC2:AI17" si="9">(LEN($W2)-LEN(SUBSTITUTE($W2,AC$1,"")))/LEN(AC$1)</f>
+        <f t="shared" ref="AC2:AI17" si="7">(LEN($W2)-LEN(SUBSTITUTE($W2,AC$1,"")))/LEN(AC$1)</f>
         <v>9</v>
       </c>
       <c r="AD2" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AE2" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AF2" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AG2" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH2" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AI2" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ2" s="39" t="s">
@@ -3313,77 +3313,82 @@
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q3" s="38" t="str">
-        <f t="shared" ref="Q3:Q19" si="10">E3&amp;"%n"&amp;F3</f>
+        <f t="shared" ref="Q3:Q19" si="8">E3&amp;"%n"&amp;F3</f>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="R3" s="38" t="str">
-        <f t="shared" ref="R3:R19" si="11">G3&amp;"%n"&amp;H3</f>
+        <f t="shared" ref="R3:R19" si="9">G3&amp;"%n"&amp;H3</f>
         <v>Pick%n🔓🔊</v>
       </c>
       <c r="S3" s="38" t="str">
-        <f t="shared" ref="S3:S19" si="12">I3&amp;"%n"&amp;J3</f>
+        <f t="shared" ref="S3:S19" si="10">I3&amp;"%n"&amp;J3</f>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="T3" s="37" t="str">
-        <f t="shared" ref="T3:T19" si="13">K3&amp;"%n"&amp;L3</f>
+        <f t="shared" ref="T3:T19" si="11">K3&amp;"%n"&amp;L3</f>
         <v>Study%n💡💡</v>
       </c>
       <c r="U3" s="38" t="str">
-        <f t="shared" ref="U3:U19" si="14">M3&amp;"%n"&amp;N3</f>
+        <f t="shared" ref="U3:U19" si="12">M3&amp;"%n"&amp;N3</f>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="V3" s="38" t="str">
-        <f t="shared" ref="V3:V19" si="15">O3&amp;"%n"&amp;P3</f>
+        <f t="shared" ref="V3:V19" si="13">O3&amp;"%n"&amp;P3</f>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="W3" s="35" t="str">
-        <f t="shared" si="6"/>
-        <v>Run%n🔊🔊➜➜%nPick%n🔓🔊%nRun%n🔊🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <f t="shared" ref="W3:W19" si="14">Q3 &amp; "/"
+&amp; R3 &amp; "/"
+&amp; S3 &amp; "/"
+&amp; T3 &amp; "/"
+&amp; U3 &amp; "/"
+&amp; V3</f>
+        <v>Run%n🔊🔊➜➜/Pick%n🔓🔊/Run%n🔊🔊➜➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="X3" s="38" t="s">
         <v>36</v>
       </c>
       <c r="Y3" s="36" t="str">
-        <f t="shared" si="7"/>
-        <v>Dash%n🔊➜➜%nPick%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <f>IF(X3="(none)","",VLOOKUP(X3,$A$2:$W$19,23,FALSE))</f>
+        <v>Dash%n🔊➜➜/Pick%n🔓🔊/Sleeper Hold%n👊➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="Z3" s="38" t="s">
         <v>68</v>
       </c>
       <c r="AA3" s="35" t="str">
-        <f t="shared" si="8"/>
-        <v>Dash%n🔊➜➜%nPick%n🔓🔊%nSneak%n📷🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <f t="shared" si="6"/>
+        <v>Dash%n🔊➜➜/Pick%n🔓🔊/Sneak%n📷🔊➜➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="AB3" s="40">
-        <f t="shared" ref="AB3:AI19" si="16">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
+        <f t="shared" ref="AB3:AI19" si="15">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
         <v>5</v>
       </c>
       <c r="AC3" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="AD3" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AE3" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF3" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG3" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AH3" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI3" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="33" t="s">
@@ -3472,77 +3477,77 @@
         <v>🔊🔊🔊➜➜</v>
       </c>
       <c r="Q4" s="50" t="str">
+        <f t="shared" si="8"/>
+        <v>Discover%n🔍🔍</v>
+      </c>
+      <c r="R4" s="52" t="str">
+        <f t="shared" si="9"/>
+        <v>Strongarm%n🔓👊🔊🔊➜</v>
+      </c>
+      <c r="S4" s="52" t="str">
         <f t="shared" si="10"/>
-        <v>Discover%n🔍🔍</v>
-      </c>
-      <c r="R4" s="52" t="str">
+        <v>Short%n🔓📷🔊🔊➜</v>
+      </c>
+      <c r="T4" s="50" t="str">
         <f t="shared" si="11"/>
-        <v>Strongarm%n🔓👊🔊🔊➜</v>
-      </c>
-      <c r="S4" s="52" t="str">
+        <v>Zap%n👊📷🔊🔊➜</v>
+      </c>
+      <c r="U4" s="50" t="str">
         <f t="shared" si="12"/>
-        <v>Short%n🔓📷🔊🔊➜</v>
-      </c>
-      <c r="T4" s="50" t="str">
+        <v>Grab%n💰🔊</v>
+      </c>
+      <c r="V4" s="50" t="str">
         <f t="shared" si="13"/>
-        <v>Zap%n👊📷🔊🔊➜</v>
-      </c>
-      <c r="U4" s="50" t="str">
+        <v>Scamper%n🔊🔊🔊➜➜</v>
+      </c>
+      <c r="W4" s="53" t="str">
         <f t="shared" si="14"/>
-        <v>Grab%n💰🔊</v>
-      </c>
-      <c r="V4" s="50" t="str">
-        <f t="shared" si="15"/>
-        <v>Scamper%n🔊🔊🔊➜➜</v>
-      </c>
-      <c r="W4" s="53" t="str">
-        <f t="shared" si="6"/>
-        <v>Discover%n🔍🔍%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nScamper%n🔊🔊🔊➜➜</v>
+        <v>Discover%n🔍🔍/Strongarm%n🔓👊🔊🔊➜/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Scamper%n🔊🔊🔊➜➜</v>
       </c>
       <c r="X4" s="50" t="s">
         <v>174</v>
       </c>
       <c r="Y4" s="51" t="str">
-        <f t="shared" si="7"/>
-        <v>Study%n💡💡%nSpy Stuff%n🔓👊🔊%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nRun%n🔊🔊➜➜</v>
+        <f>IF(X4="(none)","",VLOOKUP(X4,$A$2:$W$19,23,FALSE))</f>
+        <v>Study%n💡💡/Spy Stuff%n🔓👊🔊/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Run%n🔊🔊➜➜</v>
       </c>
       <c r="Z4" s="50" t="s">
         <v>125</v>
       </c>
       <c r="AA4" s="53" t="str">
-        <f t="shared" si="8"/>
-        <v>Redirect%n🔓👊📷🔊🔊%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nDash%n🔊➜➜</v>
+        <f t="shared" si="6"/>
+        <v>Redirect%n🔓👊📷🔊🔊/Strongarm%n🔓👊🔊🔊➜/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Dash%n🔊➜➜</v>
       </c>
       <c r="AB4" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AC4" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="AD4" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="AE4" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AF4" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AG4" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AH4" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AI4" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ4" s="54" t="s">
@@ -3631,77 +3636,77 @@
         <v>💡💡</v>
       </c>
       <c r="Q5" s="61" t="str">
+        <f t="shared" si="8"/>
+        <v>Hit%n👊🔊</v>
+      </c>
+      <c r="R5" s="61" t="str">
+        <f t="shared" si="9"/>
+        <v>Run%n🔊🔊➜➜</v>
+      </c>
+      <c r="S5" s="61" t="str">
         <f t="shared" si="10"/>
-        <v>Hit%n👊🔊</v>
-      </c>
-      <c r="R5" s="61" t="str">
+        <v>Bash%n👊👊🔊</v>
+      </c>
+      <c r="T5" s="61" t="str">
         <f t="shared" si="11"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
-      <c r="S5" s="61" t="str">
+      <c r="U5" s="61" t="str">
         <f t="shared" si="12"/>
-        <v>Bash%n👊👊🔊</v>
-      </c>
-      <c r="T5" s="61" t="str">
+        <v>Hit%n👊🔊</v>
+      </c>
+      <c r="V5" s="61" t="str">
         <f t="shared" si="13"/>
-        <v>Run%n🔊🔊➜➜</v>
-      </c>
-      <c r="U5" s="61" t="str">
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="W5" s="63" t="str">
         <f t="shared" si="14"/>
-        <v>Hit%n👊🔊</v>
-      </c>
-      <c r="V5" s="61" t="str">
-        <f t="shared" si="15"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="W5" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>Hit%n👊🔊%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nRun%n🔊🔊➜➜%nHit%n👊🔊%nStudy%n💡💡</v>
+        <v>Hit%n👊🔊/Run%n🔊🔊➜➜/Bash%n👊👊🔊/Run%n🔊🔊➜➜/Hit%n👊🔊/Study%n💡💡</v>
       </c>
       <c r="X5" s="61" t="s">
         <v>115</v>
       </c>
       <c r="Y5" s="62" t="str">
-        <f t="shared" si="7"/>
-        <v>Bash%n👊👊🔊%nRun%n🔊🔊➜➜%nRampage%n👊👊🔊🔊🔊➜➜%nRun%n🔊🔊➜➜%nStrongarm%n🔓👊🔊🔊➜%nStudy%n💡💡</v>
+        <f>IF(X5="(none)","",VLOOKUP(X5,$A$2:$W$19,23,FALSE))</f>
+        <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Rampage%n👊👊🔊🔊🔊➜➜/Run%n🔊🔊➜➜/Strongarm%n🔓👊🔊🔊➜/Study%n💡💡</v>
       </c>
       <c r="Z5" s="61" t="s">
         <v>355</v>
       </c>
       <c r="AA5" s="63" t="str">
-        <f t="shared" si="8"/>
-        <v>Bash%n👊👊🔊%nRun%n🔊🔊➜➜%nDetonate%n🔓👊👊📷🔊⚠%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nStudy%n💡💡</v>
+        <f t="shared" si="6"/>
+        <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Detonate%n🔓👊👊📷🔊⚠/Run%n🔊🔊➜➜/Bash%n👊👊🔊/Study%n💡💡</v>
       </c>
       <c r="AB5" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC5" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AD5" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AE5" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF5" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AG5" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH5" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI5" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="64" t="s">
@@ -3790,77 +3795,77 @@
         <v>🔓🔊</v>
       </c>
       <c r="Q6" s="70" t="str">
+        <f t="shared" si="8"/>
+        <v>Bump%n🔓🔓🔊🔊➜</v>
+      </c>
+      <c r="R6" s="70" t="str">
+        <f t="shared" si="9"/>
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="S6" s="72" t="str">
         <f t="shared" si="10"/>
-        <v>Bump%n🔓🔓🔊🔊➜</v>
-      </c>
-      <c r="R6" s="70" t="str">
+        <v>Pick%n🔓🔊</v>
+      </c>
+      <c r="T6" s="70" t="str">
         <f t="shared" si="11"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="S6" s="72" t="str">
+        <v>Sprint%n🔊🔊➜➜➜</v>
+      </c>
+      <c r="U6" s="72" t="str">
         <f t="shared" si="12"/>
+        <v>Run%n🔊🔊➜➜</v>
+      </c>
+      <c r="V6" s="72" t="str">
+        <f t="shared" si="13"/>
         <v>Pick%n🔓🔊</v>
       </c>
-      <c r="T6" s="70" t="str">
-        <f t="shared" si="13"/>
-        <v>Sprint%n🔊🔊➜➜➜</v>
-      </c>
-      <c r="U6" s="72" t="str">
+      <c r="W6" s="73" t="str">
         <f t="shared" si="14"/>
-        <v>Run%n🔊🔊➜➜</v>
-      </c>
-      <c r="V6" s="72" t="str">
-        <f t="shared" si="15"/>
-        <v>Pick%n🔓🔊</v>
-      </c>
-      <c r="W6" s="73" t="str">
-        <f t="shared" si="6"/>
-        <v>Bump%n🔓🔓🔊🔊➜%nStudy%n💡💡%nPick%n🔓🔊%nSprint%n🔊🔊➜➜➜%nRun%n🔊🔊➜➜%nPick%n🔓🔊</v>
+        <v>Bump%n🔓🔓🔊🔊➜/Study%n💡💡/Pick%n🔓🔊/Sprint%n🔊🔊➜➜➜/Run%n🔊🔊➜➜/Pick%n🔓🔊</v>
       </c>
       <c r="X6" s="72" t="s">
         <v>362</v>
       </c>
       <c r="Y6" s="71" t="str">
-        <f t="shared" si="7"/>
-        <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nPick%n🔓🔊</v>
+        <f>IF(X6="(none)","",VLOOKUP(X6,$A$2:$W$19,23,FALSE))</f>
+        <v>Rake%n🔓🔓🔊➜/Recon%n💡💡🔊🔍/Swipe%n🔓💰/Sprint%n🔊🔊➜➜➜/Dash%n🔊➜➜/Pick%n🔓🔊</v>
       </c>
       <c r="Z6" s="72" t="s">
         <v>138</v>
       </c>
       <c r="AA6" s="73" t="str">
-        <f t="shared" si="8"/>
-        <v>Rake%n🔓🔓🔊➜%nStudy%n💡💡%nSpy Stuff%n🔓👊🔊%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShort%n🔓📷🔊🔊➜</v>
+        <f t="shared" si="6"/>
+        <v>Rake%n🔓🔓🔊➜/Study%n💡💡/Spy Stuff%n🔓👊🔊/Sprint%n🔊🔊➜➜➜/Dash%n🔊➜➜/Short%n🔓📷🔊🔊➜</v>
       </c>
       <c r="AB6" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="AD6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AE6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AH6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="74" t="s">
@@ -3949,77 +3954,77 @@
         <v>📷🔊🔊➜</v>
       </c>
       <c r="Q7" s="129" t="str">
+        <f t="shared" si="8"/>
+        <v>Shatter%n📷📷🔊🔊➜</v>
+      </c>
+      <c r="R7" s="129" t="str">
+        <f t="shared" si="9"/>
+        <v>Sprint%n🔊🔊➜➜➜</v>
+      </c>
+      <c r="S7" s="129" t="str">
         <f t="shared" si="10"/>
-        <v>Shatter%n📷📷🔊🔊➜</v>
-      </c>
-      <c r="R7" s="129" t="str">
+        <v>Smash%n📷🔊🔊➜</v>
+      </c>
+      <c r="T7" s="129" t="str">
         <f t="shared" si="11"/>
-        <v>Sprint%n🔊🔊➜➜➜</v>
-      </c>
-      <c r="S7" s="129" t="str">
+        <v>Discover%n🔍🔍</v>
+      </c>
+      <c r="U7" s="136" t="str">
         <f t="shared" si="12"/>
+        <v>Examine%n💡💡💡🔊</v>
+      </c>
+      <c r="V7" s="136" t="str">
+        <f t="shared" si="13"/>
         <v>Smash%n📷🔊🔊➜</v>
       </c>
-      <c r="T7" s="129" t="str">
-        <f t="shared" si="13"/>
-        <v>Discover%n🔍🔍</v>
-      </c>
-      <c r="U7" s="136" t="str">
+      <c r="W7" s="137" t="str">
         <f t="shared" si="14"/>
-        <v>Examine%n💡💡💡🔊</v>
-      </c>
-      <c r="V7" s="136" t="str">
-        <f t="shared" si="15"/>
-        <v>Smash%n📷🔊🔊➜</v>
-      </c>
-      <c r="W7" s="137" t="str">
-        <f t="shared" si="6"/>
-        <v>Shatter%n📷📷🔊🔊➜%nSprint%n🔊🔊➜➜➜%nSmash%n📷🔊🔊➜%nDiscover%n🔍🔍%nExamine%n💡💡💡🔊%nSmash%n📷🔊🔊➜</v>
+        <v>Shatter%n📷📷🔊🔊➜/Sprint%n🔊🔊➜➜➜/Smash%n📷🔊🔊➜/Discover%n🔍🔍/Examine%n💡💡💡🔊/Smash%n📷🔊🔊➜</v>
       </c>
       <c r="X7" s="136" t="s">
         <v>63</v>
       </c>
       <c r="Y7" s="130" t="str">
-        <f t="shared" si="7"/>
-        <v>Unplug%n📷📷🔊➜%nSprint%n🔊🔊➜➜➜%nDisable%n📷🔊➜%nDiscover%n🔍🔍%nRecon%n💡💡🔊🔍%nDisable%n📷🔊➜</v>
+        <f>IF(X7="(none)","",VLOOKUP(X7,$A$2:$W$19,23,FALSE))</f>
+        <v>Unplug%n📷📷🔊➜/Sprint%n🔊🔊➜➜➜/Disable%n📷🔊➜/Discover%n🔍🔍/Recon%n💡💡🔊🔍/Disable%n📷🔊➜</v>
       </c>
       <c r="Z7" s="136" t="s">
         <v>367</v>
       </c>
       <c r="AA7" s="137" t="str">
-        <f t="shared" si="8"/>
-        <v>Unplug%n📷📷🔊➜%nStride%n🔊➜🔍%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
+        <f t="shared" si="6"/>
+        <v>Unplug%n📷📷🔊➜/Stride%n🔊➜🔍/Disable%n📷🔊➜/Stride%n🔊➜🔍/Study%n💡💡/Disable%n📷🔊➜</v>
       </c>
       <c r="AB7" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="AC7" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="AD7" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AE7" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AF7" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG7" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH7" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AI7" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="138" t="s">
@@ -4108,77 +4113,77 @@
         <v>💰💰🔊</v>
       </c>
       <c r="Q8" s="40" t="str">
+        <f t="shared" si="8"/>
+        <v>Flip%n👊🔊➜</v>
+      </c>
+      <c r="R8" s="42" t="str">
+        <f t="shared" si="9"/>
+        <v>Disable%n📷🔊➜</v>
+      </c>
+      <c r="S8" s="42" t="str">
         <f t="shared" si="10"/>
-        <v>Flip%n👊🔊➜</v>
-      </c>
-      <c r="R8" s="42" t="str">
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="T8" s="42" t="str">
         <f t="shared" si="11"/>
-        <v>Disable%n📷🔊➜</v>
-      </c>
-      <c r="S8" s="42" t="str">
+        <v>Punch%n👊🔊🔊➜</v>
+      </c>
+      <c r="U8" s="42" t="str">
         <f t="shared" si="12"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="T8" s="42" t="str">
+        <v>Smash%n📷🔊🔊➜</v>
+      </c>
+      <c r="V8" s="42" t="str">
         <f t="shared" si="13"/>
-        <v>Punch%n👊🔊🔊➜</v>
-      </c>
-      <c r="U8" s="42" t="str">
+        <v>Ransack%n💰💰🔊</v>
+      </c>
+      <c r="W8" s="44" t="str">
         <f t="shared" si="14"/>
-        <v>Smash%n📷🔊🔊➜</v>
-      </c>
-      <c r="V8" s="42" t="str">
-        <f t="shared" si="15"/>
-        <v>Ransack%n💰💰🔊</v>
-      </c>
-      <c r="W8" s="44" t="str">
-        <f t="shared" si="6"/>
-        <v>Flip%n👊🔊➜%nDisable%n📷🔊➜%nStudy%n💡💡%nPunch%n👊🔊🔊➜%nSmash%n📷🔊🔊➜%nRansack%n💰💰🔊</v>
+        <v>Flip%n👊🔊➜/Disable%n📷🔊➜/Study%n💡💡/Punch%n👊🔊🔊➜/Smash%n📷🔊🔊➜/Ransack%n💰💰🔊</v>
       </c>
       <c r="X8" s="42" t="s">
         <v>139</v>
       </c>
       <c r="Y8" s="45" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X8="(none)","",VLOOKUP(X8,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z8" s="42" t="s">
         <v>139</v>
       </c>
       <c r="AA8" s="43" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB8" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC8" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AD8" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AE8" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AF8" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AG8" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH8" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI8" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AJ8" s="144" t="s">
@@ -4267,77 +4272,77 @@
         <v>💰🔊</v>
       </c>
       <c r="Q9" s="48" t="str">
+        <f t="shared" si="8"/>
+        <v>Punch%n👊🔊🔊➜</v>
+      </c>
+      <c r="R9" s="47" t="str">
+        <f t="shared" si="9"/>
+        <v>Unplug%n📷📷🔊➜</v>
+      </c>
+      <c r="S9" s="47" t="str">
         <f t="shared" si="10"/>
-        <v>Punch%n👊🔊🔊➜</v>
-      </c>
-      <c r="R9" s="47" t="str">
+        <v>Key In%n🔍🔓🔊</v>
+      </c>
+      <c r="T9" s="48" t="str">
         <f t="shared" si="11"/>
-        <v>Unplug%n📷📷🔊➜</v>
-      </c>
-      <c r="S9" s="47" t="str">
+        <v>Flip%n👊🔊➜</v>
+      </c>
+      <c r="U9" s="48" t="str">
         <f t="shared" si="12"/>
-        <v>Key In%n🔍🔓🔊</v>
-      </c>
-      <c r="T9" s="48" t="str">
+        <v>Disable%n📷🔊➜</v>
+      </c>
+      <c r="V9" s="48" t="str">
         <f t="shared" si="13"/>
-        <v>Flip%n👊🔊➜</v>
-      </c>
-      <c r="U9" s="48" t="str">
+        <v>Grab%n💰🔊</v>
+      </c>
+      <c r="W9" s="44" t="str">
         <f t="shared" si="14"/>
-        <v>Disable%n📷🔊➜</v>
-      </c>
-      <c r="V9" s="48" t="str">
-        <f t="shared" si="15"/>
-        <v>Grab%n💰🔊</v>
-      </c>
-      <c r="W9" s="44" t="str">
-        <f t="shared" si="6"/>
-        <v>Punch%n👊🔊🔊➜%nUnplug%n📷📷🔊➜%nKey In%n🔍🔓🔊%nFlip%n👊🔊➜%nDisable%n📷🔊➜%nGrab%n💰🔊</v>
+        <v>Punch%n👊🔊🔊➜/Unplug%n📷📷🔊➜/Key In%n🔍🔓🔊/Flip%n👊🔊➜/Disable%n📷🔊➜/Grab%n💰🔊</v>
       </c>
       <c r="X9" s="47" t="s">
         <v>139</v>
       </c>
       <c r="Y9" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X9="(none)","",VLOOKUP(X9,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z9" s="47" t="s">
         <v>139</v>
       </c>
       <c r="AA9" s="43" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB9" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AC9" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AD9" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AE9" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="AF9" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AG9" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AH9" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AI9" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ9" s="46" t="s">
@@ -4426,77 +4431,77 @@
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q10" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>Dash%n🔊➜➜</v>
+      </c>
+      <c r="R10" s="37" t="str">
+        <f t="shared" si="9"/>
+        <v>Pick%n🔓🔊</v>
+      </c>
+      <c r="S10" s="37" t="str">
         <f t="shared" si="10"/>
-        <v>Dash%n🔊➜➜</v>
-      </c>
-      <c r="R10" s="37" t="str">
+        <v>Sleeper Hold%n👊➜</v>
+      </c>
+      <c r="T10" s="38" t="str">
         <f t="shared" si="11"/>
-        <v>Pick%n🔓🔊</v>
-      </c>
-      <c r="S10" s="37" t="str">
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="U10" s="38" t="str">
         <f t="shared" si="12"/>
-        <v>Sleeper Hold%n👊➜</v>
-      </c>
-      <c r="T10" s="38" t="str">
+        <v>Sprint%n🔊🔊➜➜➜</v>
+      </c>
+      <c r="V10" s="38" t="str">
         <f t="shared" si="13"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="U10" s="38" t="str">
+        <v>Examine%n💡💡💡🔊</v>
+      </c>
+      <c r="W10" s="35" t="str">
         <f t="shared" si="14"/>
-        <v>Sprint%n🔊🔊➜➜➜</v>
-      </c>
-      <c r="V10" s="38" t="str">
-        <f t="shared" si="15"/>
-        <v>Examine%n💡💡💡🔊</v>
-      </c>
-      <c r="W10" s="35" t="str">
-        <f t="shared" si="6"/>
-        <v>Dash%n🔊➜➜%nPick%n🔓🔊%nSleeper Hold%n👊➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Dash%n🔊➜➜/Pick%n🔓🔊/Sleeper Hold%n👊➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="X10" s="37" t="s">
         <v>139</v>
       </c>
       <c r="Y10" s="35" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X10="(none)","",VLOOKUP(X10,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z10" s="37" t="s">
         <v>139</v>
       </c>
       <c r="AA10" s="35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB10" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="AC10" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="AD10" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AE10" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF10" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AG10" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AH10" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI10" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ10" s="146" t="s">
@@ -4585,77 +4590,77 @@
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q11" s="38" t="str">
+        <f t="shared" si="8"/>
+        <v>Dash%n🔊➜➜</v>
+      </c>
+      <c r="R11" s="38" t="str">
+        <f t="shared" si="9"/>
+        <v>Pick%n🔓🔊</v>
+      </c>
+      <c r="S11" s="37" t="str">
         <f t="shared" si="10"/>
-        <v>Dash%n🔊➜➜</v>
-      </c>
-      <c r="R11" s="38" t="str">
+        <v>Sneak%n📷🔊➜➜</v>
+      </c>
+      <c r="T11" s="38" t="str">
         <f t="shared" si="11"/>
-        <v>Pick%n🔓🔊</v>
-      </c>
-      <c r="S11" s="37" t="str">
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="U11" s="38" t="str">
         <f t="shared" si="12"/>
-        <v>Sneak%n📷🔊➜➜</v>
-      </c>
-      <c r="T11" s="38" t="str">
+        <v>Sprint%n🔊🔊➜➜➜</v>
+      </c>
+      <c r="V11" s="37" t="str">
         <f t="shared" si="13"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="U11" s="38" t="str">
+        <v>Examine%n💡💡💡🔊</v>
+      </c>
+      <c r="W11" s="35" t="str">
         <f t="shared" si="14"/>
-        <v>Sprint%n🔊🔊➜➜➜</v>
-      </c>
-      <c r="V11" s="37" t="str">
-        <f t="shared" si="15"/>
-        <v>Examine%n💡💡💡🔊</v>
-      </c>
-      <c r="W11" s="35" t="str">
-        <f t="shared" si="6"/>
-        <v>Dash%n🔊➜➜%nPick%n🔓🔊%nSneak%n📷🔊➜➜%nStudy%n💡💡%nSprint%n🔊🔊➜➜➜%nExamine%n💡💡💡🔊</v>
+        <v>Dash%n🔊➜➜/Pick%n🔓🔊/Sneak%n📷🔊➜➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="X11" s="37" t="s">
         <v>139</v>
       </c>
       <c r="Y11" s="35" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X11="(none)","",VLOOKUP(X11,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z11" s="37" t="s">
         <v>139</v>
       </c>
       <c r="AA11" s="35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB11" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="AC11" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AD11" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AE11" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AF11" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG11" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AH11" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI11" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="146" t="s">
@@ -4744,77 +4749,77 @@
         <v>🔊🔊➜➜</v>
       </c>
       <c r="Q12" s="52" t="str">
+        <f t="shared" si="8"/>
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="R12" s="52" t="str">
+        <f t="shared" si="9"/>
+        <v>Spy Stuff%n🔓👊🔊</v>
+      </c>
+      <c r="S12" s="50" t="str">
         <f t="shared" si="10"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="R12" s="52" t="str">
+        <v>Short%n🔓📷🔊🔊➜</v>
+      </c>
+      <c r="T12" s="52" t="str">
         <f t="shared" si="11"/>
-        <v>Spy Stuff%n🔓👊🔊</v>
-      </c>
-      <c r="S12" s="50" t="str">
+        <v>Zap%n👊📷🔊🔊➜</v>
+      </c>
+      <c r="U12" s="50" t="str">
         <f t="shared" si="12"/>
-        <v>Short%n🔓📷🔊🔊➜</v>
-      </c>
-      <c r="T12" s="52" t="str">
+        <v>Grab%n💰🔊</v>
+      </c>
+      <c r="V12" s="52" t="str">
         <f t="shared" si="13"/>
-        <v>Zap%n👊📷🔊🔊➜</v>
-      </c>
-      <c r="U12" s="50" t="str">
+        <v>Run%n🔊🔊➜➜</v>
+      </c>
+      <c r="W12" s="56" t="str">
         <f t="shared" si="14"/>
-        <v>Grab%n💰🔊</v>
-      </c>
-      <c r="V12" s="52" t="str">
-        <f t="shared" si="15"/>
-        <v>Run%n🔊🔊➜➜</v>
-      </c>
-      <c r="W12" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Study%n💡💡%nSpy Stuff%n🔓👊🔊%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nRun%n🔊🔊➜➜</v>
+        <v>Study%n💡💡/Spy Stuff%n🔓👊🔊/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Run%n🔊🔊➜➜</v>
       </c>
       <c r="X12" s="52" t="s">
         <v>139</v>
       </c>
       <c r="Y12" s="57" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X12="(none)","",VLOOKUP(X12,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z12" s="52" t="s">
         <v>139</v>
       </c>
       <c r="AA12" s="56" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB12" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC12" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="AD12" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AE12" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AF12" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AG12" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AH12" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI12" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ12" s="54" t="s">
@@ -4903,77 +4908,77 @@
         <v>🔊➜➜</v>
       </c>
       <c r="Q13" s="60" t="str">
+        <f t="shared" si="8"/>
+        <v>Redirect%n🔓👊📷🔊🔊</v>
+      </c>
+      <c r="R13" s="59" t="str">
+        <f t="shared" si="9"/>
+        <v>Strongarm%n🔓👊🔊🔊➜</v>
+      </c>
+      <c r="S13" s="59" t="str">
         <f t="shared" si="10"/>
-        <v>Redirect%n🔓👊📷🔊🔊</v>
-      </c>
-      <c r="R13" s="59" t="str">
+        <v>Short%n🔓📷🔊🔊➜</v>
+      </c>
+      <c r="T13" s="59" t="str">
         <f t="shared" si="11"/>
-        <v>Strongarm%n🔓👊🔊🔊➜</v>
-      </c>
-      <c r="S13" s="59" t="str">
+        <v>Zap%n👊📷🔊🔊➜</v>
+      </c>
+      <c r="U13" s="60" t="str">
         <f t="shared" si="12"/>
-        <v>Short%n🔓📷🔊🔊➜</v>
-      </c>
-      <c r="T13" s="59" t="str">
+        <v>Grab%n💰🔊</v>
+      </c>
+      <c r="V13" s="60" t="str">
         <f t="shared" si="13"/>
-        <v>Zap%n👊📷🔊🔊➜</v>
-      </c>
-      <c r="U13" s="60" t="str">
+        <v>Dash%n🔊➜➜</v>
+      </c>
+      <c r="W13" s="56" t="str">
         <f t="shared" si="14"/>
-        <v>Grab%n💰🔊</v>
-      </c>
-      <c r="V13" s="60" t="str">
-        <f t="shared" si="15"/>
-        <v>Dash%n🔊➜➜</v>
-      </c>
-      <c r="W13" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Redirect%n🔓👊📷🔊🔊%nStrongarm%n🔓👊🔊🔊➜%nShort%n🔓📷🔊🔊➜%nZap%n👊📷🔊🔊➜%nGrab%n💰🔊%nDash%n🔊➜➜</v>
+        <v>Redirect%n🔓👊📷🔊🔊/Strongarm%n🔓👊🔊🔊➜/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Dash%n🔊➜➜</v>
       </c>
       <c r="X13" s="59" t="s">
         <v>139</v>
       </c>
       <c r="Y13" s="57" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X13="(none)","",VLOOKUP(X13,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z13" s="59" t="s">
         <v>139</v>
       </c>
       <c r="AA13" s="56" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB13" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AC13" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="AD13" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="AE13" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="AF13" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="AG13" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="AH13" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI13" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ13" s="54" t="s">
@@ -5062,77 +5067,77 @@
         <v>💡💡</v>
       </c>
       <c r="Q14" s="66" t="str">
+        <f t="shared" si="8"/>
+        <v>Bash%n👊👊🔊</v>
+      </c>
+      <c r="R14" s="67" t="str">
+        <f t="shared" si="9"/>
+        <v>Run%n🔊🔊➜➜</v>
+      </c>
+      <c r="S14" s="67" t="str">
         <f t="shared" si="10"/>
-        <v>Bash%n👊👊🔊</v>
-      </c>
-      <c r="R14" s="67" t="str">
+        <v>Rampage%n👊👊🔊🔊🔊➜➜</v>
+      </c>
+      <c r="T14" s="61" t="str">
         <f t="shared" si="11"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
-      <c r="S14" s="67" t="str">
+      <c r="U14" s="66" t="str">
         <f t="shared" si="12"/>
-        <v>Rampage%n👊👊🔊🔊🔊➜➜</v>
-      </c>
-      <c r="T14" s="61" t="str">
+        <v>Strongarm%n🔓👊🔊🔊➜</v>
+      </c>
+      <c r="V14" s="67" t="str">
         <f t="shared" si="13"/>
-        <v>Run%n🔊🔊➜➜</v>
-      </c>
-      <c r="U14" s="66" t="str">
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="W14" s="68" t="str">
         <f t="shared" si="14"/>
-        <v>Strongarm%n🔓👊🔊🔊➜</v>
-      </c>
-      <c r="V14" s="67" t="str">
-        <f t="shared" si="15"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="W14" s="68" t="str">
-        <f t="shared" si="6"/>
-        <v>Bash%n👊👊🔊%nRun%n🔊🔊➜➜%nRampage%n👊👊🔊🔊🔊➜➜%nRun%n🔊🔊➜➜%nStrongarm%n🔓👊🔊🔊➜%nStudy%n💡💡</v>
+        <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Rampage%n👊👊🔊🔊🔊➜➜/Run%n🔊🔊➜➜/Strongarm%n🔓👊🔊🔊➜/Study%n💡💡</v>
       </c>
       <c r="X14" s="66" t="s">
         <v>139</v>
       </c>
       <c r="Y14" s="63" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X14="(none)","",VLOOKUP(X14,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z14" s="66" t="s">
         <v>139</v>
       </c>
       <c r="AA14" s="63" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB14" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC14" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="AD14" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AE14" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF14" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="AG14" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AH14" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI14" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="64" t="s">
@@ -5221,77 +5226,77 @@
         <v>💡💡</v>
       </c>
       <c r="Q15" s="66" t="str">
+        <f t="shared" si="8"/>
+        <v>Bash%n👊👊🔊</v>
+      </c>
+      <c r="R15" s="61" t="str">
+        <f t="shared" si="9"/>
+        <v>Run%n🔊🔊➜➜</v>
+      </c>
+      <c r="S15" s="66" t="str">
         <f t="shared" si="10"/>
-        <v>Bash%n👊👊🔊</v>
-      </c>
-      <c r="R15" s="61" t="str">
+        <v>Detonate%n🔓👊👊📷🔊⚠</v>
+      </c>
+      <c r="T15" s="66" t="str">
         <f t="shared" si="11"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
-      <c r="S15" s="66" t="str">
+      <c r="U15" s="66" t="str">
         <f t="shared" si="12"/>
-        <v>Detonate%n🔓👊👊📷🔊⚠</v>
-      </c>
-      <c r="T15" s="66" t="str">
+        <v>Bash%n👊👊🔊</v>
+      </c>
+      <c r="V15" s="67" t="str">
         <f t="shared" si="13"/>
-        <v>Run%n🔊🔊➜➜</v>
-      </c>
-      <c r="U15" s="66" t="str">
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="W15" s="68" t="str">
         <f t="shared" si="14"/>
-        <v>Bash%n👊👊🔊</v>
-      </c>
-      <c r="V15" s="67" t="str">
-        <f t="shared" si="15"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="W15" s="68" t="str">
-        <f t="shared" si="6"/>
-        <v>Bash%n👊👊🔊%nRun%n🔊🔊➜➜%nDetonate%n🔓👊👊📷🔊⚠%nRun%n🔊🔊➜➜%nBash%n👊👊🔊%nStudy%n💡💡</v>
+        <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Detonate%n🔓👊👊📷🔊⚠/Run%n🔊🔊➜➜/Bash%n👊👊🔊/Study%n💡💡</v>
       </c>
       <c r="X15" s="66" t="s">
         <v>139</v>
       </c>
       <c r="Y15" s="63" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X15="(none)","",VLOOKUP(X15,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z15" s="66" t="s">
         <v>139</v>
       </c>
       <c r="AA15" s="63" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB15" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC15" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AD15" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AE15" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AF15" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AG15" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AH15" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI15" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="64" t="s">
@@ -5378,77 +5383,77 @@
         <v>🔓🔊</v>
       </c>
       <c r="Q16" s="72" t="str">
+        <f t="shared" si="8"/>
+        <v>Rake%n🔓🔓🔊➜</v>
+      </c>
+      <c r="R16" s="70" t="str">
+        <f t="shared" si="9"/>
+        <v>Recon%n💡💡🔊🔍</v>
+      </c>
+      <c r="S16" s="70" t="str">
         <f t="shared" si="10"/>
-        <v>Rake%n🔓🔓🔊➜</v>
-      </c>
-      <c r="R16" s="70" t="str">
+        <v>Swipe%n🔓💰</v>
+      </c>
+      <c r="T16" s="76" t="str">
         <f t="shared" si="11"/>
-        <v>Recon%n💡💡🔊🔍</v>
-      </c>
-      <c r="S16" s="70" t="str">
+        <v>Sprint%n🔊🔊➜➜➜</v>
+      </c>
+      <c r="U16" s="76" t="str">
         <f t="shared" si="12"/>
-        <v>Swipe%n🔓💰</v>
-      </c>
-      <c r="T16" s="76" t="str">
+        <v>Dash%n🔊➜➜</v>
+      </c>
+      <c r="V16" s="76" t="str">
         <f t="shared" si="13"/>
-        <v>Sprint%n🔊🔊➜➜➜</v>
-      </c>
-      <c r="U16" s="76" t="str">
+        <v>Pick%n🔓🔊</v>
+      </c>
+      <c r="W16" s="78" t="str">
         <f t="shared" si="14"/>
-        <v>Dash%n🔊➜➜</v>
-      </c>
-      <c r="V16" s="76" t="str">
-        <f t="shared" si="15"/>
-        <v>Pick%n🔓🔊</v>
-      </c>
-      <c r="W16" s="78" t="str">
-        <f t="shared" si="6"/>
-        <v>Rake%n🔓🔓🔊➜%nRecon%n💡💡🔊🔍%nSwipe%n🔓💰%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nPick%n🔓🔊</v>
+        <v>Rake%n🔓🔓🔊➜/Recon%n💡💡🔊🔍/Swipe%n🔓💰/Sprint%n🔊🔊➜➜➜/Dash%n🔊➜➜/Pick%n🔓🔊</v>
       </c>
       <c r="X16" s="72" t="s">
         <v>139</v>
       </c>
       <c r="Y16" s="77" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X16="(none)","",VLOOKUP(X16,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z16" s="72" t="s">
         <v>139</v>
       </c>
       <c r="AA16" s="78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB16" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC16" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AD16" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AE16" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF16" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG16" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AH16" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AI16" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ16" s="74" t="s">
@@ -5537,77 +5542,77 @@
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="Q17" s="72" t="str">
+        <f t="shared" si="8"/>
+        <v>Rake%n🔓🔓🔊➜</v>
+      </c>
+      <c r="R17" s="72" t="str">
+        <f t="shared" si="9"/>
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="S17" s="70" t="str">
         <f t="shared" si="10"/>
-        <v>Rake%n🔓🔓🔊➜</v>
-      </c>
-      <c r="R17" s="72" t="str">
+        <v>Spy Stuff%n🔓👊🔊</v>
+      </c>
+      <c r="T17" s="70" t="str">
         <f t="shared" si="11"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="S17" s="70" t="str">
+        <v>Sprint%n🔊🔊➜➜➜</v>
+      </c>
+      <c r="U17" s="79" t="str">
         <f t="shared" si="12"/>
-        <v>Spy Stuff%n🔓👊🔊</v>
-      </c>
-      <c r="T17" s="70" t="str">
+        <v>Dash%n🔊➜➜</v>
+      </c>
+      <c r="V17" s="70" t="str">
         <f t="shared" si="13"/>
-        <v>Sprint%n🔊🔊➜➜➜</v>
-      </c>
-      <c r="U17" s="79" t="str">
+        <v>Short%n🔓📷🔊🔊➜</v>
+      </c>
+      <c r="W17" s="78" t="str">
         <f t="shared" si="14"/>
-        <v>Dash%n🔊➜➜</v>
-      </c>
-      <c r="V17" s="70" t="str">
-        <f t="shared" si="15"/>
-        <v>Short%n🔓📷🔊🔊➜</v>
-      </c>
-      <c r="W17" s="78" t="str">
-        <f t="shared" si="6"/>
-        <v>Rake%n🔓🔓🔊➜%nStudy%n💡💡%nSpy Stuff%n🔓👊🔊%nSprint%n🔊🔊➜➜➜%nDash%n🔊➜➜%nShort%n🔓📷🔊🔊➜</v>
+        <v>Rake%n🔓🔓🔊➜/Study%n💡💡/Spy Stuff%n🔓👊🔊/Sprint%n🔊🔊➜➜➜/Dash%n🔊➜➜/Short%n🔓📷🔊🔊➜</v>
       </c>
       <c r="X17" s="72" t="s">
         <v>139</v>
       </c>
       <c r="Y17" s="73" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X17="(none)","",VLOOKUP(X17,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z17" s="72" t="s">
         <v>139</v>
       </c>
       <c r="AA17" s="73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB17" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC17" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AD17" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AE17" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AF17" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AG17" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AH17" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI17" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="74" t="s">
@@ -5696,77 +5701,77 @@
         <v>📷🔊➜</v>
       </c>
       <c r="Q18" s="129" t="str">
+        <f t="shared" si="8"/>
+        <v>Unplug%n📷📷🔊➜</v>
+      </c>
+      <c r="R18" s="129" t="str">
+        <f t="shared" si="9"/>
+        <v>Sprint%n🔊🔊➜➜➜</v>
+      </c>
+      <c r="S18" s="129" t="str">
         <f t="shared" si="10"/>
-        <v>Unplug%n📷📷🔊➜</v>
-      </c>
-      <c r="R18" s="129" t="str">
+        <v>Disable%n📷🔊➜</v>
+      </c>
+      <c r="T18" s="129" t="str">
         <f t="shared" si="11"/>
-        <v>Sprint%n🔊🔊➜➜➜</v>
-      </c>
-      <c r="S18" s="129" t="str">
+        <v>Discover%n🔍🔍</v>
+      </c>
+      <c r="U18" s="129" t="str">
         <f t="shared" si="12"/>
+        <v>Recon%n💡💡🔊🔍</v>
+      </c>
+      <c r="V18" s="136" t="str">
+        <f t="shared" si="13"/>
         <v>Disable%n📷🔊➜</v>
       </c>
-      <c r="T18" s="129" t="str">
-        <f t="shared" si="13"/>
-        <v>Discover%n🔍🔍</v>
-      </c>
-      <c r="U18" s="129" t="str">
+      <c r="W18" s="140" t="str">
         <f t="shared" si="14"/>
-        <v>Recon%n💡💡🔊🔍</v>
-      </c>
-      <c r="V18" s="136" t="str">
-        <f t="shared" si="15"/>
-        <v>Disable%n📷🔊➜</v>
-      </c>
-      <c r="W18" s="140" t="str">
-        <f t="shared" si="6"/>
-        <v>Unplug%n📷📷🔊➜%nSprint%n🔊🔊➜➜➜%nDisable%n📷🔊➜%nDiscover%n🔍🔍%nRecon%n💡💡🔊🔍%nDisable%n📷🔊➜</v>
+        <v>Unplug%n📷📷🔊➜/Sprint%n🔊🔊➜➜➜/Disable%n📷🔊➜/Discover%n🔍🔍/Recon%n💡💡🔊🔍/Disable%n📷🔊➜</v>
       </c>
       <c r="X18" s="136" t="s">
         <v>139</v>
       </c>
       <c r="Y18" s="141" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X18="(none)","",VLOOKUP(X18,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z18" s="136" t="s">
         <v>139</v>
       </c>
       <c r="AA18" s="140" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB18" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC18" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="AD18" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="AE18" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="AF18" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AG18" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AH18" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="AI18" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ18" s="138" t="s">
@@ -5852,77 +5857,77 @@
         <v>📷🔊➜</v>
       </c>
       <c r="Q19" s="143" t="str">
+        <f t="shared" si="8"/>
+        <v>Unplug%n📷📷🔊➜</v>
+      </c>
+      <c r="R19" s="129" t="str">
+        <f t="shared" si="9"/>
+        <v>Stride%n🔊➜🔍</v>
+      </c>
+      <c r="S19" s="129" t="str">
         <f t="shared" si="10"/>
-        <v>Unplug%n📷📷🔊➜</v>
-      </c>
-      <c r="R19" s="129" t="str">
+        <v>Disable%n📷🔊➜</v>
+      </c>
+      <c r="T19" s="129" t="str">
         <f t="shared" si="11"/>
         <v>Stride%n🔊➜🔍</v>
       </c>
-      <c r="S19" s="129" t="str">
+      <c r="U19" s="129" t="str">
         <f t="shared" si="12"/>
+        <v>Study%n💡💡</v>
+      </c>
+      <c r="V19" s="129" t="str">
+        <f t="shared" si="13"/>
         <v>Disable%n📷🔊➜</v>
       </c>
-      <c r="T19" s="129" t="str">
-        <f t="shared" si="13"/>
-        <v>Stride%n🔊➜🔍</v>
-      </c>
-      <c r="U19" s="129" t="str">
+      <c r="W19" s="140" t="str">
         <f t="shared" si="14"/>
-        <v>Study%n💡💡</v>
-      </c>
-      <c r="V19" s="129" t="str">
-        <f t="shared" si="15"/>
-        <v>Disable%n📷🔊➜</v>
-      </c>
-      <c r="W19" s="140" t="str">
-        <f t="shared" si="6"/>
-        <v>Unplug%n📷📷🔊➜%nStride%n🔊➜🔍%nDisable%n📷🔊➜%nStride%n🔊➜🔍%nStudy%n💡💡%nDisable%n📷🔊➜</v>
+        <v>Unplug%n📷📷🔊➜/Stride%n🔊➜🔍/Disable%n📷🔊➜/Stride%n🔊➜🔍/Study%n💡💡/Disable%n📷🔊➜</v>
       </c>
       <c r="X19" s="136" t="s">
         <v>139</v>
       </c>
       <c r="Y19" s="137" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(X19="(none)","",VLOOKUP(X19,$A$2:$W$19,23,FALSE))</f>
         <v/>
       </c>
       <c r="Z19" s="136" t="s">
         <v>139</v>
       </c>
       <c r="AA19" s="137" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB19" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AC19" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="AD19" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="AE19" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="AF19" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AG19" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AH19" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AI19" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ19" s="138" t="s">

</xml_diff>

<commit_message>
characters: revised angry locksmith to be pickier
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="407">
   <si>
     <t>Name</t>
   </si>
@@ -598,15 +598,9 @@
     <t>I CAN HEARTBLEED%nIf outdoors, may spend 💡 to 🔍</t>
   </si>
   <si>
-    <t>PICKER%nGain 💡 when you 🔓</t>
-  </si>
-  <si>
     <t>EARLY WARNING%nWhen outdoors, may 🔍 once per turn%n %nMISDIRECT%nOnce per heist, may use 💡💡💡 to change the security roll by 1.</t>
   </si>
   <si>
-    <t>PICKER%nGain 💡 when you 🔓%n %nI'LL WALK YOU THROUGH IT%nMay use  💡💡 to enable one player to 🔓</t>
-  </si>
-  <si>
     <t>DIG!%nMay begin the heist on any non-security tile on bordering the outside of the map for 🔊🔊</t>
   </si>
   <si>
@@ -1240,9 +1234,6 @@
     <t>Hit</t>
   </si>
   <si>
-    <t>PICKER%nGain 💡 when you 🔓%n %nBREACH%nMay spend your action and💡💡💡💡 to create a new Exit on an open, external side of the current tile. Initiate Escape phase immediately.</t>
-  </si>
-  <si>
     <t>ADRENALINE%nGain 💡 when you 👊%n %nBRING IT ON%nBash gets an additional 🔓 after Reinforcements event triggered.</t>
   </si>
   <si>
@@ -1253,6 +1244,12 @@
   </si>
   <si>
     <t>BOLT%nUse this action to spend 💡for 🔊➜➜, %nor 💡💡 for 🔊➜➜➜</t>
+  </si>
+  <si>
+    <t>EFFICIENT PICKER%nIf your action has a 🔓, you may spend 💡 for an additional ➜🔊</t>
+  </si>
+  <si>
+    <t>EFFICIENT PICKER%nIf your action has a 🔓, you may spend 💡 for an additional ➜🔊%n %nBREACH%nMay spend your action and💡💡💡💡 to create a new Exit on an open, external side of the current tile. Initiate Escape phase immediately.</t>
   </si>
 </sst>
 </file>
@@ -2172,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2220,7 +2217,7 @@
         <v>141</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J1" s="32" t="s">
         <v>152</v>
@@ -2258,17 +2255,17 @@
         <v>142</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>189</v>
+        <v>405</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>81</v>
@@ -2297,13 +2294,13 @@
         <v>142</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>191</v>
+        <v>405</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>81</v>
@@ -2311,7 +2308,7 @@
     </row>
     <row r="4" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>157</v>
@@ -2332,15 +2329,15 @@
         <v>142</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>81</v>
@@ -2373,13 +2370,13 @@
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="M5" s="20" t="s">
         <v>81</v>
@@ -2387,7 +2384,7 @@
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>25</v>
@@ -2414,7 +2411,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>81</v>
@@ -2443,13 +2440,13 @@
         <v>142</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="M7" s="20" t="s">
         <v>81</v>
@@ -2460,7 +2457,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
@@ -2488,7 +2485,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>81</v>
@@ -2499,7 +2496,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2523,7 +2520,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="M9" s="19"/>
     </row>
@@ -2532,7 +2529,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -2547,16 +2544,16 @@
         <v>3</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>81</v>
@@ -2582,10 +2579,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="24" t="s">
@@ -2595,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M11" s="22"/>
     </row>
@@ -2619,16 +2616,16 @@
         <v>6</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>81</v>
@@ -2654,16 +2651,16 @@
         <v>6</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>81</v>
@@ -2692,7 +2689,7 @@
         <v>142</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>132</v>
@@ -2704,7 +2701,7 @@
         <v>15</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>81</v>
@@ -2733,13 +2730,13 @@
         <v>142</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>132</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="M15" s="21" t="s">
         <v>81</v>
@@ -2768,7 +2765,7 @@
         <v>142</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>132</v>
@@ -2776,7 +2773,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>81</v>
@@ -2802,20 +2799,20 @@
         <v>4</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H17" s="27" t="s">
         <v>132</v>
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K17" s="26" t="s">
         <v>39</v>
       </c>
       <c r="L17" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M17" s="23" t="s">
         <v>81</v>
@@ -2823,7 +2820,7 @@
     </row>
     <row r="18" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>151</v>
@@ -2841,14 +2838,14 @@
         <v>3</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H18" s="27" t="s">
         <v>131</v>
       </c>
       <c r="I18" s="27"/>
       <c r="L18" s="23" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M18" s="23" t="s">
         <v>81</v>
@@ -2874,14 +2871,14 @@
         <v>5</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I19" s="27"/>
       <c r="L19" s="23" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="M19" s="23" t="s">
         <v>81</v>
@@ -2906,7 +2903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2971,40 +2968,40 @@
         <v>164</v>
       </c>
       <c r="E1" s="99" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F1" s="95" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G1" s="112" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" s="94" t="s">
+        <v>263</v>
+      </c>
+      <c r="I1" s="99" t="s">
         <v>264</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="J1" s="95" t="s">
         <v>265</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="K1" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="J1" s="95" t="s">
+      <c r="L1" s="94" t="s">
         <v>267</v>
       </c>
-      <c r="K1" s="112" t="s">
+      <c r="M1" s="99" t="s">
         <v>268</v>
       </c>
-      <c r="L1" s="94" t="s">
+      <c r="N1" s="95" t="s">
         <v>269</v>
       </c>
-      <c r="M1" s="99" t="s">
+      <c r="O1" s="112" t="s">
         <v>270</v>
       </c>
-      <c r="N1" s="95" t="s">
+      <c r="P1" s="95" t="s">
         <v>271</v>
-      </c>
-      <c r="O1" s="112" t="s">
-        <v>272</v>
-      </c>
-      <c r="P1" s="95" t="s">
-        <v>273</v>
       </c>
       <c r="Q1" s="94">
         <v>1</v>
@@ -3064,16 +3061,16 @@
         <v>155</v>
       </c>
       <c r="AJ1" s="93" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AK1" s="93" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AL1" s="93" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AM1" s="93" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AN1" s="147"/>
       <c r="AO1" s="147"/>
@@ -3107,42 +3104,42 @@
         <v>126</v>
       </c>
       <c r="E2" s="100" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F2" s="81" t="str">
         <f t="shared" ref="F2:F19" si="0">VLOOKUP(E2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G2" s="113" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H2" s="41" t="str">
         <f t="shared" ref="H2:H19" si="1">VLOOKUP(G2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="I2" s="100" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J2" s="81" t="str">
         <f t="shared" ref="J2:J19" si="2">VLOOKUP(I2,Actions,2,FALSE)</f>
         <v>🔍🔍</v>
       </c>
       <c r="K2" s="113" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L2" s="41" t="str">
         <f t="shared" ref="L2:L19" si="3">VLOOKUP(K2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M2" s="100" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="N2" s="81" t="str">
         <f t="shared" ref="N2:N19" si="4">VLOOKUP(M2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O2" s="113" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P2" s="81" t="str">
         <f t="shared" ref="P2:P19" si="5">VLOOKUP(O2,Actions,2,FALSE)</f>
@@ -3185,14 +3182,14 @@
         <v>156</v>
       </c>
       <c r="Y2" s="41" t="str">
-        <f>IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" ref="Y2:Y19" si="6">IF(X2="(none)","",VLOOKUP(X2,$A$2:$W$19,23,FALSE))</f>
         <v>Flip%n👊🔊➜/Disable%n📷🔊➜/Study%n💡💡/Punch%n👊🔊🔊➜/Smash%n📷🔊🔊➜/Ransack%n💰💰🔊</v>
       </c>
       <c r="Z2" s="40" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AA2" s="43" t="str">
-        <f t="shared" ref="AA2:AA19" si="6">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" ref="AA2:AA19" si="7">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
         <v>Punch%n👊🔊🔊➜/Unplug%n📷📷🔊➜/Key In%n🔍🔓🔊/Flip%n👊🔊➜/Disable%n📷🔊➜/Grab%n💰🔊</v>
       </c>
       <c r="AB2" s="40">
@@ -3200,44 +3197,44 @@
         <v>0</v>
       </c>
       <c r="AC2" s="40">
-        <f t="shared" ref="AC2:AI17" si="7">(LEN($W2)-LEN(SUBSTITUTE($W2,AC$1,"")))/LEN(AC$1)</f>
+        <f t="shared" ref="AC2:AI17" si="8">(LEN($W2)-LEN(SUBSTITUTE($W2,AC$1,"")))/LEN(AC$1)</f>
         <v>9</v>
       </c>
       <c r="AD2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AE2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AF2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AG2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AI2" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AJ2" s="39" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AK2" s="39" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AL2" s="39" t="s">
         <v>154</v>
       </c>
       <c r="AM2" s="39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AN2" s="149"/>
       <c r="AO2" s="149"/>
@@ -3271,73 +3268,73 @@
         <v>127</v>
       </c>
       <c r="E3" s="102" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F3" s="83" t="str">
         <f t="shared" si="0"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G3" s="115" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H3" s="36" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I3" s="103" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J3" s="83" t="str">
         <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K3" s="121" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L3" s="36" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M3" s="103" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N3" s="83" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O3" s="115" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P3" s="83" t="str">
         <f t="shared" si="5"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q3" s="38" t="str">
-        <f t="shared" ref="Q3:Q19" si="8">E3&amp;"%n"&amp;F3</f>
+        <f t="shared" ref="Q3:Q19" si="9">E3&amp;"%n"&amp;F3</f>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="R3" s="38" t="str">
-        <f t="shared" ref="R3:R19" si="9">G3&amp;"%n"&amp;H3</f>
+        <f t="shared" ref="R3:R19" si="10">G3&amp;"%n"&amp;H3</f>
         <v>Pick%n🔓🔊</v>
       </c>
       <c r="S3" s="38" t="str">
-        <f t="shared" ref="S3:S19" si="10">I3&amp;"%n"&amp;J3</f>
+        <f t="shared" ref="S3:S19" si="11">I3&amp;"%n"&amp;J3</f>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="T3" s="37" t="str">
-        <f t="shared" ref="T3:T19" si="11">K3&amp;"%n"&amp;L3</f>
+        <f t="shared" ref="T3:T19" si="12">K3&amp;"%n"&amp;L3</f>
         <v>Study%n💡💡</v>
       </c>
       <c r="U3" s="38" t="str">
-        <f t="shared" ref="U3:U19" si="12">M3&amp;"%n"&amp;N3</f>
+        <f t="shared" ref="U3:U19" si="13">M3&amp;"%n"&amp;N3</f>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="V3" s="38" t="str">
-        <f t="shared" ref="V3:V19" si="13">O3&amp;"%n"&amp;P3</f>
+        <f t="shared" ref="V3:V19" si="14">O3&amp;"%n"&amp;P3</f>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="W3" s="35" t="str">
-        <f t="shared" ref="W3:W19" si="14">Q3 &amp; "/"
+        <f t="shared" ref="W3:W19" si="15">Q3 &amp; "/"
 &amp; R3 &amp; "/"
 &amp; S3 &amp; "/"
 &amp; T3 &amp; "/"
@@ -3349,59 +3346,59 @@
         <v>36</v>
       </c>
       <c r="Y3" s="36" t="str">
-        <f>IF(X3="(none)","",VLOOKUP(X3,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v>Dash%n🔊➜➜/Pick%n🔓🔊/Sleeper Hold%n👊➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="Z3" s="38" t="s">
         <v>68</v>
       </c>
       <c r="AA3" s="35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Dash%n🔊➜➜/Pick%n🔓🔊/Sneak%n📷🔊➜➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="AB3" s="40">
-        <f t="shared" ref="AB3:AI19" si="15">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
+        <f t="shared" ref="AB3:AI19" si="16">(LEN($W3)-LEN(SUBSTITUTE($W3,AB$1,"")))/LEN(AB$1)</f>
         <v>5</v>
       </c>
       <c r="AC3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="AD3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AE3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AH3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI3" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="33" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AK3" s="33" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AL3" s="33" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AM3" s="33" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AN3" s="149"/>
       <c r="AO3" s="149"/>
@@ -3423,7 +3420,7 @@
     </row>
     <row r="4" spans="1:56" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B4" s="50">
         <v>2</v>
@@ -3432,135 +3429,135 @@
         <v>1</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F4" s="85" t="str">
         <f t="shared" si="0"/>
         <v>🔍🔍</v>
       </c>
       <c r="G4" s="116" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H4" s="51" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="I4" s="105" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J4" s="85" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K4" s="123" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L4" s="51" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M4" s="105" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="N4" s="85" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O4" s="116" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="P4" s="85" t="str">
         <f t="shared" si="5"/>
         <v>🔊🔊🔊➜➜</v>
       </c>
       <c r="Q4" s="50" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Discover%n🔍🔍</v>
       </c>
       <c r="R4" s="52" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Strongarm%n🔓👊🔊🔊➜</v>
       </c>
       <c r="S4" s="52" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Short%n🔓📷🔊🔊➜</v>
       </c>
       <c r="T4" s="50" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Zap%n👊📷🔊🔊➜</v>
       </c>
       <c r="U4" s="50" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Grab%n💰🔊</v>
       </c>
       <c r="V4" s="50" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Scamper%n🔊🔊🔊➜➜</v>
       </c>
       <c r="W4" s="53" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Discover%n🔍🔍/Strongarm%n🔓👊🔊🔊➜/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Scamper%n🔊🔊🔊➜➜</v>
       </c>
       <c r="X4" s="50" t="s">
         <v>174</v>
       </c>
       <c r="Y4" s="51" t="str">
-        <f>IF(X4="(none)","",VLOOKUP(X4,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v>Study%n💡💡/Spy Stuff%n🔓👊🔊/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Run%n🔊🔊➜➜</v>
       </c>
       <c r="Z4" s="50" t="s">
         <v>125</v>
       </c>
       <c r="AA4" s="53" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Redirect%n🔓👊📷🔊🔊/Strongarm%n🔓👊🔊🔊➜/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Dash%n🔊➜➜</v>
       </c>
       <c r="AB4" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="AD4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AE4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AF4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AG4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AH4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AI4" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AJ4" s="54" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AK4" s="54" t="s">
         <v>161</v>
       </c>
       <c r="AL4" s="54" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AM4" s="54" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AN4" s="149"/>
       <c r="AO4" s="149"/>
@@ -3582,7 +3579,7 @@
     </row>
     <row r="5" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B5" s="61">
         <v>2</v>
@@ -3591,135 +3588,135 @@
         <v>1</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E5" s="106" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F5" s="87" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊</v>
       </c>
       <c r="G5" s="117" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H5" s="62" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I5" s="107" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J5" s="87" t="str">
         <f t="shared" si="2"/>
         <v>👊👊🔊</v>
       </c>
       <c r="K5" s="125" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L5" s="62" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M5" s="107" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="N5" s="87" t="str">
         <f t="shared" si="4"/>
         <v>👊🔊</v>
       </c>
       <c r="O5" s="117" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P5" s="87" t="str">
         <f t="shared" si="5"/>
         <v>💡💡</v>
       </c>
       <c r="Q5" s="61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Hit%n👊🔊</v>
       </c>
       <c r="R5" s="61" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="S5" s="61" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Bash%n👊👊🔊</v>
       </c>
       <c r="T5" s="61" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="U5" s="61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Hit%n👊🔊</v>
       </c>
       <c r="V5" s="61" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="W5" s="63" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Hit%n👊🔊/Run%n🔊🔊➜➜/Bash%n👊👊🔊/Run%n🔊🔊➜➜/Hit%n👊🔊/Study%n💡💡</v>
       </c>
       <c r="X5" s="61" t="s">
         <v>115</v>
       </c>
       <c r="Y5" s="62" t="str">
-        <f>IF(X5="(none)","",VLOOKUP(X5,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Rampage%n👊👊🔊🔊🔊➜➜/Run%n🔊🔊➜➜/Strongarm%n🔓👊🔊🔊➜/Study%n💡💡</v>
       </c>
       <c r="Z5" s="61" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AA5" s="63" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Detonate%n🔓👊👊📷🔊⚠/Run%n🔊🔊➜➜/Bash%n👊👊🔊/Study%n💡💡</v>
       </c>
       <c r="AB5" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AD5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AE5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AG5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI5" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="64" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AK5" s="64" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AL5" s="64" t="s">
         <v>161</v>
       </c>
       <c r="AM5" s="64" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AN5" s="149"/>
       <c r="AO5" s="149"/>
@@ -3753,132 +3750,132 @@
         <v>130</v>
       </c>
       <c r="E6" s="108" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F6" s="89" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="G6" s="118" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H6" s="71" t="str">
         <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I6" s="109" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J6" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔓🔊</v>
       </c>
       <c r="K6" s="126" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L6" s="71" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M6" s="109" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N6" s="89" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="O6" s="118" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="P6" s="89" t="str">
         <f t="shared" si="5"/>
         <v>🔓🔊</v>
       </c>
       <c r="Q6" s="70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Bump%n🔓🔓🔊🔊➜</v>
       </c>
       <c r="R6" s="70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="S6" s="72" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Pick%n🔓🔊</v>
       </c>
       <c r="T6" s="70" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="U6" s="72" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="V6" s="72" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Pick%n🔓🔊</v>
       </c>
       <c r="W6" s="73" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Bump%n🔓🔓🔊🔊➜/Study%n💡💡/Pick%n🔓🔊/Sprint%n🔊🔊➜➜➜/Run%n🔊🔊➜➜/Pick%n🔓🔊</v>
       </c>
       <c r="X6" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="Y6" s="71" t="str">
-        <f>IF(X6="(none)","",VLOOKUP(X6,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v>Rake%n🔓🔓🔊➜/Recon%n💡💡🔊🔍/Swipe%n🔓💰/Sprint%n🔊🔊➜➜➜/Dash%n🔊➜➜/Pick%n🔓🔊</v>
       </c>
       <c r="Z6" s="72" t="s">
         <v>138</v>
       </c>
       <c r="AA6" s="73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Rake%n🔓🔓🔊➜/Study%n💡💡/Spy Stuff%n🔓👊🔊/Sprint%n🔊🔊➜➜➜/Dash%n🔊➜➜/Short%n🔓📷🔊🔊➜</v>
       </c>
       <c r="AB6" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="AD6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AE6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AH6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI6" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="74" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AK6" s="74" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AL6" s="74" t="s">
         <v>161</v>
       </c>
       <c r="AM6" s="74" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AN6" s="149"/>
       <c r="AO6" s="149"/>
@@ -3912,132 +3909,132 @@
         <v>59</v>
       </c>
       <c r="E7" s="131" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F7" s="132" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊🔊➜</v>
       </c>
       <c r="G7" s="133" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H7" s="130" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I7" s="134" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="J7" s="132" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="K7" s="135" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L7" s="130" t="str">
         <f t="shared" si="3"/>
         <v>🔍🔍</v>
       </c>
       <c r="M7" s="134" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N7" s="132" t="str">
         <f t="shared" si="4"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="O7" s="133" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P7" s="132" t="str">
         <f t="shared" si="5"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="Q7" s="129" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Shatter%n📷📷🔊🔊➜</v>
       </c>
       <c r="R7" s="129" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="S7" s="129" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Smash%n📷🔊🔊➜</v>
       </c>
       <c r="T7" s="129" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Discover%n🔍🔍</v>
       </c>
       <c r="U7" s="136" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="V7" s="136" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Smash%n📷🔊🔊➜</v>
       </c>
       <c r="W7" s="137" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Shatter%n📷📷🔊🔊➜/Sprint%n🔊🔊➜➜➜/Smash%n📷🔊🔊➜/Discover%n🔍🔍/Examine%n💡💡💡🔊/Smash%n📷🔊🔊➜</v>
       </c>
       <c r="X7" s="136" t="s">
         <v>63</v>
       </c>
       <c r="Y7" s="130" t="str">
-        <f>IF(X7="(none)","",VLOOKUP(X7,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v>Unplug%n📷📷🔊➜/Sprint%n🔊🔊➜➜➜/Disable%n📷🔊➜/Discover%n🔍🔍/Recon%n💡💡🔊🔍/Disable%n📷🔊➜</v>
       </c>
       <c r="Z7" s="136" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AA7" s="137" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Unplug%n📷📷🔊➜/Stride%n🔊➜🔍/Disable%n📷🔊➜/Stride%n🔊➜🔍/Study%n💡💡/Disable%n📷🔊➜</v>
       </c>
       <c r="AB7" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="AC7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="AD7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AE7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AF7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AI7" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="138" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AK7" s="138" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AL7" s="138" t="s">
         <v>168</v>
       </c>
       <c r="AM7" s="138" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AN7" s="150"/>
       <c r="AO7" s="150"/>
@@ -4071,132 +4068,132 @@
         <v>126</v>
       </c>
       <c r="E8" s="101" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F8" s="82" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊➜</v>
       </c>
       <c r="G8" s="114" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H8" s="43" t="str">
         <f t="shared" si="1"/>
         <v>📷🔊➜</v>
       </c>
       <c r="I8" s="101" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J8" s="82" t="str">
         <f t="shared" si="2"/>
         <v>💡💡</v>
       </c>
       <c r="K8" s="114" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L8" s="43" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M8" s="101" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="N8" s="82" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O8" s="114" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="P8" s="82" t="str">
         <f t="shared" si="5"/>
         <v>💰💰🔊</v>
       </c>
       <c r="Q8" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Flip%n👊🔊➜</v>
       </c>
       <c r="R8" s="42" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="S8" s="42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="T8" s="42" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Punch%n👊🔊🔊➜</v>
       </c>
       <c r="U8" s="42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Smash%n📷🔊🔊➜</v>
       </c>
       <c r="V8" s="42" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Ransack%n💰💰🔊</v>
       </c>
       <c r="W8" s="44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Flip%n👊🔊➜/Disable%n📷🔊➜/Study%n💡💡/Punch%n👊🔊🔊➜/Smash%n📷🔊🔊➜/Ransack%n💰💰🔊</v>
       </c>
       <c r="X8" s="42" t="s">
         <v>139</v>
       </c>
       <c r="Y8" s="45" t="str">
-        <f>IF(X8="(none)","",VLOOKUP(X8,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z8" s="42" t="s">
         <v>139</v>
       </c>
       <c r="AA8" s="43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB8" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AD8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AE8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AF8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AG8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI8" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AJ8" s="144" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AK8" s="144" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AL8" s="144" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AM8" s="144" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AN8" s="149"/>
       <c r="AO8" s="149"/>
@@ -4218,7 +4215,7 @@
     </row>
     <row r="9" spans="1:56" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B9" s="47">
         <v>2</v>
@@ -4230,132 +4227,132 @@
         <v>126</v>
       </c>
       <c r="E9" s="101" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F9" s="82" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G9" s="114" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H9" s="43" t="str">
         <f t="shared" si="1"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="I9" s="101" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J9" s="82" t="str">
         <f t="shared" si="2"/>
         <v>🔍🔓🔊</v>
       </c>
       <c r="K9" s="114" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="L9" s="43" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊➜</v>
       </c>
       <c r="M9" s="101" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="N9" s="82" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊➜</v>
       </c>
       <c r="O9" s="114" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P9" s="82" t="str">
         <f t="shared" si="5"/>
         <v>💰🔊</v>
       </c>
       <c r="Q9" s="48" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Punch%n👊🔊🔊➜</v>
       </c>
       <c r="R9" s="47" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Unplug%n📷📷🔊➜</v>
       </c>
       <c r="S9" s="47" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Key In%n🔍🔓🔊</v>
       </c>
       <c r="T9" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Flip%n👊🔊➜</v>
       </c>
       <c r="U9" s="48" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="V9" s="48" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Grab%n💰🔊</v>
       </c>
       <c r="W9" s="44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Punch%n👊🔊🔊➜/Unplug%n📷📷🔊➜/Key In%n🔍🔓🔊/Flip%n👊🔊➜/Disable%n📷🔊➜/Grab%n💰🔊</v>
       </c>
       <c r="X9" s="47" t="s">
         <v>139</v>
       </c>
       <c r="Y9" s="44" t="str">
-        <f>IF(X9="(none)","",VLOOKUP(X9,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z9" s="47" t="s">
         <v>139</v>
       </c>
       <c r="AA9" s="43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB9" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AD9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AE9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="AF9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AG9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AH9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AI9" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AJ9" s="46" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AK9" s="46" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AL9" s="46" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AM9" s="46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AN9" s="150"/>
       <c r="AO9" s="150"/>
@@ -4389,132 +4386,132 @@
         <v>127</v>
       </c>
       <c r="E10" s="103" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F10" s="84" t="str">
         <f t="shared" si="0"/>
         <v>🔊➜➜</v>
       </c>
       <c r="G10" s="115" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H10" s="34" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I10" s="103" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J10" s="84" t="str">
         <f t="shared" si="2"/>
         <v>👊➜</v>
       </c>
       <c r="K10" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L10" s="34" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M10" s="103" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N10" s="84" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O10" s="115" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P10" s="84" t="str">
         <f t="shared" si="5"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q10" s="37" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="R10" s="37" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Pick%n🔓🔊</v>
       </c>
       <c r="S10" s="37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Sleeper Hold%n👊➜</v>
       </c>
       <c r="T10" s="38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="U10" s="38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="V10" s="38" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="W10" s="35" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Dash%n🔊➜➜/Pick%n🔓🔊/Sleeper Hold%n👊➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="X10" s="37" t="s">
         <v>139</v>
       </c>
       <c r="Y10" s="35" t="str">
-        <f>IF(X10="(none)","",VLOOKUP(X10,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z10" s="37" t="s">
         <v>139</v>
       </c>
       <c r="AA10" s="35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB10" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AC10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AD10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AE10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AG10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AH10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI10" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ10" s="146" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="AK10" s="146" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AL10" s="146" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AM10" s="146" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AN10" s="150"/>
       <c r="AO10" s="150"/>
@@ -4548,132 +4545,132 @@
         <v>127</v>
       </c>
       <c r="E11" s="103" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F11" s="84" t="str">
         <f t="shared" si="0"/>
         <v>🔊➜➜</v>
       </c>
       <c r="G11" s="115" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H11" s="35" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I11" s="103" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J11" s="84" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜➜</v>
       </c>
       <c r="K11" s="122" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L11" s="35" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M11" s="103" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N11" s="84" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O11" s="115" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P11" s="84" t="str">
         <f t="shared" si="5"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="Q11" s="38" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="R11" s="38" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Pick%n🔓🔊</v>
       </c>
       <c r="S11" s="37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Sneak%n📷🔊➜➜</v>
       </c>
       <c r="T11" s="38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="U11" s="38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="V11" s="37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Examine%n💡💡💡🔊</v>
       </c>
       <c r="W11" s="35" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Dash%n🔊➜➜/Pick%n🔓🔊/Sneak%n📷🔊➜➜/Study%n💡💡/Sprint%n🔊🔊➜➜➜/Examine%n💡💡💡🔊</v>
       </c>
       <c r="X11" s="37" t="s">
         <v>139</v>
       </c>
       <c r="Y11" s="35" t="str">
-        <f>IF(X11="(none)","",VLOOKUP(X11,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z11" s="37" t="s">
         <v>139</v>
       </c>
       <c r="AA11" s="35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB11" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AC11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AD11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AE11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AF11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AH11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI11" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="146" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AK11" s="145" t="s">
         <v>167</v>
       </c>
       <c r="AL11" s="145" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AM11" s="145" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AN11" s="149"/>
       <c r="AO11" s="149"/>
@@ -4704,135 +4701,135 @@
         <v>2</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E12" s="105" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F12" s="86" t="str">
         <f t="shared" si="0"/>
         <v>💡💡</v>
       </c>
       <c r="G12" s="116" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H12" s="53" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊</v>
       </c>
       <c r="I12" s="105" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J12" s="86" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K12" s="116" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L12" s="53" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M12" s="105" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="N12" s="86" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O12" s="116" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P12" s="86" t="str">
         <f t="shared" si="5"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="Q12" s="52" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="R12" s="52" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Spy Stuff%n🔓👊🔊</v>
       </c>
       <c r="S12" s="50" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Short%n🔓📷🔊🔊➜</v>
       </c>
       <c r="T12" s="52" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Zap%n👊📷🔊🔊➜</v>
       </c>
       <c r="U12" s="50" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Grab%n💰🔊</v>
       </c>
       <c r="V12" s="52" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="W12" s="56" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Study%n💡💡/Spy Stuff%n🔓👊🔊/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Run%n🔊🔊➜➜</v>
       </c>
       <c r="X12" s="52" t="s">
         <v>139</v>
       </c>
       <c r="Y12" s="57" t="str">
-        <f>IF(X12="(none)","",VLOOKUP(X12,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z12" s="52" t="s">
         <v>139</v>
       </c>
       <c r="AA12" s="56" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="AD12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AE12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AF12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AG12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AH12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI12" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AJ12" s="54" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AK12" s="54" t="s">
         <v>168</v>
       </c>
       <c r="AL12" s="54" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AM12" s="54" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AN12" s="149"/>
       <c r="AO12" s="149"/>
@@ -4863,135 +4860,135 @@
         <v>2</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E13" s="105" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F13" s="86" t="str">
         <f t="shared" si="0"/>
         <v>🔓👊📷🔊🔊</v>
       </c>
       <c r="G13" s="116" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H13" s="56" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="I13" s="105" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J13" s="86" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K13" s="124" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L13" s="56" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M13" s="105" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="N13" s="86" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O13" s="116" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="P13" s="86" t="str">
         <f t="shared" si="5"/>
         <v>🔊➜➜</v>
       </c>
       <c r="Q13" s="60" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Redirect%n🔓👊📷🔊🔊</v>
       </c>
       <c r="R13" s="59" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Strongarm%n🔓👊🔊🔊➜</v>
       </c>
       <c r="S13" s="59" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Short%n🔓📷🔊🔊➜</v>
       </c>
       <c r="T13" s="59" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Zap%n👊📷🔊🔊➜</v>
       </c>
       <c r="U13" s="60" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Grab%n💰🔊</v>
       </c>
       <c r="V13" s="60" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="W13" s="56" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Redirect%n🔓👊📷🔊🔊/Strongarm%n🔓👊🔊🔊➜/Short%n🔓📷🔊🔊➜/Zap%n👊📷🔊🔊➜/Grab%n💰🔊/Dash%n🔊➜➜</v>
       </c>
       <c r="X13" s="59" t="s">
         <v>139</v>
       </c>
       <c r="Y13" s="57" t="str">
-        <f>IF(X13="(none)","",VLOOKUP(X13,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z13" s="59" t="s">
         <v>139</v>
       </c>
       <c r="AA13" s="56" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB13" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="AD13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AE13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="AF13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="AG13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="AH13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI13" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AJ13" s="54" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AK13" s="54" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AL13" s="54" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AM13" s="54" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AN13" s="149"/>
       <c r="AO13" s="149"/>
@@ -5022,135 +5019,135 @@
         <v>2</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E14" s="107" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F14" s="88" t="str">
         <f t="shared" si="0"/>
         <v>👊👊🔊</v>
       </c>
       <c r="G14" s="117" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H14" s="63" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I14" s="107" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J14" s="88" t="str">
         <f t="shared" si="2"/>
         <v>👊👊🔊🔊🔊➜➜</v>
       </c>
       <c r="K14" s="117" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L14" s="63" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M14" s="107" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="N14" s="88" t="str">
         <f t="shared" si="4"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="O14" s="117" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P14" s="88" t="str">
         <f t="shared" si="5"/>
         <v>💡💡</v>
       </c>
       <c r="Q14" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Bash%n👊👊🔊</v>
       </c>
       <c r="R14" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="S14" s="67" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Rampage%n👊👊🔊🔊🔊➜➜</v>
       </c>
       <c r="T14" s="61" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="U14" s="66" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Strongarm%n🔓👊🔊🔊➜</v>
       </c>
       <c r="V14" s="67" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="W14" s="68" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Rampage%n👊👊🔊🔊🔊➜➜/Run%n🔊🔊➜➜/Strongarm%n🔓👊🔊🔊➜/Study%n💡💡</v>
       </c>
       <c r="X14" s="66" t="s">
         <v>139</v>
       </c>
       <c r="Y14" s="63" t="str">
-        <f>IF(X14="(none)","",VLOOKUP(X14,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z14" s="66" t="s">
         <v>139</v>
       </c>
       <c r="AA14" s="63" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB14" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="AD14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AE14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AG14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AH14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI14" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="64" t="s">
+        <v>313</v>
+      </c>
+      <c r="AK14" s="64" t="s">
+        <v>341</v>
+      </c>
+      <c r="AL14" s="64" t="s">
+        <v>352</v>
+      </c>
+      <c r="AM14" s="64" t="s">
         <v>315</v>
-      </c>
-      <c r="AK14" s="64" t="s">
-        <v>343</v>
-      </c>
-      <c r="AL14" s="64" t="s">
-        <v>354</v>
-      </c>
-      <c r="AM14" s="64" t="s">
-        <v>317</v>
       </c>
       <c r="AN14" s="149"/>
       <c r="AO14" s="149"/>
@@ -5172,7 +5169,7 @@
     </row>
     <row r="15" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B15" s="66">
         <v>2</v>
@@ -5181,133 +5178,133 @@
         <v>2</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E15" s="107" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F15" s="88" t="str">
         <f t="shared" si="0"/>
         <v>👊👊🔊</v>
       </c>
       <c r="G15" s="117" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H15" s="63" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I15" s="107" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J15" s="88" t="str">
         <f>VLOOKUP(I15,Actions,2,FALSE)</f>
         <v>🔓👊👊📷🔊⚠</v>
       </c>
       <c r="K15" s="117" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L15" s="63" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M15" s="107" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N15" s="88" t="str">
         <f t="shared" si="4"/>
         <v>👊👊🔊</v>
       </c>
       <c r="O15" s="117" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P15" s="88" t="str">
         <f t="shared" si="5"/>
         <v>💡💡</v>
       </c>
       <c r="Q15" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Bash%n👊👊🔊</v>
       </c>
       <c r="R15" s="61" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="S15" s="66" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Detonate%n🔓👊👊📷🔊⚠</v>
       </c>
       <c r="T15" s="66" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Run%n🔊🔊➜➜</v>
       </c>
       <c r="U15" s="66" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Bash%n👊👊🔊</v>
       </c>
       <c r="V15" s="67" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="W15" s="68" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Detonate%n🔓👊👊📷🔊⚠/Run%n🔊🔊➜➜/Bash%n👊👊🔊/Study%n💡💡</v>
       </c>
       <c r="X15" s="66" t="s">
         <v>139</v>
       </c>
       <c r="Y15" s="63" t="str">
-        <f>IF(X15="(none)","",VLOOKUP(X15,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z15" s="66" t="s">
         <v>139</v>
       </c>
       <c r="AA15" s="63" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB15" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AD15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AE15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AF15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AG15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AH15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI15" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="64" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AK15" s="64"/>
       <c r="AL15" s="64" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AM15" s="64" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AN15" s="149"/>
       <c r="AO15" s="149"/>
@@ -5329,7 +5326,7 @@
     </row>
     <row r="16" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B16" s="76">
         <v>2</v>
@@ -5341,132 +5338,132 @@
         <v>130</v>
       </c>
       <c r="E16" s="108" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F16" s="89" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G16" s="118" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H16" s="77" t="str">
         <f t="shared" si="1"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="I16" s="109" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J16" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔓💰</v>
       </c>
       <c r="K16" s="127" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L16" s="77" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M16" s="109" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N16" s="89" t="str">
         <f t="shared" si="4"/>
         <v>🔊➜➜</v>
       </c>
       <c r="O16" s="118" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="P16" s="89" t="str">
         <f t="shared" si="5"/>
         <v>🔓🔊</v>
       </c>
       <c r="Q16" s="72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rake%n🔓🔓🔊➜</v>
       </c>
       <c r="R16" s="70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Recon%n💡💡🔊🔍</v>
       </c>
       <c r="S16" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Swipe%n🔓💰</v>
       </c>
       <c r="T16" s="76" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="U16" s="76" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="V16" s="76" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Pick%n🔓🔊</v>
       </c>
       <c r="W16" s="78" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Rake%n🔓🔓🔊➜/Recon%n💡💡🔊🔍/Swipe%n🔓💰/Sprint%n🔊🔊➜➜➜/Dash%n🔊➜➜/Pick%n🔓🔊</v>
       </c>
       <c r="X16" s="72" t="s">
         <v>139</v>
       </c>
       <c r="Y16" s="77" t="str">
-        <f>IF(X16="(none)","",VLOOKUP(X16,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z16" s="72" t="s">
         <v>139</v>
       </c>
       <c r="AA16" s="78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB16" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AD16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AE16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AH16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AI16" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AJ16" s="74" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AK16" s="74" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AL16" s="74" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AM16" s="74" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AN16" s="149"/>
       <c r="AO16" s="149"/>
@@ -5500,132 +5497,132 @@
         <v>130</v>
       </c>
       <c r="E17" s="109" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F17" s="90" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G17" s="118" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H17" s="73" t="str">
         <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I17" s="109" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J17" s="90" t="str">
         <f t="shared" si="2"/>
         <v>🔓👊🔊</v>
       </c>
       <c r="K17" s="118" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L17" s="73" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M17" s="109" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N17" s="90" t="str">
         <f t="shared" si="4"/>
         <v>🔊➜➜</v>
       </c>
       <c r="O17" s="118" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="P17" s="90" t="str">
         <f t="shared" si="5"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="Q17" s="72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rake%n🔓🔓🔊➜</v>
       </c>
       <c r="R17" s="72" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="S17" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Spy Stuff%n🔓👊🔊</v>
       </c>
       <c r="T17" s="70" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="U17" s="79" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Dash%n🔊➜➜</v>
       </c>
       <c r="V17" s="70" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Short%n🔓📷🔊🔊➜</v>
       </c>
       <c r="W17" s="78" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Rake%n🔓🔓🔊➜/Study%n💡💡/Spy Stuff%n🔓👊🔊/Sprint%n🔊🔊➜➜➜/Dash%n🔊➜➜/Short%n🔓📷🔊🔊➜</v>
       </c>
       <c r="X17" s="72" t="s">
         <v>139</v>
       </c>
       <c r="Y17" s="73" t="str">
-        <f>IF(X17="(none)","",VLOOKUP(X17,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z17" s="72" t="s">
         <v>139</v>
       </c>
       <c r="AA17" s="73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB17" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AD17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AE17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AF17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AG17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AH17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI17" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="74" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AK17" s="74" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="AL17" s="74" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AM17" s="74" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AN17" s="150"/>
       <c r="AO17" s="150"/>
@@ -5659,129 +5656,129 @@
         <v>59</v>
       </c>
       <c r="E18" s="134" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F18" s="139" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="G18" s="133" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H18" s="137" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I18" s="134" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J18" s="139" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K18" s="133" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L18" s="137" t="str">
         <f t="shared" si="3"/>
         <v>🔍🔍</v>
       </c>
       <c r="M18" s="134" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N18" s="139" t="str">
         <f t="shared" si="4"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="O18" s="133" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P18" s="139" t="str">
         <f t="shared" si="5"/>
         <v>📷🔊➜</v>
       </c>
       <c r="Q18" s="129" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Unplug%n📷📷🔊➜</v>
       </c>
       <c r="R18" s="129" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Sprint%n🔊🔊➜➜➜</v>
       </c>
       <c r="S18" s="129" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="T18" s="129" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Discover%n🔍🔍</v>
       </c>
       <c r="U18" s="129" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Recon%n💡💡🔊🔍</v>
       </c>
       <c r="V18" s="136" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="W18" s="140" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Unplug%n📷📷🔊➜/Sprint%n🔊🔊➜➜➜/Disable%n📷🔊➜/Discover%n🔍🔍/Recon%n💡💡🔊🔍/Disable%n📷🔊➜</v>
       </c>
       <c r="X18" s="136" t="s">
         <v>139</v>
       </c>
       <c r="Y18" s="141" t="str">
-        <f>IF(X18="(none)","",VLOOKUP(X18,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z18" s="136" t="s">
         <v>139</v>
       </c>
       <c r="AA18" s="140" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB18" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC18" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="AD18" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="AE18" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="AF18" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG18" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AH18" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="AI18" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AJ18" s="138" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AK18" s="138" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AM18" s="138" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AN18" s="150"/>
       <c r="AO18" s="150"/>
@@ -5803,7 +5800,7 @@
     </row>
     <row r="19" spans="1:56" s="138" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="137" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B19" s="136">
         <v>2</v>
@@ -5815,132 +5812,132 @@
         <v>59</v>
       </c>
       <c r="E19" s="134" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F19" s="139" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="G19" s="133" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H19" s="137" t="str">
         <f t="shared" si="1"/>
         <v>🔊➜🔍</v>
       </c>
       <c r="I19" s="134" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J19" s="139" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K19" s="133" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L19" s="137" t="str">
         <f t="shared" si="3"/>
         <v>🔊➜🔍</v>
       </c>
       <c r="M19" s="134" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N19" s="139" t="str">
         <f t="shared" si="4"/>
         <v>💡💡</v>
       </c>
       <c r="O19" s="133" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P19" s="139" t="str">
         <f t="shared" si="5"/>
         <v>📷🔊➜</v>
       </c>
       <c r="Q19" s="143" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Unplug%n📷📷🔊➜</v>
       </c>
       <c r="R19" s="129" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Stride%n🔊➜🔍</v>
       </c>
       <c r="S19" s="129" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="T19" s="129" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Stride%n🔊➜🔍</v>
       </c>
       <c r="U19" s="129" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Study%n💡💡</v>
       </c>
       <c r="V19" s="129" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Disable%n📷🔊➜</v>
       </c>
       <c r="W19" s="140" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Unplug%n📷📷🔊➜/Stride%n🔊➜🔍/Disable%n📷🔊➜/Stride%n🔊➜🔍/Study%n💡💡/Disable%n📷🔊➜</v>
       </c>
       <c r="X19" s="136" t="s">
         <v>139</v>
       </c>
       <c r="Y19" s="137" t="str">
-        <f>IF(X19="(none)","",VLOOKUP(X19,$A$2:$W$19,23,FALSE))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z19" s="136" t="s">
         <v>139</v>
       </c>
       <c r="AA19" s="137" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB19" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AC19" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AD19" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="AE19" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="AF19" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG19" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AH19" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AI19" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AJ19" s="138" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AK19" s="138" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AL19" s="138" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="AM19" s="138" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AN19" s="150"/>
       <c r="AO19" s="150"/>
@@ -6069,7 +6066,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -6096,7 +6093,7 @@
         <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6112,7 +6109,7 @@
         <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6154,24 +6151,24 @@
   <sheetData>
     <row r="1" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -6183,10 +6180,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -6198,10 +6195,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -6213,10 +6210,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -6228,10 +6225,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -6243,10 +6240,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -6258,10 +6255,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C8" t="s">
         <v>166</v>
@@ -6273,10 +6270,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C9" t="s">
         <v>166</v>
@@ -6288,10 +6285,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C10" t="s">
         <v>166</v>
@@ -6303,10 +6300,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B11" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C11" t="s">
         <v>166</v>
@@ -6318,10 +6315,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C12" t="s">
         <v>166</v>
@@ -6333,10 +6330,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C13" t="s">
         <v>166</v>
@@ -6348,10 +6345,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C14" t="s">
         <v>166</v>
@@ -6363,10 +6360,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B15" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D15" s="1">
         <f>COUNTIF(Skills!E:E,A15) + COUNTIF(Skills!I:I,A15) + COUNTIF(Skills!K:K,A15) + COUNTIF(Skills!M:M,A15) + COUNTIF(Skills!O:O,A15)</f>
@@ -6375,10 +6372,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C16" t="s">
         <v>161</v>
@@ -6390,7 +6387,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s">
         <v>107</v>
@@ -6405,10 +6402,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C18" t="s">
         <v>161</v>
@@ -6420,10 +6417,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C19" t="s">
         <v>161</v>
@@ -6435,10 +6432,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C20" t="s">
         <v>154</v>
@@ -6450,10 +6447,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C21" t="s">
         <v>154</v>
@@ -6465,7 +6462,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B22" t="s">
         <v>103</v>
@@ -6480,10 +6477,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -6495,10 +6492,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
@@ -6510,10 +6507,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B25" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -6525,10 +6522,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
@@ -6540,10 +6537,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
@@ -6555,10 +6552,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B28" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>
@@ -6570,10 +6567,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C29" t="s">
         <v>168</v>
@@ -6585,10 +6582,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B30" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C30" t="s">
         <v>168</v>
@@ -6600,10 +6597,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B31" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C31" t="s">
         <v>168</v>
@@ -6630,10 +6627,10 @@
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B33" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C33" t="s">
         <v>167</v>
@@ -6645,10 +6642,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C34" t="s">
         <v>167</v>
@@ -6660,10 +6657,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C35" t="s">
         <v>167</v>
@@ -6675,10 +6672,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B36" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D36" s="1">
         <f>COUNTIF(Skills!E:E,A36) + COUNTIF(Skills!I:I,A36) + COUNTIF(Skills!K:K,A36) + COUNTIF(Skills!M:M,A36) + COUNTIF(Skills!O:O,A36)</f>
@@ -6687,10 +6684,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B37" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C37" t="s">
         <v>167</v>
@@ -6702,10 +6699,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B38" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C38" t="s">
         <v>167</v>
@@ -6717,10 +6714,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B39" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C39" t="s">
         <v>167</v>
@@ -6732,10 +6729,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B40" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C40" t="s">
         <v>167</v>
@@ -6747,10 +6744,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B41" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C41" t="s">
         <v>167</v>
@@ -6777,10 +6774,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B43" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -6792,10 +6789,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B44" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
@@ -6807,10 +6804,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B45" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
@@ -6822,10 +6819,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D46" s="1">
         <f>COUNTIF(Skills!E:E,A46) + COUNTIF(Skills!I:I,A46) + COUNTIF(Skills!K:K,A46) + COUNTIF(Skills!M:M,A46) + COUNTIF(Skills!O:O,A46)</f>
@@ -8212,7 +8209,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="69" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -8242,7 +8239,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="55" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -8277,12 +8274,12 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="69" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" ref="B48:B55" si="0">VLOOKUP(A48,Actions,2,FALSE)</f>
@@ -8291,7 +8288,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
@@ -8300,7 +8297,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
@@ -8309,7 +8306,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -8318,7 +8315,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
@@ -8327,7 +8324,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B53" t="e">
         <f t="shared" si="0"/>
@@ -8336,7 +8333,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
@@ -8345,7 +8342,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
@@ -8354,12 +8351,12 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="69" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" ref="B58:B63" si="1">VLOOKUP(A58,Actions,2,FALSE)</f>
@@ -8368,7 +8365,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="1"/>
@@ -8377,7 +8374,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="1"/>
@@ -8428,13 +8425,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E1" s="69" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="69" t="s">
         <v>274</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>275</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8451,13 +8448,13 @@
         <v>143</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>281</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8474,10 +8471,10 @@
         <v>144</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8494,13 +8491,13 @@
         <v>145</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>288</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8517,7 +8514,7 @@
         <v>146</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8534,13 +8531,13 @@
         <v>148</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8557,13 +8554,13 @@
         <v>147</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -8618,7 +8615,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -8652,32 +8649,32 @@
         <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="80" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -8708,7 +8705,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
         <v>182</v>
@@ -8716,34 +8713,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
characters: exploit --> autopwn, exploit II --> exploit
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1207,9 +1207,6 @@
     <t>Exploit%n(above)</t>
   </si>
   <si>
-    <t>Exploit II%n(above)</t>
-  </si>
-  <si>
     <t>Dart%n(above)</t>
   </si>
   <si>
@@ -1219,12 +1216,6 @@
     <t>Mover</t>
   </si>
   <si>
-    <t>HAS THE CODE%nOnce per heist may spend 💡💡 to re-position up to 4 planning tokens of any color(s)%n %nEXPLOIT II%nUse this Action to enable another character to 👊🔊, 📷🔊, or 🔓🔊</t>
-  </si>
-  <si>
-    <t>I CAN HAZ TEH CODES?%nOnce per heist may spend 💡💡 to re-position up to 3 planning tokens of any color(s)%n %nEXPLOIT%nUse this Action and a 💡 to enable another character to 👊🔊, 📷🔊, or 🔓🔊</t>
-  </si>
-  <si>
     <t>Pick II%n🔓🔓🔊</t>
   </si>
   <si>
@@ -1250,6 +1241,15 @@
   </si>
   <si>
     <t>EFFICIENT PICKER%nIf your action has a 🔓, you may spend 💡 for an additional ➜🔊%n %nBREACH%nMay spend your action and💡💡💡💡 to create a new Exit on an open, external side of the current tile. Initiate Escape phase immediately.</t>
+  </si>
+  <si>
+    <t>Autopwn%n(above)</t>
+  </si>
+  <si>
+    <t>I CAN HAZ TEH CODES?%nOnce per heist may spend 💡💡 to re-position up to 3 planning tokens of any color(s)%n %nAUTOPWN%nUse this Action and a 💡 to enable another character to 👊🔊, 📷🔊, or 🔓🔊</t>
+  </si>
+  <si>
+    <t>HAS THE CODE%nOnce per heist may spend 💡💡 to re-position up to 4 planning tokens of any color(s)%n %nEXPLOIT%nUse this Action to enable another character to 👊🔊, 📷🔊, or 🔓🔊</t>
   </si>
 </sst>
 </file>
@@ -2170,7 +2170,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,7 +2265,7 @@
         <v>208</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>81</v>
@@ -2294,13 +2294,13 @@
         <v>142</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>81</v>
@@ -2337,7 +2337,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>81</v>
@@ -2411,7 +2411,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>81</v>
@@ -2446,7 +2446,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="M7" s="20" t="s">
         <v>81</v>
@@ -2457,7 +2457,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
@@ -2485,7 +2485,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>81</v>
@@ -2496,7 +2496,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2520,7 +2520,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="M9" s="19"/>
     </row>
@@ -2529,7 +2529,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -2553,7 +2553,7 @@
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>81</v>
@@ -2582,7 +2582,7 @@
         <v>295</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>391</v>
+        <v>404</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="24" t="s">
@@ -2592,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="M11" s="22"/>
     </row>
@@ -2619,13 +2619,13 @@
         <v>367</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>391</v>
+        <v>404</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>81</v>
@@ -2654,13 +2654,13 @@
         <v>295</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>81</v>
@@ -2689,7 +2689,7 @@
         <v>142</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>132</v>
@@ -2730,7 +2730,7 @@
         <v>142</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>132</v>
@@ -2765,7 +2765,7 @@
         <v>142</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>132</v>
@@ -2773,7 +2773,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>81</v>
@@ -3591,7 +3591,7 @@
         <v>311</v>
       </c>
       <c r="E5" s="106" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F5" s="87" t="str">
         <f t="shared" si="0"/>
@@ -3619,7 +3619,7 @@
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M5" s="107" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="N5" s="87" t="str">
         <f t="shared" si="4"/>
@@ -6744,7 +6744,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B41" t="s">
         <v>312</v>

</xml_diff>

<commit_message>
characters: add shadows, tweak artwork
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1189,15 +1189,9 @@
     <t>🔊🔊🔊➜➜</t>
   </si>
   <si>
-    <t>DART%nUse this action to spend 💡for 🔊➜➜</t>
-  </si>
-  <si>
     <t>Default3</t>
   </si>
   <si>
-    <t>DART%nUse this action to spend 💡for 🔊➜➜%n %nSEWER CRAWL%nFor 🔊🔊⚠, may treat a tile directly across 1 non-tiled gap as adjacent.</t>
-  </si>
-  <si>
     <t>Breach%n(above)</t>
   </si>
   <si>
@@ -1234,9 +1228,6 @@
     <t>THERE ARE BETTER WAYS%nCannot 👊. For 💡, may exit space(s) with guard(s) for the rest of your turn. In Escape, you require only 1 Escape Move to exit a space with guards.%n %nINSPIRE%nUse this action and a 🔊 to give a free💡💡  to a player of your choosing.</t>
   </si>
   <si>
-    <t>BOLT%nUse this action to spend 💡for 🔊➜➜, %nor 💡💡 for 🔊➜➜➜</t>
-  </si>
-  <si>
     <t>EFFICIENT PICKER%nIf your action has a 🔓, you may spend 💡 for an additional ➜🔊</t>
   </si>
   <si>
@@ -1250,6 +1241,15 @@
   </si>
   <si>
     <t>HAS THE CODE%nOnce per heist may spend 💡💡 to re-position up to 4 planning tokens of any color(s)%n %nEXPLOIT%nUse this Action to enable another character to 👊🔊, 📷🔊, or 🔓🔊</t>
+  </si>
+  <si>
+    <t>DART%nUse this action to spend%n💡for 🔊➜➜</t>
+  </si>
+  <si>
+    <t>DART%nUse this action to spend%n💡for 🔊➜➜%n %nSEWER CRAWL%nFor 🔊🔊⚠, may treat a tile directly across 1 non-tiled gap as adjacent.</t>
+  </si>
+  <si>
+    <t>BOLT%nUse this action to spend%n💡for 🔊➜➜, %nor 💡💡 for 🔊➜➜➜</t>
   </si>
 </sst>
 </file>
@@ -2169,26 +2169,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.75" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.25" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.75" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.125" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.75" style="28" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="133" style="28" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="28"/>
+    <col min="13" max="13" width="10.375" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
         <v>141</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J1" s="32" t="s">
         <v>152</v>
@@ -2265,7 +2265,7 @@
         <v>208</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>81</v>
@@ -2294,13 +2294,13 @@
         <v>142</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>81</v>
@@ -2332,12 +2332,12 @@
         <v>370</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>81</v>
@@ -2411,7 +2411,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>81</v>
@@ -2446,7 +2446,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M7" s="20" t="s">
         <v>81</v>
@@ -2457,7 +2457,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
@@ -2485,7 +2485,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>81</v>
@@ -2496,7 +2496,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2520,7 +2520,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M9" s="19"/>
     </row>
@@ -2529,7 +2529,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -2547,13 +2547,13 @@
         <v>367</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>81</v>
@@ -2582,7 +2582,7 @@
         <v>295</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="24" t="s">
@@ -2592,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="M11" s="22"/>
     </row>
@@ -2619,13 +2619,13 @@
         <v>367</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>81</v>
@@ -2654,13 +2654,13 @@
         <v>295</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>81</v>
@@ -2689,7 +2689,7 @@
         <v>142</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>132</v>
@@ -2701,7 +2701,7 @@
         <v>15</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>81</v>
@@ -2730,13 +2730,13 @@
         <v>142</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>132</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>388</v>
+        <v>405</v>
       </c>
       <c r="M15" s="21" t="s">
         <v>81</v>
@@ -2765,7 +2765,7 @@
         <v>142</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>132</v>
@@ -2773,7 +2773,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>81</v>
@@ -2910,48 +2910,48 @@
       <selection pane="bottomRight" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="111" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="92" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="120" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="111" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="92" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="120" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="111" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="92" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" style="120" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="92" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="5.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="111" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="92" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.125" style="120" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" style="111" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.125" style="92" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.125" style="120" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.125" style="111" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.125" style="92" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="120" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.125" style="92" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25" style="3" customWidth="1"/>
     <col min="18" max="18" width="20" style="3" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="25.140625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="20.140625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="25.140625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="130.140625" style="4" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="20.75" style="3" customWidth="1"/>
+    <col min="20" max="20" width="25.125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="20.125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="25.125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="130.125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="15.125" style="3" customWidth="1"/>
     <col min="25" max="25" width="13" style="4" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="15.125" style="3" customWidth="1"/>
     <col min="27" max="27" width="14" style="4" customWidth="1"/>
-    <col min="28" max="28" width="3.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="3.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="3.7109375" style="3" customWidth="1"/>
-    <col min="35" max="35" width="3.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="34.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="40" max="56" width="9.140625" style="149"/>
-    <col min="57" max="16384" width="9.140625" style="6"/>
+    <col min="28" max="28" width="3.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="3.75" style="3" customWidth="1"/>
+    <col min="35" max="35" width="3.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="34.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="56" width="9.125" style="149"/>
+    <col min="57" max="16384" width="9.125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" s="93" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3591,7 +3591,7 @@
         <v>311</v>
       </c>
       <c r="E5" s="106" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F5" s="87" t="str">
         <f t="shared" si="0"/>
@@ -3619,7 +3619,7 @@
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M5" s="107" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="N5" s="87" t="str">
         <f t="shared" si="4"/>
@@ -6042,7 +6042,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.75" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6143,10 +6143,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
@@ -6744,7 +6744,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B41" t="s">
         <v>312</v>
@@ -6848,16 +6848,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8415,12 +8415,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -8633,7 +8633,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -8692,7 +8692,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
characters: tunneler --> demolitions guy
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -655,9 +655,6 @@
     <t>Convert a camera to a double-camera.</t>
   </si>
   <si>
-    <t>Tunneler</t>
-  </si>
-  <si>
     <t>1-action</t>
   </si>
   <si>
@@ -1250,6 +1247,9 @@
   </si>
   <si>
     <t>BOLT%nUse this action to spend%n💡for 🔊➜➜, %nor 💡💡 for 🔊➜➜➜</t>
+  </si>
+  <si>
+    <t>Demolitions Guy</t>
   </si>
 </sst>
 </file>
@@ -2169,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,7 +2185,7 @@
     <col min="8" max="8" width="22.25" style="29" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.75" style="29" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.125" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.75" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.875" style="28" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="133" style="28" customWidth="1"/>
     <col min="13" max="13" width="10.375" style="28" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.125" style="28"/>
@@ -2217,7 +2217,7 @@
         <v>141</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J1" s="32" t="s">
         <v>152</v>
@@ -2255,17 +2255,17 @@
         <v>142</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>208</v>
+        <v>406</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>81</v>
@@ -2294,13 +2294,13 @@
         <v>142</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>81</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="4" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>208</v>
+        <v>406</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>157</v>
@@ -2329,15 +2329,15 @@
         <v>142</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>81</v>
@@ -2376,7 +2376,7 @@
         <v>8</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M5" s="20" t="s">
         <v>81</v>
@@ -2411,7 +2411,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>81</v>
@@ -2440,13 +2440,13 @@
         <v>142</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M7" s="20" t="s">
         <v>81</v>
@@ -2457,7 +2457,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
@@ -2485,7 +2485,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>81</v>
@@ -2496,7 +2496,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2520,7 +2520,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M9" s="19"/>
     </row>
@@ -2529,7 +2529,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -2544,16 +2544,16 @@
         <v>3</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>81</v>
@@ -2579,10 +2579,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="24" t="s">
@@ -2592,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M11" s="22"/>
     </row>
@@ -2616,16 +2616,16 @@
         <v>6</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>81</v>
@@ -2651,16 +2651,16 @@
         <v>6</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>81</v>
@@ -2689,7 +2689,7 @@
         <v>142</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>132</v>
@@ -2701,7 +2701,7 @@
         <v>15</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>81</v>
@@ -2730,13 +2730,13 @@
         <v>142</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>132</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M15" s="21" t="s">
         <v>81</v>
@@ -2765,7 +2765,7 @@
         <v>142</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>132</v>
@@ -2773,7 +2773,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>81</v>
@@ -2799,14 +2799,14 @@
         <v>4</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H17" s="27" t="s">
         <v>132</v>
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K17" s="26" t="s">
         <v>39</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="18" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>151</v>
@@ -2838,14 +2838,14 @@
         <v>3</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H18" s="27" t="s">
         <v>131</v>
       </c>
       <c r="I18" s="27"/>
       <c r="L18" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M18" s="23" t="s">
         <v>81</v>
@@ -2871,14 +2871,14 @@
         <v>5</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I19" s="27"/>
       <c r="L19" s="23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M19" s="23" t="s">
         <v>81</v>
@@ -2968,40 +2968,40 @@
         <v>164</v>
       </c>
       <c r="E1" s="99" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="95" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="95" t="s">
-        <v>210</v>
-      </c>
       <c r="G1" s="112" t="s">
+        <v>261</v>
+      </c>
+      <c r="H1" s="94" t="s">
         <v>262</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="I1" s="99" t="s">
         <v>263</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="J1" s="95" t="s">
         <v>264</v>
       </c>
-      <c r="J1" s="95" t="s">
+      <c r="K1" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="K1" s="112" t="s">
+      <c r="L1" s="94" t="s">
         <v>266</v>
       </c>
-      <c r="L1" s="94" t="s">
+      <c r="M1" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="M1" s="99" t="s">
+      <c r="N1" s="95" t="s">
         <v>268</v>
       </c>
-      <c r="N1" s="95" t="s">
+      <c r="O1" s="112" t="s">
         <v>269</v>
       </c>
-      <c r="O1" s="112" t="s">
+      <c r="P1" s="95" t="s">
         <v>270</v>
-      </c>
-      <c r="P1" s="95" t="s">
-        <v>271</v>
       </c>
       <c r="Q1" s="94">
         <v>1</v>
@@ -3061,16 +3061,16 @@
         <v>155</v>
       </c>
       <c r="AJ1" s="93" t="s">
+        <v>295</v>
+      </c>
+      <c r="AK1" s="93" t="s">
+        <v>305</v>
+      </c>
+      <c r="AL1" s="93" t="s">
         <v>296</v>
       </c>
-      <c r="AK1" s="93" t="s">
-        <v>306</v>
-      </c>
-      <c r="AL1" s="93" t="s">
-        <v>297</v>
-      </c>
       <c r="AM1" s="93" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AN1" s="147"/>
       <c r="AO1" s="147"/>
@@ -3104,42 +3104,42 @@
         <v>126</v>
       </c>
       <c r="E2" s="100" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F2" s="81" t="str">
         <f t="shared" ref="F2:F19" si="0">VLOOKUP(E2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G2" s="113" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H2" s="41" t="str">
         <f t="shared" ref="H2:H19" si="1">VLOOKUP(G2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="I2" s="100" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J2" s="81" t="str">
         <f t="shared" ref="J2:J19" si="2">VLOOKUP(I2,Actions,2,FALSE)</f>
         <v>🔍🔍</v>
       </c>
       <c r="K2" s="113" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L2" s="41" t="str">
         <f t="shared" ref="L2:L19" si="3">VLOOKUP(K2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M2" s="100" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N2" s="81" t="str">
         <f t="shared" ref="N2:N19" si="4">VLOOKUP(M2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O2" s="113" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="P2" s="81" t="str">
         <f t="shared" ref="P2:P19" si="5">VLOOKUP(O2,Actions,2,FALSE)</f>
@@ -3186,7 +3186,7 @@
         <v>Flip%n👊🔊➜/Disable%n📷🔊➜/Study%n💡💡/Punch%n👊🔊🔊➜/Smash%n📷🔊🔊➜/Ransack%n💰💰🔊</v>
       </c>
       <c r="Z2" s="40" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AA2" s="43" t="str">
         <f t="shared" ref="AA2:AA19" si="7">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
@@ -3225,16 +3225,16 @@
         <v>1</v>
       </c>
       <c r="AJ2" s="39" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AK2" s="39" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AL2" s="39" t="s">
         <v>154</v>
       </c>
       <c r="AM2" s="39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN2" s="149"/>
       <c r="AO2" s="149"/>
@@ -3268,42 +3268,42 @@
         <v>127</v>
       </c>
       <c r="E3" s="102" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F3" s="83" t="str">
         <f t="shared" si="0"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G3" s="115" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H3" s="36" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I3" s="103" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J3" s="83" t="str">
         <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K3" s="121" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L3" s="36" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M3" s="103" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N3" s="83" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O3" s="115" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P3" s="83" t="str">
         <f t="shared" si="5"/>
@@ -3389,16 +3389,16 @@
         <v>0</v>
       </c>
       <c r="AJ3" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AK3" s="33" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AL3" s="33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AM3" s="33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AN3" s="149"/>
       <c r="AO3" s="149"/>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="4" spans="1:56" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B4" s="50">
         <v>2</v>
@@ -3429,45 +3429,45 @@
         <v>1</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F4" s="85" t="str">
         <f t="shared" si="0"/>
         <v>🔍🔍</v>
       </c>
       <c r="G4" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H4" s="51" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="I4" s="105" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J4" s="85" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K4" s="123" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L4" s="51" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M4" s="105" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N4" s="85" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O4" s="116" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="P4" s="85" t="str">
         <f t="shared" si="5"/>
@@ -3548,16 +3548,16 @@
         <v>1</v>
       </c>
       <c r="AJ4" s="54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AK4" s="54" t="s">
         <v>161</v>
       </c>
       <c r="AL4" s="54" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AM4" s="54" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN4" s="149"/>
       <c r="AO4" s="149"/>
@@ -3579,7 +3579,7 @@
     </row>
     <row r="5" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B5" s="61">
         <v>2</v>
@@ -3588,45 +3588,45 @@
         <v>1</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E5" s="106" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F5" s="87" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊</v>
       </c>
       <c r="G5" s="117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H5" s="62" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I5" s="107" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J5" s="87" t="str">
         <f t="shared" si="2"/>
         <v>👊👊🔊</v>
       </c>
       <c r="K5" s="125" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L5" s="62" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M5" s="107" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N5" s="87" t="str">
         <f t="shared" si="4"/>
         <v>👊🔊</v>
       </c>
       <c r="O5" s="117" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P5" s="87" t="str">
         <f t="shared" si="5"/>
@@ -3668,7 +3668,7 @@
         <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Rampage%n👊👊🔊🔊🔊➜➜/Run%n🔊🔊➜➜/Strongarm%n🔓👊🔊🔊➜/Study%n💡💡</v>
       </c>
       <c r="Z5" s="61" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AA5" s="63" t="str">
         <f t="shared" si="7"/>
@@ -3707,16 +3707,16 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="64" t="s">
+        <v>312</v>
+      </c>
+      <c r="AK5" s="64" t="s">
         <v>313</v>
-      </c>
-      <c r="AK5" s="64" t="s">
-        <v>314</v>
       </c>
       <c r="AL5" s="64" t="s">
         <v>161</v>
       </c>
       <c r="AM5" s="64" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AN5" s="149"/>
       <c r="AO5" s="149"/>
@@ -3750,42 +3750,42 @@
         <v>130</v>
       </c>
       <c r="E6" s="108" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F6" s="89" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="G6" s="118" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H6" s="71" t="str">
         <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I6" s="109" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J6" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔓🔊</v>
       </c>
       <c r="K6" s="126" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L6" s="71" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M6" s="109" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N6" s="89" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="O6" s="118" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P6" s="89" t="str">
         <f t="shared" si="5"/>
@@ -3820,7 +3820,7 @@
         <v>Bump%n🔓🔓🔊🔊➜/Study%n💡💡/Pick%n🔓🔊/Sprint%n🔊🔊➜➜➜/Run%n🔊🔊➜➜/Pick%n🔓🔊</v>
       </c>
       <c r="X6" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Y6" s="71" t="str">
         <f t="shared" si="6"/>
@@ -3866,16 +3866,16 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="74" t="s">
+        <v>317</v>
+      </c>
+      <c r="AK6" s="74" t="s">
         <v>318</v>
-      </c>
-      <c r="AK6" s="74" t="s">
-        <v>319</v>
       </c>
       <c r="AL6" s="74" t="s">
         <v>161</v>
       </c>
       <c r="AM6" s="74" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN6" s="149"/>
       <c r="AO6" s="149"/>
@@ -3909,42 +3909,42 @@
         <v>59</v>
       </c>
       <c r="E7" s="131" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F7" s="132" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊🔊➜</v>
       </c>
       <c r="G7" s="133" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H7" s="130" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I7" s="134" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J7" s="132" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="K7" s="135" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L7" s="130" t="str">
         <f t="shared" si="3"/>
         <v>🔍🔍</v>
       </c>
       <c r="M7" s="134" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N7" s="132" t="str">
         <f t="shared" si="4"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="O7" s="133" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P7" s="132" t="str">
         <f t="shared" si="5"/>
@@ -3986,7 +3986,7 @@
         <v>Unplug%n📷📷🔊➜/Sprint%n🔊🔊➜➜➜/Disable%n📷🔊➜/Discover%n🔍🔍/Recon%n💡💡🔊🔍/Disable%n📷🔊➜</v>
       </c>
       <c r="Z7" s="136" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AA7" s="137" t="str">
         <f t="shared" si="7"/>
@@ -4025,16 +4025,16 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="138" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AK7" s="138" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AL7" s="138" t="s">
         <v>168</v>
       </c>
       <c r="AM7" s="138" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN7" s="150"/>
       <c r="AO7" s="150"/>
@@ -4068,42 +4068,42 @@
         <v>126</v>
       </c>
       <c r="E8" s="101" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F8" s="82" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊➜</v>
       </c>
       <c r="G8" s="114" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H8" s="43" t="str">
         <f t="shared" si="1"/>
         <v>📷🔊➜</v>
       </c>
       <c r="I8" s="101" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J8" s="82" t="str">
         <f t="shared" si="2"/>
         <v>💡💡</v>
       </c>
       <c r="K8" s="114" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L8" s="43" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M8" s="101" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N8" s="82" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O8" s="114" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P8" s="82" t="str">
         <f t="shared" si="5"/>
@@ -4184,16 +4184,16 @@
         <v>2</v>
       </c>
       <c r="AJ8" s="144" t="s">
+        <v>331</v>
+      </c>
+      <c r="AK8" s="144" t="s">
         <v>332</v>
       </c>
-      <c r="AK8" s="144" t="s">
-        <v>333</v>
-      </c>
       <c r="AL8" s="144" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AM8" s="144" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AN8" s="149"/>
       <c r="AO8" s="149"/>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="9" spans="1:56" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B9" s="47">
         <v>2</v>
@@ -4227,42 +4227,42 @@
         <v>126</v>
       </c>
       <c r="E9" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F9" s="82" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G9" s="114" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H9" s="43" t="str">
         <f t="shared" si="1"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="I9" s="101" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J9" s="82" t="str">
         <f t="shared" si="2"/>
         <v>🔍🔓🔊</v>
       </c>
       <c r="K9" s="114" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L9" s="43" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊➜</v>
       </c>
       <c r="M9" s="101" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N9" s="82" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊➜</v>
       </c>
       <c r="O9" s="114" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="P9" s="82" t="str">
         <f t="shared" si="5"/>
@@ -4343,16 +4343,16 @@
         <v>1</v>
       </c>
       <c r="AJ9" s="46" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AK9" s="46" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AL9" s="46" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AM9" s="46" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AN9" s="150"/>
       <c r="AO9" s="150"/>
@@ -4386,42 +4386,42 @@
         <v>127</v>
       </c>
       <c r="E10" s="103" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F10" s="84" t="str">
         <f t="shared" si="0"/>
         <v>🔊➜➜</v>
       </c>
       <c r="G10" s="115" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H10" s="34" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I10" s="103" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J10" s="84" t="str">
         <f t="shared" si="2"/>
         <v>👊➜</v>
       </c>
       <c r="K10" s="115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L10" s="34" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M10" s="103" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N10" s="84" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O10" s="115" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P10" s="84" t="str">
         <f t="shared" si="5"/>
@@ -4502,16 +4502,16 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="146" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AK10" s="146" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AL10" s="146" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AM10" s="146" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AN10" s="150"/>
       <c r="AO10" s="150"/>
@@ -4545,42 +4545,42 @@
         <v>127</v>
       </c>
       <c r="E11" s="103" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F11" s="84" t="str">
         <f t="shared" si="0"/>
         <v>🔊➜➜</v>
       </c>
       <c r="G11" s="115" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H11" s="35" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I11" s="103" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J11" s="84" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜➜</v>
       </c>
       <c r="K11" s="122" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L11" s="35" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M11" s="103" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N11" s="84" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O11" s="115" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P11" s="84" t="str">
         <f t="shared" si="5"/>
@@ -4661,16 +4661,16 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="146" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AK11" s="145" t="s">
         <v>167</v>
       </c>
       <c r="AL11" s="145" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AM11" s="145" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AN11" s="149"/>
       <c r="AO11" s="149"/>
@@ -4701,45 +4701,45 @@
         <v>2</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E12" s="105" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F12" s="86" t="str">
         <f t="shared" si="0"/>
         <v>💡💡</v>
       </c>
       <c r="G12" s="116" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H12" s="53" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊</v>
       </c>
       <c r="I12" s="105" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J12" s="86" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K12" s="116" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L12" s="53" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M12" s="105" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N12" s="86" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O12" s="116" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P12" s="86" t="str">
         <f t="shared" si="5"/>
@@ -4820,16 +4820,16 @@
         <v>1</v>
       </c>
       <c r="AJ12" s="54" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AK12" s="54" t="s">
         <v>168</v>
       </c>
       <c r="AL12" s="54" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AM12" s="54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AN12" s="149"/>
       <c r="AO12" s="149"/>
@@ -4860,45 +4860,45 @@
         <v>2</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E13" s="105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F13" s="86" t="str">
         <f t="shared" si="0"/>
         <v>🔓👊📷🔊🔊</v>
       </c>
       <c r="G13" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H13" s="56" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="I13" s="105" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J13" s="86" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K13" s="124" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L13" s="56" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M13" s="105" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N13" s="86" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O13" s="116" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P13" s="86" t="str">
         <f t="shared" si="5"/>
@@ -4979,16 +4979,16 @@
         <v>1</v>
       </c>
       <c r="AJ13" s="54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AK13" s="54" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AL13" s="54" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AM13" s="54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AN13" s="149"/>
       <c r="AO13" s="149"/>
@@ -5019,45 +5019,45 @@
         <v>2</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E14" s="107" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F14" s="88" t="str">
         <f t="shared" si="0"/>
         <v>👊👊🔊</v>
       </c>
       <c r="G14" s="117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H14" s="63" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I14" s="107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J14" s="88" t="str">
         <f t="shared" si="2"/>
         <v>👊👊🔊🔊🔊➜➜</v>
       </c>
       <c r="K14" s="117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L14" s="63" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M14" s="107" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N14" s="88" t="str">
         <f t="shared" si="4"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="O14" s="117" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P14" s="88" t="str">
         <f t="shared" si="5"/>
@@ -5138,16 +5138,16 @@
         <v>0</v>
       </c>
       <c r="AJ14" s="64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AK14" s="64" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AL14" s="64" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AM14" s="64" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AN14" s="149"/>
       <c r="AO14" s="149"/>
@@ -5169,7 +5169,7 @@
     </row>
     <row r="15" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B15" s="66">
         <v>2</v>
@@ -5178,45 +5178,45 @@
         <v>2</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E15" s="107" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F15" s="88" t="str">
         <f t="shared" si="0"/>
         <v>👊👊🔊</v>
       </c>
       <c r="G15" s="117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H15" s="63" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I15" s="107" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J15" s="88" t="str">
         <f>VLOOKUP(I15,Actions,2,FALSE)</f>
         <v>🔓👊👊📷🔊⚠</v>
       </c>
       <c r="K15" s="117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L15" s="63" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M15" s="107" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N15" s="88" t="str">
         <f t="shared" si="4"/>
         <v>👊👊🔊</v>
       </c>
       <c r="O15" s="117" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P15" s="88" t="str">
         <f t="shared" si="5"/>
@@ -5297,14 +5297,14 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AK15" s="64"/>
       <c r="AL15" s="64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AM15" s="64" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AN15" s="149"/>
       <c r="AO15" s="149"/>
@@ -5326,7 +5326,7 @@
     </row>
     <row r="16" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B16" s="76">
         <v>2</v>
@@ -5338,42 +5338,42 @@
         <v>130</v>
       </c>
       <c r="E16" s="108" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F16" s="89" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G16" s="118" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H16" s="77" t="str">
         <f t="shared" si="1"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="I16" s="109" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J16" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔓💰</v>
       </c>
       <c r="K16" s="127" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L16" s="77" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M16" s="109" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N16" s="89" t="str">
         <f t="shared" si="4"/>
         <v>🔊➜➜</v>
       </c>
       <c r="O16" s="118" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P16" s="89" t="str">
         <f t="shared" si="5"/>
@@ -5454,16 +5454,16 @@
         <v>1</v>
       </c>
       <c r="AJ16" s="74" t="s">
+        <v>317</v>
+      </c>
+      <c r="AK16" s="74" t="s">
         <v>318</v>
       </c>
-      <c r="AK16" s="74" t="s">
-        <v>319</v>
-      </c>
       <c r="AL16" s="74" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AM16" s="74" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AN16" s="149"/>
       <c r="AO16" s="149"/>
@@ -5497,42 +5497,42 @@
         <v>130</v>
       </c>
       <c r="E17" s="109" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F17" s="90" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G17" s="118" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H17" s="73" t="str">
         <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I17" s="109" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J17" s="90" t="str">
         <f t="shared" si="2"/>
         <v>🔓👊🔊</v>
       </c>
       <c r="K17" s="118" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L17" s="73" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M17" s="109" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N17" s="90" t="str">
         <f t="shared" si="4"/>
         <v>🔊➜➜</v>
       </c>
       <c r="O17" s="118" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P17" s="90" t="str">
         <f t="shared" si="5"/>
@@ -5613,16 +5613,16 @@
         <v>0</v>
       </c>
       <c r="AJ17" s="74" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AK17" s="74" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AL17" s="74" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AM17" s="74" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AN17" s="150"/>
       <c r="AO17" s="150"/>
@@ -5656,42 +5656,42 @@
         <v>59</v>
       </c>
       <c r="E18" s="134" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F18" s="139" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="G18" s="133" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H18" s="137" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I18" s="134" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J18" s="139" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K18" s="133" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L18" s="137" t="str">
         <f t="shared" si="3"/>
         <v>🔍🔍</v>
       </c>
       <c r="M18" s="134" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N18" s="139" t="str">
         <f t="shared" si="4"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="O18" s="133" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P18" s="139" t="str">
         <f t="shared" si="5"/>
@@ -5772,13 +5772,13 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="138" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AK18" s="138" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AM18" s="138" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AN18" s="150"/>
       <c r="AO18" s="150"/>
@@ -5800,7 +5800,7 @@
     </row>
     <row r="19" spans="1:56" s="138" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="137" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B19" s="136">
         <v>2</v>
@@ -5812,42 +5812,42 @@
         <v>59</v>
       </c>
       <c r="E19" s="134" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F19" s="139" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="G19" s="133" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H19" s="137" t="str">
         <f t="shared" si="1"/>
         <v>🔊➜🔍</v>
       </c>
       <c r="I19" s="134" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J19" s="139" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K19" s="133" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L19" s="137" t="str">
         <f t="shared" si="3"/>
         <v>🔊➜🔍</v>
       </c>
       <c r="M19" s="134" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N19" s="139" t="str">
         <f t="shared" si="4"/>
         <v>💡💡</v>
       </c>
       <c r="O19" s="133" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P19" s="139" t="str">
         <f t="shared" si="5"/>
@@ -5928,16 +5928,16 @@
         <v>0</v>
       </c>
       <c r="AJ19" s="138" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AK19" s="138" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AL19" s="138" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AM19" s="138" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AN19" s="150"/>
       <c r="AO19" s="150"/>
@@ -6066,7 +6066,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -6093,7 +6093,7 @@
         <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6109,7 +6109,7 @@
         <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6154,21 +6154,21 @@
         <v>192</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C1" s="69" t="s">
         <v>193</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -6180,10 +6180,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
         <v>229</v>
-      </c>
-      <c r="B3" t="s">
-        <v>230</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -6195,10 +6195,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -6210,10 +6210,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -6225,10 +6225,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B6" t="s">
         <v>320</v>
-      </c>
-      <c r="B6" t="s">
-        <v>321</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -6240,10 +6240,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -6255,10 +6255,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C8" t="s">
         <v>166</v>
@@ -6270,10 +6270,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C9" t="s">
         <v>166</v>
@@ -6285,10 +6285,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C10" t="s">
         <v>166</v>
@@ -6300,10 +6300,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C11" t="s">
         <v>166</v>
@@ -6315,10 +6315,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C12" t="s">
         <v>166</v>
@@ -6330,10 +6330,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C13" t="s">
         <v>166</v>
@@ -6345,10 +6345,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C14" t="s">
         <v>166</v>
@@ -6360,10 +6360,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D15" s="1">
         <f>COUNTIF(Skills!E:E,A15) + COUNTIF(Skills!I:I,A15) + COUNTIF(Skills!K:K,A15) + COUNTIF(Skills!M:M,A15) + COUNTIF(Skills!O:O,A15)</f>
@@ -6372,10 +6372,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C16" t="s">
         <v>161</v>
@@ -6387,7 +6387,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B17" t="s">
         <v>107</v>
@@ -6402,10 +6402,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C18" t="s">
         <v>161</v>
@@ -6417,10 +6417,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C19" t="s">
         <v>161</v>
@@ -6432,10 +6432,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C20" t="s">
         <v>154</v>
@@ -6447,10 +6447,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C21" t="s">
         <v>154</v>
@@ -6462,7 +6462,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s">
         <v>103</v>
@@ -6477,10 +6477,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>225</v>
+      </c>
+      <c r="B23" t="s">
         <v>226</v>
-      </c>
-      <c r="B23" t="s">
-        <v>227</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -6492,10 +6492,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
@@ -6507,10 +6507,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>383</v>
+      </c>
+      <c r="B25" t="s">
         <v>384</v>
-      </c>
-      <c r="B25" t="s">
-        <v>385</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -6522,10 +6522,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" t="s">
         <v>247</v>
-      </c>
-      <c r="B26" t="s">
-        <v>248</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
@@ -6537,10 +6537,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>249</v>
+      </c>
+      <c r="B27" t="s">
         <v>250</v>
-      </c>
-      <c r="B27" t="s">
-        <v>251</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
@@ -6552,10 +6552,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>
@@ -6567,10 +6567,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>230</v>
+      </c>
+      <c r="B29" t="s">
         <v>231</v>
-      </c>
-      <c r="B29" t="s">
-        <v>232</v>
       </c>
       <c r="C29" t="s">
         <v>168</v>
@@ -6582,10 +6582,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C30" t="s">
         <v>168</v>
@@ -6597,10 +6597,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>292</v>
+      </c>
+      <c r="B31" t="s">
         <v>293</v>
-      </c>
-      <c r="B31" t="s">
-        <v>294</v>
       </c>
       <c r="C31" t="s">
         <v>168</v>
@@ -6627,10 +6627,10 @@
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" t="s">
         <v>223</v>
-      </c>
-      <c r="B33" t="s">
-        <v>224</v>
       </c>
       <c r="C33" t="s">
         <v>167</v>
@@ -6642,10 +6642,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>234</v>
+      </c>
+      <c r="B34" t="s">
         <v>235</v>
-      </c>
-      <c r="B34" t="s">
-        <v>236</v>
       </c>
       <c r="C34" t="s">
         <v>167</v>
@@ -6657,10 +6657,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>236</v>
+      </c>
+      <c r="B35" t="s">
         <v>237</v>
-      </c>
-      <c r="B35" t="s">
-        <v>238</v>
       </c>
       <c r="C35" t="s">
         <v>167</v>
@@ -6672,10 +6672,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>333</v>
+      </c>
+      <c r="B36" t="s">
         <v>334</v>
-      </c>
-      <c r="B36" t="s">
-        <v>335</v>
       </c>
       <c r="D36" s="1">
         <f>COUNTIF(Skills!E:E,A36) + COUNTIF(Skills!I:I,A36) + COUNTIF(Skills!K:K,A36) + COUNTIF(Skills!M:M,A36) + COUNTIF(Skills!O:O,A36)</f>
@@ -6684,10 +6684,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C37" t="s">
         <v>167</v>
@@ -6699,10 +6699,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B38" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C38" t="s">
         <v>167</v>
@@ -6714,10 +6714,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C39" t="s">
         <v>167</v>
@@ -6729,10 +6729,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C40" t="s">
         <v>167</v>
@@ -6744,10 +6744,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B41" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C41" t="s">
         <v>167</v>
@@ -6774,10 +6774,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B43" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -6789,10 +6789,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
@@ -6804,10 +6804,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B45" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
@@ -6819,10 +6819,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B46" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D46" s="1">
         <f>COUNTIF(Skills!E:E,A46) + COUNTIF(Skills!I:I,A46) + COUNTIF(Skills!K:K,A46) + COUNTIF(Skills!M:M,A46) + COUNTIF(Skills!O:O,A46)</f>
@@ -8209,7 +8209,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="69" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -8239,7 +8239,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -8274,12 +8274,12 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="69" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" ref="B48:B55" si="0">VLOOKUP(A48,Actions,2,FALSE)</f>
@@ -8288,7 +8288,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
@@ -8297,7 +8297,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
@@ -8306,7 +8306,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -8315,7 +8315,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
@@ -8324,7 +8324,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B53" t="e">
         <f t="shared" si="0"/>
@@ -8333,7 +8333,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
@@ -8342,7 +8342,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
@@ -8351,12 +8351,12 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="69" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" ref="B58:B63" si="1">VLOOKUP(A58,Actions,2,FALSE)</f>
@@ -8365,7 +8365,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="1"/>
@@ -8374,7 +8374,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="1"/>
@@ -8425,13 +8425,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E1" s="69" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="69" t="s">
         <v>272</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="G1" s="69" t="s">
         <v>273</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8448,13 +8448,13 @@
         <v>143</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8471,10 +8471,10 @@
         <v>144</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="G3" t="s">
         <v>276</v>
-      </c>
-      <c r="G3" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8491,13 +8491,13 @@
         <v>145</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8514,7 +8514,7 @@
         <v>146</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8531,13 +8531,13 @@
         <v>148</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>288</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8554,13 +8554,13 @@
         <v>147</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -8674,7 +8674,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rules: more figures and formatting
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1228,9 +1228,6 @@
     <t>EFFICIENT PICKER%nIf your action has a 🔓, you may spend 💡 for an additional ➜🔊</t>
   </si>
   <si>
-    <t>EFFICIENT PICKER%nIf your action has a 🔓, you may spend 💡 for an additional ➜🔊%n %nBREACH%nMay spend your action and💡💡💡💡 to create a new Exit on an open, external side of the current tile. Initiate Escape phase immediately.</t>
-  </si>
-  <si>
     <t>Autopwn%n(above)</t>
   </si>
   <si>
@@ -1250,6 +1247,9 @@
   </si>
   <si>
     <t>Demolitions Guy</t>
+  </si>
+  <si>
+    <t>EFFICIENT PICKER%nIf your action has a 🔓, you may spend 💡 for an additional ➜🔊%n %nBREACH%nMay spend your action and💡💡💡💡 to create a new Exit on an external side of the current tile. Initiate Escape phase immediately.</t>
   </si>
 </sst>
 </file>
@@ -2169,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,7 +2262,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>398</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="4" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>157</v>
@@ -2337,7 +2337,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>81</v>
@@ -2582,7 +2582,7 @@
         <v>294</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="24" t="s">
@@ -2592,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M11" s="22"/>
     </row>
@@ -2619,13 +2619,13 @@
         <v>366</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>81</v>
@@ -2660,7 +2660,7 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>81</v>
@@ -2701,7 +2701,7 @@
         <v>15</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>81</v>
@@ -2736,7 +2736,7 @@
         <v>132</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M15" s="21" t="s">
         <v>81</v>
@@ -2773,7 +2773,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
characters: inside man --> tunneler
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="408">
   <si>
     <t>Name</t>
   </si>
@@ -598,9 +598,6 @@
     <t>I CAN HEARTBLEED%nIf outdoors, may spend 💡 to 🔍</t>
   </si>
   <si>
-    <t>EARLY WARNING%nWhen outdoors, may 🔍 once per turn%n %nMISDIRECT%nOnce per heist, may use 💡💡💡 to change the security roll by 1.</t>
-  </si>
-  <si>
     <t>DIG!%nMay begin the heist on any non-security tile on bordering the outside of the map for 🔊🔊</t>
   </si>
   <si>
@@ -1141,9 +1138,6 @@
     <t>Pick%n🔓🔊</t>
   </si>
   <si>
-    <t>Key In%n🔍🔓🔊</t>
-  </si>
-  <si>
     <t>🔓👊📷🔊🔊</t>
   </si>
   <si>
@@ -1162,9 +1156,6 @@
     <t>ADRENALINE%nGain 💡 when you 👊</t>
   </si>
   <si>
-    <t>THEY TRUST ME%nMay start the heist on any Reinforcements space for 🔊🔊. Security events involving adjacency to Active Guards and Live Cameras do not apply to this character.</t>
-  </si>
-  <si>
     <t>👊👊🔊🔊🔊➜➜</t>
   </si>
   <si>
@@ -1250,6 +1241,18 @@
   </si>
   <si>
     <t>EFFICIENT PICKER%nIf your action has a 🔓, you may spend 💡 for an additional ➜🔊%n %nBREACH%nMay spend your action and💡💡💡💡 to create a new Exit on an external side of the current tile. Initiate Escape phase immediately.</t>
+  </si>
+  <si>
+    <t>Tunneler</t>
+  </si>
+  <si>
+    <t>Tunnel%n(above)</t>
+  </si>
+  <si>
+    <t>EARLY WARNING%nWhen outdoors, may 🔍 once per turn%n %nMISDIRECT%nOnce per heist, may use 💡💡💡 to change the security roll by 1.%n %nTUNNEL%nIf outdoors, use this action and 💡💡💡🔊 to teleport to the tile of any other player.</t>
+  </si>
+  <si>
+    <t>EARLY WARNING%nWhen outdoors, may 🔍 once per turn%n %nMISDIRECT%nOnce per heist, may use💡💡💡 to change the security roll by 1.</t>
   </si>
 </sst>
 </file>
@@ -2170,7 +2173,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,7 +2220,7 @@
         <v>141</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J1" s="32" t="s">
         <v>152</v>
@@ -2255,17 +2258,17 @@
         <v>142</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>81</v>
@@ -2294,13 +2297,13 @@
         <v>142</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>81</v>
@@ -2308,7 +2311,7 @@
     </row>
     <row r="4" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>157</v>
@@ -2329,15 +2332,15 @@
         <v>142</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>81</v>
@@ -2370,13 +2373,13 @@
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="M5" s="20" t="s">
         <v>81</v>
@@ -2384,7 +2387,7 @@
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>25</v>
@@ -2411,7 +2414,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>81</v>
@@ -2440,13 +2443,13 @@
         <v>142</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="M7" s="20" t="s">
         <v>81</v>
@@ -2457,7 +2460,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
@@ -2485,7 +2488,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>81</v>
@@ -2496,7 +2499,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2520,7 +2523,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="M9" s="19"/>
     </row>
@@ -2529,7 +2532,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -2544,16 +2547,16 @@
         <v>3</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>81</v>
@@ -2579,10 +2582,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="24" t="s">
@@ -2592,7 +2595,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="M11" s="22"/>
     </row>
@@ -2616,16 +2619,16 @@
         <v>6</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>81</v>
@@ -2651,16 +2654,16 @@
         <v>6</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>81</v>
@@ -2689,7 +2692,7 @@
         <v>142</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>132</v>
@@ -2701,7 +2704,7 @@
         <v>15</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>81</v>
@@ -2730,13 +2733,13 @@
         <v>142</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>132</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="M15" s="21" t="s">
         <v>81</v>
@@ -2765,7 +2768,7 @@
         <v>142</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>132</v>
@@ -2773,7 +2776,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>81</v>
@@ -2799,20 +2802,20 @@
         <v>4</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H17" s="27" t="s">
         <v>132</v>
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K17" s="26" t="s">
         <v>39</v>
       </c>
       <c r="L17" s="23" t="s">
-        <v>189</v>
+        <v>407</v>
       </c>
       <c r="M17" s="23" t="s">
         <v>81</v>
@@ -2820,7 +2823,7 @@
     </row>
     <row r="18" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>151</v>
@@ -2838,14 +2841,14 @@
         <v>3</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H18" s="27" t="s">
         <v>131</v>
       </c>
       <c r="I18" s="27"/>
       <c r="L18" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M18" s="23" t="s">
         <v>81</v>
@@ -2853,7 +2856,7 @@
     </row>
     <row r="19" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>39</v>
+        <v>404</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>151</v>
@@ -2868,17 +2871,19 @@
         <v>8</v>
       </c>
       <c r="F19" s="27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>370</v>
-      </c>
-      <c r="I19" s="27"/>
+        <v>132</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>405</v>
+      </c>
       <c r="L19" s="23" t="s">
-        <v>377</v>
+        <v>406</v>
       </c>
       <c r="M19" s="23" t="s">
         <v>81</v>
@@ -2968,40 +2973,40 @@
         <v>164</v>
       </c>
       <c r="E1" s="99" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" s="95" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="95" t="s">
-        <v>209</v>
-      </c>
       <c r="G1" s="112" t="s">
+        <v>260</v>
+      </c>
+      <c r="H1" s="94" t="s">
         <v>261</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="I1" s="99" t="s">
         <v>262</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="J1" s="95" t="s">
         <v>263</v>
       </c>
-      <c r="J1" s="95" t="s">
+      <c r="K1" s="112" t="s">
         <v>264</v>
       </c>
-      <c r="K1" s="112" t="s">
+      <c r="L1" s="94" t="s">
         <v>265</v>
       </c>
-      <c r="L1" s="94" t="s">
+      <c r="M1" s="99" t="s">
         <v>266</v>
       </c>
-      <c r="M1" s="99" t="s">
+      <c r="N1" s="95" t="s">
         <v>267</v>
       </c>
-      <c r="N1" s="95" t="s">
+      <c r="O1" s="112" t="s">
         <v>268</v>
       </c>
-      <c r="O1" s="112" t="s">
+      <c r="P1" s="95" t="s">
         <v>269</v>
-      </c>
-      <c r="P1" s="95" t="s">
-        <v>270</v>
       </c>
       <c r="Q1" s="94">
         <v>1</v>
@@ -3061,16 +3066,16 @@
         <v>155</v>
       </c>
       <c r="AJ1" s="93" t="s">
+        <v>294</v>
+      </c>
+      <c r="AK1" s="93" t="s">
+        <v>304</v>
+      </c>
+      <c r="AL1" s="93" t="s">
         <v>295</v>
       </c>
-      <c r="AK1" s="93" t="s">
-        <v>305</v>
-      </c>
-      <c r="AL1" s="93" t="s">
-        <v>296</v>
-      </c>
       <c r="AM1" s="93" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AN1" s="147"/>
       <c r="AO1" s="147"/>
@@ -3104,42 +3109,42 @@
         <v>126</v>
       </c>
       <c r="E2" s="100" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F2" s="81" t="str">
         <f t="shared" ref="F2:F19" si="0">VLOOKUP(E2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G2" s="113" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H2" s="41" t="str">
         <f t="shared" ref="H2:H19" si="1">VLOOKUP(G2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="I2" s="100" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J2" s="81" t="str">
         <f t="shared" ref="J2:J19" si="2">VLOOKUP(I2,Actions,2,FALSE)</f>
         <v>🔍🔍</v>
       </c>
       <c r="K2" s="113" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L2" s="41" t="str">
         <f t="shared" ref="L2:L19" si="3">VLOOKUP(K2,Actions,2,FALSE)</f>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M2" s="100" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N2" s="81" t="str">
         <f t="shared" ref="N2:N19" si="4">VLOOKUP(M2,Actions,2,FALSE)</f>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O2" s="113" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P2" s="81" t="str">
         <f t="shared" ref="P2:P19" si="5">VLOOKUP(O2,Actions,2,FALSE)</f>
@@ -3186,7 +3191,7 @@
         <v>Flip%n👊🔊➜/Disable%n📷🔊➜/Study%n💡💡/Punch%n👊🔊🔊➜/Smash%n📷🔊🔊➜/Ransack%n💰💰🔊</v>
       </c>
       <c r="Z2" s="40" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AA2" s="43" t="str">
         <f t="shared" ref="AA2:AA19" si="7">IF(Z2="(none)","",VLOOKUP(Z2,$A$2:$W$19,23,FALSE))</f>
@@ -3225,16 +3230,16 @@
         <v>1</v>
       </c>
       <c r="AJ2" s="39" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AK2" s="39" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AL2" s="39" t="s">
         <v>154</v>
       </c>
       <c r="AM2" s="39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AN2" s="149"/>
       <c r="AO2" s="149"/>
@@ -3268,42 +3273,42 @@
         <v>127</v>
       </c>
       <c r="E3" s="102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F3" s="83" t="str">
         <f t="shared" si="0"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="G3" s="115" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H3" s="36" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I3" s="103" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J3" s="83" t="str">
         <f t="shared" si="2"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="K3" s="121" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L3" s="36" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M3" s="103" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N3" s="83" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O3" s="115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P3" s="83" t="str">
         <f t="shared" si="5"/>
@@ -3389,16 +3394,16 @@
         <v>0</v>
       </c>
       <c r="AJ3" s="33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AK3" s="33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AL3" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AM3" s="33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN3" s="149"/>
       <c r="AO3" s="149"/>
@@ -3420,7 +3425,7 @@
     </row>
     <row r="4" spans="1:56" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B4" s="50">
         <v>2</v>
@@ -3429,45 +3434,45 @@
         <v>1</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F4" s="85" t="str">
         <f t="shared" si="0"/>
         <v>🔍🔍</v>
       </c>
       <c r="G4" s="116" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H4" s="51" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="I4" s="105" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J4" s="85" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K4" s="123" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L4" s="51" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M4" s="105" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N4" s="85" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O4" s="116" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="P4" s="85" t="str">
         <f t="shared" si="5"/>
@@ -3548,16 +3553,16 @@
         <v>1</v>
       </c>
       <c r="AJ4" s="54" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AK4" s="54" t="s">
         <v>161</v>
       </c>
       <c r="AL4" s="54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AM4" s="54" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AN4" s="149"/>
       <c r="AO4" s="149"/>
@@ -3579,7 +3584,7 @@
     </row>
     <row r="5" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B5" s="61">
         <v>2</v>
@@ -3588,45 +3593,45 @@
         <v>1</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E5" s="106" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F5" s="87" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊</v>
       </c>
       <c r="G5" s="117" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H5" s="62" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I5" s="107" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J5" s="87" t="str">
         <f t="shared" si="2"/>
         <v>👊👊🔊</v>
       </c>
       <c r="K5" s="125" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L5" s="62" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M5" s="107" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="N5" s="87" t="str">
         <f t="shared" si="4"/>
         <v>👊🔊</v>
       </c>
       <c r="O5" s="117" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P5" s="87" t="str">
         <f t="shared" si="5"/>
@@ -3668,7 +3673,7 @@
         <v>Bash%n👊👊🔊/Run%n🔊🔊➜➜/Rampage%n👊👊🔊🔊🔊➜➜/Run%n🔊🔊➜➜/Strongarm%n🔓👊🔊🔊➜/Study%n💡💡</v>
       </c>
       <c r="Z5" s="61" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AA5" s="63" t="str">
         <f t="shared" si="7"/>
@@ -3707,16 +3712,16 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="64" t="s">
+        <v>311</v>
+      </c>
+      <c r="AK5" s="64" t="s">
         <v>312</v>
-      </c>
-      <c r="AK5" s="64" t="s">
-        <v>313</v>
       </c>
       <c r="AL5" s="64" t="s">
         <v>161</v>
       </c>
       <c r="AM5" s="64" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN5" s="149"/>
       <c r="AO5" s="149"/>
@@ -3750,42 +3755,42 @@
         <v>130</v>
       </c>
       <c r="E6" s="108" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F6" s="89" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊🔊➜</v>
       </c>
       <c r="G6" s="118" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H6" s="71" t="str">
         <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I6" s="109" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J6" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔓🔊</v>
       </c>
       <c r="K6" s="126" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L6" s="71" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M6" s="109" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N6" s="89" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="O6" s="118" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P6" s="89" t="str">
         <f t="shared" si="5"/>
@@ -3820,7 +3825,7 @@
         <v>Bump%n🔓🔓🔊🔊➜/Study%n💡💡/Pick%n🔓🔊/Sprint%n🔊🔊➜➜➜/Run%n🔊🔊➜➜/Pick%n🔓🔊</v>
       </c>
       <c r="X6" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Y6" s="71" t="str">
         <f t="shared" si="6"/>
@@ -3866,16 +3871,16 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="74" t="s">
+        <v>316</v>
+      </c>
+      <c r="AK6" s="74" t="s">
         <v>317</v>
-      </c>
-      <c r="AK6" s="74" t="s">
-        <v>318</v>
       </c>
       <c r="AL6" s="74" t="s">
         <v>161</v>
       </c>
       <c r="AM6" s="74" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AN6" s="149"/>
       <c r="AO6" s="149"/>
@@ -3909,42 +3914,42 @@
         <v>59</v>
       </c>
       <c r="E7" s="131" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F7" s="132" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊🔊➜</v>
       </c>
       <c r="G7" s="133" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H7" s="130" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I7" s="134" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J7" s="132" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="K7" s="135" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L7" s="130" t="str">
         <f t="shared" si="3"/>
         <v>🔍🔍</v>
       </c>
       <c r="M7" s="134" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N7" s="132" t="str">
         <f t="shared" si="4"/>
         <v>💡💡💡🔊</v>
       </c>
       <c r="O7" s="133" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P7" s="132" t="str">
         <f t="shared" si="5"/>
@@ -3986,7 +3991,7 @@
         <v>Unplug%n📷📷🔊➜/Sprint%n🔊🔊➜➜➜/Disable%n📷🔊➜/Discover%n🔍🔍/Recon%n💡💡🔊🔍/Disable%n📷🔊➜</v>
       </c>
       <c r="Z7" s="136" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AA7" s="137" t="str">
         <f t="shared" si="7"/>
@@ -4025,16 +4030,16 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="138" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AK7" s="138" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AL7" s="138" t="s">
         <v>168</v>
       </c>
       <c r="AM7" s="138" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AN7" s="150"/>
       <c r="AO7" s="150"/>
@@ -4068,42 +4073,42 @@
         <v>126</v>
       </c>
       <c r="E8" s="101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F8" s="82" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊➜</v>
       </c>
       <c r="G8" s="114" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H8" s="43" t="str">
         <f t="shared" si="1"/>
         <v>📷🔊➜</v>
       </c>
       <c r="I8" s="101" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J8" s="82" t="str">
         <f t="shared" si="2"/>
         <v>💡💡</v>
       </c>
       <c r="K8" s="114" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L8" s="43" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="M8" s="101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N8" s="82" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊🔊➜</v>
       </c>
       <c r="O8" s="114" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="P8" s="82" t="str">
         <f t="shared" si="5"/>
@@ -4184,16 +4189,16 @@
         <v>2</v>
       </c>
       <c r="AJ8" s="144" t="s">
+        <v>330</v>
+      </c>
+      <c r="AK8" s="144" t="s">
         <v>331</v>
       </c>
-      <c r="AK8" s="144" t="s">
-        <v>332</v>
-      </c>
       <c r="AL8" s="144" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AM8" s="144" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN8" s="149"/>
       <c r="AO8" s="149"/>
@@ -4215,7 +4220,7 @@
     </row>
     <row r="9" spans="1:56" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B9" s="47">
         <v>2</v>
@@ -4227,42 +4232,42 @@
         <v>126</v>
       </c>
       <c r="E9" s="101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F9" s="82" t="str">
         <f t="shared" si="0"/>
         <v>👊🔊🔊➜</v>
       </c>
       <c r="G9" s="114" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H9" s="43" t="str">
         <f t="shared" si="1"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="I9" s="101" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J9" s="82" t="str">
         <f t="shared" si="2"/>
         <v>🔍🔓🔊</v>
       </c>
       <c r="K9" s="114" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L9" s="43" t="str">
         <f t="shared" si="3"/>
         <v>👊🔊➜</v>
       </c>
       <c r="M9" s="101" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N9" s="82" t="str">
         <f t="shared" si="4"/>
         <v>📷🔊➜</v>
       </c>
       <c r="O9" s="114" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P9" s="82" t="str">
         <f t="shared" si="5"/>
@@ -4343,16 +4348,16 @@
         <v>1</v>
       </c>
       <c r="AJ9" s="46" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AK9" s="46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AL9" s="46" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AM9" s="46" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN9" s="150"/>
       <c r="AO9" s="150"/>
@@ -4386,42 +4391,42 @@
         <v>127</v>
       </c>
       <c r="E10" s="103" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F10" s="84" t="str">
         <f t="shared" si="0"/>
         <v>🔊➜➜</v>
       </c>
       <c r="G10" s="115" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H10" s="34" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I10" s="103" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J10" s="84" t="str">
         <f t="shared" si="2"/>
         <v>👊➜</v>
       </c>
       <c r="K10" s="115" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L10" s="34" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M10" s="103" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N10" s="84" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O10" s="115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P10" s="84" t="str">
         <f t="shared" si="5"/>
@@ -4502,16 +4507,16 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="146" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AK10" s="146" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AL10" s="146" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AM10" s="146" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN10" s="150"/>
       <c r="AO10" s="150"/>
@@ -4545,42 +4550,42 @@
         <v>127</v>
       </c>
       <c r="E11" s="103" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F11" s="84" t="str">
         <f t="shared" si="0"/>
         <v>🔊➜➜</v>
       </c>
       <c r="G11" s="115" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H11" s="35" t="str">
         <f t="shared" si="1"/>
         <v>🔓🔊</v>
       </c>
       <c r="I11" s="103" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J11" s="84" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜➜</v>
       </c>
       <c r="K11" s="122" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L11" s="35" t="str">
         <f t="shared" si="3"/>
         <v>💡💡</v>
       </c>
       <c r="M11" s="103" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N11" s="84" t="str">
         <f t="shared" si="4"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="O11" s="115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P11" s="84" t="str">
         <f t="shared" si="5"/>
@@ -4661,16 +4666,16 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="146" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AK11" s="145" t="s">
         <v>167</v>
       </c>
       <c r="AL11" s="145" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AM11" s="145" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN11" s="149"/>
       <c r="AO11" s="149"/>
@@ -4701,45 +4706,45 @@
         <v>2</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E12" s="105" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F12" s="86" t="str">
         <f t="shared" si="0"/>
         <v>💡💡</v>
       </c>
       <c r="G12" s="116" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H12" s="53" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊</v>
       </c>
       <c r="I12" s="105" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J12" s="86" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K12" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L12" s="53" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M12" s="105" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N12" s="86" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O12" s="116" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P12" s="86" t="str">
         <f t="shared" si="5"/>
@@ -4820,16 +4825,16 @@
         <v>1</v>
       </c>
       <c r="AJ12" s="54" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AK12" s="54" t="s">
         <v>168</v>
       </c>
       <c r="AL12" s="54" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AM12" s="54" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN12" s="149"/>
       <c r="AO12" s="149"/>
@@ -4860,45 +4865,45 @@
         <v>2</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E13" s="105" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F13" s="86" t="str">
         <f t="shared" si="0"/>
         <v>🔓👊📷🔊🔊</v>
       </c>
       <c r="G13" s="116" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H13" s="56" t="str">
         <f t="shared" si="1"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="I13" s="105" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J13" s="86" t="str">
         <f t="shared" si="2"/>
         <v>🔓📷🔊🔊➜</v>
       </c>
       <c r="K13" s="124" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L13" s="56" t="str">
         <f t="shared" si="3"/>
         <v>👊📷🔊🔊➜</v>
       </c>
       <c r="M13" s="105" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N13" s="86" t="str">
         <f t="shared" si="4"/>
         <v>💰🔊</v>
       </c>
       <c r="O13" s="116" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P13" s="86" t="str">
         <f t="shared" si="5"/>
@@ -4979,16 +4984,16 @@
         <v>1</v>
       </c>
       <c r="AJ13" s="54" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AK13" s="54" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AL13" s="54" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AM13" s="54" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN13" s="149"/>
       <c r="AO13" s="149"/>
@@ -5019,45 +5024,45 @@
         <v>2</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E14" s="107" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F14" s="88" t="str">
         <f t="shared" si="0"/>
         <v>👊👊🔊</v>
       </c>
       <c r="G14" s="117" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H14" s="63" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I14" s="107" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J14" s="88" t="str">
         <f t="shared" si="2"/>
         <v>👊👊🔊🔊🔊➜➜</v>
       </c>
       <c r="K14" s="117" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L14" s="63" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M14" s="107" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N14" s="88" t="str">
         <f t="shared" si="4"/>
         <v>🔓👊🔊🔊➜</v>
       </c>
       <c r="O14" s="117" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P14" s="88" t="str">
         <f t="shared" si="5"/>
@@ -5138,16 +5143,16 @@
         <v>0</v>
       </c>
       <c r="AJ14" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AK14" s="64" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AL14" s="64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AM14" s="64" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN14" s="149"/>
       <c r="AO14" s="149"/>
@@ -5169,7 +5174,7 @@
     </row>
     <row r="15" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B15" s="66">
         <v>2</v>
@@ -5178,45 +5183,45 @@
         <v>2</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E15" s="107" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F15" s="88" t="str">
         <f t="shared" si="0"/>
         <v>👊👊🔊</v>
       </c>
       <c r="G15" s="117" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H15" s="63" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="I15" s="107" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J15" s="88" t="str">
         <f>VLOOKUP(I15,Actions,2,FALSE)</f>
         <v>🔓👊👊📷🔊⚠</v>
       </c>
       <c r="K15" s="117" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L15" s="63" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜</v>
       </c>
       <c r="M15" s="107" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N15" s="88" t="str">
         <f t="shared" si="4"/>
         <v>👊👊🔊</v>
       </c>
       <c r="O15" s="117" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P15" s="88" t="str">
         <f t="shared" si="5"/>
@@ -5297,14 +5302,14 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AK15" s="64"/>
       <c r="AL15" s="64" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AM15" s="64" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AN15" s="149"/>
       <c r="AO15" s="149"/>
@@ -5326,7 +5331,7 @@
     </row>
     <row r="16" spans="1:56" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B16" s="76">
         <v>2</v>
@@ -5338,42 +5343,42 @@
         <v>130</v>
       </c>
       <c r="E16" s="108" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F16" s="89" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G16" s="118" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H16" s="77" t="str">
         <f t="shared" si="1"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="I16" s="109" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J16" s="89" t="str">
         <f t="shared" si="2"/>
         <v>🔓💰</v>
       </c>
       <c r="K16" s="127" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L16" s="77" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M16" s="109" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N16" s="89" t="str">
         <f t="shared" si="4"/>
         <v>🔊➜➜</v>
       </c>
       <c r="O16" s="118" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P16" s="89" t="str">
         <f t="shared" si="5"/>
@@ -5454,16 +5459,16 @@
         <v>1</v>
       </c>
       <c r="AJ16" s="74" t="s">
+        <v>316</v>
+      </c>
+      <c r="AK16" s="74" t="s">
         <v>317</v>
       </c>
-      <c r="AK16" s="74" t="s">
-        <v>318</v>
-      </c>
       <c r="AL16" s="74" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AM16" s="74" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN16" s="149"/>
       <c r="AO16" s="149"/>
@@ -5497,42 +5502,42 @@
         <v>130</v>
       </c>
       <c r="E17" s="109" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F17" s="90" t="str">
         <f t="shared" si="0"/>
         <v>🔓🔓🔊➜</v>
       </c>
       <c r="G17" s="118" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H17" s="73" t="str">
         <f t="shared" si="1"/>
         <v>💡💡</v>
       </c>
       <c r="I17" s="109" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J17" s="90" t="str">
         <f t="shared" si="2"/>
         <v>🔓👊🔊</v>
       </c>
       <c r="K17" s="118" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L17" s="73" t="str">
         <f t="shared" si="3"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="M17" s="109" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N17" s="90" t="str">
         <f t="shared" si="4"/>
         <v>🔊➜➜</v>
       </c>
       <c r="O17" s="118" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P17" s="90" t="str">
         <f t="shared" si="5"/>
@@ -5613,16 +5618,16 @@
         <v>0</v>
       </c>
       <c r="AJ17" s="74" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AK17" s="74" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AL17" s="74" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AM17" s="74" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN17" s="150"/>
       <c r="AO17" s="150"/>
@@ -5656,42 +5661,42 @@
         <v>59</v>
       </c>
       <c r="E18" s="134" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F18" s="139" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="G18" s="133" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H18" s="137" t="str">
         <f t="shared" si="1"/>
         <v>🔊🔊➜➜➜</v>
       </c>
       <c r="I18" s="134" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J18" s="139" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K18" s="133" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L18" s="137" t="str">
         <f t="shared" si="3"/>
         <v>🔍🔍</v>
       </c>
       <c r="M18" s="134" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N18" s="139" t="str">
         <f t="shared" si="4"/>
         <v>💡💡🔊🔍</v>
       </c>
       <c r="O18" s="133" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P18" s="139" t="str">
         <f t="shared" si="5"/>
@@ -5772,13 +5777,13 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="138" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AK18" s="138" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AM18" s="138" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN18" s="150"/>
       <c r="AO18" s="150"/>
@@ -5800,7 +5805,7 @@
     </row>
     <row r="19" spans="1:56" s="138" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="137" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B19" s="136">
         <v>2</v>
@@ -5812,42 +5817,42 @@
         <v>59</v>
       </c>
       <c r="E19" s="134" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F19" s="139" t="str">
         <f t="shared" si="0"/>
         <v>📷📷🔊➜</v>
       </c>
       <c r="G19" s="133" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H19" s="137" t="str">
         <f t="shared" si="1"/>
         <v>🔊➜🔍</v>
       </c>
       <c r="I19" s="134" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J19" s="139" t="str">
         <f t="shared" si="2"/>
         <v>📷🔊➜</v>
       </c>
       <c r="K19" s="133" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L19" s="137" t="str">
         <f t="shared" si="3"/>
         <v>🔊➜🔍</v>
       </c>
       <c r="M19" s="134" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N19" s="139" t="str">
         <f t="shared" si="4"/>
         <v>💡💡</v>
       </c>
       <c r="O19" s="133" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P19" s="139" t="str">
         <f t="shared" si="5"/>
@@ -5928,16 +5933,16 @@
         <v>0</v>
       </c>
       <c r="AJ19" s="138" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AK19" s="138" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AL19" s="138" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AM19" s="138" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN19" s="150"/>
       <c r="AO19" s="150"/>
@@ -6066,7 +6071,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -6093,7 +6098,7 @@
         <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6109,7 +6114,7 @@
         <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6151,24 +6156,24 @@
   <sheetData>
     <row r="1" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="69" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>193</v>
-      </c>
       <c r="D1" s="69" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -6180,10 +6185,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" t="s">
         <v>228</v>
-      </c>
-      <c r="B3" t="s">
-        <v>229</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -6195,10 +6200,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -6210,10 +6215,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -6225,10 +6230,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B6" t="s">
         <v>319</v>
-      </c>
-      <c r="B6" t="s">
-        <v>320</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -6240,10 +6245,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -6255,10 +6260,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C8" t="s">
         <v>166</v>
@@ -6270,10 +6275,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C9" t="s">
         <v>166</v>
@@ -6285,10 +6290,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B10" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C10" t="s">
         <v>166</v>
@@ -6300,10 +6305,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B11" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C11" t="s">
         <v>166</v>
@@ -6315,10 +6320,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C12" t="s">
         <v>166</v>
@@ -6330,10 +6335,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C13" t="s">
         <v>166</v>
@@ -6345,10 +6350,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C14" t="s">
         <v>166</v>
@@ -6360,10 +6365,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D15" s="1">
         <f>COUNTIF(Skills!E:E,A15) + COUNTIF(Skills!I:I,A15) + COUNTIF(Skills!K:K,A15) + COUNTIF(Skills!M:M,A15) + COUNTIF(Skills!O:O,A15)</f>
@@ -6372,10 +6377,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C16" t="s">
         <v>161</v>
@@ -6387,7 +6392,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s">
         <v>107</v>
@@ -6402,10 +6407,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C18" t="s">
         <v>161</v>
@@ -6417,10 +6422,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C19" t="s">
         <v>161</v>
@@ -6432,10 +6437,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C20" t="s">
         <v>154</v>
@@ -6447,10 +6452,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C21" t="s">
         <v>154</v>
@@ -6462,7 +6467,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B22" t="s">
         <v>103</v>
@@ -6477,10 +6482,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B23" t="s">
         <v>225</v>
-      </c>
-      <c r="B23" t="s">
-        <v>226</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -6492,10 +6497,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
@@ -6507,10 +6512,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B25" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -6522,10 +6527,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" t="s">
         <v>246</v>
-      </c>
-      <c r="B26" t="s">
-        <v>247</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
@@ -6537,10 +6542,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>248</v>
+      </c>
+      <c r="B27" t="s">
         <v>249</v>
-      </c>
-      <c r="B27" t="s">
-        <v>250</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
@@ -6552,10 +6557,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>
@@ -6567,10 +6572,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" t="s">
         <v>230</v>
-      </c>
-      <c r="B29" t="s">
-        <v>231</v>
       </c>
       <c r="C29" t="s">
         <v>168</v>
@@ -6582,10 +6587,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C30" t="s">
         <v>168</v>
@@ -6597,10 +6602,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>291</v>
+      </c>
+      <c r="B31" t="s">
         <v>292</v>
-      </c>
-      <c r="B31" t="s">
-        <v>293</v>
       </c>
       <c r="C31" t="s">
         <v>168</v>
@@ -6627,10 +6632,10 @@
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>221</v>
+      </c>
+      <c r="B33" t="s">
         <v>222</v>
-      </c>
-      <c r="B33" t="s">
-        <v>223</v>
       </c>
       <c r="C33" t="s">
         <v>167</v>
@@ -6642,10 +6647,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>233</v>
+      </c>
+      <c r="B34" t="s">
         <v>234</v>
-      </c>
-      <c r="B34" t="s">
-        <v>235</v>
       </c>
       <c r="C34" t="s">
         <v>167</v>
@@ -6657,10 +6662,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>235</v>
+      </c>
+      <c r="B35" t="s">
         <v>236</v>
-      </c>
-      <c r="B35" t="s">
-        <v>237</v>
       </c>
       <c r="C35" t="s">
         <v>167</v>
@@ -6672,10 +6677,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>332</v>
+      </c>
+      <c r="B36" t="s">
         <v>333</v>
-      </c>
-      <c r="B36" t="s">
-        <v>334</v>
       </c>
       <c r="D36" s="1">
         <f>COUNTIF(Skills!E:E,A36) + COUNTIF(Skills!I:I,A36) + COUNTIF(Skills!K:K,A36) + COUNTIF(Skills!M:M,A36) + COUNTIF(Skills!O:O,A36)</f>
@@ -6684,10 +6689,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C37" t="s">
         <v>167</v>
@@ -6699,10 +6704,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B38" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C38" t="s">
         <v>167</v>
@@ -6714,10 +6719,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C39" t="s">
         <v>167</v>
@@ -6729,10 +6734,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C40" t="s">
         <v>167</v>
@@ -6744,10 +6749,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B41" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C41" t="s">
         <v>167</v>
@@ -6774,10 +6779,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B43" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -6789,10 +6794,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
@@ -6804,10 +6809,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
@@ -6819,10 +6824,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B46" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D46" s="1">
         <f>COUNTIF(Skills!E:E,A46) + COUNTIF(Skills!I:I,A46) + COUNTIF(Skills!K:K,A46) + COUNTIF(Skills!M:M,A46) + COUNTIF(Skills!O:O,A46)</f>
@@ -8209,7 +8214,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="69" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -8239,7 +8244,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="55" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -8274,12 +8279,12 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="69" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" ref="B48:B55" si="0">VLOOKUP(A48,Actions,2,FALSE)</f>
@@ -8288,7 +8293,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
@@ -8297,7 +8302,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
@@ -8306,7 +8311,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -8315,7 +8320,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
@@ -8324,7 +8329,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B53" t="e">
         <f t="shared" si="0"/>
@@ -8333,7 +8338,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
@@ -8342,7 +8347,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
@@ -8351,12 +8356,12 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="69" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" ref="B58:B63" si="1">VLOOKUP(A58,Actions,2,FALSE)</f>
@@ -8365,7 +8370,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="1"/>
@@ -8374,7 +8379,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="1"/>
@@ -8425,13 +8430,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E1" s="69" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" s="69" t="s">
         <v>271</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="G1" s="69" t="s">
         <v>272</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8448,13 +8453,13 @@
         <v>143</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8471,10 +8476,10 @@
         <v>144</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" t="s">
         <v>275</v>
-      </c>
-      <c r="G3" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8491,13 +8496,13 @@
         <v>145</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8514,7 +8519,7 @@
         <v>146</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8531,13 +8536,13 @@
         <v>148</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>287</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8554,13 +8559,13 @@
         <v>147</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -8615,7 +8620,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -8649,32 +8654,32 @@
         <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -8705,7 +8710,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
         <v>182</v>
@@ -8713,34 +8718,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
         <v>197</v>
-      </c>
-      <c r="B3" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" t="s">
         <v>199</v>
-      </c>
-      <c r="B4" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" t="s">
         <v>201</v>
-      </c>
-      <c r="B5" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" t="s">
         <v>204</v>
-      </c>
-      <c r="B6" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
events: convert tracker to event cards
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
-    <sheet name="Helps" sheetId="3" r:id="rId3"/>
-    <sheet name="Actions" sheetId="6" r:id="rId4"/>
-    <sheet name="Skill Ideas" sheetId="4" r:id="rId5"/>
-    <sheet name="Character Ideas" sheetId="5" r:id="rId6"/>
-    <sheet name="Event Ideas" sheetId="7" r:id="rId7"/>
-    <sheet name="Tile ideas" sheetId="8" r:id="rId8"/>
+    <sheet name="Events" sheetId="9" r:id="rId3"/>
+    <sheet name="Helps" sheetId="3" r:id="rId4"/>
+    <sheet name="Actions" sheetId="6" r:id="rId5"/>
+    <sheet name="Skill Ideas" sheetId="4" r:id="rId6"/>
+    <sheet name="Character Ideas" sheetId="5" r:id="rId7"/>
+    <sheet name="Event Ideas" sheetId="7" r:id="rId8"/>
+    <sheet name="Tile ideas" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Actions">Actions!$A$2:$B$47</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="449">
   <si>
     <t>Name</t>
   </si>
@@ -1280,6 +1281,102 @@
   </si>
   <si>
     <t>SWINDLER%nYou may pick up items in an adjacent tile, and may drop items on an adjacent tile as if it were on your tile.%n %nTOSS LOOT%nUse this action to place any of your loot up to two tiles away in a single direction. You may not toss over locked tiles or gaps.</t>
+  </si>
+  <si>
+    <t>Outta My Way!</t>
+  </si>
+  <si>
+    <t>Caught in a Reflection</t>
+  </si>
+  <si>
+    <t>Suspicious Guards</t>
+  </si>
+  <si>
+    <t>Let Me Go!</t>
+  </si>
+  <si>
+    <t>Reboot</t>
+  </si>
+  <si>
+    <t>Lockdown</t>
+  </si>
+  <si>
+    <t>I Thought I Had Him</t>
+  </si>
+  <si>
+    <t>Hey You!</t>
+  </si>
+  <si>
+    <t>Call It In</t>
+  </si>
+  <si>
+    <t>Alarm!</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Img</t>
+  </si>
+  <si>
+    <t>figure_alerts_neighboring.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_adj_camera.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_adj_guard.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_on_disabled.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_power_on.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_lockdown.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_unsubdue.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_hey_you.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_call_it_in.svg</t>
+  </si>
+  <si>
+    <t>figure_alerts_alarm.svg</t>
+  </si>
+  <si>
+    <t>For each hex tile with at least 2 characters on it, increase the alert bar by 1. For Entrance tiles, 2 alerts.</t>
+  </si>
+  <si>
+    <t>Make every Disabled Camera Live. Increase ⚠ every time you do this.</t>
+  </si>
+  <si>
+    <t>Close the next Gate, starting with "A". Remove the tile. If a character is on it, they are immediately Busted. Increase alert for each ⚠ shown.</t>
+  </si>
+  <si>
+    <t>Replace every Disabled Camera with a Guard.</t>
+  </si>
+  <si>
+    <t>Initiate Escape Phase.</t>
+  </si>
+  <si>
+    <t>Increase Alert(⚠) for each Live Camera adjacent to a character.</t>
+  </si>
+  <si>
+    <t>For each character adjacent to at least one Camera, add a Guard to the character's current tile.</t>
+  </si>
+  <si>
+    <t>⚠ for each Character on a Subdued Guard. Also, ⚠ for each Character on a Disabled Camera.</t>
+  </si>
+  <si>
+    <t>⚠ for each Unsubuded Guard adjacent to a character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase ⚠⚠.%nFor each Subdued Guard that shares a tile with a Character, Un-Subdue that guard. </t>
   </si>
 </sst>
 </file>
@@ -2212,7 +2309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6173,6 +6270,182 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="131.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>444</v>
+      </c>
+      <c r="D3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>447</v>
+      </c>
+      <c r="D4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>446</v>
+      </c>
+      <c r="D5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>440</v>
+      </c>
+      <c r="D6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>422</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>441</v>
+      </c>
+      <c r="D7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>423</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>448</v>
+      </c>
+      <c r="D8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>445</v>
+      </c>
+      <c r="D9" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>425</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>442</v>
+      </c>
+      <c r="D10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>426</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>443</v>
+      </c>
+      <c r="D11" t="s">
+        <v>438</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6272,7 +6545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
@@ -6977,7 +7250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:S63"/>
   <sheetViews>
@@ -8544,7 +8817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
@@ -8762,7 +9035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -8821,7 +9094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>

<commit_message>
events: convert to cards
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18720" windowHeight="11175" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="461">
   <si>
     <t>Name</t>
   </si>
@@ -1283,36 +1283,18 @@
     <t>SWINDLER%nYou may pick up items in an adjacent tile, and may drop items on an adjacent tile as if it were on your tile.%n %nTOSS LOOT%nUse this action to place any of your loot up to two tiles away in a single direction. You may not toss over locked tiles or gaps.</t>
   </si>
   <si>
-    <t>Outta My Way!</t>
-  </si>
-  <si>
     <t>Caught in a Reflection</t>
   </si>
   <si>
     <t>Suspicious Guards</t>
   </si>
   <si>
-    <t>Let Me Go!</t>
-  </si>
-  <si>
-    <t>Reboot</t>
-  </si>
-  <si>
-    <t>Lockdown</t>
-  </si>
-  <si>
     <t>I Thought I Had Him</t>
   </si>
   <si>
     <t>Hey You!</t>
   </si>
   <si>
-    <t>Call It In</t>
-  </si>
-  <si>
-    <t>Alarm!</t>
-  </si>
-  <si>
     <t>Order</t>
   </si>
   <si>
@@ -1352,31 +1334,85 @@
     <t>For each hex tile with at least 2 characters on it, increase the alert bar by 1. For Entrance tiles, 2 alerts.</t>
   </si>
   <si>
-    <t>Make every Disabled Camera Live. Increase ⚠ every time you do this.</t>
-  </si>
-  <si>
-    <t>Close the next Gate, starting with "A". Remove the tile. If a character is on it, they are immediately Busted. Increase alert for each ⚠ shown.</t>
-  </si>
-  <si>
     <t>Replace every Disabled Camera with a Guard.</t>
   </si>
   <si>
     <t>Initiate Escape Phase.</t>
   </si>
   <si>
-    <t>Increase Alert(⚠) for each Live Camera adjacent to a character.</t>
-  </si>
-  <si>
-    <t>For each character adjacent to at least one Camera, add a Guard to the character's current tile.</t>
-  </si>
-  <si>
-    <t>⚠ for each Character on a Subdued Guard. Also, ⚠ for each Character on a Disabled Camera.</t>
-  </si>
-  <si>
-    <t>⚠ for each Unsubuded Guard adjacent to a character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increase ⚠⚠.%nFor each Subdued Guard that shares a tile with a Character, Un-Subdue that guard. </t>
+    <t>Go Check on It</t>
+  </si>
+  <si>
+    <t>Get Outta My Way!</t>
+  </si>
+  <si>
+    <t>Shut the Gate!</t>
+  </si>
+  <si>
+    <t>Sound the Alarm!</t>
+  </si>
+  <si>
+    <t>Add a Guard from the supply to each tile that has a Character adjacent to at least one Live Camera.</t>
+  </si>
+  <si>
+    <t>Tripped Over Stuff</t>
+  </si>
+  <si>
+    <t>figure_alerts_lockdown_two_alerts.svg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close the next Gate, starting with "A". Remove the tile. If a character is on it, they are immediately Busted. </t>
+  </si>
+  <si>
+    <t>figure_alerts_lockdown_one_alert.svg</t>
+  </si>
+  <si>
+    <t>System Reboot</t>
+  </si>
+  <si>
+    <t>Increased Suspician</t>
+  </si>
+  <si>
+    <t>Raise ⚠ for each Character adjacent to an Unsubdued Guard. Also, Raise ⚠ for each Character adjacent to a Live Camera.</t>
+  </si>
+  <si>
+    <t>figure_alerts_adj_camera_guard.svg</t>
+  </si>
+  <si>
+    <t>Raise ⚠ for each hex tile with at least two Characters. %n Raise ⚠ for each Entrance tile with at least two Characters.</t>
+  </si>
+  <si>
+    <t>Raise ⚠ for each Live Camera adjacent to a character.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raise ⚠ for each Character adjacent to an Unsubuded Guard </t>
+  </si>
+  <si>
+    <t>Raise ⚠ for each Character on a Subdued Guard.%nRaise ⚠ for each Character on a Disabled Camera.</t>
+  </si>
+  <si>
+    <t>Make every Disabled Camera Live. Raise ⚠ every time you do this.</t>
+  </si>
+  <si>
+    <t>Close the next Gate, starting with "A". Remove the tile. If a Character is on it, they are Busted. %nRaise ⚠⚠.</t>
+  </si>
+  <si>
+    <t>Raise ⚠⚠.%nUn-Subdue every Subdued Guard that shares a tile with a Character.</t>
+  </si>
+  <si>
+    <t>Shut the Gates!</t>
+  </si>
+  <si>
+    <t>Close the next Gate, starting with "A". Remove the tile. If a Character is on it, they are Busted. %nRaise ⚠.</t>
+  </si>
+  <si>
+    <t>Un-Subdue every Subdued Guard that shares a tile with a Character.</t>
+  </si>
+  <si>
+    <t>Ties Broke!</t>
+  </si>
+  <si>
+    <t>figure_alerts_unsubdue_alerts.svg</t>
   </si>
 </sst>
 </file>
@@ -6270,10 +6306,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6289,153 +6325,307 @@
         <v>0</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C1" s="69" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>417</v>
+        <v>437</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="D2" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>418</v>
+        <v>437</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="D3" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="D4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="D5" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>421</v>
+        <v>441</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="D6" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>422</v>
+        <v>445</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="D7" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>423</v>
+        <v>438</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D8" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>424</v>
+        <v>446</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D9" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>425</v>
+        <v>441</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="D10" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>426</v>
+        <v>445</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>453</v>
+      </c>
+      <c r="D11" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>419</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>455</v>
+      </c>
+      <c r="D12" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>446</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>447</v>
+      </c>
+      <c r="D13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>454</v>
+      </c>
+      <c r="D14" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>441</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>452</v>
+      </c>
+      <c r="D15" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>420</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>440</v>
+      </c>
+      <c r="D16" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>446</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>447</v>
+      </c>
+      <c r="D17" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>438</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>457</v>
+      </c>
+      <c r="D18" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>459</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>458</v>
+      </c>
+      <c r="D19" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>436</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>434</v>
+      </c>
+      <c r="D20" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>456</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
         <v>443</v>
       </c>
-      <c r="D11" t="s">
-        <v>438</v>
+      <c r="D21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>435</v>
+      </c>
+      <c r="D22" t="s">
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new ideas for components
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -15,12 +15,14 @@
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
     <sheet name="Events" sheetId="9" r:id="rId3"/>
-    <sheet name="Helps" sheetId="3" r:id="rId4"/>
-    <sheet name="Actions" sheetId="6" r:id="rId5"/>
-    <sheet name="Skill Ideas" sheetId="4" r:id="rId6"/>
-    <sheet name="Character Ideas" sheetId="5" r:id="rId7"/>
-    <sheet name="Event Ideas" sheetId="7" r:id="rId8"/>
-    <sheet name="Tile ideas" sheetId="8" r:id="rId9"/>
+    <sheet name="Special Events" sheetId="10" r:id="rId4"/>
+    <sheet name="NPC" sheetId="11" r:id="rId5"/>
+    <sheet name="Helps" sheetId="3" r:id="rId6"/>
+    <sheet name="Actions" sheetId="6" r:id="rId7"/>
+    <sheet name="Skill Ideas" sheetId="4" r:id="rId8"/>
+    <sheet name="Character Ideas" sheetId="5" r:id="rId9"/>
+    <sheet name="Event Ideas" sheetId="7" r:id="rId10"/>
+    <sheet name="Tile ideas" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="Actions">Actions!$A$2:$B$47</definedName>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="469">
   <si>
     <t>Name</t>
   </si>
@@ -1331,9 +1333,6 @@
     <t>figure_alerts_alarm.svg</t>
   </si>
   <si>
-    <t>For each hex tile with at least 2 characters on it, increase the alert bar by 1. For Entrance tiles, 2 alerts.</t>
-  </si>
-  <si>
     <t>Replace every Disabled Camera with a Guard.</t>
   </si>
   <si>
@@ -1379,9 +1378,6 @@
     <t>figure_alerts_adj_camera_guard.svg</t>
   </si>
   <si>
-    <t>Raise ⚠ for each hex tile with at least two Characters. %n Raise ⚠ for each Entrance tile with at least two Characters.</t>
-  </si>
-  <si>
     <t>Raise ⚠ for each Live Camera adjacent to a character.</t>
   </si>
   <si>
@@ -1413,6 +1409,36 @@
   </si>
   <si>
     <t>figure_alerts_unsubdue_alerts.svg</t>
+  </si>
+  <si>
+    <t>Reinforcements</t>
+  </si>
+  <si>
+    <t>Guards at the Exit</t>
+  </si>
+  <si>
+    <t>Move the Paintings!</t>
+  </si>
+  <si>
+    <t>Roll6</t>
+  </si>
+  <si>
+    <t>Feeble Prisoner</t>
+  </si>
+  <si>
+    <t>Able Prisoner</t>
+  </si>
+  <si>
+    <t>Lose Ideas!</t>
+  </si>
+  <si>
+    <t>Locks Re-Lock!</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Raise ⚠ for each hex tile with at least two Characters. %n Raise ⚠ ⚠ for each Entrance tile with at least two Characters.</t>
   </si>
 </sst>
 </file>
@@ -2346,7 +2372,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3168,6 +3194,131 @@
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="80" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6306,21 +6457,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="131.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="131.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
@@ -6328,303 +6480,306 @@
         <v>421</v>
       </c>
       <c r="C1" s="69" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="E1" s="69" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>449</v>
-      </c>
       <c r="D2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E2" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>433</v>
-      </c>
       <c r="D3" t="s">
+        <v>468</v>
+      </c>
+      <c r="E3" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>417</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>450</v>
-      </c>
       <c r="D4" t="s">
+        <v>448</v>
+      </c>
+      <c r="E4" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>418</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>451</v>
-      </c>
       <c r="D5" t="s">
+        <v>449</v>
+      </c>
+      <c r="E5" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>452</v>
-      </c>
       <c r="D6" t="s">
+        <v>450</v>
+      </c>
+      <c r="E6" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>453</v>
-      </c>
       <c r="D7" t="s">
+        <v>451</v>
+      </c>
+      <c r="E7" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>454</v>
-      </c>
       <c r="D8" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+      <c r="E8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>446</v>
+      </c>
+      <c r="E9" t="s">
         <v>447</v>
       </c>
-      <c r="D9" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
-        <v>452</v>
-      </c>
       <c r="D10" t="s">
+        <v>450</v>
+      </c>
+      <c r="E10" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>453</v>
-      </c>
       <c r="D11" t="s">
+        <v>451</v>
+      </c>
+      <c r="E11" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>419</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
-        <v>455</v>
-      </c>
       <c r="D12" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+      <c r="E12" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>446</v>
+      </c>
+      <c r="E13" t="s">
         <v>447</v>
       </c>
-      <c r="D13" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
-        <v>454</v>
-      </c>
       <c r="D14" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+      <c r="E14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>452</v>
-      </c>
       <c r="D15" t="s">
+        <v>450</v>
+      </c>
+      <c r="E15" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>420</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
-        <v>440</v>
-      </c>
       <c r="D16" t="s">
+        <v>439</v>
+      </c>
+      <c r="E16" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>446</v>
+      </c>
+      <c r="E17" t="s">
         <v>447</v>
       </c>
-      <c r="D17" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>455</v>
+      </c>
+      <c r="E18" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>457</v>
-      </c>
-      <c r="D18" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>459</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
-        <v>458</v>
-      </c>
       <c r="D19" t="s">
+        <v>456</v>
+      </c>
+      <c r="E19" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>434</v>
-      </c>
       <c r="D20" t="s">
+        <v>433</v>
+      </c>
+      <c r="E20" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>443</v>
-      </c>
       <c r="D21" t="s">
+        <v>442</v>
+      </c>
+      <c r="E21" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
-        <v>435</v>
-      </c>
       <c r="D22" t="s">
+        <v>434</v>
+      </c>
+      <c r="E22" t="s">
         <v>432</v>
       </c>
     </row>
@@ -6635,6 +6790,106 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>467</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>466</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -6735,7 +6990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
@@ -7440,7 +7695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:S63"/>
   <sheetViews>
@@ -9007,7 +9262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
@@ -9223,129 +9478,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="80" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>197</v>
-      </c>
-      <c r="B4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
events: more special event ideas
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18720" windowHeight="11175" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="475">
   <si>
     <t>Name</t>
   </si>
@@ -1429,16 +1429,34 @@
     <t>Able Prisoner</t>
   </si>
   <si>
-    <t>Lose Ideas!</t>
-  </si>
-  <si>
-    <t>Locks Re-Lock!</t>
-  </si>
-  <si>
     <t>Story</t>
   </si>
   <si>
     <t>Raise ⚠ for each hex tile with at least two Characters. %n Raise ⚠ ⚠ for each Entrance tile with at least two Characters.</t>
+  </si>
+  <si>
+    <t>Prisoners Panic!</t>
+  </si>
+  <si>
+    <t>Flip the prisoner cards over</t>
+  </si>
+  <si>
+    <t>Watchtower</t>
+  </si>
+  <si>
+    <t>Add a Guard to every hex with a Character on it in a direct line emanating from the Watchtower token</t>
+  </si>
+  <si>
+    <t>(Maybe multiple of these events?)</t>
+  </si>
+  <si>
+    <t>Add a Guard token to every hex adjacent to an Exit</t>
+  </si>
+  <si>
+    <t>Add a Lock to any loot not yet stolen</t>
+  </si>
+  <si>
+    <t>Lock the Goods!</t>
   </si>
 </sst>
 </file>
@@ -6459,7 +6477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -6480,7 +6498,7 @@
         <v>421</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D1" s="69" t="s">
         <v>26</v>
@@ -6497,7 +6515,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E2" t="s">
         <v>423</v>
@@ -6511,7 +6529,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E3" t="s">
         <v>423</v>
@@ -6791,53 +6809,73 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C1" s="69" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+      <c r="C5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>466</v>
+        <v>467</v>
+      </c>
+      <c r="C6" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>469</v>
+      </c>
+      <c r="C7" t="s">
+        <v>470</v>
+      </c>
+      <c r="D7" t="s">
+        <v>471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
events: bigger cards, stories added
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -28,11 +28,12 @@
     <definedName name="Actions">Actions!$A$2:$B$47</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="490">
   <si>
     <t>Name</t>
   </si>
@@ -1354,9 +1355,6 @@
     <t>Add a Guard from the supply to each tile that has a Character adjacent to at least one Live Camera.</t>
   </si>
   <si>
-    <t>Tripped Over Stuff</t>
-  </si>
-  <si>
     <t>figure_alerts_lockdown_two_alerts.svg</t>
   </si>
   <si>
@@ -1384,9 +1382,6 @@
     <t xml:space="preserve">Raise ⚠ for each Character adjacent to an Unsubuded Guard </t>
   </si>
   <si>
-    <t>Raise ⚠ for each Character on a Subdued Guard.%nRaise ⚠ for each Character on a Disabled Camera.</t>
-  </si>
-  <si>
     <t>Make every Disabled Camera Live. Raise ⚠ every time you do this.</t>
   </si>
   <si>
@@ -1457,6 +1452,57 @@
   </si>
   <si>
     <t>Lock the Goods!</t>
+  </si>
+  <si>
+    <t>Teammates in the same spots get anxious and start bickering as they get started, raising suspicion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The guard monitoring the cameras sees movement in a reflection and looks a little closer. </t>
+  </si>
+  <si>
+    <t>Guards are getting suspcious of movement.</t>
+  </si>
+  <si>
+    <t>Guard Spills Beans</t>
+  </si>
+  <si>
+    <t>Raise ⚠ for each Character on a Subdued Guard.%nGive 💡💡 to each of those Characters too.</t>
+  </si>
+  <si>
+    <t>Fearful of what might happen to him, a guard begins blabbing. He's noisy, but provides useful intel.</t>
+  </si>
+  <si>
+    <t>The Guards notice that some cameras are not working. They turning them off and on again.</t>
+  </si>
+  <si>
+    <t>An automatic system initiates, closing the next lockdown gate.</t>
+  </si>
+  <si>
+    <t>An automatic system initiates, closing the next two lockdown gates.</t>
+  </si>
+  <si>
+    <t>More movement gets noticed.</t>
+  </si>
+  <si>
+    <t>Guards are shouting at each other now, about ready to pull the alarm.</t>
+  </si>
+  <si>
+    <t>Emboldened by the alerts that have been raised, the Guards begin escaping their bonds.</t>
+  </si>
+  <si>
+    <t>Guards begin showing up to investigate all of the broken cameras.</t>
+  </si>
+  <si>
+    <t>This is it.</t>
+  </si>
+  <si>
+    <t>Subduing guards got a little sloppy.</t>
+  </si>
+  <si>
+    <t>Guards are studying the cameras more closely now.</t>
+  </si>
+  <si>
+    <t>Increased Suspicion</t>
   </si>
 </sst>
 </file>
@@ -3348,7 +3394,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W2" sqref="W2"/>
+      <selection pane="bottomRight" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6477,15 +6523,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="131.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -6498,7 +6544,7 @@
         <v>421</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D1" s="69" t="s">
         <v>26</v>
@@ -6514,8 +6560,11 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>473</v>
+      </c>
       <c r="D2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E2" t="s">
         <v>423</v>
@@ -6528,8 +6577,11 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>473</v>
+      </c>
       <c r="D3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E3" t="s">
         <v>423</v>
@@ -6542,8 +6594,11 @@
       <c r="B4">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>474</v>
+      </c>
       <c r="D4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E4" t="s">
         <v>424</v>
@@ -6556,8 +6611,11 @@
       <c r="B5">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>475</v>
+      </c>
       <c r="D5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E5" t="s">
         <v>425</v>
@@ -6565,13 +6623,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>478</v>
+      </c>
       <c r="D6" t="s">
-        <v>450</v>
+        <v>477</v>
       </c>
       <c r="E6" t="s">
         <v>426</v>
@@ -6579,13 +6640,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>479</v>
+      </c>
       <c r="D7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E7" t="s">
         <v>427</v>
@@ -6598,36 +6662,45 @@
       <c r="B8">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>480</v>
+      </c>
       <c r="D8" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>445</v>
+        <v>489</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>482</v>
+      </c>
       <c r="D9" t="s">
+        <v>445</v>
+      </c>
+      <c r="E9" t="s">
         <v>446</v>
-      </c>
-      <c r="E9" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
+      <c r="C10" t="s">
+        <v>478</v>
+      </c>
       <c r="D10" t="s">
-        <v>450</v>
+        <v>477</v>
       </c>
       <c r="E10" t="s">
         <v>426</v>
@@ -6635,13 +6708,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>479</v>
+      </c>
       <c r="D11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E11" t="s">
         <v>427</v>
@@ -6654,25 +6730,31 @@
       <c r="B12">
         <v>11</v>
       </c>
+      <c r="C12" t="s">
+        <v>487</v>
+      </c>
       <c r="D12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
+      <c r="C13" t="s">
+        <v>482</v>
+      </c>
       <c r="D13" t="s">
+        <v>445</v>
+      </c>
+      <c r="E13" t="s">
         <v>446</v>
-      </c>
-      <c r="E13" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6682,22 +6764,28 @@
       <c r="B14">
         <v>13</v>
       </c>
+      <c r="C14" t="s">
+        <v>480</v>
+      </c>
       <c r="D14" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
+      <c r="C15" t="s">
+        <v>478</v>
+      </c>
       <c r="D15" t="s">
-        <v>450</v>
+        <v>477</v>
       </c>
       <c r="E15" t="s">
         <v>426</v>
@@ -6710,6 +6798,9 @@
       <c r="B16">
         <v>15</v>
       </c>
+      <c r="C16" t="s">
+        <v>488</v>
+      </c>
       <c r="D16" t="s">
         <v>439</v>
       </c>
@@ -6719,16 +6810,19 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>445</v>
+        <v>489</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
+      <c r="C17" t="s">
+        <v>483</v>
+      </c>
       <c r="D17" t="s">
+        <v>445</v>
+      </c>
+      <c r="E17" t="s">
         <v>446</v>
-      </c>
-      <c r="E17" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -6738,22 +6832,28 @@
       <c r="B18">
         <v>17</v>
       </c>
+      <c r="C18" t="s">
+        <v>480</v>
+      </c>
       <c r="D18" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
+      <c r="C19" t="s">
+        <v>484</v>
+      </c>
       <c r="D19" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E19" t="s">
         <v>429</v>
@@ -6766,6 +6866,9 @@
       <c r="B20">
         <v>19</v>
       </c>
+      <c r="C20" t="s">
+        <v>485</v>
+      </c>
       <c r="D20" t="s">
         <v>433</v>
       </c>
@@ -6775,13 +6878,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
+      <c r="C21" t="s">
+        <v>481</v>
+      </c>
       <c r="D21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E21" t="s">
         <v>428</v>
@@ -6793,6 +6899,9 @@
       </c>
       <c r="B22">
         <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>486</v>
       </c>
       <c r="D22" t="s">
         <v>434</v>
@@ -6811,8 +6920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6827,7 +6936,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C1" s="69" t="s">
         <v>26</v>
@@ -6835,47 +6944,47 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>467</v>
+      </c>
+      <c r="C7" t="s">
+        <v>468</v>
+      </c>
+      <c r="D7" t="s">
         <v>469</v>
-      </c>
-      <c r="C7" t="s">
-        <v>470</v>
-      </c>
-      <c r="D7" t="s">
-        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -6909,17 +7018,17 @@
         <v>139</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
special events: they exist now!
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="493">
   <si>
     <t>Name</t>
   </si>
@@ -1367,9 +1367,6 @@
     <t>System Reboot</t>
   </si>
   <si>
-    <t>Increased Suspician</t>
-  </si>
-  <si>
     <t>Raise ⚠ for each Character adjacent to an Unsubdued Guard. Also, Raise ⚠ for each Character adjacent to a Live Camera.</t>
   </si>
   <si>
@@ -1436,15 +1433,6 @@
     <t>Flip the prisoner cards over</t>
   </si>
   <si>
-    <t>Watchtower</t>
-  </si>
-  <si>
-    <t>Add a Guard to every hex with a Character on it in a direct line emanating from the Watchtower token</t>
-  </si>
-  <si>
-    <t>(Maybe multiple of these events?)</t>
-  </si>
-  <si>
     <t>Add a Guard token to every hex adjacent to an Exit</t>
   </si>
   <si>
@@ -1463,9 +1451,6 @@
     <t>Guards are getting suspcious of movement.</t>
   </si>
   <si>
-    <t>Guard Spills Beans</t>
-  </si>
-  <si>
     <t>Raise ⚠ for each Character on a Subdued Guard.%nGive 💡💡 to each of those Characters too.</t>
   </si>
   <si>
@@ -1503,6 +1488,30 @@
   </si>
   <si>
     <t>Increased Suspicion</t>
+  </si>
+  <si>
+    <t>special_events_reinforcements.svg</t>
+  </si>
+  <si>
+    <t>special_events_watchtower.svg</t>
+  </si>
+  <si>
+    <t>The Watchtower performs a sweep in every direction.</t>
+  </si>
+  <si>
+    <t>Watchtower Sweep</t>
+  </si>
+  <si>
+    <t>Add a Guard to every hex with a Character on it in a direct line originating from a Watchtower token.</t>
+  </si>
+  <si>
+    <t>A group of guards rally at one of their waypoints.</t>
+  </si>
+  <si>
+    <t>Unsubdue/Re-lock/Re-enable every Guard/Lock/Camera adjacent to each Reinforcement token. Add a Guard to empty spaces adjacent to the token. Replace the token with two Guards.</t>
+  </si>
+  <si>
+    <t>Guard Starts Blabbing</t>
   </si>
 </sst>
 </file>
@@ -6524,7 +6533,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6544,7 +6553,7 @@
         <v>421</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D1" s="69" t="s">
         <v>26</v>
@@ -6561,10 +6570,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E2" t="s">
         <v>423</v>
@@ -6578,10 +6587,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E3" t="s">
         <v>423</v>
@@ -6595,10 +6604,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E4" t="s">
         <v>424</v>
@@ -6612,10 +6621,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E5" t="s">
         <v>425</v>
@@ -6623,16 +6632,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>476</v>
+        <v>492</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="D6" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="E6" t="s">
         <v>426</v>
@@ -6646,10 +6655,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E7" t="s">
         <v>427</v>
@@ -6663,10 +6672,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E8" t="s">
         <v>440</v>
@@ -6674,33 +6683,33 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D9" t="s">
+        <v>444</v>
+      </c>
+      <c r="E9" t="s">
         <v>445</v>
-      </c>
-      <c r="E9" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>476</v>
+        <v>492</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="D10" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="E10" t="s">
         <v>426</v>
@@ -6714,10 +6723,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E11" t="s">
         <v>427</v>
@@ -6731,30 +6740,30 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E12" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>444</v>
+        <v>484</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D13" t="s">
+        <v>444</v>
+      </c>
+      <c r="E13" t="s">
         <v>445</v>
-      </c>
-      <c r="E13" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6765,10 +6774,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E14" t="s">
         <v>440</v>
@@ -6776,16 +6785,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>476</v>
+        <v>492</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="D15" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="E15" t="s">
         <v>426</v>
@@ -6799,7 +6808,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D16" t="s">
         <v>439</v>
@@ -6810,19 +6819,19 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="D17" t="s">
+        <v>444</v>
+      </c>
+      <c r="E17" t="s">
         <v>445</v>
-      </c>
-      <c r="E17" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -6833,10 +6842,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D18" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E18" t="s">
         <v>442</v>
@@ -6844,16 +6853,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D19" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E19" t="s">
         <v>429</v>
@@ -6867,7 +6876,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D20" t="s">
         <v>433</v>
@@ -6878,13 +6887,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D21" t="s">
         <v>441</v>
@@ -6901,7 +6910,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="D22" t="s">
         <v>434</v>
@@ -6921,7 +6930,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6929,6 +6938,7 @@
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="93" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
@@ -6936,55 +6946,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C1" s="69" t="s">
         <v>26</v>
       </c>
+      <c r="D1" s="69" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>457</v>
+        <v>456</v>
+      </c>
+      <c r="B2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" t="s">
+        <v>491</v>
+      </c>
+      <c r="D2" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>458</v>
+        <v>488</v>
+      </c>
+      <c r="B3" t="s">
+        <v>487</v>
       </c>
       <c r="C3" t="s">
-        <v>470</v>
+        <v>489</v>
+      </c>
+      <c r="D3" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>459</v>
+        <v>457</v>
+      </c>
+      <c r="C4" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>472</v>
-      </c>
-      <c r="C5" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="C6" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C7" t="s">
-        <v>468</v>
-      </c>
-      <c r="D7" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -7018,17 +7043,17 @@
         <v>139</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
events: bring back camera on a character
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -1489,9 +1489,6 @@
     <t>A group of guards rally at one of their waypoints.</t>
   </si>
   <si>
-    <t>Unsubdue/Re-lock/Re-enable every Guard/Lock/Camera adjacent to each Reinforcement token. Add a Guard to empty spaces adjacent to the token. Replace the token with two Guards.</t>
-  </si>
-  <si>
     <t>Guard Starts Blabbing</t>
   </si>
   <si>
@@ -1520,6 +1517,9 @@
   </si>
   <si>
     <t>THERE ARE BETTER WAYS%nCannot 👊. For 💡, may exit Guarded spaces for the rest of your turn. In Escape, you require only 1 Escape Move to exit a space with guards.%n %nINSPIRE%nUse this action and a 🔊 to give a free💡💡  to a player of your choosing.</t>
+  </si>
+  <si>
+    <t>Unsubdue/Re-lock/Re-enable every Guard/Lock/Camera adjacent to each Reinforcement token. Raise ⚠ for any Character on a re-enabled Cameras. Add a Guard to empty spaces adjacent to the token. Replace the token with two Guards.</t>
   </si>
 </sst>
 </file>
@@ -2517,10 +2517,10 @@
         <v>121</v>
       </c>
       <c r="L1" s="29" t="s">
+        <v>486</v>
+      </c>
+      <c r="M1" s="29" t="s">
         <v>487</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2761,7 +2761,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L8" s="19" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nWalk🔊➜ ⇒%nDash🔊➜➜%n %nHeistate 💡⇒%nStudy💡💡"</f>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="H9" s="16"/>
       <c r="K9" s="19" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>79</v>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="H10" s="16"/>
       <c r="K10" s="19" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>79</v>
@@ -3060,7 +3060,7 @@
         <v>362</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="23" t="s">
@@ -3070,7 +3070,7 @@
         <v>398</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L17" s="22" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nGOOD IN A PINCH⇒%nGREAT IN A PINCH"</f>
@@ -3101,11 +3101,11 @@
         <v>362</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H18" s="24"/>
       <c r="K18" s="22" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L18" s="22" t="s">
         <v>79</v>
@@ -3131,13 +3131,13 @@
         <v>362</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>399</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>79</v>
@@ -3385,7 +3385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6519,7 +6519,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6618,7 +6618,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -6686,7 +6686,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -6771,7 +6771,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -6915,8 +6915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6949,13 +6949,13 @@
         <v>450</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>484</v>
       </c>
       <c r="D2" t="s">
-        <v>485</v>
+        <v>495</v>
       </c>
       <c r="E2" t="s">
         <v>479</v>
@@ -7426,7 +7426,7 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C17" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
events: padded events for longer heists
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="499">
   <si>
     <t>Name</t>
   </si>
@@ -1520,6 +1520,15 @@
   </si>
   <si>
     <t>Unsubdue/Re-lock/Re-enable every Guard/Lock/Camera adjacent to each Reinforcement token. Raise ⚠ for any Character on a re-enabled Cameras. Add a Guard to empty spaces adjacent to the token. Replace the token with two Guards.</t>
+  </si>
+  <si>
+    <t>20a</t>
+  </si>
+  <si>
+    <t>20b</t>
+  </si>
+  <si>
+    <t>20c</t>
   </si>
 </sst>
 </file>
@@ -6516,16 +6525,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="131.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
@@ -6535,7 +6544,7 @@
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="154" t="s">
         <v>415</v>
       </c>
       <c r="C1" s="66" t="s">
@@ -6552,7 +6561,7 @@
       <c r="A2" t="s">
         <v>430</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -6569,7 +6578,7 @@
       <c r="A3" t="s">
         <v>430</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -6586,7 +6595,7 @@
       <c r="A4" t="s">
         <v>411</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -6603,7 +6612,7 @@
       <c r="A5" t="s">
         <v>412</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" t="s">
@@ -6620,7 +6629,7 @@
       <c r="A6" t="s">
         <v>485</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" t="s">
@@ -6637,7 +6646,7 @@
       <c r="A7" t="s">
         <v>437</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" t="s">
@@ -6654,7 +6663,7 @@
       <c r="A8" t="s">
         <v>431</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -6671,7 +6680,7 @@
       <c r="A9" t="s">
         <v>478</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" t="s">
@@ -6688,7 +6697,7 @@
       <c r="A10" t="s">
         <v>485</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" t="s">
@@ -6705,7 +6714,7 @@
       <c r="A11" t="s">
         <v>437</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>10</v>
       </c>
       <c r="C11" t="s">
@@ -6722,7 +6731,7 @@
       <c r="A12" t="s">
         <v>413</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" t="s">
@@ -6739,7 +6748,7 @@
       <c r="A13" t="s">
         <v>478</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" t="s">
@@ -6756,7 +6765,7 @@
       <c r="A14" t="s">
         <v>431</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>13</v>
       </c>
       <c r="C14" t="s">
@@ -6773,7 +6782,7 @@
       <c r="A15" t="s">
         <v>485</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" t="s">
@@ -6790,7 +6799,7 @@
       <c r="A16" t="s">
         <v>414</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>15</v>
       </c>
       <c r="C16" t="s">
@@ -6807,7 +6816,7 @@
       <c r="A17" t="s">
         <v>478</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>16</v>
       </c>
       <c r="C17" t="s">
@@ -6824,7 +6833,7 @@
       <c r="A18" t="s">
         <v>431</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>17</v>
       </c>
       <c r="C18" t="s">
@@ -6841,7 +6850,7 @@
       <c r="A19" t="s">
         <v>448</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>18</v>
       </c>
       <c r="C19" t="s">
@@ -6858,7 +6867,7 @@
       <c r="A20" t="s">
         <v>429</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>19</v>
       </c>
       <c r="C20" t="s">
@@ -6875,7 +6884,7 @@
       <c r="A21" t="s">
         <v>445</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>20</v>
       </c>
       <c r="C21" t="s">
@@ -6892,7 +6901,7 @@
       <c r="A22" t="s">
         <v>432</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>21</v>
       </c>
       <c r="C22" t="s">
@@ -6903,6 +6912,57 @@
       </c>
       <c r="E22" t="s">
         <v>426</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>448</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C23" t="s">
+        <v>473</v>
+      </c>
+      <c r="D23" t="s">
+        <v>447</v>
+      </c>
+      <c r="E23" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>414</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C24" t="s">
+        <v>477</v>
+      </c>
+      <c r="D24" t="s">
+        <v>433</v>
+      </c>
+      <c r="E24" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>445</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C25" t="s">
+        <v>470</v>
+      </c>
+      <c r="D25" t="s">
+        <v>435</v>
+      </c>
+      <c r="E25" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -6915,7 +6975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
events: lockdown gates is a special event
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="504">
   <si>
     <t>Name</t>
   </si>
@@ -1411,9 +1411,6 @@
     <t>Prisoners Panic!</t>
   </si>
   <si>
-    <t>Flip the prisoner cards over</t>
-  </si>
-  <si>
     <t>Add a Guard token to every hex adjacent to an Exit</t>
   </si>
   <si>
@@ -1529,6 +1526,24 @@
   </si>
   <si>
     <t>20c</t>
+  </si>
+  <si>
+    <t>Shut Two Gates!!</t>
+  </si>
+  <si>
+    <t>In an attempt to isolate your team, the guards shut two lockdown gates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close the next two Gates, starting with "A". Remove the tile. If a character is on it, they are immediately Busted. </t>
+  </si>
+  <si>
+    <t>Flip the prisoner cards over.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The </t>
+  </si>
+  <si>
+    <t>special_events_gates.svg</t>
   </si>
 </sst>
 </file>
@@ -2526,10 +2541,10 @@
         <v>121</v>
       </c>
       <c r="L1" s="29" t="s">
+        <v>485</v>
+      </c>
+      <c r="M1" s="29" t="s">
         <v>486</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2770,7 +2785,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L8" s="19" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nWalk🔊➜ ⇒%nDash🔊➜➜%n %nHeistate 💡⇒%nStudy💡💡"</f>
@@ -2805,7 +2820,7 @@
       </c>
       <c r="H9" s="16"/>
       <c r="K9" s="19" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>79</v>
@@ -2835,7 +2850,7 @@
       </c>
       <c r="H10" s="16"/>
       <c r="K10" s="19" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>79</v>
@@ -3069,7 +3084,7 @@
         <v>362</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="23" t="s">
@@ -3079,7 +3094,7 @@
         <v>398</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L17" s="22" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nGOOD IN A PINCH⇒%nGREAT IN A PINCH"</f>
@@ -3110,11 +3125,11 @@
         <v>362</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H18" s="24"/>
       <c r="K18" s="22" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L18" s="22" t="s">
         <v>79</v>
@@ -3140,13 +3155,13 @@
         <v>362</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>399</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>79</v>
@@ -6527,8 +6542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6565,7 +6580,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D2" t="s">
         <v>457</v>
@@ -6582,7 +6597,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D3" t="s">
         <v>457</v>
@@ -6599,7 +6614,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D4" t="s">
         <v>440</v>
@@ -6616,7 +6631,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D5" t="s">
         <v>441</v>
@@ -6627,16 +6642,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E6" t="s">
         <v>420</v>
@@ -6650,7 +6665,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D7" t="s">
         <v>442</v>
@@ -6667,7 +6682,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D8" t="s">
         <v>443</v>
@@ -6678,13 +6693,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D9" t="s">
         <v>438</v>
@@ -6695,16 +6710,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E10" t="s">
         <v>420</v>
@@ -6718,7 +6733,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D11" t="s">
         <v>442</v>
@@ -6735,7 +6750,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D12" t="s">
         <v>444</v>
@@ -6746,13 +6761,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D13" t="s">
         <v>438</v>
@@ -6769,7 +6784,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D14" t="s">
         <v>443</v>
@@ -6780,16 +6795,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E15" t="s">
         <v>420</v>
@@ -6803,7 +6818,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D16" t="s">
         <v>433</v>
@@ -6814,13 +6829,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D17" t="s">
         <v>438</v>
@@ -6837,7 +6852,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D18" t="s">
         <v>446</v>
@@ -6854,7 +6869,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D19" t="s">
         <v>447</v>
@@ -6871,7 +6886,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D20" t="s">
         <v>427</v>
@@ -6888,10 +6903,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D21" t="s">
-        <v>435</v>
+        <v>500</v>
       </c>
       <c r="E21" t="s">
         <v>422</v>
@@ -6905,7 +6920,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D22" t="s">
         <v>428</v>
@@ -6919,10 +6934,10 @@
         <v>448</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C23" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D23" t="s">
         <v>447</v>
@@ -6936,10 +6951,10 @@
         <v>414</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C24" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D24" t="s">
         <v>433</v>
@@ -6953,10 +6968,10 @@
         <v>445</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C25" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D25" t="s">
         <v>435</v>
@@ -6973,10 +6988,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7012,71 +7027,91 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D3" t="s">
         <v>482</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>481</v>
-      </c>
-      <c r="D3" t="s">
-        <v>483</v>
-      </c>
       <c r="E3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>451</v>
+        <v>498</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>499</v>
       </c>
       <c r="D4" t="s">
-        <v>460</v>
+        <v>500</v>
+      </c>
+      <c r="E4" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
+      <c r="D5" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>461</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>459</v>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>458</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>502</v>
+      </c>
+      <c r="D8" t="s">
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -7486,7 +7521,7 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C17" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
some NPC ideas, scenario smoothing
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="518">
   <si>
     <t>Name</t>
   </si>
@@ -1396,12 +1396,6 @@
     <t>Roll6</t>
   </si>
   <si>
-    <t>Feeble Prisoner</t>
-  </si>
-  <si>
-    <t>Able Prisoner</t>
-  </si>
-  <si>
     <t>Story</t>
   </si>
   <si>
@@ -1544,6 +1538,54 @@
   </si>
   <si>
     <t>special_events_gates.svg</t>
+  </si>
+  <si>
+    <t>Panicked Prisoner</t>
+  </si>
+  <si>
+    <t>Freed Prisoner</t>
+  </si>
+  <si>
+    <t>Hostage</t>
+  </si>
+  <si>
+    <t>Dash🔊➜➜</t>
+  </si>
+  <si>
+    <t>Crawl➜</t>
+  </si>
+  <si>
+    <t>Must share a tile with a Player Character at the end of every Character Action phase.</t>
+  </si>
+  <si>
+    <t>Run🔊🔊➜➜</t>
+  </si>
+  <si>
+    <t>Panicked Hostage</t>
+  </si>
+  <si>
+    <t>Handle👊📷🔓</t>
+  </si>
+  <si>
+    <t>Walk🔊➜</t>
+  </si>
+  <si>
+    <t>Cannot Pass. Must share a tile with a Player Character at the end of every Character Action phase.</t>
+  </si>
+  <si>
+    <t>Cannot Pass.</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>Panicked Guide</t>
+  </si>
+  <si>
+    <t>Discover🔍🔍</t>
+  </si>
+  <si>
+    <t>Reveal🔍</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2173,6 +2215,12 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2541,10 +2589,10 @@
         <v>121</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2785,7 +2833,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="L8" s="19" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nWalk🔊➜ ⇒%nDash🔊➜➜%n %nHeistate 💡⇒%nStudy💡💡"</f>
@@ -2820,7 +2868,7 @@
       </c>
       <c r="H9" s="16"/>
       <c r="K9" s="19" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>79</v>
@@ -2850,7 +2898,7 @@
       </c>
       <c r="H10" s="16"/>
       <c r="K10" s="19" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>79</v>
@@ -3084,7 +3132,7 @@
         <v>362</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="23" t="s">
@@ -3094,7 +3142,7 @@
         <v>398</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="L17" s="22" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nGOOD IN A PINCH⇒%nGREAT IN A PINCH"</f>
@@ -3125,11 +3173,11 @@
         <v>362</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H18" s="24"/>
       <c r="K18" s="22" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="L18" s="22" t="s">
         <v>79</v>
@@ -3155,13 +3203,13 @@
         <v>362</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>399</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>79</v>
@@ -3413,7 +3461,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U7" sqref="U7"/>
+      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6563,7 +6611,7 @@
         <v>415</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>25</v>
@@ -6580,10 +6628,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E2" t="s">
         <v>417</v>
@@ -6597,10 +6645,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E3" t="s">
         <v>417</v>
@@ -6614,7 +6662,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D4" t="s">
         <v>440</v>
@@ -6631,7 +6679,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D5" t="s">
         <v>441</v>
@@ -6642,16 +6690,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E6" t="s">
         <v>420</v>
@@ -6665,7 +6713,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D7" t="s">
         <v>442</v>
@@ -6682,7 +6730,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D8" t="s">
         <v>443</v>
@@ -6693,13 +6741,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D9" t="s">
         <v>438</v>
@@ -6710,16 +6758,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D10" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E10" t="s">
         <v>420</v>
@@ -6733,7 +6781,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D11" t="s">
         <v>442</v>
@@ -6750,7 +6798,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D12" t="s">
         <v>444</v>
@@ -6761,13 +6809,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D13" t="s">
         <v>438</v>
@@ -6784,7 +6832,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D14" t="s">
         <v>443</v>
@@ -6795,16 +6843,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E15" t="s">
         <v>420</v>
@@ -6818,7 +6866,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D16" t="s">
         <v>433</v>
@@ -6829,13 +6877,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D17" t="s">
         <v>438</v>
@@ -6852,7 +6900,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D18" t="s">
         <v>446</v>
@@ -6869,7 +6917,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D19" t="s">
         <v>447</v>
@@ -6886,7 +6934,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D20" t="s">
         <v>427</v>
@@ -6903,10 +6951,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D21" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E21" t="s">
         <v>422</v>
@@ -6920,7 +6968,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D22" t="s">
         <v>428</v>
@@ -6934,10 +6982,10 @@
         <v>448</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C23" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D23" t="s">
         <v>447</v>
@@ -6951,10 +6999,10 @@
         <v>414</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D24" t="s">
         <v>433</v>
@@ -6968,10 +7016,10 @@
         <v>445</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C25" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D25" t="s">
         <v>435</v>
@@ -6990,7 +7038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -7010,7 +7058,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>25</v>
@@ -7027,47 +7075,47 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>478</v>
+      </c>
+      <c r="D3" t="s">
         <v>480</v>
       </c>
-      <c r="D3" t="s">
-        <v>482</v>
-      </c>
       <c r="E3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>496</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>497</v>
+      </c>
+      <c r="D4" t="s">
         <v>498</v>
       </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>499</v>
-      </c>
-      <c r="D4" t="s">
-        <v>500</v>
-      </c>
       <c r="E4" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -7078,7 +7126,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -7091,27 +7139,27 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -7121,41 +7169,136 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25" style="155" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="66" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
-        <v>25</v>
+      <c r="B1" s="154" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="66" t="s">
         <v>138</v>
       </c>
       <c r="D1" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="66" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="156" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>506</v>
+      </c>
+      <c r="E2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>455</v>
+        <v>502</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>508</v>
+      </c>
+      <c r="E3" t="s">
+        <v>511</v>
+      </c>
+      <c r="F3" s="155" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>504</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>506</v>
+      </c>
+      <c r="D4" t="s">
+        <v>510</v>
+      </c>
+      <c r="F4" s="155" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>508</v>
+      </c>
+      <c r="E5" t="s">
+        <v>511</v>
+      </c>
+      <c r="F5" s="155" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>517</v>
+      </c>
+      <c r="E6" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>508</v>
+      </c>
+      <c r="E7" t="s">
+        <v>511</v>
+      </c>
+      <c r="F7" s="155" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -7269,7 +7412,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7521,7 +7664,7 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C17" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
characters: continue sketching new ones
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\project-timber-wolf\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\code\timber-wolf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="528">
   <si>
     <t>Name</t>
   </si>
@@ -1261,12 +1261,6 @@
     <t>Toss Loot%n(above)</t>
   </si>
   <si>
-    <t>LARCENIST%nYou may pick up items in an adjacent tile as if it were on your tile.</t>
-  </si>
-  <si>
-    <t>SWINDLER%nYou may pick up items in an adjacent tile, and may drop items on an adjacent tile as if it were on your tile.%n %nTOSS LOOT%nUse this action to place any of your loot up to two tiles away in a single direction. You may not toss over locked tiles or gaps.</t>
-  </si>
-  <si>
     <t>Caught in a Reflection</t>
   </si>
   <si>
@@ -1492,9 +1486,6 @@
     <t>💡🔍🔊</t>
   </si>
   <si>
-    <t>Observe%n💡🔍🔊</t>
-  </si>
-  <si>
     <t>VANTAGE POINT%nWhen outdoors, may 🔍 once per turn%n %nGOOD IN A PINCH%nDuring Escape, may spend %n💡💡 to give 💡 to any player, one time.</t>
   </si>
   <si>
@@ -1586,6 +1577,45 @@
   </si>
   <si>
     <t>Reveal🔍</t>
+  </si>
+  <si>
+    <t>Patch In%n(above)</t>
+  </si>
+  <si>
+    <t>Shutter Bug</t>
+  </si>
+  <si>
+    <t>Surveillance</t>
+  </si>
+  <si>
+    <t>Short%n📷📷🔊</t>
+  </si>
+  <si>
+    <t>Report%n💡🔍🔊</t>
+  </si>
+  <si>
+    <t>FOLLOWER%nFor 💡, may 🔊➜ as long as the destination of the move has another character at the time of the move.%n %nPATCH IN%nWhen adjacent to a live camera, use this action for 💡💡🔍🔊</t>
+  </si>
+  <si>
+    <t>PATCH IN%nWhen adjacent to a live camera, use this action for 💡💡🔍🔊</t>
+  </si>
+  <si>
+    <t>LOOP FOOTAGE%nFor 💡💡, use this action to allow all characters to avoid raising ⚠ due to cameras this action and event phase.%n %nPATCH IN%nWhen adjacent to a live camera, use this action for 💡💡🔍🔊</t>
+  </si>
+  <si>
+    <t>Loop Footage%n(above)</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>Hit%n👊🔊</t>
+  </si>
+  <si>
+    <t>LARCENIST%nFor 💡, you may pick up items in an adjacent, not locked tile as if it were on your tile for the rest of the phase.</t>
+  </si>
+  <si>
+    <t>SWINDLER%nFor 💡, you may pick up or drop items in an adjacent, not locked tile as if it were on your tile for the rest of the phase.%n %nTOSS LOOT%nUse this action to place any of your loot up to two tiles away in a single direction. You may not toss over locked tiles or gaps.</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2221,6 +2251,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2531,16 +2568,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="26" bestFit="1" customWidth="1"/>
@@ -2549,7 +2586,7 @@
     <col min="8" max="8" width="19" style="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5703125" style="25" customWidth="1"/>
+    <col min="11" max="11" width="240.140625" style="25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" style="25" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="25"/>
   </cols>
@@ -2589,10 +2626,10 @@
         <v>121</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2827,13 +2864,13 @@
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="13" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="L8" s="19" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nWalk🔊➜ ⇒%nDash🔊➜➜%n %nHeistate 💡⇒%nStudy💡💡"</f>
@@ -2868,7 +2905,7 @@
       </c>
       <c r="H9" s="16"/>
       <c r="K9" s="19" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>79</v>
@@ -2898,7 +2935,7 @@
       </c>
       <c r="H10" s="16"/>
       <c r="K10" s="19" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>79</v>
@@ -3132,7 +3169,7 @@
         <v>362</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>486</v>
+        <v>519</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="23" t="s">
@@ -3142,7 +3179,7 @@
         <v>398</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="L17" s="22" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nGOOD IN A PINCH⇒%nGREAT IN A PINCH"</f>
@@ -3173,11 +3210,11 @@
         <v>362</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>486</v>
+        <v>519</v>
       </c>
       <c r="H18" s="24"/>
       <c r="K18" s="22" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="L18" s="22" t="s">
         <v>79</v>
@@ -3203,13 +3240,13 @@
         <v>362</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>486</v>
+        <v>519</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>399</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>79</v>
@@ -3235,17 +3272,17 @@
         <v>140</v>
       </c>
       <c r="G20" s="149" t="s">
-        <v>406</v>
+        <v>525</v>
       </c>
       <c r="H20" s="149"/>
       <c r="I20" s="150" t="s">
         <v>12</v>
       </c>
       <c r="J20" s="150" t="s">
-        <v>405</v>
+        <v>14</v>
       </c>
       <c r="K20" s="150" t="s">
-        <v>409</v>
+        <v>526</v>
       </c>
       <c r="L20" s="150" t="str">
         <f>"+1 Memory%n+1 Initial 💡%n %nLARCENIST⇒%nSWINDLER%n %n+TOSS LOOT"</f>
@@ -3270,19 +3307,19 @@
         <v>8</v>
       </c>
       <c r="E21" s="149">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="149" t="s">
         <v>140</v>
       </c>
       <c r="G21" s="149" t="s">
-        <v>406</v>
+        <v>525</v>
       </c>
       <c r="H21" s="149" t="s">
         <v>408</v>
       </c>
       <c r="K21" s="150" t="s">
-        <v>410</v>
+        <v>527</v>
       </c>
       <c r="L21" s="150" t="s">
         <v>79</v>
@@ -3290,7 +3327,7 @@
     </row>
     <row r="22" spans="1:13" s="150" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="150" t="s">
-        <v>405</v>
+        <v>14</v>
       </c>
       <c r="B22" s="148" t="s">
         <v>401</v>
@@ -3305,17 +3342,110 @@
         <v>3</v>
       </c>
       <c r="F22" s="149" t="s">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="G22" s="149" t="s">
-        <v>364</v>
+        <v>525</v>
       </c>
       <c r="H22" s="149"/>
       <c r="K22" s="150" t="s">
-        <v>409</v>
+        <v>526</v>
       </c>
       <c r="L22" s="150" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="157" t="s">
+        <v>516</v>
+      </c>
+      <c r="B23" s="158" t="s">
+        <v>517</v>
+      </c>
+      <c r="C23" s="159">
+        <v>1</v>
+      </c>
+      <c r="D23" s="159">
+        <v>7</v>
+      </c>
+      <c r="E23" s="159">
+        <v>3</v>
+      </c>
+      <c r="F23" s="159" t="s">
+        <v>140</v>
+      </c>
+      <c r="G23" s="159" t="s">
+        <v>406</v>
+      </c>
+      <c r="H23" s="159" t="s">
+        <v>515</v>
+      </c>
+      <c r="I23" s="157" t="s">
+        <v>524</v>
+      </c>
+      <c r="J23" s="157" t="s">
+        <v>405</v>
+      </c>
+      <c r="K23" s="157" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="157" t="s">
+        <v>524</v>
+      </c>
+      <c r="B24" s="157" t="s">
+        <v>517</v>
+      </c>
+      <c r="C24" s="159">
+        <v>2</v>
+      </c>
+      <c r="D24" s="159">
+        <v>9</v>
+      </c>
+      <c r="E24" s="159">
+        <v>4</v>
+      </c>
+      <c r="F24" s="159" t="s">
+        <v>407</v>
+      </c>
+      <c r="G24" s="159" t="s">
+        <v>523</v>
+      </c>
+      <c r="H24" s="159" t="s">
+        <v>515</v>
+      </c>
+      <c r="K24" s="157" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="157" t="s">
+        <v>405</v>
+      </c>
+      <c r="B25" s="158" t="s">
+        <v>517</v>
+      </c>
+      <c r="C25" s="159">
+        <v>2</v>
+      </c>
+      <c r="D25" s="159">
+        <v>8</v>
+      </c>
+      <c r="E25" s="159">
+        <v>5</v>
+      </c>
+      <c r="F25" s="159" t="s">
+        <v>364</v>
+      </c>
+      <c r="G25" s="159" t="s">
+        <v>518</v>
+      </c>
+      <c r="H25" s="159" t="s">
+        <v>515</v>
+      </c>
+      <c r="K25" s="157" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -6608,424 +6738,424 @@
         <v>0</v>
       </c>
       <c r="B1" s="154" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="66" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D3" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D8" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E8" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D9" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E9" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E10" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D11" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E11" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D13" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D14" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D15" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E15" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D16" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E16" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D17" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E17" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D18" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E18" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D19" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D20" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E20" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D21" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E21" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D22" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E22" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C23" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D23" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E23" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D24" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E24" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C25" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D25" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E25" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -7058,80 +7188,80 @@
         <v>1</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="66" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D3" t="s">
         <v>478</v>
       </c>
-      <c r="D3" t="s">
-        <v>480</v>
-      </c>
       <c r="E3" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D4" t="s">
+        <v>495</v>
+      </c>
+      <c r="E4" t="s">
         <v>498</v>
-      </c>
-      <c r="E4" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -7139,27 +7269,27 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D8" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -7171,8 +7301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7199,7 +7329,7 @@
         <v>139</v>
       </c>
       <c r="E1" s="66" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F1" s="156" t="s">
         <v>25</v>
@@ -7207,98 +7337,98 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>503</v>
       </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>506</v>
-      </c>
       <c r="E2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>505</v>
+      </c>
+      <c r="E3" t="s">
         <v>508</v>
       </c>
-      <c r="E3" t="s">
-        <v>511</v>
-      </c>
       <c r="F3" s="155" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D4" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="F4" s="155" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>505</v>
+      </c>
+      <c r="E5" t="s">
         <v>508</v>
       </c>
-      <c r="E5" t="s">
-        <v>511</v>
-      </c>
       <c r="F5" s="155" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E6" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>505</v>
+      </c>
+      <c r="E7" t="s">
         <v>508</v>
       </c>
-      <c r="E7" t="s">
-        <v>511</v>
-      </c>
       <c r="F7" s="155" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -7412,7 +7542,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7664,7 +7794,7 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C17" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
special events: minor revisions
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18450" windowHeight="10905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="527">
   <si>
     <t>Name</t>
   </si>
@@ -1381,9 +1381,6 @@
     <t>Reinforcements</t>
   </si>
   <si>
-    <t>Guards at the Exit</t>
-  </si>
-  <si>
     <t>Move the Paintings!</t>
   </si>
   <si>
@@ -1396,12 +1393,6 @@
     <t>Raise ⚠ for each hex tile with at least two Characters. %n Raise ⚠ ⚠ for each Entrance tile with at least two Characters.</t>
   </si>
   <si>
-    <t>Prisoners Panic!</t>
-  </si>
-  <si>
-    <t>Add a Guard token to every hex adjacent to an Exit</t>
-  </si>
-  <si>
     <t>Add a Lock to any loot not yet stolen</t>
   </si>
   <si>
@@ -1468,9 +1459,6 @@
     <t>Watchtower Sweep</t>
   </si>
   <si>
-    <t>Add a Guard to every hex with a Character on it in a direct line originating from a Watchtower token.</t>
-  </si>
-  <si>
     <t>A group of guards rally at one of their waypoints.</t>
   </si>
   <si>
@@ -1501,9 +1489,6 @@
     <t>THERE ARE BETTER WAYS%nCannot 👊. For 💡, may exit Guarded spaces for the rest of your turn. In Escape, you require only 1 Escape Move to exit a space with guards.%n %nINSPIRE%nUse this action and a 🔊 to give a free💡💡  to a player of your choosing.</t>
   </si>
   <si>
-    <t>Unsubdue/Re-lock/Re-enable every Guard/Lock/Camera adjacent to each Reinforcement token. Raise ⚠ for any Character on a re-enabled Cameras. Add a Guard to empty spaces adjacent to the token. Replace the token with two Guards.</t>
-  </si>
-  <si>
     <t>20a</t>
   </si>
   <si>
@@ -1522,12 +1507,6 @@
     <t xml:space="preserve">Close the next two Gates, starting with "A". Remove the tile. If a character is on it, they are immediately Busted. </t>
   </si>
   <si>
-    <t>Flip the prisoner cards over.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The </t>
-  </si>
-  <si>
     <t>special_events_gates.svg</t>
   </si>
   <si>
@@ -1616,6 +1595,24 @@
   </si>
   <si>
     <t>SWINDLER%nFor 💡, you may pick up or drop items in an adjacent, not locked tile as if it were on your tile for the rest of the phase.%n %nTOSS LOOT%nUse this action to place any of your loot up to two tiles away in a single direction. You may not toss over locked tiles or gaps.</t>
+  </si>
+  <si>
+    <t>Panic!</t>
+  </si>
+  <si>
+    <t>Flip over every non-player character card.</t>
+  </si>
+  <si>
+    <t>special_events_panic.svg</t>
+  </si>
+  <si>
+    <t>Everyone has a breaking point.</t>
+  </si>
+  <si>
+    <t>Add a Guard to every hex with a Character on it in a direct line originating from a Watchtower token. Excludes being on the tile with a Watchtower.</t>
+  </si>
+  <si>
+    <t>Unsubdue/Re-lock/Re-enable every Guard/Lock/Camera adjacent to each Reinforcement token. Raise ⚠ for every Character on a re-enabled Camera. Add a Guard to empty spaces adjacent to the token. Replace the token with two Guards.</t>
   </si>
 </sst>
 </file>
@@ -2570,7 +2567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -2626,10 +2623,10 @@
         <v>121</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2870,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="L8" s="19" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nWalk🔊➜ ⇒%nDash🔊➜➜%n %nHeistate 💡⇒%nStudy💡💡"</f>
@@ -2905,7 +2902,7 @@
       </c>
       <c r="H9" s="16"/>
       <c r="K9" s="19" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>79</v>
@@ -2935,7 +2932,7 @@
       </c>
       <c r="H10" s="16"/>
       <c r="K10" s="19" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>79</v>
@@ -3169,7 +3166,7 @@
         <v>362</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="23" t="s">
@@ -3179,7 +3176,7 @@
         <v>398</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="L17" s="22" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nGOOD IN A PINCH⇒%nGREAT IN A PINCH"</f>
@@ -3210,11 +3207,11 @@
         <v>362</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="H18" s="24"/>
       <c r="K18" s="22" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="L18" s="22" t="s">
         <v>79</v>
@@ -3240,13 +3237,13 @@
         <v>362</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>399</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>79</v>
@@ -3272,7 +3269,7 @@
         <v>140</v>
       </c>
       <c r="G20" s="149" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="H20" s="149"/>
       <c r="I20" s="150" t="s">
@@ -3282,7 +3279,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="150" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="L20" s="150" t="str">
         <f>"+1 Memory%n+1 Initial 💡%n %nLARCENIST⇒%nSWINDLER%n %n+TOSS LOOT"</f>
@@ -3313,13 +3310,13 @@
         <v>140</v>
       </c>
       <c r="G21" s="149" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="H21" s="149" t="s">
         <v>408</v>
       </c>
       <c r="K21" s="150" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="L21" s="150" t="s">
         <v>79</v>
@@ -3345,11 +3342,11 @@
         <v>140</v>
       </c>
       <c r="G22" s="149" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="H22" s="149"/>
       <c r="K22" s="150" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="L22" s="150" t="s">
         <v>79</v>
@@ -3357,10 +3354,10 @@
     </row>
     <row r="23" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="157" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="B23" s="158" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="C23" s="159">
         <v>1</v>
@@ -3378,16 +3375,16 @@
         <v>406</v>
       </c>
       <c r="H23" s="159" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="I23" s="157" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="J23" s="157" t="s">
         <v>405</v>
       </c>
       <c r="K23" s="157" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="L23" s="157" t="str">
         <f>"+2 Memory%n+ 1 Initial 💡%n %nWalk &amp; Smash⇒%nDisable📷🔊➜%n %n+Loop Footage"</f>
@@ -3400,10 +3397,10 @@
     </row>
     <row r="24" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="157" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="B24" s="157" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="C24" s="159">
         <v>2</v>
@@ -3418,13 +3415,13 @@
         <v>407</v>
       </c>
       <c r="G24" s="159" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="H24" s="159" t="s">
+        <v>508</v>
+      </c>
+      <c r="K24" s="157" t="s">
         <v>515</v>
-      </c>
-      <c r="K24" s="157" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
@@ -3432,7 +3429,7 @@
         <v>405</v>
       </c>
       <c r="B25" s="158" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="C25" s="159">
         <v>2</v>
@@ -3447,13 +3444,13 @@
         <v>364</v>
       </c>
       <c r="G25" s="159" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="H25" s="159" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="K25" s="157" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -6749,7 +6746,7 @@
         <v>413</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>25</v>
@@ -6766,10 +6763,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E2" t="s">
         <v>415</v>
@@ -6783,10 +6780,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E3" t="s">
         <v>415</v>
@@ -6800,7 +6797,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D4" t="s">
         <v>438</v>
@@ -6817,7 +6814,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D5" t="s">
         <v>439</v>
@@ -6828,16 +6825,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D6" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E6" t="s">
         <v>418</v>
@@ -6851,7 +6848,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D7" t="s">
         <v>440</v>
@@ -6868,7 +6865,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D8" t="s">
         <v>441</v>
@@ -6879,13 +6876,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D9" t="s">
         <v>436</v>
@@ -6896,16 +6893,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D10" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E10" t="s">
         <v>418</v>
@@ -6919,7 +6916,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D11" t="s">
         <v>440</v>
@@ -6936,7 +6933,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D12" t="s">
         <v>442</v>
@@ -6947,13 +6944,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D13" t="s">
         <v>436</v>
@@ -6970,7 +6967,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D14" t="s">
         <v>441</v>
@@ -6981,16 +6978,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D15" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E15" t="s">
         <v>418</v>
@@ -7004,7 +7001,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D16" t="s">
         <v>431</v>
@@ -7015,13 +7012,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D17" t="s">
         <v>436</v>
@@ -7038,7 +7035,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D18" t="s">
         <v>444</v>
@@ -7055,7 +7052,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D19" t="s">
         <v>445</v>
@@ -7072,7 +7069,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D20" t="s">
         <v>425</v>
@@ -7089,10 +7086,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D21" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E21" t="s">
         <v>420</v>
@@ -7106,7 +7103,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D22" t="s">
         <v>426</v>
@@ -7120,10 +7117,10 @@
         <v>446</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="C23" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D23" t="s">
         <v>445</v>
@@ -7137,10 +7134,10 @@
         <v>412</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="C24" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D24" t="s">
         <v>431</v>
@@ -7154,10 +7151,10 @@
         <v>443</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="C25" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D25" t="s">
         <v>433</v>
@@ -7174,10 +7171,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7185,7 +7182,8 @@
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="66" customFormat="1" x14ac:dyDescent="0.25">
@@ -7196,7 +7194,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>25</v>
@@ -7213,47 +7211,47 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D2" t="s">
-        <v>489</v>
+        <v>526</v>
       </c>
       <c r="E2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D3" t="s">
-        <v>478</v>
+        <v>525</v>
       </c>
       <c r="E3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D4" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E4" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -7263,41 +7261,33 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>455</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
+      <c r="D6" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>457</v>
+        <v>521</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
+      <c r="C7" t="s">
+        <v>524</v>
+      </c>
       <c r="D7" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>454</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>497</v>
-      </c>
-      <c r="D8" t="s">
-        <v>496</v>
+        <v>522</v>
+      </c>
+      <c r="E7" t="s">
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -7310,7 +7300,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7337,7 +7327,7 @@
         <v>139</v>
       </c>
       <c r="E1" s="66" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F1" s="156" t="s">
         <v>25</v>
@@ -7345,98 +7335,98 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="E2" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="E3" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="F3" s="155" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="D4" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="F4" s="155" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="E5" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="F5" s="155" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="E6" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="E7" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="F7" s="155" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -7802,7 +7792,7 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C17" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
scenarios: more stories, more ideas
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\code\timber-wolf\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\project-timber-wolf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="556">
   <si>
     <t>Name</t>
   </si>
@@ -1638,31 +1638,6 @@
   </si>
   <si>
     <t>3 Days</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Your Last Heist</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Break out of Cell Block A
-- Mention that they had a bunch of amateurs escape recently, so security is on edge.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1687,30 +1662,6 @@
       <t xml:space="preserve">
 - Break into The Gallery to put the paintings back.
 - The Fence discovers he can pull together a Long Con on The Collector by putting them back.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Collector</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Break into The Collector and get the real paintings, leaving fakes</t>
     </r>
   </si>
   <si>
@@ -1812,84 +1763,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>The Tip</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Friend at Customs gets a tip of a shipment of artwork coming in, destined for The Collector's mansion
-- Stolen goods already, so they won't miss it</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Fence</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Introduce The Fence as your narrator
-- Break out of prison to make some money.
-- Cell Block B. 
-- "They've never had a breakout of this prison. Let's blaze that trail."</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Warehouse Job</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Fence points you to The Job
-- Meets with the Boss of the Smugglers, gets a new job
-- Gets busted; they knew you were coming.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>The Incident</t>
     </r>
     <r>
@@ -1902,60 +1775,6 @@
       </rPr>
       <t xml:space="preserve">
 The Fence gets thrown in jail, losing his buddy, Glasses, in a failed deal with The Collector. They were both tunnel rats with the Demo Guy and their Sergeant. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Demo Guy Heist #2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- The Fence joins up with you, and is your Guide. "We're working on a bigger play for this guy."
-- Everyone gets busted anyway. 
-- The Fall guys should get mentioned here too, as if there's this big raid that the cops somehow knew about.
-- Demo guy and Fence mysteriously disappear (goes to Collector's mansion)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Forced Job</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Hostages
-- Forced by The Collector, clearly the villain
-- Get a letter from The Fence explaining The Incident and what he needs.
-- Need to give solid motivation to save these guys and take down The Collector. "That wasn't his real collection - the only way for us to get to his real collection was to get caught." I knew this was our guy when I found the shattered, bloody glasses when we busted into that Estate. </t>
     </r>
   </si>
   <si>
@@ -1987,8 +1806,15 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">The Setup Job
-- </t>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Warehouse Job</t>
     </r>
     <r>
       <rPr>
@@ -1998,10 +1824,139 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Side job where you can get anyone you want from prior Heists who survived. Any team you want (Collector made lots of enemies)
-- Super tough board with that long hallway
-- Teach skills, or buy skills
-- Swap the jewel in for explosives. You get to keep the jewel. He can't resist putting it in his collection</t>
+      <t xml:space="preserve">
+- Your friend from Customs gets you a new job.
+- Gets busted; they knew you were coming. Your friend is there with the cops, takes the goods and a momento from screwing you over and says "This will look good in my collection" (Establishes Villain)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Tip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- "Friend" at Customs gets a tip of a shipment of artwork coming in
+- Stolen goods already, so they won't miss it
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Your Last Heist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Break out of Cell Block B
+- Mention that they had a bunch of amateurs escape recently, so security is a bit on edge.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Fence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Introduce The Fence as your narrator
+- Break out of prison to make some money.
+- Cell Block A. 
+- "They've never had a breakout of this prison. Let's blaze that trail."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Collector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Break into The Collector and get the real paintings, leaving fakes
+- Leaves some bait for The Collector.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Hostage Job</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Hostages
+- Forced by The Collector, clearly the villain
+- Get a letter from The Fence explaining The Incident and what he needs.
+- Need to give solid motivation to save these guys and take down The Collector. "That wasn't his real collection - the only way for us to get to his real collection was to get caught." I knew this was our guy when I found the shattered, bloody glasses when we busted into that Estate. </t>
     </r>
   </si>
   <si>
@@ -2028,7 +1983,60 @@
 - Rescue Fence &amp; Demo Guy
 - Get The Collectors main stash because he keeps the prisoners right next to the stash and the Demo guy busts you out. 
 - The Collector tries to show his paintings as real, can't sell them.
+- (Need one more bad thing to happen to The Collector)
 - "There's always a bigger play"</t>
+    </r>
+  </si>
+  <si>
+    <t>The Forum</t>
+  </si>
+  <si>
+    <t>Standalone board: easy objective, can get new characters and level up. They always have money so it's a good sidetrack. Four entrances so pretty easy.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Demo Guy Heist #2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- The Fence joins up with you, and is your Guide. "We're working on a bigger play for this guy."
+- Everyone gets busted anyway. 
+- The Fall guys should get mentioned here too, as if there's this big raid that the cops somehow knew about.
+- Demo guy and Fence mysteriously disappear (goes to Collector's vault)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Bait
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>You can get anyone you want from prior Heists who survived. (Collector made lots of enemies)
+- Super tough board with that long hallway
+- Teach skills for free, or buy skills
+- Drop the "jewel" in for explosives. You get to keep the jewel. He can't resist putting it in his collection. Make it look like you dropped it on your way out.</t>
     </r>
   </si>
 </sst>
@@ -4042,10 +4050,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,7 +4065,7 @@
     <row r="1" spans="1:10" s="162" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="167"/>
       <c r="B1" s="160" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C1" s="160" t="s">
         <v>530</v>
@@ -4084,20 +4092,20 @@
         <v>527</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="164" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="164" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="168" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B2" s="163"/>
       <c r="C2" s="163"/>
       <c r="E2" s="163" t="s">
+        <v>546</v>
+      </c>
+      <c r="F2" s="163" t="s">
         <v>545</v>
       </c>
-      <c r="F2" s="163" t="s">
+      <c r="G2" s="163" t="s">
         <v>547</v>
-      </c>
-      <c r="G2" s="163" t="s">
-        <v>535</v>
       </c>
       <c r="H2" s="163"/>
       <c r="I2" s="163"/>
@@ -4105,23 +4113,23 @@
     </row>
     <row r="3" spans="1:10" s="164" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="168" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B3" s="163"/>
       <c r="C3" s="163" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="D3" s="163" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E3" s="163" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F3" s="166" t="s">
-        <v>537</v>
+        <v>549</v>
       </c>
       <c r="G3" s="163" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H3" s="163"/>
       <c r="I3" s="163"/>
@@ -4129,31 +4137,39 @@
     </row>
     <row r="4" spans="1:10" s="164" customFormat="1" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" s="168" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B4" s="163"/>
       <c r="E4" s="163" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="F4" s="163" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="G4" s="163" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H4" s="163" t="s">
         <v>550</v>
       </c>
       <c r="I4" s="165" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="J4" s="163" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="163" t="s">
-        <v>548</v>
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="168" t="s">
+        <v>552</v>
+      </c>
+      <c r="B6" s="161" t="s">
+        <v>553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scenarios: lots of writin'
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\project-timber-wolf\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\code\timber-wolf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1649,31 +1649,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>The Redemption Job</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Break into The Gallery to put the paintings back.
-- The Fence discovers he can pull together a Long Con on The Collector by putting them back.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>The Provenance</t>
     </r>
     <r>
@@ -2022,7 +1997,33 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Restoration Job</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- The Fence goes missing, but gives you direction to put the paintings back and to await instructions.
+- The Fence discovers he can pull together a Long Con on The Collector by embarassing him.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">The Bait
+- "I showed him that he never stole the real paintings. He's infuriated."
 - </t>
     </r>
     <r>
@@ -2033,10 +2034,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>You can get anyone you want from prior Heists who survived. (Collector made lots of enemies)
+      <t xml:space="preserve">You can get anyone you want from prior Heists who survived. (Collector made lots of enemies)
 - Super tough board with that long hallway
 - Teach skills for free, or buy skills
-- Drop the "jewel" in for explosives. You get to keep the jewel. He can't resist putting it in his collection. Make it look like you dropped it on your way out.</t>
+- Drop the "jewel" in for explosives. You get to keep the jewel. He can't resist putting it in his collection. Make it look like you dropped it on your way out.
+</t>
     </r>
   </si>
 </sst>
@@ -4052,8 +4054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4065,7 +4067,7 @@
     <row r="1" spans="1:10" s="162" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="167"/>
       <c r="B1" s="160" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C1" s="160" t="s">
         <v>530</v>
@@ -4094,18 +4096,18 @@
     </row>
     <row r="2" spans="1:10" s="164" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="168" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B2" s="163"/>
       <c r="C2" s="163"/>
       <c r="E2" s="163" t="s">
+        <v>545</v>
+      </c>
+      <c r="F2" s="163" t="s">
+        <v>544</v>
+      </c>
+      <c r="G2" s="163" t="s">
         <v>546</v>
-      </c>
-      <c r="F2" s="163" t="s">
-        <v>545</v>
-      </c>
-      <c r="G2" s="163" t="s">
-        <v>547</v>
       </c>
       <c r="H2" s="163"/>
       <c r="I2" s="163"/>
@@ -4113,63 +4115,63 @@
     </row>
     <row r="3" spans="1:10" s="164" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="168" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B3" s="163"/>
       <c r="C3" s="163" t="s">
+        <v>547</v>
+      </c>
+      <c r="D3" s="163" t="s">
+        <v>536</v>
+      </c>
+      <c r="E3" s="163" t="s">
+        <v>535</v>
+      </c>
+      <c r="F3" s="166" t="s">
         <v>548</v>
       </c>
-      <c r="D3" s="163" t="s">
-        <v>537</v>
-      </c>
-      <c r="E3" s="163" t="s">
-        <v>536</v>
-      </c>
-      <c r="F3" s="166" t="s">
-        <v>549</v>
-      </c>
       <c r="G3" s="163" t="s">
-        <v>535</v>
+        <v>554</v>
       </c>
       <c r="H3" s="163"/>
       <c r="I3" s="163"/>
       <c r="J3" s="163"/>
     </row>
-    <row r="4" spans="1:10" s="164" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="164" customFormat="1" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="168" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B4" s="163"/>
       <c r="E4" s="163" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F4" s="163" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G4" s="163" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H4" s="163" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I4" s="165" t="s">
         <v>555</v>
       </c>
       <c r="J4" s="163" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="163" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="168" t="s">
+        <v>551</v>
+      </c>
+      <c r="B6" s="161" t="s">
         <v>552</v>
-      </c>
-      <c r="B6" s="161" t="s">
-        <v>553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
characters: new art beginning to port
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1481,9 +1481,6 @@
     <t>VANTAGE POINT%nWhen outdoors, may 🔍 once per turn%n %nGREAT IN A PINCH%nDuring Escape, may spend %n💡💡 to give 💡 to any player, any number of times.</t>
   </si>
   <si>
-    <t>VANTAGE POINT%nWhen outdoors, may 🔍 once per turn%n %nGOOD IN A PINCH%nDuring Escape, may spend %n💡💡 to give 💡 to any player, one time.%n %nTUNNEL%nIf outdoors, use this action and 💡💡💡🔊 to teleport to the tile of any other player.</t>
-  </si>
-  <si>
     <t>THERE ARE BETTER WAYS%nCannot 👊. For 💡, may exit Guarded spaces for the rest of your turn. In Escape, you require only 1 Escape Move to exit a space with guards.</t>
   </si>
   <si>
@@ -2046,6 +2043,9 @@
   </si>
   <si>
     <t>Whimper🔊</t>
+  </si>
+  <si>
+    <t>VANTAGE POINT%nWhen outdoors, may 🔍 once per turn%n %nGOOD IN A PINCH%nDuring Escape, may spend %n💡💡 to give 💡 to any player, one time.%n %nTUNNEL%nMove character to the Tunnel token.</t>
   </si>
 </sst>
 </file>
@@ -3036,7 +3036,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3335,7 +3335,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L8" s="19" t="str">
         <f>"+3 Memory%n+1 Initial 💡%n %nWalk🔊➜ ⇒%nDash🔊➜➜%n %nHeistate 💡⇒%nStudy💡💡"</f>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="H9" s="16"/>
       <c r="K9" s="19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>79</v>
@@ -3400,7 +3400,7 @@
       </c>
       <c r="H10" s="16"/>
       <c r="K10" s="19" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>79</v>
@@ -3634,7 +3634,7 @@
         <v>362</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="23" t="s">
@@ -3675,7 +3675,7 @@
         <v>362</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H18" s="24"/>
       <c r="K18" s="22" t="s">
@@ -3705,13 +3705,13 @@
         <v>362</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>399</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>482</v>
+        <v>557</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>79</v>
@@ -3737,7 +3737,7 @@
         <v>140</v>
       </c>
       <c r="G20" s="149" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H20" s="149"/>
       <c r="I20" s="150" t="s">
@@ -3747,7 +3747,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="150" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L20" s="150" t="str">
         <f>"+1 Memory%n+1 Initial 💡%n %nLARCENIST⇒%nSWINDLER%n %n+TOSS LOOT"</f>
@@ -3778,13 +3778,13 @@
         <v>140</v>
       </c>
       <c r="G21" s="149" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H21" s="149" t="s">
         <v>408</v>
       </c>
       <c r="K21" s="150" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L21" s="150" t="s">
         <v>79</v>
@@ -3810,11 +3810,11 @@
         <v>140</v>
       </c>
       <c r="G22" s="149" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H22" s="149"/>
       <c r="K22" s="150" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L22" s="150" t="s">
         <v>79</v>
@@ -3822,10 +3822,10 @@
     </row>
     <row r="23" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="157" t="s">
+        <v>507</v>
+      </c>
+      <c r="B23" s="158" t="s">
         <v>508</v>
-      </c>
-      <c r="B23" s="158" t="s">
-        <v>509</v>
       </c>
       <c r="C23" s="159">
         <v>1</v>
@@ -3843,16 +3843,16 @@
         <v>406</v>
       </c>
       <c r="H23" s="159" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I23" s="157" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J23" s="157" t="s">
         <v>405</v>
       </c>
       <c r="K23" s="157" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L23" s="157" t="str">
         <f>"+2 Memory%n+ 1 Initial 💡%n %nWalk &amp; Smash⇒%nDisable📷🔊➜%n %n+Loop Footage"</f>
@@ -3865,10 +3865,10 @@
     </row>
     <row r="24" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="157" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B24" s="157" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C24" s="159">
         <v>2</v>
@@ -3883,13 +3883,13 @@
         <v>407</v>
       </c>
       <c r="G24" s="159" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H24" s="159" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K24" s="157" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="157" customFormat="1" x14ac:dyDescent="0.25">
@@ -3897,7 +3897,7 @@
         <v>405</v>
       </c>
       <c r="B25" s="158" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C25" s="159">
         <v>2</v>
@@ -3912,13 +3912,13 @@
         <v>364</v>
       </c>
       <c r="G25" s="159" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H25" s="159" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K25" s="157" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -4073,47 +4073,47 @@
     <row r="1" spans="1:10" s="162" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="167"/>
       <c r="B1" s="160" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C1" s="160" t="s">
+        <v>528</v>
+      </c>
+      <c r="D1" s="160" t="s">
         <v>529</v>
       </c>
-      <c r="D1" s="160" t="s">
+      <c r="E1" s="160" t="s">
         <v>530</v>
       </c>
-      <c r="E1" s="160" t="s">
+      <c r="F1" s="160" t="s">
         <v>531</v>
       </c>
-      <c r="F1" s="160" t="s">
+      <c r="G1" s="160" t="s">
         <v>532</v>
       </c>
-      <c r="G1" s="160" t="s">
-        <v>533</v>
-      </c>
       <c r="H1" s="160" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I1" s="160" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J1" s="160" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="164" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="168" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B2" s="163"/>
       <c r="C2" s="163"/>
       <c r="E2" s="163" t="s">
+        <v>543</v>
+      </c>
+      <c r="F2" s="163" t="s">
+        <v>542</v>
+      </c>
+      <c r="G2" s="163" t="s">
         <v>544</v>
-      </c>
-      <c r="F2" s="163" t="s">
-        <v>543</v>
-      </c>
-      <c r="G2" s="163" t="s">
-        <v>545</v>
       </c>
       <c r="H2" s="163"/>
       <c r="I2" s="163"/>
@@ -4121,23 +4121,23 @@
     </row>
     <row r="3" spans="1:10" s="164" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="168" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B3" s="163"/>
       <c r="C3" s="163" t="s">
+        <v>545</v>
+      </c>
+      <c r="D3" s="163" t="s">
+        <v>534</v>
+      </c>
+      <c r="E3" s="163" t="s">
+        <v>533</v>
+      </c>
+      <c r="F3" s="166" t="s">
         <v>546</v>
       </c>
-      <c r="D3" s="163" t="s">
-        <v>535</v>
-      </c>
-      <c r="E3" s="163" t="s">
-        <v>534</v>
-      </c>
-      <c r="F3" s="166" t="s">
-        <v>547</v>
-      </c>
       <c r="G3" s="163" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H3" s="163"/>
       <c r="I3" s="163"/>
@@ -4145,39 +4145,39 @@
     </row>
     <row r="4" spans="1:10" s="164" customFormat="1" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="168" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B4" s="163"/>
       <c r="E4" s="163" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F4" s="163" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G4" s="163" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H4" s="163" t="s">
+        <v>547</v>
+      </c>
+      <c r="I4" s="165" t="s">
+        <v>553</v>
+      </c>
+      <c r="J4" s="163" t="s">
         <v>548</v>
-      </c>
-      <c r="I4" s="165" t="s">
-        <v>554</v>
-      </c>
-      <c r="J4" s="163" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="5